<commit_message>
load enemy info frome excel file
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/SceneQuest.xlsx
+++ b/ConfigData/Xlsx/SceneQuest.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
   <si>
     <t>int</t>
     <phoneticPr fontId="18" type="noConversion"/>
@@ -67,6 +67,14 @@
   </si>
   <si>
     <t>海洋</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>EnemyId</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>怪物id</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -754,13 +762,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A1:D4" totalsRowShown="0">
-  <autoFilter ref="A1:D4"/>
-  <tableColumns count="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A1:E4" totalsRowShown="0">
+  <autoFilter ref="A1:E4"/>
+  <tableColumns count="5">
     <tableColumn id="1" name="Id"/>
     <tableColumn id="2" name="Name"/>
     <tableColumn id="10" name="Figue"/>
     <tableColumn id="11" name="Script"/>
+    <tableColumn id="3" name="EnemyId"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1053,10 +1062,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1065,7 +1074,7 @@
     <col min="6" max="7" width="9.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -1078,8 +1087,11 @@
       <c r="D1" t="s">
         <v>8</v>
       </c>
+      <c r="E1" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1092,8 +1104,11 @@
       <c r="D2" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="E2" s="1" t="s">
+        <v>0</v>
+      </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -1106,8 +1121,11 @@
       <c r="D3" s="2" t="s">
         <v>9</v>
       </c>
+      <c r="E3" s="2" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A4">
         <v>42000001</v>
       </c>
@@ -1119,6 +1137,9 @@
       </c>
       <c r="D4" t="s">
         <v>10</v>
+      </c>
+      <c r="E4">
+        <v>43000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
rearannge of code of virtual region
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/SceneQuest.xlsx
+++ b/ConfigData/Xlsx/SceneQuest.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\TOMClassicGit\ConfigData\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\TOMClassicGit\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="25">
   <si>
     <t>int</t>
     <phoneticPr fontId="18" type="noConversion"/>
@@ -75,6 +75,46 @@
   </si>
   <si>
     <t>怪物id</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Level</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>int</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>事件等级</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>int</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>金币奖励系数</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>食物奖励系数</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>经验奖励系数</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>RewardGold</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>RewardFood</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>RewardExp</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -750,6 +790,74 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -762,14 +870,18 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A1:E4" totalsRowShown="0">
-  <autoFilter ref="A1:E4"/>
-  <tableColumns count="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A1:I4" totalsRowShown="0">
+  <autoFilter ref="A1:I4"/>
+  <tableColumns count="9">
     <tableColumn id="1" name="Id"/>
     <tableColumn id="2" name="Name"/>
+    <tableColumn id="4" name="Level"/>
     <tableColumn id="10" name="Figue"/>
     <tableColumn id="11" name="Script"/>
     <tableColumn id="3" name="EnemyId"/>
+    <tableColumn id="5" name="RewardGold"/>
+    <tableColumn id="6" name="RewardFood"/>
+    <tableColumn id="7" name="RewardExp"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -783,7 +895,7 @@
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr val="window" lastClr="CAEACD"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -1062,10 +1174,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1074,7 +1186,7 @@
     <col min="6" max="7" width="9.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -1082,16 +1194,28 @@
         <v>6</v>
       </c>
       <c r="C1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" t="s">
         <v>7</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>8</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>13</v>
       </c>
+      <c r="G1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I1" t="s">
+        <v>24</v>
+      </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1099,16 +1223,28 @@
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="E2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="G2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>0</v>
+      </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -1116,30 +1252,54 @@
         <v>3</v>
       </c>
       <c r="C3" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="E3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="F3" s="2" t="s">
         <v>14</v>
       </c>
+      <c r="G3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>21</v>
+      </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A4">
         <v>42000001</v>
       </c>
       <c r="B4" t="s">
         <v>12</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4" t="s">
         <v>11</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>10</v>
       </c>
-      <c r="E4">
+      <c r="F4">
         <v>43000001</v>
+      </c>
+      <c r="G4">
+        <v>100</v>
+      </c>
+      <c r="H4">
+        <v>100</v>
+      </c>
+      <c r="I4">
+        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
some new event type of scene quest
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/SceneQuest.xlsx
+++ b/ConfigData/Xlsx/SceneQuest.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="46">
   <si>
     <t>int</t>
     <phoneticPr fontId="18" type="noConversion"/>
@@ -115,6 +115,86 @@
   </si>
   <si>
     <t>RewardExp</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>RewardItem1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>奖励道具1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>RewardItem2</t>
+  </si>
+  <si>
+    <t>奖励道具2</t>
+  </si>
+  <si>
+    <t>PunishGold</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>PunishFood</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>金币惩罚系数</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>食物惩罚系数</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>poppyfield</t>
+  </si>
+  <si>
+    <t>poppyfield</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>罂粟花田</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>下水道</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>sewer</t>
+  </si>
+  <si>
+    <t>PunishHealth</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>PunishMental</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>健康惩罚系数</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>精神惩罚系数</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>RewardHealth</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>RewardMental</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>健康奖励系数</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>精神奖励系数</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -302,7 +382,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="36">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -485,6 +565,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -733,7 +825,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -741,6 +833,15 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -870,9 +971,9 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A1:I4" totalsRowShown="0">
-  <autoFilter ref="A1:I4"/>
-  <tableColumns count="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A1:Q6" totalsRowShown="0">
+  <autoFilter ref="A1:Q6"/>
+  <tableColumns count="17">
     <tableColumn id="1" name="Id"/>
     <tableColumn id="2" name="Name"/>
     <tableColumn id="4" name="Level"/>
@@ -881,7 +982,15 @@
     <tableColumn id="3" name="EnemyId"/>
     <tableColumn id="5" name="RewardGold"/>
     <tableColumn id="6" name="RewardFood"/>
+    <tableColumn id="16" name="RewardHealth"/>
+    <tableColumn id="17" name="RewardMental"/>
     <tableColumn id="7" name="RewardExp"/>
+    <tableColumn id="8" name="RewardItem1"/>
+    <tableColumn id="9" name="RewardItem2"/>
+    <tableColumn id="12" name="PunishGold"/>
+    <tableColumn id="13" name="PunishFood"/>
+    <tableColumn id="18" name="PunishHealth"/>
+    <tableColumn id="19" name="PunishMental"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1174,10 +1283,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:Q6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1186,7 +1295,7 @@
     <col min="6" max="7" width="9.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -1212,10 +1321,34 @@
         <v>23</v>
       </c>
       <c r="I1" t="s">
+        <v>42</v>
+      </c>
+      <c r="J1" t="s">
+        <v>43</v>
+      </c>
+      <c r="K1" t="s">
         <v>24</v>
       </c>
+      <c r="L1" t="s">
+        <v>25</v>
+      </c>
+      <c r="M1" t="s">
+        <v>27</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q1" s="3" t="s">
+        <v>39</v>
+      </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1243,8 +1376,32 @@
       <c r="I2" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="J2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="N2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="O2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="P2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q2" s="4" t="s">
+        <v>0</v>
+      </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -1270,10 +1427,34 @@
         <v>20</v>
       </c>
       <c r="I3" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="K3" s="2" t="s">
         <v>21</v>
       </c>
+      <c r="L3" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="N3" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="O3" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="P3" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q3" s="5" t="s">
+        <v>41</v>
+      </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A4">
         <v>42000001</v>
       </c>
@@ -1299,6 +1480,73 @@
         <v>100</v>
       </c>
       <c r="I4">
+        <v>100</v>
+      </c>
+      <c r="J4">
+        <v>100</v>
+      </c>
+      <c r="K4">
+        <v>100</v>
+      </c>
+      <c r="L4">
+        <v>22011180</v>
+      </c>
+      <c r="M4">
+        <v>0</v>
+      </c>
+      <c r="N4">
+        <v>100</v>
+      </c>
+      <c r="O4">
+        <v>100</v>
+      </c>
+      <c r="P4">
+        <v>100</v>
+      </c>
+      <c r="Q4">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="A5">
+        <v>42000002</v>
+      </c>
+      <c r="B5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="A6">
+        <v>42000003</v>
+      </c>
+      <c r="B6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6" t="s">
+        <v>37</v>
+      </c>
+      <c r="E6" t="s">
+        <v>37</v>
+      </c>
+      <c r="F6">
+        <v>43000001</v>
+      </c>
+      <c r="G6">
+        <v>70</v>
+      </c>
+      <c r="H6">
         <v>100</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fix some broken files
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/SceneQuest.xlsx
+++ b/ConfigData/Xlsx/SceneQuest.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17571"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\TOMClassicGit\ConfigData\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\code\TOMClassicGit\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -241,7 +241,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -931,74 +931,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1037,14 +969,14 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="CAEACD"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -1112,6 +1044,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1147,6 +1096,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1326,7 +1292,7 @@
   <dimension ref="A1:Q11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1679,7 +1645,7 @@
         <v>0</v>
       </c>
       <c r="D10" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="E10" t="s">
         <v>51</v>

</xml_diff>

<commit_message>
balance the resource cost of scene quest
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/SceneQuest.xlsx
+++ b/ConfigData/Xlsx/SceneQuest.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17571"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\TOMClassicGit\ConfigData\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\code\TOMClassicGit\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="76">
   <si>
     <t>int</t>
     <phoneticPr fontId="18" type="noConversion"/>
@@ -297,12 +297,24 @@
   </si>
   <si>
     <t>oneline</t>
+  </si>
+  <si>
+    <t>TriggerMulti</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>bool</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>触发多次</t>
+    <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -935,7 +947,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -955,6 +967,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1004,74 +1019,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1084,14 +1031,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A1:R17" totalsRowShown="0">
-  <autoFilter ref="A1:R17"/>
-  <tableColumns count="18">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A1:S17" totalsRowShown="0">
+  <autoFilter ref="A1:S17"/>
+  <tableColumns count="19">
     <tableColumn id="1" name="Id"/>
     <tableColumn id="2" name="Name"/>
     <tableColumn id="4" name="Level"/>
     <tableColumn id="10" name="Figue"/>
     <tableColumn id="11" name="Script"/>
+    <tableColumn id="15" name="TriggerMulti"/>
     <tableColumn id="3" name="EnemyId"/>
     <tableColumn id="14" name="BattleMap"/>
     <tableColumn id="5" name="RewardGold"/>
@@ -1111,14 +1059,14 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="CAEACD"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -1186,6 +1134,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1221,6 +1186,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1397,10 +1379,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R17"/>
+  <dimension ref="A1:S17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1410,7 +1392,7 @@
     <col min="13" max="13" width="9.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -1427,46 +1409,49 @@
         <v>8</v>
       </c>
       <c r="F1" t="s">
+        <v>73</v>
+      </c>
+      <c r="G1" t="s">
         <v>12</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>71</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>21</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>22</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>39</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>40</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>23</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>51</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>52</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="P1" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="P1" s="3" t="s">
+      <c r="Q1" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="Q1" s="3" t="s">
+      <c r="R1" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="R1" s="3" t="s">
+      <c r="S1" s="3" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1483,17 +1468,17 @@
         <v>1</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>0</v>
+        <v>74</v>
       </c>
       <c r="G2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H2" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="I2" s="1" t="s">
-        <v>0</v>
-      </c>
       <c r="J2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1509,7 +1494,7 @@
       <c r="N2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="O2" s="4" t="s">
+      <c r="O2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="P2" s="4" t="s">
@@ -1521,8 +1506,11 @@
       <c r="R2" s="4" t="s">
         <v>0</v>
       </c>
+      <c r="S2" s="4" t="s">
+        <v>0</v>
+      </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -1539,46 +1527,49 @@
         <v>9</v>
       </c>
       <c r="F3" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="G3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="H3" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="I3" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="I3" s="2" t="s">
+      <c r="J3" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="J3" s="2" t="s">
+      <c r="K3" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="K3" s="2" t="s">
+      <c r="L3" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="L3" s="2" t="s">
+      <c r="M3" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="M3" s="2" t="s">
+      <c r="N3" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="N3" s="2" t="s">
+      <c r="O3" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="O3" s="5" t="s">
+      <c r="P3" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="P3" s="5" t="s">
+      <c r="Q3" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="Q3" s="5" t="s">
+      <c r="R3" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="R3" s="5" t="s">
+      <c r="S3" s="5" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A4">
         <v>42000001</v>
       </c>
@@ -1594,14 +1585,12 @@
       <c r="E4" t="s">
         <v>10</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="7"/>
+      <c r="G4">
         <v>43000001</v>
       </c>
-      <c r="G4" s="6" t="s">
+      <c r="H4" s="6" t="s">
         <v>72</v>
-      </c>
-      <c r="H4">
-        <v>100</v>
       </c>
       <c r="I4">
         <v>100</v>
@@ -1616,10 +1605,10 @@
         <v>100</v>
       </c>
       <c r="M4">
+        <v>100</v>
+      </c>
+      <c r="N4">
         <v>22011180</v>
-      </c>
-      <c r="O4">
-        <v>100</v>
       </c>
       <c r="P4">
         <v>100</v>
@@ -1630,8 +1619,11 @@
       <c r="R4">
         <v>100</v>
       </c>
+      <c r="S4">
+        <v>100</v>
+      </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A5">
         <v>42000002</v>
       </c>
@@ -1647,8 +1639,9 @@
       <c r="E5" t="s">
         <v>30</v>
       </c>
+      <c r="F5" s="7"/>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A6">
         <v>42000003</v>
       </c>
@@ -1664,23 +1657,24 @@
       <c r="E6" t="s">
         <v>34</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="7"/>
+      <c r="G6">
         <v>43000001</v>
       </c>
-      <c r="G6" s="6" t="s">
+      <c r="H6" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="H6">
+      <c r="I6">
         <v>70</v>
       </c>
-      <c r="I6">
+      <c r="J6">
         <v>100</v>
       </c>
-      <c r="Q6">
+      <c r="R6">
         <v>70</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A7">
         <v>42000004</v>
       </c>
@@ -1696,17 +1690,18 @@
       <c r="E7" t="s">
         <v>46</v>
       </c>
-      <c r="L7">
-        <v>30</v>
-      </c>
-      <c r="O7">
+      <c r="F7" s="7"/>
+      <c r="M7">
         <v>30</v>
       </c>
       <c r="P7">
         <v>30</v>
       </c>
+      <c r="Q7">
+        <v>30</v>
+      </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A8">
         <v>42000005</v>
       </c>
@@ -1722,14 +1717,15 @@
       <c r="E8" t="s">
         <v>45</v>
       </c>
-      <c r="I8">
+      <c r="F8" s="7"/>
+      <c r="J8">
         <v>100</v>
       </c>
-      <c r="K8">
+      <c r="L8">
         <v>100</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A9">
         <v>42000006</v>
       </c>
@@ -1745,23 +1741,24 @@
       <c r="E9" t="s">
         <v>48</v>
       </c>
-      <c r="F9">
+      <c r="F9" s="7"/>
+      <c r="G9">
         <v>43000002</v>
       </c>
-      <c r="G9" s="6" t="s">
+      <c r="H9" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="H9">
+      <c r="I9">
         <v>100</v>
       </c>
-      <c r="L9">
+      <c r="M9">
         <v>50</v>
       </c>
-      <c r="Q9">
+      <c r="R9">
         <v>100</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A10">
         <v>42000007</v>
       </c>
@@ -1777,17 +1774,18 @@
       <c r="E10" t="s">
         <v>50</v>
       </c>
-      <c r="H10">
+      <c r="F10" s="7"/>
+      <c r="I10">
         <v>250</v>
       </c>
-      <c r="O10">
+      <c r="P10">
         <v>250</v>
       </c>
-      <c r="R10">
+      <c r="S10">
         <v>50</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A11">
         <v>42000008</v>
       </c>
@@ -1803,14 +1801,15 @@
       <c r="E11" t="s">
         <v>53</v>
       </c>
-      <c r="I11">
+      <c r="F11" s="7"/>
+      <c r="J11">
         <v>100</v>
       </c>
-      <c r="N11">
+      <c r="O11">
         <v>23000001</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A12">
         <v>42000009</v>
       </c>
@@ -1826,11 +1825,12 @@
       <c r="E12" t="s">
         <v>53</v>
       </c>
-      <c r="N12">
+      <c r="F12" s="7"/>
+      <c r="O12">
         <v>23000002</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A13">
         <v>42000010</v>
       </c>
@@ -1846,14 +1846,15 @@
       <c r="E13" t="s">
         <v>60</v>
       </c>
-      <c r="N13">
+      <c r="F13" s="7"/>
+      <c r="O13">
         <v>23000003</v>
       </c>
-      <c r="Q13">
+      <c r="R13">
         <v>50</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A14">
         <v>42000011</v>
       </c>
@@ -1869,14 +1870,15 @@
       <c r="E14" t="s">
         <v>61</v>
       </c>
-      <c r="K14">
+      <c r="F14" s="7"/>
+      <c r="L14">
         <v>150</v>
       </c>
-      <c r="N14">
+      <c r="O14">
         <v>23000004</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A15">
         <v>42000012</v>
       </c>
@@ -1892,8 +1894,9 @@
       <c r="E15" t="s">
         <v>66</v>
       </c>
+      <c r="F15" s="7"/>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A16">
         <v>42000013</v>
       </c>
@@ -1909,8 +1912,9 @@
       <c r="E16" t="s">
         <v>65</v>
       </c>
+      <c r="F16" s="7"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A17">
         <v>42000014</v>
       </c>
@@ -1926,6 +1930,7 @@
       <c r="E17" t="s">
         <v>67</v>
       </c>
+      <c r="F17" s="7"/>
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>

</xml_diff>

<commit_message>
finish npc scenequest and draw
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/SceneQuest.xlsx
+++ b/ConfigData/Xlsx/SceneQuest.xlsx
@@ -1,25 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17571"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\code\TOMClassicGit\ConfigData\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\TOMClassicGit\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385"/>
+    <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="SceneQuest" sheetId="1" r:id="rId1"/>
+    <sheet name="MapSetting" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="79">
   <si>
     <t>int</t>
     <phoneticPr fontId="18" type="noConversion"/>
@@ -308,13 +309,24 @@
   </si>
   <si>
     <t>触发多次</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>true</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>npcqiaosiji</t>
+  </si>
+  <si>
+    <t>乔斯基</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1058,8 +1070,36 @@
 </table>
 </file>
 
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表1_3" displayName="表1_3" ref="A1:S4" totalsRowShown="0">
+  <autoFilter ref="A1:S4"/>
+  <tableColumns count="19">
+    <tableColumn id="1" name="Id"/>
+    <tableColumn id="2" name="Name"/>
+    <tableColumn id="4" name="Level"/>
+    <tableColumn id="10" name="Figue"/>
+    <tableColumn id="11" name="Script"/>
+    <tableColumn id="15" name="TriggerMulti"/>
+    <tableColumn id="3" name="EnemyId"/>
+    <tableColumn id="14" name="BattleMap"/>
+    <tableColumn id="5" name="RewardGold"/>
+    <tableColumn id="6" name="RewardFood"/>
+    <tableColumn id="16" name="RewardHealth"/>
+    <tableColumn id="17" name="RewardMental"/>
+    <tableColumn id="7" name="RewardExp"/>
+    <tableColumn id="8" name="RewardItem"/>
+    <tableColumn id="9" name="RewardDrop"/>
+    <tableColumn id="12" name="PunishGold"/>
+    <tableColumn id="13" name="PunishFood"/>
+    <tableColumn id="18" name="PunishHealth"/>
+    <tableColumn id="19" name="PunishMental"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1134,23 +1174,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1186,23 +1209,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1381,8 +1387,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1940,4 +1946,227 @@
     <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:S4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19" x14ac:dyDescent="0.15">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" t="s">
+        <v>73</v>
+      </c>
+      <c r="G1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" t="s">
+        <v>71</v>
+      </c>
+      <c r="I1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J1" t="s">
+        <v>22</v>
+      </c>
+      <c r="K1" t="s">
+        <v>39</v>
+      </c>
+      <c r="L1" t="s">
+        <v>40</v>
+      </c>
+      <c r="M1" t="s">
+        <v>23</v>
+      </c>
+      <c r="N1" t="s">
+        <v>51</v>
+      </c>
+      <c r="O1" t="s">
+        <v>52</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q1" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="R1" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="S1" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.15">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="P2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="R2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="S2" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.15">
+      <c r="A3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="N3" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="O3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="P3" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q3" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="R3" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="S3" s="5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.15">
+      <c r="A4">
+        <v>42100001</v>
+      </c>
+      <c r="B4" t="s">
+        <v>78</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4" t="s">
+        <v>77</v>
+      </c>
+      <c r="E4" t="s">
+        <v>77</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="H4" s="6"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="18" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
finish the scene tooltip
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/SceneQuest.xlsx
+++ b/ConfigData/Xlsx/SceneQuest.xlsx
@@ -9,18 +9,18 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385" activeTab="1"/>
+    <workbookView minimized="1" xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="SceneQuest" sheetId="1" r:id="rId1"/>
     <sheet name="MapSetting" sheetId="3" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="81">
   <si>
     <t>int</t>
     <phoneticPr fontId="18" type="noConversion"/>
@@ -320,6 +320,13 @@
   </si>
   <si>
     <t>乔斯基</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>npcsainisi</t>
+  </si>
+  <si>
+    <t>塞尼斯</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -1071,8 +1078,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表1_3" displayName="表1_3" ref="A1:S4" totalsRowShown="0">
-  <autoFilter ref="A1:S4"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表1_3" displayName="表1_3" ref="A1:S5" totalsRowShown="0">
+  <autoFilter ref="A1:S5"/>
   <tableColumns count="19">
     <tableColumn id="1" name="Id"/>
     <tableColumn id="2" name="Name"/>
@@ -1388,7 +1395,7 @@
   <dimension ref="A1:S17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD4"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1950,10 +1957,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S4"/>
+  <dimension ref="A1:S5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -2161,6 +2168,35 @@
       </c>
       <c r="H4" s="6"/>
     </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.15">
+      <c r="A5">
+        <v>42100002</v>
+      </c>
+      <c r="B5" t="s">
+        <v>80</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5" t="s">
+        <v>79</v>
+      </c>
+      <c r="E5" t="s">
+        <v>79</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="G5">
+        <v>43000101</v>
+      </c>
+      <c r="H5" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="N5">
+        <v>22036101</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
finish the trade mechanical and the relative npcs
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/SceneQuest.xlsx
+++ b/ConfigData/Xlsx/SceneQuest.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385" activeTab="1"/>
+    <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385"/>
   </bookViews>
   <sheets>
     <sheet name="SceneQuest" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="97">
   <si>
     <t>int</t>
     <phoneticPr fontId="18" type="noConversion"/>
@@ -164,10 +164,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>健康惩罚系数</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>精神惩罚系数</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -180,10 +176,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>健康奖励系数</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>精神奖励系数</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -332,6 +324,60 @@
   <si>
     <t>mini</t>
     <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>TradeGold</t>
+  </si>
+  <si>
+    <t>TradeFood</t>
+  </si>
+  <si>
+    <t>TradeHealth</t>
+  </si>
+  <si>
+    <t>TradeMental</t>
+  </si>
+  <si>
+    <t>int</t>
+  </si>
+  <si>
+    <t>金币交易系数</t>
+  </si>
+  <si>
+    <t>食物交易系数</t>
+  </si>
+  <si>
+    <t>精神交易系数</t>
+  </si>
+  <si>
+    <t>治疗巫师</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>curemagician</t>
+  </si>
+  <si>
+    <t>curemagician</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>angel</t>
+  </si>
+  <si>
+    <t>天使</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>sandpile</t>
+  </si>
+  <si>
+    <t>生命奖励系数</t>
+  </si>
+  <si>
+    <t>生命惩罚系数</t>
+  </si>
+  <si>
+    <t>生命交易系数</t>
   </si>
 </sst>
 </file>
@@ -518,7 +564,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="36">
+  <fills count="40">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -713,6 +759,30 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -970,7 +1040,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -993,6 +1063,24 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="37" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="37" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="39" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="38" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="38" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1054,9 +1142,9 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A1:S17" totalsRowShown="0">
-  <autoFilter ref="A1:S17"/>
-  <tableColumns count="19">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A1:W19" totalsRowShown="0">
+  <autoFilter ref="A1:W19"/>
+  <tableColumns count="23">
     <tableColumn id="1" name="Id"/>
     <tableColumn id="2" name="Name"/>
     <tableColumn id="4" name="Level"/>
@@ -1076,15 +1164,19 @@
     <tableColumn id="13" name="PunishFood"/>
     <tableColumn id="18" name="PunishHealth"/>
     <tableColumn id="19" name="PunishMental"/>
+    <tableColumn id="20" name="TradeGold"/>
+    <tableColumn id="21" name="TradeFood"/>
+    <tableColumn id="22" name="TradeHealth"/>
+    <tableColumn id="23" name="TradeMental"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表1_3" displayName="表1_3" ref="A1:S5" totalsRowShown="0">
-  <autoFilter ref="A1:S5"/>
-  <tableColumns count="19">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表1_3" displayName="表1_3" ref="A1:W5" totalsRowShown="0">
+  <autoFilter ref="A1:W5"/>
+  <tableColumns count="23">
     <tableColumn id="1" name="Id"/>
     <tableColumn id="2" name="Name"/>
     <tableColumn id="4" name="Level"/>
@@ -1104,6 +1196,10 @@
     <tableColumn id="13" name="PunishFood"/>
     <tableColumn id="18" name="PunishHealth"/>
     <tableColumn id="19" name="PunishMental"/>
+    <tableColumn id="20" name="TradeGold"/>
+    <tableColumn id="21" name="TradeFood"/>
+    <tableColumn id="22" name="TradeHealth"/>
+    <tableColumn id="23" name="TradeMental"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1396,10 +1492,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S17"/>
+  <dimension ref="A1:W19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1409,7 +1505,7 @@
     <col min="13" max="13" width="9.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -1426,34 +1522,34 @@
         <v>8</v>
       </c>
       <c r="F1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="G1" t="s">
         <v>12</v>
       </c>
       <c r="H1" t="s">
-        <v>71</v>
-      </c>
-      <c r="I1" t="s">
+        <v>69</v>
+      </c>
+      <c r="I1" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="L1" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="L1" t="s">
-        <v>40</v>
-      </c>
-      <c r="M1" t="s">
+      <c r="M1" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="N1" t="s">
-        <v>51</v>
-      </c>
-      <c r="O1" t="s">
-        <v>52</v>
+      <c r="N1" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="O1" s="8" t="s">
+        <v>50</v>
       </c>
       <c r="P1" s="3" t="s">
         <v>26</v>
@@ -1467,8 +1563,20 @@
       <c r="S1" s="3" t="s">
         <v>36</v>
       </c>
+      <c r="T1" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="U1" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="V1" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="W1" s="11" t="s">
+        <v>83</v>
+      </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1485,33 +1593,33 @@
         <v>1</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="I2" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="I2" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="J2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="O2" s="1" t="s">
+      <c r="J2" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="K2" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="L2" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="M2" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="N2" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="O2" s="9" t="s">
         <v>0</v>
       </c>
       <c r="P2" s="4" t="s">
@@ -1526,8 +1634,20 @@
       <c r="S2" s="4" t="s">
         <v>0</v>
       </c>
+      <c r="T2" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="U2" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="V2" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="W2" s="12" t="s">
+        <v>84</v>
+      </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -1544,33 +1664,33 @@
         <v>9</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>13</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="I3" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="I3" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="J3" s="2" t="s">
+      <c r="J3" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="K3" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="L3" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="M3" s="2" t="s">
+      <c r="K3" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="L3" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="M3" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="N3" s="2" t="s">
+      <c r="N3" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="O3" s="2" t="s">
+      <c r="O3" s="10" t="s">
         <v>25</v>
       </c>
       <c r="P3" s="5" t="s">
@@ -1580,18 +1700,30 @@
         <v>29</v>
       </c>
       <c r="R3" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="S3" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="S3" s="5" t="s">
-        <v>38</v>
+      <c r="T3" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="U3" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="V3" s="13" t="s">
+        <v>96</v>
+      </c>
+      <c r="W3" s="13" t="s">
+        <v>87</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A4">
         <v>42000001</v>
       </c>
       <c r="B4" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C4">
         <v>0</v>
@@ -1607,7 +1739,7 @@
         <v>43000001</v>
       </c>
       <c r="H4" s="6" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="I4">
         <v>100</v>
@@ -1640,7 +1772,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A5">
         <v>42000002</v>
       </c>
@@ -1658,7 +1790,7 @@
       </c>
       <c r="F5" s="7"/>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A6">
         <v>42000003</v>
       </c>
@@ -1679,7 +1811,7 @@
         <v>43000001</v>
       </c>
       <c r="H6" s="6" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="I6">
         <v>70</v>
@@ -1691,21 +1823,21 @@
         <v>70</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A7">
         <v>42000004</v>
       </c>
       <c r="B7" t="s">
+        <v>42</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7" t="s">
         <v>44</v>
       </c>
-      <c r="C7">
-        <v>0</v>
-      </c>
-      <c r="D7" t="s">
-        <v>46</v>
-      </c>
       <c r="E7" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="F7" s="7"/>
       <c r="M7">
@@ -1718,21 +1850,21 @@
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A8">
         <v>42000005</v>
       </c>
       <c r="B8" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C8">
         <v>0</v>
       </c>
       <c r="D8" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E8" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F8" s="7"/>
       <c r="J8">
@@ -1742,28 +1874,28 @@
         <v>100</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A9">
         <v>42000006</v>
       </c>
       <c r="B9" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C9">
         <v>0</v>
       </c>
       <c r="D9" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E9" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="F9" s="7"/>
       <c r="G9">
         <v>43000002</v>
       </c>
       <c r="H9" s="6" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="I9">
         <v>100</v>
@@ -1775,21 +1907,21 @@
         <v>100</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A10">
         <v>42000007</v>
       </c>
       <c r="B10" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C10">
         <v>0</v>
       </c>
       <c r="D10" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E10" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F10" s="7"/>
       <c r="I10">
@@ -1802,21 +1934,21 @@
         <v>50</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A11">
         <v>42000008</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C11">
         <v>0</v>
       </c>
       <c r="D11" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E11" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F11" s="7"/>
       <c r="J11">
@@ -1826,42 +1958,42 @@
         <v>23000001</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A12">
         <v>42000009</v>
       </c>
       <c r="B12" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C12">
         <v>0</v>
       </c>
       <c r="D12" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E12" t="s">
-        <v>53</v>
+        <v>93</v>
       </c>
       <c r="F12" s="7"/>
       <c r="O12">
         <v>23000002</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A13">
         <v>42000010</v>
       </c>
       <c r="B13" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C13">
         <v>0</v>
       </c>
       <c r="D13" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E13" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F13" s="7"/>
       <c r="O13">
@@ -1871,21 +2003,21 @@
         <v>50</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A14">
         <v>42000011</v>
       </c>
       <c r="B14" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C14">
         <v>0</v>
       </c>
       <c r="D14" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E14" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="F14" s="7"/>
       <c r="L14">
@@ -1895,59 +2027,107 @@
         <v>23000004</v>
       </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A15">
         <v>42000012</v>
       </c>
       <c r="B15" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C15">
         <v>0</v>
       </c>
       <c r="D15" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E15" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F15" s="7"/>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A16">
         <v>42000013</v>
       </c>
       <c r="B16" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C16">
         <v>0</v>
       </c>
       <c r="D16" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E16" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="F16" s="7"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A17">
         <v>42000014</v>
       </c>
       <c r="B17" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C17">
         <v>0</v>
       </c>
       <c r="D17" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E17" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="F17" s="7"/>
+    </row>
+    <row r="18" spans="1:23" x14ac:dyDescent="0.15">
+      <c r="A18">
+        <v>42000015</v>
+      </c>
+      <c r="B18" t="s">
+        <v>88</v>
+      </c>
+      <c r="C18">
+        <v>0</v>
+      </c>
+      <c r="D18" t="s">
+        <v>90</v>
+      </c>
+      <c r="E18" t="s">
+        <v>89</v>
+      </c>
+      <c r="F18" s="7"/>
+      <c r="T18">
+        <v>-100</v>
+      </c>
+      <c r="V18">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="19" spans="1:23" x14ac:dyDescent="0.15">
+      <c r="A19">
+        <v>42000016</v>
+      </c>
+      <c r="B19" t="s">
+        <v>92</v>
+      </c>
+      <c r="C19">
+        <v>0</v>
+      </c>
+      <c r="D19" t="s">
+        <v>91</v>
+      </c>
+      <c r="E19" t="s">
+        <v>89</v>
+      </c>
+      <c r="F19" s="7"/>
+      <c r="T19">
+        <v>-100</v>
+      </c>
+      <c r="W19">
+        <v>100</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
@@ -1961,10 +2141,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S5"/>
+  <dimension ref="A1:W5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1974,7 +2154,7 @@
     <col min="13" max="13" width="9.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -1991,34 +2171,34 @@
         <v>8</v>
       </c>
       <c r="F1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="G1" t="s">
         <v>12</v>
       </c>
       <c r="H1" t="s">
-        <v>71</v>
-      </c>
-      <c r="I1" t="s">
+        <v>69</v>
+      </c>
+      <c r="I1" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="L1" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="L1" t="s">
-        <v>40</v>
-      </c>
-      <c r="M1" t="s">
+      <c r="M1" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="N1" t="s">
-        <v>51</v>
-      </c>
-      <c r="O1" t="s">
-        <v>52</v>
+      <c r="N1" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="O1" s="8" t="s">
+        <v>50</v>
       </c>
       <c r="P1" s="3" t="s">
         <v>26</v>
@@ -2032,8 +2212,20 @@
       <c r="S1" s="3" t="s">
         <v>36</v>
       </c>
+      <c r="T1" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="U1" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="V1" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="W1" s="11" t="s">
+        <v>83</v>
+      </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -2050,7 +2242,7 @@
         <v>1</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>0</v>
@@ -2058,25 +2250,25 @@
       <c r="H2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="I2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="O2" s="1" t="s">
+      <c r="I2" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="J2" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="K2" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="L2" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="M2" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="N2" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="O2" s="9" t="s">
         <v>0</v>
       </c>
       <c r="P2" s="4" t="s">
@@ -2091,8 +2283,20 @@
       <c r="S2" s="4" t="s">
         <v>0</v>
       </c>
+      <c r="T2" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="U2" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="V2" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="W2" s="12" t="s">
+        <v>84</v>
+      </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -2109,33 +2313,33 @@
         <v>9</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>13</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="I3" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="I3" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="J3" s="2" t="s">
+      <c r="J3" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="K3" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="L3" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="M3" s="2" t="s">
+      <c r="K3" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="L3" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="M3" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="N3" s="2" t="s">
+      <c r="N3" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="O3" s="2" t="s">
+      <c r="O3" s="10" t="s">
         <v>25</v>
       </c>
       <c r="P3" s="5" t="s">
@@ -2145,57 +2349,69 @@
         <v>29</v>
       </c>
       <c r="R3" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="S3" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="S3" s="5" t="s">
-        <v>38</v>
+      <c r="T3" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="U3" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="V3" s="13" t="s">
+        <v>96</v>
+      </c>
+      <c r="W3" s="13" t="s">
+        <v>87</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A4">
         <v>42100001</v>
       </c>
       <c r="B4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C4">
         <v>0</v>
       </c>
       <c r="D4" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E4" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="H4" s="6"/>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A5">
         <v>42100002</v>
       </c>
       <c r="B5" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C5">
         <v>0</v>
       </c>
       <c r="D5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="G5">
         <v>43000101</v>
       </c>
       <c r="H5" s="6" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="N5">
         <v>22036101</v>

</xml_diff>

<commit_message>
add the danger for the scenequest
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/SceneQuest.xlsx
+++ b/ConfigData/Xlsx/SceneQuest.xlsx
@@ -19,8 +19,44 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>real</author>
+  </authors>
+  <commentList>
+    <comment ref="D1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t>real:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t xml:space="preserve">
+0-3</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="135">
   <si>
     <t>int</t>
     <phoneticPr fontId="18" type="noConversion"/>
@@ -490,6 +526,22 @@
   </si>
   <si>
     <t>stone</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>stone</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>危险系数</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>int</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Danger</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -497,7 +549,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="21" x14ac:knownFonts="1">
+  <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -676,6 +728,21 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+    </font>
   </fonts>
   <fills count="41">
     <fill>
@@ -1287,15 +1354,16 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="表3" displayName="表3" ref="A3:X25" totalsRowShown="0" headerRowDxfId="1">
-  <autoFilter ref="A3:X25"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="表3" displayName="表3" ref="A3:Y25" totalsRowShown="0" headerRowDxfId="1">
+  <autoFilter ref="A3:Y25"/>
   <sortState ref="A4:W19">
     <sortCondition ref="A3:A19"/>
   </sortState>
-  <tableColumns count="24">
+  <tableColumns count="25">
     <tableColumn id="1" name="Id"/>
     <tableColumn id="2" name="Name"/>
     <tableColumn id="3" name="Level"/>
+    <tableColumn id="25" name="Danger"/>
     <tableColumn id="24" name="Ename"/>
     <tableColumn id="4" name="Figue"/>
     <tableColumn id="5" name="Script"/>
@@ -1323,15 +1391,16 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="表3_5" displayName="表3_5" ref="A3:X8" totalsRowShown="0" headerRowDxfId="0">
-  <autoFilter ref="A3:X8"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="表3_5" displayName="表3_5" ref="A3:Y8" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="A3:Y8"/>
   <sortState ref="A4:W6">
     <sortCondition ref="A3:A6"/>
   </sortState>
-  <tableColumns count="24">
+  <tableColumns count="25">
     <tableColumn id="1" name="Id"/>
     <tableColumn id="2" name="Name"/>
     <tableColumn id="3" name="Level"/>
+    <tableColumn id="25" name="Danger"/>
     <tableColumn id="24" name="Ename"/>
     <tableColumn id="4" name="Figue"/>
     <tableColumn id="5" name="Script"/>
@@ -1644,27 +1713,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X25"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Y25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S25" sqref="S25"/>
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.875" customWidth="1"/>
-    <col min="4" max="4" width="8.75" customWidth="1"/>
-    <col min="7" max="7" width="5.375" customWidth="1"/>
-    <col min="8" max="8" width="9.75" customWidth="1"/>
-    <col min="9" max="9" width="9.375" customWidth="1"/>
-    <col min="10" max="14" width="4.875" customWidth="1"/>
-    <col min="15" max="16" width="9.375" customWidth="1"/>
-    <col min="17" max="24" width="4.625" customWidth="1"/>
+    <col min="3" max="4" width="5.875" customWidth="1"/>
+    <col min="5" max="5" width="8.75" customWidth="1"/>
+    <col min="8" max="8" width="5.375" customWidth="1"/>
+    <col min="9" max="9" width="9.75" customWidth="1"/>
+    <col min="10" max="10" width="9.375" customWidth="1"/>
+    <col min="11" max="15" width="4.875" customWidth="1"/>
+    <col min="16" max="17" width="9.375" customWidth="1"/>
+    <col min="18" max="25" width="4.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="2" t="s">
         <v>82</v>
       </c>
@@ -1675,70 +1744,73 @@
         <v>84</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="J1" s="10" t="s">
+      <c r="K1" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="K1" s="10" t="s">
+      <c r="L1" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="L1" s="10" t="s">
+      <c r="M1" s="10" t="s">
         <v>87</v>
       </c>
-      <c r="M1" s="10" t="s">
+      <c r="N1" s="10" t="s">
         <v>88</v>
       </c>
-      <c r="N1" s="10" t="s">
+      <c r="O1" s="10" t="s">
         <v>89</v>
       </c>
-      <c r="O1" s="10" t="s">
+      <c r="P1" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="P1" s="10" t="s">
+      <c r="Q1" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="Q1" s="5" t="s">
+      <c r="R1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="R1" s="5" t="s">
+      <c r="S1" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="S1" s="5" t="s">
+      <c r="T1" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="T1" s="5" t="s">
+      <c r="U1" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="U1" s="13" t="s">
+      <c r="V1" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="V1" s="13" t="s">
+      <c r="W1" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="W1" s="13" t="s">
+      <c r="X1" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="X1" s="13" t="s">
+      <c r="Y1" s="13" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>62</v>
       </c>
@@ -1749,31 +1821,31 @@
         <v>64</v>
       </c>
       <c r="D2" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>103</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>63</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>63</v>
       </c>
       <c r="G2" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="H2" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="J2" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="J2" s="9" t="s">
+      <c r="K2" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="K2" s="9" t="s">
+      <c r="L2" s="9" t="s">
         <v>0</v>
-      </c>
-      <c r="L2" s="9" t="s">
-        <v>62</v>
       </c>
       <c r="M2" s="9" t="s">
         <v>62</v>
@@ -1782,13 +1854,13 @@
         <v>62</v>
       </c>
       <c r="O2" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="P2" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="P2" s="9" t="s">
+      <c r="Q2" s="9" t="s">
         <v>62</v>
-      </c>
-      <c r="Q2" s="4" t="s">
-        <v>0</v>
       </c>
       <c r="R2" s="4" t="s">
         <v>0</v>
@@ -1797,10 +1869,10 @@
         <v>0</v>
       </c>
       <c r="T2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="U2" s="4" t="s">
         <v>62</v>
-      </c>
-      <c r="U2" s="12" t="s">
-        <v>28</v>
       </c>
       <c r="V2" s="12" t="s">
         <v>28</v>
@@ -1811,8 +1883,11 @@
       <c r="X2" s="12" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.15">
+      <c r="Y2" s="12" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A3" s="11" t="s">
         <v>67</v>
       </c>
@@ -1823,70 +1898,73 @@
         <v>69</v>
       </c>
       <c r="D3" s="11" t="s">
+        <v>134</v>
+      </c>
+      <c r="E3" s="11" t="s">
         <v>104</v>
       </c>
-      <c r="E3" s="11" t="s">
+      <c r="F3" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="F3" s="11" t="s">
+      <c r="G3" s="11" t="s">
         <v>71</v>
       </c>
-      <c r="G3" s="11" t="s">
+      <c r="H3" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="H3" s="11" t="s">
+      <c r="I3" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="I3" s="11" t="s">
+      <c r="J3" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="J3" s="8" t="s">
+      <c r="K3" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="K3" s="8" t="s">
+      <c r="L3" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="L3" s="8" t="s">
+      <c r="M3" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="M3" s="8" t="s">
+      <c r="N3" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="N3" s="8" t="s">
+      <c r="O3" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="O3" s="8" t="s">
+      <c r="P3" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="P3" s="8" t="s">
+      <c r="Q3" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="Q3" s="3" t="s">
+      <c r="R3" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="R3" s="3" t="s">
+      <c r="S3" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="S3" s="3" t="s">
+      <c r="T3" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="T3" s="3" t="s">
+      <c r="U3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="U3" s="11" t="s">
+      <c r="V3" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="V3" s="11" t="s">
+      <c r="W3" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="W3" s="11" t="s">
+      <c r="X3" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="X3" s="11" t="s">
+      <c r="Y3" s="11" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A4">
         <v>42000001</v>
       </c>
@@ -1896,23 +1974,20 @@
       <c r="C4">
         <v>0</v>
       </c>
-      <c r="D4" t="s">
-        <v>40</v>
-      </c>
       <c r="E4" t="s">
         <v>40</v>
       </c>
       <c r="F4" t="s">
+        <v>40</v>
+      </c>
+      <c r="G4" t="s">
         <v>41</v>
       </c>
-      <c r="H4">
+      <c r="I4">
         <v>43000001</v>
       </c>
-      <c r="I4" t="s">
+      <c r="J4" t="s">
         <v>17</v>
-      </c>
-      <c r="J4">
-        <v>100</v>
       </c>
       <c r="K4">
         <v>100</v>
@@ -1927,10 +2002,10 @@
         <v>100</v>
       </c>
       <c r="O4">
+        <v>100</v>
+      </c>
+      <c r="P4">
         <v>22011180</v>
-      </c>
-      <c r="Q4">
-        <v>100</v>
       </c>
       <c r="R4">
         <v>100</v>
@@ -1941,8 +2016,11 @@
       <c r="T4">
         <v>100</v>
       </c>
-    </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.15">
+      <c r="U4">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A5" s="14">
         <v>42000002</v>
       </c>
@@ -1952,17 +2030,17 @@
       <c r="C5">
         <v>1</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>109</v>
-      </c>
-      <c r="E5" t="s">
-        <v>15</v>
       </c>
       <c r="F5" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.15">
+      <c r="G5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A6" s="14">
         <v>42000003</v>
       </c>
@@ -1972,17 +2050,17 @@
       <c r="C6">
         <v>1</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>107</v>
-      </c>
-      <c r="E6" t="s">
-        <v>14</v>
       </c>
       <c r="F6" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.15">
+      <c r="G6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A7" s="14">
         <v>42000004</v>
       </c>
@@ -1992,17 +2070,17 @@
       <c r="C7">
         <v>1</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>108</v>
-      </c>
-      <c r="E7" t="s">
-        <v>58</v>
       </c>
       <c r="F7" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.15">
+      <c r="G7" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="8" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A8" s="14">
         <v>42000005</v>
       </c>
@@ -2012,23 +2090,23 @@
       <c r="C8">
         <v>1</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>106</v>
-      </c>
-      <c r="E8" t="s">
-        <v>32</v>
       </c>
       <c r="F8" t="s">
         <v>32</v>
       </c>
-      <c r="U8">
+      <c r="G8" t="s">
+        <v>32</v>
+      </c>
+      <c r="V8">
         <v>-100</v>
       </c>
-      <c r="W8">
+      <c r="X8">
         <v>100</v>
       </c>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A9" s="14">
         <v>42000006</v>
       </c>
@@ -2038,23 +2116,23 @@
       <c r="C9">
         <v>1</v>
       </c>
-      <c r="D9" t="s">
-        <v>33</v>
-      </c>
       <c r="E9" t="s">
         <v>33</v>
       </c>
       <c r="F9" t="s">
+        <v>33</v>
+      </c>
+      <c r="G9" t="s">
         <v>32</v>
       </c>
-      <c r="U9">
+      <c r="V9">
         <v>-100</v>
       </c>
-      <c r="X9">
+      <c r="Y9">
         <v>100</v>
       </c>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A10" s="14">
         <v>42000007</v>
       </c>
@@ -2064,23 +2142,23 @@
       <c r="C10">
         <v>1</v>
       </c>
-      <c r="D10" t="s">
-        <v>93</v>
-      </c>
       <c r="E10" t="s">
         <v>93</v>
       </c>
       <c r="F10" t="s">
+        <v>93</v>
+      </c>
+      <c r="G10" t="s">
         <v>32</v>
       </c>
-      <c r="U10">
+      <c r="V10">
         <v>-100</v>
       </c>
-      <c r="V10">
+      <c r="W10">
         <v>100</v>
       </c>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A11">
         <v>42010002</v>
       </c>
@@ -2090,17 +2168,20 @@
       <c r="C11">
         <v>0</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11" t="s">
         <v>111</v>
-      </c>
-      <c r="E11" t="s">
-        <v>6</v>
       </c>
       <c r="F11" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.15">
+      <c r="G11" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A12">
         <v>42010003</v>
       </c>
@@ -2110,32 +2191,35 @@
       <c r="C12">
         <v>0</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12" t="s">
         <v>110</v>
-      </c>
-      <c r="E12" t="s">
-        <v>7</v>
       </c>
       <c r="F12" t="s">
         <v>7</v>
       </c>
-      <c r="H12">
+      <c r="G12" t="s">
+        <v>7</v>
+      </c>
+      <c r="I12">
         <v>43000001</v>
       </c>
-      <c r="I12" t="s">
+      <c r="J12" t="s">
         <v>44</v>
       </c>
-      <c r="J12">
+      <c r="K12">
         <v>70</v>
       </c>
-      <c r="K12">
+      <c r="L12">
         <v>100</v>
       </c>
-      <c r="S12">
+      <c r="T12">
         <v>70</v>
       </c>
     </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A13">
         <v>42010004</v>
       </c>
@@ -2145,26 +2229,29 @@
       <c r="C13">
         <v>0</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13" t="s">
         <v>112</v>
-      </c>
-      <c r="E13" t="s">
-        <v>46</v>
       </c>
       <c r="F13" t="s">
         <v>46</v>
       </c>
-      <c r="N13">
-        <v>30</v>
-      </c>
-      <c r="Q13">
+      <c r="G13" t="s">
+        <v>46</v>
+      </c>
+      <c r="O13">
         <v>30</v>
       </c>
       <c r="R13">
         <v>30</v>
       </c>
-    </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.15">
+      <c r="S13">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A14">
         <v>42010005</v>
       </c>
@@ -2174,23 +2261,23 @@
       <c r="C14">
         <v>0</v>
       </c>
-      <c r="D14" t="s">
+      <c r="E14" t="s">
         <v>113</v>
-      </c>
-      <c r="E14" t="s">
-        <v>9</v>
       </c>
       <c r="F14" t="s">
         <v>9</v>
       </c>
-      <c r="K14">
+      <c r="G14" t="s">
+        <v>9</v>
+      </c>
+      <c r="L14">
         <v>100</v>
       </c>
-      <c r="M14">
+      <c r="N14">
         <v>100</v>
       </c>
     </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A15">
         <v>42010006</v>
       </c>
@@ -2200,32 +2287,35 @@
       <c r="C15">
         <v>0</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="E15" t="s">
         <v>115</v>
-      </c>
-      <c r="E15" t="s">
-        <v>49</v>
       </c>
       <c r="F15" t="s">
         <v>49</v>
       </c>
-      <c r="H15">
+      <c r="G15" t="s">
+        <v>49</v>
+      </c>
+      <c r="I15">
         <v>43000002</v>
       </c>
-      <c r="I15" t="s">
+      <c r="J15" t="s">
         <v>44</v>
       </c>
-      <c r="J15">
+      <c r="K15">
         <v>100</v>
       </c>
-      <c r="N15">
+      <c r="O15">
         <v>50</v>
       </c>
-      <c r="S15">
+      <c r="T15">
         <v>100</v>
       </c>
     </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A16">
         <v>42010007</v>
       </c>
@@ -2235,26 +2325,29 @@
       <c r="C16">
         <v>0</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D16">
+        <v>1</v>
+      </c>
+      <c r="E16" t="s">
         <v>116</v>
-      </c>
-      <c r="E16" t="s">
-        <v>51</v>
       </c>
       <c r="F16" t="s">
         <v>51</v>
       </c>
-      <c r="J16">
+      <c r="G16" t="s">
+        <v>51</v>
+      </c>
+      <c r="K16">
         <v>250</v>
       </c>
-      <c r="Q16">
+      <c r="R16">
         <v>250</v>
       </c>
-      <c r="T16">
+      <c r="U16">
         <v>50</v>
       </c>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A17">
         <v>42010008</v>
       </c>
@@ -2264,23 +2357,23 @@
       <c r="C17">
         <v>0</v>
       </c>
-      <c r="D17" t="s">
+      <c r="E17" t="s">
         <v>117</v>
-      </c>
-      <c r="E17" t="s">
-        <v>53</v>
       </c>
       <c r="F17" t="s">
         <v>53</v>
       </c>
-      <c r="K17">
+      <c r="G17" t="s">
+        <v>53</v>
+      </c>
+      <c r="L17">
         <v>100</v>
       </c>
-      <c r="P17">
+      <c r="Q17">
         <v>23000001</v>
       </c>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A18">
         <v>42010009</v>
       </c>
@@ -2290,20 +2383,20 @@
       <c r="C18">
         <v>0</v>
       </c>
-      <c r="D18" t="s">
-        <v>34</v>
-      </c>
       <c r="E18" t="s">
         <v>34</v>
       </c>
       <c r="F18" t="s">
+        <v>34</v>
+      </c>
+      <c r="G18" t="s">
         <v>126</v>
       </c>
-      <c r="P18">
+      <c r="Q18">
         <v>23000002</v>
       </c>
     </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A19">
         <v>42010010</v>
       </c>
@@ -2313,23 +2406,23 @@
       <c r="C19">
         <v>0</v>
       </c>
-      <c r="D19" t="s">
-        <v>54</v>
-      </c>
       <c r="E19" t="s">
         <v>54</v>
       </c>
       <c r="F19" t="s">
+        <v>54</v>
+      </c>
+      <c r="G19" t="s">
         <v>127</v>
       </c>
-      <c r="P19">
+      <c r="Q19">
         <v>23000003</v>
       </c>
-      <c r="S19">
+      <c r="T19">
         <v>50</v>
       </c>
     </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A20">
         <v>42010011</v>
       </c>
@@ -2339,23 +2432,23 @@
       <c r="C20">
         <v>0</v>
       </c>
-      <c r="D20" t="s">
+      <c r="E20" t="s">
         <v>114</v>
-      </c>
-      <c r="E20" t="s">
-        <v>55</v>
       </c>
       <c r="F20" t="s">
         <v>55</v>
       </c>
-      <c r="M20">
+      <c r="G20" t="s">
+        <v>55</v>
+      </c>
+      <c r="N20">
         <v>150</v>
       </c>
-      <c r="P20">
+      <c r="Q20">
         <v>23000004</v>
       </c>
     </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A21">
         <v>42010012</v>
       </c>
@@ -2365,38 +2458,41 @@
       <c r="C21">
         <v>0</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D21">
+        <v>2</v>
+      </c>
+      <c r="E21" t="s">
         <v>128</v>
-      </c>
-      <c r="E21" t="s">
-        <v>118</v>
       </c>
       <c r="F21" t="s">
         <v>118</v>
       </c>
-      <c r="H21">
+      <c r="G21" t="s">
+        <v>118</v>
+      </c>
+      <c r="I21">
         <v>43000005</v>
       </c>
-      <c r="I21" t="s">
+      <c r="J21" t="s">
         <v>17</v>
       </c>
-      <c r="J21">
+      <c r="K21">
         <v>200</v>
       </c>
-      <c r="K21">
+      <c r="L21">
         <v>50</v>
       </c>
-      <c r="P21">
+      <c r="Q21">
         <v>23000102</v>
-      </c>
-      <c r="S21">
-        <v>150</v>
       </c>
       <c r="T21">
         <v>150</v>
       </c>
-    </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.15">
+      <c r="U21">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="22" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A22">
         <v>42010013</v>
       </c>
@@ -2406,8 +2502,8 @@
       <c r="C22">
         <v>0</v>
       </c>
-      <c r="D22" t="s">
-        <v>121</v>
+      <c r="D22">
+        <v>1</v>
       </c>
       <c r="E22" t="s">
         <v>121</v>
@@ -2415,23 +2511,26 @@
       <c r="F22" t="s">
         <v>121</v>
       </c>
-      <c r="H22">
+      <c r="G22" t="s">
+        <v>121</v>
+      </c>
+      <c r="I22">
         <v>43000007</v>
       </c>
-      <c r="I22" t="s">
+      <c r="J22" t="s">
         <v>44</v>
       </c>
-      <c r="J22">
+      <c r="K22">
         <v>50</v>
       </c>
-      <c r="K22">
+      <c r="L22">
         <v>150</v>
       </c>
-      <c r="S22">
+      <c r="T22">
         <v>100</v>
       </c>
     </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A23">
         <v>42010014</v>
       </c>
@@ -2441,8 +2540,8 @@
       <c r="C23">
         <v>0</v>
       </c>
-      <c r="D23" t="s">
-        <v>123</v>
+      <c r="D23">
+        <v>2</v>
       </c>
       <c r="E23" t="s">
         <v>123</v>
@@ -2450,29 +2549,32 @@
       <c r="F23" t="s">
         <v>123</v>
       </c>
-      <c r="H23">
+      <c r="G23" t="s">
+        <v>123</v>
+      </c>
+      <c r="I23">
         <v>43000004</v>
       </c>
-      <c r="I23" t="s">
+      <c r="J23" t="s">
         <v>17</v>
       </c>
-      <c r="J23">
+      <c r="K23">
         <v>100</v>
       </c>
-      <c r="N23">
+      <c r="O23">
         <v>100</v>
       </c>
-      <c r="P23">
+      <c r="Q23">
         <v>23000101</v>
-      </c>
-      <c r="S23">
-        <v>100</v>
       </c>
       <c r="T23">
         <v>100</v>
       </c>
-    </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.15">
+      <c r="U23">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="24" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A24">
         <v>42010015</v>
       </c>
@@ -2482,17 +2584,17 @@
       <c r="C24">
         <v>0</v>
       </c>
-      <c r="D24" t="s">
-        <v>125</v>
-      </c>
       <c r="E24" t="s">
         <v>125</v>
       </c>
       <c r="F24" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.15">
+      <c r="G24" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="25" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A25">
         <v>42010016</v>
       </c>
@@ -2502,51 +2604,55 @@
       <c r="C25">
         <v>0</v>
       </c>
-      <c r="D25" t="s">
-        <v>130</v>
+      <c r="D25">
+        <v>3</v>
       </c>
       <c r="E25" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="F25" t="s">
         <v>130</v>
       </c>
-      <c r="S25">
+      <c r="G25" t="s">
+        <v>130</v>
+      </c>
+      <c r="T25">
         <v>80</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X8"/>
+  <dimension ref="A1:Y8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="D1" sqref="D1:D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.5" customWidth="1"/>
-    <col min="4" max="4" width="9.25" customWidth="1"/>
-    <col min="7" max="7" width="5.5" customWidth="1"/>
-    <col min="8" max="8" width="9.75" customWidth="1"/>
-    <col min="9" max="9" width="11.75" customWidth="1"/>
-    <col min="10" max="14" width="4.125" customWidth="1"/>
-    <col min="15" max="15" width="9.75" customWidth="1"/>
-    <col min="16" max="16" width="7.5" customWidth="1"/>
-    <col min="17" max="24" width="5" customWidth="1"/>
+    <col min="3" max="4" width="5.5" customWidth="1"/>
+    <col min="5" max="5" width="9.25" customWidth="1"/>
+    <col min="8" max="8" width="5.5" customWidth="1"/>
+    <col min="9" max="9" width="9.75" customWidth="1"/>
+    <col min="10" max="10" width="11.75" customWidth="1"/>
+    <col min="11" max="15" width="4.125" customWidth="1"/>
+    <col min="16" max="16" width="9.75" customWidth="1"/>
+    <col min="17" max="17" width="7.5" customWidth="1"/>
+    <col min="18" max="25" width="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="2" t="s">
         <v>82</v>
       </c>
@@ -2557,70 +2663,73 @@
         <v>84</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="J1" s="10" t="s">
+      <c r="K1" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="K1" s="10" t="s">
+      <c r="L1" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="L1" s="10" t="s">
+      <c r="M1" s="10" t="s">
         <v>87</v>
       </c>
-      <c r="M1" s="10" t="s">
+      <c r="N1" s="10" t="s">
         <v>88</v>
       </c>
-      <c r="N1" s="10" t="s">
+      <c r="O1" s="10" t="s">
         <v>89</v>
       </c>
-      <c r="O1" s="10" t="s">
+      <c r="P1" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="P1" s="10" t="s">
+      <c r="Q1" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="Q1" s="5" t="s">
+      <c r="R1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="R1" s="5" t="s">
+      <c r="S1" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="S1" s="5" t="s">
+      <c r="T1" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="T1" s="5" t="s">
+      <c r="U1" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="U1" s="13" t="s">
+      <c r="V1" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="V1" s="13" t="s">
+      <c r="W1" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="W1" s="13" t="s">
+      <c r="X1" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="X1" s="13" t="s">
+      <c r="Y1" s="13" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>62</v>
       </c>
@@ -2631,31 +2740,31 @@
         <v>64</v>
       </c>
       <c r="D2" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>103</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>63</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>63</v>
       </c>
       <c r="G2" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="H2" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="J2" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="J2" s="9" t="s">
+      <c r="K2" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="K2" s="9" t="s">
+      <c r="L2" s="9" t="s">
         <v>0</v>
-      </c>
-      <c r="L2" s="9" t="s">
-        <v>62</v>
       </c>
       <c r="M2" s="9" t="s">
         <v>62</v>
@@ -2664,13 +2773,13 @@
         <v>62</v>
       </c>
       <c r="O2" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="P2" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="P2" s="9" t="s">
+      <c r="Q2" s="9" t="s">
         <v>62</v>
-      </c>
-      <c r="Q2" s="4" t="s">
-        <v>0</v>
       </c>
       <c r="R2" s="4" t="s">
         <v>0</v>
@@ -2679,10 +2788,10 @@
         <v>0</v>
       </c>
       <c r="T2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="U2" s="4" t="s">
         <v>62</v>
-      </c>
-      <c r="U2" s="12" t="s">
-        <v>28</v>
       </c>
       <c r="V2" s="12" t="s">
         <v>28</v>
@@ -2693,8 +2802,11 @@
       <c r="X2" s="12" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.15">
+      <c r="Y2" s="12" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A3" s="11" t="s">
         <v>67</v>
       </c>
@@ -2705,70 +2817,73 @@
         <v>69</v>
       </c>
       <c r="D3" s="11" t="s">
+        <v>134</v>
+      </c>
+      <c r="E3" s="11" t="s">
         <v>104</v>
       </c>
-      <c r="E3" s="11" t="s">
+      <c r="F3" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="F3" s="11" t="s">
+      <c r="G3" s="11" t="s">
         <v>71</v>
       </c>
-      <c r="G3" s="11" t="s">
+      <c r="H3" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="H3" s="11" t="s">
+      <c r="I3" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="I3" s="11" t="s">
+      <c r="J3" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="J3" s="8" t="s">
+      <c r="K3" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="K3" s="8" t="s">
+      <c r="L3" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="L3" s="8" t="s">
+      <c r="M3" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="M3" s="8" t="s">
+      <c r="N3" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="N3" s="8" t="s">
+      <c r="O3" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="O3" s="8" t="s">
+      <c r="P3" s="8" t="s">
         <v>99</v>
       </c>
-      <c r="P3" s="8" t="s">
+      <c r="Q3" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="Q3" s="3" t="s">
+      <c r="R3" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="R3" s="3" t="s">
+      <c r="S3" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="S3" s="3" t="s">
+      <c r="T3" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="T3" s="3" t="s">
+      <c r="U3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="U3" s="11" t="s">
+      <c r="V3" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="V3" s="11" t="s">
+      <c r="W3" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="W3" s="11" t="s">
+      <c r="X3" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="X3" s="11" t="s">
+      <c r="Y3" s="11" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A4" s="14">
         <v>42020001</v>
       </c>
@@ -2778,30 +2893,30 @@
       <c r="C4">
         <v>0</v>
       </c>
-      <c r="D4" t="s">
-        <v>97</v>
-      </c>
       <c r="E4" t="s">
         <v>97</v>
       </c>
       <c r="F4" t="s">
         <v>97</v>
       </c>
-      <c r="G4" s="7" t="s">
+      <c r="G4" t="s">
+        <v>97</v>
+      </c>
+      <c r="H4" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="I4" s="15"/>
-      <c r="U4">
+      <c r="J4" s="15"/>
+      <c r="V4">
         <v>-300</v>
-      </c>
-      <c r="W4">
-        <v>1000</v>
       </c>
       <c r="X4">
         <v>1000</v>
       </c>
-    </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.15">
+      <c r="Y4">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A5" s="14">
         <v>42020002</v>
       </c>
@@ -2811,27 +2926,27 @@
       <c r="C5">
         <v>0</v>
       </c>
-      <c r="D5" t="s">
-        <v>98</v>
-      </c>
       <c r="E5" t="s">
         <v>98</v>
       </c>
       <c r="F5" t="s">
         <v>98</v>
       </c>
-      <c r="G5" s="7" t="s">
+      <c r="G5" t="s">
+        <v>98</v>
+      </c>
+      <c r="H5" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="I5" s="15"/>
-      <c r="U5">
+      <c r="J5" s="15"/>
+      <c r="V5">
         <v>-200</v>
       </c>
-      <c r="V5">
+      <c r="W5">
         <v>1000</v>
       </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A6" s="14">
         <v>42020003</v>
       </c>
@@ -2841,21 +2956,21 @@
       <c r="C6">
         <v>0</v>
       </c>
-      <c r="D6" t="s">
-        <v>102</v>
-      </c>
       <c r="E6" t="s">
         <v>102</v>
       </c>
       <c r="F6" t="s">
+        <v>102</v>
+      </c>
+      <c r="G6" t="s">
         <v>101</v>
       </c>
-      <c r="G6" s="7" t="s">
+      <c r="H6" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="I6" s="15"/>
-    </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.15">
+      <c r="J6" s="15"/>
+    </row>
+    <row r="7" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A7">
         <v>42030001</v>
       </c>
@@ -2865,21 +2980,21 @@
       <c r="C7">
         <v>0</v>
       </c>
-      <c r="D7" t="s">
-        <v>20</v>
-      </c>
       <c r="E7" t="s">
         <v>20</v>
       </c>
       <c r="F7" t="s">
         <v>20</v>
       </c>
-      <c r="G7" s="7" t="s">
+      <c r="G7" t="s">
+        <v>20</v>
+      </c>
+      <c r="H7" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="I7" s="6"/>
-    </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.15">
+      <c r="J7" s="6"/>
+    </row>
+    <row r="8" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A8">
         <v>42030002</v>
       </c>
@@ -2889,25 +3004,25 @@
       <c r="C8">
         <v>0</v>
       </c>
-      <c r="D8" t="s">
-        <v>22</v>
-      </c>
       <c r="E8" t="s">
         <v>22</v>
       </c>
       <c r="F8" t="s">
         <v>22</v>
       </c>
-      <c r="G8" s="7" t="s">
+      <c r="G8" t="s">
+        <v>22</v>
+      </c>
+      <c r="H8" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="H8">
+      <c r="I8">
         <v>43000101</v>
       </c>
-      <c r="I8" s="16" t="s">
+      <c r="J8" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="O8">
+      <c r="P8">
         <v>22036101</v>
       </c>
     </row>

</xml_diff>

<commit_message>
enable quest to open rival
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/SceneQuest.xlsx
+++ b/ConfigData/Xlsx/SceneQuest.xlsx
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="145">
   <si>
     <t>int</t>
     <phoneticPr fontId="18" type="noConversion"/>
@@ -569,6 +569,18 @@
   </si>
   <si>
     <t>ruintown1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>解锁对象</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>int</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>RivalId</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -1381,12 +1393,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="表3" displayName="表3" ref="A3:Y27" totalsRowShown="0" headerRowDxfId="1">
-  <autoFilter ref="A3:Y27"/>
-  <sortState ref="A4:Y27">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="表3" displayName="表3" ref="A3:Z27" totalsRowShown="0" headerRowDxfId="1">
+  <autoFilter ref="A3:Z27"/>
+  <sortState ref="A4:Z27">
     <sortCondition ref="A3:A27"/>
   </sortState>
-  <tableColumns count="25">
+  <tableColumns count="26">
     <tableColumn id="1" name="Id"/>
     <tableColumn id="2" name="Name"/>
     <tableColumn id="3" name="Level"/>
@@ -1404,6 +1416,7 @@
     <tableColumn id="13" name="RewardExp"/>
     <tableColumn id="14" name="RewardItem"/>
     <tableColumn id="15" name="RewardDrop"/>
+    <tableColumn id="26" name="RivalId"/>
     <tableColumn id="16" name="PunishGold"/>
     <tableColumn id="17" name="PunishFood"/>
     <tableColumn id="18" name="PunishHealth"/>
@@ -1418,12 +1431,12 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="表3_5" displayName="表3_5" ref="A3:Y8" totalsRowShown="0" headerRowDxfId="0">
-  <autoFilter ref="A3:Y8"/>
-  <sortState ref="A4:W6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="表3_5" displayName="表3_5" ref="A3:Z8" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="A3:Z8"/>
+  <sortState ref="A4:X6">
     <sortCondition ref="A3:A6"/>
   </sortState>
-  <tableColumns count="25">
+  <tableColumns count="26">
     <tableColumn id="1" name="Id"/>
     <tableColumn id="2" name="Name"/>
     <tableColumn id="3" name="Level"/>
@@ -1441,6 +1454,7 @@
     <tableColumn id="13" name="RewardExp"/>
     <tableColumn id="14" name="RewardItem"/>
     <tableColumn id="15" name="RewardDrop"/>
+    <tableColumn id="26" name="RivalId"/>
     <tableColumn id="16" name="PunishGold"/>
     <tableColumn id="17" name="PunishFood"/>
     <tableColumn id="18" name="PunishHealth"/>
@@ -1775,10 +1789,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y27"/>
+  <dimension ref="A1:Z27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M16" sqref="M16"/>
+      <selection activeCell="R1" sqref="R1:R3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1790,11 +1804,11 @@
     <col min="9" max="9" width="9.75" customWidth="1"/>
     <col min="10" max="10" width="9.375" customWidth="1"/>
     <col min="11" max="15" width="4.875" customWidth="1"/>
-    <col min="16" max="17" width="9.375" customWidth="1"/>
-    <col min="18" max="25" width="4.625" customWidth="1"/>
+    <col min="16" max="18" width="9.375" customWidth="1"/>
+    <col min="19" max="26" width="4.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="2" t="s">
         <v>82</v>
       </c>
@@ -1846,32 +1860,35 @@
       <c r="Q1" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="R1" s="5" t="s">
+      <c r="R1" s="10" t="s">
+        <v>142</v>
+      </c>
+      <c r="S1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="S1" s="5" t="s">
+      <c r="T1" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="T1" s="5" t="s">
+      <c r="U1" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="U1" s="5" t="s">
+      <c r="V1" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="V1" s="13" t="s">
+      <c r="W1" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="W1" s="13" t="s">
+      <c r="X1" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="X1" s="13" t="s">
+      <c r="Y1" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="Y1" s="13" t="s">
+      <c r="Z1" s="13" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>62</v>
       </c>
@@ -1923,8 +1940,8 @@
       <c r="Q2" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="R2" s="4" t="s">
-        <v>0</v>
+      <c r="R2" s="9" t="s">
+        <v>143</v>
       </c>
       <c r="S2" s="4" t="s">
         <v>0</v>
@@ -1933,10 +1950,10 @@
         <v>0</v>
       </c>
       <c r="U2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="V2" s="4" t="s">
         <v>62</v>
-      </c>
-      <c r="V2" s="12" t="s">
-        <v>28</v>
       </c>
       <c r="W2" s="12" t="s">
         <v>28</v>
@@ -1947,8 +1964,11 @@
       <c r="Y2" s="12" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.15">
+      <c r="Z2" s="12" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A3" s="11" t="s">
         <v>67</v>
       </c>
@@ -2000,32 +2020,35 @@
       <c r="Q3" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="R3" s="3" t="s">
+      <c r="R3" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="S3" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="S3" s="3" t="s">
+      <c r="T3" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="T3" s="3" t="s">
+      <c r="U3" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="U3" s="3" t="s">
+      <c r="V3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="V3" s="11" t="s">
+      <c r="W3" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="W3" s="11" t="s">
+      <c r="X3" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="X3" s="11" t="s">
+      <c r="Y3" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="Y3" s="11" t="s">
+      <c r="Z3" s="11" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A4">
         <v>42000001</v>
       </c>
@@ -2068,9 +2091,6 @@
       <c r="P4">
         <v>22011180</v>
       </c>
-      <c r="R4">
-        <v>100</v>
-      </c>
       <c r="S4">
         <v>100</v>
       </c>
@@ -2080,8 +2100,11 @@
       <c r="U4">
         <v>100</v>
       </c>
-    </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.15">
+      <c r="V4">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A5" s="14">
         <v>42000002</v>
       </c>
@@ -2101,7 +2124,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A6" s="14">
         <v>42000003</v>
       </c>
@@ -2121,7 +2144,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A7" s="14">
         <v>42000004</v>
       </c>
@@ -2141,7 +2164,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A8" s="14">
         <v>42000005</v>
       </c>
@@ -2160,14 +2183,14 @@
       <c r="G8" t="s">
         <v>32</v>
       </c>
-      <c r="V8">
+      <c r="W8">
         <v>-100</v>
       </c>
-      <c r="X8">
+      <c r="Y8">
         <v>100</v>
       </c>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A9" s="14">
         <v>42000006</v>
       </c>
@@ -2186,14 +2209,14 @@
       <c r="G9" t="s">
         <v>32</v>
       </c>
-      <c r="V9">
+      <c r="W9">
         <v>-100</v>
       </c>
-      <c r="Y9">
+      <c r="Z9">
         <v>100</v>
       </c>
     </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A10" s="14">
         <v>42000007</v>
       </c>
@@ -2212,14 +2235,14 @@
       <c r="G10" t="s">
         <v>32</v>
       </c>
-      <c r="V10">
+      <c r="W10">
         <v>-100</v>
       </c>
-      <c r="W10">
+      <c r="X10">
         <v>100</v>
       </c>
     </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A11">
         <v>42010001</v>
       </c>
@@ -2239,7 +2262,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A12">
         <v>42010002</v>
       </c>
@@ -2262,7 +2285,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A13">
         <v>42010003</v>
       </c>
@@ -2296,11 +2319,11 @@
       <c r="L13">
         <v>100</v>
       </c>
-      <c r="T13">
+      <c r="U13">
         <v>70</v>
       </c>
     </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A14">
         <v>42010004</v>
       </c>
@@ -2325,14 +2348,14 @@
       <c r="O14">
         <v>30</v>
       </c>
-      <c r="R14">
-        <v>30</v>
-      </c>
       <c r="S14">
         <v>30</v>
       </c>
-    </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.15">
+      <c r="T14">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A15">
         <v>42010005</v>
       </c>
@@ -2358,7 +2381,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A16">
         <v>42010006</v>
       </c>
@@ -2392,11 +2415,11 @@
       <c r="O16">
         <v>50</v>
       </c>
-      <c r="T16">
+      <c r="U16">
         <v>100</v>
       </c>
     </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:22" x14ac:dyDescent="0.15">
       <c r="A17">
         <v>42010007</v>
       </c>
@@ -2421,14 +2444,14 @@
       <c r="K17">
         <v>250</v>
       </c>
-      <c r="R17">
+      <c r="S17">
         <v>250</v>
       </c>
-      <c r="U17">
+      <c r="V17">
         <v>50</v>
       </c>
     </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:22" x14ac:dyDescent="0.15">
       <c r="A18">
         <v>42010008</v>
       </c>
@@ -2454,7 +2477,7 @@
         <v>23000001</v>
       </c>
     </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:22" x14ac:dyDescent="0.15">
       <c r="A19">
         <v>42010009</v>
       </c>
@@ -2477,7 +2500,7 @@
         <v>23000002</v>
       </c>
     </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:22" x14ac:dyDescent="0.15">
       <c r="A20">
         <v>42010010</v>
       </c>
@@ -2499,11 +2522,11 @@
       <c r="Q20">
         <v>23000003</v>
       </c>
-      <c r="T20">
+      <c r="U20">
         <v>50</v>
       </c>
     </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:22" x14ac:dyDescent="0.15">
       <c r="A21">
         <v>42010011</v>
       </c>
@@ -2529,7 +2552,7 @@
         <v>23000004</v>
       </c>
     </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:22" x14ac:dyDescent="0.15">
       <c r="A22">
         <v>42010012</v>
       </c>
@@ -2566,14 +2589,14 @@
       <c r="Q22">
         <v>23000102</v>
       </c>
-      <c r="T22">
-        <v>150</v>
-      </c>
       <c r="U22">
         <v>150</v>
       </c>
-    </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.15">
+      <c r="V22">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="23" spans="1:22" x14ac:dyDescent="0.15">
       <c r="A23">
         <v>42010013</v>
       </c>
@@ -2607,11 +2630,11 @@
       <c r="L23">
         <v>150</v>
       </c>
-      <c r="T23">
+      <c r="U23">
         <v>100</v>
       </c>
     </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:22" x14ac:dyDescent="0.15">
       <c r="A24">
         <v>42010014</v>
       </c>
@@ -2648,14 +2671,14 @@
       <c r="Q24">
         <v>23000101</v>
       </c>
-      <c r="T24">
-        <v>100</v>
-      </c>
       <c r="U24">
         <v>100</v>
       </c>
-    </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.15">
+      <c r="V24">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="25" spans="1:22" x14ac:dyDescent="0.15">
       <c r="A25">
         <v>42010015</v>
       </c>
@@ -2677,11 +2700,11 @@
       <c r="G25" t="s">
         <v>130</v>
       </c>
-      <c r="T25">
+      <c r="U25">
         <v>80</v>
       </c>
     </row>
-    <row r="26" spans="1:21" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:22" x14ac:dyDescent="0.15">
       <c r="A26">
         <v>42010016</v>
       </c>
@@ -2704,7 +2727,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="27" spans="1:21" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:22" x14ac:dyDescent="0.15">
       <c r="A27">
         <v>42010017</v>
       </c>
@@ -2744,7 +2767,7 @@
       <c r="Q27">
         <v>23000102</v>
       </c>
-      <c r="T27">
+      <c r="U27">
         <v>100</v>
       </c>
     </row>
@@ -2760,10 +2783,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y8"/>
+  <dimension ref="A1:Z8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D3"/>
+      <selection activeCell="R3" sqref="R1:R3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -2777,10 +2800,11 @@
     <col min="11" max="15" width="4.125" customWidth="1"/>
     <col min="16" max="16" width="9.75" customWidth="1"/>
     <col min="17" max="17" width="7.5" customWidth="1"/>
-    <col min="18" max="25" width="5" customWidth="1"/>
+    <col min="18" max="18" width="9.375" customWidth="1"/>
+    <col min="19" max="26" width="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="2" t="s">
         <v>82</v>
       </c>
@@ -2832,32 +2856,35 @@
       <c r="Q1" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="R1" s="5" t="s">
+      <c r="R1" s="10" t="s">
+        <v>142</v>
+      </c>
+      <c r="S1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="S1" s="5" t="s">
+      <c r="T1" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="T1" s="5" t="s">
+      <c r="U1" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="U1" s="5" t="s">
+      <c r="V1" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="V1" s="13" t="s">
+      <c r="W1" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="W1" s="13" t="s">
+      <c r="X1" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="X1" s="13" t="s">
+      <c r="Y1" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="Y1" s="13" t="s">
+      <c r="Z1" s="13" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>62</v>
       </c>
@@ -2909,8 +2936,8 @@
       <c r="Q2" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="R2" s="4" t="s">
-        <v>0</v>
+      <c r="R2" s="9" t="s">
+        <v>143</v>
       </c>
       <c r="S2" s="4" t="s">
         <v>0</v>
@@ -2919,10 +2946,10 @@
         <v>0</v>
       </c>
       <c r="U2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="V2" s="4" t="s">
         <v>62</v>
-      </c>
-      <c r="V2" s="12" t="s">
-        <v>28</v>
       </c>
       <c r="W2" s="12" t="s">
         <v>28</v>
@@ -2933,8 +2960,11 @@
       <c r="Y2" s="12" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.15">
+      <c r="Z2" s="12" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A3" s="11" t="s">
         <v>67</v>
       </c>
@@ -2986,32 +3016,35 @@
       <c r="Q3" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="R3" s="3" t="s">
+      <c r="R3" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="S3" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="S3" s="3" t="s">
+      <c r="T3" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="T3" s="3" t="s">
+      <c r="U3" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="U3" s="3" t="s">
+      <c r="V3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="V3" s="11" t="s">
+      <c r="W3" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="W3" s="11" t="s">
+      <c r="X3" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="X3" s="11" t="s">
+      <c r="Y3" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="Y3" s="11" t="s">
+      <c r="Z3" s="11" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A4" s="14">
         <v>42020001</v>
       </c>
@@ -3034,17 +3067,17 @@
         <v>19</v>
       </c>
       <c r="J4" s="15"/>
-      <c r="V4">
+      <c r="W4">
         <v>-300</v>
-      </c>
-      <c r="X4">
-        <v>1000</v>
       </c>
       <c r="Y4">
         <v>1000</v>
       </c>
-    </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.15">
+      <c r="Z4">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A5" s="14">
         <v>42020002</v>
       </c>
@@ -3067,14 +3100,14 @@
         <v>19</v>
       </c>
       <c r="J5" s="15"/>
-      <c r="V5">
+      <c r="W5">
         <v>-200</v>
       </c>
-      <c r="W5">
+      <c r="X5">
         <v>1000</v>
       </c>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A6" s="14">
         <v>42020003</v>
       </c>
@@ -3098,7 +3131,7 @@
       </c>
       <c r="J6" s="15"/>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A7">
         <v>42030001</v>
       </c>
@@ -3122,7 +3155,7 @@
       </c>
       <c r="J7" s="6"/>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A8">
         <v>42030002</v>
       </c>
@@ -3150,8 +3183,8 @@
       <c r="J8" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="P8">
-        <v>22036101</v>
+      <c r="R8">
+        <v>43000101</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add some npc to scenequest
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/SceneQuest.xlsx
+++ b/ConfigData/Xlsx/SceneQuest.xlsx
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="178">
   <si>
     <t>int</t>
     <phoneticPr fontId="18" type="noConversion"/>
@@ -656,6 +656,49 @@
   <si>
     <t>Flag</t>
     <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>奥莱伊李</t>
+  </si>
+  <si>
+    <t>npcaolai</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>npckedi</t>
+  </si>
+  <si>
+    <t>科迪</t>
+  </si>
+  <si>
+    <t>威阿伊丁</t>
+  </si>
+  <si>
+    <t>npcweia</t>
+  </si>
+  <si>
+    <t>米兰达</t>
+  </si>
+  <si>
+    <t>贝露凯伊鲁</t>
+  </si>
+  <si>
+    <t>雷洛比克</t>
+  </si>
+  <si>
+    <t>巴鲁迪亚斯</t>
+  </si>
+  <si>
+    <t>npcmilanda</t>
+  </si>
+  <si>
+    <t>npcleiluo</t>
+  </si>
+  <si>
+    <t>npcbaludi</t>
+  </si>
+  <si>
+    <t>npcbeilukai</t>
   </si>
 </sst>
 </file>
@@ -1515,8 +1558,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="表3_5" displayName="表3_5" ref="A3:AB10" totalsRowShown="0" headerRowDxfId="1">
-  <autoFilter ref="A3:AB10"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="表3_5" displayName="表3_5" ref="A3:AB17" totalsRowShown="0" headerRowDxfId="1">
+  <autoFilter ref="A3:AB17"/>
   <sortState ref="A4:X6">
     <sortCondition ref="A3:A6"/>
   </sortState>
@@ -3002,10 +3045,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AB10"/>
+  <dimension ref="A1:AB17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S9" sqref="S9"/>
+      <selection activeCell="F15" sqref="F15:H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -3500,6 +3543,195 @@
         <v>162</v>
       </c>
     </row>
+    <row r="11" spans="1:28" x14ac:dyDescent="0.15">
+      <c r="A11">
+        <v>42030005</v>
+      </c>
+      <c r="B11" t="s">
+        <v>164</v>
+      </c>
+      <c r="C11" s="14">
+        <v>2</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="F11" t="s">
+        <v>165</v>
+      </c>
+      <c r="G11" t="s">
+        <v>165</v>
+      </c>
+      <c r="H11" t="s">
+        <v>165</v>
+      </c>
+      <c r="I11" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="K11" s="16"/>
+    </row>
+    <row r="12" spans="1:28" x14ac:dyDescent="0.15">
+      <c r="A12">
+        <v>42030006</v>
+      </c>
+      <c r="B12" t="s">
+        <v>167</v>
+      </c>
+      <c r="C12" s="14">
+        <v>2</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="F12" t="s">
+        <v>166</v>
+      </c>
+      <c r="G12" t="s">
+        <v>166</v>
+      </c>
+      <c r="H12" t="s">
+        <v>166</v>
+      </c>
+      <c r="I12" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="K12" s="16"/>
+    </row>
+    <row r="13" spans="1:28" x14ac:dyDescent="0.15">
+      <c r="A13">
+        <v>42030007</v>
+      </c>
+      <c r="B13" t="s">
+        <v>168</v>
+      </c>
+      <c r="C13" s="14">
+        <v>2</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="F13" t="s">
+        <v>169</v>
+      </c>
+      <c r="G13" t="s">
+        <v>169</v>
+      </c>
+      <c r="H13" t="s">
+        <v>169</v>
+      </c>
+      <c r="I13" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="K13" s="16"/>
+    </row>
+    <row r="14" spans="1:28" x14ac:dyDescent="0.15">
+      <c r="A14">
+        <v>42030008</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>170</v>
+      </c>
+      <c r="C14" s="14">
+        <v>2</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="F14" t="s">
+        <v>174</v>
+      </c>
+      <c r="G14" t="s">
+        <v>174</v>
+      </c>
+      <c r="H14" t="s">
+        <v>174</v>
+      </c>
+      <c r="I14" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="K14" s="16"/>
+    </row>
+    <row r="15" spans="1:28" x14ac:dyDescent="0.15">
+      <c r="A15">
+        <v>42030009</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>171</v>
+      </c>
+      <c r="C15" s="14">
+        <v>2</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="F15" t="s">
+        <v>177</v>
+      </c>
+      <c r="G15" t="s">
+        <v>177</v>
+      </c>
+      <c r="H15" t="s">
+        <v>177</v>
+      </c>
+      <c r="I15" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="K15" s="16"/>
+    </row>
+    <row r="16" spans="1:28" x14ac:dyDescent="0.15">
+      <c r="A16">
+        <v>42030010</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>172</v>
+      </c>
+      <c r="C16" s="14">
+        <v>2</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="F16" t="s">
+        <v>175</v>
+      </c>
+      <c r="G16" t="s">
+        <v>175</v>
+      </c>
+      <c r="H16" t="s">
+        <v>175</v>
+      </c>
+      <c r="I16" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="K16" s="16"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A17">
+        <v>42030011</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="C17" s="14">
+        <v>2</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+      <c r="F17" t="s">
+        <v>176</v>
+      </c>
+      <c r="G17" t="s">
+        <v>176</v>
+      </c>
+      <c r="H17" t="s">
+        <v>176</v>
+      </c>
+      <c r="I17" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="K17" s="16"/>
+    </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
remove the task related code. add the replace quest function
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/SceneQuest.xlsx
+++ b/ConfigData/Xlsx/SceneQuest.xlsx
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="183">
   <si>
     <t>int</t>
     <phoneticPr fontId="18" type="noConversion"/>
@@ -706,6 +706,18 @@
   </si>
   <si>
     <t>Aolai</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>替换</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>int</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>ReplaceId</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -1526,12 +1538,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="表3" displayName="表3" ref="A3:AB29" totalsRowShown="0" headerRowDxfId="2">
-  <autoFilter ref="A3:AB29"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="表3" displayName="表3" ref="A3:AC29" totalsRowShown="0" headerRowDxfId="2">
+  <autoFilter ref="A3:AC29"/>
   <sortState ref="A4:AA28">
     <sortCondition ref="A3:A28"/>
   </sortState>
-  <tableColumns count="28">
+  <tableColumns count="29">
     <tableColumn id="1" name="Id"/>
     <tableColumn id="2" name="Name"/>
     <tableColumn id="28" name="Type"/>
@@ -1552,6 +1564,7 @@
     <tableColumn id="15" name="RewardDrop"/>
     <tableColumn id="26" name="RivalId"/>
     <tableColumn id="27" name="Flag"/>
+    <tableColumn id="29" name="ReplaceId"/>
     <tableColumn id="16" name="PunishGold"/>
     <tableColumn id="17" name="PunishFood"/>
     <tableColumn id="18" name="PunishHealth"/>
@@ -1566,12 +1579,12 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="表3_5" displayName="表3_5" ref="A3:AB17" totalsRowShown="0" headerRowDxfId="1">
-  <autoFilter ref="A3:AB17"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="表3_5" displayName="表3_5" ref="A3:AC17" totalsRowShown="0" headerRowDxfId="1">
+  <autoFilter ref="A3:AC17"/>
   <sortState ref="A4:X6">
     <sortCondition ref="A3:A6"/>
   </sortState>
-  <tableColumns count="28">
+  <tableColumns count="29">
     <tableColumn id="1" name="Id"/>
     <tableColumn id="2" name="Name"/>
     <tableColumn id="27" name="Type" dataDxfId="0"/>
@@ -1592,6 +1605,7 @@
     <tableColumn id="15" name="RewardDrop"/>
     <tableColumn id="26" name="RivalId"/>
     <tableColumn id="28" name="Flag"/>
+    <tableColumn id="29" name="ReplaceId"/>
     <tableColumn id="16" name="PunishGold"/>
     <tableColumn id="17" name="PunishFood"/>
     <tableColumn id="18" name="PunishHealth"/>
@@ -1892,27 +1906,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AB29"/>
+  <dimension ref="A1:AC29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="T3" sqref="T3"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.875" customWidth="1"/>
-    <col min="4" max="5" width="5.875" customWidth="1"/>
+    <col min="3" max="5" width="2.75" customWidth="1"/>
     <col min="6" max="6" width="8.75" customWidth="1"/>
     <col min="9" max="9" width="5.375" customWidth="1"/>
     <col min="10" max="10" width="9.75" customWidth="1"/>
     <col min="11" max="11" width="9.375" customWidth="1"/>
     <col min="12" max="16" width="4.875" customWidth="1"/>
-    <col min="17" max="20" width="9.375" customWidth="1"/>
-    <col min="21" max="28" width="4.625" customWidth="1"/>
+    <col min="17" max="19" width="9.375" customWidth="1"/>
+    <col min="20" max="21" width="4.25" customWidth="1"/>
+    <col min="22" max="29" width="4.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="2" t="s">
         <v>82</v>
       </c>
@@ -1973,32 +1987,35 @@
       <c r="T1" s="10" t="s">
         <v>160</v>
       </c>
-      <c r="U1" s="5" t="s">
+      <c r="U1" s="10" t="s">
+        <v>180</v>
+      </c>
+      <c r="V1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="V1" s="5" t="s">
+      <c r="W1" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="W1" s="5" t="s">
+      <c r="X1" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="X1" s="5" t="s">
+      <c r="Y1" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="Y1" s="13" t="s">
+      <c r="Z1" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="Z1" s="13" t="s">
+      <c r="AA1" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="AA1" s="13" t="s">
+      <c r="AB1" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="AB1" s="13" t="s">
+      <c r="AC1" s="13" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>62</v>
       </c>
@@ -2059,8 +2076,8 @@
       <c r="T2" s="9" t="s">
         <v>161</v>
       </c>
-      <c r="U2" s="4" t="s">
-        <v>0</v>
+      <c r="U2" s="9" t="s">
+        <v>181</v>
       </c>
       <c r="V2" s="4" t="s">
         <v>0</v>
@@ -2069,10 +2086,10 @@
         <v>0</v>
       </c>
       <c r="X2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="Y2" s="4" t="s">
         <v>62</v>
-      </c>
-      <c r="Y2" s="12" t="s">
-        <v>28</v>
       </c>
       <c r="Z2" s="12" t="s">
         <v>28</v>
@@ -2083,8 +2100,11 @@
       <c r="AB2" s="12" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.15">
+      <c r="AC2" s="12" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A3" s="11" t="s">
         <v>67</v>
       </c>
@@ -2145,32 +2165,35 @@
       <c r="T3" s="8" t="s">
         <v>163</v>
       </c>
-      <c r="U3" s="3" t="s">
+      <c r="U3" s="8" t="s">
+        <v>182</v>
+      </c>
+      <c r="V3" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="V3" s="3" t="s">
+      <c r="W3" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="W3" s="3" t="s">
+      <c r="X3" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="X3" s="3" t="s">
+      <c r="Y3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="Y3" s="11" t="s">
+      <c r="Z3" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="Z3" s="11" t="s">
+      <c r="AA3" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="AA3" s="11" t="s">
+      <c r="AB3" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="AB3" s="11" t="s">
+      <c r="AC3" s="11" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A4">
         <v>42000001</v>
       </c>
@@ -2216,9 +2239,6 @@
       <c r="Q4">
         <v>22011180</v>
       </c>
-      <c r="U4">
-        <v>100</v>
-      </c>
       <c r="V4">
         <v>100</v>
       </c>
@@ -2228,8 +2248,11 @@
       <c r="X4">
         <v>100</v>
       </c>
-    </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.15">
+      <c r="Y4">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A5" s="14">
         <v>42000002</v>
       </c>
@@ -2252,7 +2275,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A6" s="14">
         <v>42000003</v>
       </c>
@@ -2275,7 +2298,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A7" s="14">
         <v>42000004</v>
       </c>
@@ -2298,7 +2321,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A8" s="14">
         <v>42000005</v>
       </c>
@@ -2320,14 +2343,14 @@
       <c r="H8" t="s">
         <v>32</v>
       </c>
-      <c r="Y8">
+      <c r="Z8">
         <v>-100</v>
       </c>
-      <c r="AA8">
+      <c r="AB8">
         <v>100</v>
       </c>
     </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A9" s="14">
         <v>42000006</v>
       </c>
@@ -2349,14 +2372,14 @@
       <c r="H9" t="s">
         <v>32</v>
       </c>
-      <c r="Y9">
+      <c r="Z9">
         <v>-100</v>
       </c>
-      <c r="AB9">
+      <c r="AC9">
         <v>100</v>
       </c>
     </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A10" s="14">
         <v>42000007</v>
       </c>
@@ -2378,14 +2401,14 @@
       <c r="H10" t="s">
         <v>32</v>
       </c>
-      <c r="Y10">
+      <c r="Z10">
         <v>-100</v>
       </c>
-      <c r="Z10">
+      <c r="AA10">
         <v>100</v>
       </c>
     </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A11">
         <v>42010001</v>
       </c>
@@ -2408,7 +2431,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A12">
         <v>42010002</v>
       </c>
@@ -2434,7 +2457,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A13">
         <v>42010003</v>
       </c>
@@ -2471,11 +2494,11 @@
       <c r="M13">
         <v>100</v>
       </c>
-      <c r="W13">
+      <c r="X13">
         <v>70</v>
       </c>
     </row>
-    <row r="14" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A14">
         <v>42010004</v>
       </c>
@@ -2503,14 +2526,14 @@
       <c r="P14">
         <v>30</v>
       </c>
-      <c r="U14">
-        <v>30</v>
-      </c>
       <c r="V14">
         <v>30</v>
       </c>
-    </row>
-    <row r="15" spans="1:28" x14ac:dyDescent="0.15">
+      <c r="W14">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A15">
         <v>42010005</v>
       </c>
@@ -2539,7 +2562,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="16" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A16">
         <v>42010006</v>
       </c>
@@ -2576,11 +2599,11 @@
       <c r="P16">
         <v>50</v>
       </c>
-      <c r="W16">
+      <c r="X16">
         <v>100</v>
       </c>
     </row>
-    <row r="17" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A17">
         <v>42010007</v>
       </c>
@@ -2608,14 +2631,14 @@
       <c r="L17">
         <v>250</v>
       </c>
-      <c r="U17">
+      <c r="V17">
         <v>250</v>
       </c>
-      <c r="X17">
+      <c r="Y17">
         <v>50</v>
       </c>
     </row>
-    <row r="18" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A18">
         <v>42010008</v>
       </c>
@@ -2644,7 +2667,7 @@
         <v>23000001</v>
       </c>
     </row>
-    <row r="19" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A19">
         <v>42010009</v>
       </c>
@@ -2670,7 +2693,7 @@
         <v>23000002</v>
       </c>
     </row>
-    <row r="20" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A20">
         <v>42010010</v>
       </c>
@@ -2695,11 +2718,11 @@
       <c r="R20">
         <v>23000003</v>
       </c>
-      <c r="W20">
+      <c r="X20">
         <v>50</v>
       </c>
     </row>
-    <row r="21" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A21">
         <v>42010011</v>
       </c>
@@ -2728,7 +2751,7 @@
         <v>23000004</v>
       </c>
     </row>
-    <row r="22" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A22">
         <v>42010013</v>
       </c>
@@ -2765,11 +2788,11 @@
       <c r="M22">
         <v>150</v>
       </c>
-      <c r="W22">
+      <c r="X22">
         <v>100</v>
       </c>
     </row>
-    <row r="23" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A23">
         <v>42010014</v>
       </c>
@@ -2809,14 +2832,14 @@
       <c r="R23">
         <v>23000101</v>
       </c>
-      <c r="W23">
-        <v>100</v>
-      </c>
       <c r="X23">
         <v>100</v>
       </c>
-    </row>
-    <row r="24" spans="1:24" x14ac:dyDescent="0.15">
+      <c r="Y23">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="24" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A24">
         <v>42010015</v>
       </c>
@@ -2841,11 +2864,11 @@
       <c r="H24" t="s">
         <v>129</v>
       </c>
-      <c r="W24">
+      <c r="X24">
         <v>80</v>
       </c>
     </row>
-    <row r="25" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A25">
         <v>42010016</v>
       </c>
@@ -2871,7 +2894,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="26" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A26">
         <v>42010017</v>
       </c>
@@ -2914,11 +2937,11 @@
       <c r="R26">
         <v>23000102</v>
       </c>
-      <c r="W26">
+      <c r="X26">
         <v>100</v>
       </c>
     </row>
-    <row r="27" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A27">
         <v>42040001</v>
       </c>
@@ -2955,14 +2978,14 @@
       <c r="S27">
         <v>1</v>
       </c>
-      <c r="W27">
-        <v>200</v>
-      </c>
       <c r="X27">
         <v>200</v>
       </c>
-    </row>
-    <row r="28" spans="1:24" x14ac:dyDescent="0.15">
+      <c r="Y27">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="28" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A28">
         <v>42040002</v>
       </c>
@@ -3002,14 +3025,14 @@
       <c r="R28">
         <v>23000102</v>
       </c>
-      <c r="W28">
-        <v>150</v>
-      </c>
       <c r="X28">
         <v>150</v>
       </c>
-    </row>
-    <row r="29" spans="1:24" x14ac:dyDescent="0.15">
+      <c r="Y28">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="29" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A29">
         <v>42040003</v>
       </c>
@@ -3034,10 +3057,10 @@
       <c r="H29" t="s">
         <v>150</v>
       </c>
-      <c r="U29">
+      <c r="V29">
         <v>100</v>
       </c>
-      <c r="W29">
+      <c r="X29">
         <v>100</v>
       </c>
     </row>
@@ -3053,17 +3076,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AB17"/>
+  <dimension ref="A1:AC17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L11" sqref="L11:M11"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.5" customWidth="1"/>
-    <col min="4" max="5" width="5.5" customWidth="1"/>
+    <col min="3" max="5" width="3" customWidth="1"/>
     <col min="6" max="6" width="9.25" customWidth="1"/>
     <col min="9" max="9" width="5.5" customWidth="1"/>
     <col min="10" max="10" width="9.75" customWidth="1"/>
@@ -3071,11 +3093,11 @@
     <col min="12" max="16" width="4.125" customWidth="1"/>
     <col min="17" max="17" width="9.75" customWidth="1"/>
     <col min="18" max="18" width="7.5" customWidth="1"/>
-    <col min="19" max="20" width="9.375" customWidth="1"/>
-    <col min="21" max="28" width="5" customWidth="1"/>
+    <col min="19" max="21" width="9.375" customWidth="1"/>
+    <col min="22" max="29" width="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="2" t="s">
         <v>82</v>
       </c>
@@ -3136,32 +3158,35 @@
       <c r="T1" s="10" t="s">
         <v>160</v>
       </c>
-      <c r="U1" s="5" t="s">
+      <c r="U1" s="10" t="s">
+        <v>180</v>
+      </c>
+      <c r="V1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="V1" s="5" t="s">
+      <c r="W1" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="W1" s="5" t="s">
+      <c r="X1" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="X1" s="5" t="s">
+      <c r="Y1" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="Y1" s="13" t="s">
+      <c r="Z1" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="Z1" s="13" t="s">
+      <c r="AA1" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="AA1" s="13" t="s">
+      <c r="AB1" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="AB1" s="13" t="s">
+      <c r="AC1" s="13" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>62</v>
       </c>
@@ -3222,8 +3247,8 @@
       <c r="T2" s="9" t="s">
         <v>161</v>
       </c>
-      <c r="U2" s="4" t="s">
-        <v>0</v>
+      <c r="U2" s="9" t="s">
+        <v>181</v>
       </c>
       <c r="V2" s="4" t="s">
         <v>0</v>
@@ -3232,10 +3257,10 @@
         <v>0</v>
       </c>
       <c r="X2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="Y2" s="4" t="s">
         <v>62</v>
-      </c>
-      <c r="Y2" s="12" t="s">
-        <v>28</v>
       </c>
       <c r="Z2" s="12" t="s">
         <v>28</v>
@@ -3246,8 +3271,11 @@
       <c r="AB2" s="12" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.15">
+      <c r="AC2" s="12" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A3" s="11" t="s">
         <v>67</v>
       </c>
@@ -3308,32 +3336,35 @@
       <c r="T3" s="8" t="s">
         <v>163</v>
       </c>
-      <c r="U3" s="3" t="s">
+      <c r="U3" s="8" t="s">
+        <v>182</v>
+      </c>
+      <c r="V3" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="V3" s="3" t="s">
+      <c r="W3" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="W3" s="3" t="s">
+      <c r="X3" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="X3" s="3" t="s">
+      <c r="Y3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="Y3" s="11" t="s">
+      <c r="Z3" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="Z3" s="11" t="s">
+      <c r="AA3" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="AA3" s="11" t="s">
+      <c r="AB3" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="AB3" s="11" t="s">
+      <c r="AC3" s="11" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A4" s="14">
         <v>42020001</v>
       </c>
@@ -3359,17 +3390,17 @@
         <v>19</v>
       </c>
       <c r="K4" s="15"/>
-      <c r="Y4">
+      <c r="Z4">
         <v>-300</v>
-      </c>
-      <c r="AA4">
-        <v>1000</v>
       </c>
       <c r="AB4">
         <v>1000</v>
       </c>
-    </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.15">
+      <c r="AC4">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A5" s="14">
         <v>42020002</v>
       </c>
@@ -3395,14 +3426,14 @@
         <v>19</v>
       </c>
       <c r="K5" s="15"/>
-      <c r="Y5">
+      <c r="Z5">
         <v>-200</v>
       </c>
-      <c r="Z5">
+      <c r="AA5">
         <v>1000</v>
       </c>
     </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A6" s="14">
         <v>42020003</v>
       </c>
@@ -3429,7 +3460,7 @@
       </c>
       <c r="K6" s="15"/>
     </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A7">
         <v>42030001</v>
       </c>
@@ -3456,7 +3487,7 @@
       </c>
       <c r="K7" s="6"/>
     </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A8">
         <v>42030002</v>
       </c>
@@ -3491,7 +3522,7 @@
         <v>43020101</v>
       </c>
     </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A9">
         <v>42030003</v>
       </c>
@@ -3518,7 +3549,7 @@
       </c>
       <c r="K9" s="16"/>
     </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A10">
         <v>42030004</v>
       </c>
@@ -3551,7 +3582,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A11">
         <v>42030005</v>
       </c>
@@ -3590,7 +3621,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A12">
         <v>42030006</v>
       </c>
@@ -3617,7 +3648,7 @@
       </c>
       <c r="K12" s="16"/>
     </row>
-    <row r="13" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A13">
         <v>42030007</v>
       </c>
@@ -3644,7 +3675,7 @@
       </c>
       <c r="K13" s="16"/>
     </row>
-    <row r="14" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A14">
         <v>42030008</v>
       </c>
@@ -3671,7 +3702,7 @@
       </c>
       <c r="K14" s="16"/>
     </row>
-    <row r="15" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A15">
         <v>42030009</v>
       </c>
@@ -3698,7 +3729,7 @@
       </c>
       <c r="K15" s="16"/>
     </row>
-    <row r="16" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A16">
         <v>42030010</v>
       </c>

</xml_diff>

<commit_message>
finish the scene object replace engine
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/SceneQuest.xlsx
+++ b/ConfigData/Xlsx/SceneQuest.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385" activeTab="1"/>
+    <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="4" r:id="rId1"/>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="187">
   <si>
     <t>int</t>
     <phoneticPr fontId="18" type="noConversion"/>
@@ -718,6 +718,21 @@
   </si>
   <si>
     <t>ReplaceId</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>hiddeway</t>
+  </si>
+  <si>
+    <t>隐藏通道</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>npcaolai2</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>npcaolai2</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -1538,8 +1553,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="表3" displayName="表3" ref="A3:AC29" totalsRowShown="0" headerRowDxfId="2">
-  <autoFilter ref="A3:AC29"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="表3" displayName="表3" ref="A3:AC30" totalsRowShown="0" headerRowDxfId="2">
+  <autoFilter ref="A3:AC30"/>
   <sortState ref="A4:AA28">
     <sortCondition ref="A3:A28"/>
   </sortState>
@@ -1579,8 +1594,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="表3_5" displayName="表3_5" ref="A3:AC17" totalsRowShown="0" headerRowDxfId="1">
-  <autoFilter ref="A3:AC17"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="表3_5" displayName="表3_5" ref="A3:AC18" totalsRowShown="0" headerRowDxfId="1">
+  <autoFilter ref="A3:AC18"/>
   <sortState ref="A4:X6">
     <sortCondition ref="A3:A6"/>
   </sortState>
@@ -1906,10 +1921,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AC29"/>
+  <dimension ref="A1:AC30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="U4" sqref="U4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -2943,54 +2958,33 @@
     </row>
     <row r="27" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A27">
-        <v>42040001</v>
+        <v>42010018</v>
       </c>
       <c r="B27" t="s">
-        <v>144</v>
+        <v>184</v>
       </c>
       <c r="C27">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D27">
         <v>0</v>
       </c>
-      <c r="E27">
-        <v>1</v>
-      </c>
       <c r="F27" t="s">
-        <v>145</v>
+        <v>183</v>
       </c>
       <c r="G27" t="s">
-        <v>145</v>
+        <v>183</v>
       </c>
       <c r="H27" t="s">
-        <v>145</v>
-      </c>
-      <c r="J27">
-        <v>1</v>
-      </c>
-      <c r="K27" t="s">
-        <v>17</v>
-      </c>
-      <c r="P27">
-        <v>100</v>
-      </c>
-      <c r="S27">
-        <v>1</v>
-      </c>
-      <c r="X27">
-        <v>200</v>
-      </c>
-      <c r="Y27">
-        <v>200</v>
+        <v>183</v>
       </c>
     </row>
     <row r="28" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A28">
-        <v>42040002</v>
+        <v>42040001</v>
       </c>
       <c r="B28" t="s">
-        <v>119</v>
+        <v>144</v>
       </c>
       <c r="C28">
         <v>3</v>
@@ -2999,45 +2993,42 @@
         <v>0</v>
       </c>
       <c r="E28">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F28" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="G28" t="s">
-        <v>118</v>
+        <v>145</v>
       </c>
       <c r="H28" t="s">
-        <v>118</v>
+        <v>145</v>
       </c>
       <c r="J28">
-        <v>43000005</v>
+        <v>1</v>
       </c>
       <c r="K28" t="s">
         <v>17</v>
       </c>
-      <c r="L28">
+      <c r="P28">
+        <v>100</v>
+      </c>
+      <c r="S28">
+        <v>1</v>
+      </c>
+      <c r="X28">
         <v>200</v>
       </c>
-      <c r="M28">
-        <v>50</v>
-      </c>
-      <c r="R28">
-        <v>23000102</v>
-      </c>
-      <c r="X28">
-        <v>150</v>
-      </c>
       <c r="Y28">
-        <v>150</v>
+        <v>200</v>
       </c>
     </row>
     <row r="29" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A29">
-        <v>42040003</v>
+        <v>42040002</v>
       </c>
       <c r="B29" t="s">
-        <v>151</v>
+        <v>119</v>
       </c>
       <c r="C29">
         <v>3</v>
@@ -3046,40 +3037,88 @@
         <v>0</v>
       </c>
       <c r="E29">
+        <v>2</v>
+      </c>
+      <c r="F29" t="s">
+        <v>149</v>
+      </c>
+      <c r="G29" t="s">
+        <v>118</v>
+      </c>
+      <c r="H29" t="s">
+        <v>118</v>
+      </c>
+      <c r="J29">
+        <v>43000005</v>
+      </c>
+      <c r="K29" t="s">
+        <v>17</v>
+      </c>
+      <c r="L29">
+        <v>200</v>
+      </c>
+      <c r="M29">
+        <v>50</v>
+      </c>
+      <c r="R29">
+        <v>23000102</v>
+      </c>
+      <c r="X29">
+        <v>150</v>
+      </c>
+      <c r="Y29">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="30" spans="1:25" x14ac:dyDescent="0.15">
+      <c r="A30">
+        <v>42040003</v>
+      </c>
+      <c r="B30" t="s">
+        <v>151</v>
+      </c>
+      <c r="C30">
         <v>3</v>
       </c>
-      <c r="F29" t="s">
+      <c r="D30">
+        <v>0</v>
+      </c>
+      <c r="E30">
+        <v>3</v>
+      </c>
+      <c r="F30" t="s">
         <v>152</v>
       </c>
-      <c r="G29" t="s">
+      <c r="G30" t="s">
         <v>150</v>
       </c>
-      <c r="H29" t="s">
+      <c r="H30" t="s">
         <v>150</v>
       </c>
-      <c r="V29">
+      <c r="V30">
         <v>100</v>
       </c>
-      <c r="X29">
+      <c r="X30">
         <v>100</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AC17"/>
+  <dimension ref="A1:AC18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="U11" sqref="U11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -3620,6 +3659,9 @@
       <c r="T11" t="s">
         <v>179</v>
       </c>
+      <c r="U11">
+        <v>42030012</v>
+      </c>
     </row>
     <row r="12" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A12">
@@ -3756,7 +3798,7 @@
       </c>
       <c r="K16" s="16"/>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A17">
         <v>42030011</v>
       </c>
@@ -3782,6 +3824,41 @@
         <v>19</v>
       </c>
       <c r="K17" s="16"/>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.15">
+      <c r="A18">
+        <v>42030012</v>
+      </c>
+      <c r="B18" t="s">
+        <v>164</v>
+      </c>
+      <c r="C18" s="14">
+        <v>2</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+      <c r="F18" t="s">
+        <v>186</v>
+      </c>
+      <c r="G18" t="s">
+        <v>165</v>
+      </c>
+      <c r="H18" t="s">
+        <v>185</v>
+      </c>
+      <c r="I18" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="J18">
+        <v>43020105</v>
+      </c>
+      <c r="K18" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="S18">
+        <v>43020105</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>

</xml_diff>

<commit_message>
close #99 finish the npc bless function of academy
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/SceneQuest.xlsx
+++ b/ConfigData/Xlsx/SceneQuest.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385"/>
+    <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="4" r:id="rId1"/>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="410" uniqueCount="208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="211">
   <si>
     <t>int</t>
     <phoneticPr fontId="18" type="noConversion"/>
@@ -814,6 +814,17 @@
   </si>
   <si>
     <t>女巫小屋</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>academy</t>
+  </si>
+  <si>
+    <t>学院</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>academy</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -1597,7 +1608,12 @@
   </cellStyles>
   <dxfs count="4">
     <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <fill>
@@ -1608,12 +1624,7 @@
       </fill>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
+      <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
     <dxf>
       <fill>
@@ -1637,7 +1648,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="表3" displayName="表3" ref="A3:AE35" totalsRowShown="0" headerRowDxfId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="表3" displayName="表3" ref="A3:AE35" totalsRowShown="0" headerRowDxfId="3">
   <autoFilter ref="A3:AE35"/>
   <sortState ref="A4:AC28">
     <sortCondition ref="A3:A28"/>
@@ -1651,7 +1662,7 @@
     <tableColumn id="24" name="Ename"/>
     <tableColumn id="4" name="Figue"/>
     <tableColumn id="5" name="Script"/>
-    <tableColumn id="6" name="TriggerMulti" dataDxfId="0"/>
+    <tableColumn id="6" name="TriggerMulti" dataDxfId="2"/>
     <tableColumn id="7" name="EnemyId"/>
     <tableColumn id="8" name="BattleMap"/>
     <tableColumn id="9" name="RewardGold"/>
@@ -1680,15 +1691,15 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="表3_5" displayName="表3_5" ref="A3:AE19" totalsRowShown="0" headerRowDxfId="3">
-  <autoFilter ref="A3:AE19"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="表3_5" displayName="表3_5" ref="A3:AE20" totalsRowShown="0" headerRowDxfId="1">
+  <autoFilter ref="A3:AE20"/>
   <sortState ref="A4:Y6">
     <sortCondition ref="A3:A6"/>
   </sortState>
   <tableColumns count="31">
     <tableColumn id="1" name="Id"/>
     <tableColumn id="2" name="Name"/>
-    <tableColumn id="27" name="Type" dataDxfId="2"/>
+    <tableColumn id="27" name="Type" dataDxfId="0"/>
     <tableColumn id="3" name="Level"/>
     <tableColumn id="25" name="Danger"/>
     <tableColumn id="24" name="Ename"/>
@@ -2045,7 +2056,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="AA35" sqref="AA35"/>
     </sheetView>
@@ -3460,11 +3471,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AE19"/>
+  <dimension ref="A1:AE20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AA2" sqref="AA2"/>
+      <selection pane="bottomLeft" activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -3891,11 +3902,11 @@
       </c>
     </row>
     <row r="8" spans="1:31" x14ac:dyDescent="0.15">
-      <c r="A8">
-        <v>42030001</v>
-      </c>
-      <c r="B8" t="s">
-        <v>20</v>
+      <c r="A8" s="14">
+        <v>42020005</v>
+      </c>
+      <c r="B8" s="14" t="s">
+        <v>209</v>
       </c>
       <c r="C8" s="14">
         <v>2</v>
@@ -3904,25 +3915,25 @@
         <v>0</v>
       </c>
       <c r="F8" t="s">
-        <v>19</v>
+        <v>210</v>
       </c>
       <c r="G8" t="s">
-        <v>19</v>
+        <v>208</v>
       </c>
       <c r="H8" t="s">
-        <v>19</v>
+        <v>208</v>
       </c>
       <c r="I8" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="K8" s="6"/>
+      <c r="K8" s="15"/>
     </row>
     <row r="9" spans="1:31" x14ac:dyDescent="0.15">
       <c r="A9">
-        <v>42030002</v>
+        <v>42030001</v>
       </c>
       <c r="B9" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C9" s="14">
         <v>2</v>
@@ -3931,33 +3942,25 @@
         <v>0</v>
       </c>
       <c r="F9" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="G9" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="H9" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="I9" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="J9">
-        <v>43020101</v>
-      </c>
-      <c r="K9" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="S9">
-        <v>43020101</v>
-      </c>
+      <c r="K9" s="6"/>
     </row>
     <row r="10" spans="1:31" x14ac:dyDescent="0.15">
       <c r="A10">
-        <v>42030003</v>
+        <v>42030002</v>
       </c>
       <c r="B10" t="s">
-        <v>151</v>
+        <v>22</v>
       </c>
       <c r="C10" s="14">
         <v>2</v>
@@ -3966,25 +3969,33 @@
         <v>0</v>
       </c>
       <c r="F10" t="s">
-        <v>152</v>
+        <v>21</v>
       </c>
       <c r="G10" t="s">
-        <v>150</v>
+        <v>21</v>
       </c>
       <c r="H10" t="s">
-        <v>150</v>
+        <v>21</v>
       </c>
       <c r="I10" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="K10" s="16"/>
+      <c r="J10">
+        <v>43020101</v>
+      </c>
+      <c r="K10" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="S10">
+        <v>43020101</v>
+      </c>
     </row>
     <row r="11" spans="1:31" x14ac:dyDescent="0.15">
       <c r="A11">
-        <v>42030004</v>
+        <v>42030003</v>
       </c>
       <c r="B11" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="C11" s="14">
         <v>2</v>
@@ -3993,31 +4004,25 @@
         <v>0</v>
       </c>
       <c r="F11" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G11" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="H11" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="I11" s="7" t="s">
-        <v>156</v>
+        <v>18</v>
       </c>
       <c r="K11" s="16"/>
-      <c r="S11">
-        <v>43020102</v>
-      </c>
-      <c r="T11" t="s">
-        <v>159</v>
-      </c>
     </row>
     <row r="12" spans="1:31" x14ac:dyDescent="0.15">
       <c r="A12">
-        <v>42030005</v>
+        <v>42030004</v>
       </c>
       <c r="B12" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="C12" s="14">
         <v>2</v>
@@ -4026,40 +4031,31 @@
         <v>0</v>
       </c>
       <c r="F12" t="s">
-        <v>175</v>
+        <v>153</v>
       </c>
       <c r="G12" t="s">
-        <v>162</v>
+        <v>153</v>
       </c>
       <c r="H12" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="I12" s="7" t="s">
-        <v>18</v>
+        <v>156</v>
       </c>
       <c r="K12" s="16"/>
-      <c r="L12">
-        <v>300</v>
-      </c>
-      <c r="M12">
-        <v>200</v>
-      </c>
-      <c r="Q12">
-        <v>22031011</v>
+      <c r="S12">
+        <v>43020102</v>
       </c>
       <c r="T12" t="s">
-        <v>176</v>
-      </c>
-      <c r="U12">
-        <v>42030012</v>
+        <v>159</v>
       </c>
     </row>
     <row r="13" spans="1:31" x14ac:dyDescent="0.15">
       <c r="A13">
-        <v>42030006</v>
+        <v>42030005</v>
       </c>
       <c r="B13" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="C13" s="14">
         <v>2</v>
@@ -4068,25 +4064,40 @@
         <v>0</v>
       </c>
       <c r="F13" t="s">
-        <v>163</v>
+        <v>175</v>
       </c>
       <c r="G13" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H13" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="I13" s="7" t="s">
         <v>18</v>
       </c>
       <c r="K13" s="16"/>
+      <c r="L13">
+        <v>300</v>
+      </c>
+      <c r="M13">
+        <v>200</v>
+      </c>
+      <c r="Q13">
+        <v>22031011</v>
+      </c>
+      <c r="T13" t="s">
+        <v>176</v>
+      </c>
+      <c r="U13">
+        <v>42030012</v>
+      </c>
     </row>
     <row r="14" spans="1:31" x14ac:dyDescent="0.15">
       <c r="A14">
-        <v>42030007</v>
+        <v>42030006</v>
       </c>
       <c r="B14" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C14" s="14">
         <v>2</v>
@@ -4095,13 +4106,13 @@
         <v>0</v>
       </c>
       <c r="F14" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="G14" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="H14" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="I14" s="7" t="s">
         <v>18</v>
@@ -4110,10 +4121,10 @@
     </row>
     <row r="15" spans="1:31" x14ac:dyDescent="0.15">
       <c r="A15">
-        <v>42030008</v>
-      </c>
-      <c r="B15" s="6" t="s">
-        <v>167</v>
+        <v>42030007</v>
+      </c>
+      <c r="B15" t="s">
+        <v>165</v>
       </c>
       <c r="C15" s="14">
         <v>2</v>
@@ -4122,13 +4133,13 @@
         <v>0</v>
       </c>
       <c r="F15" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="G15" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="H15" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="I15" s="7" t="s">
         <v>18</v>
@@ -4137,10 +4148,10 @@
     </row>
     <row r="16" spans="1:31" x14ac:dyDescent="0.15">
       <c r="A16">
-        <v>42030009</v>
+        <v>42030008</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C16" s="14">
         <v>2</v>
@@ -4149,13 +4160,13 @@
         <v>0</v>
       </c>
       <c r="F16" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="G16" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="H16" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="I16" s="7" t="s">
         <v>18</v>
@@ -4164,10 +4175,10 @@
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A17">
-        <v>42030010</v>
+        <v>42030009</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C17" s="14">
         <v>2</v>
@@ -4176,13 +4187,13 @@
         <v>0</v>
       </c>
       <c r="F17" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="G17" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="H17" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="I17" s="7" t="s">
         <v>18</v>
@@ -4191,10 +4202,10 @@
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A18">
-        <v>42030011</v>
+        <v>42030010</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C18" s="14">
         <v>2</v>
@@ -4203,13 +4214,13 @@
         <v>0</v>
       </c>
       <c r="F18" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="G18" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="H18" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="I18" s="7" t="s">
         <v>18</v>
@@ -4218,10 +4229,10 @@
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A19">
-        <v>42030012</v>
-      </c>
-      <c r="B19" t="s">
-        <v>161</v>
+        <v>42030011</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>170</v>
       </c>
       <c r="C19" s="14">
         <v>2</v>
@@ -4230,24 +4241,51 @@
         <v>0</v>
       </c>
       <c r="F19" t="s">
-        <v>183</v>
+        <v>173</v>
       </c>
       <c r="G19" t="s">
-        <v>162</v>
+        <v>173</v>
       </c>
       <c r="H19" t="s">
-        <v>182</v>
+        <v>173</v>
       </c>
       <c r="I19" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="J19">
+      <c r="K19" s="16"/>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.15">
+      <c r="A20">
+        <v>42030012</v>
+      </c>
+      <c r="B20" t="s">
+        <v>161</v>
+      </c>
+      <c r="C20" s="14">
+        <v>2</v>
+      </c>
+      <c r="D20">
+        <v>0</v>
+      </c>
+      <c r="F20" t="s">
+        <v>183</v>
+      </c>
+      <c r="G20" t="s">
+        <v>162</v>
+      </c>
+      <c r="H20" t="s">
+        <v>182</v>
+      </c>
+      <c r="I20" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="J20">
         <v>43020105</v>
       </c>
-      <c r="K19" s="16" t="s">
+      <c r="K20" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="S19">
+      <c r="S20">
         <v>43020105</v>
       </c>
     </row>

</xml_diff>

<commit_message>
made the forestinner map
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/SceneQuest.xlsx
+++ b/ConfigData/Xlsx/SceneQuest.xlsx
@@ -3532,7 +3532,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I17" sqref="I17"/>
+      <selection pane="bottomLeft" activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -4389,7 +4389,7 @@
         <v>215</v>
       </c>
       <c r="G21" t="s">
-        <v>162</v>
+        <v>215</v>
       </c>
       <c r="H21" t="s">
         <v>216</v>

</xml_diff>

<commit_message>
#99 finish the random maze function
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/SceneQuest.xlsx
+++ b/ConfigData/Xlsx/SceneQuest.xlsx
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="426" uniqueCount="217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="431" uniqueCount="217">
   <si>
     <t>int</t>
     <phoneticPr fontId="18" type="noConversion"/>
@@ -1738,8 +1738,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="表3_5" displayName="表3_5" ref="A3:AF21" totalsRowShown="0" headerRowDxfId="2">
-  <autoFilter ref="A3:AF21"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="表3_5" displayName="表3_5" ref="A3:AF22" totalsRowShown="0" headerRowDxfId="2">
+  <autoFilter ref="A3:AF22"/>
   <sortState ref="A4:Z6">
     <sortCondition ref="A3:A6"/>
   </sortState>
@@ -3528,11 +3528,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AF21"/>
+  <dimension ref="A1:AF22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G21" sqref="G21"/>
+      <selection pane="bottomLeft" activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -4402,6 +4402,36 @@
         <v>13020001</v>
       </c>
     </row>
+    <row r="22" spans="1:20" x14ac:dyDescent="0.15">
+      <c r="A22">
+        <v>42050002</v>
+      </c>
+      <c r="B22" t="s">
+        <v>211</v>
+      </c>
+      <c r="C22" s="14">
+        <v>2</v>
+      </c>
+      <c r="D22">
+        <v>0</v>
+      </c>
+      <c r="F22" t="s">
+        <v>215</v>
+      </c>
+      <c r="G22" t="s">
+        <v>215</v>
+      </c>
+      <c r="H22" t="s">
+        <v>216</v>
+      </c>
+      <c r="I22" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="K22" s="16"/>
+      <c r="L22" s="16">
+        <v>13020002</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
suppor reward or punish to follow another action
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/SceneQuest.xlsx
+++ b/ConfigData/Xlsx/SceneQuest.xlsx
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="431" uniqueCount="217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="431" uniqueCount="218">
   <si>
     <t>int</t>
     <phoneticPr fontId="18" type="noConversion"/>
@@ -849,6 +849,10 @@
   </si>
   <si>
     <t>dungeonentry</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>forestentry2</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -2105,8 +2109,8 @@
   <dimension ref="A1:AF35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H35" sqref="H35"/>
+      <pane ySplit="3" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -2446,6 +2450,9 @@
       <c r="K4" t="s">
         <v>16</v>
       </c>
+      <c r="L4" s="16">
+        <v>13020001</v>
+      </c>
       <c r="M4">
         <v>100</v>
       </c>
@@ -3532,7 +3539,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I22" sqref="I22"/>
+      <selection pane="bottomLeft" activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -4416,7 +4423,7 @@
         <v>0</v>
       </c>
       <c r="F22" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="G22" t="s">
         <v>215</v>

</xml_diff>

<commit_message>
dungeon boss qiongqi design #98
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/SceneQuest.xlsx
+++ b/ConfigData/Xlsx/SceneQuest.xlsx
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="431" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="221">
   <si>
     <t>int</t>
     <phoneticPr fontId="18" type="noConversion"/>
@@ -853,6 +853,18 @@
   </si>
   <si>
     <t>forestentry2</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>qiongqi</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>穷奇</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Qiongqi</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -1742,8 +1754,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="表3_5" displayName="表3_5" ref="A3:AF22" totalsRowShown="0" headerRowDxfId="2">
-  <autoFilter ref="A3:AF22"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="表3_5" displayName="表3_5" ref="A3:AF23" totalsRowShown="0" headerRowDxfId="2">
+  <autoFilter ref="A3:AF23"/>
   <sortState ref="A4:Z6">
     <sortCondition ref="A3:A6"/>
   </sortState>
@@ -3535,11 +3547,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AF22"/>
+  <dimension ref="A1:AF23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F21" sqref="F21"/>
+      <selection pane="bottomLeft" activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -4259,7 +4271,7 @@
       <c r="K16" s="16"/>
       <c r="L16" s="16"/>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A17">
         <v>42030009</v>
       </c>
@@ -4287,7 +4299,7 @@
       <c r="K17" s="16"/>
       <c r="L17" s="16"/>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A18">
         <v>42030010</v>
       </c>
@@ -4315,7 +4327,7 @@
       <c r="K18" s="16"/>
       <c r="L18" s="16"/>
     </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A19">
         <v>42030011</v>
       </c>
@@ -4343,7 +4355,7 @@
       <c r="K19" s="16"/>
       <c r="L19" s="16"/>
     </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A20">
         <v>42030012</v>
       </c>
@@ -4379,7 +4391,7 @@
         <v>43020105</v>
       </c>
     </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A21">
         <v>42050001</v>
       </c>
@@ -4409,7 +4421,7 @@
         <v>13020001</v>
       </c>
     </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A22">
         <v>42050002</v>
       </c>
@@ -4437,6 +4449,68 @@
       <c r="K22" s="16"/>
       <c r="L22" s="16">
         <v>13020002</v>
+      </c>
+    </row>
+    <row r="23" spans="1:27" x14ac:dyDescent="0.15">
+      <c r="A23">
+        <v>42050003</v>
+      </c>
+      <c r="B23" t="s">
+        <v>219</v>
+      </c>
+      <c r="C23" s="14">
+        <v>2</v>
+      </c>
+      <c r="D23">
+        <v>0</v>
+      </c>
+      <c r="E23">
+        <v>3</v>
+      </c>
+      <c r="F23" t="s">
+        <v>218</v>
+      </c>
+      <c r="G23" t="s">
+        <v>218</v>
+      </c>
+      <c r="H23" t="s">
+        <v>218</v>
+      </c>
+      <c r="I23" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="J23">
+        <v>43000019</v>
+      </c>
+      <c r="K23" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="L23" s="16">
+        <v>13000002</v>
+      </c>
+      <c r="M23">
+        <v>300</v>
+      </c>
+      <c r="N23">
+        <v>500</v>
+      </c>
+      <c r="O23">
+        <v>500</v>
+      </c>
+      <c r="P23">
+        <v>500</v>
+      </c>
+      <c r="Q23">
+        <v>300</v>
+      </c>
+      <c r="U23" t="s">
+        <v>220</v>
+      </c>
+      <c r="Z23">
+        <v>200</v>
+      </c>
+      <c r="AA23">
+        <v>200</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
#100 chenk and set quest on scenequest
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/SceneQuest.xlsx
+++ b/ConfigData/Xlsx/SceneQuest.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\TOMClassicGit\ConfigData\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\TOMClassicGit\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView minimized="1" xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385"/>
+    <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="4" r:id="rId1"/>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="453" uniqueCount="230">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="459" uniqueCount="233">
   <si>
     <t>int</t>
     <phoneticPr fontId="18" type="noConversion"/>
@@ -900,6 +900,18 @@
   </si>
   <si>
     <t>高级素材袋</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>任务</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>int</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>QuestId</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -1731,74 +1743,6 @@
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1811,12 +1755,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="表3" displayName="表3" ref="A3:AF38" totalsRowShown="0" headerRowDxfId="4">
-  <autoFilter ref="A3:AF38"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="表3" displayName="表3" ref="A3:AG38" totalsRowShown="0" headerRowDxfId="4">
+  <autoFilter ref="A3:AG38"/>
   <sortState ref="A4:AD28">
     <sortCondition ref="A3:A28"/>
   </sortState>
-  <tableColumns count="32">
+  <tableColumns count="33">
     <tableColumn id="1" name="Id"/>
     <tableColumn id="2" name="Name"/>
     <tableColumn id="28" name="Type"/>
@@ -1836,10 +1780,11 @@
     <tableColumn id="13" name="RewardExp"/>
     <tableColumn id="14" name="RewardItem"/>
     <tableColumn id="15" name="RewardDrop"/>
+    <tableColumn id="30" name="RewardBlessLevel"/>
     <tableColumn id="26" name="RivalId"/>
+    <tableColumn id="33" name="QuestId"/>
     <tableColumn id="27" name="Flag"/>
     <tableColumn id="29" name="ReplaceId"/>
-    <tableColumn id="30" name="RewardBlessLevel"/>
     <tableColumn id="16" name="PunishGold"/>
     <tableColumn id="17" name="PunishFood"/>
     <tableColumn id="18" name="PunishHealth"/>
@@ -1855,12 +1800,12 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="表3_5" displayName="表3_5" ref="A3:AF23" totalsRowShown="0" headerRowDxfId="2">
-  <autoFilter ref="A3:AF23"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="表3_5" displayName="表3_5" ref="A3:AG23" totalsRowShown="0" headerRowDxfId="2">
+  <autoFilter ref="A3:AG23"/>
   <sortState ref="A4:Z6">
     <sortCondition ref="A3:A6"/>
   </sortState>
-  <tableColumns count="32">
+  <tableColumns count="33">
     <tableColumn id="1" name="Id"/>
     <tableColumn id="2" name="Name"/>
     <tableColumn id="27" name="Type" dataDxfId="1"/>
@@ -1880,10 +1825,11 @@
     <tableColumn id="13" name="RewardExp"/>
     <tableColumn id="14" name="RewardItem"/>
     <tableColumn id="15" name="RewardDrop"/>
+    <tableColumn id="31" name="RewardBlessLevel"/>
     <tableColumn id="26" name="RivalId"/>
+    <tableColumn id="33" name="QuestId"/>
     <tableColumn id="28" name="Flag"/>
     <tableColumn id="29" name="ReplaceId"/>
-    <tableColumn id="31" name="RewardBlessLevel"/>
     <tableColumn id="16" name="PunishGold"/>
     <tableColumn id="17" name="PunishFood"/>
     <tableColumn id="18" name="PunishHealth"/>
@@ -1906,7 +1852,7 @@
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="CAEACD"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -2185,11 +2131,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AF38"/>
+  <dimension ref="A1:AG38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I10" sqref="I10"/>
+      <selection pane="bottomLeft" activeCell="O4" sqref="O4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -2201,12 +2147,14 @@
     <col min="10" max="10" width="9.75" customWidth="1"/>
     <col min="11" max="12" width="9.375" customWidth="1"/>
     <col min="13" max="17" width="4.875" customWidth="1"/>
-    <col min="18" max="20" width="9.375" customWidth="1"/>
-    <col min="21" max="23" width="4.25" customWidth="1"/>
-    <col min="24" max="32" width="4.75" customWidth="1"/>
+    <col min="18" max="19" width="9.375" customWidth="1"/>
+    <col min="20" max="20" width="4.25" customWidth="1"/>
+    <col min="21" max="22" width="9.375" customWidth="1"/>
+    <col min="23" max="24" width="4.25" customWidth="1"/>
+    <col min="26" max="34" width="4.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" ht="69" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:33" ht="69" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="14" t="s">
         <v>79</v>
       </c>
@@ -2265,46 +2213,49 @@
         <v>77</v>
       </c>
       <c r="T1" s="15" t="s">
+        <v>200</v>
+      </c>
+      <c r="U1" s="15" t="s">
         <v>137</v>
       </c>
-      <c r="U1" s="15" t="s">
+      <c r="V1" s="15" t="s">
+        <v>230</v>
+      </c>
+      <c r="W1" s="15" t="s">
         <v>156</v>
       </c>
-      <c r="V1" s="15" t="s">
+      <c r="X1" s="15" t="s">
         <v>176</v>
       </c>
-      <c r="W1" s="15" t="s">
-        <v>200</v>
-      </c>
-      <c r="X1" s="16" t="s">
+      <c r="Y1" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="Y1" s="16" t="s">
+      <c r="Z1" s="16" t="s">
         <v>88</v>
       </c>
-      <c r="Z1" s="16" t="s">
+      <c r="AA1" s="16" t="s">
         <v>78</v>
       </c>
-      <c r="AA1" s="16" t="s">
+      <c r="AB1" s="16" t="s">
         <v>89</v>
       </c>
-      <c r="AB1" s="16" t="s">
+      <c r="AC1" s="16" t="s">
         <v>201</v>
       </c>
-      <c r="AC1" s="17" t="s">
+      <c r="AD1" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" s="17" t="s">
+      <c r="AE1" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" s="17" t="s">
+      <c r="AF1" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="AF1" s="17" t="s">
+      <c r="AG1" s="17" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:32" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:33" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>59</v>
       </c>
@@ -2363,20 +2314,20 @@
         <v>59</v>
       </c>
       <c r="T2" s="7" t="s">
+        <v>199</v>
+      </c>
+      <c r="U2" s="7" t="s">
         <v>138</v>
       </c>
-      <c r="U2" s="7" t="s">
+      <c r="V2" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="W2" s="7" t="s">
         <v>157</v>
       </c>
-      <c r="V2" s="7" t="s">
+      <c r="X2" s="7" t="s">
         <v>177</v>
       </c>
-      <c r="W2" s="7" t="s">
-        <v>199</v>
-      </c>
-      <c r="X2" s="3" t="s">
-        <v>0</v>
-      </c>
       <c r="Y2" s="3" t="s">
         <v>0</v>
       </c>
@@ -2384,13 +2335,13 @@
         <v>0</v>
       </c>
       <c r="AA2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="AB2" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="AB2" s="3" t="s">
+      <c r="AC2" s="3" t="s">
         <v>202</v>
-      </c>
-      <c r="AC2" s="9" t="s">
-        <v>27</v>
       </c>
       <c r="AD2" s="9" t="s">
         <v>27</v>
@@ -2401,8 +2352,11 @@
       <c r="AF2" s="9" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="3" spans="1:32" x14ac:dyDescent="0.15">
+      <c r="AG2" s="9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:33" x14ac:dyDescent="0.15">
       <c r="A3" s="8" t="s">
         <v>64</v>
       </c>
@@ -2461,46 +2415,49 @@
         <v>35</v>
       </c>
       <c r="T3" s="6" t="s">
+        <v>198</v>
+      </c>
+      <c r="U3" s="6" t="s">
         <v>139</v>
       </c>
-      <c r="U3" s="6" t="s">
+      <c r="V3" s="6" t="s">
+        <v>232</v>
+      </c>
+      <c r="W3" s="6" t="s">
         <v>159</v>
       </c>
-      <c r="V3" s="6" t="s">
+      <c r="X3" s="6" t="s">
         <v>178</v>
       </c>
-      <c r="W3" s="6" t="s">
-        <v>198</v>
-      </c>
-      <c r="X3" s="2" t="s">
+      <c r="Y3" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="Y3" s="2" t="s">
+      <c r="Z3" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="Z3" s="2" t="s">
+      <c r="AA3" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="AA3" s="2" t="s">
+      <c r="AB3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="AB3" s="2" t="s">
+      <c r="AC3" s="2" t="s">
         <v>203</v>
       </c>
-      <c r="AC3" s="8" t="s">
+      <c r="AD3" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="AD3" s="8" t="s">
+      <c r="AE3" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="AE3" s="8" t="s">
+      <c r="AF3" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="AF3" s="8" t="s">
+      <c r="AG3" s="8" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:32" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:33" x14ac:dyDescent="0.15">
       <c r="A4">
         <v>42000001</v>
       </c>
@@ -2550,9 +2507,6 @@
       <c r="R4">
         <v>22011180</v>
       </c>
-      <c r="X4">
-        <v>100</v>
-      </c>
       <c r="Y4">
         <v>100</v>
       </c>
@@ -2562,8 +2516,11 @@
       <c r="AA4">
         <v>100</v>
       </c>
-    </row>
-    <row r="5" spans="1:32" x14ac:dyDescent="0.15">
+      <c r="AB4">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" spans="1:33" x14ac:dyDescent="0.15">
       <c r="A5" s="10">
         <v>42000002</v>
       </c>
@@ -2587,7 +2544,7 @@
       </c>
       <c r="I5" s="5"/>
     </row>
-    <row r="6" spans="1:32" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:33" x14ac:dyDescent="0.15">
       <c r="A6" s="10">
         <v>42000003</v>
       </c>
@@ -2611,7 +2568,7 @@
       </c>
       <c r="I6" s="5"/>
     </row>
-    <row r="7" spans="1:32" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:33" x14ac:dyDescent="0.15">
       <c r="A7" s="10">
         <v>42000004</v>
       </c>
@@ -2635,7 +2592,7 @@
       </c>
       <c r="I7" s="5"/>
     </row>
-    <row r="8" spans="1:32" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:33" x14ac:dyDescent="0.15">
       <c r="A8" s="10">
         <v>42000005</v>
       </c>
@@ -2658,14 +2615,14 @@
         <v>31</v>
       </c>
       <c r="I8" s="5"/>
-      <c r="AC8">
+      <c r="AD8">
         <v>-100</v>
       </c>
-      <c r="AE8">
+      <c r="AF8">
         <v>100</v>
       </c>
     </row>
-    <row r="9" spans="1:32" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:33" x14ac:dyDescent="0.15">
       <c r="A9" s="10">
         <v>42000006</v>
       </c>
@@ -2688,14 +2645,14 @@
         <v>31</v>
       </c>
       <c r="I9" s="5"/>
-      <c r="AC9">
+      <c r="AD9">
         <v>-100</v>
       </c>
-      <c r="AF9">
+      <c r="AG9">
         <v>100</v>
       </c>
     </row>
-    <row r="10" spans="1:32" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:33" x14ac:dyDescent="0.15">
       <c r="A10" s="10">
         <v>42000007</v>
       </c>
@@ -2718,14 +2675,14 @@
         <v>31</v>
       </c>
       <c r="I10" s="5"/>
-      <c r="AC10">
+      <c r="AD10">
         <v>-100</v>
       </c>
-      <c r="AD10">
+      <c r="AE10">
         <v>100</v>
       </c>
     </row>
-    <row r="11" spans="1:32" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:33" x14ac:dyDescent="0.15">
       <c r="A11">
         <v>42010001</v>
       </c>
@@ -2749,7 +2706,7 @@
       </c>
       <c r="I11" s="5"/>
     </row>
-    <row r="12" spans="1:32" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:33" x14ac:dyDescent="0.15">
       <c r="A12">
         <v>42010002</v>
       </c>
@@ -2776,7 +2733,7 @@
       </c>
       <c r="I12" s="5"/>
     </row>
-    <row r="13" spans="1:32" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:33" x14ac:dyDescent="0.15">
       <c r="A13">
         <v>42010003</v>
       </c>
@@ -2814,11 +2771,11 @@
       <c r="N13">
         <v>100</v>
       </c>
-      <c r="Z13">
+      <c r="AA13">
         <v>70</v>
       </c>
     </row>
-    <row r="14" spans="1:32" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:33" x14ac:dyDescent="0.15">
       <c r="A14">
         <v>42010004</v>
       </c>
@@ -2847,14 +2804,14 @@
       <c r="Q14">
         <v>30</v>
       </c>
-      <c r="X14">
-        <v>30</v>
-      </c>
       <c r="Y14">
         <v>30</v>
       </c>
-    </row>
-    <row r="15" spans="1:32" x14ac:dyDescent="0.15">
+      <c r="Z14">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15" spans="1:33" x14ac:dyDescent="0.15">
       <c r="A15">
         <v>42010005</v>
       </c>
@@ -2884,7 +2841,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="16" spans="1:32" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:33" x14ac:dyDescent="0.15">
       <c r="A16">
         <v>42010006</v>
       </c>
@@ -2922,11 +2879,11 @@
       <c r="Q16">
         <v>50</v>
       </c>
-      <c r="Z16">
+      <c r="AA16">
         <v>100</v>
       </c>
     </row>
-    <row r="17" spans="1:27" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A17">
         <v>42010007</v>
       </c>
@@ -2955,14 +2912,14 @@
       <c r="M17">
         <v>250</v>
       </c>
-      <c r="X17">
+      <c r="Y17">
         <v>250</v>
       </c>
-      <c r="AA17">
+      <c r="AB17">
         <v>50</v>
       </c>
     </row>
-    <row r="18" spans="1:27" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A18">
         <v>42010008</v>
       </c>
@@ -2992,7 +2949,7 @@
         <v>23000002</v>
       </c>
     </row>
-    <row r="19" spans="1:27" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A19">
         <v>42010009</v>
       </c>
@@ -3019,7 +2976,7 @@
         <v>23000003</v>
       </c>
     </row>
-    <row r="20" spans="1:27" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A20">
         <v>42010010</v>
       </c>
@@ -3045,11 +3002,11 @@
       <c r="S20">
         <v>23000004</v>
       </c>
-      <c r="Z20">
+      <c r="AA20">
         <v>50</v>
       </c>
     </row>
-    <row r="21" spans="1:27" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A21">
         <v>42010011</v>
       </c>
@@ -3079,7 +3036,7 @@
         <v>23000005</v>
       </c>
     </row>
-    <row r="22" spans="1:27" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A22">
         <v>42010012</v>
       </c>
@@ -3117,11 +3074,11 @@
       <c r="N22">
         <v>100</v>
       </c>
-      <c r="Z22">
+      <c r="AA22">
         <v>150</v>
       </c>
     </row>
-    <row r="23" spans="1:27" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A23">
         <v>42010013</v>
       </c>
@@ -3159,11 +3116,11 @@
       <c r="N23">
         <v>150</v>
       </c>
-      <c r="Z23">
+      <c r="AA23">
         <v>100</v>
       </c>
     </row>
-    <row r="24" spans="1:27" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A24">
         <v>42010014</v>
       </c>
@@ -3204,14 +3161,14 @@
       <c r="S24">
         <v>23000101</v>
       </c>
-      <c r="Z24">
-        <v>100</v>
-      </c>
       <c r="AA24">
         <v>100</v>
       </c>
-    </row>
-    <row r="25" spans="1:27" x14ac:dyDescent="0.15">
+      <c r="AB24">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="25" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A25">
         <v>42010015</v>
       </c>
@@ -3237,11 +3194,11 @@
         <v>125</v>
       </c>
       <c r="I25" s="5"/>
-      <c r="Z25">
+      <c r="AA25">
         <v>80</v>
       </c>
     </row>
-    <row r="26" spans="1:27" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A26">
         <v>42010016</v>
       </c>
@@ -3268,7 +3225,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="27" spans="1:27" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A27">
         <v>42010017</v>
       </c>
@@ -3312,11 +3269,11 @@
       <c r="S27">
         <v>23000102</v>
       </c>
-      <c r="Z27">
+      <c r="AA27">
         <v>100</v>
       </c>
     </row>
-    <row r="28" spans="1:27" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A28">
         <v>42010018</v>
       </c>
@@ -3342,7 +3299,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="29" spans="1:27" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A29">
         <v>42010019</v>
       </c>
@@ -3370,14 +3327,14 @@
       <c r="I29" s="5" t="s">
         <v>183</v>
       </c>
-      <c r="Y29">
+      <c r="Z29">
         <v>100</v>
       </c>
-      <c r="Z29">
+      <c r="AA29">
         <v>50</v>
       </c>
     </row>
-    <row r="30" spans="1:27" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A30">
         <v>42010020</v>
       </c>
@@ -3405,14 +3362,14 @@
       <c r="I30" s="5" t="s">
         <v>183</v>
       </c>
-      <c r="Y30">
+      <c r="Z30">
         <v>50</v>
       </c>
-      <c r="Z30">
+      <c r="AA30">
         <v>100</v>
       </c>
     </row>
-    <row r="31" spans="1:27" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A31">
         <v>42010021</v>
       </c>
@@ -3438,11 +3395,11 @@
         <v>192</v>
       </c>
       <c r="I31" s="5"/>
-      <c r="AA31">
+      <c r="AB31">
         <v>200</v>
       </c>
     </row>
-    <row r="32" spans="1:27" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A32">
         <v>42010022</v>
       </c>
@@ -3480,11 +3437,11 @@
       <c r="R32">
         <v>22031101</v>
       </c>
-      <c r="Z32">
+      <c r="AA32">
         <v>150</v>
       </c>
     </row>
-    <row r="33" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A33">
         <v>42040001</v>
       </c>
@@ -3519,17 +3476,17 @@
       <c r="Q33">
         <v>100</v>
       </c>
-      <c r="T33">
-        <v>1</v>
-      </c>
-      <c r="Z33">
-        <v>200</v>
+      <c r="U33">
+        <v>1</v>
       </c>
       <c r="AA33">
         <v>200</v>
       </c>
-    </row>
-    <row r="34" spans="1:28" x14ac:dyDescent="0.15">
+      <c r="AB33">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="34" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A34">
         <v>42040002</v>
       </c>
@@ -3570,14 +3527,14 @@
       <c r="S34">
         <v>23000102</v>
       </c>
-      <c r="Z34">
-        <v>150</v>
-      </c>
       <c r="AA34">
         <v>150</v>
       </c>
-    </row>
-    <row r="35" spans="1:28" x14ac:dyDescent="0.15">
+      <c r="AB34">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="35" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A35">
         <v>42040003</v>
       </c>
@@ -3603,14 +3560,14 @@
         <v>146</v>
       </c>
       <c r="I35" s="5"/>
-      <c r="X35">
+      <c r="Y35">
         <v>100</v>
       </c>
-      <c r="Z35">
+      <c r="AA35">
         <v>100</v>
       </c>
     </row>
-    <row r="36" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A36">
         <v>42040004</v>
       </c>
@@ -3636,14 +3593,14 @@
         <v>204</v>
       </c>
       <c r="I36" s="5"/>
-      <c r="W36">
-        <v>1</v>
-      </c>
-      <c r="AB36">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:28" x14ac:dyDescent="0.15">
+      <c r="T36">
+        <v>1</v>
+      </c>
+      <c r="AC36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A37">
         <v>42040005</v>
       </c>
@@ -3681,14 +3638,14 @@
       <c r="N37">
         <v>150</v>
       </c>
-      <c r="X37">
-        <v>200</v>
-      </c>
       <c r="Y37">
         <v>200</v>
       </c>
-    </row>
-    <row r="38" spans="1:28" x14ac:dyDescent="0.15">
+      <c r="Z37">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="38" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A38">
         <v>42040006</v>
       </c>
@@ -3726,7 +3683,7 @@
       <c r="Q38">
         <v>200</v>
       </c>
-      <c r="Z38">
+      <c r="AA38">
         <v>300</v>
       </c>
     </row>
@@ -3743,11 +3700,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AF23"/>
+  <dimension ref="A1:AG23"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="H1" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N12" sqref="N12"/>
+      <selection pane="bottomLeft" activeCell="V3" sqref="V1:V3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -3762,12 +3719,12 @@
     <col min="13" max="17" width="4.125" customWidth="1"/>
     <col min="18" max="18" width="9.75" customWidth="1"/>
     <col min="19" max="19" width="7.5" customWidth="1"/>
-    <col min="20" max="22" width="9.375" customWidth="1"/>
-    <col min="23" max="23" width="5.125" customWidth="1"/>
-    <col min="24" max="32" width="5" customWidth="1"/>
+    <col min="20" max="20" width="5.125" customWidth="1"/>
+    <col min="21" max="24" width="9.375" customWidth="1"/>
+    <col min="26" max="34" width="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" ht="55.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:33" ht="55.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="14" t="s">
         <v>79</v>
       </c>
@@ -3826,46 +3783,49 @@
         <v>77</v>
       </c>
       <c r="T1" s="15" t="s">
+        <v>200</v>
+      </c>
+      <c r="U1" s="15" t="s">
         <v>137</v>
       </c>
-      <c r="U1" s="15" t="s">
+      <c r="V1" s="15" t="s">
+        <v>230</v>
+      </c>
+      <c r="W1" s="15" t="s">
         <v>156</v>
       </c>
-      <c r="V1" s="15" t="s">
+      <c r="X1" s="15" t="s">
         <v>176</v>
       </c>
-      <c r="W1" s="15" t="s">
+      <c r="Y1" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="Z1" s="16" t="s">
+        <v>88</v>
+      </c>
+      <c r="AA1" s="16" t="s">
+        <v>78</v>
+      </c>
+      <c r="AB1" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="AC1" s="16" t="s">
         <v>200</v>
       </c>
-      <c r="X1" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="Y1" s="16" t="s">
-        <v>88</v>
-      </c>
-      <c r="Z1" s="16" t="s">
-        <v>78</v>
-      </c>
-      <c r="AA1" s="16" t="s">
-        <v>89</v>
-      </c>
-      <c r="AB1" s="16" t="s">
-        <v>200</v>
-      </c>
-      <c r="AC1" s="17" t="s">
+      <c r="AD1" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" s="17" t="s">
+      <c r="AE1" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" s="17" t="s">
+      <c r="AF1" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="AF1" s="17" t="s">
+      <c r="AG1" s="17" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:32" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:33" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>59</v>
       </c>
@@ -3924,20 +3884,20 @@
         <v>59</v>
       </c>
       <c r="T2" s="7" t="s">
+        <v>199</v>
+      </c>
+      <c r="U2" s="7" t="s">
         <v>138</v>
       </c>
-      <c r="U2" s="7" t="s">
+      <c r="V2" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="W2" s="7" t="s">
         <v>157</v>
       </c>
-      <c r="V2" s="7" t="s">
+      <c r="X2" s="7" t="s">
         <v>177</v>
       </c>
-      <c r="W2" s="7" t="s">
-        <v>199</v>
-      </c>
-      <c r="X2" s="3" t="s">
-        <v>0</v>
-      </c>
       <c r="Y2" s="3" t="s">
         <v>0</v>
       </c>
@@ -3945,13 +3905,13 @@
         <v>0</v>
       </c>
       <c r="AA2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="AB2" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="AB2" s="3" t="s">
+      <c r="AC2" s="3" t="s">
         <v>202</v>
-      </c>
-      <c r="AC2" s="9" t="s">
-        <v>27</v>
       </c>
       <c r="AD2" s="9" t="s">
         <v>27</v>
@@ -3962,8 +3922,11 @@
       <c r="AF2" s="9" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="3" spans="1:32" x14ac:dyDescent="0.15">
+      <c r="AG2" s="9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:33" x14ac:dyDescent="0.15">
       <c r="A3" s="8" t="s">
         <v>64</v>
       </c>
@@ -4022,46 +3985,49 @@
         <v>35</v>
       </c>
       <c r="T3" s="6" t="s">
+        <v>198</v>
+      </c>
+      <c r="U3" s="6" t="s">
         <v>139</v>
       </c>
-      <c r="U3" s="6" t="s">
+      <c r="V3" s="6" t="s">
+        <v>232</v>
+      </c>
+      <c r="W3" s="6" t="s">
         <v>159</v>
       </c>
-      <c r="V3" s="6" t="s">
+      <c r="X3" s="6" t="s">
         <v>178</v>
       </c>
-      <c r="W3" s="6" t="s">
-        <v>198</v>
-      </c>
-      <c r="X3" s="2" t="s">
+      <c r="Y3" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="Y3" s="2" t="s">
+      <c r="Z3" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="Z3" s="2" t="s">
+      <c r="AA3" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="AA3" s="2" t="s">
+      <c r="AB3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="AB3" s="2" t="s">
+      <c r="AC3" s="2" t="s">
         <v>203</v>
       </c>
-      <c r="AC3" s="8" t="s">
+      <c r="AD3" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="AD3" s="8" t="s">
+      <c r="AE3" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="AE3" s="8" t="s">
+      <c r="AF3" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="AF3" s="8" t="s">
+      <c r="AG3" s="8" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:32" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:33" x14ac:dyDescent="0.15">
       <c r="A4" s="10">
         <v>42020001</v>
       </c>
@@ -4088,17 +4054,17 @@
       </c>
       <c r="K4" s="11"/>
       <c r="L4" s="13"/>
-      <c r="AC4">
+      <c r="AD4">
         <v>-300</v>
-      </c>
-      <c r="AE4">
-        <v>1000</v>
       </c>
       <c r="AF4">
         <v>1000</v>
       </c>
-    </row>
-    <row r="5" spans="1:32" x14ac:dyDescent="0.15">
+      <c r="AG4">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:33" x14ac:dyDescent="0.15">
       <c r="A5" s="10">
         <v>42020002</v>
       </c>
@@ -4125,14 +4091,14 @@
       </c>
       <c r="K5" s="11"/>
       <c r="L5" s="13"/>
-      <c r="AC5">
+      <c r="AD5">
         <v>-200</v>
       </c>
-      <c r="AD5">
+      <c r="AE5">
         <v>1000</v>
       </c>
     </row>
-    <row r="6" spans="1:32" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:33" x14ac:dyDescent="0.15">
       <c r="A6" s="10">
         <v>42020003</v>
       </c>
@@ -4160,7 +4126,7 @@
       <c r="K6" s="11"/>
       <c r="L6" s="13"/>
     </row>
-    <row r="7" spans="1:32" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:33" x14ac:dyDescent="0.15">
       <c r="A7" s="10">
         <v>42020004</v>
       </c>
@@ -4186,7 +4152,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:32" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:33" x14ac:dyDescent="0.15">
       <c r="A8" s="10">
         <v>42020005</v>
       </c>
@@ -4214,7 +4180,7 @@
       <c r="K8" s="11"/>
       <c r="L8" s="13"/>
     </row>
-    <row r="9" spans="1:32" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:33" x14ac:dyDescent="0.15">
       <c r="A9">
         <v>42030001</v>
       </c>
@@ -4242,7 +4208,7 @@
       <c r="K9" s="4"/>
       <c r="L9" s="12"/>
     </row>
-    <row r="10" spans="1:32" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:33" x14ac:dyDescent="0.15">
       <c r="A10">
         <v>42030002</v>
       </c>
@@ -4274,11 +4240,11 @@
         <v>16</v>
       </c>
       <c r="L10" s="12"/>
-      <c r="T10">
+      <c r="U10">
         <v>43020101</v>
       </c>
     </row>
-    <row r="11" spans="1:32" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:33" x14ac:dyDescent="0.15">
       <c r="A11">
         <v>42030003</v>
       </c>
@@ -4306,7 +4272,7 @@
       <c r="K11" s="12"/>
       <c r="L11" s="12"/>
     </row>
-    <row r="12" spans="1:32" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:33" x14ac:dyDescent="0.15">
       <c r="A12">
         <v>42030004</v>
       </c>
@@ -4333,14 +4299,14 @@
       </c>
       <c r="K12" s="12"/>
       <c r="L12" s="12"/>
-      <c r="T12">
+      <c r="U12">
         <v>43020102</v>
       </c>
-      <c r="U12" t="s">
+      <c r="W12" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="13" spans="1:32" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:33" x14ac:dyDescent="0.15">
       <c r="A13">
         <v>42030005</v>
       </c>
@@ -4376,14 +4342,14 @@
       <c r="R13">
         <v>22031011</v>
       </c>
-      <c r="U13" t="s">
+      <c r="W13" t="s">
         <v>175</v>
       </c>
-      <c r="V13">
+      <c r="X13">
         <v>42030012</v>
       </c>
     </row>
-    <row r="14" spans="1:32" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:33" x14ac:dyDescent="0.15">
       <c r="A14">
         <v>42030006</v>
       </c>
@@ -4411,7 +4377,7 @@
       <c r="K14" s="12"/>
       <c r="L14" s="12"/>
     </row>
-    <row r="15" spans="1:32" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:33" x14ac:dyDescent="0.15">
       <c r="A15">
         <v>42030007</v>
       </c>
@@ -4439,7 +4405,7 @@
       <c r="K15" s="12"/>
       <c r="L15" s="12"/>
     </row>
-    <row r="16" spans="1:32" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:33" x14ac:dyDescent="0.15">
       <c r="A16">
         <v>42030008</v>
       </c>
@@ -4467,7 +4433,7 @@
       <c r="K16" s="12"/>
       <c r="L16" s="12"/>
     </row>
-    <row r="17" spans="1:27" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A17">
         <v>42030009</v>
       </c>
@@ -4495,7 +4461,7 @@
       <c r="K17" s="12"/>
       <c r="L17" s="12"/>
     </row>
-    <row r="18" spans="1:27" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A18">
         <v>42030010</v>
       </c>
@@ -4523,7 +4489,7 @@
       <c r="K18" s="12"/>
       <c r="L18" s="12"/>
     </row>
-    <row r="19" spans="1:27" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A19">
         <v>42030011</v>
       </c>
@@ -4551,7 +4517,7 @@
       <c r="K19" s="12"/>
       <c r="L19" s="12"/>
     </row>
-    <row r="20" spans="1:27" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A20">
         <v>42030012</v>
       </c>
@@ -4583,11 +4549,11 @@
         <v>16</v>
       </c>
       <c r="L20" s="12"/>
-      <c r="T20">
+      <c r="U20">
         <v>43020105</v>
       </c>
     </row>
-    <row r="21" spans="1:27" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A21">
         <v>42050001</v>
       </c>
@@ -4617,7 +4583,7 @@
         <v>13020001</v>
       </c>
     </row>
-    <row r="22" spans="1:27" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A22">
         <v>42050002</v>
       </c>
@@ -4647,7 +4613,7 @@
         <v>13020002</v>
       </c>
     </row>
-    <row r="23" spans="1:27" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A23">
         <v>42050003</v>
       </c>
@@ -4699,13 +4665,13 @@
       <c r="Q23">
         <v>300</v>
       </c>
-      <c r="U23" t="s">
+      <c r="W23" t="s">
         <v>218</v>
       </c>
-      <c r="Z23">
+      <c r="AA23">
         <v>200</v>
       </c>
-      <c r="AA23">
+      <c r="AB23">
         <v>200</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fill the quest content
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/SceneQuest.xlsx
+++ b/ConfigData/Xlsx/SceneQuest.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\Code\TOMClassicGit\ConfigData\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\TOMClassicGit\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="476" uniqueCount="240">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="482" uniqueCount="248">
   <si>
     <t>int</t>
     <phoneticPr fontId="18" type="noConversion"/>
@@ -940,6 +940,38 @@
   </si>
   <si>
     <t>TriggerHourEnd</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>npcsainisi</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>dungeonentry</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>EnemyId</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>SceneId</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>任务要求</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>int</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>QuestNeed</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>npcqiaosiji</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -1142,7 +1174,7 @@
       <charset val="134"/>
     </font>
   </fonts>
-  <fills count="41">
+  <fills count="43">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1370,6 +1402,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="11">
     <border>
@@ -1624,7 +1668,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1678,6 +1722,15 @@
     </xf>
     <xf numFmtId="0" fontId="20" fillId="38" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="42" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="42" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="41" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1724,13 +1777,7 @@
     <cellStyle name="着色 6" xfId="38" builtinId="49" customBuiltin="1"/>
     <cellStyle name="注释" xfId="15" builtinId="10" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="9">
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
+  <dxfs count="11">
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
@@ -1755,6 +1802,12 @@
       </font>
     </dxf>
     <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -1774,6 +1827,12 @@
       <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -1783,74 +1842,6 @@
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1863,12 +1854,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="表3" displayName="表3" ref="A3:AI38" totalsRowShown="0" headerRowDxfId="8">
-  <autoFilter ref="A3:AI38"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="表3" displayName="表3" ref="A3:AJ38" totalsRowShown="0" headerRowDxfId="10">
+  <autoFilter ref="A3:AJ38"/>
   <sortState ref="A4:AD28">
     <sortCondition ref="A3:A28"/>
   </sortState>
-  <tableColumns count="35">
+  <tableColumns count="36">
     <tableColumn id="1" name="Id"/>
     <tableColumn id="2" name="Name"/>
     <tableColumn id="28" name="Type"/>
@@ -1877,9 +1868,10 @@
     <tableColumn id="24" name="Ename"/>
     <tableColumn id="4" name="Figue"/>
     <tableColumn id="5" name="Script"/>
-    <tableColumn id="6" name="TriggerMulti" dataDxfId="7"/>
-    <tableColumn id="35" name="TriggerHourBegin" dataDxfId="2"/>
-    <tableColumn id="34" name="TriggerHourEnd" dataDxfId="3"/>
+    <tableColumn id="6" name="TriggerMulti" dataDxfId="9"/>
+    <tableColumn id="35" name="TriggerHourBegin" dataDxfId="8"/>
+    <tableColumn id="34" name="TriggerHourEnd" dataDxfId="7"/>
+    <tableColumn id="37" name="QuestNeed" dataDxfId="0"/>
     <tableColumn id="7" name="EnemyId"/>
     <tableColumn id="8" name="BattleMap"/>
     <tableColumn id="32" name="SceneId"/>
@@ -1910,12 +1902,12 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="表3_5" displayName="表3_5" ref="A3:AI24" totalsRowShown="0" headerRowDxfId="6">
-  <autoFilter ref="A3:AI24"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="表3_5" displayName="表3_5" ref="A3:AJ24" totalsRowShown="0" headerRowDxfId="6">
+  <autoFilter ref="A3:AJ24"/>
   <sortState ref="A4:Z6">
     <sortCondition ref="A3:A6"/>
   </sortState>
-  <tableColumns count="35">
+  <tableColumns count="36">
     <tableColumn id="1" name="Id"/>
     <tableColumn id="2" name="Name"/>
     <tableColumn id="27" name="Type" dataDxfId="5"/>
@@ -1925,11 +1917,12 @@
     <tableColumn id="4" name="Figue"/>
     <tableColumn id="5" name="Script"/>
     <tableColumn id="6" name="TriggerMulti"/>
-    <tableColumn id="35" name="TriggerHourBegin" dataDxfId="0"/>
-    <tableColumn id="34" name="TriggerHourEnd" dataDxfId="1"/>
+    <tableColumn id="35" name="TriggerHourBegin" dataDxfId="4"/>
+    <tableColumn id="34" name="TriggerHourEnd" dataDxfId="3"/>
+    <tableColumn id="36" name="QuestNeed" dataDxfId="1"/>
     <tableColumn id="7" name="EnemyId"/>
     <tableColumn id="8" name="BattleMap"/>
-    <tableColumn id="32" name="SceneId" dataDxfId="4"/>
+    <tableColumn id="32" name="SceneId" dataDxfId="2"/>
     <tableColumn id="9" name="RewardGold"/>
     <tableColumn id="10" name="RewardFood"/>
     <tableColumn id="11" name="RewardHealth"/>
@@ -1964,7 +1957,7 @@
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="CAEACD"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -2243,11 +2236,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AI38"/>
+  <dimension ref="A1:AJ38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J1" sqref="J1:K3"/>
+      <pane ySplit="3" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M34" sqref="M34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -2255,19 +2248,19 @@
     <col min="1" max="1" width="9.5" bestFit="1" customWidth="1"/>
     <col min="3" max="5" width="2.75" customWidth="1"/>
     <col min="6" max="6" width="8.75" customWidth="1"/>
-    <col min="9" max="11" width="4.875" customWidth="1"/>
-    <col min="12" max="12" width="9.75" customWidth="1"/>
-    <col min="13" max="13" width="6.75" customWidth="1"/>
-    <col min="14" max="14" width="9.375" customWidth="1"/>
-    <col min="15" max="19" width="4.875" customWidth="1"/>
-    <col min="20" max="21" width="9.375" customWidth="1"/>
-    <col min="22" max="22" width="4.25" customWidth="1"/>
-    <col min="23" max="24" width="9.375" customWidth="1"/>
-    <col min="25" max="26" width="4.25" customWidth="1"/>
-    <col min="28" max="36" width="4.75" customWidth="1"/>
+    <col min="9" max="12" width="4.875" customWidth="1"/>
+    <col min="13" max="13" width="9.75" customWidth="1"/>
+    <col min="14" max="14" width="6.75" customWidth="1"/>
+    <col min="15" max="15" width="9.375" customWidth="1"/>
+    <col min="16" max="20" width="4.875" customWidth="1"/>
+    <col min="21" max="22" width="9.375" customWidth="1"/>
+    <col min="23" max="23" width="4.25" customWidth="1"/>
+    <col min="24" max="25" width="9.375" customWidth="1"/>
+    <col min="26" max="27" width="4.25" customWidth="1"/>
+    <col min="29" max="37" width="4.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" ht="69" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:36" ht="69" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="14" t="s">
         <v>79</v>
       </c>
@@ -2302,79 +2295,82 @@
         <v>238</v>
       </c>
       <c r="L1" s="14" t="s">
+        <v>244</v>
+      </c>
+      <c r="M1" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="M1" s="14" t="s">
+      <c r="N1" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="N1" s="14" t="s">
+      <c r="O1" s="18" t="s">
         <v>210</v>
       </c>
-      <c r="O1" s="15" t="s">
+      <c r="P1" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="P1" s="15" t="s">
+      <c r="Q1" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="Q1" s="15" t="s">
+      <c r="R1" s="15" t="s">
         <v>84</v>
       </c>
-      <c r="R1" s="15" t="s">
+      <c r="S1" s="15" t="s">
         <v>85</v>
       </c>
-      <c r="S1" s="15" t="s">
+      <c r="T1" s="15" t="s">
         <v>86</v>
       </c>
-      <c r="T1" s="15" t="s">
+      <c r="U1" s="15" t="s">
         <v>87</v>
       </c>
-      <c r="U1" s="15" t="s">
+      <c r="V1" s="15" t="s">
         <v>77</v>
       </c>
-      <c r="V1" s="15" t="s">
+      <c r="W1" s="15" t="s">
         <v>200</v>
       </c>
-      <c r="W1" s="15" t="s">
+      <c r="X1" s="15" t="s">
         <v>137</v>
       </c>
-      <c r="X1" s="15" t="s">
+      <c r="Y1" s="15" t="s">
         <v>230</v>
       </c>
-      <c r="Y1" s="15" t="s">
+      <c r="Z1" s="15" t="s">
         <v>156</v>
       </c>
-      <c r="Z1" s="15" t="s">
+      <c r="AA1" s="15" t="s">
         <v>176</v>
       </c>
-      <c r="AA1" s="16" t="s">
+      <c r="AB1" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="AB1" s="16" t="s">
+      <c r="AC1" s="16" t="s">
         <v>88</v>
       </c>
-      <c r="AC1" s="16" t="s">
+      <c r="AD1" s="16" t="s">
         <v>78</v>
       </c>
-      <c r="AD1" s="16" t="s">
+      <c r="AE1" s="16" t="s">
         <v>89</v>
       </c>
-      <c r="AE1" s="16" t="s">
+      <c r="AF1" s="16" t="s">
         <v>201</v>
       </c>
-      <c r="AF1" s="17" t="s">
+      <c r="AG1" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="AG1" s="17" t="s">
+      <c r="AH1" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="AH1" s="17" t="s">
+      <c r="AI1" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="AI1" s="17" t="s">
+      <c r="AJ1" s="17" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>59</v>
       </c>
@@ -2409,22 +2405,22 @@
         <v>236</v>
       </c>
       <c r="L2" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="M2" s="19" t="s">
         <v>59</v>
       </c>
-      <c r="M2" s="1" t="s">
+      <c r="N2" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="N2" s="1" t="s">
+      <c r="O2" s="19" t="s">
         <v>211</v>
       </c>
-      <c r="O2" s="7" t="s">
+      <c r="P2" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="P2" s="7" t="s">
-        <v>0</v>
-      </c>
       <c r="Q2" s="7" t="s">
-        <v>59</v>
+        <v>0</v>
       </c>
       <c r="R2" s="7" t="s">
         <v>59</v>
@@ -2433,29 +2429,29 @@
         <v>59</v>
       </c>
       <c r="T2" s="7" t="s">
-        <v>0</v>
+        <v>59</v>
       </c>
       <c r="U2" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="V2" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="V2" s="7" t="s">
+      <c r="W2" s="7" t="s">
         <v>199</v>
       </c>
-      <c r="W2" s="7" t="s">
+      <c r="X2" s="7" t="s">
         <v>138</v>
       </c>
-      <c r="X2" s="7" t="s">
+      <c r="Y2" s="7" t="s">
         <v>231</v>
       </c>
-      <c r="Y2" s="7" t="s">
+      <c r="Z2" s="7" t="s">
         <v>157</v>
       </c>
-      <c r="Z2" s="7" t="s">
+      <c r="AA2" s="7" t="s">
         <v>177</v>
       </c>
-      <c r="AA2" s="3" t="s">
-        <v>0</v>
-      </c>
       <c r="AB2" s="3" t="s">
         <v>0</v>
       </c>
@@ -2463,13 +2459,13 @@
         <v>0</v>
       </c>
       <c r="AD2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="AE2" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="AE2" s="3" t="s">
+      <c r="AF2" s="3" t="s">
         <v>202</v>
-      </c>
-      <c r="AF2" s="9" t="s">
-        <v>27</v>
       </c>
       <c r="AG2" s="9" t="s">
         <v>27</v>
@@ -2480,8 +2476,11 @@
       <c r="AI2" s="9" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.15">
+      <c r="AJ2" s="9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A3" s="8" t="s">
         <v>64</v>
       </c>
@@ -2516,79 +2515,82 @@
         <v>239</v>
       </c>
       <c r="L3" s="8" t="s">
+        <v>246</v>
+      </c>
+      <c r="M3" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="M3" s="8" t="s">
+      <c r="N3" s="20" t="s">
         <v>70</v>
       </c>
-      <c r="N3" s="8" t="s">
+      <c r="O3" s="20" t="s">
         <v>212</v>
       </c>
-      <c r="O3" s="6" t="s">
+      <c r="P3" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="P3" s="6" t="s">
+      <c r="Q3" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="Q3" s="6" t="s">
+      <c r="R3" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="R3" s="6" t="s">
+      <c r="S3" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="S3" s="6" t="s">
+      <c r="T3" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="T3" s="6" t="s">
+      <c r="U3" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="U3" s="6" t="s">
+      <c r="V3" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="V3" s="6" t="s">
+      <c r="W3" s="6" t="s">
         <v>198</v>
       </c>
-      <c r="W3" s="6" t="s">
+      <c r="X3" s="6" t="s">
         <v>139</v>
       </c>
-      <c r="X3" s="6" t="s">
+      <c r="Y3" s="6" t="s">
         <v>232</v>
       </c>
-      <c r="Y3" s="6" t="s">
+      <c r="Z3" s="6" t="s">
         <v>159</v>
       </c>
-      <c r="Z3" s="6" t="s">
+      <c r="AA3" s="6" t="s">
         <v>178</v>
       </c>
-      <c r="AA3" s="2" t="s">
+      <c r="AB3" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="AB3" s="2" t="s">
+      <c r="AC3" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="AC3" s="2" t="s">
+      <c r="AD3" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="AD3" s="2" t="s">
+      <c r="AE3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="AE3" s="2" t="s">
+      <c r="AF3" s="2" t="s">
         <v>203</v>
       </c>
-      <c r="AF3" s="8" t="s">
+      <c r="AG3" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="AG3" s="8" t="s">
+      <c r="AH3" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="AH3" s="8" t="s">
+      <c r="AI3" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="AI3" s="8" t="s">
+      <c r="AJ3" s="8" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A4">
         <v>42000001</v>
       </c>
@@ -2613,17 +2615,15 @@
       <c r="I4" s="5"/>
       <c r="J4" s="5"/>
       <c r="K4" s="5"/>
-      <c r="L4">
+      <c r="L4" s="5"/>
+      <c r="M4">
         <v>43000001</v>
       </c>
-      <c r="M4" t="s">
+      <c r="N4" t="s">
         <v>16</v>
       </c>
-      <c r="N4" s="12">
+      <c r="O4" s="12">
         <v>13020001</v>
-      </c>
-      <c r="O4">
-        <v>100</v>
       </c>
       <c r="P4">
         <v>100</v>
@@ -2638,10 +2638,10 @@
         <v>100</v>
       </c>
       <c r="T4">
+        <v>100</v>
+      </c>
+      <c r="U4">
         <v>22011180</v>
-      </c>
-      <c r="AA4">
-        <v>100</v>
       </c>
       <c r="AB4">
         <v>100</v>
@@ -2652,8 +2652,11 @@
       <c r="AD4">
         <v>100</v>
       </c>
-    </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.15">
+      <c r="AE4">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A5" s="10">
         <v>42000002</v>
       </c>
@@ -2678,8 +2681,9 @@
       <c r="I5" s="5"/>
       <c r="J5" s="5"/>
       <c r="K5" s="5"/>
-    </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.15">
+      <c r="L5" s="5"/>
+    </row>
+    <row r="6" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A6" s="10">
         <v>42000003</v>
       </c>
@@ -2704,8 +2708,9 @@
       <c r="I6" s="5"/>
       <c r="J6" s="5"/>
       <c r="K6" s="5"/>
-    </row>
-    <row r="7" spans="1:35" x14ac:dyDescent="0.15">
+      <c r="L6" s="5"/>
+    </row>
+    <row r="7" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A7" s="10">
         <v>42000004</v>
       </c>
@@ -2730,8 +2735,9 @@
       <c r="I7" s="5"/>
       <c r="J7" s="5"/>
       <c r="K7" s="5"/>
-    </row>
-    <row r="8" spans="1:35" x14ac:dyDescent="0.15">
+      <c r="L7" s="5"/>
+    </row>
+    <row r="8" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A8" s="10">
         <v>42000005</v>
       </c>
@@ -2756,14 +2762,15 @@
       <c r="I8" s="5"/>
       <c r="J8" s="5"/>
       <c r="K8" s="5"/>
-      <c r="AF8">
+      <c r="L8" s="5"/>
+      <c r="AG8">
         <v>-100</v>
       </c>
-      <c r="AH8">
+      <c r="AI8">
         <v>100</v>
       </c>
     </row>
-    <row r="9" spans="1:35" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A9" s="10">
         <v>42000006</v>
       </c>
@@ -2788,14 +2795,15 @@
       <c r="I9" s="5"/>
       <c r="J9" s="5"/>
       <c r="K9" s="5"/>
-      <c r="AF9">
+      <c r="L9" s="5"/>
+      <c r="AG9">
         <v>-100</v>
       </c>
-      <c r="AI9">
+      <c r="AJ9">
         <v>100</v>
       </c>
     </row>
-    <row r="10" spans="1:35" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A10" s="10">
         <v>42000007</v>
       </c>
@@ -2820,14 +2828,15 @@
       <c r="I10" s="5"/>
       <c r="J10" s="5"/>
       <c r="K10" s="5"/>
-      <c r="AF10">
+      <c r="L10" s="5"/>
+      <c r="AG10">
         <v>-100</v>
       </c>
-      <c r="AG10">
+      <c r="AH10">
         <v>100</v>
       </c>
     </row>
-    <row r="11" spans="1:35" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A11">
         <v>42010001</v>
       </c>
@@ -2852,8 +2861,9 @@
       <c r="I11" s="5"/>
       <c r="J11" s="5"/>
       <c r="K11" s="5"/>
-    </row>
-    <row r="12" spans="1:35" x14ac:dyDescent="0.15">
+      <c r="L11" s="5"/>
+    </row>
+    <row r="12" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A12">
         <v>42010002</v>
       </c>
@@ -2881,8 +2891,9 @@
       <c r="I12" s="5"/>
       <c r="J12" s="5"/>
       <c r="K12" s="5"/>
-    </row>
-    <row r="13" spans="1:35" x14ac:dyDescent="0.15">
+      <c r="L12" s="5"/>
+    </row>
+    <row r="13" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A13">
         <v>42010003</v>
       </c>
@@ -2910,23 +2921,24 @@
       <c r="I13" s="5"/>
       <c r="J13" s="5"/>
       <c r="K13" s="5"/>
-      <c r="L13">
+      <c r="L13" s="5"/>
+      <c r="M13">
         <v>43000001</v>
       </c>
-      <c r="M13" t="s">
+      <c r="N13" t="s">
         <v>42</v>
       </c>
-      <c r="O13">
+      <c r="P13">
         <v>70</v>
       </c>
-      <c r="P13">
+      <c r="Q13">
         <v>100</v>
       </c>
-      <c r="AC13">
+      <c r="AD13">
         <v>70</v>
       </c>
     </row>
-    <row r="14" spans="1:35" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A14">
         <v>42010004</v>
       </c>
@@ -2954,17 +2966,18 @@
       <c r="I14" s="5"/>
       <c r="J14" s="5"/>
       <c r="K14" s="5"/>
-      <c r="S14">
-        <v>30</v>
-      </c>
-      <c r="AA14">
+      <c r="L14" s="5"/>
+      <c r="T14">
         <v>30</v>
       </c>
       <c r="AB14">
         <v>30</v>
       </c>
-    </row>
-    <row r="15" spans="1:35" x14ac:dyDescent="0.15">
+      <c r="AC14">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A15">
         <v>42010005</v>
       </c>
@@ -2989,14 +3002,15 @@
       <c r="I15" s="5"/>
       <c r="J15" s="5"/>
       <c r="K15" s="5"/>
-      <c r="P15">
+      <c r="L15" s="5"/>
+      <c r="Q15">
         <v>100</v>
       </c>
-      <c r="R15">
+      <c r="S15">
         <v>100</v>
       </c>
     </row>
-    <row r="16" spans="1:35" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A16">
         <v>42010006</v>
       </c>
@@ -3024,23 +3038,24 @@
       <c r="I16" s="5"/>
       <c r="J16" s="5"/>
       <c r="K16" s="5"/>
-      <c r="L16">
+      <c r="L16" s="5"/>
+      <c r="M16">
         <v>43000002</v>
       </c>
-      <c r="M16" t="s">
+      <c r="N16" t="s">
         <v>42</v>
       </c>
-      <c r="O16">
+      <c r="P16">
         <v>100</v>
       </c>
-      <c r="S16">
+      <c r="T16">
         <v>50</v>
       </c>
-      <c r="AC16">
+      <c r="AD16">
         <v>100</v>
       </c>
     </row>
-    <row r="17" spans="1:30" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:31" x14ac:dyDescent="0.15">
       <c r="A17">
         <v>42010007</v>
       </c>
@@ -3068,17 +3083,18 @@
       <c r="I17" s="5"/>
       <c r="J17" s="5"/>
       <c r="K17" s="5"/>
-      <c r="O17">
+      <c r="L17" s="5"/>
+      <c r="P17">
         <v>250</v>
       </c>
-      <c r="AA17">
+      <c r="AB17">
         <v>250</v>
       </c>
-      <c r="AD17">
+      <c r="AE17">
         <v>50</v>
       </c>
     </row>
-    <row r="18" spans="1:30" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:31" x14ac:dyDescent="0.15">
       <c r="A18">
         <v>42010008</v>
       </c>
@@ -3103,14 +3119,15 @@
       <c r="I18" s="5"/>
       <c r="J18" s="5"/>
       <c r="K18" s="5"/>
-      <c r="P18">
+      <c r="L18" s="5"/>
+      <c r="Q18">
         <v>100</v>
       </c>
-      <c r="U18">
+      <c r="V18">
         <v>23000002</v>
       </c>
     </row>
-    <row r="19" spans="1:30" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:31" x14ac:dyDescent="0.15">
       <c r="A19">
         <v>42010009</v>
       </c>
@@ -3135,11 +3152,12 @@
       <c r="I19" s="5"/>
       <c r="J19" s="5"/>
       <c r="K19" s="5"/>
-      <c r="U19">
+      <c r="L19" s="5"/>
+      <c r="V19">
         <v>23000003</v>
       </c>
     </row>
-    <row r="20" spans="1:30" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:31" x14ac:dyDescent="0.15">
       <c r="A20">
         <v>42010010</v>
       </c>
@@ -3164,14 +3182,15 @@
       <c r="I20" s="5"/>
       <c r="J20" s="5"/>
       <c r="K20" s="5"/>
-      <c r="U20">
+      <c r="L20" s="5"/>
+      <c r="V20">
         <v>23000004</v>
       </c>
-      <c r="AC20">
+      <c r="AD20">
         <v>50</v>
       </c>
     </row>
-    <row r="21" spans="1:30" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:31" x14ac:dyDescent="0.15">
       <c r="A21">
         <v>42010011</v>
       </c>
@@ -3196,14 +3215,15 @@
       <c r="I21" s="5"/>
       <c r="J21" s="5"/>
       <c r="K21" s="5"/>
-      <c r="R21">
+      <c r="L21" s="5"/>
+      <c r="S21">
         <v>150</v>
       </c>
-      <c r="U21">
+      <c r="V21">
         <v>23000005</v>
       </c>
     </row>
-    <row r="22" spans="1:30" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:31" x14ac:dyDescent="0.15">
       <c r="A22">
         <v>42010012</v>
       </c>
@@ -3231,23 +3251,24 @@
       <c r="I22" s="5"/>
       <c r="J22" s="5"/>
       <c r="K22" s="5"/>
-      <c r="L22">
+      <c r="L22" s="5"/>
+      <c r="M22">
         <v>43000011</v>
       </c>
-      <c r="M22" t="s">
+      <c r="N22" t="s">
         <v>16</v>
-      </c>
-      <c r="O22">
-        <v>100</v>
       </c>
       <c r="P22">
         <v>100</v>
       </c>
-      <c r="AC22">
+      <c r="Q22">
+        <v>100</v>
+      </c>
+      <c r="AD22">
         <v>150</v>
       </c>
     </row>
-    <row r="23" spans="1:30" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:31" x14ac:dyDescent="0.15">
       <c r="A23">
         <v>42010013</v>
       </c>
@@ -3275,23 +3296,24 @@
       <c r="I23" s="5"/>
       <c r="J23" s="5"/>
       <c r="K23" s="5"/>
-      <c r="L23">
+      <c r="L23" s="5"/>
+      <c r="M23">
         <v>43000007</v>
       </c>
-      <c r="M23" t="s">
+      <c r="N23" t="s">
         <v>42</v>
       </c>
-      <c r="O23">
+      <c r="P23">
         <v>50</v>
       </c>
-      <c r="P23">
+      <c r="Q23">
         <v>150</v>
       </c>
-      <c r="AC23">
+      <c r="AD23">
         <v>100</v>
       </c>
     </row>
-    <row r="24" spans="1:30" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:31" x14ac:dyDescent="0.15">
       <c r="A24">
         <v>42010014</v>
       </c>
@@ -3319,29 +3341,30 @@
       <c r="I24" s="5"/>
       <c r="J24" s="5"/>
       <c r="K24" s="5"/>
-      <c r="L24">
+      <c r="L24" s="5"/>
+      <c r="M24">
         <v>43000004</v>
       </c>
-      <c r="M24" t="s">
+      <c r="N24" t="s">
         <v>16</v>
       </c>
-      <c r="O24">
+      <c r="P24">
         <v>100</v>
       </c>
-      <c r="S24">
+      <c r="T24">
         <v>100</v>
       </c>
-      <c r="U24">
+      <c r="V24">
         <v>23000101</v>
-      </c>
-      <c r="AC24">
-        <v>100</v>
       </c>
       <c r="AD24">
         <v>100</v>
       </c>
-    </row>
-    <row r="25" spans="1:30" x14ac:dyDescent="0.15">
+      <c r="AE24">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="25" spans="1:31" x14ac:dyDescent="0.15">
       <c r="A25">
         <v>42010015</v>
       </c>
@@ -3369,11 +3392,12 @@
       <c r="I25" s="5"/>
       <c r="J25" s="5"/>
       <c r="K25" s="5"/>
-      <c r="AC25">
+      <c r="L25" s="5"/>
+      <c r="AD25">
         <v>80</v>
       </c>
     </row>
-    <row r="26" spans="1:30" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:31" x14ac:dyDescent="0.15">
       <c r="A26">
         <v>42010016</v>
       </c>
@@ -3398,11 +3422,12 @@
       <c r="I26" s="5"/>
       <c r="J26" s="5"/>
       <c r="K26" s="5"/>
-      <c r="P26">
+      <c r="L26" s="5"/>
+      <c r="Q26">
         <v>50</v>
       </c>
     </row>
-    <row r="27" spans="1:30" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:31" x14ac:dyDescent="0.15">
       <c r="A27">
         <v>42010017</v>
       </c>
@@ -3430,29 +3455,30 @@
       <c r="I27" s="5"/>
       <c r="J27" s="5"/>
       <c r="K27" s="5"/>
-      <c r="L27">
+      <c r="L27" s="5"/>
+      <c r="M27">
         <v>43000016</v>
       </c>
-      <c r="M27" t="s">
+      <c r="N27" t="s">
         <v>16</v>
       </c>
-      <c r="O27">
+      <c r="P27">
         <v>200</v>
       </c>
-      <c r="P27">
+      <c r="Q27">
         <v>100</v>
       </c>
-      <c r="S27">
+      <c r="T27">
         <v>100</v>
       </c>
-      <c r="U27">
+      <c r="V27">
         <v>23000102</v>
       </c>
-      <c r="AC27">
+      <c r="AD27">
         <v>100</v>
       </c>
     </row>
-    <row r="28" spans="1:30" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:31" x14ac:dyDescent="0.15">
       <c r="A28">
         <v>42010018</v>
       </c>
@@ -3479,8 +3505,9 @@
       </c>
       <c r="J28" s="5"/>
       <c r="K28" s="5"/>
-    </row>
-    <row r="29" spans="1:30" x14ac:dyDescent="0.15">
+      <c r="L28" s="5"/>
+    </row>
+    <row r="29" spans="1:31" x14ac:dyDescent="0.15">
       <c r="A29">
         <v>42010019</v>
       </c>
@@ -3510,14 +3537,15 @@
       </c>
       <c r="J29" s="5"/>
       <c r="K29" s="5"/>
-      <c r="AB29">
+      <c r="L29" s="5"/>
+      <c r="AC29">
         <v>100</v>
       </c>
-      <c r="AC29">
+      <c r="AD29">
         <v>50</v>
       </c>
     </row>
-    <row r="30" spans="1:30" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:31" x14ac:dyDescent="0.15">
       <c r="A30">
         <v>42010020</v>
       </c>
@@ -3547,14 +3575,15 @@
       </c>
       <c r="J30" s="5"/>
       <c r="K30" s="5"/>
-      <c r="AB30">
+      <c r="L30" s="5"/>
+      <c r="AC30">
         <v>50</v>
       </c>
-      <c r="AC30">
+      <c r="AD30">
         <v>100</v>
       </c>
     </row>
-    <row r="31" spans="1:30" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:31" x14ac:dyDescent="0.15">
       <c r="A31">
         <v>42010021</v>
       </c>
@@ -3582,11 +3611,12 @@
       <c r="I31" s="5"/>
       <c r="J31" s="5"/>
       <c r="K31" s="5"/>
-      <c r="AD31">
+      <c r="L31" s="5"/>
+      <c r="AE31">
         <v>200</v>
       </c>
     </row>
-    <row r="32" spans="1:30" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:31" x14ac:dyDescent="0.15">
       <c r="A32">
         <v>42010022</v>
       </c>
@@ -3614,23 +3644,24 @@
       <c r="I32" s="5"/>
       <c r="J32" s="5"/>
       <c r="K32" s="5"/>
-      <c r="L32">
+      <c r="L32" s="5"/>
+      <c r="M32">
         <v>43000034</v>
       </c>
-      <c r="M32" t="s">
+      <c r="N32" t="s">
         <v>16</v>
       </c>
-      <c r="S32">
+      <c r="T32">
         <v>100</v>
       </c>
-      <c r="T32">
+      <c r="U32">
         <v>22031101</v>
       </c>
-      <c r="AC32">
+      <c r="AD32">
         <v>150</v>
       </c>
     </row>
-    <row r="33" spans="1:31" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:32" x14ac:dyDescent="0.15">
       <c r="A33">
         <v>42040001</v>
       </c>
@@ -3658,26 +3689,27 @@
       <c r="I33" s="5"/>
       <c r="J33" s="5"/>
       <c r="K33" s="5"/>
-      <c r="L33">
-        <v>1</v>
-      </c>
-      <c r="M33" t="s">
+      <c r="L33" s="5"/>
+      <c r="M33">
+        <v>1</v>
+      </c>
+      <c r="N33" t="s">
         <v>16</v>
       </c>
-      <c r="S33">
+      <c r="T33">
         <v>100</v>
       </c>
-      <c r="W33">
-        <v>1</v>
-      </c>
-      <c r="AC33">
-        <v>200</v>
+      <c r="X33">
+        <v>1</v>
       </c>
       <c r="AD33">
         <v>200</v>
       </c>
-    </row>
-    <row r="34" spans="1:31" x14ac:dyDescent="0.15">
+      <c r="AE33">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="34" spans="1:32" x14ac:dyDescent="0.15">
       <c r="A34">
         <v>42040002</v>
       </c>
@@ -3705,29 +3737,30 @@
       <c r="I34" s="5"/>
       <c r="J34" s="5"/>
       <c r="K34" s="5"/>
-      <c r="L34">
+      <c r="L34" s="5"/>
+      <c r="M34">
         <v>43000005</v>
       </c>
-      <c r="M34" t="s">
+      <c r="N34" t="s">
         <v>16</v>
       </c>
-      <c r="O34">
+      <c r="P34">
         <v>200</v>
       </c>
-      <c r="P34">
+      <c r="Q34">
         <v>50</v>
       </c>
-      <c r="U34">
+      <c r="V34">
         <v>23000102</v>
-      </c>
-      <c r="AC34">
-        <v>150</v>
       </c>
       <c r="AD34">
         <v>150</v>
       </c>
-    </row>
-    <row r="35" spans="1:31" x14ac:dyDescent="0.15">
+      <c r="AE34">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="35" spans="1:32" x14ac:dyDescent="0.15">
       <c r="A35">
         <v>42040003</v>
       </c>
@@ -3755,14 +3788,15 @@
       <c r="I35" s="5"/>
       <c r="J35" s="5"/>
       <c r="K35" s="5"/>
-      <c r="AA35">
+      <c r="L35" s="5"/>
+      <c r="AB35">
         <v>100</v>
       </c>
-      <c r="AC35">
+      <c r="AD35">
         <v>100</v>
       </c>
     </row>
-    <row r="36" spans="1:31" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:32" x14ac:dyDescent="0.15">
       <c r="A36">
         <v>42040004</v>
       </c>
@@ -3790,14 +3824,15 @@
       <c r="I36" s="5"/>
       <c r="J36" s="5"/>
       <c r="K36" s="5"/>
-      <c r="V36">
-        <v>1</v>
-      </c>
-      <c r="AE36">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:31" x14ac:dyDescent="0.15">
+      <c r="L36" s="5"/>
+      <c r="W36">
+        <v>1</v>
+      </c>
+      <c r="AF36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:32" x14ac:dyDescent="0.15">
       <c r="A37">
         <v>42040005</v>
       </c>
@@ -3825,26 +3860,27 @@
       <c r="I37" s="5"/>
       <c r="J37" s="5"/>
       <c r="K37" s="5"/>
-      <c r="L37">
+      <c r="L37" s="5"/>
+      <c r="M37">
         <v>43000020</v>
       </c>
-      <c r="M37" t="s">
+      <c r="N37" t="s">
         <v>16</v>
-      </c>
-      <c r="O37">
-        <v>150</v>
       </c>
       <c r="P37">
         <v>150</v>
       </c>
-      <c r="AA37">
-        <v>200</v>
+      <c r="Q37">
+        <v>150</v>
       </c>
       <c r="AB37">
         <v>200</v>
       </c>
-    </row>
-    <row r="38" spans="1:31" x14ac:dyDescent="0.15">
+      <c r="AC37">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="38" spans="1:32" x14ac:dyDescent="0.15">
       <c r="A38">
         <v>42040006</v>
       </c>
@@ -3872,19 +3908,20 @@
       <c r="I38" s="5"/>
       <c r="J38" s="5"/>
       <c r="K38" s="5"/>
-      <c r="L38">
+      <c r="L38" s="5"/>
+      <c r="M38">
         <v>43000015</v>
       </c>
-      <c r="M38" t="s">
+      <c r="N38" t="s">
         <v>16</v>
       </c>
-      <c r="O38">
+      <c r="P38">
         <v>300</v>
       </c>
-      <c r="S38">
+      <c r="T38">
         <v>200</v>
       </c>
-      <c r="AC38">
+      <c r="AD38">
         <v>300</v>
       </c>
     </row>
@@ -3901,11 +3938,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AI24"/>
+  <dimension ref="A1:AJ24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J1" sqref="J1:K3"/>
+      <pane ySplit="3" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="Y21" sqref="Y21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -3914,18 +3951,19 @@
     <col min="3" max="5" width="3" customWidth="1"/>
     <col min="6" max="6" width="9.25" customWidth="1"/>
     <col min="9" max="11" width="5.5" customWidth="1"/>
-    <col min="12" max="12" width="9.75" customWidth="1"/>
-    <col min="13" max="13" width="6.625" customWidth="1"/>
-    <col min="14" max="14" width="9.25" customWidth="1"/>
-    <col min="15" max="19" width="4.125" customWidth="1"/>
-    <col min="20" max="20" width="9.75" customWidth="1"/>
-    <col min="21" max="21" width="7.5" customWidth="1"/>
-    <col min="22" max="22" width="5.125" customWidth="1"/>
-    <col min="23" max="26" width="9.375" customWidth="1"/>
-    <col min="28" max="36" width="5" customWidth="1"/>
+    <col min="12" max="12" width="8.75" customWidth="1"/>
+    <col min="13" max="13" width="9.75" customWidth="1"/>
+    <col min="14" max="14" width="6.625" customWidth="1"/>
+    <col min="15" max="15" width="9.25" customWidth="1"/>
+    <col min="16" max="20" width="4.125" customWidth="1"/>
+    <col min="21" max="21" width="9.75" customWidth="1"/>
+    <col min="22" max="22" width="7.5" customWidth="1"/>
+    <col min="23" max="23" width="5.125" customWidth="1"/>
+    <col min="24" max="27" width="9.375" customWidth="1"/>
+    <col min="29" max="37" width="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" ht="55.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:36" ht="69.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="14" t="s">
         <v>79</v>
       </c>
@@ -3960,79 +3998,82 @@
         <v>238</v>
       </c>
       <c r="L1" s="14" t="s">
+        <v>244</v>
+      </c>
+      <c r="M1" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="M1" s="14" t="s">
+      <c r="N1" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="N1" s="14" t="s">
+      <c r="O1" s="18" t="s">
         <v>210</v>
       </c>
-      <c r="O1" s="15" t="s">
+      <c r="P1" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="P1" s="15" t="s">
+      <c r="Q1" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="Q1" s="15" t="s">
+      <c r="R1" s="15" t="s">
         <v>84</v>
       </c>
-      <c r="R1" s="15" t="s">
+      <c r="S1" s="15" t="s">
         <v>85</v>
       </c>
-      <c r="S1" s="15" t="s">
+      <c r="T1" s="15" t="s">
         <v>86</v>
       </c>
-      <c r="T1" s="15" t="s">
+      <c r="U1" s="15" t="s">
         <v>87</v>
       </c>
-      <c r="U1" s="15" t="s">
+      <c r="V1" s="15" t="s">
         <v>77</v>
       </c>
-      <c r="V1" s="15" t="s">
+      <c r="W1" s="15" t="s">
         <v>200</v>
       </c>
-      <c r="W1" s="15" t="s">
+      <c r="X1" s="15" t="s">
         <v>137</v>
       </c>
-      <c r="X1" s="15" t="s">
+      <c r="Y1" s="15" t="s">
         <v>230</v>
       </c>
-      <c r="Y1" s="15" t="s">
+      <c r="Z1" s="15" t="s">
         <v>156</v>
       </c>
-      <c r="Z1" s="15" t="s">
+      <c r="AA1" s="15" t="s">
         <v>176</v>
       </c>
-      <c r="AA1" s="16" t="s">
+      <c r="AB1" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="AB1" s="16" t="s">
+      <c r="AC1" s="16" t="s">
         <v>88</v>
       </c>
-      <c r="AC1" s="16" t="s">
+      <c r="AD1" s="16" t="s">
         <v>78</v>
       </c>
-      <c r="AD1" s="16" t="s">
+      <c r="AE1" s="16" t="s">
         <v>89</v>
       </c>
-      <c r="AE1" s="16" t="s">
+      <c r="AF1" s="16" t="s">
         <v>200</v>
       </c>
-      <c r="AF1" s="17" t="s">
+      <c r="AG1" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="AG1" s="17" t="s">
+      <c r="AH1" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="AH1" s="17" t="s">
+      <c r="AI1" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="AI1" s="17" t="s">
+      <c r="AJ1" s="17" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>59</v>
       </c>
@@ -4067,22 +4108,22 @@
         <v>236</v>
       </c>
       <c r="L2" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="M2" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="N2" s="19" t="s">
+        <v>60</v>
+      </c>
+      <c r="O2" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="P2" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="M2" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>211</v>
-      </c>
-      <c r="O2" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="P2" s="7" t="s">
-        <v>0</v>
-      </c>
       <c r="Q2" s="7" t="s">
-        <v>59</v>
+        <v>0</v>
       </c>
       <c r="R2" s="7" t="s">
         <v>59</v>
@@ -4091,29 +4132,29 @@
         <v>59</v>
       </c>
       <c r="T2" s="7" t="s">
-        <v>0</v>
+        <v>59</v>
       </c>
       <c r="U2" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="V2" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="V2" s="7" t="s">
+      <c r="W2" s="7" t="s">
         <v>199</v>
       </c>
-      <c r="W2" s="7" t="s">
+      <c r="X2" s="7" t="s">
         <v>138</v>
       </c>
-      <c r="X2" s="7" t="s">
+      <c r="Y2" s="7" t="s">
         <v>231</v>
       </c>
-      <c r="Y2" s="7" t="s">
+      <c r="Z2" s="7" t="s">
         <v>157</v>
       </c>
-      <c r="Z2" s="7" t="s">
+      <c r="AA2" s="7" t="s">
         <v>177</v>
       </c>
-      <c r="AA2" s="3" t="s">
-        <v>0</v>
-      </c>
       <c r="AB2" s="3" t="s">
         <v>0</v>
       </c>
@@ -4121,13 +4162,13 @@
         <v>0</v>
       </c>
       <c r="AD2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="AE2" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="AE2" s="3" t="s">
+      <c r="AF2" s="3" t="s">
         <v>202</v>
-      </c>
-      <c r="AF2" s="9" t="s">
-        <v>27</v>
       </c>
       <c r="AG2" s="9" t="s">
         <v>27</v>
@@ -4138,8 +4179,11 @@
       <c r="AI2" s="9" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.15">
+      <c r="AJ2" s="9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A3" s="8" t="s">
         <v>64</v>
       </c>
@@ -4174,79 +4218,82 @@
         <v>239</v>
       </c>
       <c r="L3" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="M3" s="8" t="s">
+        <v>246</v>
+      </c>
+      <c r="M3" s="20" t="s">
+        <v>242</v>
+      </c>
+      <c r="N3" s="20" t="s">
         <v>70</v>
       </c>
-      <c r="N3" s="8" t="s">
-        <v>212</v>
-      </c>
-      <c r="O3" s="6" t="s">
+      <c r="O3" s="20" t="s">
+        <v>243</v>
+      </c>
+      <c r="P3" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="P3" s="6" t="s">
+      <c r="Q3" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="Q3" s="6" t="s">
+      <c r="R3" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="R3" s="6" t="s">
+      <c r="S3" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="S3" s="6" t="s">
+      <c r="T3" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="T3" s="6" t="s">
+      <c r="U3" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="U3" s="6" t="s">
+      <c r="V3" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="V3" s="6" t="s">
+      <c r="W3" s="6" t="s">
         <v>198</v>
       </c>
-      <c r="W3" s="6" t="s">
+      <c r="X3" s="6" t="s">
         <v>139</v>
       </c>
-      <c r="X3" s="6" t="s">
+      <c r="Y3" s="6" t="s">
         <v>232</v>
       </c>
-      <c r="Y3" s="6" t="s">
+      <c r="Z3" s="6" t="s">
         <v>159</v>
       </c>
-      <c r="Z3" s="6" t="s">
+      <c r="AA3" s="6" t="s">
         <v>178</v>
       </c>
-      <c r="AA3" s="2" t="s">
+      <c r="AB3" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="AB3" s="2" t="s">
+      <c r="AC3" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="AC3" s="2" t="s">
+      <c r="AD3" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="AD3" s="2" t="s">
+      <c r="AE3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="AE3" s="2" t="s">
+      <c r="AF3" s="2" t="s">
         <v>203</v>
       </c>
-      <c r="AF3" s="8" t="s">
+      <c r="AG3" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="AG3" s="8" t="s">
+      <c r="AH3" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="AH3" s="8" t="s">
+      <c r="AI3" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="AI3" s="8" t="s">
+      <c r="AJ3" s="8" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A4" s="10">
         <v>42020001</v>
       </c>
@@ -4273,19 +4320,20 @@
       </c>
       <c r="J4" s="5"/>
       <c r="K4" s="5"/>
-      <c r="M4" s="11"/>
-      <c r="N4" s="13"/>
-      <c r="AF4">
+      <c r="L4" s="5"/>
+      <c r="N4" s="11"/>
+      <c r="O4" s="13"/>
+      <c r="AG4">
         <v>-300</v>
-      </c>
-      <c r="AH4">
-        <v>1000</v>
       </c>
       <c r="AI4">
         <v>1000</v>
       </c>
-    </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.15">
+      <c r="AJ4">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A5" s="10">
         <v>42020002</v>
       </c>
@@ -4312,16 +4360,17 @@
       </c>
       <c r="J5" s="5"/>
       <c r="K5" s="5"/>
-      <c r="M5" s="11"/>
-      <c r="N5" s="13"/>
-      <c r="AF5">
+      <c r="L5" s="5"/>
+      <c r="N5" s="11"/>
+      <c r="O5" s="13"/>
+      <c r="AG5">
         <v>-200</v>
       </c>
-      <c r="AG5">
+      <c r="AH5">
         <v>1000</v>
       </c>
     </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A6" s="10">
         <v>42020003</v>
       </c>
@@ -4348,10 +4397,11 @@
       </c>
       <c r="J6" s="5"/>
       <c r="K6" s="5"/>
-      <c r="M6" s="11"/>
-      <c r="N6" s="13"/>
-    </row>
-    <row r="7" spans="1:35" x14ac:dyDescent="0.15">
+      <c r="L6" s="5"/>
+      <c r="N6" s="11"/>
+      <c r="O6" s="13"/>
+    </row>
+    <row r="7" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A7" s="10">
         <v>42020004</v>
       </c>
@@ -4378,8 +4428,9 @@
       </c>
       <c r="J7" s="5"/>
       <c r="K7" s="5"/>
-    </row>
-    <row r="8" spans="1:35" x14ac:dyDescent="0.15">
+      <c r="L7" s="5"/>
+    </row>
+    <row r="8" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A8" s="10">
         <v>42020005</v>
       </c>
@@ -4406,10 +4457,11 @@
       </c>
       <c r="J8" s="5"/>
       <c r="K8" s="5"/>
-      <c r="M8" s="11"/>
-      <c r="N8" s="13"/>
-    </row>
-    <row r="9" spans="1:35" x14ac:dyDescent="0.15">
+      <c r="L8" s="5"/>
+      <c r="N8" s="11"/>
+      <c r="O8" s="13"/>
+    </row>
+    <row r="9" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A9">
         <v>42030001</v>
       </c>
@@ -4429,23 +4481,26 @@
         <v>19</v>
       </c>
       <c r="H9" t="s">
-        <v>19</v>
+        <v>247</v>
       </c>
       <c r="I9" s="5" t="s">
         <v>18</v>
       </c>
       <c r="J9" s="5"/>
       <c r="K9" s="5"/>
-      <c r="M9" s="4"/>
-      <c r="N9" s="12"/>
-      <c r="O9">
+      <c r="L9">
+        <v>12000001</v>
+      </c>
+      <c r="N9" s="4"/>
+      <c r="O9" s="12"/>
+      <c r="P9">
         <v>50</v>
       </c>
-      <c r="X9">
+      <c r="Y9">
         <v>12000001</v>
       </c>
     </row>
-    <row r="10" spans="1:35" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A10">
         <v>42030002</v>
       </c>
@@ -4459,7 +4514,7 @@
         <v>0</v>
       </c>
       <c r="F10" t="s">
-        <v>21</v>
+        <v>240</v>
       </c>
       <c r="G10" t="s">
         <v>21</v>
@@ -4473,17 +4528,20 @@
       <c r="J10" s="5"/>
       <c r="K10" s="5"/>
       <c r="L10">
+        <v>12000001</v>
+      </c>
+      <c r="M10">
         <v>43020101</v>
       </c>
-      <c r="M10" s="12" t="s">
+      <c r="N10" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="N10" s="12"/>
-      <c r="W10">
+      <c r="O10" s="12"/>
+      <c r="X10">
         <v>43020101</v>
       </c>
     </row>
-    <row r="11" spans="1:35" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A11">
         <v>42030003</v>
       </c>
@@ -4510,10 +4568,11 @@
       </c>
       <c r="J11" s="5"/>
       <c r="K11" s="5"/>
-      <c r="M11" s="12"/>
+      <c r="L11" s="5"/>
       <c r="N11" s="12"/>
-    </row>
-    <row r="12" spans="1:35" x14ac:dyDescent="0.15">
+      <c r="O11" s="12"/>
+    </row>
+    <row r="12" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A12">
         <v>42030004</v>
       </c>
@@ -4540,16 +4599,17 @@
       </c>
       <c r="J12" s="5"/>
       <c r="K12" s="5"/>
-      <c r="M12" s="12"/>
+      <c r="L12" s="5"/>
       <c r="N12" s="12"/>
-      <c r="W12">
+      <c r="O12" s="12"/>
+      <c r="X12">
         <v>43020102</v>
       </c>
-      <c r="Y12" t="s">
+      <c r="Z12" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="13" spans="1:35" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A13">
         <v>42030005</v>
       </c>
@@ -4576,25 +4636,26 @@
       </c>
       <c r="J13" s="5"/>
       <c r="K13" s="5"/>
-      <c r="M13" s="12"/>
+      <c r="L13" s="5"/>
       <c r="N13" s="12"/>
-      <c r="O13">
+      <c r="O13" s="12"/>
+      <c r="P13">
         <v>300</v>
       </c>
-      <c r="P13">
+      <c r="Q13">
         <v>200</v>
       </c>
-      <c r="T13">
+      <c r="U13">
         <v>22031011</v>
       </c>
-      <c r="Y13" t="s">
+      <c r="Z13" t="s">
         <v>175</v>
       </c>
-      <c r="Z13">
+      <c r="AA13">
         <v>42030012</v>
       </c>
     </row>
-    <row r="14" spans="1:35" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A14">
         <v>42030006</v>
       </c>
@@ -4621,10 +4682,11 @@
       </c>
       <c r="J14" s="5"/>
       <c r="K14" s="5"/>
-      <c r="M14" s="12"/>
+      <c r="L14" s="5"/>
       <c r="N14" s="12"/>
-    </row>
-    <row r="15" spans="1:35" x14ac:dyDescent="0.15">
+      <c r="O14" s="12"/>
+    </row>
+    <row r="15" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A15">
         <v>42030007</v>
       </c>
@@ -4651,10 +4713,11 @@
       </c>
       <c r="J15" s="5"/>
       <c r="K15" s="5"/>
-      <c r="M15" s="12"/>
+      <c r="L15" s="5"/>
       <c r="N15" s="12"/>
-    </row>
-    <row r="16" spans="1:35" x14ac:dyDescent="0.15">
+      <c r="O15" s="12"/>
+    </row>
+    <row r="16" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A16">
         <v>42030008</v>
       </c>
@@ -4681,10 +4744,11 @@
       </c>
       <c r="J16" s="5"/>
       <c r="K16" s="5"/>
-      <c r="M16" s="12"/>
+      <c r="L16" s="5"/>
       <c r="N16" s="12"/>
-    </row>
-    <row r="17" spans="1:30" x14ac:dyDescent="0.15">
+      <c r="O16" s="12"/>
+    </row>
+    <row r="17" spans="1:31" x14ac:dyDescent="0.15">
       <c r="A17">
         <v>42030009</v>
       </c>
@@ -4711,10 +4775,11 @@
       </c>
       <c r="J17" s="5"/>
       <c r="K17" s="5"/>
-      <c r="M17" s="12"/>
+      <c r="L17" s="5"/>
       <c r="N17" s="12"/>
-    </row>
-    <row r="18" spans="1:30" x14ac:dyDescent="0.15">
+      <c r="O17" s="12"/>
+    </row>
+    <row r="18" spans="1:31" x14ac:dyDescent="0.15">
       <c r="A18">
         <v>42030010</v>
       </c>
@@ -4741,10 +4806,11 @@
       </c>
       <c r="J18" s="5"/>
       <c r="K18" s="5"/>
-      <c r="M18" s="12"/>
+      <c r="L18" s="5"/>
       <c r="N18" s="12"/>
-    </row>
-    <row r="19" spans="1:30" x14ac:dyDescent="0.15">
+      <c r="O18" s="12"/>
+    </row>
+    <row r="19" spans="1:31" x14ac:dyDescent="0.15">
       <c r="A19">
         <v>42030011</v>
       </c>
@@ -4771,10 +4837,11 @@
       </c>
       <c r="J19" s="5"/>
       <c r="K19" s="5"/>
-      <c r="M19" s="12"/>
+      <c r="L19" s="5"/>
       <c r="N19" s="12"/>
-    </row>
-    <row r="20" spans="1:30" x14ac:dyDescent="0.15">
+      <c r="O19" s="12"/>
+    </row>
+    <row r="20" spans="1:31" x14ac:dyDescent="0.15">
       <c r="A20">
         <v>42030012</v>
       </c>
@@ -4801,18 +4868,19 @@
       </c>
       <c r="J20" s="5"/>
       <c r="K20" s="5"/>
-      <c r="L20">
+      <c r="L20" s="5"/>
+      <c r="M20">
         <v>43020105</v>
       </c>
-      <c r="M20" s="12" t="s">
+      <c r="N20" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="N20" s="12"/>
-      <c r="W20">
+      <c r="O20" s="12"/>
+      <c r="X20">
         <v>43020105</v>
       </c>
     </row>
-    <row r="21" spans="1:30" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:31" x14ac:dyDescent="0.15">
       <c r="A21">
         <v>42050001</v>
       </c>
@@ -4839,12 +4907,15 @@
       </c>
       <c r="J21" s="5"/>
       <c r="K21" s="5"/>
-      <c r="M21" s="12"/>
-      <c r="N21" s="12">
+      <c r="L21">
+        <v>12000001</v>
+      </c>
+      <c r="N21" s="12"/>
+      <c r="O21" s="12">
         <v>13020001</v>
       </c>
     </row>
-    <row r="22" spans="1:30" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:31" x14ac:dyDescent="0.15">
       <c r="A22">
         <v>42050002</v>
       </c>
@@ -4864,19 +4935,20 @@
         <v>213</v>
       </c>
       <c r="H22" t="s">
-        <v>214</v>
+        <v>241</v>
       </c>
       <c r="I22" s="5" t="s">
         <v>18</v>
       </c>
       <c r="J22" s="5"/>
       <c r="K22" s="5"/>
-      <c r="M22" s="12"/>
-      <c r="N22" s="12">
+      <c r="L22" s="5"/>
+      <c r="N22" s="12"/>
+      <c r="O22" s="12">
         <v>13020002</v>
       </c>
     </row>
-    <row r="23" spans="1:30" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:31" x14ac:dyDescent="0.15">
       <c r="A23">
         <v>42050003</v>
       </c>
@@ -4906,20 +4978,18 @@
       </c>
       <c r="J23" s="5"/>
       <c r="K23" s="5"/>
-      <c r="L23">
+      <c r="L23" s="5"/>
+      <c r="M23">
         <v>43000019</v>
       </c>
-      <c r="M23" s="12" t="s">
+      <c r="N23" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="N23" s="12">
+      <c r="O23" s="12">
         <v>13010002</v>
       </c>
-      <c r="O23">
+      <c r="P23">
         <v>300</v>
-      </c>
-      <c r="P23">
-        <v>500</v>
       </c>
       <c r="Q23">
         <v>500</v>
@@ -4928,19 +4998,25 @@
         <v>500</v>
       </c>
       <c r="S23">
+        <v>500</v>
+      </c>
+      <c r="T23">
         <v>300</v>
       </c>
-      <c r="Y23" t="s">
+      <c r="Y23">
+        <v>12000002</v>
+      </c>
+      <c r="Z23" t="s">
         <v>218</v>
-      </c>
-      <c r="AC23">
-        <v>200</v>
       </c>
       <c r="AD23">
         <v>200</v>
       </c>
-    </row>
-    <row r="24" spans="1:30" x14ac:dyDescent="0.15">
+      <c r="AE23">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="24" spans="1:31" x14ac:dyDescent="0.15">
       <c r="A24">
         <v>42050004</v>
       </c>
@@ -4967,8 +5043,9 @@
       </c>
       <c r="J24" s="5"/>
       <c r="K24" s="5"/>
-      <c r="M24" s="12"/>
-      <c r="N24" s="12">
+      <c r="L24" s="5"/>
+      <c r="N24" s="12"/>
+      <c r="O24" s="12">
         <v>13020011</v>
       </c>
     </row>

</xml_diff>

<commit_message>
setup the clue of npc
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/SceneQuest.xlsx
+++ b/ConfigData/Xlsx/SceneQuest.xlsx
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="489" uniqueCount="253">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="499" uniqueCount="257">
   <si>
     <t>int</t>
     <phoneticPr fontId="18" type="noConversion"/>
@@ -991,6 +991,20 @@
   </si>
   <si>
     <t>小男孩</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>npccunfu</t>
+  </si>
+  <si>
+    <t>npclaozhe</t>
+  </si>
+  <si>
+    <t>村长</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>玛莎</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -1995,8 +2009,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="表3_5" displayName="表3_5" ref="A3:AJ25" totalsRowShown="0" headerRowDxfId="6">
-  <autoFilter ref="A3:AJ25"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="表3_5" displayName="表3_5" ref="A3:AJ27" totalsRowShown="0" headerRowDxfId="6">
+  <autoFilter ref="A3:AJ27"/>
   <sortState ref="A4:Z6">
     <sortCondition ref="A3:A6"/>
   </sortState>
@@ -4031,11 +4045,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AJ25"/>
+  <dimension ref="A1:AJ27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L21" sqref="L21"/>
+      <selection pane="bottomLeft" activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -5027,10 +5041,10 @@
     </row>
     <row r="22" spans="1:31" x14ac:dyDescent="0.15">
       <c r="A22">
-        <v>42050001</v>
+        <v>42030014</v>
       </c>
       <c r="B22" t="s">
-        <v>208</v>
+        <v>256</v>
       </c>
       <c r="C22" s="10">
         <v>2</v>
@@ -5039,34 +5053,32 @@
         <v>0</v>
       </c>
       <c r="F22" t="s">
-        <v>212</v>
+        <v>253</v>
       </c>
       <c r="G22" t="s">
-        <v>212</v>
+        <v>253</v>
       </c>
       <c r="H22" t="s">
-        <v>213</v>
+        <v>253</v>
       </c>
       <c r="I22" s="5" t="s">
         <v>18</v>
       </c>
       <c r="J22" s="5"/>
       <c r="K22" s="5"/>
-      <c r="L22">
-        <v>12000001</v>
+      <c r="L22" s="21">
+        <v>12000002</v>
       </c>
       <c r="N22" s="12"/>
-      <c r="O22" s="12">
-        <v>13020001</v>
-      </c>
+      <c r="O22" s="12"/>
       <c r="AA22" s="5"/>
     </row>
     <row r="23" spans="1:31" x14ac:dyDescent="0.15">
       <c r="A23">
-        <v>42050002</v>
-      </c>
-      <c r="B23" t="s">
-        <v>208</v>
+        <v>42030015</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>255</v>
       </c>
       <c r="C23" s="10">
         <v>2</v>
@@ -5075,32 +5087,32 @@
         <v>0</v>
       </c>
       <c r="F23" t="s">
-        <v>214</v>
+        <v>254</v>
       </c>
       <c r="G23" t="s">
-        <v>212</v>
+        <v>254</v>
       </c>
       <c r="H23" t="s">
-        <v>240</v>
+        <v>254</v>
       </c>
       <c r="I23" s="5" t="s">
         <v>18</v>
       </c>
       <c r="J23" s="5"/>
       <c r="K23" s="5"/>
-      <c r="L23" s="5"/>
+      <c r="L23" s="21">
+        <v>12000002</v>
+      </c>
       <c r="N23" s="12"/>
-      <c r="O23" s="12">
-        <v>13020002</v>
-      </c>
+      <c r="O23" s="12"/>
       <c r="AA23" s="5"/>
     </row>
     <row r="24" spans="1:31" x14ac:dyDescent="0.15">
       <c r="A24">
-        <v>42050003</v>
+        <v>42050001</v>
       </c>
       <c r="B24" t="s">
-        <v>216</v>
+        <v>208</v>
       </c>
       <c r="C24" s="10">
         <v>2</v>
@@ -5108,70 +5120,35 @@
       <c r="D24">
         <v>0</v>
       </c>
-      <c r="E24">
-        <v>3</v>
-      </c>
       <c r="F24" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="G24" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="H24" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="I24" s="5" t="s">
         <v>18</v>
       </c>
       <c r="J24" s="5"/>
       <c r="K24" s="5"/>
-      <c r="L24" s="5"/>
-      <c r="M24">
-        <v>43000019</v>
-      </c>
-      <c r="N24" s="12" t="s">
-        <v>16</v>
-      </c>
+      <c r="L24">
+        <v>12000001</v>
+      </c>
+      <c r="N24" s="12"/>
       <c r="O24" s="12">
-        <v>13010002</v>
-      </c>
-      <c r="P24">
-        <v>300</v>
-      </c>
-      <c r="Q24">
-        <v>500</v>
-      </c>
-      <c r="R24">
-        <v>500</v>
-      </c>
-      <c r="S24">
-        <v>500</v>
-      </c>
-      <c r="T24">
-        <v>300</v>
-      </c>
-      <c r="Y24">
-        <v>12000002</v>
-      </c>
-      <c r="Z24" t="s">
-        <v>217</v>
-      </c>
-      <c r="AA24" s="5" t="s">
-        <v>251</v>
-      </c>
-      <c r="AD24">
-        <v>200</v>
-      </c>
-      <c r="AE24">
-        <v>200</v>
-      </c>
+        <v>13020001</v>
+      </c>
+      <c r="AA24" s="5"/>
     </row>
     <row r="25" spans="1:31" x14ac:dyDescent="0.15">
       <c r="A25">
-        <v>42050004</v>
+        <v>42050002</v>
       </c>
       <c r="B25" t="s">
-        <v>233</v>
+        <v>208</v>
       </c>
       <c r="C25" s="10">
         <v>2</v>
@@ -5180,13 +5157,13 @@
         <v>0</v>
       </c>
       <c r="F25" t="s">
-        <v>232</v>
+        <v>214</v>
       </c>
       <c r="G25" t="s">
-        <v>232</v>
+        <v>212</v>
       </c>
       <c r="H25" t="s">
-        <v>213</v>
+        <v>240</v>
       </c>
       <c r="I25" s="5" t="s">
         <v>18</v>
@@ -5196,9 +5173,114 @@
       <c r="L25" s="5"/>
       <c r="N25" s="12"/>
       <c r="O25" s="12">
+        <v>13020002</v>
+      </c>
+      <c r="AA25" s="5"/>
+    </row>
+    <row r="26" spans="1:31" x14ac:dyDescent="0.15">
+      <c r="A26">
+        <v>42050003</v>
+      </c>
+      <c r="B26" t="s">
+        <v>216</v>
+      </c>
+      <c r="C26" s="10">
+        <v>2</v>
+      </c>
+      <c r="D26">
+        <v>0</v>
+      </c>
+      <c r="E26">
+        <v>3</v>
+      </c>
+      <c r="F26" t="s">
+        <v>215</v>
+      </c>
+      <c r="G26" t="s">
+        <v>215</v>
+      </c>
+      <c r="H26" t="s">
+        <v>215</v>
+      </c>
+      <c r="I26" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="J26" s="5"/>
+      <c r="K26" s="5"/>
+      <c r="L26" s="5"/>
+      <c r="M26">
+        <v>43000019</v>
+      </c>
+      <c r="N26" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="O26" s="12">
+        <v>13010002</v>
+      </c>
+      <c r="P26">
+        <v>300</v>
+      </c>
+      <c r="Q26">
+        <v>500</v>
+      </c>
+      <c r="R26">
+        <v>500</v>
+      </c>
+      <c r="S26">
+        <v>500</v>
+      </c>
+      <c r="T26">
+        <v>300</v>
+      </c>
+      <c r="Y26">
+        <v>12000002</v>
+      </c>
+      <c r="Z26" t="s">
+        <v>217</v>
+      </c>
+      <c r="AA26" s="5" t="s">
+        <v>251</v>
+      </c>
+      <c r="AD26">
+        <v>200</v>
+      </c>
+      <c r="AE26">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="27" spans="1:31" x14ac:dyDescent="0.15">
+      <c r="A27">
+        <v>42050004</v>
+      </c>
+      <c r="B27" t="s">
+        <v>233</v>
+      </c>
+      <c r="C27" s="10">
+        <v>2</v>
+      </c>
+      <c r="D27">
+        <v>0</v>
+      </c>
+      <c r="F27" t="s">
+        <v>232</v>
+      </c>
+      <c r="G27" t="s">
+        <v>232</v>
+      </c>
+      <c r="H27" t="s">
+        <v>213</v>
+      </c>
+      <c r="I27" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="J27" s="5"/>
+      <c r="K27" s="5"/>
+      <c r="L27" s="5"/>
+      <c r="N27" s="12"/>
+      <c r="O27" s="12">
         <v>13020011</v>
       </c>
-      <c r="AA25" s="5"/>
+      <c r="AA27" s="5"/>
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>

</xml_diff>

<commit_message>
finish a duplicate scenequest system
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/SceneQuest.xlsx
+++ b/ConfigData/Xlsx/SceneQuest.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Code\TOMClassicGit\ConfigData\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\TOMClassicGit\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="535" uniqueCount="274">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="527" uniqueCount="268">
   <si>
     <t>int</t>
     <phoneticPr fontId="18" type="noConversion"/>
@@ -692,14 +692,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>替换</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>ReplaceId</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>hiddeway</t>
   </si>
   <si>
@@ -931,154 +923,138 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
+    <t>npcsainisi</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>dungeonentry</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>EnemyId</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>SceneId</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>任务要求</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>int</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>QuestNeed</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>npcqiaosiji</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>npckid1</t>
+  </si>
+  <si>
+    <t>小男孩</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>npccunfu</t>
+  </si>
+  <si>
+    <t>npclaozhe</t>
+  </si>
+  <si>
+    <t>村长</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>玛莎</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>npclaozhe</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>cliff</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>绝壁</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>colorpool</t>
+  </si>
+  <si>
+    <t>七彩池</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>废弃谷仓</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>barn</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>string</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>标记没有时</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>标记有时</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>npcsaibasi</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Qiaqia</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>AolaiFight</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>woodhouse</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>木屋</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>npcwoodhouse</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
     <t>TriggerHourEnd</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>npcsainisi</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>dungeonentry</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>EnemyId</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>SceneId</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>任务要求</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>int</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>QuestNeed</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>npcqiaosiji</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>npckid1</t>
-  </si>
-  <si>
-    <t>ReplaceId</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>int[]</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>42030005,42030010</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>42030002,42030013</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>小男孩</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>npccunfu</t>
-  </si>
-  <si>
-    <t>npclaozhe</t>
-  </si>
-  <si>
-    <t>村长</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>玛莎</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>npclaozhe</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>cliff</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>绝壁</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>colorpool</t>
-  </si>
-  <si>
-    <t>七彩池</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>废弃谷仓</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>barn</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>string</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>标记没有时</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>TiggerFlagNoExist</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>TiggerFlagExist</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>标记有时</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>npcsaibasi</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>Qiaqia</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>AolaiFight</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>woodhouse</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>木屋</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>npcwoodhouse</t>
+    <t>TriggerFlagNoExist</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>TriggerFlagExist</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1901,10 +1877,7 @@
     <cellStyle name="着色 6" xfId="38" builtinId="49" customBuiltin="1"/>
     <cellStyle name="注释" xfId="15" builtinId="10" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="16">
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
+  <dxfs count="15">
     <dxf>
       <font>
         <b val="0"/>
@@ -1993,12 +1966,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="表3" displayName="表3" ref="A3:AL41" totalsRowShown="0" headerRowDxfId="15">
-  <autoFilter ref="A3:AL41"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="表3" displayName="表3" ref="A3:AK41" totalsRowShown="0" headerRowDxfId="14">
+  <autoFilter ref="A3:AK41"/>
   <sortState ref="A4:AD28">
     <sortCondition ref="A3:A28"/>
   </sortState>
-  <tableColumns count="38">
+  <tableColumns count="37">
     <tableColumn id="1" name="Id"/>
     <tableColumn id="2" name="Name"/>
     <tableColumn id="28" name="Type"/>
@@ -2007,12 +1980,12 @@
     <tableColumn id="24" name="Ename"/>
     <tableColumn id="4" name="Figue"/>
     <tableColumn id="5" name="Script"/>
-    <tableColumn id="6" name="TriggerMulti" dataDxfId="14"/>
-    <tableColumn id="35" name="TriggerHourBegin" dataDxfId="13"/>
-    <tableColumn id="34" name="TriggerHourEnd" dataDxfId="12"/>
-    <tableColumn id="36" name="TiggerFlagNoExist" dataDxfId="11"/>
-    <tableColumn id="38" name="TiggerFlagExist" dataDxfId="10"/>
-    <tableColumn id="37" name="QuestNeed" dataDxfId="9"/>
+    <tableColumn id="6" name="TriggerMulti" dataDxfId="13"/>
+    <tableColumn id="35" name="TriggerHourBegin" dataDxfId="12"/>
+    <tableColumn id="34" name="TriggerHourEnd" dataDxfId="11"/>
+    <tableColumn id="36" name="TriggerFlagNoExist" dataDxfId="10"/>
+    <tableColumn id="38" name="TriggerFlagExist" dataDxfId="9"/>
+    <tableColumn id="37" name="QuestNeed" dataDxfId="8"/>
     <tableColumn id="7" name="EnemyId"/>
     <tableColumn id="8" name="BattleMap"/>
     <tableColumn id="32" name="SceneId"/>
@@ -2027,7 +2000,6 @@
     <tableColumn id="26" name="RivalId"/>
     <tableColumn id="33" name="QuestId"/>
     <tableColumn id="27" name="Flag"/>
-    <tableColumn id="29" name="ReplaceId"/>
     <tableColumn id="16" name="PunishGold"/>
     <tableColumn id="17" name="PunishFood"/>
     <tableColumn id="18" name="PunishHealth"/>
@@ -2043,29 +2015,29 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="表3_5" displayName="表3_5" ref="A3:AL28" totalsRowShown="0" headerRowDxfId="8">
-  <autoFilter ref="A3:AL28"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="表3_5" displayName="表3_5" ref="A3:AK28" totalsRowShown="0" headerRowDxfId="7">
+  <autoFilter ref="A3:AK28"/>
   <sortState ref="A4:Z6">
     <sortCondition ref="A3:A6"/>
   </sortState>
-  <tableColumns count="38">
+  <tableColumns count="37">
     <tableColumn id="1" name="Id"/>
     <tableColumn id="2" name="Name"/>
-    <tableColumn id="27" name="Type" dataDxfId="7"/>
+    <tableColumn id="27" name="Type" dataDxfId="6"/>
     <tableColumn id="3" name="Level"/>
     <tableColumn id="25" name="Danger"/>
     <tableColumn id="24" name="Ename"/>
     <tableColumn id="4" name="Figue"/>
     <tableColumn id="5" name="Script"/>
     <tableColumn id="6" name="TriggerMulti"/>
-    <tableColumn id="35" name="TriggerHourBegin" dataDxfId="6"/>
-    <tableColumn id="34" name="TriggerHourEnd" dataDxfId="5"/>
-    <tableColumn id="37" name="TiggerFlagNoExist" dataDxfId="4"/>
-    <tableColumn id="38" name="TiggerFlagExist" dataDxfId="3"/>
-    <tableColumn id="36" name="QuestNeed" dataDxfId="2"/>
+    <tableColumn id="35" name="TriggerHourBegin" dataDxfId="5"/>
+    <tableColumn id="34" name="TriggerHourEnd" dataDxfId="4"/>
+    <tableColumn id="37" name="TriggerFlagNoExist" dataDxfId="3"/>
+    <tableColumn id="38" name="TriggerFlagExist" dataDxfId="2"/>
+    <tableColumn id="36" name="QuestNeed" dataDxfId="1"/>
     <tableColumn id="7" name="EnemyId"/>
     <tableColumn id="8" name="BattleMap"/>
-    <tableColumn id="32" name="SceneId" dataDxfId="1"/>
+    <tableColumn id="32" name="SceneId" dataDxfId="0"/>
     <tableColumn id="9" name="RewardGold"/>
     <tableColumn id="10" name="RewardFood"/>
     <tableColumn id="11" name="RewardHealth"/>
@@ -2077,7 +2049,6 @@
     <tableColumn id="26" name="RivalId"/>
     <tableColumn id="33" name="QuestId"/>
     <tableColumn id="28" name="Flag"/>
-    <tableColumn id="29" name="ReplaceId" dataDxfId="0"/>
     <tableColumn id="16" name="PunishGold"/>
     <tableColumn id="17" name="PunishFood"/>
     <tableColumn id="18" name="PunishHealth"/>
@@ -2093,7 +2064,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -2379,11 +2350,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AL41"/>
+  <dimension ref="A1:AK41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M1" sqref="M1"/>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J3" sqref="J3:M3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -2399,11 +2370,11 @@
     <col min="23" max="24" width="9.375" customWidth="1"/>
     <col min="25" max="25" width="4.25" customWidth="1"/>
     <col min="26" max="27" width="9.375" customWidth="1"/>
-    <col min="28" max="29" width="4.25" customWidth="1"/>
-    <col min="31" max="39" width="4.75" customWidth="1"/>
+    <col min="28" max="28" width="4.25" customWidth="1"/>
+    <col min="30" max="38" width="4.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:38" ht="69" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:37" ht="69" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="14" t="s">
         <v>79</v>
       </c>
@@ -2432,19 +2403,19 @@
         <v>83</v>
       </c>
       <c r="J1" s="22" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="K1" s="22" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="L1" s="22" t="s">
-        <v>264</v>
+        <v>257</v>
       </c>
       <c r="M1" s="22" t="s">
-        <v>267</v>
+        <v>258</v>
       </c>
       <c r="N1" s="14" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="O1" s="18" t="s">
         <v>2</v>
@@ -2453,7 +2424,7 @@
         <v>15</v>
       </c>
       <c r="Q1" s="18" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="R1" s="15" t="s">
         <v>3</v>
@@ -2477,49 +2448,46 @@
         <v>77</v>
       </c>
       <c r="Y1" s="15" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="Z1" s="15" t="s">
         <v>137</v>
       </c>
       <c r="AA1" s="15" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="AB1" s="15" t="s">
         <v>156</v>
       </c>
-      <c r="AC1" s="15" t="s">
-        <v>175</v>
+      <c r="AC1" s="16" t="s">
+        <v>5</v>
       </c>
       <c r="AD1" s="16" t="s">
-        <v>5</v>
+        <v>88</v>
       </c>
       <c r="AE1" s="16" t="s">
-        <v>88</v>
+        <v>78</v>
       </c>
       <c r="AF1" s="16" t="s">
-        <v>78</v>
+        <v>89</v>
       </c>
       <c r="AG1" s="16" t="s">
-        <v>89</v>
-      </c>
-      <c r="AH1" s="16" t="s">
-        <v>199</v>
+        <v>197</v>
+      </c>
+      <c r="AH1" s="17" t="s">
+        <v>28</v>
       </c>
       <c r="AI1" s="17" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="AJ1" s="17" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="AK1" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="AL1" s="17" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:38" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:37" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>59</v>
       </c>
@@ -2554,13 +2522,13 @@
         <v>0</v>
       </c>
       <c r="L2" s="23" t="s">
-        <v>263</v>
+        <v>256</v>
       </c>
       <c r="M2" s="23" t="s">
-        <v>263</v>
+        <v>256</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="O2" s="19" t="s">
         <v>59</v>
@@ -2569,7 +2537,7 @@
         <v>63</v>
       </c>
       <c r="Q2" s="19" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="R2" s="7" t="s">
         <v>59</v>
@@ -2593,19 +2561,19 @@
         <v>59</v>
       </c>
       <c r="Y2" s="7" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="Z2" s="7" t="s">
         <v>138</v>
       </c>
       <c r="AA2" s="7" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="AB2" s="7" t="s">
         <v>157</v>
       </c>
-      <c r="AC2" s="7" t="s">
-        <v>248</v>
+      <c r="AC2" s="3" t="s">
+        <v>0</v>
       </c>
       <c r="AD2" s="3" t="s">
         <v>0</v>
@@ -2614,13 +2582,13 @@
         <v>0</v>
       </c>
       <c r="AF2" s="3" t="s">
-        <v>0</v>
+        <v>59</v>
       </c>
       <c r="AG2" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="AH2" s="3" t="s">
-        <v>200</v>
+        <v>198</v>
+      </c>
+      <c r="AH2" s="9" t="s">
+        <v>27</v>
       </c>
       <c r="AI2" s="9" t="s">
         <v>27</v>
@@ -2631,11 +2599,8 @@
       <c r="AK2" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="AL2" s="9" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="3" spans="1:38" x14ac:dyDescent="0.15">
+    </row>
+    <row r="3" spans="1:37" x14ac:dyDescent="0.15">
       <c r="A3" s="8" t="s">
         <v>64</v>
       </c>
@@ -2664,19 +2629,19 @@
         <v>17</v>
       </c>
       <c r="J3" s="24" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="K3" s="24" t="s">
-        <v>237</v>
+        <v>265</v>
       </c>
       <c r="L3" s="24" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="M3" s="24" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="N3" s="8" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="O3" s="20" t="s">
         <v>69</v>
@@ -2685,7 +2650,7 @@
         <v>70</v>
       </c>
       <c r="Q3" s="20" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="R3" s="6" t="s">
         <v>71</v>
@@ -2709,49 +2674,46 @@
         <v>35</v>
       </c>
       <c r="Y3" s="6" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="Z3" s="6" t="s">
         <v>139</v>
       </c>
       <c r="AA3" s="6" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="AB3" s="6" t="s">
         <v>158</v>
       </c>
-      <c r="AC3" s="6" t="s">
-        <v>176</v>
+      <c r="AC3" s="2" t="s">
+        <v>75</v>
       </c>
       <c r="AD3" s="2" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="AE3" s="2" t="s">
-        <v>76</v>
+        <v>36</v>
       </c>
       <c r="AF3" s="2" t="s">
-        <v>36</v>
+        <v>8</v>
       </c>
       <c r="AG3" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="AH3" s="2" t="s">
-        <v>201</v>
+        <v>199</v>
+      </c>
+      <c r="AH3" s="8" t="s">
+        <v>23</v>
       </c>
       <c r="AI3" s="8" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="AJ3" s="8" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="AK3" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="AL3" s="8" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:38" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:37" x14ac:dyDescent="0.15">
       <c r="A4">
         <v>42000001</v>
       </c>
@@ -2806,6 +2768,9 @@
       <c r="W4">
         <v>22011180</v>
       </c>
+      <c r="AC4">
+        <v>100</v>
+      </c>
       <c r="AD4">
         <v>100</v>
       </c>
@@ -2815,11 +2780,8 @@
       <c r="AF4">
         <v>100</v>
       </c>
-      <c r="AG4">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="5" spans="1:38" x14ac:dyDescent="0.15">
+    </row>
+    <row r="5" spans="1:37" x14ac:dyDescent="0.15">
       <c r="A5" s="10">
         <v>42000002</v>
       </c>
@@ -2848,7 +2810,7 @@
       <c r="M5" s="5"/>
       <c r="N5" s="5"/>
     </row>
-    <row r="6" spans="1:38" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:37" x14ac:dyDescent="0.15">
       <c r="A6" s="10">
         <v>42000003</v>
       </c>
@@ -2877,7 +2839,7 @@
       <c r="M6" s="5"/>
       <c r="N6" s="5"/>
     </row>
-    <row r="7" spans="1:38" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:37" x14ac:dyDescent="0.15">
       <c r="A7" s="10">
         <v>42000004</v>
       </c>
@@ -2906,7 +2868,7 @@
       <c r="M7" s="5"/>
       <c r="N7" s="5"/>
     </row>
-    <row r="8" spans="1:38" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:37" x14ac:dyDescent="0.15">
       <c r="A8" s="10">
         <v>42000005</v>
       </c>
@@ -2934,14 +2896,14 @@
       <c r="L8" s="5"/>
       <c r="M8" s="5"/>
       <c r="N8" s="5"/>
-      <c r="AI8">
+      <c r="AH8">
         <v>-100</v>
       </c>
-      <c r="AK8">
+      <c r="AJ8">
         <v>100</v>
       </c>
     </row>
-    <row r="9" spans="1:38" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:37" x14ac:dyDescent="0.15">
       <c r="A9" s="10">
         <v>42000006</v>
       </c>
@@ -2969,14 +2931,14 @@
       <c r="L9" s="5"/>
       <c r="M9" s="5"/>
       <c r="N9" s="5"/>
-      <c r="AI9">
+      <c r="AH9">
         <v>-100</v>
       </c>
-      <c r="AL9">
+      <c r="AK9">
         <v>100</v>
       </c>
     </row>
-    <row r="10" spans="1:38" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:37" x14ac:dyDescent="0.15">
       <c r="A10" s="10">
         <v>42000007</v>
       </c>
@@ -3004,14 +2966,14 @@
       <c r="L10" s="5"/>
       <c r="M10" s="5"/>
       <c r="N10" s="5"/>
+      <c r="AH10">
+        <v>-100</v>
+      </c>
       <c r="AI10">
-        <v>-100</v>
-      </c>
-      <c r="AJ10">
         <v>100</v>
       </c>
     </row>
-    <row r="11" spans="1:38" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:37" x14ac:dyDescent="0.15">
       <c r="A11">
         <v>42010001</v>
       </c>
@@ -3025,7 +2987,7 @@
         <v>0</v>
       </c>
       <c r="F11" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="G11" t="s">
         <v>122</v>
@@ -3040,7 +3002,7 @@
       <c r="M11" s="5"/>
       <c r="N11" s="5"/>
     </row>
-    <row r="12" spans="1:38" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:37" x14ac:dyDescent="0.15">
       <c r="A12">
         <v>42010002</v>
       </c>
@@ -3072,7 +3034,7 @@
       <c r="M12" s="5"/>
       <c r="N12" s="5"/>
     </row>
-    <row r="13" spans="1:38" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:37" x14ac:dyDescent="0.15">
       <c r="A13">
         <v>42010003</v>
       </c>
@@ -3115,11 +3077,11 @@
       <c r="S13">
         <v>100</v>
       </c>
-      <c r="AF13">
+      <c r="AE13">
         <v>70</v>
       </c>
     </row>
-    <row r="14" spans="1:38" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:37" x14ac:dyDescent="0.15">
       <c r="A14">
         <v>42010004</v>
       </c>
@@ -3153,14 +3115,14 @@
       <c r="V14">
         <v>30</v>
       </c>
+      <c r="AC14">
+        <v>30</v>
+      </c>
       <c r="AD14">
         <v>30</v>
       </c>
-      <c r="AE14">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="15" spans="1:38" x14ac:dyDescent="0.15">
+    </row>
+    <row r="15" spans="1:37" x14ac:dyDescent="0.15">
       <c r="A15">
         <v>42010005</v>
       </c>
@@ -3195,12 +3157,12 @@
         <v>100</v>
       </c>
     </row>
-    <row r="16" spans="1:38" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:37" x14ac:dyDescent="0.15">
       <c r="A16">
         <v>42010006</v>
       </c>
       <c r="B16" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="C16">
         <v>1</v>
@@ -3238,11 +3200,11 @@
       <c r="V16">
         <v>50</v>
       </c>
-      <c r="AF16">
+      <c r="AE16">
         <v>100</v>
       </c>
     </row>
-    <row r="17" spans="1:33" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:32" x14ac:dyDescent="0.15">
       <c r="A17">
         <v>42010007</v>
       </c>
@@ -3276,14 +3238,14 @@
       <c r="R17">
         <v>250</v>
       </c>
-      <c r="AD17">
+      <c r="AC17">
         <v>250</v>
       </c>
-      <c r="AG17">
+      <c r="AF17">
         <v>50</v>
       </c>
     </row>
-    <row r="18" spans="1:33" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:32" x14ac:dyDescent="0.15">
       <c r="A18">
         <v>42010008</v>
       </c>
@@ -3318,12 +3280,12 @@
         <v>23000002</v>
       </c>
     </row>
-    <row r="19" spans="1:33" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:32" x14ac:dyDescent="0.15">
       <c r="A19">
         <v>42010009</v>
       </c>
       <c r="B19" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C19">
         <v>1</v>
@@ -3332,13 +3294,13 @@
         <v>0</v>
       </c>
       <c r="F19" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="G19" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="H19" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="I19" s="5"/>
       <c r="J19" s="5"/>
@@ -3350,7 +3312,7 @@
         <v>23000003</v>
       </c>
     </row>
-    <row r="20" spans="1:33" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:32" x14ac:dyDescent="0.15">
       <c r="A20">
         <v>42010010</v>
       </c>
@@ -3381,11 +3343,11 @@
       <c r="X20">
         <v>23000004</v>
       </c>
-      <c r="AF20">
+      <c r="AE20">
         <v>50</v>
       </c>
     </row>
-    <row r="21" spans="1:33" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:32" x14ac:dyDescent="0.15">
       <c r="A21">
         <v>42010011</v>
       </c>
@@ -3420,12 +3382,12 @@
         <v>23000005</v>
       </c>
     </row>
-    <row r="22" spans="1:33" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:32" x14ac:dyDescent="0.15">
       <c r="A22">
         <v>42010012</v>
       </c>
       <c r="B22" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="C22">
         <v>1</v>
@@ -3437,13 +3399,13 @@
         <v>1</v>
       </c>
       <c r="F22" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="G22" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="H22" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="I22" s="5"/>
       <c r="J22" s="5"/>
@@ -3463,11 +3425,11 @@
       <c r="S22">
         <v>100</v>
       </c>
-      <c r="AF22">
+      <c r="AE22">
         <v>150</v>
       </c>
     </row>
-    <row r="23" spans="1:33" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:32" x14ac:dyDescent="0.15">
       <c r="A23">
         <v>42010013</v>
       </c>
@@ -3510,11 +3472,11 @@
       <c r="S23">
         <v>150</v>
       </c>
-      <c r="AF23">
+      <c r="AE23">
         <v>100</v>
       </c>
     </row>
-    <row r="24" spans="1:33" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:32" x14ac:dyDescent="0.15">
       <c r="A24">
         <v>42010014</v>
       </c>
@@ -3560,14 +3522,14 @@
       <c r="X24">
         <v>23000101</v>
       </c>
+      <c r="AE24">
+        <v>100</v>
+      </c>
       <c r="AF24">
         <v>100</v>
       </c>
-      <c r="AG24">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="25" spans="1:33" x14ac:dyDescent="0.15">
+    </row>
+    <row r="25" spans="1:32" x14ac:dyDescent="0.15">
       <c r="A25">
         <v>42010015</v>
       </c>
@@ -3598,11 +3560,11 @@
       <c r="L25" s="5"/>
       <c r="M25" s="5"/>
       <c r="N25" s="5"/>
-      <c r="AF25">
+      <c r="AE25">
         <v>80</v>
       </c>
     </row>
-    <row r="26" spans="1:33" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:32" x14ac:dyDescent="0.15">
       <c r="A26">
         <v>42010016</v>
       </c>
@@ -3634,7 +3596,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="27" spans="1:33" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:32" x14ac:dyDescent="0.15">
       <c r="A27">
         <v>42010017</v>
       </c>
@@ -3683,16 +3645,16 @@
       <c r="X27">
         <v>23000102</v>
       </c>
-      <c r="AF27">
+      <c r="AE27">
         <v>100</v>
       </c>
     </row>
-    <row r="28" spans="1:33" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:32" x14ac:dyDescent="0.15">
       <c r="A28">
         <v>42010018</v>
       </c>
       <c r="B28" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C28">
         <v>1</v>
@@ -3701,16 +3663,16 @@
         <v>0</v>
       </c>
       <c r="F28" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="G28" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="H28" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="I28" s="5" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="J28" s="5"/>
       <c r="K28" s="5"/>
@@ -3718,12 +3680,12 @@
       <c r="M28" s="5"/>
       <c r="N28" s="5"/>
     </row>
-    <row r="29" spans="1:33" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:32" x14ac:dyDescent="0.15">
       <c r="A29">
         <v>42010019</v>
       </c>
       <c r="B29" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C29">
         <v>1</v>
@@ -3735,35 +3697,35 @@
         <v>2</v>
       </c>
       <c r="F29" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="G29" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="H29" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="I29" s="5" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="J29" s="5"/>
       <c r="K29" s="5"/>
       <c r="L29" s="5"/>
       <c r="M29" s="5"/>
       <c r="N29" s="5"/>
+      <c r="AD29">
+        <v>100</v>
+      </c>
       <c r="AE29">
-        <v>100</v>
-      </c>
-      <c r="AF29">
         <v>50</v>
       </c>
     </row>
-    <row r="30" spans="1:33" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:32" x14ac:dyDescent="0.15">
       <c r="A30">
         <v>42010020</v>
       </c>
       <c r="B30" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C30">
         <v>1</v>
@@ -3775,35 +3737,35 @@
         <v>2</v>
       </c>
       <c r="F30" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="G30" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="H30" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="I30" s="5" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="J30" s="5"/>
       <c r="K30" s="5"/>
       <c r="L30" s="5"/>
       <c r="M30" s="5"/>
       <c r="N30" s="5"/>
+      <c r="AD30">
+        <v>50</v>
+      </c>
       <c r="AE30">
-        <v>50</v>
-      </c>
-      <c r="AF30">
         <v>100</v>
       </c>
     </row>
-    <row r="31" spans="1:33" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:32" x14ac:dyDescent="0.15">
       <c r="A31">
         <v>42010021</v>
       </c>
       <c r="B31" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="C31">
         <v>1</v>
@@ -3815,13 +3777,13 @@
         <v>1</v>
       </c>
       <c r="F31" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="G31" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="H31" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="I31" s="5"/>
       <c r="J31" s="5"/>
@@ -3829,16 +3791,16 @@
       <c r="L31" s="5"/>
       <c r="M31" s="5"/>
       <c r="N31" s="5"/>
-      <c r="AG31">
+      <c r="AF31">
         <v>200</v>
       </c>
     </row>
-    <row r="32" spans="1:33" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:32" x14ac:dyDescent="0.15">
       <c r="A32">
         <v>42010022</v>
       </c>
       <c r="B32" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C32">
         <v>1</v>
@@ -3850,13 +3812,13 @@
         <v>2</v>
       </c>
       <c r="F32" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="G32" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="H32" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="I32" s="5"/>
       <c r="J32" s="5"/>
@@ -3876,16 +3838,16 @@
       <c r="W32">
         <v>22031101</v>
       </c>
-      <c r="AF32">
+      <c r="AE32">
         <v>150</v>
       </c>
     </row>
-    <row r="33" spans="1:34" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:33" x14ac:dyDescent="0.15">
       <c r="A33">
         <v>42010023</v>
       </c>
       <c r="B33" t="s">
-        <v>258</v>
+        <v>251</v>
       </c>
       <c r="C33">
         <v>1</v>
@@ -3897,13 +3859,13 @@
         <v>1</v>
       </c>
       <c r="F33" t="s">
-        <v>257</v>
+        <v>250</v>
       </c>
       <c r="G33" t="s">
-        <v>257</v>
+        <v>250</v>
       </c>
       <c r="H33" t="s">
-        <v>257</v>
+        <v>250</v>
       </c>
       <c r="I33" s="5"/>
       <c r="J33" s="5"/>
@@ -3917,16 +3879,16 @@
       <c r="T33">
         <v>100</v>
       </c>
-      <c r="AF33">
+      <c r="AE33">
         <v>100</v>
       </c>
     </row>
-    <row r="34" spans="1:34" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:33" x14ac:dyDescent="0.15">
       <c r="A34">
         <v>42010024</v>
       </c>
       <c r="B34" t="s">
-        <v>260</v>
+        <v>253</v>
       </c>
       <c r="C34">
         <v>1</v>
@@ -3935,13 +3897,13 @@
         <v>0</v>
       </c>
       <c r="F34" t="s">
-        <v>259</v>
+        <v>252</v>
       </c>
       <c r="G34" t="s">
-        <v>259</v>
+        <v>252</v>
       </c>
       <c r="H34" t="s">
-        <v>259</v>
+        <v>252</v>
       </c>
       <c r="I34" s="5"/>
       <c r="J34" s="5"/>
@@ -3953,12 +3915,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:34" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:33" x14ac:dyDescent="0.15">
       <c r="A35">
         <v>42010025</v>
       </c>
       <c r="B35" t="s">
-        <v>261</v>
+        <v>254</v>
       </c>
       <c r="C35">
         <v>1</v>
@@ -3967,13 +3929,13 @@
         <v>0</v>
       </c>
       <c r="F35" t="s">
-        <v>262</v>
+        <v>255</v>
       </c>
       <c r="G35" t="s">
-        <v>262</v>
+        <v>255</v>
       </c>
       <c r="H35" t="s">
-        <v>262</v>
+        <v>255</v>
       </c>
       <c r="I35" s="5"/>
       <c r="J35" s="5"/>
@@ -3985,7 +3947,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="36" spans="1:34" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:33" x14ac:dyDescent="0.15">
       <c r="A36">
         <v>42040001</v>
       </c>
@@ -4028,14 +3990,14 @@
       <c r="Z36">
         <v>1</v>
       </c>
+      <c r="AE36">
+        <v>200</v>
+      </c>
       <c r="AF36">
         <v>200</v>
       </c>
-      <c r="AG36">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="37" spans="1:34" x14ac:dyDescent="0.15">
+    </row>
+    <row r="37" spans="1:33" x14ac:dyDescent="0.15">
       <c r="A37">
         <v>42040002</v>
       </c>
@@ -4081,14 +4043,14 @@
       <c r="X37">
         <v>23000102</v>
       </c>
+      <c r="AE37">
+        <v>150</v>
+      </c>
       <c r="AF37">
         <v>150</v>
       </c>
-      <c r="AG37">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="38" spans="1:34" x14ac:dyDescent="0.15">
+    </row>
+    <row r="38" spans="1:33" x14ac:dyDescent="0.15">
       <c r="A38">
         <v>42040003</v>
       </c>
@@ -4119,19 +4081,19 @@
       <c r="L38" s="5"/>
       <c r="M38" s="5"/>
       <c r="N38" s="5"/>
-      <c r="AD38">
+      <c r="AC38">
         <v>100</v>
       </c>
-      <c r="AF38">
+      <c r="AE38">
         <v>100</v>
       </c>
     </row>
-    <row r="39" spans="1:34" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:33" x14ac:dyDescent="0.15">
       <c r="A39">
         <v>42040004</v>
       </c>
       <c r="B39" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="C39">
         <v>3</v>
@@ -4143,13 +4105,13 @@
         <v>1</v>
       </c>
       <c r="F39" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="G39" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="H39" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="I39" s="5"/>
       <c r="J39" s="5"/>
@@ -4160,16 +4122,16 @@
       <c r="Y39">
         <v>1</v>
       </c>
-      <c r="AH39">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="40" spans="1:34" x14ac:dyDescent="0.15">
+      <c r="AG39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:33" x14ac:dyDescent="0.15">
       <c r="A40">
         <v>42040005</v>
       </c>
       <c r="B40" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="C40">
         <v>3</v>
@@ -4181,13 +4143,13 @@
         <v>1</v>
       </c>
       <c r="F40" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="G40" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="H40" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="I40" s="5"/>
       <c r="J40" s="5"/>
@@ -4207,19 +4169,19 @@
       <c r="S40">
         <v>150</v>
       </c>
+      <c r="AC40">
+        <v>200</v>
+      </c>
       <c r="AD40">
         <v>200</v>
       </c>
-      <c r="AE40">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="41" spans="1:34" x14ac:dyDescent="0.15">
+    </row>
+    <row r="41" spans="1:33" x14ac:dyDescent="0.15">
       <c r="A41">
         <v>42040006</v>
       </c>
       <c r="B41" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="C41">
         <v>3</v>
@@ -4231,13 +4193,13 @@
         <v>3</v>
       </c>
       <c r="F41" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="G41" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="H41" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="I41" s="5"/>
       <c r="J41" s="5"/>
@@ -4257,7 +4219,7 @@
       <c r="V41">
         <v>200</v>
       </c>
-      <c r="AF41">
+      <c r="AE41">
         <v>300</v>
       </c>
     </row>
@@ -4274,11 +4236,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AL28"/>
+  <dimension ref="A1:AK28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AA24" sqref="AA24"/>
+      <selection pane="bottomLeft" activeCell="J3" sqref="J3:M3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -4297,11 +4259,10 @@
     <col min="25" max="25" width="5.125" customWidth="1"/>
     <col min="26" max="27" width="9.375" customWidth="1"/>
     <col min="28" max="28" width="7.375" customWidth="1"/>
-    <col min="29" max="29" width="4.625" customWidth="1"/>
-    <col min="31" max="39" width="5" customWidth="1"/>
+    <col min="30" max="38" width="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:38" ht="69.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:37" ht="69.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="14" t="s">
         <v>79</v>
       </c>
@@ -4330,19 +4291,19 @@
         <v>83</v>
       </c>
       <c r="J1" s="22" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="K1" s="22" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="L1" s="22" t="s">
-        <v>264</v>
+        <v>257</v>
       </c>
       <c r="M1" s="22" t="s">
-        <v>267</v>
+        <v>258</v>
       </c>
       <c r="N1" s="14" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="O1" s="18" t="s">
         <v>2</v>
@@ -4351,7 +4312,7 @@
         <v>15</v>
       </c>
       <c r="Q1" s="18" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="R1" s="15" t="s">
         <v>3</v>
@@ -4375,49 +4336,46 @@
         <v>77</v>
       </c>
       <c r="Y1" s="15" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="Z1" s="15" t="s">
         <v>137</v>
       </c>
       <c r="AA1" s="15" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="AB1" s="15" t="s">
         <v>156</v>
       </c>
-      <c r="AC1" s="15" t="s">
-        <v>175</v>
+      <c r="AC1" s="16" t="s">
+        <v>5</v>
       </c>
       <c r="AD1" s="16" t="s">
-        <v>5</v>
+        <v>88</v>
       </c>
       <c r="AE1" s="16" t="s">
-        <v>88</v>
+        <v>78</v>
       </c>
       <c r="AF1" s="16" t="s">
-        <v>78</v>
+        <v>89</v>
       </c>
       <c r="AG1" s="16" t="s">
-        <v>89</v>
-      </c>
-      <c r="AH1" s="16" t="s">
-        <v>198</v>
+        <v>196</v>
+      </c>
+      <c r="AH1" s="17" t="s">
+        <v>28</v>
       </c>
       <c r="AI1" s="17" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="AJ1" s="17" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="AK1" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="AL1" s="17" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:38" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:37" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>59</v>
       </c>
@@ -4446,19 +4404,19 @@
         <v>62</v>
       </c>
       <c r="J2" s="23" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="K2" s="23" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="L2" s="23" t="s">
-        <v>263</v>
+        <v>256</v>
       </c>
       <c r="M2" s="23" t="s">
-        <v>263</v>
+        <v>256</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="O2" s="19" t="s">
         <v>0</v>
@@ -4491,19 +4449,19 @@
         <v>59</v>
       </c>
       <c r="Y2" s="7" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="Z2" s="7" t="s">
         <v>138</v>
       </c>
       <c r="AA2" s="7" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="AB2" s="7" t="s">
         <v>157</v>
       </c>
-      <c r="AC2" s="7" t="s">
-        <v>248</v>
+      <c r="AC2" s="3" t="s">
+        <v>0</v>
       </c>
       <c r="AD2" s="3" t="s">
         <v>0</v>
@@ -4512,13 +4470,13 @@
         <v>0</v>
       </c>
       <c r="AF2" s="3" t="s">
-        <v>0</v>
+        <v>59</v>
       </c>
       <c r="AG2" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="AH2" s="3" t="s">
-        <v>200</v>
+        <v>198</v>
+      </c>
+      <c r="AH2" s="9" t="s">
+        <v>27</v>
       </c>
       <c r="AI2" s="9" t="s">
         <v>27</v>
@@ -4529,11 +4487,8 @@
       <c r="AK2" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="AL2" s="9" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="3" spans="1:38" x14ac:dyDescent="0.15">
+    </row>
+    <row r="3" spans="1:37" x14ac:dyDescent="0.15">
       <c r="A3" s="8" t="s">
         <v>64</v>
       </c>
@@ -4562,28 +4517,28 @@
         <v>17</v>
       </c>
       <c r="J3" s="24" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="K3" s="24" t="s">
+        <v>265</v>
+      </c>
+      <c r="L3" s="24" t="s">
+        <v>266</v>
+      </c>
+      <c r="M3" s="24" t="s">
+        <v>267</v>
+      </c>
+      <c r="N3" s="8" t="s">
+        <v>241</v>
+      </c>
+      <c r="O3" s="20" t="s">
         <v>237</v>
-      </c>
-      <c r="L3" s="24" t="s">
-        <v>265</v>
-      </c>
-      <c r="M3" s="24" t="s">
-        <v>266</v>
-      </c>
-      <c r="N3" s="8" t="s">
-        <v>244</v>
-      </c>
-      <c r="O3" s="20" t="s">
-        <v>240</v>
       </c>
       <c r="P3" s="20" t="s">
         <v>70</v>
       </c>
       <c r="Q3" s="20" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="R3" s="6" t="s">
         <v>71</v>
@@ -4607,49 +4562,46 @@
         <v>35</v>
       </c>
       <c r="Y3" s="6" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="Z3" s="6" t="s">
         <v>139</v>
       </c>
       <c r="AA3" s="6" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="AB3" s="6" t="s">
         <v>158</v>
       </c>
-      <c r="AC3" s="6" t="s">
-        <v>247</v>
+      <c r="AC3" s="2" t="s">
+        <v>75</v>
       </c>
       <c r="AD3" s="2" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="AE3" s="2" t="s">
-        <v>76</v>
+        <v>36</v>
       </c>
       <c r="AF3" s="2" t="s">
-        <v>36</v>
+        <v>8</v>
       </c>
       <c r="AG3" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="AH3" s="2" t="s">
-        <v>201</v>
+        <v>199</v>
+      </c>
+      <c r="AH3" s="8" t="s">
+        <v>23</v>
       </c>
       <c r="AI3" s="8" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="AJ3" s="8" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="AK3" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="AL3" s="8" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:38" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:37" x14ac:dyDescent="0.15">
       <c r="A4" s="10">
         <v>42020001</v>
       </c>
@@ -4681,18 +4633,17 @@
       <c r="N4" s="5"/>
       <c r="P4" s="11"/>
       <c r="Q4" s="13"/>
-      <c r="AC4" s="5"/>
-      <c r="AI4">
+      <c r="AH4">
         <v>-300</v>
+      </c>
+      <c r="AJ4">
+        <v>1000</v>
       </c>
       <c r="AK4">
         <v>1000</v>
       </c>
-      <c r="AL4">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="5" spans="1:38" x14ac:dyDescent="0.15">
+    </row>
+    <row r="5" spans="1:37" x14ac:dyDescent="0.15">
       <c r="A5" s="10">
         <v>42020002</v>
       </c>
@@ -4724,15 +4675,14 @@
       <c r="N5" s="5"/>
       <c r="P5" s="11"/>
       <c r="Q5" s="13"/>
-      <c r="AC5" s="5"/>
+      <c r="AH5">
+        <v>-200</v>
+      </c>
       <c r="AI5">
-        <v>-200</v>
-      </c>
-      <c r="AJ5">
         <v>1000</v>
       </c>
     </row>
-    <row r="6" spans="1:38" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:37" x14ac:dyDescent="0.15">
       <c r="A6" s="10">
         <v>42020003</v>
       </c>
@@ -4764,14 +4714,13 @@
       <c r="N6" s="5"/>
       <c r="P6" s="11"/>
       <c r="Q6" s="13"/>
-      <c r="AC6" s="5"/>
-    </row>
-    <row r="7" spans="1:38" x14ac:dyDescent="0.15">
+    </row>
+    <row r="7" spans="1:37" x14ac:dyDescent="0.15">
       <c r="A7" s="10">
         <v>42020004</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="C7" s="10">
         <v>2</v>
@@ -4780,13 +4729,13 @@
         <v>0</v>
       </c>
       <c r="F7" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="G7" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="H7" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="I7" s="5" t="s">
         <v>18</v>
@@ -4796,14 +4745,13 @@
       <c r="L7" s="5"/>
       <c r="M7" s="5"/>
       <c r="N7" s="5"/>
-      <c r="AC7" s="5"/>
-    </row>
-    <row r="8" spans="1:38" x14ac:dyDescent="0.15">
+    </row>
+    <row r="8" spans="1:37" x14ac:dyDescent="0.15">
       <c r="A8" s="10">
         <v>42020005</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="C8" s="10">
         <v>2</v>
@@ -4812,13 +4760,13 @@
         <v>0</v>
       </c>
       <c r="F8" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="G8" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="H8" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="I8" s="5" t="s">
         <v>18</v>
@@ -4830,9 +4778,8 @@
       <c r="N8" s="5"/>
       <c r="P8" s="11"/>
       <c r="Q8" s="13"/>
-      <c r="AC8" s="5"/>
-    </row>
-    <row r="9" spans="1:38" x14ac:dyDescent="0.15">
+    </row>
+    <row r="9" spans="1:37" x14ac:dyDescent="0.15">
       <c r="A9">
         <v>42030001</v>
       </c>
@@ -4852,7 +4799,7 @@
         <v>19</v>
       </c>
       <c r="H9" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="I9" s="5" t="s">
         <v>18</v>
@@ -4872,9 +4819,8 @@
       <c r="AA9">
         <v>12000001</v>
       </c>
-      <c r="AC9" s="5"/>
-    </row>
-    <row r="10" spans="1:38" x14ac:dyDescent="0.15">
+    </row>
+    <row r="10" spans="1:37" x14ac:dyDescent="0.15">
       <c r="A10">
         <v>42030002</v>
       </c>
@@ -4888,7 +4834,7 @@
         <v>0</v>
       </c>
       <c r="F10" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="G10" t="s">
         <v>21</v>
@@ -4902,7 +4848,7 @@
       <c r="J10" s="5"/>
       <c r="K10" s="5"/>
       <c r="L10" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="M10" s="5"/>
       <c r="N10">
@@ -4918,9 +4864,8 @@
       <c r="Z10">
         <v>43020101</v>
       </c>
-      <c r="AC10" s="5"/>
-    </row>
-    <row r="11" spans="1:38" x14ac:dyDescent="0.15">
+    </row>
+    <row r="11" spans="1:37" x14ac:dyDescent="0.15">
       <c r="A11">
         <v>42030003</v>
       </c>
@@ -4940,7 +4885,7 @@
         <v>149</v>
       </c>
       <c r="H11" t="s">
-        <v>268</v>
+        <v>259</v>
       </c>
       <c r="I11" s="5" t="s">
         <v>18</v>
@@ -4948,15 +4893,14 @@
       <c r="J11" s="5"/>
       <c r="K11" s="5"/>
       <c r="L11" t="s">
-        <v>270</v>
+        <v>261</v>
       </c>
       <c r="M11" s="5"/>
       <c r="N11" s="5"/>
       <c r="P11" s="12"/>
       <c r="Q11" s="12"/>
-      <c r="AC11" s="5"/>
-    </row>
-    <row r="12" spans="1:38" x14ac:dyDescent="0.15">
+    </row>
+    <row r="12" spans="1:37" x14ac:dyDescent="0.15">
       <c r="A12">
         <v>42030004</v>
       </c>
@@ -4992,11 +4936,10 @@
         <v>43020102</v>
       </c>
       <c r="AB12" t="s">
-        <v>269</v>
-      </c>
-      <c r="AC12" s="5"/>
-    </row>
-    <row r="13" spans="1:38" x14ac:dyDescent="0.15">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="13" spans="1:37" x14ac:dyDescent="0.15">
       <c r="A13">
         <v>42030005</v>
       </c>
@@ -5042,11 +4985,8 @@
       <c r="AB13" t="s">
         <v>174</v>
       </c>
-      <c r="AC13" s="5" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="14" spans="1:38" x14ac:dyDescent="0.15">
+    </row>
+    <row r="14" spans="1:37" x14ac:dyDescent="0.15">
       <c r="A14">
         <v>42030006</v>
       </c>
@@ -5078,9 +5018,8 @@
       <c r="N14" s="5"/>
       <c r="P14" s="12"/>
       <c r="Q14" s="12"/>
-      <c r="AC14" s="5"/>
-    </row>
-    <row r="15" spans="1:38" x14ac:dyDescent="0.15">
+    </row>
+    <row r="15" spans="1:37" x14ac:dyDescent="0.15">
       <c r="A15">
         <v>42030007</v>
       </c>
@@ -5112,9 +5051,8 @@
       <c r="N15" s="5"/>
       <c r="P15" s="12"/>
       <c r="Q15" s="12"/>
-      <c r="AC15" s="5"/>
-    </row>
-    <row r="16" spans="1:38" x14ac:dyDescent="0.15">
+    </row>
+    <row r="16" spans="1:37" x14ac:dyDescent="0.15">
       <c r="A16">
         <v>42030008</v>
       </c>
@@ -5146,9 +5084,8 @@
       <c r="N16" s="5"/>
       <c r="P16" s="12"/>
       <c r="Q16" s="12"/>
-      <c r="AC16" s="5"/>
-    </row>
-    <row r="17" spans="1:33" x14ac:dyDescent="0.15">
+    </row>
+    <row r="17" spans="1:32" x14ac:dyDescent="0.15">
       <c r="A17">
         <v>42030009</v>
       </c>
@@ -5180,9 +5117,8 @@
       <c r="N17" s="5"/>
       <c r="P17" s="12"/>
       <c r="Q17" s="12"/>
-      <c r="AC17" s="5"/>
-    </row>
-    <row r="18" spans="1:33" x14ac:dyDescent="0.15">
+    </row>
+    <row r="18" spans="1:32" x14ac:dyDescent="0.15">
       <c r="A18">
         <v>42030010</v>
       </c>
@@ -5214,9 +5150,8 @@
       <c r="N18" s="5"/>
       <c r="P18" s="12"/>
       <c r="Q18" s="12"/>
-      <c r="AC18" s="5"/>
-    </row>
-    <row r="19" spans="1:33" x14ac:dyDescent="0.15">
+    </row>
+    <row r="19" spans="1:32" x14ac:dyDescent="0.15">
       <c r="A19">
         <v>42030011</v>
       </c>
@@ -5248,9 +5183,8 @@
       <c r="N19" s="5"/>
       <c r="P19" s="12"/>
       <c r="Q19" s="12"/>
-      <c r="AC19" s="5"/>
-    </row>
-    <row r="20" spans="1:33" x14ac:dyDescent="0.15">
+    </row>
+    <row r="20" spans="1:32" x14ac:dyDescent="0.15">
       <c r="A20">
         <v>42030012</v>
       </c>
@@ -5264,13 +5198,13 @@
         <v>0</v>
       </c>
       <c r="F20" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="G20" t="s">
         <v>160</v>
       </c>
       <c r="H20" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="I20" s="5" t="s">
         <v>18</v>
@@ -5293,16 +5227,15 @@
         <v>43020105</v>
       </c>
       <c r="AB20" t="s">
-        <v>270</v>
-      </c>
-      <c r="AC20" s="5"/>
-    </row>
-    <row r="21" spans="1:33" x14ac:dyDescent="0.15">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="21" spans="1:32" x14ac:dyDescent="0.15">
       <c r="A21">
         <v>42030013</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>251</v>
+        <v>244</v>
       </c>
       <c r="C21" s="10">
         <v>2</v>
@@ -5311,13 +5244,13 @@
         <v>0</v>
       </c>
       <c r="F21" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="G21" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="H21" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="I21" s="5" t="s">
         <v>18</v>
@@ -5326,21 +5259,20 @@
       <c r="K21" s="5"/>
       <c r="L21" s="5"/>
       <c r="M21" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="N21" s="21">
         <v>12000002</v>
       </c>
       <c r="P21" s="12"/>
       <c r="Q21" s="12"/>
-      <c r="AC21" s="5"/>
-    </row>
-    <row r="22" spans="1:33" x14ac:dyDescent="0.15">
+    </row>
+    <row r="22" spans="1:32" x14ac:dyDescent="0.15">
       <c r="A22">
         <v>42030014</v>
       </c>
       <c r="B22" t="s">
-        <v>255</v>
+        <v>248</v>
       </c>
       <c r="C22" s="10">
         <v>2</v>
@@ -5349,13 +5281,13 @@
         <v>0</v>
       </c>
       <c r="F22" t="s">
-        <v>252</v>
+        <v>245</v>
       </c>
       <c r="G22" t="s">
-        <v>252</v>
+        <v>245</v>
       </c>
       <c r="H22" t="s">
-        <v>252</v>
+        <v>245</v>
       </c>
       <c r="I22" s="5" t="s">
         <v>18</v>
@@ -5369,14 +5301,13 @@
       </c>
       <c r="P22" s="12"/>
       <c r="Q22" s="12"/>
-      <c r="AC22" s="5"/>
-    </row>
-    <row r="23" spans="1:33" x14ac:dyDescent="0.15">
+    </row>
+    <row r="23" spans="1:32" x14ac:dyDescent="0.15">
       <c r="A23">
         <v>42030015</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>254</v>
+        <v>247</v>
       </c>
       <c r="C23" s="10">
         <v>2</v>
@@ -5385,13 +5316,13 @@
         <v>0</v>
       </c>
       <c r="F23" t="s">
-        <v>253</v>
+        <v>246</v>
       </c>
       <c r="G23" t="s">
-        <v>256</v>
+        <v>249</v>
       </c>
       <c r="H23" t="s">
-        <v>253</v>
+        <v>246</v>
       </c>
       <c r="I23" s="5" t="s">
         <v>18</v>
@@ -5405,14 +5336,13 @@
       </c>
       <c r="P23" s="12"/>
       <c r="Q23" s="12"/>
-      <c r="AC23" s="5"/>
-    </row>
-    <row r="24" spans="1:33" x14ac:dyDescent="0.15">
+    </row>
+    <row r="24" spans="1:32" x14ac:dyDescent="0.15">
       <c r="A24">
         <v>42030016</v>
       </c>
       <c r="B24" t="s">
-        <v>272</v>
+        <v>263</v>
       </c>
       <c r="C24" s="10">
         <v>2</v>
@@ -5421,13 +5351,13 @@
         <v>0</v>
       </c>
       <c r="F24" t="s">
-        <v>273</v>
+        <v>264</v>
       </c>
       <c r="G24" t="s">
-        <v>271</v>
+        <v>262</v>
       </c>
       <c r="H24" t="s">
-        <v>273</v>
+        <v>264</v>
       </c>
       <c r="I24" s="5" t="s">
         <v>18</v>
@@ -5436,7 +5366,7 @@
       <c r="K24" s="5"/>
       <c r="L24" s="5"/>
       <c r="M24" t="s">
-        <v>270</v>
+        <v>261</v>
       </c>
       <c r="N24" s="21">
         <v>12000002</v>
@@ -5446,14 +5376,13 @@
       <c r="AA24">
         <v>12000003</v>
       </c>
-      <c r="AC24" s="5"/>
-    </row>
-    <row r="25" spans="1:33" x14ac:dyDescent="0.15">
+    </row>
+    <row r="25" spans="1:32" x14ac:dyDescent="0.15">
       <c r="A25">
         <v>42050001</v>
       </c>
       <c r="B25" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="C25" s="10">
         <v>2</v>
@@ -5462,13 +5391,13 @@
         <v>0</v>
       </c>
       <c r="F25" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="G25" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="H25" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="I25" s="5" t="s">
         <v>18</v>
@@ -5484,14 +5413,13 @@
       <c r="Q25" s="12">
         <v>13020001</v>
       </c>
-      <c r="AC25" s="5"/>
-    </row>
-    <row r="26" spans="1:33" x14ac:dyDescent="0.15">
+    </row>
+    <row r="26" spans="1:32" x14ac:dyDescent="0.15">
       <c r="A26">
         <v>42050002</v>
       </c>
       <c r="B26" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="C26" s="10">
         <v>2</v>
@@ -5500,13 +5428,13 @@
         <v>0</v>
       </c>
       <c r="F26" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="G26" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="H26" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="I26" s="5" t="s">
         <v>18</v>
@@ -5520,14 +5448,13 @@
       <c r="Q26" s="12">
         <v>13020002</v>
       </c>
-      <c r="AC26" s="5"/>
-    </row>
-    <row r="27" spans="1:33" x14ac:dyDescent="0.15">
+    </row>
+    <row r="27" spans="1:32" x14ac:dyDescent="0.15">
       <c r="A27">
         <v>42050003</v>
       </c>
       <c r="B27" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="C27" s="10">
         <v>2</v>
@@ -5539,13 +5466,13 @@
         <v>3</v>
       </c>
       <c r="F27" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="G27" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="H27" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="I27" s="5" t="s">
         <v>18</v>
@@ -5583,24 +5510,21 @@
         <v>12000002</v>
       </c>
       <c r="AB27" t="s">
-        <v>216</v>
-      </c>
-      <c r="AC27" s="5" t="s">
-        <v>250</v>
+        <v>214</v>
+      </c>
+      <c r="AE27">
+        <v>200</v>
       </c>
       <c r="AF27">
         <v>200</v>
       </c>
-      <c r="AG27">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="28" spans="1:33" x14ac:dyDescent="0.15">
+    </row>
+    <row r="28" spans="1:32" x14ac:dyDescent="0.15">
       <c r="A28">
         <v>42050004</v>
       </c>
       <c r="B28" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="C28" s="10">
         <v>2</v>
@@ -5609,13 +5533,13 @@
         <v>0</v>
       </c>
       <c r="F28" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="G28" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="H28" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="I28" s="5" t="s">
         <v>18</v>
@@ -5629,7 +5553,6 @@
       <c r="Q28" s="12">
         <v>13020011</v>
       </c>
-      <c r="AC28" s="5"/>
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>

</xml_diff>

<commit_message>
rearrange the id of scenequests
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/SceneQuest.xlsx
+++ b/ConfigData/Xlsx/SceneQuest.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17766"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17927"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\code\TOMClassicGit\ConfigData\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Code\TOMClassicGit\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -2133,12 +2133,6 @@
   </cellStyles>
   <dxfs count="20">
     <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -2191,6 +2185,9 @@
       <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -2205,6 +2202,9 @@
           <bgColor theme="7" tint="-0.249977111117893"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
@@ -2264,13 +2264,13 @@
     <tableColumn id="4" name="Figue"/>
     <tableColumn id="5" name="Script"/>
     <tableColumn id="6" name="TriggerMulti" dataDxfId="18"/>
-    <tableColumn id="40" name="Catalog" dataDxfId="1"/>
-    <tableColumn id="35" name="TriggerHourBegin" dataDxfId="17"/>
-    <tableColumn id="34" name="TriggerHourEnd" dataDxfId="16"/>
-    <tableColumn id="36" name="TriggerFlagNoExist" dataDxfId="15"/>
-    <tableColumn id="38" name="TriggerFlagExist" dataDxfId="14"/>
-    <tableColumn id="39" name="TriggerRate" dataDxfId="13"/>
-    <tableColumn id="37" name="QuestNeed" dataDxfId="12"/>
+    <tableColumn id="40" name="Catalog" dataDxfId="17"/>
+    <tableColumn id="35" name="TriggerHourBegin" dataDxfId="16"/>
+    <tableColumn id="34" name="TriggerHourEnd" dataDxfId="15"/>
+    <tableColumn id="36" name="TriggerFlagNoExist" dataDxfId="14"/>
+    <tableColumn id="38" name="TriggerFlagExist" dataDxfId="13"/>
+    <tableColumn id="39" name="TriggerRate" dataDxfId="12"/>
+    <tableColumn id="37" name="QuestNeed" dataDxfId="11"/>
     <tableColumn id="7" name="EnemyId"/>
     <tableColumn id="8" name="BattleMap"/>
     <tableColumn id="32" name="SceneId"/>
@@ -2301,7 +2301,7 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="表3_5" displayName="表3_5" ref="A3:AN33" totalsRowShown="0" headerRowDxfId="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="表3_5" displayName="表3_5" ref="A3:AN33" totalsRowShown="0" headerRowDxfId="10">
   <autoFilter ref="A3:AN33"/>
   <sortState ref="A4:AA6">
     <sortCondition ref="A3:A6"/>
@@ -2309,24 +2309,24 @@
   <tableColumns count="40">
     <tableColumn id="1" name="Id"/>
     <tableColumn id="2" name="Name"/>
-    <tableColumn id="27" name="Type" dataDxfId="10"/>
+    <tableColumn id="27" name="Type" dataDxfId="9"/>
     <tableColumn id="3" name="Level"/>
     <tableColumn id="25" name="Danger"/>
     <tableColumn id="24" name="Ename"/>
     <tableColumn id="4" name="Figue"/>
     <tableColumn id="5" name="Script"/>
     <tableColumn id="6" name="TriggerMulti"/>
-    <tableColumn id="40" name="Catalog" dataDxfId="0"/>
-    <tableColumn id="35" name="TriggerHourBegin" dataDxfId="9"/>
-    <tableColumn id="34" name="TriggerHourEnd" dataDxfId="8"/>
-    <tableColumn id="37" name="TriggerFlagNoExist" dataDxfId="7"/>
-    <tableColumn id="38" name="TriggerFlagExist" dataDxfId="6"/>
-    <tableColumn id="39" name="TriggerRate" dataDxfId="5"/>
-    <tableColumn id="36" name="QuestNeed" dataDxfId="4"/>
+    <tableColumn id="40" name="Catalog" dataDxfId="8"/>
+    <tableColumn id="35" name="TriggerHourBegin" dataDxfId="7"/>
+    <tableColumn id="34" name="TriggerHourEnd" dataDxfId="6"/>
+    <tableColumn id="37" name="TriggerFlagNoExist" dataDxfId="5"/>
+    <tableColumn id="38" name="TriggerFlagExist" dataDxfId="4"/>
+    <tableColumn id="39" name="TriggerRate" dataDxfId="3"/>
+    <tableColumn id="36" name="QuestNeed" dataDxfId="2"/>
     <tableColumn id="7" name="EnemyId"/>
     <tableColumn id="8" name="BattleMap"/>
-    <tableColumn id="32" name="SceneId" dataDxfId="3"/>
-    <tableColumn id="29" name="Position" dataDxfId="2"/>
+    <tableColumn id="32" name="SceneId" dataDxfId="1"/>
+    <tableColumn id="29" name="Position" dataDxfId="0"/>
     <tableColumn id="9" name="RewardGold"/>
     <tableColumn id="10" name="RewardFood"/>
     <tableColumn id="11" name="RewardHealth"/>
@@ -2676,8 +2676,8 @@
   <dimension ref="A1:AN48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E38" sqref="E38"/>
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -4619,7 +4619,7 @@
     </row>
     <row r="41" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A41">
-        <v>42040001</v>
+        <v>42020001</v>
       </c>
       <c r="B41" t="s">
         <v>140</v>
@@ -4673,7 +4673,7 @@
     </row>
     <row r="42" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A42">
-        <v>42040002</v>
+        <v>42020002</v>
       </c>
       <c r="B42" t="s">
         <v>116</v>
@@ -4730,7 +4730,7 @@
     </row>
     <row r="43" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A43">
-        <v>42040003</v>
+        <v>42020003</v>
       </c>
       <c r="B43" t="s">
         <v>147</v>
@@ -4772,7 +4772,7 @@
     </row>
     <row r="44" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A44">
-        <v>42040004</v>
+        <v>42020004</v>
       </c>
       <c r="B44" t="s">
         <v>200</v>
@@ -4814,7 +4814,7 @@
     </row>
     <row r="45" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A45">
-        <v>42040005</v>
+        <v>42020005</v>
       </c>
       <c r="B45" t="s">
         <v>220</v>
@@ -4868,7 +4868,7 @@
     </row>
     <row r="46" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A46">
-        <v>42040006</v>
+        <v>42020006</v>
       </c>
       <c r="B46" t="s">
         <v>222</v>
@@ -4919,7 +4919,7 @@
     </row>
     <row r="47" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A47">
-        <v>42040007</v>
+        <v>42020007</v>
       </c>
       <c r="B47" t="s">
         <v>302</v>
@@ -4952,7 +4952,7 @@
     </row>
     <row r="48" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A48">
-        <v>42040008</v>
+        <v>42020008</v>
       </c>
       <c r="B48" t="s">
         <v>315</v>
@@ -5000,7 +5000,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J1" sqref="J1:J3"/>
+      <selection pane="bottomLeft" activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -5391,7 +5391,7 @@
     </row>
     <row r="4" spans="1:40" x14ac:dyDescent="0.15">
       <c r="A4" s="10">
-        <v>42020001</v>
+        <v>42110001</v>
       </c>
       <c r="B4" s="10" t="s">
         <v>92</v>
@@ -5436,7 +5436,7 @@
     </row>
     <row r="5" spans="1:40" x14ac:dyDescent="0.15">
       <c r="A5" s="10">
-        <v>42020002</v>
+        <v>42110002</v>
       </c>
       <c r="B5" s="10" t="s">
         <v>93</v>
@@ -5478,7 +5478,7 @@
     </row>
     <row r="6" spans="1:40" x14ac:dyDescent="0.15">
       <c r="A6" s="10">
-        <v>42020003</v>
+        <v>42110003</v>
       </c>
       <c r="B6" s="10" t="s">
         <v>97</v>
@@ -5514,7 +5514,7 @@
     </row>
     <row r="7" spans="1:40" x14ac:dyDescent="0.15">
       <c r="A7" s="10">
-        <v>42020004</v>
+        <v>42110004</v>
       </c>
       <c r="B7" s="10" t="s">
         <v>189</v>
@@ -5547,7 +5547,7 @@
     </row>
     <row r="8" spans="1:40" x14ac:dyDescent="0.15">
       <c r="A8" s="10">
-        <v>42020005</v>
+        <v>42110005</v>
       </c>
       <c r="B8" s="10" t="s">
         <v>202</v>
@@ -5583,7 +5583,7 @@
     </row>
     <row r="9" spans="1:40" x14ac:dyDescent="0.15">
       <c r="A9">
-        <v>42030001</v>
+        <v>42120001</v>
       </c>
       <c r="B9" t="s">
         <v>20</v>
@@ -5627,7 +5627,7 @@
     </row>
     <row r="10" spans="1:40" x14ac:dyDescent="0.15">
       <c r="A10">
-        <v>42030002</v>
+        <v>42120002</v>
       </c>
       <c r="B10" t="s">
         <v>22</v>
@@ -5675,7 +5675,7 @@
     </row>
     <row r="11" spans="1:40" x14ac:dyDescent="0.15">
       <c r="A11">
-        <v>42030003</v>
+        <v>42120003</v>
       </c>
       <c r="B11" t="s">
         <v>150</v>
@@ -5713,7 +5713,7 @@
     </row>
     <row r="12" spans="1:40" x14ac:dyDescent="0.15">
       <c r="A12">
-        <v>42030004</v>
+        <v>42120004</v>
       </c>
       <c r="B12" t="s">
         <v>153</v>
@@ -5755,7 +5755,7 @@
     </row>
     <row r="13" spans="1:40" x14ac:dyDescent="0.15">
       <c r="A13">
-        <v>42030005</v>
+        <v>42120005</v>
       </c>
       <c r="B13" t="s">
         <v>159</v>
@@ -5805,7 +5805,7 @@
     </row>
     <row r="14" spans="1:40" x14ac:dyDescent="0.15">
       <c r="A14">
-        <v>42030006</v>
+        <v>42120006</v>
       </c>
       <c r="B14" t="s">
         <v>162</v>
@@ -5865,7 +5865,7 @@
     </row>
     <row r="15" spans="1:40" x14ac:dyDescent="0.15">
       <c r="A15">
-        <v>42030007</v>
+        <v>42120007</v>
       </c>
       <c r="B15" t="s">
         <v>163</v>
@@ -5901,7 +5901,7 @@
     </row>
     <row r="16" spans="1:40" x14ac:dyDescent="0.15">
       <c r="A16">
-        <v>42030008</v>
+        <v>42120008</v>
       </c>
       <c r="B16" s="4" t="s">
         <v>165</v>
@@ -5937,7 +5937,7 @@
     </row>
     <row r="17" spans="1:35" x14ac:dyDescent="0.15">
       <c r="A17">
-        <v>42030009</v>
+        <v>42120009</v>
       </c>
       <c r="B17" s="4" t="s">
         <v>166</v>
@@ -5973,7 +5973,7 @@
     </row>
     <row r="18" spans="1:35" x14ac:dyDescent="0.15">
       <c r="A18">
-        <v>42030010</v>
+        <v>42120010</v>
       </c>
       <c r="B18" s="4" t="s">
         <v>167</v>
@@ -6009,7 +6009,7 @@
     </row>
     <row r="19" spans="1:35" x14ac:dyDescent="0.15">
       <c r="A19">
-        <v>42030011</v>
+        <v>42120011</v>
       </c>
       <c r="B19" s="4" t="s">
         <v>168</v>
@@ -6045,7 +6045,7 @@
     </row>
     <row r="20" spans="1:35" x14ac:dyDescent="0.15">
       <c r="A20">
-        <v>42030012</v>
+        <v>42120012</v>
       </c>
       <c r="B20" t="s">
         <v>159</v>
@@ -6093,7 +6093,7 @@
     </row>
     <row r="21" spans="1:35" x14ac:dyDescent="0.15">
       <c r="A21">
-        <v>42030013</v>
+        <v>42120013</v>
       </c>
       <c r="B21" s="4" t="s">
         <v>242</v>
@@ -6132,7 +6132,7 @@
     </row>
     <row r="22" spans="1:35" x14ac:dyDescent="0.15">
       <c r="A22">
-        <v>42030014</v>
+        <v>42120014</v>
       </c>
       <c r="B22" t="s">
         <v>246</v>
@@ -6170,7 +6170,7 @@
     </row>
     <row r="23" spans="1:35" x14ac:dyDescent="0.15">
       <c r="A23">
-        <v>42030015</v>
+        <v>42120015</v>
       </c>
       <c r="B23" s="4" t="s">
         <v>245</v>
@@ -6208,7 +6208,7 @@
     </row>
     <row r="24" spans="1:35" x14ac:dyDescent="0.15">
       <c r="A24">
-        <v>42030016</v>
+        <v>42120016</v>
       </c>
       <c r="B24" t="s">
         <v>261</v>
@@ -6250,7 +6250,7 @@
     </row>
     <row r="25" spans="1:35" x14ac:dyDescent="0.15">
       <c r="A25">
-        <v>42030017</v>
+        <v>42120017</v>
       </c>
       <c r="B25" t="s">
         <v>268</v>
@@ -6288,7 +6288,7 @@
     </row>
     <row r="26" spans="1:35" x14ac:dyDescent="0.15">
       <c r="A26">
-        <v>42030018</v>
+        <v>42120018</v>
       </c>
       <c r="B26" t="s">
         <v>285</v>
@@ -6326,7 +6326,7 @@
     </row>
     <row r="27" spans="1:35" x14ac:dyDescent="0.15">
       <c r="A27">
-        <v>42030019</v>
+        <v>42120019</v>
       </c>
       <c r="B27" t="s">
         <v>281</v>
@@ -6364,7 +6364,7 @@
     </row>
     <row r="28" spans="1:35" x14ac:dyDescent="0.15">
       <c r="A28">
-        <v>42050001</v>
+        <v>42130001</v>
       </c>
       <c r="B28" t="s">
         <v>204</v>
@@ -6404,7 +6404,7 @@
     </row>
     <row r="29" spans="1:35" x14ac:dyDescent="0.15">
       <c r="A29">
-        <v>42050002</v>
+        <v>42130002</v>
       </c>
       <c r="B29" t="s">
         <v>204</v>
@@ -6444,7 +6444,7 @@
     </row>
     <row r="30" spans="1:35" x14ac:dyDescent="0.15">
       <c r="A30">
-        <v>42050003</v>
+        <v>42130003</v>
       </c>
       <c r="B30" t="s">
         <v>212</v>
@@ -6517,7 +6517,7 @@
     </row>
     <row r="31" spans="1:35" x14ac:dyDescent="0.15">
       <c r="A31">
-        <v>42050004</v>
+        <v>42130004</v>
       </c>
       <c r="B31" t="s">
         <v>228</v>
@@ -6555,7 +6555,7 @@
     </row>
     <row r="32" spans="1:35" x14ac:dyDescent="0.15">
       <c r="A32">
-        <v>42050005</v>
+        <v>42130005</v>
       </c>
       <c r="B32" t="s">
         <v>273</v>
@@ -6593,7 +6593,7 @@
     </row>
     <row r="33" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A33">
-        <v>42050006</v>
+        <v>42130006</v>
       </c>
       <c r="B33" t="s">
         <v>277</v>

</xml_diff>

<commit_message>
add ctrl-v and up/down func for gmcommand; add a base minigame based scenequest
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/SceneQuest.xlsx
+++ b/ConfigData/Xlsx/SceneQuest.xlsx
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="640" uniqueCount="319">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="651" uniqueCount="325">
   <si>
     <t>int</t>
     <phoneticPr fontId="18" type="noConversion"/>
@@ -1244,6 +1244,30 @@
   </si>
   <si>
     <t>batcrowd</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>gamecook</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>烹饪</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>游戏</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>小游戏id</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>int</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>MiniGameId</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -1986,7 +2010,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -2084,6 +2108,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="37" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="40" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -2131,7 +2158,26 @@
     <cellStyle name="着色 6" xfId="38" builtinId="49" customBuiltin="1"/>
     <cellStyle name="注释" xfId="15" builtinId="10" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="20">
+  <dxfs count="21">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -2249,12 +2295,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="表3" displayName="表3" ref="A3:AN48" totalsRowShown="0" headerRowDxfId="19">
-  <autoFilter ref="A3:AN48"/>
-  <sortState ref="A4:AN48">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="表3" displayName="表3" ref="A3:AO49" totalsRowShown="0" headerRowDxfId="20">
+  <autoFilter ref="A3:AO49"/>
+  <sortState ref="A4:AO48">
     <sortCondition ref="A3:A48"/>
   </sortState>
-  <tableColumns count="40">
+  <tableColumns count="41">
     <tableColumn id="1" name="Id"/>
     <tableColumn id="2" name="Name"/>
     <tableColumn id="28" name="Type"/>
@@ -2263,18 +2309,19 @@
     <tableColumn id="24" name="Ename"/>
     <tableColumn id="4" name="Figue"/>
     <tableColumn id="5" name="Script"/>
-    <tableColumn id="6" name="TriggerMulti" dataDxfId="18"/>
-    <tableColumn id="40" name="Catalog" dataDxfId="17"/>
-    <tableColumn id="35" name="TriggerHourBegin" dataDxfId="16"/>
-    <tableColumn id="34" name="TriggerHourEnd" dataDxfId="15"/>
-    <tableColumn id="36" name="TriggerFlagNoExist" dataDxfId="14"/>
-    <tableColumn id="38" name="TriggerFlagExist" dataDxfId="13"/>
-    <tableColumn id="39" name="TriggerRate" dataDxfId="12"/>
-    <tableColumn id="37" name="QuestNeed" dataDxfId="11"/>
+    <tableColumn id="6" name="TriggerMulti" dataDxfId="19"/>
+    <tableColumn id="40" name="Catalog" dataDxfId="18"/>
+    <tableColumn id="35" name="TriggerHourBegin" dataDxfId="17"/>
+    <tableColumn id="34" name="TriggerHourEnd" dataDxfId="16"/>
+    <tableColumn id="36" name="TriggerFlagNoExist" dataDxfId="15"/>
+    <tableColumn id="38" name="TriggerFlagExist" dataDxfId="14"/>
+    <tableColumn id="39" name="TriggerRate" dataDxfId="13"/>
+    <tableColumn id="37" name="QuestNeed" dataDxfId="12"/>
     <tableColumn id="7" name="EnemyId"/>
     <tableColumn id="8" name="BattleMap"/>
     <tableColumn id="32" name="SceneId"/>
     <tableColumn id="29" name="Position"/>
+    <tableColumn id="41" name="MiniGameId"/>
     <tableColumn id="9" name="RewardGold"/>
     <tableColumn id="10" name="RewardFood"/>
     <tableColumn id="11" name="RewardHealth"/>
@@ -2301,32 +2348,33 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="表3_5" displayName="表3_5" ref="A3:AN33" totalsRowShown="0" headerRowDxfId="10">
-  <autoFilter ref="A3:AN33"/>
-  <sortState ref="A4:AA6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="表3_5" displayName="表3_5" ref="A3:AO33" totalsRowShown="0" headerRowDxfId="11">
+  <autoFilter ref="A3:AO33"/>
+  <sortState ref="A4:AB6">
     <sortCondition ref="A3:A6"/>
   </sortState>
-  <tableColumns count="40">
+  <tableColumns count="41">
     <tableColumn id="1" name="Id"/>
     <tableColumn id="2" name="Name"/>
-    <tableColumn id="27" name="Type" dataDxfId="9"/>
+    <tableColumn id="27" name="Type" dataDxfId="10"/>
     <tableColumn id="3" name="Level"/>
     <tableColumn id="25" name="Danger"/>
     <tableColumn id="24" name="Ename"/>
     <tableColumn id="4" name="Figue"/>
     <tableColumn id="5" name="Script"/>
     <tableColumn id="6" name="TriggerMulti"/>
-    <tableColumn id="40" name="Catalog" dataDxfId="8"/>
-    <tableColumn id="35" name="TriggerHourBegin" dataDxfId="7"/>
-    <tableColumn id="34" name="TriggerHourEnd" dataDxfId="6"/>
-    <tableColumn id="37" name="TriggerFlagNoExist" dataDxfId="5"/>
-    <tableColumn id="38" name="TriggerFlagExist" dataDxfId="4"/>
-    <tableColumn id="39" name="TriggerRate" dataDxfId="3"/>
-    <tableColumn id="36" name="QuestNeed" dataDxfId="2"/>
+    <tableColumn id="40" name="Catalog" dataDxfId="9"/>
+    <tableColumn id="35" name="TriggerHourBegin" dataDxfId="8"/>
+    <tableColumn id="34" name="TriggerHourEnd" dataDxfId="7"/>
+    <tableColumn id="37" name="TriggerFlagNoExist" dataDxfId="6"/>
+    <tableColumn id="38" name="TriggerFlagExist" dataDxfId="5"/>
+    <tableColumn id="39" name="TriggerRate" dataDxfId="4"/>
+    <tableColumn id="36" name="QuestNeed" dataDxfId="3"/>
     <tableColumn id="7" name="EnemyId"/>
     <tableColumn id="8" name="BattleMap"/>
-    <tableColumn id="32" name="SceneId" dataDxfId="1"/>
-    <tableColumn id="29" name="Position" dataDxfId="0"/>
+    <tableColumn id="32" name="SceneId" dataDxfId="2"/>
+    <tableColumn id="29" name="Position" dataDxfId="1"/>
+    <tableColumn id="41" name="MiniGameId" dataDxfId="0"/>
     <tableColumn id="9" name="RewardGold"/>
     <tableColumn id="10" name="RewardFood"/>
     <tableColumn id="11" name="RewardHealth"/>
@@ -2673,11 +2721,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AN48"/>
+  <dimension ref="A1:AO49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B17" sqref="B17"/>
+      <pane ySplit="3" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="V49" sqref="V49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -2689,16 +2737,16 @@
     <col min="17" max="17" width="9.75" customWidth="1"/>
     <col min="18" max="18" width="6.75" customWidth="1"/>
     <col min="19" max="19" width="9.375" customWidth="1"/>
-    <col min="20" max="20" width="6.5" customWidth="1"/>
-    <col min="21" max="25" width="4.875" customWidth="1"/>
-    <col min="26" max="27" width="9.375" customWidth="1"/>
-    <col min="28" max="28" width="4.25" customWidth="1"/>
-    <col min="29" max="30" width="9.375" customWidth="1"/>
-    <col min="31" max="31" width="4.25" customWidth="1"/>
-    <col min="33" max="41" width="4.75" customWidth="1"/>
+    <col min="20" max="21" width="6.5" customWidth="1"/>
+    <col min="22" max="26" width="4.875" customWidth="1"/>
+    <col min="27" max="28" width="9.375" customWidth="1"/>
+    <col min="29" max="29" width="4.25" customWidth="1"/>
+    <col min="30" max="31" width="9.375" customWidth="1"/>
+    <col min="32" max="32" width="4.25" customWidth="1"/>
+    <col min="34" max="42" width="4.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:40" ht="69" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:41" ht="69" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="14" t="s">
         <v>79</v>
       </c>
@@ -2759,68 +2807,71 @@
       <c r="T1" s="18" t="s">
         <v>270</v>
       </c>
-      <c r="U1" s="15" t="s">
+      <c r="U1" s="18" t="s">
+        <v>322</v>
+      </c>
+      <c r="V1" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="V1" s="15" t="s">
+      <c r="W1" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="W1" s="15" t="s">
+      <c r="X1" s="15" t="s">
         <v>84</v>
       </c>
-      <c r="X1" s="15" t="s">
+      <c r="Y1" s="15" t="s">
         <v>85</v>
       </c>
-      <c r="Y1" s="15" t="s">
+      <c r="Z1" s="15" t="s">
         <v>86</v>
       </c>
-      <c r="Z1" s="15" t="s">
+      <c r="AA1" s="15" t="s">
         <v>87</v>
       </c>
-      <c r="AA1" s="15" t="s">
+      <c r="AB1" s="15" t="s">
         <v>77</v>
       </c>
-      <c r="AB1" s="15" t="s">
+      <c r="AC1" s="15" t="s">
         <v>195</v>
       </c>
-      <c r="AC1" s="15" t="s">
+      <c r="AD1" s="15" t="s">
         <v>137</v>
       </c>
-      <c r="AD1" s="15" t="s">
+      <c r="AE1" s="15" t="s">
         <v>224</v>
       </c>
-      <c r="AE1" s="15" t="s">
+      <c r="AF1" s="15" t="s">
         <v>156</v>
       </c>
-      <c r="AF1" s="16" t="s">
+      <c r="AG1" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="AG1" s="16" t="s">
+      <c r="AH1" s="16" t="s">
         <v>88</v>
       </c>
-      <c r="AH1" s="16" t="s">
+      <c r="AI1" s="16" t="s">
         <v>78</v>
       </c>
-      <c r="AI1" s="16" t="s">
+      <c r="AJ1" s="16" t="s">
         <v>89</v>
       </c>
-      <c r="AJ1" s="16" t="s">
+      <c r="AK1" s="16" t="s">
         <v>196</v>
       </c>
-      <c r="AK1" s="17" t="s">
+      <c r="AL1" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="AL1" s="17" t="s">
+      <c r="AM1" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="AM1" s="17" t="s">
+      <c r="AN1" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="AN1" s="17" t="s">
+      <c r="AO1" s="17" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:40" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:41" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>59</v>
       </c>
@@ -2881,14 +2932,14 @@
       <c r="T2" s="19" t="s">
         <v>271</v>
       </c>
-      <c r="U2" s="7" t="s">
+      <c r="U2" s="19" t="s">
+        <v>323</v>
+      </c>
+      <c r="V2" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="V2" s="7" t="s">
-        <v>0</v>
-      </c>
       <c r="W2" s="7" t="s">
-        <v>59</v>
+        <v>0</v>
       </c>
       <c r="X2" s="7" t="s">
         <v>59</v>
@@ -2897,26 +2948,26 @@
         <v>59</v>
       </c>
       <c r="Z2" s="7" t="s">
-        <v>0</v>
+        <v>59</v>
       </c>
       <c r="AA2" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="AB2" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="AB2" s="7" t="s">
+      <c r="AC2" s="7" t="s">
         <v>194</v>
       </c>
-      <c r="AC2" s="7" t="s">
+      <c r="AD2" s="7" t="s">
         <v>138</v>
       </c>
-      <c r="AD2" s="7" t="s">
+      <c r="AE2" s="7" t="s">
         <v>225</v>
       </c>
-      <c r="AE2" s="7" t="s">
+      <c r="AF2" s="7" t="s">
         <v>157</v>
       </c>
-      <c r="AF2" s="3" t="s">
-        <v>0</v>
-      </c>
       <c r="AG2" s="3" t="s">
         <v>0</v>
       </c>
@@ -2924,13 +2975,13 @@
         <v>0</v>
       </c>
       <c r="AI2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="AJ2" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="AJ2" s="3" t="s">
+      <c r="AK2" s="3" t="s">
         <v>197</v>
-      </c>
-      <c r="AK2" s="9" t="s">
-        <v>27</v>
       </c>
       <c r="AL2" s="9" t="s">
         <v>27</v>
@@ -2941,8 +2992,11 @@
       <c r="AN2" s="9" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="3" spans="1:40" x14ac:dyDescent="0.15">
+      <c r="AO2" s="9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:41" x14ac:dyDescent="0.15">
       <c r="A3" s="8" t="s">
         <v>64</v>
       </c>
@@ -3003,68 +3057,71 @@
       <c r="T3" s="20" t="s">
         <v>272</v>
       </c>
-      <c r="U3" s="6" t="s">
+      <c r="U3" s="20" t="s">
+        <v>324</v>
+      </c>
+      <c r="V3" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="V3" s="6" t="s">
+      <c r="W3" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="W3" s="6" t="s">
+      <c r="X3" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="X3" s="6" t="s">
+      <c r="Y3" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="Y3" s="6" t="s">
+      <c r="Z3" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="Z3" s="6" t="s">
+      <c r="AA3" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="AA3" s="6" t="s">
+      <c r="AB3" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="AB3" s="6" t="s">
+      <c r="AC3" s="6" t="s">
         <v>193</v>
       </c>
-      <c r="AC3" s="6" t="s">
+      <c r="AD3" s="6" t="s">
         <v>139</v>
       </c>
-      <c r="AD3" s="6" t="s">
+      <c r="AE3" s="6" t="s">
         <v>226</v>
       </c>
-      <c r="AE3" s="6" t="s">
+      <c r="AF3" s="6" t="s">
         <v>158</v>
       </c>
-      <c r="AF3" s="2" t="s">
+      <c r="AG3" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="AG3" s="2" t="s">
+      <c r="AH3" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="AH3" s="2" t="s">
+      <c r="AI3" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="AI3" s="2" t="s">
+      <c r="AJ3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="AJ3" s="2" t="s">
+      <c r="AK3" s="2" t="s">
         <v>198</v>
       </c>
-      <c r="AK3" s="8" t="s">
+      <c r="AL3" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="AL3" s="8" t="s">
+      <c r="AM3" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="AM3" s="8" t="s">
+      <c r="AN3" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="AN3" s="8" t="s">
+      <c r="AO3" s="8" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:40" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:41" x14ac:dyDescent="0.15">
       <c r="A4">
         <v>42000001</v>
       </c>
@@ -3104,9 +3161,7 @@
         <v>13020001</v>
       </c>
       <c r="T4" s="12"/>
-      <c r="U4">
-        <v>100</v>
-      </c>
+      <c r="U4" s="12"/>
       <c r="V4">
         <v>100</v>
       </c>
@@ -3120,10 +3175,10 @@
         <v>100</v>
       </c>
       <c r="Z4">
+        <v>100</v>
+      </c>
+      <c r="AA4">
         <v>22011180</v>
-      </c>
-      <c r="AF4">
-        <v>100</v>
       </c>
       <c r="AG4">
         <v>100</v>
@@ -3134,8 +3189,11 @@
       <c r="AI4">
         <v>100</v>
       </c>
-    </row>
-    <row r="5" spans="1:40" x14ac:dyDescent="0.15">
+      <c r="AJ4">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" spans="1:41" x14ac:dyDescent="0.15">
       <c r="A5" s="10">
         <v>42000002</v>
       </c>
@@ -3166,7 +3224,7 @@
       <c r="O5" s="5"/>
       <c r="P5" s="5"/>
     </row>
-    <row r="6" spans="1:40" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:41" x14ac:dyDescent="0.15">
       <c r="A6" s="10">
         <v>42000003</v>
       </c>
@@ -3197,7 +3255,7 @@
       <c r="O6" s="5"/>
       <c r="P6" s="5"/>
     </row>
-    <row r="7" spans="1:40" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:41" x14ac:dyDescent="0.15">
       <c r="A7" s="10">
         <v>42000004</v>
       </c>
@@ -3228,7 +3286,7 @@
       <c r="O7" s="5"/>
       <c r="P7" s="5"/>
     </row>
-    <row r="8" spans="1:40" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:41" x14ac:dyDescent="0.15">
       <c r="A8" s="10">
         <v>42000005</v>
       </c>
@@ -3258,14 +3316,14 @@
       <c r="N8" s="5"/>
       <c r="O8" s="5"/>
       <c r="P8" s="5"/>
-      <c r="AK8">
+      <c r="AL8">
         <v>-100</v>
       </c>
-      <c r="AM8">
+      <c r="AN8">
         <v>100</v>
       </c>
     </row>
-    <row r="9" spans="1:40" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:41" x14ac:dyDescent="0.15">
       <c r="A9" s="10">
         <v>42000006</v>
       </c>
@@ -3295,14 +3353,14 @@
       <c r="N9" s="5"/>
       <c r="O9" s="5"/>
       <c r="P9" s="5"/>
-      <c r="AK9">
+      <c r="AL9">
         <v>-100</v>
       </c>
-      <c r="AN9">
+      <c r="AO9">
         <v>100</v>
       </c>
     </row>
-    <row r="10" spans="1:40" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:41" x14ac:dyDescent="0.15">
       <c r="A10" s="10">
         <v>42000007</v>
       </c>
@@ -3332,14 +3390,14 @@
       <c r="N10" s="5"/>
       <c r="O10" s="5"/>
       <c r="P10" s="5"/>
-      <c r="AK10">
+      <c r="AL10">
         <v>-100</v>
       </c>
-      <c r="AL10">
+      <c r="AM10">
         <v>100</v>
       </c>
     </row>
-    <row r="11" spans="1:40" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:41" x14ac:dyDescent="0.15">
       <c r="A11">
         <v>42010001</v>
       </c>
@@ -3372,7 +3430,7 @@
       <c r="O11" s="5"/>
       <c r="P11" s="5"/>
     </row>
-    <row r="12" spans="1:40" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:41" x14ac:dyDescent="0.15">
       <c r="A12">
         <v>42010002</v>
       </c>
@@ -3408,7 +3466,7 @@
       <c r="O12" s="5"/>
       <c r="P12" s="5"/>
     </row>
-    <row r="13" spans="1:40" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:41" x14ac:dyDescent="0.15">
       <c r="A13">
         <v>42010003</v>
       </c>
@@ -3449,17 +3507,17 @@
       <c r="R13" t="s">
         <v>42</v>
       </c>
-      <c r="U13">
+      <c r="V13">
         <v>70</v>
       </c>
-      <c r="V13">
+      <c r="W13">
         <v>100</v>
       </c>
-      <c r="AH13">
+      <c r="AI13">
         <v>70</v>
       </c>
     </row>
-    <row r="14" spans="1:40" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:41" x14ac:dyDescent="0.15">
       <c r="A14">
         <v>42010004</v>
       </c>
@@ -3494,17 +3552,17 @@
       <c r="N14" s="5"/>
       <c r="O14" s="5"/>
       <c r="P14" s="5"/>
-      <c r="Y14">
-        <v>30</v>
-      </c>
-      <c r="AF14">
+      <c r="Z14">
         <v>30</v>
       </c>
       <c r="AG14">
         <v>30</v>
       </c>
-    </row>
-    <row r="15" spans="1:40" x14ac:dyDescent="0.15">
+      <c r="AH14">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15" spans="1:41" x14ac:dyDescent="0.15">
       <c r="A15">
         <v>42010005</v>
       </c>
@@ -3536,14 +3594,14 @@
       <c r="N15" s="5"/>
       <c r="O15" s="5"/>
       <c r="P15" s="5"/>
-      <c r="V15">
+      <c r="W15">
         <v>100</v>
       </c>
-      <c r="X15">
+      <c r="Y15">
         <v>100</v>
       </c>
     </row>
-    <row r="16" spans="1:40" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:41" x14ac:dyDescent="0.15">
       <c r="A16">
         <v>42010006</v>
       </c>
@@ -3584,17 +3642,17 @@
       <c r="R16" t="s">
         <v>42</v>
       </c>
-      <c r="U16">
+      <c r="V16">
         <v>100</v>
       </c>
-      <c r="Y16">
+      <c r="Z16">
         <v>50</v>
       </c>
-      <c r="AH16">
+      <c r="AI16">
         <v>100</v>
       </c>
     </row>
-    <row r="17" spans="1:35" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A17">
         <v>42010007</v>
       </c>
@@ -3629,17 +3687,17 @@
       <c r="N17" s="5"/>
       <c r="O17" s="5"/>
       <c r="P17" s="5"/>
-      <c r="U17">
+      <c r="V17">
         <v>250</v>
       </c>
-      <c r="AF17">
+      <c r="AG17">
         <v>250</v>
       </c>
-      <c r="AI17">
+      <c r="AJ17">
         <v>50</v>
       </c>
     </row>
-    <row r="18" spans="1:35" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A18">
         <v>42010008</v>
       </c>
@@ -3671,14 +3729,14 @@
       <c r="N18" s="5"/>
       <c r="O18" s="5"/>
       <c r="P18" s="5"/>
-      <c r="V18">
+      <c r="W18">
         <v>100</v>
       </c>
-      <c r="AA18">
+      <c r="AB18">
         <v>23000002</v>
       </c>
     </row>
-    <row r="19" spans="1:35" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A19">
         <v>42010009</v>
       </c>
@@ -3710,11 +3768,11 @@
       <c r="N19" s="5"/>
       <c r="O19" s="5"/>
       <c r="P19" s="5"/>
-      <c r="AA19">
+      <c r="AB19">
         <v>23000003</v>
       </c>
     </row>
-    <row r="20" spans="1:35" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A20">
         <v>42010010</v>
       </c>
@@ -3746,14 +3804,14 @@
       <c r="N20" s="5"/>
       <c r="O20" s="5"/>
       <c r="P20" s="5"/>
-      <c r="AA20">
+      <c r="AB20">
         <v>23000004</v>
       </c>
-      <c r="AH20">
+      <c r="AI20">
         <v>50</v>
       </c>
     </row>
-    <row r="21" spans="1:35" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A21">
         <v>42010011</v>
       </c>
@@ -3785,14 +3843,14 @@
       <c r="N21" s="5"/>
       <c r="O21" s="5"/>
       <c r="P21" s="5"/>
-      <c r="X21">
+      <c r="Y21">
         <v>150</v>
       </c>
-      <c r="AA21">
+      <c r="AB21">
         <v>23000005</v>
       </c>
     </row>
-    <row r="22" spans="1:35" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A22">
         <v>42010012</v>
       </c>
@@ -3833,17 +3891,17 @@
       <c r="R22" t="s">
         <v>16</v>
       </c>
-      <c r="U22">
-        <v>100</v>
-      </c>
       <c r="V22">
         <v>100</v>
       </c>
-      <c r="AH22">
+      <c r="W22">
+        <v>100</v>
+      </c>
+      <c r="AI22">
         <v>150</v>
       </c>
     </row>
-    <row r="23" spans="1:35" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A23">
         <v>42010013</v>
       </c>
@@ -3884,17 +3942,17 @@
       <c r="R23" t="s">
         <v>42</v>
       </c>
-      <c r="U23">
+      <c r="V23">
         <v>50</v>
       </c>
-      <c r="V23">
+      <c r="W23">
         <v>150</v>
       </c>
-      <c r="AH23">
+      <c r="AI23">
         <v>100</v>
       </c>
     </row>
-    <row r="24" spans="1:35" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A24">
         <v>42010014</v>
       </c>
@@ -3935,23 +3993,23 @@
       <c r="R24" t="s">
         <v>16</v>
       </c>
-      <c r="U24">
+      <c r="V24">
         <v>100</v>
       </c>
-      <c r="Y24">
+      <c r="Z24">
         <v>100</v>
       </c>
-      <c r="AA24">
+      <c r="AB24">
         <v>23000101</v>
-      </c>
-      <c r="AH24">
-        <v>100</v>
       </c>
       <c r="AI24">
         <v>100</v>
       </c>
-    </row>
-    <row r="25" spans="1:35" x14ac:dyDescent="0.15">
+      <c r="AJ24">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="25" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A25">
         <v>42010015</v>
       </c>
@@ -3986,11 +4044,11 @@
       <c r="N25" s="5"/>
       <c r="O25" s="5"/>
       <c r="P25" s="5"/>
-      <c r="AH25">
+      <c r="AI25">
         <v>80</v>
       </c>
     </row>
-    <row r="26" spans="1:35" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A26">
         <v>42010016</v>
       </c>
@@ -4022,11 +4080,11 @@
       <c r="N26" s="5"/>
       <c r="O26" s="5"/>
       <c r="P26" s="5"/>
-      <c r="V26">
+      <c r="W26">
         <v>50</v>
       </c>
     </row>
-    <row r="27" spans="1:35" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A27">
         <v>42010017</v>
       </c>
@@ -4067,23 +4125,23 @@
       <c r="R27" t="s">
         <v>16</v>
       </c>
-      <c r="U27">
+      <c r="V27">
         <v>200</v>
       </c>
-      <c r="V27">
+      <c r="W27">
         <v>100</v>
       </c>
-      <c r="Y27">
+      <c r="Z27">
         <v>100</v>
       </c>
-      <c r="AA27">
+      <c r="AB27">
         <v>23000102</v>
       </c>
-      <c r="AH27">
+      <c r="AI27">
         <v>100</v>
       </c>
     </row>
-    <row r="28" spans="1:35" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A28">
         <v>42010018</v>
       </c>
@@ -4118,7 +4176,7 @@
       <c r="O28" s="5"/>
       <c r="P28" s="5"/>
     </row>
-    <row r="29" spans="1:35" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A29">
         <v>42010019</v>
       </c>
@@ -4155,14 +4213,14 @@
       <c r="N29" s="5"/>
       <c r="O29" s="5"/>
       <c r="P29" s="5"/>
-      <c r="AG29">
+      <c r="AH29">
         <v>100</v>
       </c>
-      <c r="AH29">
+      <c r="AI29">
         <v>50</v>
       </c>
     </row>
-    <row r="30" spans="1:35" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A30">
         <v>42010020</v>
       </c>
@@ -4199,14 +4257,14 @@
       <c r="N30" s="5"/>
       <c r="O30" s="5"/>
       <c r="P30" s="5"/>
-      <c r="AG30">
+      <c r="AH30">
         <v>50</v>
       </c>
-      <c r="AH30">
+      <c r="AI30">
         <v>100</v>
       </c>
     </row>
-    <row r="31" spans="1:35" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A31">
         <v>42010021</v>
       </c>
@@ -4241,11 +4299,11 @@
       <c r="N31" s="5"/>
       <c r="O31" s="5"/>
       <c r="P31" s="5"/>
-      <c r="AI31">
+      <c r="AJ31">
         <v>200</v>
       </c>
     </row>
-    <row r="32" spans="1:35" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A32">
         <v>42010022</v>
       </c>
@@ -4286,17 +4344,17 @@
       <c r="R32" t="s">
         <v>16</v>
       </c>
-      <c r="Y32">
+      <c r="Z32">
         <v>100</v>
       </c>
-      <c r="Z32">
+      <c r="AA32">
         <v>22031101</v>
       </c>
-      <c r="AH32">
+      <c r="AI32">
         <v>150</v>
       </c>
     </row>
-    <row r="33" spans="1:36" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:37" x14ac:dyDescent="0.15">
       <c r="A33">
         <v>42010023</v>
       </c>
@@ -4331,17 +4389,17 @@
       <c r="N33" s="5"/>
       <c r="O33" s="5"/>
       <c r="P33" s="5"/>
-      <c r="V33">
+      <c r="W33">
         <v>200</v>
       </c>
-      <c r="W33">
+      <c r="X33">
         <v>100</v>
       </c>
-      <c r="AH33">
+      <c r="AI33">
         <v>100</v>
       </c>
     </row>
-    <row r="34" spans="1:36" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:37" x14ac:dyDescent="0.15">
       <c r="A34">
         <v>42010024</v>
       </c>
@@ -4373,11 +4431,11 @@
       <c r="N34" s="5"/>
       <c r="O34" s="5"/>
       <c r="P34" s="5"/>
-      <c r="AB34">
+      <c r="AC34">
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:36" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:37" x14ac:dyDescent="0.15">
       <c r="A35">
         <v>42010025</v>
       </c>
@@ -4409,11 +4467,11 @@
       <c r="N35" s="5"/>
       <c r="O35" s="5"/>
       <c r="P35" s="5"/>
-      <c r="V35">
+      <c r="W35">
         <v>150</v>
       </c>
     </row>
-    <row r="36" spans="1:36" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:37" x14ac:dyDescent="0.15">
       <c r="A36">
         <v>42010026</v>
       </c>
@@ -4445,11 +4503,11 @@
       <c r="N36" s="5"/>
       <c r="O36" s="5"/>
       <c r="P36" s="5"/>
-      <c r="W36">
+      <c r="X36">
         <v>70</v>
       </c>
     </row>
-    <row r="37" spans="1:36" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:37" x14ac:dyDescent="0.15">
       <c r="A37">
         <v>42010027</v>
       </c>
@@ -4481,11 +4539,11 @@
       <c r="N37" s="5"/>
       <c r="O37" s="5"/>
       <c r="P37" s="5"/>
-      <c r="V37">
+      <c r="W37">
         <v>70</v>
       </c>
     </row>
-    <row r="38" spans="1:36" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:37" x14ac:dyDescent="0.15">
       <c r="A38">
         <v>42010028</v>
       </c>
@@ -4523,11 +4581,11 @@
       <c r="S38">
         <v>13010004</v>
       </c>
-      <c r="AH38">
+      <c r="AI38">
         <v>150</v>
       </c>
     </row>
-    <row r="39" spans="1:36" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:37" x14ac:dyDescent="0.15">
       <c r="A39">
         <v>42010029</v>
       </c>
@@ -4560,7 +4618,7 @@
       <c r="O39" s="5"/>
       <c r="P39" s="5"/>
     </row>
-    <row r="40" spans="1:36" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:37" x14ac:dyDescent="0.15">
       <c r="A40">
         <v>42010030</v>
       </c>
@@ -4601,23 +4659,23 @@
       <c r="R40" t="s">
         <v>42</v>
       </c>
-      <c r="U40">
+      <c r="V40">
         <v>100</v>
       </c>
-      <c r="V40">
+      <c r="W40">
         <v>150</v>
       </c>
-      <c r="Y40">
+      <c r="Z40">
         <v>100</v>
       </c>
-      <c r="AH40">
+      <c r="AI40">
         <v>100</v>
       </c>
-      <c r="AI40">
+      <c r="AJ40">
         <v>150</v>
       </c>
     </row>
-    <row r="41" spans="1:36" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:37" x14ac:dyDescent="0.15">
       <c r="A41">
         <v>42020001</v>
       </c>
@@ -4658,20 +4716,20 @@
       <c r="R41" t="s">
         <v>16</v>
       </c>
-      <c r="Y41">
+      <c r="Z41">
         <v>100</v>
       </c>
-      <c r="AC41">
+      <c r="AD41">
         <v>1</v>
-      </c>
-      <c r="AH41">
-        <v>200</v>
       </c>
       <c r="AI41">
         <v>200</v>
       </c>
-    </row>
-    <row r="42" spans="1:36" x14ac:dyDescent="0.15">
+      <c r="AJ41">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="42" spans="1:37" x14ac:dyDescent="0.15">
       <c r="A42">
         <v>42020002</v>
       </c>
@@ -4712,23 +4770,23 @@
       <c r="R42" t="s">
         <v>16</v>
       </c>
-      <c r="U42">
+      <c r="V42">
         <v>200</v>
       </c>
-      <c r="V42">
+      <c r="W42">
         <v>50</v>
       </c>
-      <c r="AA42">
+      <c r="AB42">
         <v>23000102</v>
-      </c>
-      <c r="AH42">
-        <v>150</v>
       </c>
       <c r="AI42">
         <v>150</v>
       </c>
-    </row>
-    <row r="43" spans="1:36" x14ac:dyDescent="0.15">
+      <c r="AJ42">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="43" spans="1:37" x14ac:dyDescent="0.15">
       <c r="A43">
         <v>42020003</v>
       </c>
@@ -4763,14 +4821,14 @@
       <c r="N43" s="5"/>
       <c r="O43" s="5"/>
       <c r="P43" s="5"/>
-      <c r="AF43">
+      <c r="AG43">
         <v>100</v>
       </c>
-      <c r="AH43">
+      <c r="AI43">
         <v>100</v>
       </c>
     </row>
-    <row r="44" spans="1:36" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:37" x14ac:dyDescent="0.15">
       <c r="A44">
         <v>42020004</v>
       </c>
@@ -4805,14 +4863,14 @@
       <c r="N44" s="5"/>
       <c r="O44" s="5"/>
       <c r="P44" s="5"/>
-      <c r="AB44">
+      <c r="AC44">
         <v>1</v>
       </c>
-      <c r="AJ44">
+      <c r="AK44">
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:36" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:37" x14ac:dyDescent="0.15">
       <c r="A45">
         <v>42020005</v>
       </c>
@@ -4853,20 +4911,20 @@
       <c r="R45" t="s">
         <v>16</v>
       </c>
-      <c r="U45">
-        <v>150</v>
-      </c>
       <c r="V45">
         <v>150</v>
       </c>
-      <c r="AF45">
-        <v>200</v>
+      <c r="W45">
+        <v>150</v>
       </c>
       <c r="AG45">
         <v>200</v>
       </c>
-    </row>
-    <row r="46" spans="1:36" x14ac:dyDescent="0.15">
+      <c r="AH45">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="46" spans="1:37" x14ac:dyDescent="0.15">
       <c r="A46">
         <v>42020006</v>
       </c>
@@ -4907,17 +4965,17 @@
       <c r="R46" t="s">
         <v>16</v>
       </c>
-      <c r="U46">
+      <c r="V46">
         <v>300</v>
       </c>
-      <c r="Y46">
+      <c r="Z46">
         <v>200</v>
       </c>
-      <c r="AH46">
+      <c r="AI46">
         <v>300</v>
       </c>
     </row>
-    <row r="47" spans="1:36" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:37" x14ac:dyDescent="0.15">
       <c r="A47">
         <v>42020007</v>
       </c>
@@ -4950,7 +5008,7 @@
       <c r="O47" s="5"/>
       <c r="P47" s="5"/>
     </row>
-    <row r="48" spans="1:36" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:37" x14ac:dyDescent="0.15">
       <c r="A48">
         <v>42020008</v>
       </c>
@@ -4982,6 +5040,48 @@
       <c r="N48" s="5"/>
       <c r="O48" s="5"/>
       <c r="P48" s="5"/>
+    </row>
+    <row r="49" spans="1:33" x14ac:dyDescent="0.15">
+      <c r="A49">
+        <v>42030001</v>
+      </c>
+      <c r="B49" t="s">
+        <v>320</v>
+      </c>
+      <c r="C49">
+        <v>3</v>
+      </c>
+      <c r="D49">
+        <v>0</v>
+      </c>
+      <c r="F49" t="s">
+        <v>319</v>
+      </c>
+      <c r="G49" t="s">
+        <v>314</v>
+      </c>
+      <c r="H49" t="s">
+        <v>319</v>
+      </c>
+      <c r="I49" s="5"/>
+      <c r="J49" s="33" t="s">
+        <v>321</v>
+      </c>
+      <c r="K49" s="5"/>
+      <c r="L49" s="5"/>
+      <c r="M49" s="5"/>
+      <c r="N49" s="5"/>
+      <c r="O49" s="5"/>
+      <c r="P49" s="5"/>
+      <c r="U49">
+        <v>17000001</v>
+      </c>
+      <c r="V49">
+        <v>100</v>
+      </c>
+      <c r="AG49">
+        <v>50</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
@@ -4996,11 +5096,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AN33"/>
+  <dimension ref="A1:AO33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B29" sqref="B29"/>
+      <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -5013,17 +5113,17 @@
     <col min="17" max="17" width="9.75" customWidth="1"/>
     <col min="18" max="18" width="6.625" customWidth="1"/>
     <col min="19" max="19" width="9.25" customWidth="1"/>
-    <col min="20" max="20" width="5.75" customWidth="1"/>
-    <col min="21" max="25" width="4.125" customWidth="1"/>
-    <col min="26" max="26" width="9.75" customWidth="1"/>
-    <col min="27" max="27" width="7.5" customWidth="1"/>
-    <col min="28" max="28" width="5.125" customWidth="1"/>
-    <col min="29" max="30" width="9.375" customWidth="1"/>
-    <col min="31" max="31" width="7.375" customWidth="1"/>
-    <col min="33" max="41" width="5" customWidth="1"/>
+    <col min="20" max="21" width="5.75" customWidth="1"/>
+    <col min="22" max="26" width="4.125" customWidth="1"/>
+    <col min="27" max="27" width="9.75" customWidth="1"/>
+    <col min="28" max="28" width="7.5" customWidth="1"/>
+    <col min="29" max="29" width="5.125" customWidth="1"/>
+    <col min="30" max="31" width="9.375" customWidth="1"/>
+    <col min="32" max="32" width="7.375" customWidth="1"/>
+    <col min="34" max="42" width="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:40" ht="69.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:41" ht="69.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="14" t="s">
         <v>79</v>
       </c>
@@ -5084,68 +5184,71 @@
       <c r="T1" s="18" t="s">
         <v>270</v>
       </c>
-      <c r="U1" s="15" t="s">
+      <c r="U1" s="18" t="s">
+        <v>322</v>
+      </c>
+      <c r="V1" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="V1" s="15" t="s">
+      <c r="W1" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="W1" s="15" t="s">
+      <c r="X1" s="15" t="s">
         <v>84</v>
       </c>
-      <c r="X1" s="15" t="s">
+      <c r="Y1" s="15" t="s">
         <v>85</v>
       </c>
-      <c r="Y1" s="15" t="s">
+      <c r="Z1" s="15" t="s">
         <v>86</v>
       </c>
-      <c r="Z1" s="15" t="s">
+      <c r="AA1" s="15" t="s">
         <v>87</v>
       </c>
-      <c r="AA1" s="15" t="s">
+      <c r="AB1" s="15" t="s">
         <v>77</v>
       </c>
-      <c r="AB1" s="15" t="s">
+      <c r="AC1" s="15" t="s">
         <v>195</v>
       </c>
-      <c r="AC1" s="15" t="s">
+      <c r="AD1" s="15" t="s">
         <v>137</v>
       </c>
-      <c r="AD1" s="15" t="s">
+      <c r="AE1" s="15" t="s">
         <v>224</v>
       </c>
-      <c r="AE1" s="15" t="s">
+      <c r="AF1" s="15" t="s">
         <v>156</v>
       </c>
-      <c r="AF1" s="16" t="s">
+      <c r="AG1" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="AG1" s="16" t="s">
+      <c r="AH1" s="16" t="s">
         <v>88</v>
       </c>
-      <c r="AH1" s="16" t="s">
+      <c r="AI1" s="16" t="s">
         <v>78</v>
       </c>
-      <c r="AI1" s="16" t="s">
+      <c r="AJ1" s="16" t="s">
         <v>89</v>
       </c>
-      <c r="AJ1" s="16" t="s">
+      <c r="AK1" s="16" t="s">
         <v>195</v>
       </c>
-      <c r="AK1" s="17" t="s">
+      <c r="AL1" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="AL1" s="17" t="s">
+      <c r="AM1" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="AM1" s="17" t="s">
+      <c r="AN1" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="AN1" s="17" t="s">
+      <c r="AO1" s="17" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:40" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:41" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>59</v>
       </c>
@@ -5206,14 +5309,14 @@
       <c r="T2" s="19" t="s">
         <v>271</v>
       </c>
-      <c r="U2" s="7" t="s">
+      <c r="U2" s="19" t="s">
+        <v>323</v>
+      </c>
+      <c r="V2" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="V2" s="7" t="s">
-        <v>0</v>
-      </c>
       <c r="W2" s="7" t="s">
-        <v>59</v>
+        <v>0</v>
       </c>
       <c r="X2" s="7" t="s">
         <v>59</v>
@@ -5222,26 +5325,26 @@
         <v>59</v>
       </c>
       <c r="Z2" s="7" t="s">
-        <v>0</v>
+        <v>59</v>
       </c>
       <c r="AA2" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="AB2" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="AB2" s="7" t="s">
+      <c r="AC2" s="7" t="s">
         <v>194</v>
       </c>
-      <c r="AC2" s="7" t="s">
+      <c r="AD2" s="7" t="s">
         <v>138</v>
       </c>
-      <c r="AD2" s="7" t="s">
+      <c r="AE2" s="7" t="s">
         <v>225</v>
       </c>
-      <c r="AE2" s="7" t="s">
+      <c r="AF2" s="7" t="s">
         <v>157</v>
       </c>
-      <c r="AF2" s="3" t="s">
-        <v>0</v>
-      </c>
       <c r="AG2" s="3" t="s">
         <v>0</v>
       </c>
@@ -5249,13 +5352,13 @@
         <v>0</v>
       </c>
       <c r="AI2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="AJ2" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="AJ2" s="3" t="s">
+      <c r="AK2" s="3" t="s">
         <v>197</v>
-      </c>
-      <c r="AK2" s="9" t="s">
-        <v>27</v>
       </c>
       <c r="AL2" s="9" t="s">
         <v>27</v>
@@ -5266,8 +5369,11 @@
       <c r="AN2" s="9" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="3" spans="1:40" x14ac:dyDescent="0.15">
+      <c r="AO2" s="9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:41" x14ac:dyDescent="0.15">
       <c r="A3" s="8" t="s">
         <v>64</v>
       </c>
@@ -5328,68 +5434,71 @@
       <c r="T3" s="20" t="s">
         <v>272</v>
       </c>
-      <c r="U3" s="6" t="s">
+      <c r="U3" s="20" t="s">
+        <v>324</v>
+      </c>
+      <c r="V3" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="V3" s="6" t="s">
+      <c r="W3" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="W3" s="6" t="s">
+      <c r="X3" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="X3" s="6" t="s">
+      <c r="Y3" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="Y3" s="6" t="s">
+      <c r="Z3" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="Z3" s="6" t="s">
+      <c r="AA3" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="AA3" s="6" t="s">
+      <c r="AB3" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="AB3" s="6" t="s">
+      <c r="AC3" s="6" t="s">
         <v>193</v>
       </c>
-      <c r="AC3" s="6" t="s">
+      <c r="AD3" s="6" t="s">
         <v>139</v>
       </c>
-      <c r="AD3" s="6" t="s">
+      <c r="AE3" s="6" t="s">
         <v>226</v>
       </c>
-      <c r="AE3" s="6" t="s">
+      <c r="AF3" s="6" t="s">
         <v>158</v>
       </c>
-      <c r="AF3" s="2" t="s">
+      <c r="AG3" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="AG3" s="2" t="s">
+      <c r="AH3" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="AH3" s="2" t="s">
+      <c r="AI3" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="AI3" s="2" t="s">
+      <c r="AJ3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="AJ3" s="2" t="s">
+      <c r="AK3" s="2" t="s">
         <v>198</v>
       </c>
-      <c r="AK3" s="8" t="s">
+      <c r="AL3" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="AL3" s="8" t="s">
+      <c r="AM3" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="AM3" s="8" t="s">
+      <c r="AN3" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="AN3" s="8" t="s">
+      <c r="AO3" s="8" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:40" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:41" x14ac:dyDescent="0.15">
       <c r="A4" s="10">
         <v>42110001</v>
       </c>
@@ -5424,17 +5533,18 @@
       <c r="R4" s="11"/>
       <c r="S4" s="13"/>
       <c r="T4" s="13"/>
-      <c r="AK4">
+      <c r="U4" s="13"/>
+      <c r="AL4">
         <v>-300</v>
-      </c>
-      <c r="AM4">
-        <v>1000</v>
       </c>
       <c r="AN4">
         <v>1000</v>
       </c>
-    </row>
-    <row r="5" spans="1:40" x14ac:dyDescent="0.15">
+      <c r="AO4">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:41" x14ac:dyDescent="0.15">
       <c r="A5" s="10">
         <v>42110002</v>
       </c>
@@ -5469,14 +5579,15 @@
       <c r="R5" s="11"/>
       <c r="S5" s="13"/>
       <c r="T5" s="13"/>
-      <c r="AK5">
+      <c r="U5" s="13"/>
+      <c r="AL5">
         <v>-200</v>
       </c>
-      <c r="AL5">
+      <c r="AM5">
         <v>1000</v>
       </c>
     </row>
-    <row r="6" spans="1:40" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:41" x14ac:dyDescent="0.15">
       <c r="A6" s="10">
         <v>42110003</v>
       </c>
@@ -5511,8 +5622,9 @@
       <c r="R6" s="11"/>
       <c r="S6" s="13"/>
       <c r="T6" s="13"/>
-    </row>
-    <row r="7" spans="1:40" x14ac:dyDescent="0.15">
+      <c r="U6" s="13"/>
+    </row>
+    <row r="7" spans="1:41" x14ac:dyDescent="0.15">
       <c r="A7" s="10">
         <v>42110004</v>
       </c>
@@ -5545,7 +5657,7 @@
       <c r="O7" s="5"/>
       <c r="P7" s="5"/>
     </row>
-    <row r="8" spans="1:40" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:41" x14ac:dyDescent="0.15">
       <c r="A8" s="10">
         <v>42110005</v>
       </c>
@@ -5580,8 +5692,9 @@
       <c r="R8" s="11"/>
       <c r="S8" s="13"/>
       <c r="T8" s="13"/>
-    </row>
-    <row r="9" spans="1:40" x14ac:dyDescent="0.15">
+      <c r="U8" s="13"/>
+    </row>
+    <row r="9" spans="1:41" x14ac:dyDescent="0.15">
       <c r="A9">
         <v>42120001</v>
       </c>
@@ -5618,14 +5731,15 @@
       <c r="R9" s="4"/>
       <c r="S9" s="12"/>
       <c r="T9" s="12"/>
-      <c r="U9">
+      <c r="U9" s="12"/>
+      <c r="V9">
         <v>50</v>
       </c>
-      <c r="AD9">
+      <c r="AE9">
         <v>12000001</v>
       </c>
     </row>
-    <row r="10" spans="1:40" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:41" x14ac:dyDescent="0.15">
       <c r="A10">
         <v>42120002</v>
       </c>
@@ -5669,11 +5783,12 @@
       </c>
       <c r="S10" s="12"/>
       <c r="T10" s="12"/>
-      <c r="AC10">
+      <c r="U10" s="12"/>
+      <c r="AD10">
         <v>43020101</v>
       </c>
     </row>
-    <row r="11" spans="1:40" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:41" x14ac:dyDescent="0.15">
       <c r="A11">
         <v>42120003</v>
       </c>
@@ -5710,8 +5825,9 @@
       <c r="R11" s="12"/>
       <c r="S11" s="12"/>
       <c r="T11" s="12"/>
-    </row>
-    <row r="12" spans="1:40" x14ac:dyDescent="0.15">
+      <c r="U11" s="12"/>
+    </row>
+    <row r="12" spans="1:41" x14ac:dyDescent="0.15">
       <c r="A12">
         <v>42120004</v>
       </c>
@@ -5746,14 +5862,15 @@
       <c r="R12" s="12"/>
       <c r="S12" s="12"/>
       <c r="T12" s="12"/>
-      <c r="AC12">
+      <c r="U12" s="12"/>
+      <c r="AD12">
         <v>43020102</v>
       </c>
-      <c r="AE12" t="s">
+      <c r="AF12" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="13" spans="1:40" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:41" x14ac:dyDescent="0.15">
       <c r="A13">
         <v>42120005</v>
       </c>
@@ -5790,20 +5907,21 @@
       <c r="R13" s="12"/>
       <c r="S13" s="12"/>
       <c r="T13" s="12"/>
-      <c r="U13">
+      <c r="U13" s="12"/>
+      <c r="V13">
         <v>300</v>
       </c>
-      <c r="V13">
+      <c r="W13">
         <v>200</v>
       </c>
-      <c r="Z13">
+      <c r="AA13">
         <v>22031011</v>
       </c>
-      <c r="AE13" t="s">
+      <c r="AF13" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="14" spans="1:40" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:41" x14ac:dyDescent="0.15">
       <c r="A14">
         <v>42120006</v>
       </c>
@@ -5847,23 +5965,24 @@
       <c r="T14" s="12">
         <v>3006</v>
       </c>
-      <c r="U14">
-        <v>100</v>
-      </c>
+      <c r="U14" s="12"/>
       <c r="V14">
         <v>100</v>
       </c>
       <c r="W14">
         <v>100</v>
       </c>
-      <c r="AC14">
+      <c r="X14">
+        <v>100</v>
+      </c>
+      <c r="AD14">
         <v>43020103</v>
       </c>
-      <c r="AE14" t="s">
+      <c r="AF14" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="15" spans="1:40" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:41" x14ac:dyDescent="0.15">
       <c r="A15">
         <v>42120007</v>
       </c>
@@ -5898,8 +6017,9 @@
       <c r="R15" s="12"/>
       <c r="S15" s="12"/>
       <c r="T15" s="12"/>
-    </row>
-    <row r="16" spans="1:40" x14ac:dyDescent="0.15">
+      <c r="U15" s="12"/>
+    </row>
+    <row r="16" spans="1:41" x14ac:dyDescent="0.15">
       <c r="A16">
         <v>42120008</v>
       </c>
@@ -5934,8 +6054,9 @@
       <c r="R16" s="12"/>
       <c r="S16" s="12"/>
       <c r="T16" s="12"/>
-    </row>
-    <row r="17" spans="1:35" x14ac:dyDescent="0.15">
+      <c r="U16" s="12"/>
+    </row>
+    <row r="17" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A17">
         <v>42120009</v>
       </c>
@@ -5970,8 +6091,9 @@
       <c r="R17" s="12"/>
       <c r="S17" s="12"/>
       <c r="T17" s="12"/>
-    </row>
-    <row r="18" spans="1:35" x14ac:dyDescent="0.15">
+      <c r="U17" s="12"/>
+    </row>
+    <row r="18" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A18">
         <v>42120010</v>
       </c>
@@ -6006,8 +6128,9 @@
       <c r="R18" s="12"/>
       <c r="S18" s="12"/>
       <c r="T18" s="12"/>
-    </row>
-    <row r="19" spans="1:35" x14ac:dyDescent="0.15">
+      <c r="U18" s="12"/>
+    </row>
+    <row r="19" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A19">
         <v>42120011</v>
       </c>
@@ -6042,8 +6165,9 @@
       <c r="R19" s="12"/>
       <c r="S19" s="12"/>
       <c r="T19" s="12"/>
-    </row>
-    <row r="20" spans="1:35" x14ac:dyDescent="0.15">
+      <c r="U19" s="12"/>
+    </row>
+    <row r="20" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A20">
         <v>42120012</v>
       </c>
@@ -6084,14 +6208,15 @@
       </c>
       <c r="S20" s="12"/>
       <c r="T20" s="12"/>
-      <c r="AC20">
+      <c r="U20" s="12"/>
+      <c r="AD20">
         <v>43020105</v>
       </c>
-      <c r="AE20" t="s">
+      <c r="AF20" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="21" spans="1:35" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A21">
         <v>42120013</v>
       </c>
@@ -6129,8 +6254,9 @@
       <c r="R21" s="12"/>
       <c r="S21" s="12"/>
       <c r="T21" s="12"/>
-    </row>
-    <row r="22" spans="1:35" x14ac:dyDescent="0.15">
+      <c r="U21" s="12"/>
+    </row>
+    <row r="22" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A22">
         <v>42120014</v>
       </c>
@@ -6167,8 +6293,9 @@
       <c r="R22" s="12"/>
       <c r="S22" s="12"/>
       <c r="T22" s="12"/>
-    </row>
-    <row r="23" spans="1:35" x14ac:dyDescent="0.15">
+      <c r="U22" s="12"/>
+    </row>
+    <row r="23" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A23">
         <v>42120015</v>
       </c>
@@ -6205,8 +6332,9 @@
       <c r="R23" s="12"/>
       <c r="S23" s="12"/>
       <c r="T23" s="12"/>
-    </row>
-    <row r="24" spans="1:35" x14ac:dyDescent="0.15">
+      <c r="U23" s="12"/>
+    </row>
+    <row r="24" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A24">
         <v>42120016</v>
       </c>
@@ -6244,11 +6372,12 @@
       <c r="R24" s="12"/>
       <c r="S24" s="12"/>
       <c r="T24" s="12"/>
-      <c r="AD24">
+      <c r="U24" s="12"/>
+      <c r="AE24">
         <v>12000003</v>
       </c>
     </row>
-    <row r="25" spans="1:35" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A25">
         <v>42120017</v>
       </c>
@@ -6285,8 +6414,9 @@
       <c r="T25" s="12">
         <v>3005</v>
       </c>
-    </row>
-    <row r="26" spans="1:35" x14ac:dyDescent="0.15">
+      <c r="U25" s="12"/>
+    </row>
+    <row r="26" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A26">
         <v>42120018</v>
       </c>
@@ -6323,8 +6453,9 @@
       <c r="R26" s="12"/>
       <c r="S26" s="25"/>
       <c r="T26" s="25"/>
-    </row>
-    <row r="27" spans="1:35" x14ac:dyDescent="0.15">
+      <c r="U26" s="25"/>
+    </row>
+    <row r="27" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A27">
         <v>42120019</v>
       </c>
@@ -6361,8 +6492,9 @@
       <c r="R27" s="12"/>
       <c r="S27" s="26"/>
       <c r="T27" s="26"/>
-    </row>
-    <row r="28" spans="1:35" x14ac:dyDescent="0.15">
+      <c r="U27" s="26"/>
+    </row>
+    <row r="28" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A28">
         <v>42130001</v>
       </c>
@@ -6401,8 +6533,9 @@
         <v>13020001</v>
       </c>
       <c r="T28" s="12"/>
-    </row>
-    <row r="29" spans="1:35" x14ac:dyDescent="0.15">
+      <c r="U28" s="12"/>
+    </row>
+    <row r="29" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A29">
         <v>42130002</v>
       </c>
@@ -6441,8 +6574,9 @@
         <v>13020002</v>
       </c>
       <c r="T29" s="12"/>
-    </row>
-    <row r="30" spans="1:35" x14ac:dyDescent="0.15">
+      <c r="U29" s="12"/>
+    </row>
+    <row r="30" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A30">
         <v>42130003</v>
       </c>
@@ -6487,11 +6621,9 @@
         <v>13010002</v>
       </c>
       <c r="T30" s="12"/>
-      <c r="U30">
+      <c r="U30" s="12"/>
+      <c r="V30">
         <v>300</v>
-      </c>
-      <c r="V30">
-        <v>500</v>
       </c>
       <c r="W30">
         <v>500</v>
@@ -6500,22 +6632,25 @@
         <v>500</v>
       </c>
       <c r="Y30">
+        <v>500</v>
+      </c>
+      <c r="Z30">
         <v>300</v>
       </c>
-      <c r="AD30">
+      <c r="AE30">
         <v>12000002</v>
       </c>
-      <c r="AE30" t="s">
+      <c r="AF30" t="s">
         <v>213</v>
-      </c>
-      <c r="AH30">
-        <v>200</v>
       </c>
       <c r="AI30">
         <v>200</v>
       </c>
-    </row>
-    <row r="31" spans="1:35" x14ac:dyDescent="0.15">
+      <c r="AJ30">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="31" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A31">
         <v>42130004</v>
       </c>
@@ -6552,8 +6687,9 @@
         <v>13020011</v>
       </c>
       <c r="T31" s="12"/>
-    </row>
-    <row r="32" spans="1:35" x14ac:dyDescent="0.15">
+      <c r="U31" s="12"/>
+    </row>
+    <row r="32" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A32">
         <v>42130005</v>
       </c>
@@ -6590,8 +6726,9 @@
         <v>13020021</v>
       </c>
       <c r="T32" s="12"/>
-    </row>
-    <row r="33" spans="1:20" x14ac:dyDescent="0.15">
+      <c r="U32" s="12"/>
+    </row>
+    <row r="33" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A33">
         <v>42130006</v>
       </c>
@@ -6628,6 +6765,7 @@
         <v>13010004</v>
       </c>
       <c r="T33" s="12"/>
+      <c r="U33" s="12"/>
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>

</xml_diff>

<commit_message>
remove the quest config file
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/SceneQuest.xlsx
+++ b/ConfigData/Xlsx/SceneQuest.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385" activeTab="1"/>
+    <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="4" r:id="rId1"/>
@@ -213,7 +213,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="659" uniqueCount="330">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="658" uniqueCount="329">
   <si>
     <t>int</t>
     <phoneticPr fontId="18" type="noConversion"/>
@@ -849,10 +849,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>npcaolai2</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>true</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -1161,10 +1157,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>npcwoodhouse</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>交互场景位置</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -1442,6 +1434,10 @@
   </si>
   <si>
     <t>Qiaqia</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>npckid1</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -2887,9 +2883,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AM54"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L7" sqref="L7"/>
+      <selection pane="bottomLeft" activeCell="W8" sqref="W8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -2940,22 +2936,22 @@
         <v>82</v>
       </c>
       <c r="J1" s="14" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="K1" s="22" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="L1" s="22" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="M1" s="22" t="s">
+        <v>245</v>
+      </c>
+      <c r="N1" s="22" t="s">
         <v>246</v>
       </c>
-      <c r="N1" s="22" t="s">
-        <v>247</v>
-      </c>
       <c r="O1" s="22" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="P1" s="18" t="s">
         <v>2</v>
@@ -2964,13 +2960,13 @@
         <v>15</v>
       </c>
       <c r="R1" s="18" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="S1" s="18" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="T1" s="18" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="U1" s="15" t="s">
         <v>3</v>
@@ -2994,7 +2990,7 @@
         <v>76</v>
       </c>
       <c r="AB1" s="15" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="AC1" s="15" t="s">
         <v>134</v>
@@ -3015,7 +3011,7 @@
         <v>88</v>
       </c>
       <c r="AI1" s="16" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="AJ1" s="17" t="s">
         <v>28</v>
@@ -3059,7 +3055,7 @@
         <v>61</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="K2" s="23" t="s">
         <v>0</v>
@@ -3068,13 +3064,13 @@
         <v>0</v>
       </c>
       <c r="M2" s="23" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="N2" s="23" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="O2" s="23" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="P2" s="19" t="s">
         <v>58</v>
@@ -3083,13 +3079,13 @@
         <v>62</v>
       </c>
       <c r="R2" s="19" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="S2" s="19" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="T2" s="19" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="U2" s="7" t="s">
         <v>58</v>
@@ -3113,7 +3109,7 @@
         <v>58</v>
       </c>
       <c r="AB2" s="7" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="AC2" s="7" t="s">
         <v>135</v>
@@ -3134,7 +3130,7 @@
         <v>58</v>
       </c>
       <c r="AI2" s="3" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="AJ2" s="9" t="s">
         <v>27</v>
@@ -3178,22 +3174,22 @@
         <v>17</v>
       </c>
       <c r="J3" s="8" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="K3" s="24" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="L3" s="24" t="s">
+        <v>252</v>
+      </c>
+      <c r="M3" s="24" t="s">
         <v>253</v>
       </c>
-      <c r="M3" s="24" t="s">
+      <c r="N3" s="24" t="s">
         <v>254</v>
       </c>
-      <c r="N3" s="24" t="s">
-        <v>255</v>
-      </c>
       <c r="O3" s="24" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="P3" s="20" t="s">
         <v>68</v>
@@ -3202,13 +3198,13 @@
         <v>69</v>
       </c>
       <c r="R3" s="20" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="S3" s="20" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="T3" s="20" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="U3" s="6" t="s">
         <v>70</v>
@@ -3232,7 +3228,7 @@
         <v>35</v>
       </c>
       <c r="AB3" s="6" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="AC3" s="6" t="s">
         <v>136</v>
@@ -3253,7 +3249,7 @@
         <v>8</v>
       </c>
       <c r="AI3" s="2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="AJ3" s="8" t="s">
         <v>23</v>
@@ -3551,7 +3547,7 @@
         <v>0</v>
       </c>
       <c r="F11" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="G11" t="s">
         <v>119</v>
@@ -3561,7 +3557,7 @@
       </c>
       <c r="I11" s="5"/>
       <c r="J11" s="28" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="K11" s="5"/>
       <c r="L11" s="5"/>
@@ -3596,7 +3592,7 @@
       </c>
       <c r="I12" s="5"/>
       <c r="J12" s="31" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="K12" s="5"/>
       <c r="L12" s="5"/>
@@ -3631,7 +3627,7 @@
       </c>
       <c r="I13" s="5"/>
       <c r="J13" s="29" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="K13" s="5"/>
       <c r="L13" s="5"/>
@@ -3681,7 +3677,7 @@
       </c>
       <c r="I14" s="5"/>
       <c r="J14" s="31" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="K14" s="5"/>
       <c r="L14" s="5"/>
@@ -3722,7 +3718,7 @@
       </c>
       <c r="I15" s="5"/>
       <c r="J15" s="32" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="K15" s="5"/>
       <c r="L15" s="5"/>
@@ -3741,7 +3737,7 @@
         <v>42010006</v>
       </c>
       <c r="B16" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="C16">
         <v>1</v>
@@ -3763,7 +3759,7 @@
       </c>
       <c r="I16" s="5"/>
       <c r="J16" s="29" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="K16" s="5"/>
       <c r="L16" s="5"/>
@@ -3803,17 +3799,17 @@
         <v>1</v>
       </c>
       <c r="F17" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="G17" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="H17" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="I17" s="5"/>
       <c r="J17" s="33" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="K17" s="5"/>
       <c r="L17" s="5"/>
@@ -3857,7 +3853,7 @@
       </c>
       <c r="I18" s="5"/>
       <c r="J18" s="27" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="K18" s="5"/>
       <c r="L18" s="5"/>
@@ -3876,7 +3872,7 @@
         <v>42010009</v>
       </c>
       <c r="B19" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C19">
         <v>1</v>
@@ -3885,17 +3881,17 @@
         <v>0</v>
       </c>
       <c r="F19" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="G19" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="H19" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="I19" s="5"/>
       <c r="J19" s="27" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="K19" s="5"/>
       <c r="L19" s="5"/>
@@ -3923,14 +3919,14 @@
         <v>50</v>
       </c>
       <c r="G20" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="H20" t="s">
         <v>120</v>
       </c>
       <c r="I20" s="5"/>
       <c r="J20" s="27" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="K20" s="5"/>
       <c r="L20" s="5"/>
@@ -3968,7 +3964,7 @@
       </c>
       <c r="I21" s="5"/>
       <c r="J21" s="27" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="K21" s="5"/>
       <c r="L21" s="5"/>
@@ -3987,7 +3983,7 @@
         <v>42010012</v>
       </c>
       <c r="B22" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C22">
         <v>1</v>
@@ -3999,17 +3995,17 @@
         <v>1</v>
       </c>
       <c r="F22" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="G22" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="H22" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="I22" s="5"/>
       <c r="J22" s="29" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="K22" s="5"/>
       <c r="L22" s="5"/>
@@ -4059,7 +4055,7 @@
       </c>
       <c r="I23" s="5"/>
       <c r="J23" s="29" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="K23" s="5"/>
       <c r="L23" s="5"/>
@@ -4109,7 +4105,7 @@
       </c>
       <c r="I24" s="5"/>
       <c r="J24" s="29" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="K24" s="5"/>
       <c r="L24" s="5"/>
@@ -4165,7 +4161,7 @@
       </c>
       <c r="I25" s="5"/>
       <c r="J25" s="31" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="K25" s="5"/>
       <c r="L25" s="5"/>
@@ -4200,7 +4196,7 @@
       </c>
       <c r="I26" s="5"/>
       <c r="J26" s="31" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="K26" s="5"/>
       <c r="L26" s="5"/>
@@ -4238,7 +4234,7 @@
       </c>
       <c r="I27" s="5"/>
       <c r="J27" s="29" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="K27" s="5"/>
       <c r="L27" s="5"/>
@@ -4281,7 +4277,7 @@
         <v>0</v>
       </c>
       <c r="F28" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="G28" t="s">
         <v>172</v>
@@ -4290,10 +4286,10 @@
         <v>172</v>
       </c>
       <c r="I28" s="5" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="J28" s="28" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="K28" s="5"/>
       <c r="L28" s="5"/>
@@ -4306,7 +4302,7 @@
         <v>42010019</v>
       </c>
       <c r="B29" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C29">
         <v>1</v>
@@ -4318,19 +4314,19 @@
         <v>2</v>
       </c>
       <c r="F29" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="G29" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="H29" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="I29" s="5" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="J29" s="31" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="K29" s="5"/>
       <c r="L29" s="5"/>
@@ -4349,7 +4345,7 @@
         <v>42010020</v>
       </c>
       <c r="B30" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C30">
         <v>1</v>
@@ -4361,19 +4357,19 @@
         <v>2</v>
       </c>
       <c r="F30" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="G30" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="H30" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I30" s="5" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="J30" s="31" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="K30" s="5"/>
       <c r="L30" s="5"/>
@@ -4392,7 +4388,7 @@
         <v>42010021</v>
       </c>
       <c r="B31" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C31">
         <v>1</v>
@@ -4404,17 +4400,17 @@
         <v>1</v>
       </c>
       <c r="F31" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="G31" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="H31" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="I31" s="5"/>
       <c r="J31" s="31" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="K31" s="5"/>
       <c r="L31" s="5"/>
@@ -4430,7 +4426,7 @@
         <v>42010022</v>
       </c>
       <c r="B32" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C32">
         <v>1</v>
@@ -4442,17 +4438,17 @@
         <v>2</v>
       </c>
       <c r="F32" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="G32" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="H32" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="I32" s="5"/>
       <c r="J32" s="29" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="K32" s="5"/>
       <c r="L32" s="5"/>
@@ -4480,7 +4476,7 @@
         <v>42010023</v>
       </c>
       <c r="B33" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C33">
         <v>1</v>
@@ -4492,17 +4488,17 @@
         <v>1</v>
       </c>
       <c r="F33" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="G33" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="H33" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="I33" s="5"/>
       <c r="J33" s="31" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="K33" s="5"/>
       <c r="L33" s="5"/>
@@ -4524,7 +4520,7 @@
         <v>42010024</v>
       </c>
       <c r="B34" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C34">
         <v>1</v>
@@ -4533,17 +4529,17 @@
         <v>0</v>
       </c>
       <c r="F34" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="G34" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="H34" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="I34" s="5"/>
       <c r="J34" s="32" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="K34" s="5"/>
       <c r="L34" s="5"/>
@@ -4559,7 +4555,7 @@
         <v>42010025</v>
       </c>
       <c r="B35" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C35">
         <v>1</v>
@@ -4568,17 +4564,17 @@
         <v>0</v>
       </c>
       <c r="F35" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="G35" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="H35" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="I35" s="5"/>
       <c r="J35" s="32" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="K35" s="5"/>
       <c r="L35" s="5"/>
@@ -4594,7 +4590,7 @@
         <v>42010026</v>
       </c>
       <c r="B36" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="C36">
         <v>1</v>
@@ -4603,17 +4599,17 @@
         <v>0</v>
       </c>
       <c r="F36" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="G36" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="H36" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="I36" s="5"/>
       <c r="J36" s="32" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="K36" s="5"/>
       <c r="L36" s="5"/>
@@ -4629,7 +4625,7 @@
         <v>42010027</v>
       </c>
       <c r="B37" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="C37">
         <v>1</v>
@@ -4638,17 +4634,17 @@
         <v>0</v>
       </c>
       <c r="F37" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="G37" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="H37" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="I37" s="5"/>
       <c r="J37" s="32" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="K37" s="5"/>
       <c r="L37" s="5"/>
@@ -4664,7 +4660,7 @@
         <v>42010028</v>
       </c>
       <c r="B38" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="C38">
         <v>1</v>
@@ -4676,17 +4672,17 @@
         <v>2</v>
       </c>
       <c r="F38" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="G38" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="H38" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="I38" s="5"/>
       <c r="J38" s="31" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="K38" s="5"/>
       <c r="L38" s="5"/>
@@ -4705,7 +4701,7 @@
         <v>42010029</v>
       </c>
       <c r="B39" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="C39">
         <v>1</v>
@@ -4714,17 +4710,17 @@
         <v>0</v>
       </c>
       <c r="F39" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="G39" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="H39" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="I39" s="5"/>
       <c r="J39" s="30" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="K39" s="5"/>
       <c r="L39" s="5"/>
@@ -4737,7 +4733,7 @@
         <v>42010030</v>
       </c>
       <c r="B40" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="C40">
         <v>1</v>
@@ -4749,17 +4745,17 @@
         <v>2</v>
       </c>
       <c r="F40" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="G40" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="H40" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="I40" s="5"/>
       <c r="J40" s="29" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="K40" s="5"/>
       <c r="L40" s="5"/>
@@ -4793,7 +4789,7 @@
         <v>42010031</v>
       </c>
       <c r="B41" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="C41">
         <v>1</v>
@@ -4805,17 +4801,17 @@
         <v>1</v>
       </c>
       <c r="F41" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="G41" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="H41" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="I41" s="5"/>
       <c r="J41" s="33" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="K41" s="5"/>
       <c r="L41" s="5"/>
@@ -4840,7 +4836,7 @@
         <v>42010032</v>
       </c>
       <c r="B42" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="C42">
         <v>1</v>
@@ -4849,17 +4845,17 @@
         <v>0</v>
       </c>
       <c r="F42" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="G42" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="H42" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="I42" s="5"/>
       <c r="J42" s="32" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="K42" s="5"/>
       <c r="L42" s="5"/>
@@ -4878,7 +4874,7 @@
         <v>42010033</v>
       </c>
       <c r="B43" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="C43">
         <v>1</v>
@@ -4890,17 +4886,17 @@
         <v>2</v>
       </c>
       <c r="F43" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="G43" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="H43" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="I43" s="5"/>
       <c r="J43" s="29" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="K43" s="5"/>
       <c r="L43" s="5"/>
@@ -4953,7 +4949,7 @@
       </c>
       <c r="I44" s="5"/>
       <c r="J44" s="29" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="K44" s="5"/>
       <c r="L44" s="5"/>
@@ -5006,7 +5002,7 @@
       </c>
       <c r="I45" s="5"/>
       <c r="J45" s="29" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="K45" s="5"/>
       <c r="L45" s="5"/>
@@ -5062,7 +5058,7 @@
       </c>
       <c r="I46" s="5"/>
       <c r="J46" s="31" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="K46" s="5"/>
       <c r="L46" s="5"/>
@@ -5081,7 +5077,7 @@
         <v>42020004</v>
       </c>
       <c r="B47" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C47">
         <v>3</v>
@@ -5093,17 +5089,17 @@
         <v>1</v>
       </c>
       <c r="F47" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="G47" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="H47" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="I47" s="5"/>
       <c r="J47" s="31" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="K47" s="5"/>
       <c r="L47" s="5"/>
@@ -5122,7 +5118,7 @@
         <v>42020005</v>
       </c>
       <c r="B48" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C48">
         <v>3</v>
@@ -5134,17 +5130,17 @@
         <v>1</v>
       </c>
       <c r="F48" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="G48" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="H48" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="I48" s="5"/>
       <c r="J48" s="29" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="K48" s="5"/>
       <c r="L48" s="5"/>
@@ -5175,7 +5171,7 @@
         <v>42020006</v>
       </c>
       <c r="B49" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C49">
         <v>3</v>
@@ -5187,17 +5183,17 @@
         <v>3</v>
       </c>
       <c r="F49" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="G49" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="H49" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="I49" s="5"/>
       <c r="J49" s="29" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="K49" s="5"/>
       <c r="L49" s="5"/>
@@ -5225,7 +5221,7 @@
         <v>42020007</v>
       </c>
       <c r="B50" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="C50">
         <v>3</v>
@@ -5234,17 +5230,17 @@
         <v>0</v>
       </c>
       <c r="F50" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="G50" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="H50" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="I50" s="5"/>
       <c r="J50" s="30" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="K50" s="5"/>
       <c r="L50" s="5"/>
@@ -5257,7 +5253,7 @@
         <v>42020008</v>
       </c>
       <c r="B51" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="C51">
         <v>3</v>
@@ -5266,17 +5262,17 @@
         <v>0</v>
       </c>
       <c r="F51" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="G51" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="H51" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="I51" s="5"/>
       <c r="J51" s="30" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="K51" s="5"/>
       <c r="L51" s="5"/>
@@ -5289,7 +5285,7 @@
         <v>42020009</v>
       </c>
       <c r="B52" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="C52">
         <v>3</v>
@@ -5298,17 +5294,17 @@
         <v>0</v>
       </c>
       <c r="F52" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="G52" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="H52" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="I52" s="5"/>
       <c r="J52" s="33" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="K52" s="5"/>
       <c r="L52" s="5"/>
@@ -5333,7 +5329,7 @@
         <v>42020010</v>
       </c>
       <c r="B53" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="C53">
         <v>3</v>
@@ -5342,17 +5338,17 @@
         <v>0</v>
       </c>
       <c r="F53" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="G53" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="H53" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="I53" s="5"/>
       <c r="J53" s="33" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="K53" s="5"/>
       <c r="L53" s="5"/>
@@ -5374,7 +5370,7 @@
         <v>42020011</v>
       </c>
       <c r="B54" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="C54">
         <v>3</v>
@@ -5383,17 +5379,17 @@
         <v>0</v>
       </c>
       <c r="F54" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="G54" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="H54" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="I54" s="5"/>
       <c r="J54" s="33" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="K54" s="5"/>
       <c r="L54" s="5"/>
@@ -5425,9 +5421,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AM32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H25" sqref="H25"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="Y13" sqref="Y13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -5478,22 +5474,22 @@
         <v>82</v>
       </c>
       <c r="J1" s="14" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="K1" s="22" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="L1" s="22" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="M1" s="22" t="s">
+        <v>245</v>
+      </c>
+      <c r="N1" s="22" t="s">
         <v>246</v>
       </c>
-      <c r="N1" s="22" t="s">
-        <v>247</v>
-      </c>
       <c r="O1" s="22" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="P1" s="18" t="s">
         <v>2</v>
@@ -5502,13 +5498,13 @@
         <v>15</v>
       </c>
       <c r="R1" s="18" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="S1" s="18" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="T1" s="18" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="U1" s="15" t="s">
         <v>3</v>
@@ -5532,7 +5528,7 @@
         <v>76</v>
       </c>
       <c r="AB1" s="15" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="AC1" s="15" t="s">
         <v>134</v>
@@ -5553,7 +5549,7 @@
         <v>88</v>
       </c>
       <c r="AI1" s="16" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="AJ1" s="17" t="s">
         <v>28</v>
@@ -5597,22 +5593,22 @@
         <v>61</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="K2" s="23" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="L2" s="23" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="M2" s="23" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="N2" s="23" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="O2" s="23" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="P2" s="19" t="s">
         <v>0</v>
@@ -5624,10 +5620,10 @@
         <v>0</v>
       </c>
       <c r="S2" s="19" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="T2" s="19" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="U2" s="7" t="s">
         <v>58</v>
@@ -5651,7 +5647,7 @@
         <v>58</v>
       </c>
       <c r="AB2" s="7" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="AC2" s="7" t="s">
         <v>135</v>
@@ -5672,7 +5668,7 @@
         <v>58</v>
       </c>
       <c r="AI2" s="3" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="AJ2" s="9" t="s">
         <v>27</v>
@@ -5716,37 +5712,37 @@
         <v>17</v>
       </c>
       <c r="J3" s="8" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="K3" s="24" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="L3" s="24" t="s">
+        <v>252</v>
+      </c>
+      <c r="M3" s="24" t="s">
         <v>253</v>
       </c>
-      <c r="M3" s="24" t="s">
+      <c r="N3" s="24" t="s">
         <v>254</v>
       </c>
-      <c r="N3" s="24" t="s">
-        <v>255</v>
-      </c>
       <c r="O3" s="24" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="P3" s="20" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="Q3" s="20" t="s">
         <v>69</v>
       </c>
       <c r="R3" s="20" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="S3" s="20" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="T3" s="20" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="U3" s="6" t="s">
         <v>70</v>
@@ -5770,7 +5766,7 @@
         <v>35</v>
       </c>
       <c r="AB3" s="6" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="AC3" s="6" t="s">
         <v>136</v>
@@ -5791,7 +5787,7 @@
         <v>8</v>
       </c>
       <c r="AI3" s="2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="AJ3" s="8" t="s">
         <v>23</v>
@@ -5898,7 +5894,7 @@
         <v>42110003</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="C6" s="10">
         <v>2</v>
@@ -5934,7 +5930,7 @@
         <v>42110004</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C7" s="10">
         <v>2</v>
@@ -5943,13 +5939,13 @@
         <v>0</v>
       </c>
       <c r="F7" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="G7" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="H7" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="I7" s="5" t="s">
         <v>18</v>
@@ -5966,7 +5962,7 @@
         <v>42110005</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C8" s="10">
         <v>2</v>
@@ -5975,13 +5971,13 @@
         <v>0</v>
       </c>
       <c r="F8" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="G8" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="H8" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="I8" s="5" t="s">
         <v>18</v>
@@ -6017,7 +6013,7 @@
         <v>19</v>
       </c>
       <c r="H9" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="I9" s="5" t="s">
         <v>18</v>
@@ -6050,7 +6046,7 @@
         <v>0</v>
       </c>
       <c r="F10" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="G10" t="s">
         <v>21</v>
@@ -6065,7 +6061,7 @@
       <c r="K10" s="5"/>
       <c r="L10" s="5"/>
       <c r="M10" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="N10" s="5"/>
       <c r="O10" s="5"/>
@@ -6102,7 +6098,7 @@
         <v>146</v>
       </c>
       <c r="H11" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="I11" s="5" t="s">
         <v>18</v>
@@ -6111,7 +6107,7 @@
       <c r="K11" s="5"/>
       <c r="L11" s="5"/>
       <c r="M11" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="N11" s="5"/>
       <c r="O11" s="5"/>
@@ -6159,7 +6155,7 @@
         <v>43020102</v>
       </c>
       <c r="AD12" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
     </row>
     <row r="13" spans="1:39" x14ac:dyDescent="0.15">
@@ -6205,9 +6201,6 @@
       <c r="V13">
         <v>200</v>
       </c>
-      <c r="Z13">
-        <v>22031011</v>
-      </c>
       <c r="AD13" t="s">
         <v>171</v>
       </c>
@@ -6267,7 +6260,7 @@
         <v>43020103</v>
       </c>
       <c r="AD14" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
     </row>
     <row r="15" spans="1:39" x14ac:dyDescent="0.15">
@@ -6464,7 +6457,7 @@
         <v>0</v>
       </c>
       <c r="F20" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="G20" t="s">
         <v>157</v>
@@ -6495,7 +6488,7 @@
         <v>43020105</v>
       </c>
       <c r="AD20" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="21" spans="1:34" x14ac:dyDescent="0.15">
@@ -6503,7 +6496,7 @@
         <v>42120013</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C21" s="10">
         <v>2</v>
@@ -6512,13 +6505,13 @@
         <v>0</v>
       </c>
       <c r="F21" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="G21" t="s">
-        <v>232</v>
+        <v>328</v>
       </c>
       <c r="H21" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="I21" s="5" t="s">
         <v>18</v>
@@ -6527,9 +6520,6 @@
       <c r="K21" s="5"/>
       <c r="L21" s="5"/>
       <c r="M21" s="5"/>
-      <c r="N21" t="s">
-        <v>210</v>
-      </c>
       <c r="Q21" s="12"/>
       <c r="R21" s="12"/>
       <c r="S21" s="12"/>
@@ -6540,7 +6530,7 @@
         <v>42120014</v>
       </c>
       <c r="B22" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C22" s="10">
         <v>2</v>
@@ -6549,13 +6539,13 @@
         <v>0</v>
       </c>
       <c r="F22" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="G22" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="H22" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="I22" s="5" t="s">
         <v>18</v>
@@ -6576,7 +6566,7 @@
         <v>42120015</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C23" s="10">
         <v>2</v>
@@ -6585,13 +6575,13 @@
         <v>0</v>
       </c>
       <c r="F23" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="G23" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="H23" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="I23" s="5" t="s">
         <v>18</v>
@@ -6612,7 +6602,7 @@
         <v>42120016</v>
       </c>
       <c r="B24" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C24" s="10">
         <v>2</v>
@@ -6621,13 +6611,13 @@
         <v>0</v>
       </c>
       <c r="F24" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
       <c r="G24" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="H24" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="I24" s="5" t="s">
         <v>18</v>
@@ -6636,9 +6626,6 @@
       <c r="K24" s="5"/>
       <c r="L24" s="5"/>
       <c r="M24" s="5"/>
-      <c r="N24" t="s">
-        <v>249</v>
-      </c>
       <c r="Q24" s="12"/>
       <c r="R24" s="12"/>
       <c r="S24" s="12"/>
@@ -6649,7 +6636,7 @@
         <v>42120018</v>
       </c>
       <c r="B25" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="C25" s="10">
         <v>2</v>
@@ -6658,13 +6645,13 @@
         <v>0</v>
       </c>
       <c r="F25" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="G25" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="H25" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="I25" s="5" t="s">
         <v>18</v>
@@ -6685,7 +6672,7 @@
         <v>42120019</v>
       </c>
       <c r="B26" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="C26" s="10">
         <v>2</v>
@@ -6694,13 +6681,13 @@
         <v>0</v>
       </c>
       <c r="F26" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="G26" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="H26" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="I26" s="5" t="s">
         <v>18</v>
@@ -6721,7 +6708,7 @@
         <v>42130001</v>
       </c>
       <c r="B27" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C27" s="10">
         <v>2</v>
@@ -6730,13 +6717,13 @@
         <v>0</v>
       </c>
       <c r="F27" t="s">
+        <v>204</v>
+      </c>
+      <c r="G27" t="s">
+        <v>204</v>
+      </c>
+      <c r="H27" t="s">
         <v>205</v>
-      </c>
-      <c r="G27" t="s">
-        <v>205</v>
-      </c>
-      <c r="H27" t="s">
-        <v>206</v>
       </c>
       <c r="I27" s="5" t="s">
         <v>18</v>
@@ -6759,7 +6746,7 @@
         <v>42130002</v>
       </c>
       <c r="B28" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C28" s="10">
         <v>2</v>
@@ -6768,13 +6755,13 @@
         <v>0</v>
       </c>
       <c r="F28" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="G28" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="H28" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="I28" s="5" t="s">
         <v>18</v>
@@ -6799,7 +6786,7 @@
         <v>42130003</v>
       </c>
       <c r="B29" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C29" s="10">
         <v>2</v>
@@ -6811,13 +6798,13 @@
         <v>3</v>
       </c>
       <c r="F29" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="G29" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="H29" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="I29" s="5" t="s">
         <v>18</v>
@@ -6825,7 +6812,9 @@
       <c r="J29" s="5"/>
       <c r="K29" s="5"/>
       <c r="L29" s="5"/>
-      <c r="M29" s="5"/>
+      <c r="M29" t="s">
+        <v>209</v>
+      </c>
       <c r="N29" s="5"/>
       <c r="O29" s="5"/>
       <c r="P29">
@@ -6855,7 +6844,7 @@
         <v>300</v>
       </c>
       <c r="AD29" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="AG29">
         <v>200</v>
@@ -6869,7 +6858,7 @@
         <v>42130004</v>
       </c>
       <c r="B30" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C30" s="10">
         <v>2</v>
@@ -6878,13 +6867,13 @@
         <v>0</v>
       </c>
       <c r="F30" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="G30" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="H30" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="I30" s="5" t="s">
         <v>18</v>
@@ -6907,7 +6896,7 @@
         <v>42130005</v>
       </c>
       <c r="B31" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="C31" s="10">
         <v>2</v>
@@ -6916,13 +6905,13 @@
         <v>0</v>
       </c>
       <c r="F31" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="G31" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="H31" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="I31" s="5" t="s">
         <v>18</v>
@@ -6945,7 +6934,7 @@
         <v>42130006</v>
       </c>
       <c r="B32" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="C32" s="10">
         <v>2</v>
@@ -6954,13 +6943,13 @@
         <v>0</v>
       </c>
       <c r="F32" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="G32" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="H32" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="I32" s="5" t="s">
         <v>18</v>

</xml_diff>

<commit_message>
add a new battlemap tool
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/SceneQuest.xlsx
+++ b/ConfigData/Xlsx/SceneQuest.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Code\TOMClassicGit\ConfigData\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\code\TOMClassicGit\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -2536,7 +2536,49 @@
     <cellStyle name="着色 6" xfId="38" builtinId="49" customBuiltin="1"/>
     <cellStyle name="注释" xfId="15" builtinId="10" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="31">
+  <dxfs count="37">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -2604,6 +2646,18 @@
         <charset val="134"/>
         <scheme val="minor"/>
       </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color theme="4"/>
+        </right>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -2623,18 +2677,6 @@
         <charset val="134"/>
         <scheme val="minor"/>
       </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="thin">
-          <color theme="4"/>
-        </right>
-        <top style="thin">
-          <color theme="4"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
     </dxf>
     <dxf>
       <font>
@@ -2796,7 +2838,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="表3" displayName="表3" ref="A3:AP64" totalsRowShown="0" headerRowDxfId="30">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="表3" displayName="表3" ref="A3:AP64" totalsRowShown="0" headerRowDxfId="36">
   <autoFilter ref="A3:AP64"/>
   <sortState ref="A4:AO61">
     <sortCondition ref="A3:A61"/>
@@ -2810,14 +2852,14 @@
     <tableColumn id="24" name="Ename"/>
     <tableColumn id="4" name="Figue"/>
     <tableColumn id="5" name="Script"/>
-    <tableColumn id="6" name="TriggerMulti" dataDxfId="29"/>
-    <tableColumn id="40" name="Catalog" dataDxfId="28"/>
-    <tableColumn id="35" name="TriggerHourBegin" dataDxfId="27"/>
-    <tableColumn id="34" name="TriggerHourEnd" dataDxfId="26"/>
-    <tableColumn id="36" name="TriggerQuestNotReceive" dataDxfId="25"/>
-    <tableColumn id="37" name="TriggerQuestReceived" dataDxfId="24"/>
-    <tableColumn id="38" name="TriggerQuestFinished" dataDxfId="23"/>
-    <tableColumn id="39" name="TriggerRate" dataDxfId="22"/>
+    <tableColumn id="6" name="TriggerMulti" dataDxfId="35"/>
+    <tableColumn id="40" name="Catalog" dataDxfId="34"/>
+    <tableColumn id="35" name="TriggerHourBegin" dataDxfId="33"/>
+    <tableColumn id="34" name="TriggerHourEnd" dataDxfId="32"/>
+    <tableColumn id="36" name="TriggerQuestNotReceive" dataDxfId="31"/>
+    <tableColumn id="37" name="TriggerQuestReceived" dataDxfId="30"/>
+    <tableColumn id="38" name="TriggerQuestFinished" dataDxfId="29"/>
+    <tableColumn id="39" name="TriggerRate" dataDxfId="28"/>
     <tableColumn id="7" name="EnemyName"/>
     <tableColumn id="32" name="SceneId"/>
     <tableColumn id="29" name="Position"/>
@@ -2850,7 +2892,7 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="表3_5" displayName="表3_5" ref="A3:AP33" totalsRowShown="0" headerRowDxfId="21">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="表3_5" displayName="表3_5" ref="A3:AP33" totalsRowShown="0" headerRowDxfId="27">
   <autoFilter ref="A3:AP33"/>
   <sortState ref="A4:AC6">
     <sortCondition ref="A3:A6"/>
@@ -2858,26 +2900,26 @@
   <tableColumns count="42">
     <tableColumn id="1" name="Id"/>
     <tableColumn id="2" name="Name"/>
-    <tableColumn id="27" name="Type" dataDxfId="20"/>
+    <tableColumn id="27" name="Type" dataDxfId="26"/>
     <tableColumn id="3" name="Level"/>
     <tableColumn id="25" name="Danger"/>
     <tableColumn id="24" name="Ename"/>
     <tableColumn id="4" name="Figue"/>
     <tableColumn id="5" name="Script"/>
     <tableColumn id="6" name="TriggerMulti"/>
-    <tableColumn id="40" name="Catalog" dataDxfId="19"/>
-    <tableColumn id="35" name="TriggerHourBegin" dataDxfId="18"/>
-    <tableColumn id="34" name="TriggerHourEnd" dataDxfId="17"/>
-    <tableColumn id="37" name="TriggerQuestNotReceive" dataDxfId="16"/>
-    <tableColumn id="38" name="TriggerQuestReceived" dataDxfId="15"/>
-    <tableColumn id="36" name="TriggerQuestFinished" dataDxfId="14"/>
-    <tableColumn id="39" name="TriggerRate" dataDxfId="13"/>
+    <tableColumn id="40" name="Catalog" dataDxfId="25"/>
+    <tableColumn id="35" name="TriggerHourBegin" dataDxfId="24"/>
+    <tableColumn id="34" name="TriggerHourEnd" dataDxfId="23"/>
+    <tableColumn id="37" name="TriggerQuestNotReceive" dataDxfId="22"/>
+    <tableColumn id="38" name="TriggerQuestReceived" dataDxfId="21"/>
+    <tableColumn id="36" name="TriggerQuestFinished" dataDxfId="20"/>
+    <tableColumn id="39" name="TriggerRate" dataDxfId="19"/>
     <tableColumn id="7" name="EnemyName"/>
-    <tableColumn id="32" name="SceneId" dataDxfId="12"/>
-    <tableColumn id="29" name="Position" dataDxfId="11"/>
-    <tableColumn id="28" name="NextQuest" dataDxfId="10"/>
-    <tableColumn id="8" name="ShopName" dataDxfId="7"/>
-    <tableColumn id="41" name="MiniGameId" dataDxfId="9"/>
+    <tableColumn id="32" name="SceneId" dataDxfId="18"/>
+    <tableColumn id="29" name="Position" dataDxfId="17"/>
+    <tableColumn id="28" name="NextQuest" dataDxfId="16"/>
+    <tableColumn id="8" name="ShopName" dataDxfId="15"/>
+    <tableColumn id="41" name="MiniGameId" dataDxfId="14"/>
     <tableColumn id="9" name="RewardGold"/>
     <tableColumn id="10" name="RewardFood"/>
     <tableColumn id="11" name="RewardHealth"/>
@@ -2897,7 +2939,7 @@
     <tableColumn id="21" name="TradeFood"/>
     <tableColumn id="22" name="TradeHealth"/>
     <tableColumn id="23" name="TradeMental"/>
-    <tableColumn id="33" name="TradeDropItem" dataDxfId="8"/>
+    <tableColumn id="33" name="TradeDropItem" dataDxfId="13"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3227,8 +3269,8 @@
   <dimension ref="A1:AP64"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A40" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B52" sqref="B52"/>
+      <pane ySplit="3" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="T46" sqref="T46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -5766,7 +5808,7 @@
       <c r="N53" s="5"/>
       <c r="O53" s="5"/>
       <c r="P53" s="5"/>
-      <c r="V53" t="s">
+      <c r="U53" t="s">
         <v>411</v>
       </c>
     </row>
@@ -6255,24 +6297,9 @@
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
-  <conditionalFormatting sqref="AP4:AP50 B4:AO48 I50:AP51 K49:AO49 B52:AP52 B54:AP64 W53:AP53">
-    <cfRule type="containsBlanks" dxfId="6" priority="6">
+  <conditionalFormatting sqref="B4:AP64">
+    <cfRule type="containsBlanks" dxfId="6" priority="9">
       <formula>LEN(TRIM(B4))=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B49:I49 B50:H51">
-    <cfRule type="containsBlanks" dxfId="5" priority="4">
-      <formula>LEN(TRIM(B49))=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J49">
-    <cfRule type="containsBlanks" dxfId="4" priority="3">
-      <formula>LEN(TRIM(J49))=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B53:V53">
-    <cfRule type="containsBlanks" dxfId="1" priority="1">
-      <formula>LEN(TRIM(B53))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6290,7 +6317,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="U13" sqref="U13"/>
+      <selection pane="bottomLeft" activeCell="U19" sqref="U19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -7946,19 +7973,9 @@
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
-  <conditionalFormatting sqref="B4:AO12 B14:AO33 B13:T13 V13:AO13">
+  <conditionalFormatting sqref="D4:AP33">
     <cfRule type="containsBlanks" dxfId="3" priority="3">
-      <formula>LEN(TRIM(B4))=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AP4:AP33">
-    <cfRule type="containsBlanks" dxfId="2" priority="2">
-      <formula>LEN(TRIM(AP4))=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="U13">
-    <cfRule type="containsBlanks" dxfId="0" priority="1">
-      <formula>LEN(TRIM(U13))=0</formula>
+      <formula>LEN(TRIM(D4))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
finish the hidden cell function
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/SceneQuest.xlsx
+++ b/ConfigData/Xlsx/SceneQuest.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18229"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18326"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="790" uniqueCount="438">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="797" uniqueCount="442">
   <si>
     <t>int</t>
     <phoneticPr fontId="18" type="noConversion"/>
@@ -1685,6 +1685,21 @@
   <si>
     <t>bee</t>
     <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>隐藏的房间</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>string</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>HiddenRoomQuest</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>portal</t>
   </si>
 </sst>
 </file>
@@ -2618,7 +2633,40 @@
     <cellStyle name="着色 6" xfId="38" builtinId="49" customBuiltin="1"/>
     <cellStyle name="注释" xfId="15" builtinId="10" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="27">
+  <dxfs count="28">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -2798,13 +2846,6 @@
       </fill>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
     <dxf>
@@ -2836,13 +2877,6 @@
         </patternFill>
       </fill>
     </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -2865,12 +2899,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="表3" displayName="表3" ref="A3:AQ68" totalsRowShown="0" headerRowDxfId="25">
-  <autoFilter ref="A3:AQ68"/>
-  <sortState ref="A4:AQ68">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="表3" displayName="表3" ref="A3:AR68" totalsRowShown="0" headerRowDxfId="27">
+  <autoFilter ref="A3:AR68"/>
+  <sortState ref="A4:AR68">
     <sortCondition ref="A3:A68"/>
   </sortState>
-  <tableColumns count="43">
+  <tableColumns count="44">
     <tableColumn id="1" name="Id"/>
     <tableColumn id="2" name="Name"/>
     <tableColumn id="28" name="Type"/>
@@ -2879,18 +2913,19 @@
     <tableColumn id="24" name="Ename"/>
     <tableColumn id="4" name="Figue"/>
     <tableColumn id="5" name="Script"/>
-    <tableColumn id="6" name="TriggerMulti" dataDxfId="24"/>
-    <tableColumn id="40" name="Catalog" dataDxfId="23"/>
-    <tableColumn id="35" name="TriggerHourBegin" dataDxfId="22"/>
-    <tableColumn id="34" name="TriggerHourEnd" dataDxfId="21"/>
-    <tableColumn id="36" name="TriggerQuestNotReceive" dataDxfId="20"/>
-    <tableColumn id="37" name="TriggerQuestReceived" dataDxfId="19"/>
-    <tableColumn id="38" name="TriggerQuestFinished" dataDxfId="18"/>
-    <tableColumn id="39" name="TriggerRate" dataDxfId="17"/>
+    <tableColumn id="6" name="TriggerMulti" dataDxfId="26"/>
+    <tableColumn id="40" name="Catalog" dataDxfId="25"/>
+    <tableColumn id="35" name="TriggerHourBegin" dataDxfId="24"/>
+    <tableColumn id="34" name="TriggerHourEnd" dataDxfId="23"/>
+    <tableColumn id="36" name="TriggerQuestNotReceive" dataDxfId="22"/>
+    <tableColumn id="37" name="TriggerQuestReceived" dataDxfId="21"/>
+    <tableColumn id="38" name="TriggerQuestFinished" dataDxfId="20"/>
+    <tableColumn id="39" name="TriggerRate" dataDxfId="19"/>
     <tableColumn id="7" name="EnemyName"/>
     <tableColumn id="32" name="SceneId"/>
     <tableColumn id="29" name="Position"/>
     <tableColumn id="27" name="NextQuest"/>
+    <tableColumn id="44" name="HiddenRoomQuest"/>
     <tableColumn id="8" name="ShopName"/>
     <tableColumn id="41" name="MiniGameId"/>
     <tableColumn id="43" name="PayKey"/>
@@ -2920,35 +2955,36 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="表3_5" displayName="表3_5" ref="A3:AQ33" totalsRowShown="0" headerRowDxfId="15">
-  <autoFilter ref="A3:AQ33"/>
-  <sortState ref="A4:AD6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="表3_5" displayName="表3_5" ref="A3:AR33" totalsRowShown="0" headerRowDxfId="18">
+  <autoFilter ref="A3:AR33"/>
+  <sortState ref="A4:AE6">
     <sortCondition ref="A3:A6"/>
   </sortState>
-  <tableColumns count="43">
+  <tableColumns count="44">
     <tableColumn id="1" name="Id"/>
     <tableColumn id="2" name="Name"/>
-    <tableColumn id="27" name="Type" dataDxfId="14"/>
+    <tableColumn id="27" name="Type" dataDxfId="17"/>
     <tableColumn id="3" name="Level"/>
     <tableColumn id="25" name="Danger"/>
     <tableColumn id="24" name="Ename"/>
     <tableColumn id="4" name="Figue"/>
     <tableColumn id="5" name="Script"/>
     <tableColumn id="6" name="TriggerMulti"/>
-    <tableColumn id="40" name="Catalog" dataDxfId="13"/>
-    <tableColumn id="35" name="TriggerHourBegin" dataDxfId="12"/>
-    <tableColumn id="34" name="TriggerHourEnd" dataDxfId="11"/>
-    <tableColumn id="37" name="TriggerQuestNotReceive" dataDxfId="10"/>
-    <tableColumn id="38" name="TriggerQuestReceived" dataDxfId="9"/>
-    <tableColumn id="36" name="TriggerQuestFinished" dataDxfId="8"/>
-    <tableColumn id="39" name="TriggerRate" dataDxfId="7"/>
+    <tableColumn id="40" name="Catalog" dataDxfId="16"/>
+    <tableColumn id="35" name="TriggerHourBegin" dataDxfId="15"/>
+    <tableColumn id="34" name="TriggerHourEnd" dataDxfId="14"/>
+    <tableColumn id="37" name="TriggerQuestNotReceive" dataDxfId="13"/>
+    <tableColumn id="38" name="TriggerQuestReceived" dataDxfId="12"/>
+    <tableColumn id="36" name="TriggerQuestFinished" dataDxfId="11"/>
+    <tableColumn id="39" name="TriggerRate" dataDxfId="10"/>
     <tableColumn id="7" name="EnemyName"/>
-    <tableColumn id="32" name="SceneId" dataDxfId="6"/>
-    <tableColumn id="29" name="Position" dataDxfId="5"/>
-    <tableColumn id="28" name="NextQuest" dataDxfId="4"/>
-    <tableColumn id="8" name="ShopName" dataDxfId="3"/>
-    <tableColumn id="41" name="MiniGameId" dataDxfId="2"/>
-    <tableColumn id="43" name="PayKey" dataDxfId="1"/>
+    <tableColumn id="32" name="SceneId" dataDxfId="9"/>
+    <tableColumn id="29" name="Position" dataDxfId="8"/>
+    <tableColumn id="28" name="NextQuest" dataDxfId="7"/>
+    <tableColumn id="44" name="HiddenRoomQuest" dataDxfId="0"/>
+    <tableColumn id="8" name="ShopName" dataDxfId="6"/>
+    <tableColumn id="41" name="MiniGameId" dataDxfId="5"/>
+    <tableColumn id="43" name="PayKey" dataDxfId="4"/>
     <tableColumn id="9" name="RewardGold"/>
     <tableColumn id="10" name="RewardFood"/>
     <tableColumn id="11" name="RewardHealth"/>
@@ -2968,7 +3004,7 @@
     <tableColumn id="21" name="TradeFood"/>
     <tableColumn id="22" name="TradeHealth"/>
     <tableColumn id="23" name="TradeMental"/>
-    <tableColumn id="33" name="TradeDropItem" dataDxfId="0"/>
+    <tableColumn id="33" name="TradeDropItem" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3295,11 +3331,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AQ68"/>
+  <dimension ref="A1:AR68"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A27" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Q43" sqref="Q43"/>
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="U4" sqref="U4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -3310,18 +3346,18 @@
     <col min="9" max="16" width="4.875" customWidth="1"/>
     <col min="17" max="17" width="9.75" customWidth="1"/>
     <col min="18" max="18" width="9.375" customWidth="1"/>
-    <col min="19" max="21" width="6.5" customWidth="1"/>
-    <col min="22" max="23" width="9.125" customWidth="1"/>
-    <col min="24" max="28" width="4.875" customWidth="1"/>
-    <col min="29" max="30" width="9.375" customWidth="1"/>
-    <col min="31" max="31" width="4.25" customWidth="1"/>
-    <col min="32" max="32" width="9.875" customWidth="1"/>
-    <col min="33" max="33" width="9.375" customWidth="1"/>
-    <col min="34" max="34" width="6.375" customWidth="1"/>
-    <col min="35" max="43" width="4.75" customWidth="1"/>
+    <col min="19" max="22" width="6.5" customWidth="1"/>
+    <col min="23" max="24" width="9.125" customWidth="1"/>
+    <col min="25" max="29" width="4.875" customWidth="1"/>
+    <col min="30" max="31" width="9.375" customWidth="1"/>
+    <col min="32" max="32" width="4.25" customWidth="1"/>
+    <col min="33" max="33" width="9.875" customWidth="1"/>
+    <col min="34" max="34" width="9.375" customWidth="1"/>
+    <col min="35" max="35" width="6.375" customWidth="1"/>
+    <col min="36" max="44" width="4.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:43" ht="69" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:44" ht="69" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="31" t="s">
         <v>71</v>
       </c>
@@ -3383,76 +3419,79 @@
         <v>360</v>
       </c>
       <c r="U1" s="33" t="s">
+        <v>438</v>
+      </c>
+      <c r="V1" s="33" t="s">
         <v>402</v>
       </c>
-      <c r="V1" s="33" t="s">
+      <c r="W1" s="33" t="s">
         <v>273</v>
       </c>
-      <c r="W1" s="33" t="s">
+      <c r="X1" s="33" t="s">
         <v>409</v>
       </c>
-      <c r="X1" s="34" t="s">
+      <c r="Y1" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="Y1" s="34" t="s">
+      <c r="Z1" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="Z1" s="34" t="s">
+      <c r="AA1" s="34" t="s">
         <v>76</v>
       </c>
-      <c r="AA1" s="34" t="s">
+      <c r="AB1" s="34" t="s">
         <v>77</v>
       </c>
-      <c r="AB1" s="34" t="s">
+      <c r="AC1" s="34" t="s">
         <v>78</v>
       </c>
-      <c r="AC1" s="34" t="s">
+      <c r="AD1" s="34" t="s">
         <v>79</v>
       </c>
-      <c r="AD1" s="34" t="s">
+      <c r="AE1" s="34" t="s">
         <v>69</v>
       </c>
-      <c r="AE1" s="34" t="s">
+      <c r="AF1" s="34" t="s">
         <v>170</v>
       </c>
-      <c r="AF1" s="34" t="s">
+      <c r="AG1" s="34" t="s">
         <v>395</v>
       </c>
-      <c r="AG1" s="34" t="s">
+      <c r="AH1" s="34" t="s">
         <v>125</v>
       </c>
-      <c r="AH1" s="35" t="s">
+      <c r="AI1" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="AI1" s="35" t="s">
+      <c r="AJ1" s="35" t="s">
         <v>80</v>
       </c>
-      <c r="AJ1" s="35" t="s">
+      <c r="AK1" s="35" t="s">
         <v>70</v>
       </c>
-      <c r="AK1" s="35" t="s">
+      <c r="AL1" s="35" t="s">
         <v>81</v>
       </c>
-      <c r="AL1" s="35" t="s">
+      <c r="AM1" s="35" t="s">
         <v>171</v>
       </c>
-      <c r="AM1" s="36" t="s">
+      <c r="AN1" s="36" t="s">
         <v>25</v>
       </c>
-      <c r="AN1" s="36" t="s">
+      <c r="AO1" s="36" t="s">
         <v>26</v>
       </c>
-      <c r="AO1" s="36" t="s">
+      <c r="AP1" s="36" t="s">
         <v>30</v>
       </c>
-      <c r="AP1" s="36" t="s">
+      <c r="AQ1" s="36" t="s">
         <v>27</v>
       </c>
-      <c r="AQ1" s="36" t="s">
+      <c r="AR1" s="36" t="s">
         <v>384</v>
       </c>
     </row>
-    <row r="2" spans="1:43" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>53</v>
       </c>
@@ -3514,22 +3553,22 @@
         <v>361</v>
       </c>
       <c r="U2" s="13" t="s">
+        <v>439</v>
+      </c>
+      <c r="V2" s="13" t="s">
         <v>218</v>
       </c>
-      <c r="V2" s="13" t="s">
+      <c r="W2" s="13" t="s">
         <v>274</v>
       </c>
-      <c r="W2" s="13" t="s">
+      <c r="X2" s="13" t="s">
         <v>410</v>
       </c>
-      <c r="X2" s="7" t="s">
+      <c r="Y2" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="Y2" s="7" t="s">
-        <v>0</v>
-      </c>
       <c r="Z2" s="7" t="s">
-        <v>53</v>
+        <v>0</v>
       </c>
       <c r="AA2" s="7" t="s">
         <v>53</v>
@@ -3538,23 +3577,23 @@
         <v>53</v>
       </c>
       <c r="AC2" s="7" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="AD2" s="7" t="s">
         <v>57</v>
       </c>
       <c r="AE2" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="AF2" s="7" t="s">
         <v>169</v>
       </c>
-      <c r="AF2" s="7" t="s">
+      <c r="AG2" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="AG2" s="7" t="s">
+      <c r="AH2" s="7" t="s">
         <v>356</v>
       </c>
-      <c r="AH2" s="3" t="s">
-        <v>0</v>
-      </c>
       <c r="AI2" s="3" t="s">
         <v>0</v>
       </c>
@@ -3562,13 +3601,13 @@
         <v>0</v>
       </c>
       <c r="AK2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="AL2" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="AL2" s="3" t="s">
+      <c r="AM2" s="3" t="s">
         <v>172</v>
-      </c>
-      <c r="AM2" s="9" t="s">
-        <v>24</v>
       </c>
       <c r="AN2" s="9" t="s">
         <v>24</v>
@@ -3580,10 +3619,13 @@
         <v>24</v>
       </c>
       <c r="AQ2" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="AR2" s="9" t="s">
         <v>385</v>
       </c>
     </row>
-    <row r="3" spans="1:43" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A3" s="8" t="s">
         <v>58</v>
       </c>
@@ -3645,76 +3687,79 @@
         <v>362</v>
       </c>
       <c r="U3" s="14" t="s">
+        <v>440</v>
+      </c>
+      <c r="V3" s="14" t="s">
         <v>403</v>
       </c>
-      <c r="V3" s="14" t="s">
+      <c r="W3" s="14" t="s">
         <v>275</v>
       </c>
-      <c r="W3" s="14" t="s">
+      <c r="X3" s="14" t="s">
         <v>411</v>
       </c>
-      <c r="X3" s="6" t="s">
+      <c r="Y3" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="Y3" s="6" t="s">
+      <c r="Z3" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="Z3" s="6" t="s">
+      <c r="AA3" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="AA3" s="6" t="s">
+      <c r="AB3" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="AB3" s="6" t="s">
+      <c r="AC3" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="AC3" s="6" t="s">
+      <c r="AD3" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="AD3" s="6" t="s">
+      <c r="AE3" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="AE3" s="6" t="s">
+      <c r="AF3" s="6" t="s">
         <v>168</v>
       </c>
-      <c r="AF3" s="6" t="s">
+      <c r="AG3" s="6" t="s">
         <v>396</v>
       </c>
-      <c r="AG3" s="6" t="s">
+      <c r="AH3" s="6" t="s">
         <v>334</v>
       </c>
-      <c r="AH3" s="2" t="s">
+      <c r="AI3" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="AI3" s="2" t="s">
+      <c r="AJ3" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="AJ3" s="2" t="s">
+      <c r="AK3" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="AK3" s="2" t="s">
+      <c r="AL3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="AL3" s="2" t="s">
+      <c r="AM3" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="AM3" s="8" t="s">
+      <c r="AN3" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="AN3" s="8" t="s">
+      <c r="AO3" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="AO3" s="8" t="s">
+      <c r="AP3" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="AP3" s="8" t="s">
+      <c r="AQ3" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="AQ3" s="8" t="s">
+      <c r="AR3" s="8" t="s">
         <v>386</v>
       </c>
     </row>
-    <row r="4" spans="1:43" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A4">
         <v>42000001</v>
       </c>
@@ -3752,13 +3797,13 @@
       </c>
       <c r="S4" s="11"/>
       <c r="T4" s="11"/>
-      <c r="U4" s="11"/>
+      <c r="U4" s="11" t="s">
+        <v>441</v>
+      </c>
       <c r="V4" s="11"/>
-      <c r="W4" s="11" t="s">
+      <c r="W4" s="11"/>
+      <c r="X4" s="11" t="s">
         <v>412</v>
-      </c>
-      <c r="X4">
-        <v>100</v>
       </c>
       <c r="Y4">
         <v>100</v>
@@ -3772,7 +3817,7 @@
       <c r="AB4">
         <v>100</v>
       </c>
-      <c r="AH4">
+      <c r="AC4">
         <v>100</v>
       </c>
       <c r="AI4">
@@ -3784,8 +3829,11 @@
       <c r="AK4">
         <v>100</v>
       </c>
-    </row>
-    <row r="5" spans="1:43" x14ac:dyDescent="0.15">
+      <c r="AL4">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A5" s="10">
         <v>42000002</v>
       </c>
@@ -3816,7 +3864,7 @@
       <c r="O5" s="5"/>
       <c r="P5" s="5"/>
     </row>
-    <row r="6" spans="1:43" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A6" s="10">
         <v>42000003</v>
       </c>
@@ -3849,7 +3897,7 @@
       <c r="O6" s="5"/>
       <c r="P6" s="5"/>
     </row>
-    <row r="7" spans="1:43" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A7" s="10">
         <v>42000004</v>
       </c>
@@ -3882,7 +3930,7 @@
       <c r="O7" s="5"/>
       <c r="P7" s="5"/>
     </row>
-    <row r="8" spans="1:43" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A8" s="10">
         <v>42000005</v>
       </c>
@@ -3914,14 +3962,14 @@
       <c r="N8" s="5"/>
       <c r="O8" s="5"/>
       <c r="P8" s="5"/>
-      <c r="AM8">
+      <c r="AN8">
         <v>-100</v>
       </c>
-      <c r="AO8">
+      <c r="AP8">
         <v>100</v>
       </c>
     </row>
-    <row r="9" spans="1:43" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A9" s="10">
         <v>42000006</v>
       </c>
@@ -3953,14 +4001,14 @@
       <c r="N9" s="5"/>
       <c r="O9" s="5"/>
       <c r="P9" s="5"/>
-      <c r="AM9">
+      <c r="AN9">
         <v>-100</v>
       </c>
-      <c r="AP9">
+      <c r="AQ9">
         <v>100</v>
       </c>
     </row>
-    <row r="10" spans="1:43" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A10" s="10">
         <v>42000007</v>
       </c>
@@ -3992,14 +4040,14 @@
       <c r="N10" s="5"/>
       <c r="O10" s="5"/>
       <c r="P10" s="5"/>
-      <c r="AM10">
+      <c r="AN10">
         <v>-100</v>
       </c>
-      <c r="AN10">
+      <c r="AO10">
         <v>100</v>
       </c>
     </row>
-    <row r="11" spans="1:43" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A11">
         <v>42010001</v>
       </c>
@@ -4032,7 +4080,7 @@
       <c r="O11" s="5"/>
       <c r="P11" s="5"/>
     </row>
-    <row r="12" spans="1:43" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A12">
         <v>42010002</v>
       </c>
@@ -4068,7 +4116,7 @@
       <c r="O12" s="5"/>
       <c r="P12" s="5"/>
     </row>
-    <row r="13" spans="1:43" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A13">
         <v>42010003</v>
       </c>
@@ -4106,17 +4154,17 @@
       <c r="Q13" s="4" t="s">
         <v>435</v>
       </c>
-      <c r="X13">
+      <c r="Y13">
         <v>70</v>
       </c>
-      <c r="Y13">
+      <c r="Z13">
         <v>100</v>
       </c>
-      <c r="AJ13">
+      <c r="AK13">
         <v>70</v>
       </c>
     </row>
-    <row r="14" spans="1:43" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A14">
         <v>42010004</v>
       </c>
@@ -4151,17 +4199,17 @@
       <c r="N14" s="5"/>
       <c r="O14" s="5"/>
       <c r="P14" s="5"/>
-      <c r="AB14">
-        <v>30</v>
-      </c>
-      <c r="AH14">
+      <c r="AC14">
         <v>30</v>
       </c>
       <c r="AI14">
         <v>30</v>
       </c>
-    </row>
-    <row r="15" spans="1:43" x14ac:dyDescent="0.15">
+      <c r="AJ14">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A15">
         <v>42010005</v>
       </c>
@@ -4193,14 +4241,14 @@
       <c r="N15" s="5"/>
       <c r="O15" s="5"/>
       <c r="P15" s="5"/>
-      <c r="Y15">
+      <c r="Z15">
         <v>100</v>
       </c>
-      <c r="AA15">
+      <c r="AB15">
         <v>100</v>
       </c>
     </row>
-    <row r="16" spans="1:43" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A16">
         <v>42010006</v>
       </c>
@@ -4238,17 +4286,17 @@
       <c r="Q16" s="4" t="s">
         <v>340</v>
       </c>
-      <c r="X16">
+      <c r="Y16">
         <v>100</v>
       </c>
-      <c r="AB16">
+      <c r="AC16">
         <v>50</v>
       </c>
-      <c r="AJ16">
+      <c r="AK16">
         <v>100</v>
       </c>
     </row>
-    <row r="17" spans="1:37" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A17">
         <v>42010007</v>
       </c>
@@ -4283,20 +4331,20 @@
       <c r="N17" s="5"/>
       <c r="O17" s="5"/>
       <c r="P17" s="5"/>
-      <c r="V17">
+      <c r="W17">
         <v>17000005</v>
       </c>
-      <c r="X17">
+      <c r="Y17">
         <v>150</v>
       </c>
-      <c r="AH17">
+      <c r="AI17">
         <v>150</v>
       </c>
-      <c r="AK17">
+      <c r="AL17">
         <v>50</v>
       </c>
     </row>
-    <row r="18" spans="1:37" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A18">
         <v>42010008</v>
       </c>
@@ -4328,14 +4376,14 @@
       <c r="N18" s="5"/>
       <c r="O18" s="5"/>
       <c r="P18" s="5"/>
-      <c r="Y18">
+      <c r="Z18">
         <v>100</v>
       </c>
-      <c r="AD18" s="4" t="s">
+      <c r="AE18" s="4" t="s">
         <v>307</v>
       </c>
     </row>
-    <row r="19" spans="1:37" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A19">
         <v>42010009</v>
       </c>
@@ -4367,11 +4415,11 @@
       <c r="N19" s="5"/>
       <c r="O19" s="5"/>
       <c r="P19" s="5"/>
-      <c r="AD19" t="s">
+      <c r="AE19" t="s">
         <v>308</v>
       </c>
     </row>
-    <row r="20" spans="1:37" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A20">
         <v>42010010</v>
       </c>
@@ -4403,14 +4451,14 @@
       <c r="N20" s="5"/>
       <c r="O20" s="5"/>
       <c r="P20" s="5"/>
-      <c r="AD20" t="s">
+      <c r="AE20" t="s">
         <v>309</v>
       </c>
-      <c r="AJ20">
+      <c r="AK20">
         <v>50</v>
       </c>
     </row>
-    <row r="21" spans="1:37" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A21">
         <v>42010011</v>
       </c>
@@ -4442,14 +4490,14 @@
       <c r="N21" s="5"/>
       <c r="O21" s="5"/>
       <c r="P21" s="5"/>
-      <c r="AA21">
+      <c r="AB21">
         <v>150</v>
       </c>
-      <c r="AD21" t="s">
+      <c r="AE21" t="s">
         <v>310</v>
       </c>
     </row>
-    <row r="22" spans="1:37" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A22">
         <v>42010012</v>
       </c>
@@ -4487,17 +4535,17 @@
       <c r="Q22" s="4" t="s">
         <v>341</v>
       </c>
-      <c r="X22">
-        <v>100</v>
-      </c>
       <c r="Y22">
         <v>100</v>
       </c>
-      <c r="AJ22">
+      <c r="Z22">
+        <v>100</v>
+      </c>
+      <c r="AK22">
         <v>150</v>
       </c>
     </row>
-    <row r="23" spans="1:37" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A23">
         <v>42010013</v>
       </c>
@@ -4535,17 +4583,17 @@
       <c r="Q23" s="4" t="s">
         <v>342</v>
       </c>
-      <c r="X23">
+      <c r="Y23">
         <v>50</v>
       </c>
-      <c r="Y23">
+      <c r="Z23">
         <v>150</v>
       </c>
-      <c r="AJ23">
+      <c r="AK23">
         <v>100</v>
       </c>
     </row>
-    <row r="24" spans="1:37" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A24">
         <v>42010014</v>
       </c>
@@ -4583,23 +4631,23 @@
       <c r="Q24" s="4" t="s">
         <v>343</v>
       </c>
-      <c r="X24">
+      <c r="Y24">
         <v>100</v>
       </c>
-      <c r="AB24">
+      <c r="AC24">
         <v>100</v>
       </c>
-      <c r="AD24" t="s">
+      <c r="AE24" t="s">
         <v>418</v>
-      </c>
-      <c r="AJ24">
-        <v>100</v>
       </c>
       <c r="AK24">
         <v>100</v>
       </c>
-    </row>
-    <row r="25" spans="1:37" x14ac:dyDescent="0.15">
+      <c r="AL24">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="25" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A25">
         <v>42010015</v>
       </c>
@@ -4634,11 +4682,11 @@
       <c r="N25" s="5"/>
       <c r="O25" s="5"/>
       <c r="P25" s="5"/>
-      <c r="AJ25">
+      <c r="AK25">
         <v>80</v>
       </c>
     </row>
-    <row r="26" spans="1:37" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A26">
         <v>42010016</v>
       </c>
@@ -4673,11 +4721,11 @@
       <c r="T26" t="s">
         <v>363</v>
       </c>
-      <c r="Y26">
+      <c r="Z26">
         <v>50</v>
       </c>
     </row>
-    <row r="27" spans="1:37" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A27">
         <v>42010017</v>
       </c>
@@ -4715,23 +4763,23 @@
       <c r="Q27" s="4" t="s">
         <v>344</v>
       </c>
-      <c r="X27">
+      <c r="Y27">
         <v>200</v>
       </c>
-      <c r="Y27">
+      <c r="Z27">
         <v>100</v>
       </c>
-      <c r="AB27">
+      <c r="AC27">
         <v>100</v>
       </c>
-      <c r="AD27" t="s">
+      <c r="AE27" t="s">
         <v>417</v>
       </c>
-      <c r="AJ27">
+      <c r="AK27">
         <v>100</v>
       </c>
     </row>
-    <row r="28" spans="1:37" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A28">
         <v>42010018</v>
       </c>
@@ -4766,7 +4814,7 @@
       <c r="O28" s="5"/>
       <c r="P28" s="5"/>
     </row>
-    <row r="29" spans="1:37" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A29">
         <v>42010019</v>
       </c>
@@ -4803,14 +4851,14 @@
       <c r="N29" s="5"/>
       <c r="O29" s="5"/>
       <c r="P29" s="5"/>
-      <c r="AI29">
+      <c r="AJ29">
         <v>100</v>
       </c>
-      <c r="AJ29">
+      <c r="AK29">
         <v>50</v>
       </c>
     </row>
-    <row r="30" spans="1:37" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A30">
         <v>42010020</v>
       </c>
@@ -4847,14 +4895,14 @@
       <c r="N30" s="5"/>
       <c r="O30" s="5"/>
       <c r="P30" s="5"/>
-      <c r="AI30">
+      <c r="AJ30">
         <v>50</v>
       </c>
-      <c r="AJ30">
+      <c r="AK30">
         <v>100</v>
       </c>
     </row>
-    <row r="31" spans="1:37" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A31">
         <v>42010021</v>
       </c>
@@ -4889,11 +4937,11 @@
       <c r="N31" s="5"/>
       <c r="O31" s="5"/>
       <c r="P31" s="5"/>
-      <c r="AK31">
+      <c r="AL31">
         <v>200</v>
       </c>
     </row>
-    <row r="32" spans="1:37" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A32">
         <v>42010022</v>
       </c>
@@ -4931,17 +4979,17 @@
       <c r="Q32" s="4" t="s">
         <v>345</v>
       </c>
-      <c r="AB32">
+      <c r="AC32">
         <v>100</v>
       </c>
-      <c r="AC32" t="s">
+      <c r="AD32" t="s">
         <v>304</v>
       </c>
-      <c r="AJ32">
+      <c r="AK32">
         <v>150</v>
       </c>
     </row>
-    <row r="33" spans="1:38" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:39" x14ac:dyDescent="0.15">
       <c r="A33">
         <v>42010023</v>
       </c>
@@ -4976,17 +5024,17 @@
       <c r="N33" s="5"/>
       <c r="O33" s="5"/>
       <c r="P33" s="5"/>
-      <c r="Y33">
+      <c r="Z33">
         <v>200</v>
       </c>
-      <c r="Z33">
+      <c r="AA33">
         <v>100</v>
       </c>
-      <c r="AJ33">
+      <c r="AK33">
         <v>100</v>
       </c>
     </row>
-    <row r="34" spans="1:38" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:39" x14ac:dyDescent="0.15">
       <c r="A34">
         <v>42010024</v>
       </c>
@@ -5018,11 +5066,11 @@
       <c r="N34" s="5"/>
       <c r="O34" s="5"/>
       <c r="P34" s="5"/>
-      <c r="AE34">
+      <c r="AF34">
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:38" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:39" x14ac:dyDescent="0.15">
       <c r="A35">
         <v>42010025</v>
       </c>
@@ -5054,11 +5102,11 @@
       <c r="N35" s="5"/>
       <c r="O35" s="5"/>
       <c r="P35" s="5"/>
-      <c r="Y35">
+      <c r="Z35">
         <v>150</v>
       </c>
     </row>
-    <row r="36" spans="1:38" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:39" x14ac:dyDescent="0.15">
       <c r="A36">
         <v>42010026</v>
       </c>
@@ -5090,11 +5138,11 @@
       <c r="N36" s="5"/>
       <c r="O36" s="5"/>
       <c r="P36" s="5"/>
-      <c r="Z36">
+      <c r="AA36">
         <v>70</v>
       </c>
     </row>
-    <row r="37" spans="1:38" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:39" x14ac:dyDescent="0.15">
       <c r="A37">
         <v>42010027</v>
       </c>
@@ -5126,11 +5174,11 @@
       <c r="N37" s="5"/>
       <c r="O37" s="5"/>
       <c r="P37" s="5"/>
-      <c r="Y37">
+      <c r="Z37">
         <v>70</v>
       </c>
     </row>
-    <row r="38" spans="1:38" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:39" x14ac:dyDescent="0.15">
       <c r="A38">
         <v>42010028</v>
       </c>
@@ -5168,11 +5216,11 @@
       <c r="R38">
         <v>13010004</v>
       </c>
-      <c r="AJ38">
+      <c r="AK38">
         <v>150</v>
       </c>
     </row>
-    <row r="39" spans="1:38" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:39" x14ac:dyDescent="0.15">
       <c r="A39">
         <v>42010029</v>
       </c>
@@ -5205,7 +5253,7 @@
       <c r="O39" s="5"/>
       <c r="P39" s="5"/>
     </row>
-    <row r="40" spans="1:38" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:39" x14ac:dyDescent="0.15">
       <c r="A40">
         <v>42010030</v>
       </c>
@@ -5243,23 +5291,23 @@
       <c r="Q40" s="4" t="s">
         <v>346</v>
       </c>
-      <c r="X40">
+      <c r="Y40">
         <v>100</v>
       </c>
-      <c r="Y40">
+      <c r="Z40">
         <v>150</v>
       </c>
-      <c r="AB40">
+      <c r="AC40">
         <v>100</v>
       </c>
-      <c r="AJ40">
+      <c r="AK40">
         <v>100</v>
       </c>
-      <c r="AK40">
+      <c r="AL40">
         <v>150</v>
       </c>
     </row>
-    <row r="41" spans="1:38" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:39" x14ac:dyDescent="0.15">
       <c r="A41">
         <v>42010031</v>
       </c>
@@ -5294,20 +5342,20 @@
       <c r="N41" s="5"/>
       <c r="O41" s="5"/>
       <c r="P41" s="5"/>
-      <c r="V41">
+      <c r="W41">
         <v>17000009</v>
       </c>
-      <c r="X41">
+      <c r="Y41">
         <v>100</v>
       </c>
-      <c r="AB41">
+      <c r="AC41">
         <v>50</v>
       </c>
-      <c r="AH41">
+      <c r="AI41">
         <v>50</v>
       </c>
     </row>
-    <row r="42" spans="1:38" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:39" x14ac:dyDescent="0.15">
       <c r="A42">
         <v>42010032</v>
       </c>
@@ -5339,14 +5387,14 @@
       <c r="N42" s="5"/>
       <c r="O42" s="5"/>
       <c r="P42" s="5"/>
-      <c r="Y42">
+      <c r="Z42">
         <v>50</v>
       </c>
-      <c r="AA42">
+      <c r="AB42">
         <v>50</v>
       </c>
     </row>
-    <row r="43" spans="1:38" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:39" x14ac:dyDescent="0.15">
       <c r="A43">
         <v>42010033</v>
       </c>
@@ -5384,20 +5432,20 @@
       <c r="Q43" s="4" t="s">
         <v>437</v>
       </c>
-      <c r="Y43">
+      <c r="Z43">
         <v>100</v>
       </c>
-      <c r="AB43">
+      <c r="AC43">
         <v>50</v>
       </c>
-      <c r="AJ43">
+      <c r="AK43">
         <v>100</v>
       </c>
-      <c r="AK43">
+      <c r="AL43">
         <v>50</v>
       </c>
     </row>
-    <row r="44" spans="1:38" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:39" x14ac:dyDescent="0.15">
       <c r="A44">
         <v>42010034</v>
       </c>
@@ -5435,20 +5483,20 @@
       <c r="Q44" s="4" t="s">
         <v>347</v>
       </c>
-      <c r="Y44">
+      <c r="Z44">
         <v>100</v>
       </c>
-      <c r="AB44">
+      <c r="AC44">
         <v>50</v>
       </c>
-      <c r="AJ44">
+      <c r="AK44">
         <v>100</v>
       </c>
-      <c r="AK44">
+      <c r="AL44">
         <v>50</v>
       </c>
     </row>
-    <row r="45" spans="1:38" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:39" x14ac:dyDescent="0.15">
       <c r="A45">
         <v>42010035</v>
       </c>
@@ -5486,23 +5534,23 @@
       <c r="Q45" s="11" t="s">
         <v>348</v>
       </c>
-      <c r="X45">
+      <c r="Y45">
         <v>150</v>
       </c>
-      <c r="Y45">
+      <c r="Z45">
         <v>50</v>
       </c>
-      <c r="AC45" t="s">
+      <c r="AD45" t="s">
         <v>358</v>
       </c>
-      <c r="AJ45">
+      <c r="AK45">
         <v>150</v>
       </c>
-      <c r="AK45">
+      <c r="AL45">
         <v>50</v>
       </c>
     </row>
-    <row r="46" spans="1:38" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:39" x14ac:dyDescent="0.15">
       <c r="A46">
         <v>42010036</v>
       </c>
@@ -5543,23 +5591,23 @@
       <c r="T46" t="s">
         <v>367</v>
       </c>
-      <c r="X46">
+      <c r="Y46">
         <v>100</v>
       </c>
-      <c r="AB46">
+      <c r="AC46">
         <v>200</v>
       </c>
-      <c r="AJ46">
+      <c r="AK46">
         <v>200</v>
       </c>
-      <c r="AK46">
+      <c r="AL46">
         <v>100</v>
       </c>
-      <c r="AL46">
+      <c r="AM46">
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:38" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:39" x14ac:dyDescent="0.15">
       <c r="A47">
         <v>42010037</v>
       </c>
@@ -5595,17 +5643,17 @@
       <c r="O47" s="5"/>
       <c r="P47" s="5"/>
       <c r="Q47" s="11"/>
-      <c r="X47">
-        <v>150</v>
-      </c>
-      <c r="AI47">
+      <c r="Y47">
         <v>150</v>
       </c>
       <c r="AJ47">
         <v>150</v>
       </c>
-    </row>
-    <row r="48" spans="1:38" x14ac:dyDescent="0.15">
+      <c r="AK47">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="48" spans="1:39" x14ac:dyDescent="0.15">
       <c r="A48">
         <v>42010038</v>
       </c>
@@ -5637,14 +5685,14 @@
       <c r="N48" s="5"/>
       <c r="O48" s="5"/>
       <c r="P48" s="5"/>
-      <c r="X48">
-        <v>50</v>
-      </c>
       <c r="Y48">
         <v>50</v>
       </c>
-    </row>
-    <row r="49" spans="1:43" x14ac:dyDescent="0.15">
+      <c r="Z48">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="49" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A49">
         <v>42010039</v>
       </c>
@@ -5679,20 +5727,20 @@
       <c r="N49" s="5"/>
       <c r="O49" s="5"/>
       <c r="P49" s="5"/>
-      <c r="X49">
+      <c r="Y49">
         <v>70</v>
       </c>
-      <c r="AC49" t="s">
+      <c r="AD49" t="s">
         <v>383</v>
       </c>
-      <c r="AE49">
+      <c r="AF49">
         <v>2</v>
       </c>
-      <c r="AJ49">
+      <c r="AK49">
         <v>300</v>
       </c>
     </row>
-    <row r="50" spans="1:43" x14ac:dyDescent="0.15">
+    <row r="50" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A50">
         <v>42010040</v>
       </c>
@@ -5724,14 +5772,14 @@
       <c r="N50" s="5"/>
       <c r="O50" s="5"/>
       <c r="P50" s="5"/>
-      <c r="AM50">
+      <c r="AN50">
         <v>-100</v>
       </c>
-      <c r="AQ50" t="s">
+      <c r="AR50" t="s">
         <v>390</v>
       </c>
     </row>
-    <row r="51" spans="1:43" x14ac:dyDescent="0.15">
+    <row r="51" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A51">
         <v>42010041</v>
       </c>
@@ -5769,20 +5817,20 @@
       <c r="Q51" t="s">
         <v>394</v>
       </c>
-      <c r="Y51">
+      <c r="Z51">
         <v>100</v>
       </c>
-      <c r="AB51">
+      <c r="AC51">
         <v>50</v>
-      </c>
-      <c r="AI51">
-        <v>100</v>
       </c>
       <c r="AJ51">
         <v>100</v>
       </c>
-    </row>
-    <row r="52" spans="1:43" x14ac:dyDescent="0.15">
+      <c r="AK51">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="52" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A52">
         <v>42010042</v>
       </c>
@@ -5814,11 +5862,11 @@
       <c r="N52" s="5"/>
       <c r="O52" s="5"/>
       <c r="P52" s="5"/>
-      <c r="AF52">
+      <c r="AG52">
         <v>16020001</v>
       </c>
     </row>
-    <row r="53" spans="1:43" x14ac:dyDescent="0.15">
+    <row r="53" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A53">
         <v>42010043</v>
       </c>
@@ -5850,11 +5898,11 @@
       <c r="N53" s="5"/>
       <c r="O53" s="5"/>
       <c r="P53" s="5"/>
-      <c r="U53" t="s">
+      <c r="V53" t="s">
         <v>407</v>
       </c>
     </row>
-    <row r="54" spans="1:43" x14ac:dyDescent="0.15">
+    <row r="54" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A54">
         <v>42010044</v>
       </c>
@@ -5892,21 +5940,21 @@
       <c r="Q54" s="11" t="s">
         <v>436</v>
       </c>
-      <c r="W54" t="s">
+      <c r="X54" t="s">
         <v>427</v>
-      </c>
-      <c r="Z54">
-        <v>70</v>
       </c>
       <c r="AA54">
         <v>70</v>
       </c>
-      <c r="AD54" s="38"/>
-      <c r="AJ54">
+      <c r="AB54">
+        <v>70</v>
+      </c>
+      <c r="AE54" s="38"/>
+      <c r="AK54">
         <v>100</v>
       </c>
     </row>
-    <row r="55" spans="1:43" x14ac:dyDescent="0.15">
+    <row r="55" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A55">
         <v>42010045</v>
       </c>
@@ -5938,11 +5986,8 @@
       <c r="N55" s="5"/>
       <c r="O55" s="5"/>
       <c r="P55" s="5"/>
-      <c r="W55" t="s">
+      <c r="X55" t="s">
         <v>422</v>
-      </c>
-      <c r="X55">
-        <v>120</v>
       </c>
       <c r="Y55">
         <v>120</v>
@@ -5950,8 +5995,11 @@
       <c r="Z55">
         <v>120</v>
       </c>
-    </row>
-    <row r="56" spans="1:43" x14ac:dyDescent="0.15">
+      <c r="AA55">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="56" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A56">
         <v>42010046</v>
       </c>
@@ -5983,23 +6031,23 @@
       <c r="N56" s="5"/>
       <c r="O56" s="5"/>
       <c r="P56" s="5"/>
-      <c r="W56" t="s">
+      <c r="X56" t="s">
         <v>433</v>
       </c>
-      <c r="Y56">
+      <c r="Z56">
         <v>80</v>
       </c>
-      <c r="AA56">
+      <c r="AB56">
         <v>50</v>
       </c>
-      <c r="AI56">
+      <c r="AJ56">
         <v>100</v>
       </c>
-      <c r="AK56">
+      <c r="AL56">
         <v>100</v>
       </c>
     </row>
-    <row r="57" spans="1:43" x14ac:dyDescent="0.15">
+    <row r="57" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A57">
         <v>42020001</v>
       </c>
@@ -6037,20 +6085,20 @@
       <c r="Q57" s="38" t="s">
         <v>351</v>
       </c>
-      <c r="AB57">
+      <c r="AC57">
         <v>100</v>
       </c>
-      <c r="AG57" t="s">
+      <c r="AH57" t="s">
         <v>351</v>
-      </c>
-      <c r="AJ57">
-        <v>200</v>
       </c>
       <c r="AK57">
         <v>200</v>
       </c>
-    </row>
-    <row r="58" spans="1:43" x14ac:dyDescent="0.15">
+      <c r="AL57">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="58" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A58">
         <v>42020002</v>
       </c>
@@ -6088,23 +6136,23 @@
       <c r="Q58" s="11" t="s">
         <v>348</v>
       </c>
-      <c r="X58">
+      <c r="Y58">
         <v>200</v>
       </c>
-      <c r="Y58">
+      <c r="Z58">
         <v>50</v>
       </c>
-      <c r="AD58" t="s">
+      <c r="AE58" t="s">
         <v>417</v>
-      </c>
-      <c r="AJ58">
-        <v>150</v>
       </c>
       <c r="AK58">
         <v>150</v>
       </c>
-    </row>
-    <row r="59" spans="1:43" x14ac:dyDescent="0.15">
+      <c r="AL58">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="59" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A59">
         <v>42020003</v>
       </c>
@@ -6140,14 +6188,14 @@
       <c r="O59" s="5"/>
       <c r="P59" s="5"/>
       <c r="Q59" s="38"/>
-      <c r="AH59">
+      <c r="AI59">
         <v>100</v>
       </c>
-      <c r="AJ59">
+      <c r="AK59">
         <v>100</v>
       </c>
     </row>
-    <row r="60" spans="1:43" x14ac:dyDescent="0.15">
+    <row r="60" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A60">
         <v>42020004</v>
       </c>
@@ -6182,14 +6230,14 @@
       <c r="N60" s="5"/>
       <c r="O60" s="5"/>
       <c r="P60" s="5"/>
-      <c r="AE60">
+      <c r="AF60">
         <v>1</v>
       </c>
-      <c r="AL60">
+      <c r="AM60">
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:43" x14ac:dyDescent="0.15">
+    <row r="61" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A61">
         <v>42020005</v>
       </c>
@@ -6227,20 +6275,20 @@
       <c r="Q61" s="11" t="s">
         <v>349</v>
       </c>
-      <c r="X61">
-        <v>150</v>
-      </c>
       <c r="Y61">
         <v>150</v>
       </c>
-      <c r="AH61">
-        <v>200</v>
+      <c r="Z61">
+        <v>150</v>
       </c>
       <c r="AI61">
         <v>200</v>
       </c>
-    </row>
-    <row r="62" spans="1:43" x14ac:dyDescent="0.15">
+      <c r="AJ61">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="62" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A62">
         <v>42020006</v>
       </c>
@@ -6278,17 +6326,17 @@
       <c r="Q62" s="4" t="s">
         <v>350</v>
       </c>
-      <c r="X62">
+      <c r="Y62">
         <v>300</v>
       </c>
-      <c r="AB62">
+      <c r="AC62">
         <v>200</v>
       </c>
-      <c r="AJ62">
+      <c r="AK62">
         <v>300</v>
       </c>
     </row>
-    <row r="63" spans="1:43" x14ac:dyDescent="0.15">
+    <row r="63" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A63">
         <v>42020007</v>
       </c>
@@ -6322,7 +6370,7 @@
       <c r="P63" s="5"/>
       <c r="Q63" s="38"/>
     </row>
-    <row r="64" spans="1:43" x14ac:dyDescent="0.15">
+    <row r="64" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A64">
         <v>42020008</v>
       </c>
@@ -6355,7 +6403,7 @@
       <c r="O64" s="5"/>
       <c r="P64" s="5"/>
     </row>
-    <row r="65" spans="1:37" x14ac:dyDescent="0.15">
+    <row r="65" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A65">
         <v>42020009</v>
       </c>
@@ -6387,20 +6435,20 @@
       <c r="N65" s="5"/>
       <c r="O65" s="5"/>
       <c r="P65" s="5"/>
-      <c r="V65">
+      <c r="W65">
         <v>17000001</v>
       </c>
-      <c r="X65">
+      <c r="Y65">
         <v>200</v>
       </c>
-      <c r="Y65">
+      <c r="Z65">
         <v>150</v>
       </c>
-      <c r="AC65" t="s">
+      <c r="AD65" t="s">
         <v>305</v>
       </c>
     </row>
-    <row r="66" spans="1:37" x14ac:dyDescent="0.15">
+    <row r="66" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A66">
         <v>42020010</v>
       </c>
@@ -6432,17 +6480,17 @@
       <c r="N66" s="5"/>
       <c r="O66" s="5"/>
       <c r="P66" s="5"/>
-      <c r="V66">
+      <c r="W66">
         <v>17000003</v>
       </c>
-      <c r="X66">
+      <c r="Y66">
         <v>250</v>
       </c>
-      <c r="AK66">
+      <c r="AL66">
         <v>100</v>
       </c>
     </row>
-    <row r="67" spans="1:37" x14ac:dyDescent="0.15">
+    <row r="67" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A67">
         <v>42020011</v>
       </c>
@@ -6474,17 +6522,17 @@
       <c r="N67" s="5"/>
       <c r="O67" s="5"/>
       <c r="P67" s="5"/>
-      <c r="V67">
+      <c r="W67">
         <v>17000002</v>
       </c>
-      <c r="AC67" t="s">
+      <c r="AD67" t="s">
         <v>306</v>
       </c>
-      <c r="AE67">
+      <c r="AF67">
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:37" x14ac:dyDescent="0.15">
+    <row r="68" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A68">
         <v>42020012</v>
       </c>
@@ -6516,20 +6564,20 @@
       <c r="N68" s="5"/>
       <c r="O68" s="5"/>
       <c r="P68" s="5"/>
-      <c r="W68" t="s">
+      <c r="X68" t="s">
         <v>414</v>
       </c>
-      <c r="X68">
+      <c r="Y68">
         <v>150</v>
       </c>
-      <c r="AD68" s="11" t="s">
+      <c r="AE68" s="11" t="s">
         <v>416</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
-  <conditionalFormatting sqref="B4:AQ42 B44:AQ68 B43:P43 R43:AQ43">
-    <cfRule type="containsBlanks" dxfId="26" priority="10">
+  <conditionalFormatting sqref="B4:AR42 B44:AR68 B43:P43 R43:AR43">
+    <cfRule type="containsBlanks" dxfId="2" priority="10">
       <formula>LEN(TRIM(B4))=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6544,11 +6592,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AQ33"/>
+  <dimension ref="A1:AR33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F22" sqref="F22"/>
+      <selection pane="bottomLeft" activeCell="U1" sqref="U1:U3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -6560,16 +6608,16 @@
     <col min="11" max="16" width="4.875" customWidth="1"/>
     <col min="17" max="17" width="9.75" customWidth="1"/>
     <col min="18" max="18" width="9.25" customWidth="1"/>
-    <col min="19" max="23" width="5.75" customWidth="1"/>
-    <col min="24" max="28" width="4.125" customWidth="1"/>
-    <col min="29" max="29" width="9.75" customWidth="1"/>
-    <col min="30" max="30" width="7.5" customWidth="1"/>
-    <col min="31" max="32" width="5.125" customWidth="1"/>
-    <col min="33" max="33" width="9.375" customWidth="1"/>
-    <col min="35" max="43" width="5" customWidth="1"/>
+    <col min="19" max="24" width="5.75" customWidth="1"/>
+    <col min="25" max="29" width="4.125" customWidth="1"/>
+    <col min="30" max="30" width="9.75" customWidth="1"/>
+    <col min="31" max="31" width="7.5" customWidth="1"/>
+    <col min="32" max="33" width="5.125" customWidth="1"/>
+    <col min="34" max="34" width="9.375" customWidth="1"/>
+    <col min="36" max="44" width="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:43" ht="69.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:44" ht="69.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="31" t="s">
         <v>71</v>
       </c>
@@ -6631,76 +6679,79 @@
         <v>360</v>
       </c>
       <c r="U1" s="33" t="s">
+        <v>438</v>
+      </c>
+      <c r="V1" s="33" t="s">
         <v>402</v>
       </c>
-      <c r="V1" s="33" t="s">
+      <c r="W1" s="33" t="s">
         <v>273</v>
       </c>
-      <c r="W1" s="33" t="s">
+      <c r="X1" s="33" t="s">
         <v>409</v>
       </c>
-      <c r="X1" s="34" t="s">
+      <c r="Y1" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="Y1" s="34" t="s">
+      <c r="Z1" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="Z1" s="34" t="s">
+      <c r="AA1" s="34" t="s">
         <v>76</v>
       </c>
-      <c r="AA1" s="34" t="s">
+      <c r="AB1" s="34" t="s">
         <v>77</v>
       </c>
-      <c r="AB1" s="34" t="s">
+      <c r="AC1" s="34" t="s">
         <v>78</v>
       </c>
-      <c r="AC1" s="34" t="s">
+      <c r="AD1" s="34" t="s">
         <v>79</v>
       </c>
-      <c r="AD1" s="34" t="s">
+      <c r="AE1" s="34" t="s">
         <v>69</v>
       </c>
-      <c r="AE1" s="34" t="s">
+      <c r="AF1" s="34" t="s">
         <v>397</v>
       </c>
-      <c r="AF1" s="34" t="s">
+      <c r="AG1" s="34" t="s">
         <v>395</v>
       </c>
-      <c r="AG1" s="34" t="s">
+      <c r="AH1" s="34" t="s">
         <v>125</v>
       </c>
-      <c r="AH1" s="35" t="s">
+      <c r="AI1" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="AI1" s="35" t="s">
+      <c r="AJ1" s="35" t="s">
         <v>80</v>
       </c>
-      <c r="AJ1" s="35" t="s">
+      <c r="AK1" s="35" t="s">
         <v>70</v>
       </c>
-      <c r="AK1" s="35" t="s">
+      <c r="AL1" s="35" t="s">
         <v>81</v>
       </c>
-      <c r="AL1" s="35" t="s">
+      <c r="AM1" s="35" t="s">
         <v>170</v>
       </c>
-      <c r="AM1" s="36" t="s">
+      <c r="AN1" s="36" t="s">
         <v>25</v>
       </c>
-      <c r="AN1" s="36" t="s">
+      <c r="AO1" s="36" t="s">
         <v>26</v>
       </c>
-      <c r="AO1" s="36" t="s">
+      <c r="AP1" s="36" t="s">
         <v>30</v>
       </c>
-      <c r="AP1" s="36" t="s">
+      <c r="AQ1" s="36" t="s">
         <v>27</v>
       </c>
-      <c r="AQ1" s="36" t="s">
+      <c r="AR1" s="36" t="s">
         <v>384</v>
       </c>
     </row>
-    <row r="2" spans="1:43" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>53</v>
       </c>
@@ -6762,22 +6813,22 @@
         <v>361</v>
       </c>
       <c r="U2" s="13" t="s">
+        <v>439</v>
+      </c>
+      <c r="V2" s="13" t="s">
         <v>218</v>
       </c>
-      <c r="V2" s="13" t="s">
+      <c r="W2" s="13" t="s">
         <v>274</v>
       </c>
-      <c r="W2" s="13" t="s">
+      <c r="X2" s="13" t="s">
         <v>410</v>
       </c>
-      <c r="X2" s="7" t="s">
+      <c r="Y2" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="Y2" s="7" t="s">
-        <v>0</v>
-      </c>
       <c r="Z2" s="7" t="s">
-        <v>53</v>
+        <v>0</v>
       </c>
       <c r="AA2" s="7" t="s">
         <v>53</v>
@@ -6786,23 +6837,23 @@
         <v>53</v>
       </c>
       <c r="AC2" s="7" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="AD2" s="7" t="s">
         <v>57</v>
       </c>
       <c r="AE2" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="AF2" s="7" t="s">
         <v>169</v>
       </c>
-      <c r="AF2" s="7" t="s">
+      <c r="AG2" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="AG2" s="7" t="s">
+      <c r="AH2" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="AH2" s="3" t="s">
-        <v>0</v>
-      </c>
       <c r="AI2" s="3" t="s">
         <v>0</v>
       </c>
@@ -6810,13 +6861,13 @@
         <v>0</v>
       </c>
       <c r="AK2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="AL2" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="AL2" s="3" t="s">
+      <c r="AM2" s="3" t="s">
         <v>172</v>
-      </c>
-      <c r="AM2" s="9" t="s">
-        <v>24</v>
       </c>
       <c r="AN2" s="9" t="s">
         <v>24</v>
@@ -6828,10 +6879,13 @@
         <v>24</v>
       </c>
       <c r="AQ2" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="AR2" s="9" t="s">
         <v>385</v>
       </c>
     </row>
-    <row r="3" spans="1:43" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A3" s="8" t="s">
         <v>58</v>
       </c>
@@ -6893,76 +6947,79 @@
         <v>362</v>
       </c>
       <c r="U3" s="14" t="s">
+        <v>440</v>
+      </c>
+      <c r="V3" s="14" t="s">
         <v>403</v>
       </c>
-      <c r="V3" s="14" t="s">
+      <c r="W3" s="14" t="s">
         <v>275</v>
       </c>
-      <c r="W3" s="14" t="s">
+      <c r="X3" s="14" t="s">
         <v>411</v>
       </c>
-      <c r="X3" s="6" t="s">
+      <c r="Y3" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="Y3" s="6" t="s">
+      <c r="Z3" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="Z3" s="6" t="s">
+      <c r="AA3" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="AA3" s="6" t="s">
+      <c r="AB3" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="AB3" s="6" t="s">
+      <c r="AC3" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="AC3" s="6" t="s">
+      <c r="AD3" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="AD3" s="6" t="s">
+      <c r="AE3" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="AE3" s="6" t="s">
+      <c r="AF3" s="6" t="s">
         <v>168</v>
       </c>
-      <c r="AF3" s="6" t="s">
+      <c r="AG3" s="6" t="s">
         <v>396</v>
       </c>
-      <c r="AG3" s="6" t="s">
+      <c r="AH3" s="6" t="s">
         <v>334</v>
       </c>
-      <c r="AH3" s="2" t="s">
+      <c r="AI3" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="AI3" s="2" t="s">
+      <c r="AJ3" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="AJ3" s="2" t="s">
+      <c r="AK3" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="AK3" s="2" t="s">
+      <c r="AL3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="AL3" s="2" t="s">
+      <c r="AM3" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="AM3" s="8" t="s">
+      <c r="AN3" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="AN3" s="8" t="s">
+      <c r="AO3" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="AO3" s="8" t="s">
+      <c r="AP3" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="AP3" s="8" t="s">
+      <c r="AQ3" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="AQ3" s="8" t="s">
+      <c r="AR3" s="8" t="s">
         <v>386</v>
       </c>
     </row>
-    <row r="4" spans="1:43" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A4" s="10">
         <v>42110001</v>
       </c>
@@ -7000,18 +7057,19 @@
       <c r="U4" s="12"/>
       <c r="V4" s="12"/>
       <c r="W4" s="12"/>
-      <c r="AM4">
+      <c r="X4" s="12"/>
+      <c r="AN4">
         <v>-30</v>
-      </c>
-      <c r="AO4">
-        <v>100</v>
       </c>
       <c r="AP4">
         <v>100</v>
       </c>
-      <c r="AQ4" s="29"/>
-    </row>
-    <row r="5" spans="1:43" x14ac:dyDescent="0.15">
+      <c r="AQ4">
+        <v>100</v>
+      </c>
+      <c r="AR4" s="29"/>
+    </row>
+    <row r="5" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A5" s="10">
         <v>42110002</v>
       </c>
@@ -7049,15 +7107,16 @@
       <c r="U5" s="12"/>
       <c r="V5" s="12"/>
       <c r="W5" s="12"/>
-      <c r="AM5">
+      <c r="X5" s="12"/>
+      <c r="AN5">
         <v>-20</v>
       </c>
-      <c r="AN5">
+      <c r="AO5">
         <v>100</v>
       </c>
-      <c r="AQ5" s="29"/>
-    </row>
-    <row r="6" spans="1:43" x14ac:dyDescent="0.15">
+      <c r="AR5" s="29"/>
+    </row>
+    <row r="6" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A6" s="10">
         <v>42110003</v>
       </c>
@@ -7095,9 +7154,10 @@
       <c r="U6" s="12"/>
       <c r="V6" s="12"/>
       <c r="W6" s="12"/>
-      <c r="AQ6" s="29"/>
-    </row>
-    <row r="7" spans="1:43" x14ac:dyDescent="0.15">
+      <c r="X6" s="12"/>
+      <c r="AR6" s="29"/>
+    </row>
+    <row r="7" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A7" s="10">
         <v>42110004</v>
       </c>
@@ -7129,9 +7189,9 @@
       <c r="N7" s="5"/>
       <c r="O7" s="5"/>
       <c r="P7" s="5"/>
-      <c r="AQ7" s="29"/>
-    </row>
-    <row r="8" spans="1:43" x14ac:dyDescent="0.15">
+      <c r="AR7" s="29"/>
+    </row>
+    <row r="8" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A8" s="10">
         <v>42110005</v>
       </c>
@@ -7169,9 +7229,10 @@
       <c r="U8" s="12"/>
       <c r="V8" s="12"/>
       <c r="W8" s="12"/>
-      <c r="AQ8" s="29"/>
-    </row>
-    <row r="9" spans="1:43" x14ac:dyDescent="0.15">
+      <c r="X8" s="12"/>
+      <c r="AR8" s="29"/>
+    </row>
+    <row r="9" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A9">
         <v>42120001</v>
       </c>
@@ -7209,9 +7270,10 @@
       <c r="U9" s="11"/>
       <c r="V9" s="11"/>
       <c r="W9" s="11"/>
-      <c r="AQ9" s="29"/>
-    </row>
-    <row r="10" spans="1:43" x14ac:dyDescent="0.15">
+      <c r="X9" s="11"/>
+      <c r="AR9" s="29"/>
+    </row>
+    <row r="10" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A10">
         <v>42120002</v>
       </c>
@@ -7251,12 +7313,13 @@
       <c r="U10" s="11"/>
       <c r="V10" s="11"/>
       <c r="W10" s="11"/>
-      <c r="AG10" t="s">
+      <c r="X10" s="11"/>
+      <c r="AH10" t="s">
         <v>335</v>
       </c>
-      <c r="AQ10" s="29"/>
-    </row>
-    <row r="11" spans="1:43" x14ac:dyDescent="0.15">
+      <c r="AR10" s="29"/>
+    </row>
+    <row r="11" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A11">
         <v>42120003</v>
       </c>
@@ -7293,9 +7356,10 @@
       <c r="U11" s="11"/>
       <c r="V11" s="11"/>
       <c r="W11" s="11"/>
-      <c r="AQ11" s="29"/>
-    </row>
-    <row r="12" spans="1:43" x14ac:dyDescent="0.15">
+      <c r="X11" s="11"/>
+      <c r="AR11" s="29"/>
+    </row>
+    <row r="12" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A12">
         <v>42120004</v>
       </c>
@@ -7337,12 +7401,13 @@
       <c r="U12" s="11"/>
       <c r="V12" s="11"/>
       <c r="W12" s="11"/>
-      <c r="AG12" t="s">
+      <c r="X12" s="11"/>
+      <c r="AH12" t="s">
         <v>336</v>
       </c>
-      <c r="AQ12" s="29"/>
-    </row>
-    <row r="13" spans="1:43" x14ac:dyDescent="0.15">
+      <c r="AR12" s="29"/>
+    </row>
+    <row r="13" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A13">
         <v>42120005</v>
       </c>
@@ -7376,14 +7441,15 @@
       <c r="R13" s="11"/>
       <c r="S13" s="11"/>
       <c r="T13" s="11"/>
-      <c r="U13" s="4" t="s">
+      <c r="U13" s="11"/>
+      <c r="V13" s="4" t="s">
         <v>408</v>
       </c>
-      <c r="V13" s="11"/>
       <c r="W13" s="11"/>
-      <c r="AQ13" s="29"/>
-    </row>
-    <row r="14" spans="1:43" x14ac:dyDescent="0.15">
+      <c r="X13" s="11"/>
+      <c r="AR13" s="29"/>
+    </row>
+    <row r="14" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A14">
         <v>42120006</v>
       </c>
@@ -7424,9 +7490,10 @@
       <c r="U14" s="11"/>
       <c r="V14" s="11"/>
       <c r="W14" s="11"/>
-      <c r="AQ14" s="29"/>
-    </row>
-    <row r="15" spans="1:43" x14ac:dyDescent="0.15">
+      <c r="X14" s="11"/>
+      <c r="AR14" s="29"/>
+    </row>
+    <row r="15" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A15">
         <v>42120007</v>
       </c>
@@ -7464,9 +7531,10 @@
       <c r="U15" s="11"/>
       <c r="V15" s="11"/>
       <c r="W15" s="11"/>
-      <c r="AQ15" s="29"/>
-    </row>
-    <row r="16" spans="1:43" x14ac:dyDescent="0.15">
+      <c r="X15" s="11"/>
+      <c r="AR15" s="29"/>
+    </row>
+    <row r="16" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A16">
         <v>42120008</v>
       </c>
@@ -7504,9 +7572,10 @@
       <c r="U16" s="11"/>
       <c r="V16" s="11"/>
       <c r="W16" s="11"/>
-      <c r="AQ16" s="29"/>
-    </row>
-    <row r="17" spans="1:43" x14ac:dyDescent="0.15">
+      <c r="X16" s="11"/>
+      <c r="AR16" s="29"/>
+    </row>
+    <row r="17" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A17">
         <v>42120009</v>
       </c>
@@ -7544,9 +7613,10 @@
       <c r="U17" s="11"/>
       <c r="V17" s="11"/>
       <c r="W17" s="11"/>
-      <c r="AQ17" s="29"/>
-    </row>
-    <row r="18" spans="1:43" x14ac:dyDescent="0.15">
+      <c r="X17" s="11"/>
+      <c r="AR17" s="29"/>
+    </row>
+    <row r="18" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A18">
         <v>42120010</v>
       </c>
@@ -7584,9 +7654,10 @@
       <c r="U18" s="11"/>
       <c r="V18" s="11"/>
       <c r="W18" s="11"/>
-      <c r="AQ18" s="29"/>
-    </row>
-    <row r="19" spans="1:43" x14ac:dyDescent="0.15">
+      <c r="X18" s="11"/>
+      <c r="AR18" s="29"/>
+    </row>
+    <row r="19" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A19">
         <v>42120011</v>
       </c>
@@ -7624,9 +7695,10 @@
       <c r="U19" s="11"/>
       <c r="V19" s="11"/>
       <c r="W19" s="11"/>
-      <c r="AQ19" s="29"/>
-    </row>
-    <row r="20" spans="1:43" x14ac:dyDescent="0.15">
+      <c r="X19" s="11"/>
+      <c r="AR19" s="29"/>
+    </row>
+    <row r="20" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A20">
         <v>42120013</v>
       </c>
@@ -7664,9 +7736,10 @@
       <c r="U20" s="11"/>
       <c r="V20" s="11"/>
       <c r="W20" s="11"/>
-      <c r="AQ20" s="29"/>
-    </row>
-    <row r="21" spans="1:43" x14ac:dyDescent="0.15">
+      <c r="X20" s="11"/>
+      <c r="AR20" s="29"/>
+    </row>
+    <row r="21" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A21">
         <v>42120014</v>
       </c>
@@ -7704,9 +7777,10 @@
       <c r="U21" s="11"/>
       <c r="V21" s="11"/>
       <c r="W21" s="11"/>
-      <c r="AQ21" s="29"/>
-    </row>
-    <row r="22" spans="1:43" x14ac:dyDescent="0.15">
+      <c r="X21" s="11"/>
+      <c r="AR21" s="29"/>
+    </row>
+    <row r="22" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A22">
         <v>42120015</v>
       </c>
@@ -7744,9 +7818,10 @@
       <c r="U22" s="11"/>
       <c r="V22" s="11"/>
       <c r="W22" s="11"/>
-      <c r="AQ22" s="29"/>
-    </row>
-    <row r="23" spans="1:43" x14ac:dyDescent="0.15">
+      <c r="X22" s="11"/>
+      <c r="AR22" s="29"/>
+    </row>
+    <row r="23" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A23">
         <v>42120016</v>
       </c>
@@ -7781,9 +7856,10 @@
       <c r="U23" s="11"/>
       <c r="V23" s="11"/>
       <c r="W23" s="11"/>
-      <c r="AQ23" s="29"/>
-    </row>
-    <row r="24" spans="1:43" x14ac:dyDescent="0.15">
+      <c r="X23" s="11"/>
+      <c r="AR23" s="29"/>
+    </row>
+    <row r="24" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A24">
         <v>42120017</v>
       </c>
@@ -7823,12 +7899,13 @@
       <c r="U24" s="11"/>
       <c r="V24" s="11"/>
       <c r="W24" s="11"/>
-      <c r="AB24">
+      <c r="X24" s="11"/>
+      <c r="AC24">
         <v>30</v>
       </c>
-      <c r="AQ24" s="29"/>
-    </row>
-    <row r="25" spans="1:43" x14ac:dyDescent="0.15">
+      <c r="AR24" s="29"/>
+    </row>
+    <row r="25" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A25">
         <v>42120018</v>
       </c>
@@ -7868,12 +7945,13 @@
       <c r="U25" s="18"/>
       <c r="V25" s="18"/>
       <c r="W25" s="18"/>
-      <c r="AB25">
+      <c r="X25" s="18"/>
+      <c r="AC25">
         <v>50</v>
       </c>
-      <c r="AQ25" s="29"/>
-    </row>
-    <row r="26" spans="1:43" x14ac:dyDescent="0.15">
+      <c r="AR25" s="29"/>
+    </row>
+    <row r="26" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A26">
         <v>42120019</v>
       </c>
@@ -7915,9 +7993,10 @@
       <c r="U26" s="19"/>
       <c r="V26" s="19"/>
       <c r="W26" s="19"/>
-      <c r="AQ26" s="29"/>
-    </row>
-    <row r="27" spans="1:43" x14ac:dyDescent="0.15">
+      <c r="X26" s="19"/>
+      <c r="AR26" s="29"/>
+    </row>
+    <row r="27" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A27">
         <v>42130001</v>
       </c>
@@ -7957,9 +8036,10 @@
       <c r="U27" s="11"/>
       <c r="V27" s="11"/>
       <c r="W27" s="11"/>
-      <c r="AQ27" s="29"/>
-    </row>
-    <row r="28" spans="1:43" x14ac:dyDescent="0.15">
+      <c r="X27" s="11"/>
+      <c r="AR27" s="29"/>
+    </row>
+    <row r="28" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A28">
         <v>42130002</v>
       </c>
@@ -8001,9 +8081,10 @@
       <c r="U28" s="11"/>
       <c r="V28" s="11"/>
       <c r="W28" s="11"/>
-      <c r="AQ28" s="29"/>
-    </row>
-    <row r="29" spans="1:43" x14ac:dyDescent="0.15">
+      <c r="X28" s="11"/>
+      <c r="AR28" s="29"/>
+    </row>
+    <row r="29" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A29">
         <v>42130003</v>
       </c>
@@ -8048,18 +8129,19 @@
       <c r="U29" s="11"/>
       <c r="V29" s="11"/>
       <c r="W29" s="11"/>
-      <c r="AB29">
+      <c r="X29" s="11"/>
+      <c r="AC29">
         <v>300</v>
-      </c>
-      <c r="AJ29">
-        <v>200</v>
       </c>
       <c r="AK29">
         <v>200</v>
       </c>
-      <c r="AQ29" s="29"/>
-    </row>
-    <row r="30" spans="1:43" x14ac:dyDescent="0.15">
+      <c r="AL29">
+        <v>200</v>
+      </c>
+      <c r="AR29" s="29"/>
+    </row>
+    <row r="30" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A30">
         <v>42130004</v>
       </c>
@@ -8099,9 +8181,10 @@
       <c r="U30" s="11"/>
       <c r="V30" s="11"/>
       <c r="W30" s="11"/>
-      <c r="AQ30" s="29"/>
-    </row>
-    <row r="31" spans="1:43" x14ac:dyDescent="0.15">
+      <c r="X30" s="11"/>
+      <c r="AR30" s="29"/>
+    </row>
+    <row r="31" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A31">
         <v>42130005</v>
       </c>
@@ -8141,9 +8224,10 @@
       <c r="U31" s="11"/>
       <c r="V31" s="11"/>
       <c r="W31" s="11"/>
-      <c r="AQ31" s="29"/>
-    </row>
-    <row r="32" spans="1:43" x14ac:dyDescent="0.15">
+      <c r="X31" s="11"/>
+      <c r="AR31" s="29"/>
+    </row>
+    <row r="32" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A32">
         <v>42130006</v>
       </c>
@@ -8183,9 +8267,10 @@
       <c r="U32" s="11"/>
       <c r="V32" s="11"/>
       <c r="W32" s="11"/>
-      <c r="AQ32" s="29"/>
-    </row>
-    <row r="33" spans="1:43" x14ac:dyDescent="0.15">
+      <c r="X32" s="11"/>
+      <c r="AR32" s="29"/>
+    </row>
+    <row r="33" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A33">
         <v>42130007</v>
       </c>
@@ -8227,23 +8312,24 @@
       <c r="S33" s="18"/>
       <c r="T33" s="18"/>
       <c r="U33" s="18"/>
-      <c r="V33" s="11"/>
+      <c r="V33" s="18"/>
       <c r="W33" s="11"/>
-      <c r="AB33">
+      <c r="X33" s="11"/>
+      <c r="AC33">
         <v>300</v>
-      </c>
-      <c r="AJ33">
-        <v>200</v>
       </c>
       <c r="AK33">
         <v>200</v>
       </c>
-      <c r="AQ33" s="29"/>
+      <c r="AL33">
+        <v>200</v>
+      </c>
+      <c r="AR33" s="29"/>
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
-  <conditionalFormatting sqref="D4:AQ33">
-    <cfRule type="containsBlanks" dxfId="16" priority="3">
+  <conditionalFormatting sqref="D4:AR33">
+    <cfRule type="containsBlanks" dxfId="1" priority="3">
       <formula>LEN(TRIM(D4))=0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
a base version of choose
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/SceneQuest.xlsx
+++ b/ConfigData/Xlsx/SceneQuest.xlsx
@@ -1,31 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18326"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\code\TOMClassicGit\ConfigData\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Code\TOMClassicGit\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="4" r:id="rId1"/>
     <sheet name="MapSet" sheetId="5" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>real</author>
   </authors>
   <commentList>
-    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
+    <comment ref="E1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="886" uniqueCount="497">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="892" uniqueCount="500">
   <si>
     <t>int</t>
     <phoneticPr fontId="18" type="noConversion"/>
@@ -1910,13 +1910,24 @@
   </si>
   <si>
     <t>金币交易系数</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>ChooseGold2</t>
+  </si>
+  <si>
+    <t>选择默认成功</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>ChooseWinRate</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="25" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -3140,120 +3151,122 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="表3" displayName="表3" ref="A3:AV79" totalsRowShown="0" headerRowDxfId="27">
-  <autoFilter ref="A3:AV79" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
-  <sortState ref="A4:AV74">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="表3" displayName="表3" ref="A3:AW79" totalsRowShown="0" headerRowDxfId="27">
+  <autoFilter ref="A3:AW79"/>
+  <sortState ref="A4:AW74">
     <sortCondition ref="A3:A74"/>
   </sortState>
-  <tableColumns count="48">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Id"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Name"/>
-    <tableColumn id="28" xr3:uid="{00000000-0010-0000-0000-00001C000000}" name="Type"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Level"/>
-    <tableColumn id="25" xr3:uid="{00000000-0010-0000-0000-000019000000}" name="Danger"/>
-    <tableColumn id="24" xr3:uid="{00000000-0010-0000-0000-000018000000}" name="Ename"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Figue"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Script"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="TriggerMulti" dataDxfId="26"/>
-    <tableColumn id="40" xr3:uid="{00000000-0010-0000-0000-000028000000}" name="Catalog" dataDxfId="25"/>
-    <tableColumn id="35" xr3:uid="{00000000-0010-0000-0000-000023000000}" name="TriggerHourBegin" dataDxfId="24"/>
-    <tableColumn id="34" xr3:uid="{00000000-0010-0000-0000-000022000000}" name="TriggerHourEnd" dataDxfId="23"/>
-    <tableColumn id="36" xr3:uid="{00000000-0010-0000-0000-000024000000}" name="TriggerQuestNotReceive" dataDxfId="22"/>
-    <tableColumn id="37" xr3:uid="{00000000-0010-0000-0000-000025000000}" name="TriggerQuestReceived" dataDxfId="21"/>
-    <tableColumn id="38" xr3:uid="{00000000-0010-0000-0000-000026000000}" name="TriggerQuestFinished" dataDxfId="20"/>
-    <tableColumn id="39" xr3:uid="{00000000-0010-0000-0000-000027000000}" name="TriggerRate" dataDxfId="19"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="EnemyName"/>
-    <tableColumn id="32" xr3:uid="{00000000-0010-0000-0000-000020000000}" name="SceneId"/>
-    <tableColumn id="29" xr3:uid="{00000000-0010-0000-0000-00001D000000}" name="Position"/>
-    <tableColumn id="27" xr3:uid="{00000000-0010-0000-0000-00001B000000}" name="NextQuest"/>
-    <tableColumn id="44" xr3:uid="{00000000-0010-0000-0000-00002C000000}" name="HiddenRoomQuest"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="ShopName"/>
-    <tableColumn id="41" xr3:uid="{00000000-0010-0000-0000-000029000000}" name="MiniGameId"/>
-    <tableColumn id="43" xr3:uid="{00000000-0010-0000-0000-00002B000000}" name="PayKey"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="RewardGold"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="RewardFood"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="RewardHealth"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="RewardMental"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="RewardExp"/>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="RewardItem"/>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="RewardDrop"/>
-    <tableColumn id="30" xr3:uid="{00000000-0010-0000-0000-00001E000000}" name="RewardBlessLevel"/>
-    <tableColumn id="42" xr3:uid="{00000000-0010-0000-0000-00002A000000}" name="RewardBlessId"/>
-    <tableColumn id="26" xr3:uid="{00000000-0010-0000-0000-00001A000000}" name="UnlockRival"/>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="PunishGold"/>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="PunishFood"/>
-    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="PunishHealth"/>
-    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0000-000013000000}" name="PunishMental"/>
-    <tableColumn id="31" xr3:uid="{00000000-0010-0000-0000-00001F000000}" name="PunishBlessLevel"/>
-    <tableColumn id="46" xr3:uid="{00552E44-0B9B-407A-AE91-296748ED701C}" name="ChooseGold"/>
-    <tableColumn id="47" xr3:uid="{D0866443-A86A-4FCD-B594-E53B3EC76F57}" name="ChooseGoldAddon"/>
-    <tableColumn id="45" xr3:uid="{CC71E815-AA73-46E7-A3DF-B4B3949E8312}" name="ChooseFood"/>
-    <tableColumn id="48" xr3:uid="{3B080BC5-ADB8-4DA6-9A5F-133BFD456A96}" name="ChooseFoodAddon"/>
-    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0000-000014000000}" name="TradeGold"/>
-    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0000-000015000000}" name="TradeFood"/>
-    <tableColumn id="22" xr3:uid="{00000000-0010-0000-0000-000016000000}" name="TradeHealth"/>
-    <tableColumn id="23" xr3:uid="{00000000-0010-0000-0000-000017000000}" name="TradeMental"/>
-    <tableColumn id="33" xr3:uid="{00000000-0010-0000-0000-000021000000}" name="TradeDropItem"/>
+  <tableColumns count="49">
+    <tableColumn id="1" name="Id"/>
+    <tableColumn id="2" name="Name"/>
+    <tableColumn id="28" name="Type"/>
+    <tableColumn id="3" name="Level"/>
+    <tableColumn id="25" name="Danger"/>
+    <tableColumn id="24" name="Ename"/>
+    <tableColumn id="4" name="Figue"/>
+    <tableColumn id="5" name="Script"/>
+    <tableColumn id="6" name="TriggerMulti" dataDxfId="26"/>
+    <tableColumn id="40" name="Catalog" dataDxfId="25"/>
+    <tableColumn id="35" name="TriggerHourBegin" dataDxfId="24"/>
+    <tableColumn id="34" name="TriggerHourEnd" dataDxfId="23"/>
+    <tableColumn id="36" name="TriggerQuestNotReceive" dataDxfId="22"/>
+    <tableColumn id="37" name="TriggerQuestReceived" dataDxfId="21"/>
+    <tableColumn id="38" name="TriggerQuestFinished" dataDxfId="20"/>
+    <tableColumn id="39" name="TriggerRate" dataDxfId="19"/>
+    <tableColumn id="7" name="EnemyName"/>
+    <tableColumn id="32" name="SceneId"/>
+    <tableColumn id="29" name="Position"/>
+    <tableColumn id="27" name="NextQuest"/>
+    <tableColumn id="44" name="HiddenRoomQuest"/>
+    <tableColumn id="8" name="ShopName"/>
+    <tableColumn id="41" name="MiniGameId"/>
+    <tableColumn id="43" name="PayKey"/>
+    <tableColumn id="9" name="RewardGold"/>
+    <tableColumn id="10" name="RewardFood"/>
+    <tableColumn id="11" name="RewardHealth"/>
+    <tableColumn id="12" name="RewardMental"/>
+    <tableColumn id="13" name="RewardExp"/>
+    <tableColumn id="14" name="RewardItem"/>
+    <tableColumn id="15" name="RewardDrop"/>
+    <tableColumn id="30" name="RewardBlessLevel"/>
+    <tableColumn id="42" name="RewardBlessId"/>
+    <tableColumn id="26" name="UnlockRival"/>
+    <tableColumn id="16" name="PunishGold"/>
+    <tableColumn id="17" name="PunishFood"/>
+    <tableColumn id="18" name="PunishHealth"/>
+    <tableColumn id="19" name="PunishMental"/>
+    <tableColumn id="31" name="PunishBlessLevel"/>
+    <tableColumn id="49" name="ChooseWinRate"/>
+    <tableColumn id="46" name="ChooseGold2"/>
+    <tableColumn id="47" name="ChooseGoldAddon"/>
+    <tableColumn id="45" name="ChooseFood"/>
+    <tableColumn id="48" name="ChooseFoodAddon"/>
+    <tableColumn id="20" name="TradeGold"/>
+    <tableColumn id="21" name="TradeFood"/>
+    <tableColumn id="22" name="TradeHealth"/>
+    <tableColumn id="23" name="TradeMental"/>
+    <tableColumn id="33" name="TradeDropItem"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="表3_5" displayName="表3_5" ref="A3:AV33" totalsRowShown="0" headerRowDxfId="18">
-  <autoFilter ref="A3:AV33" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="表3_5" displayName="表3_5" ref="A3:AW33" totalsRowShown="0" headerRowDxfId="18">
+  <autoFilter ref="A3:AW33"/>
   <sortState ref="A4:AE6">
     <sortCondition ref="A3:A6"/>
   </sortState>
-  <tableColumns count="48">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Id"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Name"/>
-    <tableColumn id="27" xr3:uid="{00000000-0010-0000-0100-00001B000000}" name="Type" dataDxfId="17"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Level"/>
-    <tableColumn id="25" xr3:uid="{00000000-0010-0000-0100-000019000000}" name="Danger"/>
-    <tableColumn id="24" xr3:uid="{00000000-0010-0000-0100-000018000000}" name="Ename"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Figue"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="Script"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="TriggerMulti"/>
-    <tableColumn id="40" xr3:uid="{00000000-0010-0000-0100-000028000000}" name="Catalog" dataDxfId="16"/>
-    <tableColumn id="35" xr3:uid="{00000000-0010-0000-0100-000023000000}" name="TriggerHourBegin" dataDxfId="15"/>
-    <tableColumn id="34" xr3:uid="{00000000-0010-0000-0100-000022000000}" name="TriggerHourEnd" dataDxfId="14"/>
-    <tableColumn id="37" xr3:uid="{00000000-0010-0000-0100-000025000000}" name="TriggerQuestNotReceive" dataDxfId="13"/>
-    <tableColumn id="38" xr3:uid="{00000000-0010-0000-0100-000026000000}" name="TriggerQuestReceived" dataDxfId="12"/>
-    <tableColumn id="36" xr3:uid="{00000000-0010-0000-0100-000024000000}" name="TriggerQuestFinished" dataDxfId="11"/>
-    <tableColumn id="39" xr3:uid="{00000000-0010-0000-0100-000027000000}" name="TriggerRate" dataDxfId="10"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="EnemyName"/>
-    <tableColumn id="32" xr3:uid="{00000000-0010-0000-0100-000020000000}" name="SceneId" dataDxfId="9"/>
-    <tableColumn id="29" xr3:uid="{00000000-0010-0000-0100-00001D000000}" name="Position" dataDxfId="8"/>
-    <tableColumn id="28" xr3:uid="{00000000-0010-0000-0100-00001C000000}" name="NextQuest" dataDxfId="7"/>
-    <tableColumn id="44" xr3:uid="{00000000-0010-0000-0100-00002C000000}" name="HiddenRoomQuest" dataDxfId="6"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="ShopName" dataDxfId="5"/>
-    <tableColumn id="41" xr3:uid="{00000000-0010-0000-0100-000029000000}" name="MiniGameId" dataDxfId="4"/>
-    <tableColumn id="43" xr3:uid="{00000000-0010-0000-0100-00002B000000}" name="PayKey" dataDxfId="3"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0100-000009000000}" name="RewardGold"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0100-00000A000000}" name="RewardFood"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0100-00000B000000}" name="RewardHealth"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0100-00000C000000}" name="RewardMental"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0100-00000D000000}" name="RewardExp"/>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0100-00000E000000}" name="RewardItem"/>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0100-00000F000000}" name="RewardDrop"/>
-    <tableColumn id="31" xr3:uid="{00000000-0010-0000-0100-00001F000000}" name="RewardBlessLevel"/>
-    <tableColumn id="42" xr3:uid="{00000000-0010-0000-0100-00002A000000}" name="RewardBlessId"/>
-    <tableColumn id="26" xr3:uid="{00000000-0010-0000-0100-00001A000000}" name="UnlockRival"/>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0100-000010000000}" name="PunishGold"/>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0100-000011000000}" name="PunishFood"/>
-    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0100-000012000000}" name="PunishHealth"/>
-    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0100-000013000000}" name="PunishMental"/>
-    <tableColumn id="30" xr3:uid="{00000000-0010-0000-0100-00001E000000}" name="PunishBlessLevel"/>
-    <tableColumn id="48" xr3:uid="{398FC92C-EEFA-4D11-8DDB-EE4276482D91}" name="ChooseGold"/>
-    <tableColumn id="47" xr3:uid="{BD2CD137-CB8C-4EA4-9C12-77720AA64BDA}" name="ChooseGoldAddon"/>
-    <tableColumn id="46" xr3:uid="{6A97FAE4-E6FC-4851-A2DA-BA02478846C5}" name="ChooseFood"/>
-    <tableColumn id="45" xr3:uid="{EA4C1D42-A911-482C-8AF0-AB29FCB2B650}" name="ChooseFoodAddon"/>
-    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0100-000014000000}" name="TradeGold"/>
-    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0100-000015000000}" name="TradeFood"/>
-    <tableColumn id="22" xr3:uid="{00000000-0010-0000-0100-000016000000}" name="TradeHealth"/>
-    <tableColumn id="23" xr3:uid="{00000000-0010-0000-0100-000017000000}" name="TradeMental"/>
-    <tableColumn id="33" xr3:uid="{00000000-0010-0000-0100-000021000000}" name="TradeDropItem" dataDxfId="2"/>
+  <tableColumns count="49">
+    <tableColumn id="1" name="Id"/>
+    <tableColumn id="2" name="Name"/>
+    <tableColumn id="27" name="Type" dataDxfId="17"/>
+    <tableColumn id="3" name="Level"/>
+    <tableColumn id="25" name="Danger"/>
+    <tableColumn id="24" name="Ename"/>
+    <tableColumn id="4" name="Figue"/>
+    <tableColumn id="5" name="Script"/>
+    <tableColumn id="6" name="TriggerMulti"/>
+    <tableColumn id="40" name="Catalog" dataDxfId="16"/>
+    <tableColumn id="35" name="TriggerHourBegin" dataDxfId="15"/>
+    <tableColumn id="34" name="TriggerHourEnd" dataDxfId="14"/>
+    <tableColumn id="37" name="TriggerQuestNotReceive" dataDxfId="13"/>
+    <tableColumn id="38" name="TriggerQuestReceived" dataDxfId="12"/>
+    <tableColumn id="36" name="TriggerQuestFinished" dataDxfId="11"/>
+    <tableColumn id="39" name="TriggerRate" dataDxfId="10"/>
+    <tableColumn id="7" name="EnemyName"/>
+    <tableColumn id="32" name="SceneId" dataDxfId="9"/>
+    <tableColumn id="29" name="Position" dataDxfId="8"/>
+    <tableColumn id="28" name="NextQuest" dataDxfId="7"/>
+    <tableColumn id="44" name="HiddenRoomQuest" dataDxfId="6"/>
+    <tableColumn id="8" name="ShopName" dataDxfId="5"/>
+    <tableColumn id="41" name="MiniGameId" dataDxfId="4"/>
+    <tableColumn id="43" name="PayKey" dataDxfId="3"/>
+    <tableColumn id="9" name="RewardGold"/>
+    <tableColumn id="10" name="RewardFood"/>
+    <tableColumn id="11" name="RewardHealth"/>
+    <tableColumn id="12" name="RewardMental"/>
+    <tableColumn id="13" name="RewardExp"/>
+    <tableColumn id="14" name="RewardItem"/>
+    <tableColumn id="15" name="RewardDrop"/>
+    <tableColumn id="31" name="RewardBlessLevel"/>
+    <tableColumn id="42" name="RewardBlessId"/>
+    <tableColumn id="26" name="UnlockRival"/>
+    <tableColumn id="16" name="PunishGold"/>
+    <tableColumn id="17" name="PunishFood"/>
+    <tableColumn id="18" name="PunishHealth"/>
+    <tableColumn id="19" name="PunishMental"/>
+    <tableColumn id="30" name="PunishBlessLevel"/>
+    <tableColumn id="49" name="ChooseWinRate"/>
+    <tableColumn id="48" name="ChooseGold"/>
+    <tableColumn id="47" name="ChooseGoldAddon"/>
+    <tableColumn id="46" name="ChooseFood"/>
+    <tableColumn id="45" name="ChooseFoodAddon"/>
+    <tableColumn id="20" name="TradeGold"/>
+    <tableColumn id="21" name="TradeFood"/>
+    <tableColumn id="22" name="TradeHealth"/>
+    <tableColumn id="23" name="TradeMental"/>
+    <tableColumn id="33" name="TradeDropItem" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3579,12 +3592,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AV79"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AW79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+    <sheetView topLeftCell="J1" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="V14" activeCellId="1" sqref="AN1:AQ3 V14"/>
+      <selection pane="bottomLeft" activeCell="AN1" sqref="AN1:AN3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -3603,10 +3616,10 @@
     <col min="33" max="33" width="9.875" customWidth="1"/>
     <col min="34" max="34" width="9.375" customWidth="1"/>
     <col min="35" max="35" width="6.375" customWidth="1"/>
-    <col min="36" max="48" width="4.75" customWidth="1"/>
+    <col min="36" max="49" width="4.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:48" ht="69" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:49" ht="69" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="31" t="s">
         <v>71</v>
       </c>
@@ -3725,34 +3738,37 @@
         <v>170</v>
       </c>
       <c r="AN1" s="40" t="s">
+        <v>498</v>
+      </c>
+      <c r="AO1" s="40" t="s">
         <v>490</v>
       </c>
-      <c r="AO1" s="40" t="s">
+      <c r="AP1" s="40" t="s">
         <v>492</v>
       </c>
-      <c r="AP1" s="40" t="s">
+      <c r="AQ1" s="40" t="s">
         <v>489</v>
       </c>
-      <c r="AQ1" s="40" t="s">
+      <c r="AR1" s="40" t="s">
         <v>494</v>
       </c>
-      <c r="AR1" s="36" t="s">
+      <c r="AS1" s="36" t="s">
         <v>25</v>
       </c>
-      <c r="AS1" s="36" t="s">
+      <c r="AT1" s="36" t="s">
         <v>26</v>
       </c>
-      <c r="AT1" s="36" t="s">
+      <c r="AU1" s="36" t="s">
         <v>30</v>
       </c>
-      <c r="AU1" s="36" t="s">
+      <c r="AV1" s="36" t="s">
         <v>27</v>
       </c>
-      <c r="AV1" s="36" t="s">
+      <c r="AW1" s="36" t="s">
         <v>382</v>
       </c>
     </row>
-    <row r="2" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:49" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>53</v>
       </c>
@@ -3871,7 +3887,7 @@
         <v>171</v>
       </c>
       <c r="AN2" s="41" t="s">
-        <v>487</v>
+        <v>53</v>
       </c>
       <c r="AO2" s="41" t="s">
         <v>487</v>
@@ -3882,8 +3898,8 @@
       <c r="AQ2" s="41" t="s">
         <v>487</v>
       </c>
-      <c r="AR2" s="9" t="s">
-        <v>24</v>
+      <c r="AR2" s="41" t="s">
+        <v>487</v>
       </c>
       <c r="AS2" s="9" t="s">
         <v>24</v>
@@ -3895,10 +3911,13 @@
         <v>24</v>
       </c>
       <c r="AV2" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="AW2" s="9" t="s">
         <v>383</v>
       </c>
     </row>
-    <row r="3" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:49" x14ac:dyDescent="0.15">
       <c r="A3" s="8" t="s">
         <v>58</v>
       </c>
@@ -4017,34 +4036,37 @@
         <v>172</v>
       </c>
       <c r="AN3" s="42" t="s">
-        <v>491</v>
+        <v>499</v>
       </c>
       <c r="AO3" s="42" t="s">
+        <v>497</v>
+      </c>
+      <c r="AP3" s="42" t="s">
         <v>493</v>
       </c>
-      <c r="AP3" s="42" t="s">
+      <c r="AQ3" s="42" t="s">
         <v>488</v>
       </c>
-      <c r="AQ3" s="42" t="s">
+      <c r="AR3" s="42" t="s">
         <v>495</v>
       </c>
-      <c r="AR3" s="8" t="s">
+      <c r="AS3" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="AS3" s="8" t="s">
+      <c r="AT3" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="AT3" s="8" t="s">
+      <c r="AU3" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="AU3" s="8" t="s">
+      <c r="AV3" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="AV3" s="8" t="s">
+      <c r="AW3" s="8" t="s">
         <v>384</v>
       </c>
     </row>
-    <row r="4" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:49" x14ac:dyDescent="0.15">
       <c r="A4">
         <v>42000001</v>
       </c>
@@ -4118,7 +4140,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="5" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:49" x14ac:dyDescent="0.15">
       <c r="A5" s="10">
         <v>42000002</v>
       </c>
@@ -4149,7 +4171,7 @@
       <c r="O5" s="5"/>
       <c r="P5" s="5"/>
     </row>
-    <row r="6" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:49" x14ac:dyDescent="0.15">
       <c r="A6" s="10">
         <v>42000003</v>
       </c>
@@ -4182,7 +4204,7 @@
       <c r="O6" s="5"/>
       <c r="P6" s="5"/>
     </row>
-    <row r="7" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:49" x14ac:dyDescent="0.15">
       <c r="A7" s="10">
         <v>42000004</v>
       </c>
@@ -4215,7 +4237,7 @@
       <c r="O7" s="5"/>
       <c r="P7" s="5"/>
     </row>
-    <row r="8" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:49" x14ac:dyDescent="0.15">
       <c r="A8" s="10">
         <v>42000005</v>
       </c>
@@ -4247,14 +4269,14 @@
       <c r="N8" s="5"/>
       <c r="O8" s="5"/>
       <c r="P8" s="5"/>
-      <c r="AR8">
+      <c r="AS8">
         <v>-100</v>
       </c>
-      <c r="AT8">
+      <c r="AU8">
         <v>100</v>
       </c>
     </row>
-    <row r="9" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:49" x14ac:dyDescent="0.15">
       <c r="A9" s="10">
         <v>42000006</v>
       </c>
@@ -4286,14 +4308,14 @@
       <c r="N9" s="5"/>
       <c r="O9" s="5"/>
       <c r="P9" s="5"/>
-      <c r="AR9">
+      <c r="AS9">
         <v>-100</v>
       </c>
-      <c r="AU9">
+      <c r="AV9">
         <v>100</v>
       </c>
     </row>
-    <row r="10" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:49" x14ac:dyDescent="0.15">
       <c r="A10" s="10">
         <v>42000007</v>
       </c>
@@ -4325,14 +4347,14 @@
       <c r="N10" s="5"/>
       <c r="O10" s="5"/>
       <c r="P10" s="5"/>
-      <c r="AR10">
+      <c r="AS10">
         <v>-100</v>
       </c>
-      <c r="AS10">
+      <c r="AT10">
         <v>100</v>
       </c>
     </row>
-    <row r="11" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:49" x14ac:dyDescent="0.15">
       <c r="A11">
         <v>42010001</v>
       </c>
@@ -4365,7 +4387,7 @@
       <c r="O11" s="5"/>
       <c r="P11" s="5"/>
     </row>
-    <row r="12" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:49" x14ac:dyDescent="0.15">
       <c r="A12">
         <v>42010002</v>
       </c>
@@ -4398,7 +4420,7 @@
       <c r="O12" s="5"/>
       <c r="P12" s="5"/>
     </row>
-    <row r="13" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:49" x14ac:dyDescent="0.15">
       <c r="A13">
         <v>42010003</v>
       </c>
@@ -4446,7 +4468,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="14" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:49" x14ac:dyDescent="0.15">
       <c r="A14">
         <v>42010004</v>
       </c>
@@ -4491,7 +4513,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:49" x14ac:dyDescent="0.15">
       <c r="A15">
         <v>42010005</v>
       </c>
@@ -4530,7 +4552,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="16" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:49" x14ac:dyDescent="0.15">
       <c r="A16">
         <v>42010006</v>
       </c>
@@ -5974,7 +5996,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="49" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="49" spans="1:49" x14ac:dyDescent="0.15">
       <c r="A49">
         <v>42010039</v>
       </c>
@@ -6022,7 +6044,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="50" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="50" spans="1:49" x14ac:dyDescent="0.15">
       <c r="A50">
         <v>42010040</v>
       </c>
@@ -6054,14 +6076,14 @@
       <c r="N50" s="5"/>
       <c r="O50" s="5"/>
       <c r="P50" s="5"/>
-      <c r="AR50">
+      <c r="AS50">
         <v>-100</v>
       </c>
-      <c r="AV50" t="s">
+      <c r="AW50" t="s">
         <v>388</v>
       </c>
     </row>
-    <row r="51" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="51" spans="1:49" x14ac:dyDescent="0.15">
       <c r="A51">
         <v>42010041</v>
       </c>
@@ -6112,7 +6134,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="52" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="52" spans="1:49" x14ac:dyDescent="0.15">
       <c r="A52">
         <v>42010042</v>
       </c>
@@ -6148,7 +6170,7 @@
         <v>16020001</v>
       </c>
     </row>
-    <row r="53" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="53" spans="1:49" x14ac:dyDescent="0.15">
       <c r="A53">
         <v>42010043</v>
       </c>
@@ -6184,7 +6206,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="54" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="54" spans="1:49" x14ac:dyDescent="0.15">
       <c r="A54">
         <v>42010044</v>
       </c>
@@ -6236,7 +6258,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="55" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="55" spans="1:49" x14ac:dyDescent="0.15">
       <c r="A55">
         <v>42010045</v>
       </c>
@@ -6281,7 +6303,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="56" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="56" spans="1:49" x14ac:dyDescent="0.15">
       <c r="A56">
         <v>42010046</v>
       </c>
@@ -6329,7 +6351,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="57" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="57" spans="1:49" x14ac:dyDescent="0.15">
       <c r="A57">
         <v>42010047</v>
       </c>
@@ -6371,7 +6393,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="58" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="58" spans="1:49" x14ac:dyDescent="0.15">
       <c r="A58">
         <v>42010048</v>
       </c>
@@ -6413,7 +6435,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="59" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="59" spans="1:49" x14ac:dyDescent="0.15">
       <c r="A59">
         <v>42010049</v>
       </c>
@@ -6458,7 +6480,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="60" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="60" spans="1:49" x14ac:dyDescent="0.15">
       <c r="A60">
         <v>42010050</v>
       </c>
@@ -6509,7 +6531,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="61" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="61" spans="1:49" x14ac:dyDescent="0.15">
       <c r="A61">
         <v>42010051</v>
       </c>
@@ -6554,7 +6576,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="62" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="62" spans="1:49" x14ac:dyDescent="0.15">
       <c r="A62">
         <v>42010052</v>
       </c>
@@ -6608,7 +6630,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="63" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="63" spans="1:49" x14ac:dyDescent="0.15">
       <c r="A63">
         <v>42020001</v>
       </c>
@@ -6659,7 +6681,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="64" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="64" spans="1:49" x14ac:dyDescent="0.15">
       <c r="A64">
         <v>42020002</v>
       </c>
@@ -7354,7 +7376,7 @@
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
-  <conditionalFormatting sqref="B4:AV79">
+  <conditionalFormatting sqref="B4:AW79">
     <cfRule type="containsBlanks" dxfId="1" priority="10">
       <formula>LEN(TRIM(B4))=0</formula>
     </cfRule>
@@ -7369,12 +7391,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:AV33"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AW33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="T8" sqref="T8"/>
+      <selection pane="bottomLeft" activeCell="AN1" sqref="AN1:AN3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -7392,10 +7414,10 @@
     <col min="31" max="31" width="7.5" customWidth="1"/>
     <col min="32" max="33" width="5.125" customWidth="1"/>
     <col min="34" max="34" width="9.375" customWidth="1"/>
-    <col min="36" max="48" width="5" customWidth="1"/>
+    <col min="36" max="49" width="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:48" ht="69.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:49" ht="69.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="31" t="s">
         <v>71</v>
       </c>
@@ -7514,34 +7536,37 @@
         <v>169</v>
       </c>
       <c r="AN1" s="40" t="s">
+        <v>498</v>
+      </c>
+      <c r="AO1" s="40" t="s">
         <v>490</v>
       </c>
-      <c r="AO1" s="40" t="s">
+      <c r="AP1" s="40" t="s">
         <v>492</v>
       </c>
-      <c r="AP1" s="40" t="s">
+      <c r="AQ1" s="40" t="s">
         <v>489</v>
       </c>
-      <c r="AQ1" s="40" t="s">
+      <c r="AR1" s="40" t="s">
         <v>494</v>
       </c>
-      <c r="AR1" s="36" t="s">
+      <c r="AS1" s="36" t="s">
         <v>496</v>
       </c>
-      <c r="AS1" s="36" t="s">
+      <c r="AT1" s="36" t="s">
         <v>26</v>
       </c>
-      <c r="AT1" s="36" t="s">
+      <c r="AU1" s="36" t="s">
         <v>30</v>
       </c>
-      <c r="AU1" s="36" t="s">
+      <c r="AV1" s="36" t="s">
         <v>27</v>
       </c>
-      <c r="AV1" s="36" t="s">
+      <c r="AW1" s="36" t="s">
         <v>382</v>
       </c>
     </row>
-    <row r="2" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:49" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>53</v>
       </c>
@@ -7660,7 +7685,7 @@
         <v>171</v>
       </c>
       <c r="AN2" s="41" t="s">
-        <v>487</v>
+        <v>53</v>
       </c>
       <c r="AO2" s="41" t="s">
         <v>487</v>
@@ -7671,8 +7696,8 @@
       <c r="AQ2" s="41" t="s">
         <v>487</v>
       </c>
-      <c r="AR2" s="9" t="s">
-        <v>24</v>
+      <c r="AR2" s="41" t="s">
+        <v>487</v>
       </c>
       <c r="AS2" s="9" t="s">
         <v>24</v>
@@ -7684,10 +7709,13 @@
         <v>24</v>
       </c>
       <c r="AV2" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="AW2" s="9" t="s">
         <v>383</v>
       </c>
     </row>
-    <row r="3" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:49" x14ac:dyDescent="0.15">
       <c r="A3" s="8" t="s">
         <v>58</v>
       </c>
@@ -7806,34 +7834,37 @@
         <v>172</v>
       </c>
       <c r="AN3" s="42" t="s">
+        <v>499</v>
+      </c>
+      <c r="AO3" s="42" t="s">
         <v>491</v>
       </c>
-      <c r="AO3" s="42" t="s">
+      <c r="AP3" s="42" t="s">
         <v>493</v>
       </c>
-      <c r="AP3" s="42" t="s">
+      <c r="AQ3" s="42" t="s">
         <v>488</v>
       </c>
-      <c r="AQ3" s="42" t="s">
+      <c r="AR3" s="42" t="s">
         <v>495</v>
       </c>
-      <c r="AR3" s="8" t="s">
+      <c r="AS3" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="AS3" s="8" t="s">
+      <c r="AT3" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="AT3" s="8" t="s">
+      <c r="AU3" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="AU3" s="8" t="s">
+      <c r="AV3" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="AV3" s="8" t="s">
+      <c r="AW3" s="8" t="s">
         <v>384</v>
       </c>
     </row>
-    <row r="4" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:49" x14ac:dyDescent="0.15">
       <c r="A4" s="10">
         <v>42110001</v>
       </c>
@@ -7872,18 +7903,18 @@
       <c r="V4" s="12"/>
       <c r="W4" s="12"/>
       <c r="X4" s="12"/>
-      <c r="AR4">
+      <c r="AS4">
         <v>-30</v>
-      </c>
-      <c r="AT4">
-        <v>100</v>
       </c>
       <c r="AU4">
         <v>100</v>
       </c>
-      <c r="AV4" s="29"/>
-    </row>
-    <row r="5" spans="1:48" x14ac:dyDescent="0.15">
+      <c r="AV4">
+        <v>100</v>
+      </c>
+      <c r="AW4" s="29"/>
+    </row>
+    <row r="5" spans="1:49" x14ac:dyDescent="0.15">
       <c r="A5" s="10">
         <v>42110002</v>
       </c>
@@ -7922,15 +7953,15 @@
       <c r="V5" s="12"/>
       <c r="W5" s="12"/>
       <c r="X5" s="12"/>
-      <c r="AR5">
+      <c r="AS5">
         <v>-20</v>
       </c>
-      <c r="AS5">
+      <c r="AT5">
         <v>100</v>
       </c>
-      <c r="AV5" s="29"/>
-    </row>
-    <row r="6" spans="1:48" x14ac:dyDescent="0.15">
+      <c r="AW5" s="29"/>
+    </row>
+    <row r="6" spans="1:49" x14ac:dyDescent="0.15">
       <c r="A6" s="10">
         <v>42110003</v>
       </c>
@@ -7969,9 +8000,9 @@
       <c r="V6" s="12"/>
       <c r="W6" s="12"/>
       <c r="X6" s="12"/>
-      <c r="AV6" s="29"/>
-    </row>
-    <row r="7" spans="1:48" x14ac:dyDescent="0.15">
+      <c r="AW6" s="29"/>
+    </row>
+    <row r="7" spans="1:49" x14ac:dyDescent="0.15">
       <c r="A7" s="10">
         <v>42110004</v>
       </c>
@@ -8003,9 +8034,9 @@
       <c r="N7" s="5"/>
       <c r="O7" s="5"/>
       <c r="P7" s="5"/>
-      <c r="AV7" s="29"/>
-    </row>
-    <row r="8" spans="1:48" x14ac:dyDescent="0.15">
+      <c r="AW7" s="29"/>
+    </row>
+    <row r="8" spans="1:49" x14ac:dyDescent="0.15">
       <c r="A8" s="10">
         <v>42110005</v>
       </c>
@@ -8044,9 +8075,9 @@
       <c r="V8" s="12"/>
       <c r="W8" s="12"/>
       <c r="X8" s="12"/>
-      <c r="AV8" s="29"/>
-    </row>
-    <row r="9" spans="1:48" x14ac:dyDescent="0.15">
+      <c r="AW8" s="29"/>
+    </row>
+    <row r="9" spans="1:49" x14ac:dyDescent="0.15">
       <c r="A9">
         <v>42120001</v>
       </c>
@@ -8085,9 +8116,9 @@
       <c r="V9" s="11"/>
       <c r="W9" s="11"/>
       <c r="X9" s="11"/>
-      <c r="AV9" s="29"/>
-    </row>
-    <row r="10" spans="1:48" x14ac:dyDescent="0.15">
+      <c r="AW9" s="29"/>
+    </row>
+    <row r="10" spans="1:49" x14ac:dyDescent="0.15">
       <c r="A10">
         <v>42120002</v>
       </c>
@@ -8131,9 +8162,9 @@
       <c r="AH10" t="s">
         <v>333</v>
       </c>
-      <c r="AV10" s="29"/>
-    </row>
-    <row r="11" spans="1:48" x14ac:dyDescent="0.15">
+      <c r="AW10" s="29"/>
+    </row>
+    <row r="11" spans="1:49" x14ac:dyDescent="0.15">
       <c r="A11">
         <v>42120003</v>
       </c>
@@ -8171,9 +8202,9 @@
       <c r="V11" s="11"/>
       <c r="W11" s="11"/>
       <c r="X11" s="11"/>
-      <c r="AV11" s="29"/>
-    </row>
-    <row r="12" spans="1:48" x14ac:dyDescent="0.15">
+      <c r="AW11" s="29"/>
+    </row>
+    <row r="12" spans="1:49" x14ac:dyDescent="0.15">
       <c r="A12">
         <v>42120004</v>
       </c>
@@ -8219,9 +8250,9 @@
       <c r="AH12" t="s">
         <v>334</v>
       </c>
-      <c r="AV12" s="29"/>
-    </row>
-    <row r="13" spans="1:48" x14ac:dyDescent="0.15">
+      <c r="AW12" s="29"/>
+    </row>
+    <row r="13" spans="1:49" x14ac:dyDescent="0.15">
       <c r="A13">
         <v>42120005</v>
       </c>
@@ -8261,9 +8292,9 @@
       </c>
       <c r="W13" s="11"/>
       <c r="X13" s="11"/>
-      <c r="AV13" s="29"/>
-    </row>
-    <row r="14" spans="1:48" x14ac:dyDescent="0.15">
+      <c r="AW13" s="29"/>
+    </row>
+    <row r="14" spans="1:49" x14ac:dyDescent="0.15">
       <c r="A14">
         <v>42120006</v>
       </c>
@@ -8305,9 +8336,9 @@
       <c r="V14" s="11"/>
       <c r="W14" s="11"/>
       <c r="X14" s="11"/>
-      <c r="AV14" s="29"/>
-    </row>
-    <row r="15" spans="1:48" x14ac:dyDescent="0.15">
+      <c r="AW14" s="29"/>
+    </row>
+    <row r="15" spans="1:49" x14ac:dyDescent="0.15">
       <c r="A15">
         <v>42120007</v>
       </c>
@@ -8346,9 +8377,9 @@
       <c r="V15" s="11"/>
       <c r="W15" s="11"/>
       <c r="X15" s="11"/>
-      <c r="AV15" s="29"/>
-    </row>
-    <row r="16" spans="1:48" x14ac:dyDescent="0.15">
+      <c r="AW15" s="29"/>
+    </row>
+    <row r="16" spans="1:49" x14ac:dyDescent="0.15">
       <c r="A16">
         <v>42120008</v>
       </c>
@@ -8387,9 +8418,9 @@
       <c r="V16" s="11"/>
       <c r="W16" s="11"/>
       <c r="X16" s="11"/>
-      <c r="AV16" s="29"/>
-    </row>
-    <row r="17" spans="1:48" x14ac:dyDescent="0.15">
+      <c r="AW16" s="29"/>
+    </row>
+    <row r="17" spans="1:49" x14ac:dyDescent="0.15">
       <c r="A17">
         <v>42120009</v>
       </c>
@@ -8428,9 +8459,9 @@
       <c r="V17" s="11"/>
       <c r="W17" s="11"/>
       <c r="X17" s="11"/>
-      <c r="AV17" s="29"/>
-    </row>
-    <row r="18" spans="1:48" x14ac:dyDescent="0.15">
+      <c r="AW17" s="29"/>
+    </row>
+    <row r="18" spans="1:49" x14ac:dyDescent="0.15">
       <c r="A18">
         <v>42120010</v>
       </c>
@@ -8469,9 +8500,9 @@
       <c r="V18" s="11"/>
       <c r="W18" s="11"/>
       <c r="X18" s="11"/>
-      <c r="AV18" s="29"/>
-    </row>
-    <row r="19" spans="1:48" x14ac:dyDescent="0.15">
+      <c r="AW18" s="29"/>
+    </row>
+    <row r="19" spans="1:49" x14ac:dyDescent="0.15">
       <c r="A19">
         <v>42120011</v>
       </c>
@@ -8510,9 +8541,9 @@
       <c r="V19" s="11"/>
       <c r="W19" s="11"/>
       <c r="X19" s="11"/>
-      <c r="AV19" s="29"/>
-    </row>
-    <row r="20" spans="1:48" x14ac:dyDescent="0.15">
+      <c r="AW19" s="29"/>
+    </row>
+    <row r="20" spans="1:49" x14ac:dyDescent="0.15">
       <c r="A20">
         <v>42120013</v>
       </c>
@@ -8551,9 +8582,9 @@
       <c r="V20" s="11"/>
       <c r="W20" s="11"/>
       <c r="X20" s="11"/>
-      <c r="AV20" s="29"/>
-    </row>
-    <row r="21" spans="1:48" x14ac:dyDescent="0.15">
+      <c r="AW20" s="29"/>
+    </row>
+    <row r="21" spans="1:49" x14ac:dyDescent="0.15">
       <c r="A21">
         <v>42120014</v>
       </c>
@@ -8592,9 +8623,9 @@
       <c r="V21" s="11"/>
       <c r="W21" s="11"/>
       <c r="X21" s="11"/>
-      <c r="AV21" s="29"/>
-    </row>
-    <row r="22" spans="1:48" x14ac:dyDescent="0.15">
+      <c r="AW21" s="29"/>
+    </row>
+    <row r="22" spans="1:49" x14ac:dyDescent="0.15">
       <c r="A22">
         <v>42120015</v>
       </c>
@@ -8633,9 +8664,9 @@
       <c r="V22" s="11"/>
       <c r="W22" s="11"/>
       <c r="X22" s="11"/>
-      <c r="AV22" s="29"/>
-    </row>
-    <row r="23" spans="1:48" x14ac:dyDescent="0.15">
+      <c r="AW22" s="29"/>
+    </row>
+    <row r="23" spans="1:49" x14ac:dyDescent="0.15">
       <c r="A23">
         <v>42120016</v>
       </c>
@@ -8671,9 +8702,9 @@
       <c r="V23" s="11"/>
       <c r="W23" s="11"/>
       <c r="X23" s="11"/>
-      <c r="AV23" s="29"/>
-    </row>
-    <row r="24" spans="1:48" x14ac:dyDescent="0.15">
+      <c r="AW23" s="29"/>
+    </row>
+    <row r="24" spans="1:49" x14ac:dyDescent="0.15">
       <c r="A24">
         <v>42120017</v>
       </c>
@@ -8717,9 +8748,9 @@
       <c r="AC24">
         <v>30</v>
       </c>
-      <c r="AV24" s="29"/>
-    </row>
-    <row r="25" spans="1:48" x14ac:dyDescent="0.15">
+      <c r="AW24" s="29"/>
+    </row>
+    <row r="25" spans="1:49" x14ac:dyDescent="0.15">
       <c r="A25">
         <v>42120018</v>
       </c>
@@ -8763,9 +8794,9 @@
       <c r="AC25">
         <v>50</v>
       </c>
-      <c r="AV25" s="29"/>
-    </row>
-    <row r="26" spans="1:48" x14ac:dyDescent="0.15">
+      <c r="AW25" s="29"/>
+    </row>
+    <row r="26" spans="1:49" x14ac:dyDescent="0.15">
       <c r="A26">
         <v>42120019</v>
       </c>
@@ -8808,9 +8839,9 @@
       <c r="V26" s="19"/>
       <c r="W26" s="19"/>
       <c r="X26" s="19"/>
-      <c r="AV26" s="29"/>
-    </row>
-    <row r="27" spans="1:48" x14ac:dyDescent="0.15">
+      <c r="AW26" s="29"/>
+    </row>
+    <row r="27" spans="1:49" x14ac:dyDescent="0.15">
       <c r="A27">
         <v>42130001</v>
       </c>
@@ -8851,9 +8882,9 @@
       <c r="V27" s="11"/>
       <c r="W27" s="11"/>
       <c r="X27" s="11"/>
-      <c r="AV27" s="29"/>
-    </row>
-    <row r="28" spans="1:48" x14ac:dyDescent="0.15">
+      <c r="AW27" s="29"/>
+    </row>
+    <row r="28" spans="1:49" x14ac:dyDescent="0.15">
       <c r="A28">
         <v>42130002</v>
       </c>
@@ -8896,9 +8927,9 @@
       <c r="V28" s="11"/>
       <c r="W28" s="11"/>
       <c r="X28" s="11"/>
-      <c r="AV28" s="29"/>
-    </row>
-    <row r="29" spans="1:48" x14ac:dyDescent="0.15">
+      <c r="AW28" s="29"/>
+    </row>
+    <row r="29" spans="1:49" x14ac:dyDescent="0.15">
       <c r="A29">
         <v>42130003</v>
       </c>
@@ -8953,9 +8984,9 @@
       <c r="AL29">
         <v>200</v>
       </c>
-      <c r="AV29" s="29"/>
-    </row>
-    <row r="30" spans="1:48" x14ac:dyDescent="0.15">
+      <c r="AW29" s="29"/>
+    </row>
+    <row r="30" spans="1:49" x14ac:dyDescent="0.15">
       <c r="A30">
         <v>42130004</v>
       </c>
@@ -8996,9 +9027,9 @@
       <c r="V30" s="11"/>
       <c r="W30" s="11"/>
       <c r="X30" s="11"/>
-      <c r="AV30" s="29"/>
-    </row>
-    <row r="31" spans="1:48" x14ac:dyDescent="0.15">
+      <c r="AW30" s="29"/>
+    </row>
+    <row r="31" spans="1:49" x14ac:dyDescent="0.15">
       <c r="A31">
         <v>42130005</v>
       </c>
@@ -9039,9 +9070,9 @@
       <c r="V31" s="11"/>
       <c r="W31" s="11"/>
       <c r="X31" s="11"/>
-      <c r="AV31" s="29"/>
-    </row>
-    <row r="32" spans="1:48" x14ac:dyDescent="0.15">
+      <c r="AW31" s="29"/>
+    </row>
+    <row r="32" spans="1:49" x14ac:dyDescent="0.15">
       <c r="A32">
         <v>42130006</v>
       </c>
@@ -9082,9 +9113,9 @@
       <c r="V32" s="11"/>
       <c r="W32" s="11"/>
       <c r="X32" s="11"/>
-      <c r="AV32" s="29"/>
-    </row>
-    <row r="33" spans="1:48" x14ac:dyDescent="0.15">
+      <c r="AW32" s="29"/>
+    </row>
+    <row r="33" spans="1:49" x14ac:dyDescent="0.15">
       <c r="A33">
         <v>42130007</v>
       </c>
@@ -9138,11 +9169,11 @@
       <c r="AL33">
         <v>200</v>
       </c>
-      <c r="AV33" s="29"/>
+      <c r="AW33" s="29"/>
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
-  <conditionalFormatting sqref="D4:AV33">
+  <conditionalFormatting sqref="D4:AW33">
     <cfRule type="containsBlanks" dxfId="0" priority="3">
       <formula>LEN(TRIM(D4))=0</formula>
     </cfRule>

</xml_diff>

<commit_message>
fix bug of choose mode
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/SceneQuest.xlsx
+++ b/ConfigData/Xlsx/SceneQuest.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385" activeTab="1"/>
+    <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="4" r:id="rId1"/>
@@ -2887,20 +2887,6 @@
   </cellStyles>
   <dxfs count="28">
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -3098,6 +3084,13 @@
       </fill>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
     <dxf>
@@ -3129,6 +3122,13 @@
         </patternFill>
       </fill>
     </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -3151,7 +3151,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="表3" displayName="表3" ref="A3:AW79" totalsRowShown="0" headerRowDxfId="27">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="表3" displayName="表3" ref="A3:AW79" totalsRowShown="0" headerRowDxfId="26">
   <autoFilter ref="A3:AW79"/>
   <sortState ref="A4:AW74">
     <sortCondition ref="A3:A74"/>
@@ -3165,14 +3165,14 @@
     <tableColumn id="24" name="Ename"/>
     <tableColumn id="4" name="Figue"/>
     <tableColumn id="5" name="Script"/>
-    <tableColumn id="6" name="TriggerMulti" dataDxfId="26"/>
-    <tableColumn id="40" name="Catalog" dataDxfId="25"/>
-    <tableColumn id="35" name="TriggerHourBegin" dataDxfId="24"/>
-    <tableColumn id="34" name="TriggerHourEnd" dataDxfId="23"/>
-    <tableColumn id="36" name="TriggerQuestNotReceive" dataDxfId="22"/>
-    <tableColumn id="37" name="TriggerQuestReceived" dataDxfId="21"/>
-    <tableColumn id="38" name="TriggerQuestFinished" dataDxfId="20"/>
-    <tableColumn id="39" name="TriggerRate" dataDxfId="19"/>
+    <tableColumn id="6" name="TriggerMulti" dataDxfId="25"/>
+    <tableColumn id="40" name="Catalog" dataDxfId="24"/>
+    <tableColumn id="35" name="TriggerHourBegin" dataDxfId="23"/>
+    <tableColumn id="34" name="TriggerHourEnd" dataDxfId="22"/>
+    <tableColumn id="36" name="TriggerQuestNotReceive" dataDxfId="21"/>
+    <tableColumn id="37" name="TriggerQuestReceived" dataDxfId="20"/>
+    <tableColumn id="38" name="TriggerQuestFinished" dataDxfId="19"/>
+    <tableColumn id="39" name="TriggerRate" dataDxfId="18"/>
     <tableColumn id="7" name="EnemyName"/>
     <tableColumn id="32" name="SceneId"/>
     <tableColumn id="29" name="Position"/>
@@ -3212,7 +3212,7 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="表3_5" displayName="表3_5" ref="A3:AW33" totalsRowShown="0" headerRowDxfId="18">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="表3_5" displayName="表3_5" ref="A3:AW33" totalsRowShown="0" headerRowDxfId="16">
   <autoFilter ref="A3:AW33"/>
   <sortState ref="A4:AE6">
     <sortCondition ref="A3:A6"/>
@@ -3220,28 +3220,28 @@
   <tableColumns count="49">
     <tableColumn id="1" name="Id"/>
     <tableColumn id="2" name="Name"/>
-    <tableColumn id="27" name="Type" dataDxfId="17"/>
+    <tableColumn id="27" name="Type" dataDxfId="15"/>
     <tableColumn id="3" name="Level"/>
     <tableColumn id="25" name="Danger"/>
     <tableColumn id="24" name="Ename"/>
     <tableColumn id="4" name="Figue"/>
     <tableColumn id="5" name="Script"/>
     <tableColumn id="6" name="TriggerMulti"/>
-    <tableColumn id="40" name="Catalog" dataDxfId="16"/>
-    <tableColumn id="35" name="TriggerHourBegin" dataDxfId="15"/>
-    <tableColumn id="34" name="TriggerHourEnd" dataDxfId="14"/>
-    <tableColumn id="37" name="TriggerQuestNotReceive" dataDxfId="13"/>
-    <tableColumn id="38" name="TriggerQuestReceived" dataDxfId="12"/>
-    <tableColumn id="36" name="TriggerQuestFinished" dataDxfId="11"/>
-    <tableColumn id="39" name="TriggerRate" dataDxfId="10"/>
+    <tableColumn id="40" name="Catalog" dataDxfId="14"/>
+    <tableColumn id="35" name="TriggerHourBegin" dataDxfId="13"/>
+    <tableColumn id="34" name="TriggerHourEnd" dataDxfId="12"/>
+    <tableColumn id="37" name="TriggerQuestNotReceive" dataDxfId="11"/>
+    <tableColumn id="38" name="TriggerQuestReceived" dataDxfId="10"/>
+    <tableColumn id="36" name="TriggerQuestFinished" dataDxfId="9"/>
+    <tableColumn id="39" name="TriggerRate" dataDxfId="8"/>
     <tableColumn id="7" name="EnemyName"/>
-    <tableColumn id="32" name="SceneId" dataDxfId="9"/>
-    <tableColumn id="29" name="Position" dataDxfId="8"/>
-    <tableColumn id="28" name="NextQuest" dataDxfId="7"/>
-    <tableColumn id="44" name="HiddenRoomQuest" dataDxfId="6"/>
-    <tableColumn id="8" name="ShopName" dataDxfId="5"/>
-    <tableColumn id="41" name="MiniGameId" dataDxfId="4"/>
-    <tableColumn id="43" name="PayKey" dataDxfId="3"/>
+    <tableColumn id="32" name="SceneId" dataDxfId="7"/>
+    <tableColumn id="29" name="Position" dataDxfId="6"/>
+    <tableColumn id="28" name="NextQuest" dataDxfId="5"/>
+    <tableColumn id="44" name="HiddenRoomQuest" dataDxfId="4"/>
+    <tableColumn id="8" name="ShopName" dataDxfId="3"/>
+    <tableColumn id="41" name="MiniGameId" dataDxfId="2"/>
+    <tableColumn id="43" name="PayKey" dataDxfId="1"/>
     <tableColumn id="9" name="RewardGold"/>
     <tableColumn id="10" name="RewardFood"/>
     <tableColumn id="11" name="RewardHealth"/>
@@ -3266,7 +3266,7 @@
     <tableColumn id="21" name="TradeFood"/>
     <tableColumn id="22" name="TradeHealth"/>
     <tableColumn id="23" name="TradeMental"/>
-    <tableColumn id="33" name="TradeDropItem" dataDxfId="2"/>
+    <tableColumn id="33" name="TradeDropItem" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3595,9 +3595,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AW79"/>
   <sheetViews>
-    <sheetView topLeftCell="J1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AN1" sqref="AN1:AN3"/>
+      <selection pane="bottomLeft" activeCell="AR1" sqref="AR1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -4139,6 +4139,21 @@
       <c r="AL4">
         <v>100</v>
       </c>
+      <c r="AN4">
+        <v>35</v>
+      </c>
+      <c r="AO4">
+        <v>50</v>
+      </c>
+      <c r="AP4">
+        <v>25</v>
+      </c>
+      <c r="AQ4">
+        <v>50</v>
+      </c>
+      <c r="AR4">
+        <v>35</v>
+      </c>
     </row>
     <row r="5" spans="1:49" x14ac:dyDescent="0.15">
       <c r="A5" s="10">
@@ -7377,7 +7392,7 @@
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <conditionalFormatting sqref="B4:AW79">
-    <cfRule type="containsBlanks" dxfId="1" priority="10">
+    <cfRule type="containsBlanks" dxfId="27" priority="10">
       <formula>LEN(TRIM(B4))=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7394,7 +7409,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AW33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+    <sheetView topLeftCell="H1" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="AN1" sqref="AN1:AN3"/>
     </sheetView>
@@ -9174,7 +9189,7 @@
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <conditionalFormatting sqref="D4:AW33">
-    <cfRule type="containsBlanks" dxfId="0" priority="3">
+    <cfRule type="containsBlanks" dxfId="17" priority="3">
       <formula>LEN(TRIM(D4))=0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
support attr bonus on scenequest
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/SceneQuest.xlsx
+++ b/ConfigData/Xlsx/SceneQuest.xlsx
@@ -1,31 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18528"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18326"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\code\TOMClassicGit\ConfigData\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Code\TOMClassicGit\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="4" r:id="rId1"/>
     <sheet name="MapSet" sheetId="5" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>real</author>
   </authors>
   <commentList>
-    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
+    <comment ref="E1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1017" uniqueCount="566">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1047" uniqueCount="578">
   <si>
     <t>int</t>
     <phoneticPr fontId="18" type="noConversion"/>
@@ -2256,11 +2256,59 @@
     <t>innerforest2</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
+  <si>
+    <t>属性力量</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>属性敏捷</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>属性智慧</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>属性感知</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>属性耐力</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>RewardExp</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>RewardStr</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>RewardAgi</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>RewardIntl</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>RewardPerc</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>RewardEndu</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>奖励道具1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="29" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -3077,7 +3125,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="77">
+  <cellXfs count="78">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -3307,6 +3355,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -3354,13 +3405,101 @@
     <cellStyle name="着色 6" xfId="38" builtinId="49" customBuiltin="1"/>
     <cellStyle name="注释" xfId="15" builtinId="10" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="43">
+  <dxfs count="52">
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </font>
     </dxf>
     <dxf>
       <fill>
@@ -3467,6 +3606,63 @@
         <charset val="134"/>
         <scheme val="minor"/>
       </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </font>
       <border diagonalUp="0" diagonalDown="0">
         <left/>
         <right style="thin">
@@ -3479,6 +3675,25 @@
         <vertical/>
         <horizontal/>
       </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </font>
     </dxf>
     <dxf>
       <font>
@@ -3762,6 +3977,25 @@
       </font>
     </dxf>
     <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
     <dxf>
@@ -3799,6 +4033,72 @@
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
     <mruColors>
       <color rgb="FFE969CE"/>
       <color rgb="FF0066FF"/>
@@ -3818,132 +4118,142 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="表3" displayName="表3" ref="A3:BB86" totalsRowShown="0" headerRowDxfId="42">
-  <autoFilter ref="A3:BB86" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
-  <sortState ref="A4:BB86">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="表3" displayName="表3" ref="A3:BG86" totalsRowShown="0" headerRowDxfId="51">
+  <autoFilter ref="A3:BG86"/>
+  <sortState ref="A4:BG86">
     <sortCondition ref="A3:A86"/>
   </sortState>
-  <tableColumns count="54">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Id"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Name"/>
-    <tableColumn id="28" xr3:uid="{00000000-0010-0000-0000-00001C000000}" name="Type"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Level"/>
-    <tableColumn id="25" xr3:uid="{00000000-0010-0000-0000-000019000000}" name="Danger"/>
-    <tableColumn id="24" xr3:uid="{00000000-0010-0000-0000-000018000000}" name="Ename"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Figue"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Script"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="TriggerMulti" dataDxfId="41"/>
-    <tableColumn id="40" xr3:uid="{00000000-0010-0000-0000-000028000000}" name="Catalog" dataDxfId="40"/>
-    <tableColumn id="35" xr3:uid="{00000000-0010-0000-0000-000023000000}" name="TriggerHourBegin" dataDxfId="39"/>
-    <tableColumn id="34" xr3:uid="{00000000-0010-0000-0000-000022000000}" name="TriggerHourEnd" dataDxfId="38"/>
-    <tableColumn id="36" xr3:uid="{00000000-0010-0000-0000-000024000000}" name="TriggerQuestNotReceive" dataDxfId="37"/>
-    <tableColumn id="37" xr3:uid="{00000000-0010-0000-0000-000025000000}" name="TriggerQuestReceived" dataDxfId="36"/>
-    <tableColumn id="38" xr3:uid="{00000000-0010-0000-0000-000026000000}" name="TriggerQuestFinished" dataDxfId="35"/>
-    <tableColumn id="39" xr3:uid="{00000000-0010-0000-0000-000027000000}" name="TriggerRate" dataDxfId="34"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="EnemyName"/>
-    <tableColumn id="51" xr3:uid="{00000000-0010-0000-0000-000033000000}" name="CanBribe" dataDxfId="33"/>
-    <tableColumn id="32" xr3:uid="{00000000-0010-0000-0000-000020000000}" name="SceneId"/>
-    <tableColumn id="29" xr3:uid="{00000000-0010-0000-0000-00001D000000}" name="Position"/>
-    <tableColumn id="54" xr3:uid="{6CAE7C16-0ADF-4925-90DB-49FC49332195}" name="DungeonId" dataDxfId="8"/>
-    <tableColumn id="50" xr3:uid="{00000000-0010-0000-0000-000032000000}" name="CheckQuest"/>
-    <tableColumn id="27" xr3:uid="{00000000-0010-0000-0000-00001B000000}" name="NextQuest"/>
-    <tableColumn id="44" xr3:uid="{00000000-0010-0000-0000-00002C000000}" name="HiddenRoomQuest"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="ShopName"/>
-    <tableColumn id="41" xr3:uid="{00000000-0010-0000-0000-000029000000}" name="MiniGameId"/>
-    <tableColumn id="43" xr3:uid="{00000000-0010-0000-0000-00002B000000}" name="PayKey"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="RewardGold"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="RewardFood"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="RewardHealth"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="RewardMental"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="RewardExp"/>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="RewardItem"/>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="RewardDrop"/>
-    <tableColumn id="30" xr3:uid="{00000000-0010-0000-0000-00001E000000}" name="RewardBlessLevel"/>
-    <tableColumn id="42" xr3:uid="{00000000-0010-0000-0000-00002A000000}" name="RewardBlessId"/>
-    <tableColumn id="52" xr3:uid="{00000000-0010-0000-0000-000034000000}" name="RewardResId" dataDxfId="32"/>
-    <tableColumn id="53" xr3:uid="{00000000-0010-0000-0000-000035000000}" name="RewardResAmount" dataDxfId="31"/>
-    <tableColumn id="26" xr3:uid="{00000000-0010-0000-0000-00001A000000}" name="UnlockRival"/>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="PunishGold"/>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="PunishFood"/>
-    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="PunishHealth"/>
-    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0000-000013000000}" name="PunishMental"/>
-    <tableColumn id="31" xr3:uid="{00000000-0010-0000-0000-00001F000000}" name="PunishBlessLevel"/>
-    <tableColumn id="49" xr3:uid="{00000000-0010-0000-0000-000031000000}" name="ChooseWinRate"/>
-    <tableColumn id="46" xr3:uid="{00000000-0010-0000-0000-00002E000000}" name="ChooseGold2"/>
-    <tableColumn id="47" xr3:uid="{00000000-0010-0000-0000-00002F000000}" name="ChooseGoldAddon"/>
-    <tableColumn id="45" xr3:uid="{00000000-0010-0000-0000-00002D000000}" name="ChooseFood"/>
-    <tableColumn id="48" xr3:uid="{00000000-0010-0000-0000-000030000000}" name="ChooseFoodAddon"/>
-    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0000-000014000000}" name="TradeGold"/>
-    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0000-000015000000}" name="TradeFood"/>
-    <tableColumn id="22" xr3:uid="{00000000-0010-0000-0000-000016000000}" name="TradeHealth"/>
-    <tableColumn id="23" xr3:uid="{00000000-0010-0000-0000-000017000000}" name="TradeMental"/>
-    <tableColumn id="33" xr3:uid="{00000000-0010-0000-0000-000021000000}" name="TradeDropItem"/>
+  <tableColumns count="59">
+    <tableColumn id="1" name="Id"/>
+    <tableColumn id="2" name="Name"/>
+    <tableColumn id="28" name="Type"/>
+    <tableColumn id="3" name="Level"/>
+    <tableColumn id="25" name="Danger"/>
+    <tableColumn id="24" name="Ename"/>
+    <tableColumn id="4" name="Figue"/>
+    <tableColumn id="5" name="Script"/>
+    <tableColumn id="6" name="TriggerMulti" dataDxfId="50"/>
+    <tableColumn id="40" name="Catalog" dataDxfId="49"/>
+    <tableColumn id="35" name="TriggerHourBegin" dataDxfId="48"/>
+    <tableColumn id="34" name="TriggerHourEnd" dataDxfId="47"/>
+    <tableColumn id="36" name="TriggerQuestNotReceive" dataDxfId="46"/>
+    <tableColumn id="37" name="TriggerQuestReceived" dataDxfId="45"/>
+    <tableColumn id="38" name="TriggerQuestFinished" dataDxfId="44"/>
+    <tableColumn id="39" name="TriggerRate" dataDxfId="43"/>
+    <tableColumn id="7" name="EnemyName"/>
+    <tableColumn id="51" name="CanBribe" dataDxfId="42"/>
+    <tableColumn id="32" name="SceneId"/>
+    <tableColumn id="29" name="Position"/>
+    <tableColumn id="54" name="DungeonId" dataDxfId="41"/>
+    <tableColumn id="50" name="CheckQuest"/>
+    <tableColumn id="27" name="NextQuest"/>
+    <tableColumn id="44" name="HiddenRoomQuest"/>
+    <tableColumn id="8" name="ShopName"/>
+    <tableColumn id="41" name="MiniGameId"/>
+    <tableColumn id="43" name="PayKey"/>
+    <tableColumn id="9" name="RewardGold"/>
+    <tableColumn id="10" name="RewardFood"/>
+    <tableColumn id="11" name="RewardHealth"/>
+    <tableColumn id="12" name="RewardMental"/>
+    <tableColumn id="13" name="RewardExp"/>
+    <tableColumn id="56" name="RewardStr" dataDxfId="16"/>
+    <tableColumn id="57" name="RewardAgi" dataDxfId="15"/>
+    <tableColumn id="58" name="RewardIntl" dataDxfId="14"/>
+    <tableColumn id="59" name="RewardPerc" dataDxfId="13"/>
+    <tableColumn id="60" name="RewardEndu" dataDxfId="12"/>
+    <tableColumn id="14" name="RewardItem"/>
+    <tableColumn id="15" name="RewardDrop"/>
+    <tableColumn id="30" name="RewardBlessLevel"/>
+    <tableColumn id="42" name="RewardBlessId"/>
+    <tableColumn id="52" name="RewardResId" dataDxfId="40"/>
+    <tableColumn id="53" name="RewardResAmount" dataDxfId="39"/>
+    <tableColumn id="26" name="UnlockRival"/>
+    <tableColumn id="16" name="PunishGold"/>
+    <tableColumn id="17" name="PunishFood"/>
+    <tableColumn id="18" name="PunishHealth"/>
+    <tableColumn id="19" name="PunishMental"/>
+    <tableColumn id="31" name="PunishBlessLevel"/>
+    <tableColumn id="49" name="ChooseWinRate"/>
+    <tableColumn id="46" name="ChooseGold2"/>
+    <tableColumn id="47" name="ChooseGoldAddon"/>
+    <tableColumn id="45" name="ChooseFood"/>
+    <tableColumn id="48" name="ChooseFoodAddon"/>
+    <tableColumn id="20" name="TradeGold"/>
+    <tableColumn id="21" name="TradeFood"/>
+    <tableColumn id="22" name="TradeHealth"/>
+    <tableColumn id="23" name="TradeMental"/>
+    <tableColumn id="33" name="TradeDropItem"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="表3_5" displayName="表3_5" ref="A3:BB38" totalsRowShown="0" headerRowDxfId="30">
-  <autoFilter ref="A3:BB38" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
-  <sortState ref="A4:AH6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="表3_5" displayName="表3_5" ref="A3:BG38" totalsRowShown="0" headerRowDxfId="38">
+  <autoFilter ref="A3:BG38"/>
+  <sortState ref="A4:AM6">
     <sortCondition ref="A3:A6"/>
   </sortState>
-  <tableColumns count="54">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Id"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Name"/>
-    <tableColumn id="27" xr3:uid="{00000000-0010-0000-0100-00001B000000}" name="Type" dataDxfId="29"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Level"/>
-    <tableColumn id="25" xr3:uid="{00000000-0010-0000-0100-000019000000}" name="Danger"/>
-    <tableColumn id="24" xr3:uid="{00000000-0010-0000-0100-000018000000}" name="Ename"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Figue"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="Script"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="TriggerMulti"/>
-    <tableColumn id="40" xr3:uid="{00000000-0010-0000-0100-000028000000}" name="Catalog" dataDxfId="28"/>
-    <tableColumn id="35" xr3:uid="{00000000-0010-0000-0100-000023000000}" name="TriggerHourBegin" dataDxfId="27"/>
-    <tableColumn id="34" xr3:uid="{00000000-0010-0000-0100-000022000000}" name="TriggerHourEnd" dataDxfId="26"/>
-    <tableColumn id="37" xr3:uid="{00000000-0010-0000-0100-000025000000}" name="TriggerQuestNotReceive" dataDxfId="25"/>
-    <tableColumn id="38" xr3:uid="{00000000-0010-0000-0100-000026000000}" name="TriggerQuestReceived" dataDxfId="24"/>
-    <tableColumn id="36" xr3:uid="{00000000-0010-0000-0100-000024000000}" name="TriggerQuestFinished" dataDxfId="23"/>
-    <tableColumn id="39" xr3:uid="{00000000-0010-0000-0100-000027000000}" name="TriggerRate" dataDxfId="22"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="EnemyName"/>
-    <tableColumn id="51" xr3:uid="{00000000-0010-0000-0100-000033000000}" name="CanBribe" dataDxfId="21"/>
-    <tableColumn id="32" xr3:uid="{00000000-0010-0000-0100-000020000000}" name="SceneId" dataDxfId="20"/>
-    <tableColumn id="29" xr3:uid="{00000000-0010-0000-0100-00001D000000}" name="Position" dataDxfId="19"/>
-    <tableColumn id="54" xr3:uid="{08FF1697-7ACD-430A-A485-A25F780A9ACD}" name="DungeonId" dataDxfId="9"/>
-    <tableColumn id="50" xr3:uid="{00000000-0010-0000-0100-000032000000}" name="CheckQuest" dataDxfId="18"/>
-    <tableColumn id="28" xr3:uid="{00000000-0010-0000-0100-00001C000000}" name="NextQuest" dataDxfId="17"/>
-    <tableColumn id="44" xr3:uid="{00000000-0010-0000-0100-00002C000000}" name="HiddenRoomQuest" dataDxfId="16"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="ShopName" dataDxfId="15"/>
-    <tableColumn id="41" xr3:uid="{00000000-0010-0000-0100-000029000000}" name="MiniGameId" dataDxfId="14"/>
-    <tableColumn id="43" xr3:uid="{00000000-0010-0000-0100-00002B000000}" name="PayKey" dataDxfId="13"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0100-000009000000}" name="RewardGold"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0100-00000A000000}" name="RewardFood"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0100-00000B000000}" name="RewardHealth"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0100-00000C000000}" name="RewardMental"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0100-00000D000000}" name="RewardExp"/>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0100-00000E000000}" name="RewardItem"/>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0100-00000F000000}" name="RewardDrop"/>
-    <tableColumn id="31" xr3:uid="{00000000-0010-0000-0100-00001F000000}" name="RewardBlessLevel"/>
-    <tableColumn id="42" xr3:uid="{00000000-0010-0000-0100-00002A000000}" name="RewardBlessId"/>
-    <tableColumn id="52" xr3:uid="{00000000-0010-0000-0100-000034000000}" name="RewardResId" dataDxfId="12"/>
-    <tableColumn id="53" xr3:uid="{00000000-0010-0000-0100-000035000000}" name="RewardResAmount" dataDxfId="11"/>
-    <tableColumn id="26" xr3:uid="{00000000-0010-0000-0100-00001A000000}" name="UnlockRival"/>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0100-000010000000}" name="PunishGold"/>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0100-000011000000}" name="PunishFood"/>
-    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0100-000012000000}" name="PunishHealth"/>
-    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0100-000013000000}" name="PunishMental"/>
-    <tableColumn id="30" xr3:uid="{00000000-0010-0000-0100-00001E000000}" name="PunishBlessLevel"/>
-    <tableColumn id="49" xr3:uid="{00000000-0010-0000-0100-000031000000}" name="ChooseWinRate"/>
-    <tableColumn id="48" xr3:uid="{00000000-0010-0000-0100-000030000000}" name="ChooseGold"/>
-    <tableColumn id="47" xr3:uid="{00000000-0010-0000-0100-00002F000000}" name="ChooseGoldAddon"/>
-    <tableColumn id="46" xr3:uid="{00000000-0010-0000-0100-00002E000000}" name="ChooseFood"/>
-    <tableColumn id="45" xr3:uid="{00000000-0010-0000-0100-00002D000000}" name="ChooseFoodAddon"/>
-    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0100-000014000000}" name="TradeGold"/>
-    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0100-000015000000}" name="TradeFood"/>
-    <tableColumn id="22" xr3:uid="{00000000-0010-0000-0100-000016000000}" name="TradeHealth"/>
-    <tableColumn id="23" xr3:uid="{00000000-0010-0000-0100-000017000000}" name="TradeMental"/>
-    <tableColumn id="33" xr3:uid="{00000000-0010-0000-0100-000021000000}" name="TradeDropItem" dataDxfId="10"/>
+  <tableColumns count="59">
+    <tableColumn id="1" name="Id"/>
+    <tableColumn id="2" name="Name"/>
+    <tableColumn id="27" name="Type" dataDxfId="37"/>
+    <tableColumn id="3" name="Level"/>
+    <tableColumn id="25" name="Danger"/>
+    <tableColumn id="24" name="Ename"/>
+    <tableColumn id="4" name="Figue"/>
+    <tableColumn id="5" name="Script"/>
+    <tableColumn id="6" name="TriggerMulti"/>
+    <tableColumn id="40" name="Catalog" dataDxfId="36"/>
+    <tableColumn id="35" name="TriggerHourBegin" dataDxfId="35"/>
+    <tableColumn id="34" name="TriggerHourEnd" dataDxfId="34"/>
+    <tableColumn id="37" name="TriggerQuestNotReceive" dataDxfId="33"/>
+    <tableColumn id="38" name="TriggerQuestReceived" dataDxfId="32"/>
+    <tableColumn id="36" name="TriggerQuestFinished" dataDxfId="31"/>
+    <tableColumn id="39" name="TriggerRate" dataDxfId="30"/>
+    <tableColumn id="7" name="EnemyName"/>
+    <tableColumn id="51" name="CanBribe" dataDxfId="29"/>
+    <tableColumn id="32" name="SceneId" dataDxfId="28"/>
+    <tableColumn id="29" name="Position" dataDxfId="27"/>
+    <tableColumn id="54" name="DungeonId" dataDxfId="26"/>
+    <tableColumn id="50" name="CheckQuest" dataDxfId="25"/>
+    <tableColumn id="28" name="NextQuest" dataDxfId="24"/>
+    <tableColumn id="44" name="HiddenRoomQuest" dataDxfId="23"/>
+    <tableColumn id="8" name="ShopName" dataDxfId="22"/>
+    <tableColumn id="41" name="MiniGameId" dataDxfId="21"/>
+    <tableColumn id="43" name="PayKey" dataDxfId="20"/>
+    <tableColumn id="9" name="RewardGold"/>
+    <tableColumn id="10" name="RewardFood"/>
+    <tableColumn id="11" name="RewardHealth"/>
+    <tableColumn id="12" name="RewardMental"/>
+    <tableColumn id="13" name="RewardExp"/>
+    <tableColumn id="55" name="RewardStr" dataDxfId="4"/>
+    <tableColumn id="56" name="RewardAgi" dataDxfId="3"/>
+    <tableColumn id="57" name="RewardIntl" dataDxfId="2"/>
+    <tableColumn id="58" name="RewardPerc" dataDxfId="1"/>
+    <tableColumn id="59" name="RewardEndu" dataDxfId="0"/>
+    <tableColumn id="14" name="RewardItem"/>
+    <tableColumn id="15" name="RewardDrop"/>
+    <tableColumn id="31" name="RewardBlessLevel"/>
+    <tableColumn id="42" name="RewardBlessId"/>
+    <tableColumn id="52" name="RewardResId" dataDxfId="19"/>
+    <tableColumn id="53" name="RewardResAmount" dataDxfId="18"/>
+    <tableColumn id="26" name="UnlockRival"/>
+    <tableColumn id="16" name="PunishGold"/>
+    <tableColumn id="17" name="PunishFood"/>
+    <tableColumn id="18" name="PunishHealth"/>
+    <tableColumn id="19" name="PunishMental"/>
+    <tableColumn id="30" name="PunishBlessLevel"/>
+    <tableColumn id="49" name="ChooseWinRate"/>
+    <tableColumn id="48" name="ChooseGold"/>
+    <tableColumn id="47" name="ChooseGoldAddon"/>
+    <tableColumn id="46" name="ChooseFood"/>
+    <tableColumn id="45" name="ChooseFoodAddon"/>
+    <tableColumn id="20" name="TradeGold"/>
+    <tableColumn id="21" name="TradeFood"/>
+    <tableColumn id="22" name="TradeHealth"/>
+    <tableColumn id="23" name="TradeMental"/>
+    <tableColumn id="33" name="TradeDropItem" dataDxfId="17"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3957,7 +4267,7 @@
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr val="window" lastClr="C7EDCC"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -4269,12 +4579,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BB86"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:BG86"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="P1" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="U1" sqref="U1:U3"/>
+      <selection pane="bottomLeft" activeCell="AG1" sqref="AG1:AK3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -4289,16 +4599,16 @@
     <col min="19" max="19" width="9.375" style="8" customWidth="1"/>
     <col min="20" max="25" width="6.5" style="8" customWidth="1"/>
     <col min="26" max="27" width="9.125" style="8" customWidth="1"/>
-    <col min="28" max="32" width="4.875" style="8" customWidth="1"/>
-    <col min="33" max="34" width="9.375" style="8" customWidth="1"/>
-    <col min="35" max="38" width="5.375" style="8" customWidth="1"/>
-    <col min="39" max="39" width="9.375" style="8" customWidth="1"/>
-    <col min="40" max="40" width="6.375" style="8" customWidth="1"/>
-    <col min="41" max="54" width="4.75" style="8" customWidth="1"/>
-    <col min="55" max="16384" width="9" style="8"/>
+    <col min="28" max="37" width="4.875" style="8" customWidth="1"/>
+    <col min="38" max="39" width="9.375" style="8" customWidth="1"/>
+    <col min="40" max="43" width="5.375" style="8" customWidth="1"/>
+    <col min="44" max="44" width="9.375" style="8" customWidth="1"/>
+    <col min="45" max="45" width="6.375" style="8" customWidth="1"/>
+    <col min="46" max="59" width="4.75" style="8" customWidth="1"/>
+    <col min="60" max="16384" width="9" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:54" ht="69" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:59" ht="69" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>71</v>
       </c>
@@ -4396,73 +4706,88 @@
         <v>78</v>
       </c>
       <c r="AG1" s="4" t="s">
+        <v>566</v>
+      </c>
+      <c r="AH1" s="4" t="s">
+        <v>567</v>
+      </c>
+      <c r="AI1" s="4" t="s">
+        <v>568</v>
+      </c>
+      <c r="AJ1" s="4" t="s">
+        <v>569</v>
+      </c>
+      <c r="AK1" s="4" t="s">
+        <v>570</v>
+      </c>
+      <c r="AL1" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="AH1" s="4" t="s">
+      <c r="AM1" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="AI1" s="4" t="s">
+      <c r="AN1" s="4" t="s">
         <v>169</v>
       </c>
-      <c r="AJ1" s="4" t="s">
+      <c r="AO1" s="4" t="s">
         <v>391</v>
       </c>
-      <c r="AK1" s="4" t="s">
+      <c r="AP1" s="4" t="s">
         <v>544</v>
       </c>
-      <c r="AL1" s="4" t="s">
+      <c r="AQ1" s="4" t="s">
         <v>539</v>
       </c>
-      <c r="AM1" s="4" t="s">
+      <c r="AR1" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="AN1" s="5" t="s">
+      <c r="AS1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="AO1" s="5" t="s">
+      <c r="AT1" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="AP1" s="5" t="s">
+      <c r="AU1" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="AQ1" s="5" t="s">
+      <c r="AV1" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="AR1" s="5" t="s">
+      <c r="AW1" s="5" t="s">
         <v>170</v>
       </c>
-      <c r="AS1" s="6" t="s">
+      <c r="AX1" s="6" t="s">
         <v>495</v>
       </c>
-      <c r="AT1" s="6" t="s">
+      <c r="AY1" s="6" t="s">
         <v>487</v>
       </c>
-      <c r="AU1" s="6" t="s">
+      <c r="AZ1" s="6" t="s">
         <v>489</v>
       </c>
-      <c r="AV1" s="6" t="s">
+      <c r="BA1" s="6" t="s">
         <v>486</v>
       </c>
-      <c r="AW1" s="6" t="s">
+      <c r="BB1" s="6" t="s">
         <v>491</v>
       </c>
-      <c r="AX1" s="7" t="s">
+      <c r="BC1" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="AY1" s="7" t="s">
+      <c r="BD1" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="AZ1" s="7" t="s">
+      <c r="BE1" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="BA1" s="7" t="s">
+      <c r="BF1" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="BB1" s="7" t="s">
+      <c r="BG1" s="7" t="s">
         <v>380</v>
       </c>
     </row>
-    <row r="2" spans="1:54" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:59" x14ac:dyDescent="0.15">
       <c r="A2" s="9" t="s">
         <v>53</v>
       </c>
@@ -4560,73 +4885,88 @@
         <v>53</v>
       </c>
       <c r="AG2" s="12" t="s">
+        <v>116</v>
+      </c>
+      <c r="AH2" s="12" t="s">
+        <v>116</v>
+      </c>
+      <c r="AI2" s="12" t="s">
+        <v>116</v>
+      </c>
+      <c r="AJ2" s="12" t="s">
+        <v>116</v>
+      </c>
+      <c r="AK2" s="12" t="s">
+        <v>116</v>
+      </c>
+      <c r="AL2" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="AH2" s="12" t="s">
+      <c r="AM2" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="AI2" s="12" t="s">
+      <c r="AN2" s="12" t="s">
         <v>168</v>
       </c>
-      <c r="AJ2" s="12" t="s">
+      <c r="AO2" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="AK2" s="12" t="s">
+      <c r="AP2" s="12" t="s">
         <v>542</v>
       </c>
-      <c r="AL2" s="12" t="s">
+      <c r="AQ2" s="12" t="s">
         <v>543</v>
       </c>
-      <c r="AM2" s="12" t="s">
+      <c r="AR2" s="12" t="s">
         <v>352</v>
       </c>
-      <c r="AN2" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="AO2" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="AP2" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="AQ2" s="13" t="s">
+      <c r="AS2" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="AT2" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="AU2" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="AV2" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="AR2" s="13" t="s">
+      <c r="AW2" s="13" t="s">
         <v>171</v>
       </c>
-      <c r="AS2" s="14" t="s">
+      <c r="AX2" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="AT2" s="14" t="s">
+      <c r="AY2" s="14" t="s">
         <v>484</v>
       </c>
-      <c r="AU2" s="14" t="s">
+      <c r="AZ2" s="14" t="s">
         <v>484</v>
       </c>
-      <c r="AV2" s="14" t="s">
+      <c r="BA2" s="14" t="s">
         <v>484</v>
       </c>
-      <c r="AW2" s="14" t="s">
+      <c r="BB2" s="14" t="s">
         <v>484</v>
       </c>
-      <c r="AX2" s="15" t="s">
+      <c r="BC2" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="AY2" s="15" t="s">
+      <c r="BD2" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="AZ2" s="15" t="s">
+      <c r="BE2" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="BA2" s="15" t="s">
+      <c r="BF2" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="BB2" s="15" t="s">
+      <c r="BG2" s="15" t="s">
         <v>381</v>
       </c>
     </row>
-    <row r="3" spans="1:54" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:59" x14ac:dyDescent="0.15">
       <c r="A3" s="16" t="s">
         <v>58</v>
       </c>
@@ -4720,77 +5060,92 @@
       <c r="AE3" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="AF3" s="19" t="s">
-        <v>66</v>
-      </c>
-      <c r="AG3" s="19" t="s">
+      <c r="AF3" s="77" t="s">
+        <v>571</v>
+      </c>
+      <c r="AG3" s="77" t="s">
+        <v>572</v>
+      </c>
+      <c r="AH3" s="77" t="s">
+        <v>573</v>
+      </c>
+      <c r="AI3" s="77" t="s">
+        <v>574</v>
+      </c>
+      <c r="AJ3" s="77" t="s">
+        <v>575</v>
+      </c>
+      <c r="AK3" s="77" t="s">
+        <v>576</v>
+      </c>
+      <c r="AL3" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="AH3" s="19" t="s">
+      <c r="AM3" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="AI3" s="19" t="s">
+      <c r="AN3" s="19" t="s">
         <v>167</v>
       </c>
-      <c r="AJ3" s="19" t="s">
+      <c r="AO3" s="19" t="s">
         <v>392</v>
       </c>
-      <c r="AK3" s="19" t="s">
+      <c r="AP3" s="19" t="s">
         <v>540</v>
       </c>
-      <c r="AL3" s="19" t="s">
+      <c r="AQ3" s="19" t="s">
         <v>541</v>
       </c>
-      <c r="AM3" s="19" t="s">
+      <c r="AR3" s="19" t="s">
         <v>330</v>
       </c>
-      <c r="AN3" s="20" t="s">
+      <c r="AS3" s="20" t="s">
         <v>67</v>
       </c>
-      <c r="AO3" s="20" t="s">
+      <c r="AT3" s="20" t="s">
         <v>68</v>
       </c>
-      <c r="AP3" s="20" t="s">
+      <c r="AU3" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="AQ3" s="20" t="s">
+      <c r="AV3" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="AR3" s="20" t="s">
+      <c r="AW3" s="20" t="s">
         <v>172</v>
       </c>
-      <c r="AS3" s="21" t="s">
+      <c r="AX3" s="21" t="s">
         <v>496</v>
       </c>
-      <c r="AT3" s="21" t="s">
+      <c r="AY3" s="21" t="s">
         <v>494</v>
       </c>
-      <c r="AU3" s="21" t="s">
+      <c r="AZ3" s="21" t="s">
         <v>490</v>
       </c>
-      <c r="AV3" s="21" t="s">
+      <c r="BA3" s="21" t="s">
         <v>485</v>
       </c>
-      <c r="AW3" s="21" t="s">
+      <c r="BB3" s="21" t="s">
         <v>492</v>
       </c>
-      <c r="AX3" s="16" t="s">
+      <c r="BC3" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="AY3" s="16" t="s">
+      <c r="BD3" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="AZ3" s="16" t="s">
+      <c r="BE3" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="BA3" s="16" t="s">
+      <c r="BF3" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="BB3" s="16" t="s">
+      <c r="BG3" s="16" t="s">
         <v>382</v>
       </c>
     </row>
-    <row r="4" spans="1:54" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:59" x14ac:dyDescent="0.15">
       <c r="A4" s="8">
         <v>42000001</v>
       </c>
@@ -4856,41 +5211,41 @@
       <c r="AF4" s="8">
         <v>100</v>
       </c>
-      <c r="AK4" s="8">
+      <c r="AP4" s="8">
         <v>3</v>
       </c>
-      <c r="AL4" s="8">
+      <c r="AQ4" s="8">
         <v>200</v>
       </c>
-      <c r="AN4" s="8">
+      <c r="AS4" s="8">
         <v>100</v>
       </c>
-      <c r="AO4" s="8">
+      <c r="AT4" s="8">
         <v>100</v>
       </c>
-      <c r="AP4" s="8">
+      <c r="AU4" s="8">
         <v>100</v>
       </c>
-      <c r="AQ4" s="8">
+      <c r="AV4" s="8">
         <v>100</v>
       </c>
-      <c r="AS4" s="8">
+      <c r="AX4" s="8">
         <v>35</v>
       </c>
-      <c r="AT4" s="8">
+      <c r="AY4" s="8">
         <v>50</v>
       </c>
-      <c r="AU4" s="8">
+      <c r="AZ4" s="8">
         <v>25</v>
       </c>
-      <c r="AV4" s="8">
+      <c r="BA4" s="8">
         <v>50</v>
       </c>
-      <c r="AW4" s="8">
+      <c r="BB4" s="8">
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:54" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:59" x14ac:dyDescent="0.15">
       <c r="A5" s="25">
         <v>42000002</v>
       </c>
@@ -4922,7 +5277,7 @@
       <c r="P5" s="22"/>
       <c r="R5" s="22"/>
     </row>
-    <row r="6" spans="1:54" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:59" x14ac:dyDescent="0.15">
       <c r="A6" s="25">
         <v>42000003</v>
       </c>
@@ -4956,7 +5311,7 @@
       <c r="P6" s="22"/>
       <c r="R6" s="22"/>
     </row>
-    <row r="7" spans="1:54" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:59" x14ac:dyDescent="0.15">
       <c r="A7" s="25">
         <v>42000004</v>
       </c>
@@ -4990,7 +5345,7 @@
       <c r="P7" s="22"/>
       <c r="R7" s="22"/>
     </row>
-    <row r="8" spans="1:54" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:59" x14ac:dyDescent="0.15">
       <c r="A8" s="25">
         <v>42000005</v>
       </c>
@@ -5023,14 +5378,14 @@
       <c r="O8" s="22"/>
       <c r="P8" s="22"/>
       <c r="R8" s="22"/>
-      <c r="AX8" s="8">
+      <c r="BC8" s="8">
         <v>-100</v>
       </c>
-      <c r="AZ8" s="8">
+      <c r="BE8" s="8">
         <v>100</v>
       </c>
     </row>
-    <row r="9" spans="1:54" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:59" x14ac:dyDescent="0.15">
       <c r="A9" s="25">
         <v>42000006</v>
       </c>
@@ -5063,14 +5418,14 @@
       <c r="O9" s="22"/>
       <c r="P9" s="22"/>
       <c r="R9" s="22"/>
-      <c r="AX9" s="8">
+      <c r="BC9" s="8">
         <v>-100</v>
       </c>
-      <c r="BA9" s="8">
+      <c r="BF9" s="8">
         <v>100</v>
       </c>
     </row>
-    <row r="10" spans="1:54" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:59" x14ac:dyDescent="0.15">
       <c r="A10" s="25">
         <v>42000007</v>
       </c>
@@ -5103,14 +5458,14 @@
       <c r="O10" s="22"/>
       <c r="P10" s="22"/>
       <c r="R10" s="22"/>
-      <c r="AX10" s="8">
+      <c r="BC10" s="8">
         <v>-100</v>
       </c>
-      <c r="AY10" s="8">
+      <c r="BD10" s="8">
         <v>100</v>
       </c>
     </row>
-    <row r="11" spans="1:54" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:59" x14ac:dyDescent="0.15">
       <c r="A11" s="25">
         <v>42000008</v>
       </c>
@@ -5144,7 +5499,7 @@
       <c r="P11" s="22"/>
       <c r="R11" s="22"/>
     </row>
-    <row r="12" spans="1:54" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:59" x14ac:dyDescent="0.15">
       <c r="A12" s="25">
         <v>42000009</v>
       </c>
@@ -5178,7 +5533,7 @@
       <c r="P12" s="22"/>
       <c r="R12" s="22"/>
     </row>
-    <row r="13" spans="1:54" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:59" x14ac:dyDescent="0.15">
       <c r="A13" s="8">
         <v>42010001</v>
       </c>
@@ -5212,7 +5567,7 @@
       <c r="P13" s="22"/>
       <c r="R13" s="22"/>
     </row>
-    <row r="14" spans="1:54" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:59" x14ac:dyDescent="0.15">
       <c r="A14" s="8">
         <v>42010002</v>
       </c>
@@ -5247,7 +5602,7 @@
       <c r="Q14" s="23"/>
       <c r="R14" s="22"/>
     </row>
-    <row r="15" spans="1:54" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:59" x14ac:dyDescent="0.15">
       <c r="A15" s="8">
         <v>42010003</v>
       </c>
@@ -5294,17 +5649,17 @@
       <c r="AC15" s="8">
         <v>100</v>
       </c>
-      <c r="AK15" s="8">
+      <c r="AP15" s="8">
         <v>2</v>
       </c>
-      <c r="AL15" s="8">
+      <c r="AQ15" s="8">
         <v>70</v>
       </c>
-      <c r="AP15" s="8">
+      <c r="AU15" s="8">
         <v>70</v>
       </c>
     </row>
-    <row r="16" spans="1:54" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:59" x14ac:dyDescent="0.15">
       <c r="A16" s="8">
         <v>42010004</v>
       </c>
@@ -5343,14 +5698,14 @@
       <c r="AF16" s="8">
         <v>30</v>
       </c>
-      <c r="AN16" s="8">
+      <c r="AS16" s="8">
         <v>30</v>
       </c>
-      <c r="AO16" s="8">
+      <c r="AT16" s="8">
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="1:43" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:48" x14ac:dyDescent="0.15">
       <c r="A17" s="8">
         <v>42010005</v>
       </c>
@@ -5391,7 +5746,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="18" spans="1:43" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:48" x14ac:dyDescent="0.15">
       <c r="A18" s="8">
         <v>42010006</v>
       </c>
@@ -5438,17 +5793,17 @@
       <c r="AF18" s="8">
         <v>50</v>
       </c>
-      <c r="AK18" s="8">
+      <c r="AP18" s="8">
         <v>2</v>
       </c>
-      <c r="AL18" s="8">
+      <c r="AQ18" s="8">
         <v>70</v>
       </c>
-      <c r="AP18" s="8">
+      <c r="AU18" s="8">
         <v>100</v>
       </c>
     </row>
-    <row r="19" spans="1:43" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:48" x14ac:dyDescent="0.15">
       <c r="A19" s="8">
         <v>42010007</v>
       </c>
@@ -5490,15 +5845,15 @@
       <c r="AB19" s="8">
         <v>150</v>
       </c>
-      <c r="AH19" s="23"/>
-      <c r="AN19" s="8">
+      <c r="AM19" s="23"/>
+      <c r="AS19" s="8">
         <v>150</v>
       </c>
-      <c r="AQ19" s="8">
+      <c r="AV19" s="8">
         <v>50</v>
       </c>
     </row>
-    <row r="20" spans="1:43" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:48" x14ac:dyDescent="0.15">
       <c r="A20" s="8">
         <v>42010008</v>
       </c>
@@ -5534,11 +5889,11 @@
       <c r="AC20" s="8">
         <v>100</v>
       </c>
-      <c r="AH20" s="24" t="s">
+      <c r="AM20" s="24" t="s">
         <v>304</v>
       </c>
     </row>
-    <row r="21" spans="1:43" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:48" x14ac:dyDescent="0.15">
       <c r="A21" s="8">
         <v>42010009</v>
       </c>
@@ -5571,11 +5926,11 @@
       <c r="O21" s="22"/>
       <c r="P21" s="22"/>
       <c r="R21" s="22"/>
-      <c r="AH21" s="8" t="s">
+      <c r="AM21" s="8" t="s">
         <v>305</v>
       </c>
     </row>
-    <row r="22" spans="1:43" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:48" x14ac:dyDescent="0.15">
       <c r="A22" s="8">
         <v>42010010</v>
       </c>
@@ -5608,14 +5963,14 @@
       <c r="O22" s="22"/>
       <c r="P22" s="22"/>
       <c r="R22" s="22"/>
-      <c r="AH22" s="8" t="s">
+      <c r="AM22" s="8" t="s">
         <v>306</v>
       </c>
-      <c r="AP22" s="8">
+      <c r="AU22" s="8">
         <v>50</v>
       </c>
     </row>
-    <row r="23" spans="1:43" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:48" x14ac:dyDescent="0.15">
       <c r="A23" s="8">
         <v>42010011</v>
       </c>
@@ -5652,11 +6007,11 @@
       <c r="AE23" s="8">
         <v>150</v>
       </c>
-      <c r="AH23" s="8" t="s">
+      <c r="AM23" s="8" t="s">
         <v>307</v>
       </c>
     </row>
-    <row r="24" spans="1:43" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:48" x14ac:dyDescent="0.15">
       <c r="A24" s="8">
         <v>42010012</v>
       </c>
@@ -5703,17 +6058,17 @@
       <c r="AC24" s="8">
         <v>100</v>
       </c>
-      <c r="AK24" s="8">
+      <c r="AP24" s="8">
         <v>6</v>
       </c>
-      <c r="AL24" s="8">
+      <c r="AQ24" s="8">
         <v>50</v>
       </c>
-      <c r="AP24" s="8">
+      <c r="AU24" s="8">
         <v>150</v>
       </c>
     </row>
-    <row r="25" spans="1:43" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:48" x14ac:dyDescent="0.15">
       <c r="A25" s="8">
         <v>42010013</v>
       </c>
@@ -5760,17 +6115,17 @@
       <c r="AC25" s="8">
         <v>150</v>
       </c>
-      <c r="AK25" s="8">
+      <c r="AP25" s="8">
         <v>2</v>
       </c>
-      <c r="AL25" s="8">
+      <c r="AQ25" s="8">
         <v>100</v>
       </c>
-      <c r="AP25" s="8">
+      <c r="AU25" s="8">
         <v>100</v>
       </c>
     </row>
-    <row r="26" spans="1:43" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:48" x14ac:dyDescent="0.15">
       <c r="A26" s="8">
         <v>42010014</v>
       </c>
@@ -5817,23 +6172,23 @@
       <c r="AF26" s="8">
         <v>100</v>
       </c>
-      <c r="AH26" s="8" t="s">
+      <c r="AM26" s="8" t="s">
         <v>414</v>
       </c>
-      <c r="AK26" s="8">
+      <c r="AP26" s="8">
         <v>4</v>
-      </c>
-      <c r="AL26" s="8">
-        <v>100</v>
-      </c>
-      <c r="AP26" s="8">
-        <v>100</v>
       </c>
       <c r="AQ26" s="8">
         <v>100</v>
       </c>
-    </row>
-    <row r="27" spans="1:43" x14ac:dyDescent="0.15">
+      <c r="AU26" s="8">
+        <v>100</v>
+      </c>
+      <c r="AV26" s="8">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="27" spans="1:48" x14ac:dyDescent="0.15">
       <c r="A27" s="8">
         <v>42010015</v>
       </c>
@@ -5869,11 +6224,11 @@
       <c r="O27" s="22"/>
       <c r="P27" s="22"/>
       <c r="R27" s="22"/>
-      <c r="AP27" s="8">
+      <c r="AU27" s="8">
         <v>80</v>
       </c>
     </row>
-    <row r="28" spans="1:43" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:48" x14ac:dyDescent="0.15">
       <c r="A28" s="8">
         <v>42010016</v>
       </c>
@@ -5914,7 +6269,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="29" spans="1:43" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:48" x14ac:dyDescent="0.15">
       <c r="A29" s="8">
         <v>42010017</v>
       </c>
@@ -5964,20 +6319,20 @@
       <c r="AF29" s="8">
         <v>100</v>
       </c>
-      <c r="AH29" s="8" t="s">
+      <c r="AM29" s="8" t="s">
         <v>413</v>
       </c>
-      <c r="AK29" s="8">
+      <c r="AP29" s="8">
         <v>5</v>
       </c>
-      <c r="AL29" s="8">
+      <c r="AQ29" s="8">
         <v>100</v>
       </c>
-      <c r="AP29" s="8">
+      <c r="AU29" s="8">
         <v>100</v>
       </c>
     </row>
-    <row r="30" spans="1:43" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:48" x14ac:dyDescent="0.15">
       <c r="A30" s="8">
         <v>42010018</v>
       </c>
@@ -6013,7 +6368,7 @@
       <c r="P30" s="22"/>
       <c r="R30" s="22"/>
     </row>
-    <row r="31" spans="1:43" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:48" x14ac:dyDescent="0.15">
       <c r="A31" s="8">
         <v>42010019</v>
       </c>
@@ -6051,14 +6406,14 @@
       <c r="O31" s="22"/>
       <c r="P31" s="22"/>
       <c r="R31" s="22"/>
-      <c r="AO31" s="8">
+      <c r="AT31" s="8">
         <v>100</v>
       </c>
-      <c r="AP31" s="8">
+      <c r="AU31" s="8">
         <v>50</v>
       </c>
     </row>
-    <row r="32" spans="1:43" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:48" x14ac:dyDescent="0.15">
       <c r="A32" s="8">
         <v>42010020</v>
       </c>
@@ -6096,14 +6451,14 @@
       <c r="O32" s="22"/>
       <c r="P32" s="22"/>
       <c r="R32" s="22"/>
-      <c r="AO32" s="8">
+      <c r="AT32" s="8">
         <v>50</v>
       </c>
-      <c r="AP32" s="8">
+      <c r="AU32" s="8">
         <v>100</v>
       </c>
     </row>
-    <row r="33" spans="1:44" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:49" x14ac:dyDescent="0.15">
       <c r="A33" s="8">
         <v>42010021</v>
       </c>
@@ -6140,11 +6495,11 @@
       <c r="P33" s="22"/>
       <c r="Q33" s="23"/>
       <c r="R33" s="22"/>
-      <c r="AQ33" s="8">
+      <c r="AV33" s="8">
         <v>200</v>
       </c>
     </row>
-    <row r="34" spans="1:44" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:49" x14ac:dyDescent="0.15">
       <c r="A34" s="8">
         <v>42010022</v>
       </c>
@@ -6188,14 +6543,14 @@
       <c r="AF34" s="8">
         <v>100</v>
       </c>
-      <c r="AG34" s="8" t="s">
+      <c r="AL34" s="8" t="s">
         <v>301</v>
       </c>
-      <c r="AP34" s="8">
+      <c r="AU34" s="8">
         <v>150</v>
       </c>
     </row>
-    <row r="35" spans="1:44" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:49" x14ac:dyDescent="0.15">
       <c r="A35" s="8">
         <v>42010023</v>
       </c>
@@ -6237,11 +6592,11 @@
       <c r="AD35" s="8">
         <v>100</v>
       </c>
-      <c r="AP35" s="8">
+      <c r="AU35" s="8">
         <v>100</v>
       </c>
     </row>
-    <row r="36" spans="1:44" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:49" x14ac:dyDescent="0.15">
       <c r="A36" s="8">
         <v>42010024</v>
       </c>
@@ -6274,11 +6629,11 @@
       <c r="O36" s="22"/>
       <c r="P36" s="22"/>
       <c r="R36" s="22"/>
-      <c r="AI36" s="8">
+      <c r="AN36" s="8">
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:44" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:49" x14ac:dyDescent="0.15">
       <c r="A37" s="8">
         <v>42010025</v>
       </c>
@@ -6315,7 +6670,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="38" spans="1:44" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:49" x14ac:dyDescent="0.15">
       <c r="A38" s="8">
         <v>42010026</v>
       </c>
@@ -6352,7 +6707,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="39" spans="1:44" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:49" x14ac:dyDescent="0.15">
       <c r="A39" s="8">
         <v>42010027</v>
       </c>
@@ -6389,7 +6744,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="40" spans="1:44" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:49" x14ac:dyDescent="0.15">
       <c r="A40" s="8">
         <v>42010028</v>
       </c>
@@ -6428,11 +6783,11 @@
       <c r="S40" s="8">
         <v>13010004</v>
       </c>
-      <c r="AP40" s="8">
+      <c r="AU40" s="8">
         <v>150</v>
       </c>
     </row>
-    <row r="41" spans="1:44" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:49" x14ac:dyDescent="0.15">
       <c r="A41" s="8">
         <v>42010029</v>
       </c>
@@ -6467,7 +6822,7 @@
       <c r="Q41" s="23"/>
       <c r="R41" s="22"/>
     </row>
-    <row r="42" spans="1:44" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:49" x14ac:dyDescent="0.15">
       <c r="A42" s="8">
         <v>42010030</v>
       </c>
@@ -6517,20 +6872,20 @@
       <c r="AF42" s="8">
         <v>100</v>
       </c>
-      <c r="AK42" s="8">
+      <c r="AP42" s="8">
         <v>5</v>
       </c>
-      <c r="AL42" s="8">
+      <c r="AQ42" s="8">
         <v>80</v>
       </c>
-      <c r="AP42" s="8">
+      <c r="AU42" s="8">
         <v>100</v>
       </c>
-      <c r="AQ42" s="8">
+      <c r="AV42" s="8">
         <v>150</v>
       </c>
     </row>
-    <row r="43" spans="1:44" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:49" x14ac:dyDescent="0.15">
       <c r="A43" s="8">
         <v>42010031</v>
       </c>
@@ -6575,11 +6930,11 @@
       <c r="AF43" s="8">
         <v>50</v>
       </c>
-      <c r="AN43" s="8">
+      <c r="AS43" s="8">
         <v>50</v>
       </c>
     </row>
-    <row r="44" spans="1:44" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:49" x14ac:dyDescent="0.15">
       <c r="A44" s="8">
         <v>42010032</v>
       </c>
@@ -6620,7 +6975,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="45" spans="1:44" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:49" x14ac:dyDescent="0.15">
       <c r="A45" s="8">
         <v>42010033</v>
       </c>
@@ -6667,14 +7022,14 @@
       <c r="AF45" s="8">
         <v>50</v>
       </c>
-      <c r="AP45" s="8">
+      <c r="AU45" s="8">
         <v>100</v>
       </c>
-      <c r="AQ45" s="8">
+      <c r="AV45" s="8">
         <v>50</v>
       </c>
     </row>
-    <row r="46" spans="1:44" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:49" x14ac:dyDescent="0.15">
       <c r="A46" s="8">
         <v>42010034</v>
       </c>
@@ -6721,14 +7076,14 @@
       <c r="AF46" s="8">
         <v>50</v>
       </c>
-      <c r="AP46" s="8">
+      <c r="AU46" s="8">
         <v>100</v>
       </c>
-      <c r="AQ46" s="8">
+      <c r="AV46" s="8">
         <v>50</v>
       </c>
     </row>
-    <row r="47" spans="1:44" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:49" x14ac:dyDescent="0.15">
       <c r="A47" s="8">
         <v>42010035</v>
       </c>
@@ -6775,23 +7130,23 @@
       <c r="AC47" s="8">
         <v>50</v>
       </c>
-      <c r="AG47" s="8" t="s">
+      <c r="AL47" s="8" t="s">
         <v>354</v>
       </c>
-      <c r="AK47" s="8">
+      <c r="AP47" s="8">
         <v>7</v>
       </c>
-      <c r="AL47" s="8">
+      <c r="AQ47" s="8">
         <v>100</v>
       </c>
-      <c r="AP47" s="8">
+      <c r="AU47" s="8">
         <v>150</v>
       </c>
-      <c r="AQ47" s="8">
+      <c r="AV47" s="8">
         <v>50</v>
       </c>
     </row>
-    <row r="48" spans="1:44" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:49" x14ac:dyDescent="0.15">
       <c r="A48" s="8">
         <v>42010036</v>
       </c>
@@ -6841,23 +7196,23 @@
       <c r="AF48" s="8">
         <v>200</v>
       </c>
-      <c r="AK48" s="8">
+      <c r="AP48" s="8">
         <v>3</v>
       </c>
-      <c r="AL48" s="8">
+      <c r="AQ48" s="8">
         <v>150</v>
       </c>
-      <c r="AP48" s="8">
+      <c r="AU48" s="8">
         <v>200</v>
       </c>
-      <c r="AQ48" s="8">
+      <c r="AV48" s="8">
         <v>100</v>
       </c>
-      <c r="AR48" s="8">
+      <c r="AW48" s="8">
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:54" x14ac:dyDescent="0.15">
+    <row r="49" spans="1:59" x14ac:dyDescent="0.15">
       <c r="A49" s="8">
         <v>42010037</v>
       </c>
@@ -6897,20 +7252,20 @@
       <c r="AB49" s="8">
         <v>150</v>
       </c>
-      <c r="AK49" s="8">
+      <c r="AP49" s="8">
         <v>7</v>
       </c>
-      <c r="AL49" s="8">
+      <c r="AQ49" s="8">
         <v>100</v>
       </c>
-      <c r="AO49" s="8">
+      <c r="AT49" s="8">
         <v>150</v>
       </c>
-      <c r="AP49" s="8">
+      <c r="AU49" s="8">
         <v>150</v>
       </c>
     </row>
-    <row r="50" spans="1:54" x14ac:dyDescent="0.15">
+    <row r="50" spans="1:59" x14ac:dyDescent="0.15">
       <c r="A50" s="8">
         <v>42010038</v>
       </c>
@@ -6950,7 +7305,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="51" spans="1:54" x14ac:dyDescent="0.15">
+    <row r="51" spans="1:59" x14ac:dyDescent="0.15">
       <c r="A51" s="8">
         <v>42010039</v>
       </c>
@@ -6989,23 +7344,23 @@
       <c r="AB51" s="8">
         <v>70</v>
       </c>
-      <c r="AG51" s="8" t="s">
+      <c r="AL51" s="8" t="s">
         <v>379</v>
       </c>
-      <c r="AI51" s="8">
+      <c r="AN51" s="8">
         <v>2</v>
       </c>
-      <c r="AK51" s="8">
+      <c r="AP51" s="8">
         <v>5</v>
       </c>
-      <c r="AL51" s="8">
+      <c r="AQ51" s="8">
         <v>70</v>
       </c>
-      <c r="AP51" s="8">
+      <c r="AU51" s="8">
         <v>300</v>
       </c>
     </row>
-    <row r="52" spans="1:54" x14ac:dyDescent="0.15">
+    <row r="52" spans="1:59" x14ac:dyDescent="0.15">
       <c r="A52" s="8">
         <v>42010040</v>
       </c>
@@ -7038,14 +7393,14 @@
       <c r="O52" s="22"/>
       <c r="P52" s="22"/>
       <c r="R52" s="22"/>
-      <c r="AX52" s="8">
+      <c r="BC52" s="8">
         <v>-100</v>
       </c>
-      <c r="BB52" s="8" t="s">
+      <c r="BG52" s="8" t="s">
         <v>386</v>
       </c>
     </row>
-    <row r="53" spans="1:54" x14ac:dyDescent="0.15">
+    <row r="53" spans="1:59" x14ac:dyDescent="0.15">
       <c r="A53" s="8">
         <v>42010041</v>
       </c>
@@ -7092,14 +7447,14 @@
       <c r="AF53" s="8">
         <v>50</v>
       </c>
-      <c r="AO53" s="8">
+      <c r="AT53" s="8">
         <v>100</v>
       </c>
-      <c r="AP53" s="8">
+      <c r="AU53" s="8">
         <v>100</v>
       </c>
     </row>
-    <row r="54" spans="1:54" x14ac:dyDescent="0.15">
+    <row r="54" spans="1:59" x14ac:dyDescent="0.15">
       <c r="A54" s="8">
         <v>42010042</v>
       </c>
@@ -7132,11 +7487,11 @@
       <c r="O54" s="22"/>
       <c r="P54" s="22"/>
       <c r="R54" s="22"/>
-      <c r="AJ54" s="8">
+      <c r="AO54" s="8">
         <v>16020001</v>
       </c>
     </row>
-    <row r="55" spans="1:54" x14ac:dyDescent="0.15">
+    <row r="55" spans="1:59" x14ac:dyDescent="0.15">
       <c r="A55" s="8">
         <v>42010043</v>
       </c>
@@ -7172,9 +7527,9 @@
       <c r="Y55" s="8" t="s">
         <v>403</v>
       </c>
-      <c r="AH55" s="23"/>
-    </row>
-    <row r="56" spans="1:54" x14ac:dyDescent="0.15">
+      <c r="AM55" s="23"/>
+    </row>
+    <row r="56" spans="1:59" x14ac:dyDescent="0.15">
       <c r="A56" s="8">
         <v>42010044</v>
       </c>
@@ -7224,12 +7579,12 @@
       <c r="AE56" s="8">
         <v>70</v>
       </c>
-      <c r="AH56" s="24"/>
-      <c r="AP56" s="8">
+      <c r="AM56" s="24"/>
+      <c r="AU56" s="8">
         <v>100</v>
       </c>
     </row>
-    <row r="57" spans="1:54" x14ac:dyDescent="0.15">
+    <row r="57" spans="1:59" x14ac:dyDescent="0.15">
       <c r="A57" s="8">
         <v>42010045</v>
       </c>
@@ -7274,14 +7629,14 @@
       <c r="AD57" s="8">
         <v>120</v>
       </c>
-      <c r="AK57" s="8">
+      <c r="AP57" s="8">
         <v>4</v>
       </c>
-      <c r="AL57" s="8">
+      <c r="AQ57" s="8">
         <v>100</v>
       </c>
     </row>
-    <row r="58" spans="1:54" x14ac:dyDescent="0.15">
+    <row r="58" spans="1:59" x14ac:dyDescent="0.15">
       <c r="A58" s="8">
         <v>42010046</v>
       </c>
@@ -7323,14 +7678,14 @@
       <c r="AE58" s="8">
         <v>50</v>
       </c>
-      <c r="AO58" s="8">
+      <c r="AT58" s="8">
         <v>100</v>
       </c>
-      <c r="AQ58" s="8">
+      <c r="AV58" s="8">
         <v>100</v>
       </c>
     </row>
-    <row r="59" spans="1:54" x14ac:dyDescent="0.15">
+    <row r="59" spans="1:59" x14ac:dyDescent="0.15">
       <c r="A59" s="8">
         <v>42010047</v>
       </c>
@@ -7366,20 +7721,20 @@
       <c r="O59" s="22"/>
       <c r="P59" s="22"/>
       <c r="R59" s="22"/>
-      <c r="AP59" s="8">
+      <c r="AU59" s="8">
         <v>100</v>
       </c>
-      <c r="AS59" s="8">
+      <c r="AX59" s="8">
         <v>40</v>
       </c>
-      <c r="AV59" s="8">
+      <c r="BA59" s="8">
         <v>100</v>
       </c>
-      <c r="AW59" s="8">
+      <c r="BB59" s="8">
         <v>35</v>
       </c>
     </row>
-    <row r="60" spans="1:54" x14ac:dyDescent="0.15">
+    <row r="60" spans="1:59" x14ac:dyDescent="0.15">
       <c r="A60" s="8">
         <v>42010048</v>
       </c>
@@ -7415,14 +7770,14 @@
       <c r="O60" s="22"/>
       <c r="P60" s="22"/>
       <c r="R60" s="22"/>
-      <c r="AO60" s="8">
+      <c r="AT60" s="8">
         <v>50</v>
       </c>
-      <c r="AP60" s="8">
+      <c r="AU60" s="8">
         <v>50</v>
       </c>
     </row>
-    <row r="61" spans="1:54" x14ac:dyDescent="0.15">
+    <row r="61" spans="1:59" x14ac:dyDescent="0.15">
       <c r="A61" s="8">
         <v>42010049</v>
       </c>
@@ -7464,11 +7819,11 @@
       <c r="AE61" s="8">
         <v>50</v>
       </c>
-      <c r="AG61" s="8" t="s">
+      <c r="AL61" s="8" t="s">
         <v>465</v>
       </c>
     </row>
-    <row r="62" spans="1:54" x14ac:dyDescent="0.15">
+    <row r="62" spans="1:59" x14ac:dyDescent="0.15">
       <c r="A62" s="8">
         <v>42010050</v>
       </c>
@@ -7515,14 +7870,14 @@
       <c r="AF62" s="8">
         <v>70</v>
       </c>
-      <c r="AP62" s="8">
+      <c r="AU62" s="8">
         <v>100</v>
       </c>
-      <c r="AQ62" s="8">
+      <c r="AV62" s="8">
         <v>50</v>
       </c>
     </row>
-    <row r="63" spans="1:54" x14ac:dyDescent="0.15">
+    <row r="63" spans="1:59" x14ac:dyDescent="0.15">
       <c r="A63" s="8">
         <v>42010051</v>
       </c>
@@ -7561,14 +7916,14 @@
       <c r="W63" s="8" t="s">
         <v>482</v>
       </c>
-      <c r="AP63" s="8">
+      <c r="AU63" s="8">
         <v>150</v>
       </c>
-      <c r="AQ63" s="8">
+      <c r="AV63" s="8">
         <v>150</v>
       </c>
     </row>
-    <row r="64" spans="1:54" x14ac:dyDescent="0.15">
+    <row r="64" spans="1:59" x14ac:dyDescent="0.15">
       <c r="A64" s="8">
         <v>42010052</v>
       </c>
@@ -7618,20 +7973,20 @@
       <c r="AF64" s="8">
         <v>70</v>
       </c>
-      <c r="AH64" s="8" t="s">
+      <c r="AM64" s="8" t="s">
         <v>414</v>
       </c>
-      <c r="AK64" s="8">
+      <c r="AP64" s="8">
         <v>7</v>
       </c>
-      <c r="AL64" s="8">
+      <c r="AQ64" s="8">
         <v>150</v>
       </c>
-      <c r="AP64" s="8">
+      <c r="AU64" s="8">
         <v>250</v>
       </c>
     </row>
-    <row r="65" spans="1:49" x14ac:dyDescent="0.15">
+    <row r="65" spans="1:54" x14ac:dyDescent="0.15">
       <c r="A65" s="8">
         <v>42010053</v>
       </c>
@@ -7667,32 +8022,32 @@
       <c r="O65" s="22"/>
       <c r="P65" s="22"/>
       <c r="R65" s="22"/>
-      <c r="AN65" s="8">
-        <v>50</v>
-      </c>
-      <c r="AO65" s="8">
-        <v>150</v>
-      </c>
-      <c r="AP65" s="8">
-        <v>50</v>
-      </c>
       <c r="AS65" s="8">
         <v>50</v>
       </c>
       <c r="AT65" s="8">
+        <v>150</v>
+      </c>
+      <c r="AU65" s="8">
+        <v>50</v>
+      </c>
+      <c r="AX65" s="8">
+        <v>50</v>
+      </c>
+      <c r="AY65" s="8">
         <v>70</v>
       </c>
-      <c r="AU65" s="8">
+      <c r="AZ65" s="8">
         <v>20</v>
       </c>
-      <c r="AV65" s="8">
+      <c r="BA65" s="8">
         <v>100</v>
       </c>
-      <c r="AW65" s="8">
+      <c r="BB65" s="8">
         <v>50</v>
       </c>
     </row>
-    <row r="66" spans="1:49" x14ac:dyDescent="0.15">
+    <row r="66" spans="1:54" x14ac:dyDescent="0.15">
       <c r="A66" s="8">
         <v>42010054</v>
       </c>
@@ -7736,44 +8091,44 @@
       <c r="AB66" s="8">
         <v>300</v>
       </c>
-      <c r="AG66" s="8" t="s">
+      <c r="AL66" s="8" t="s">
         <v>504</v>
       </c>
-      <c r="AH66" s="8" t="s">
+      <c r="AM66" s="8" t="s">
         <v>505</v>
       </c>
-      <c r="AK66" s="8">
+      <c r="AP66" s="8">
         <v>6</v>
       </c>
-      <c r="AL66" s="8">
+      <c r="AQ66" s="8">
         <v>70</v>
       </c>
-      <c r="AN66" s="8">
+      <c r="AS66" s="8">
         <v>150</v>
       </c>
-      <c r="AO66" s="8">
+      <c r="AT66" s="8">
         <v>100</v>
       </c>
-      <c r="AP66" s="8">
+      <c r="AU66" s="8">
         <v>150</v>
       </c>
-      <c r="AS66" s="8">
+      <c r="AX66" s="8">
         <v>40</v>
       </c>
-      <c r="AT66" s="8">
+      <c r="AY66" s="8">
         <v>120</v>
       </c>
-      <c r="AU66" s="8">
+      <c r="AZ66" s="8">
         <v>50</v>
       </c>
-      <c r="AV66" s="8">
+      <c r="BA66" s="8">
         <v>50</v>
       </c>
-      <c r="AW66" s="8">
+      <c r="BB66" s="8">
         <v>25</v>
       </c>
     </row>
-    <row r="67" spans="1:49" x14ac:dyDescent="0.15">
+    <row r="67" spans="1:54" x14ac:dyDescent="0.15">
       <c r="A67" s="8">
         <v>42010055</v>
       </c>
@@ -7823,17 +8178,17 @@
       <c r="AE67" s="8">
         <v>200</v>
       </c>
-      <c r="AI67" s="8">
+      <c r="AN67" s="8">
         <v>2</v>
       </c>
-      <c r="AP67" s="8">
+      <c r="AU67" s="8">
         <v>100</v>
       </c>
-      <c r="AQ67" s="8">
+      <c r="AV67" s="8">
         <v>50</v>
       </c>
     </row>
-    <row r="68" spans="1:49" x14ac:dyDescent="0.15">
+    <row r="68" spans="1:54" x14ac:dyDescent="0.15">
       <c r="A68" s="8">
         <v>42020001</v>
       </c>
@@ -7875,17 +8230,17 @@
       <c r="AF68" s="8">
         <v>100</v>
       </c>
-      <c r="AM68" s="8" t="s">
+      <c r="AR68" s="8" t="s">
         <v>347</v>
       </c>
-      <c r="AP68" s="8">
+      <c r="AU68" s="8">
         <v>200</v>
       </c>
-      <c r="AQ68" s="8">
+      <c r="AV68" s="8">
         <v>200</v>
       </c>
     </row>
-    <row r="69" spans="1:49" x14ac:dyDescent="0.15">
+    <row r="69" spans="1:54" x14ac:dyDescent="0.15">
       <c r="A69" s="8">
         <v>42020002</v>
       </c>
@@ -7932,23 +8287,23 @@
       <c r="AC69" s="8">
         <v>50</v>
       </c>
-      <c r="AH69" s="8" t="s">
+      <c r="AM69" s="8" t="s">
         <v>413</v>
       </c>
-      <c r="AK69" s="8">
+      <c r="AP69" s="8">
         <v>5</v>
       </c>
-      <c r="AL69" s="8">
+      <c r="AQ69" s="8">
         <v>100</v>
       </c>
-      <c r="AP69" s="8">
+      <c r="AU69" s="8">
         <v>150</v>
       </c>
-      <c r="AQ69" s="8">
+      <c r="AV69" s="8">
         <v>150</v>
       </c>
     </row>
-    <row r="70" spans="1:49" x14ac:dyDescent="0.15">
+    <row r="70" spans="1:54" x14ac:dyDescent="0.15">
       <c r="A70" s="8">
         <v>42020003</v>
       </c>
@@ -7985,14 +8340,14 @@
       <c r="P70" s="22"/>
       <c r="Q70" s="24"/>
       <c r="R70" s="22"/>
-      <c r="AN70" s="8">
+      <c r="AS70" s="8">
         <v>100</v>
       </c>
-      <c r="AP70" s="8">
+      <c r="AU70" s="8">
         <v>100</v>
       </c>
     </row>
-    <row r="71" spans="1:49" x14ac:dyDescent="0.15">
+    <row r="71" spans="1:54" x14ac:dyDescent="0.15">
       <c r="A71" s="8">
         <v>42020004</v>
       </c>
@@ -8028,14 +8383,14 @@
       <c r="O71" s="22"/>
       <c r="P71" s="22"/>
       <c r="R71" s="22"/>
-      <c r="AI71" s="8">
+      <c r="AN71" s="8">
         <v>1</v>
       </c>
-      <c r="AR71" s="8">
+      <c r="AW71" s="8">
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="1:49" x14ac:dyDescent="0.15">
+    <row r="72" spans="1:54" x14ac:dyDescent="0.15">
       <c r="A72" s="8">
         <v>42020005</v>
       </c>
@@ -8082,20 +8437,20 @@
       <c r="AC72" s="8">
         <v>150</v>
       </c>
-      <c r="AK72" s="8">
+      <c r="AP72" s="8">
         <v>4</v>
       </c>
-      <c r="AL72" s="8">
+      <c r="AQ72" s="8">
         <v>70</v>
       </c>
-      <c r="AN72" s="8">
+      <c r="AS72" s="8">
         <v>200</v>
       </c>
-      <c r="AO72" s="8">
+      <c r="AT72" s="8">
         <v>200</v>
       </c>
     </row>
-    <row r="73" spans="1:49" x14ac:dyDescent="0.15">
+    <row r="73" spans="1:54" x14ac:dyDescent="0.15">
       <c r="A73" s="8">
         <v>42020006</v>
       </c>
@@ -8142,11 +8497,11 @@
       <c r="AF73" s="8">
         <v>200</v>
       </c>
-      <c r="AP73" s="8">
+      <c r="AU73" s="8">
         <v>300</v>
       </c>
     </row>
-    <row r="74" spans="1:49" x14ac:dyDescent="0.15">
+    <row r="74" spans="1:54" x14ac:dyDescent="0.15">
       <c r="A74" s="8">
         <v>42020007</v>
       </c>
@@ -8181,7 +8536,7 @@
       <c r="Q74" s="24"/>
       <c r="R74" s="22"/>
     </row>
-    <row r="75" spans="1:49" x14ac:dyDescent="0.15">
+    <row r="75" spans="1:54" x14ac:dyDescent="0.15">
       <c r="A75" s="8">
         <v>42020008</v>
       </c>
@@ -8215,7 +8570,7 @@
       <c r="P75" s="22"/>
       <c r="R75" s="22"/>
     </row>
-    <row r="76" spans="1:49" x14ac:dyDescent="0.15">
+    <row r="76" spans="1:54" x14ac:dyDescent="0.15">
       <c r="A76" s="8">
         <v>42020009</v>
       </c>
@@ -8257,17 +8612,17 @@
       <c r="AC76" s="8">
         <v>150</v>
       </c>
-      <c r="AG76" s="8" t="s">
+      <c r="AL76" s="8" t="s">
         <v>302</v>
       </c>
-      <c r="AK76" s="8">
+      <c r="AP76" s="8">
         <v>2</v>
       </c>
-      <c r="AL76" s="8">
+      <c r="AQ76" s="8">
         <v>100</v>
       </c>
     </row>
-    <row r="77" spans="1:49" x14ac:dyDescent="0.15">
+    <row r="77" spans="1:54" x14ac:dyDescent="0.15">
       <c r="A77" s="8">
         <v>42020010</v>
       </c>
@@ -8306,17 +8661,17 @@
       <c r="AB77" s="8">
         <v>250</v>
       </c>
-      <c r="AK77" s="8">
+      <c r="AP77" s="8">
         <v>5</v>
-      </c>
-      <c r="AL77" s="8">
-        <v>100</v>
       </c>
       <c r="AQ77" s="8">
         <v>100</v>
       </c>
-    </row>
-    <row r="78" spans="1:49" x14ac:dyDescent="0.15">
+      <c r="AV77" s="8">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="78" spans="1:54" x14ac:dyDescent="0.15">
       <c r="A78" s="8">
         <v>42020011</v>
       </c>
@@ -8352,14 +8707,14 @@
       <c r="Z78" s="8">
         <v>17000002</v>
       </c>
-      <c r="AG78" s="8" t="s">
+      <c r="AL78" s="8" t="s">
         <v>303</v>
       </c>
-      <c r="AI78" s="8">
+      <c r="AN78" s="8">
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:49" x14ac:dyDescent="0.15">
+    <row r="79" spans="1:54" x14ac:dyDescent="0.15">
       <c r="A79" s="8">
         <v>42020012</v>
       </c>
@@ -8398,17 +8753,17 @@
       <c r="AB79" s="8">
         <v>150</v>
       </c>
-      <c r="AH79" s="24" t="s">
+      <c r="AM79" s="24" t="s">
         <v>412</v>
       </c>
-      <c r="AK79" s="8">
+      <c r="AP79" s="8">
         <v>6</v>
       </c>
-      <c r="AL79" s="8">
+      <c r="AQ79" s="8">
         <v>100</v>
       </c>
     </row>
-    <row r="80" spans="1:49" x14ac:dyDescent="0.15">
+    <row r="80" spans="1:54" x14ac:dyDescent="0.15">
       <c r="A80" s="8">
         <v>42020013</v>
       </c>
@@ -8444,9 +8799,9 @@
       <c r="X80" s="8" t="s">
         <v>442</v>
       </c>
-      <c r="AH80" s="24"/>
-    </row>
-    <row r="81" spans="1:54" x14ac:dyDescent="0.15">
+      <c r="AM80" s="24"/>
+    </row>
+    <row r="81" spans="1:59" x14ac:dyDescent="0.15">
       <c r="A81" s="8">
         <v>42020014</v>
       </c>
@@ -8491,12 +8846,12 @@
       <c r="AF81" s="8">
         <v>50</v>
       </c>
-      <c r="AH81" s="24"/>
-      <c r="AI81" s="8">
+      <c r="AM81" s="24"/>
+      <c r="AN81" s="8">
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="1:54" x14ac:dyDescent="0.15">
+    <row r="82" spans="1:59" x14ac:dyDescent="0.15">
       <c r="A82" s="8">
         <v>42020015</v>
       </c>
@@ -8538,9 +8893,9 @@
       <c r="AD82" s="8">
         <v>50</v>
       </c>
-      <c r="AH82" s="24"/>
-    </row>
-    <row r="83" spans="1:54" x14ac:dyDescent="0.15">
+      <c r="AM82" s="24"/>
+    </row>
+    <row r="83" spans="1:59" x14ac:dyDescent="0.15">
       <c r="A83" s="8">
         <v>42020016</v>
       </c>
@@ -8587,21 +8942,21 @@
       <c r="AE83" s="8">
         <v>150</v>
       </c>
-      <c r="AG83" s="8" t="s">
+      <c r="AL83" s="8" t="s">
         <v>454</v>
       </c>
-      <c r="AH83" s="24"/>
-      <c r="AI83" s="8">
+      <c r="AM83" s="24"/>
+      <c r="AN83" s="8">
         <v>1</v>
       </c>
-      <c r="AK83" s="8">
+      <c r="AP83" s="8">
         <v>7</v>
       </c>
-      <c r="AL83" s="8">
+      <c r="AQ83" s="8">
         <v>150</v>
       </c>
     </row>
-    <row r="84" spans="1:54" x14ac:dyDescent="0.15">
+    <row r="84" spans="1:59" x14ac:dyDescent="0.15">
       <c r="A84" s="8">
         <v>42020017</v>
       </c>
@@ -8634,12 +8989,12 @@
       <c r="O84" s="22"/>
       <c r="P84" s="22"/>
       <c r="R84" s="22"/>
-      <c r="AG84" s="8" t="s">
+      <c r="AL84" s="8" t="s">
         <v>467</v>
       </c>
-      <c r="AH84" s="23"/>
-    </row>
-    <row r="85" spans="1:54" x14ac:dyDescent="0.15">
+      <c r="AM84" s="23"/>
+    </row>
+    <row r="85" spans="1:59" x14ac:dyDescent="0.15">
       <c r="A85" s="8">
         <v>42020018</v>
       </c>
@@ -8686,29 +9041,29 @@
       <c r="AF85" s="8">
         <v>300</v>
       </c>
-      <c r="AH85" s="24" t="s">
+      <c r="AM85" s="24" t="s">
         <v>509</v>
       </c>
-      <c r="AI85" s="8">
+      <c r="AN85" s="8">
         <v>2</v>
       </c>
-      <c r="AK85" s="8">
+      <c r="AP85" s="8">
         <v>7</v>
       </c>
-      <c r="AL85" s="8">
+      <c r="AQ85" s="8">
         <v>100</v>
       </c>
-      <c r="AP85" s="8">
+      <c r="AU85" s="8">
         <v>100</v>
       </c>
-      <c r="AQ85" s="8">
+      <c r="AV85" s="8">
         <v>60</v>
       </c>
-      <c r="AR85" s="8">
+      <c r="AW85" s="8">
         <v>1</v>
       </c>
     </row>
-    <row r="86" spans="1:54" x14ac:dyDescent="0.15">
+    <row r="86" spans="1:59" x14ac:dyDescent="0.15">
       <c r="A86" s="8">
         <v>42020019</v>
       </c>
@@ -8741,17 +9096,17 @@
       <c r="O86" s="22"/>
       <c r="P86" s="22"/>
       <c r="R86" s="22"/>
-      <c r="AX86" s="8">
+      <c r="BC86" s="8">
         <v>-1</v>
       </c>
-      <c r="BB86" s="8" t="s">
+      <c r="BG86" s="8" t="s">
         <v>526</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
-  <conditionalFormatting sqref="B4:BB86">
-    <cfRule type="containsBlanks" dxfId="7" priority="13">
+  <conditionalFormatting sqref="B4:BG86">
+    <cfRule type="containsBlanks" dxfId="11" priority="13">
       <formula>LEN(TRIM(B4))=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8765,12 +9120,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:BB38"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:BG38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F33" sqref="F33"/>
+      <selection pane="bottomLeft" activeCell="AG1" sqref="AG1:AK3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -8787,17 +9142,17 @@
     <col min="20" max="20" width="5.75" style="44" customWidth="1"/>
     <col min="21" max="21" width="8.625" style="44" customWidth="1"/>
     <col min="22" max="27" width="5.75" style="44" customWidth="1"/>
-    <col min="28" max="32" width="4.125" style="44" customWidth="1"/>
-    <col min="33" max="33" width="9.75" style="44" customWidth="1"/>
-    <col min="34" max="34" width="7.5" style="44" customWidth="1"/>
-    <col min="35" max="38" width="5.125" style="44" customWidth="1"/>
-    <col min="39" max="39" width="9.375" style="44" customWidth="1"/>
-    <col min="40" max="40" width="9" style="44"/>
-    <col min="41" max="54" width="5" style="44" customWidth="1"/>
-    <col min="55" max="16384" width="9" style="44"/>
+    <col min="28" max="37" width="4.125" style="44" customWidth="1"/>
+    <col min="38" max="38" width="9.75" style="44" customWidth="1"/>
+    <col min="39" max="39" width="7.5" style="44" customWidth="1"/>
+    <col min="40" max="43" width="5.125" style="44" customWidth="1"/>
+    <col min="44" max="44" width="9.375" style="44" customWidth="1"/>
+    <col min="45" max="45" width="9" style="44"/>
+    <col min="46" max="59" width="5" style="44" customWidth="1"/>
+    <col min="60" max="16384" width="9" style="44"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:54" ht="69.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:59" ht="69.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="37" t="s">
         <v>71</v>
       </c>
@@ -8894,74 +9249,89 @@
       <c r="AF1" s="40" t="s">
         <v>78</v>
       </c>
-      <c r="AG1" s="40" t="s">
-        <v>79</v>
-      </c>
-      <c r="AH1" s="40" t="s">
+      <c r="AG1" s="4" t="s">
+        <v>566</v>
+      </c>
+      <c r="AH1" s="4" t="s">
+        <v>567</v>
+      </c>
+      <c r="AI1" s="4" t="s">
+        <v>568</v>
+      </c>
+      <c r="AJ1" s="4" t="s">
+        <v>569</v>
+      </c>
+      <c r="AK1" s="4" t="s">
+        <v>570</v>
+      </c>
+      <c r="AL1" s="4" t="s">
+        <v>577</v>
+      </c>
+      <c r="AM1" s="40" t="s">
         <v>69</v>
       </c>
-      <c r="AI1" s="40" t="s">
+      <c r="AN1" s="40" t="s">
         <v>393</v>
       </c>
-      <c r="AJ1" s="40" t="s">
+      <c r="AO1" s="40" t="s">
         <v>391</v>
       </c>
-      <c r="AK1" s="40" t="s">
+      <c r="AP1" s="40" t="s">
         <v>550</v>
       </c>
-      <c r="AL1" s="40" t="s">
+      <c r="AQ1" s="40" t="s">
         <v>539</v>
       </c>
-      <c r="AM1" s="40" t="s">
+      <c r="AR1" s="40" t="s">
         <v>124</v>
       </c>
-      <c r="AN1" s="41" t="s">
+      <c r="AS1" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="AO1" s="41" t="s">
+      <c r="AT1" s="41" t="s">
         <v>80</v>
       </c>
-      <c r="AP1" s="41" t="s">
+      <c r="AU1" s="41" t="s">
         <v>70</v>
       </c>
-      <c r="AQ1" s="41" t="s">
+      <c r="AV1" s="41" t="s">
         <v>81</v>
       </c>
-      <c r="AR1" s="41" t="s">
+      <c r="AW1" s="41" t="s">
         <v>169</v>
       </c>
-      <c r="AS1" s="42" t="s">
+      <c r="AX1" s="42" t="s">
         <v>495</v>
       </c>
-      <c r="AT1" s="42" t="s">
+      <c r="AY1" s="42" t="s">
         <v>487</v>
       </c>
-      <c r="AU1" s="42" t="s">
+      <c r="AZ1" s="42" t="s">
         <v>489</v>
       </c>
-      <c r="AV1" s="42" t="s">
+      <c r="BA1" s="42" t="s">
         <v>486</v>
       </c>
-      <c r="AW1" s="42" t="s">
+      <c r="BB1" s="42" t="s">
         <v>491</v>
       </c>
-      <c r="AX1" s="43" t="s">
+      <c r="BC1" s="43" t="s">
         <v>493</v>
       </c>
-      <c r="AY1" s="43" t="s">
+      <c r="BD1" s="43" t="s">
         <v>26</v>
       </c>
-      <c r="AZ1" s="43" t="s">
+      <c r="BE1" s="43" t="s">
         <v>30</v>
       </c>
-      <c r="BA1" s="43" t="s">
+      <c r="BF1" s="43" t="s">
         <v>27</v>
       </c>
-      <c r="BB1" s="43" t="s">
+      <c r="BG1" s="43" t="s">
         <v>380</v>
       </c>
     </row>
-    <row r="2" spans="1:54" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:59" x14ac:dyDescent="0.15">
       <c r="A2" s="45" t="s">
         <v>53</v>
       </c>
@@ -9058,74 +9428,89 @@
       <c r="AF2" s="48" t="s">
         <v>53</v>
       </c>
-      <c r="AG2" s="48" t="s">
+      <c r="AG2" s="12" t="s">
+        <v>116</v>
+      </c>
+      <c r="AH2" s="12" t="s">
+        <v>116</v>
+      </c>
+      <c r="AI2" s="12" t="s">
+        <v>116</v>
+      </c>
+      <c r="AJ2" s="12" t="s">
+        <v>116</v>
+      </c>
+      <c r="AK2" s="12" t="s">
+        <v>116</v>
+      </c>
+      <c r="AL2" s="48" t="s">
         <v>57</v>
       </c>
-      <c r="AH2" s="48" t="s">
+      <c r="AM2" s="48" t="s">
         <v>57</v>
       </c>
-      <c r="AI2" s="48" t="s">
+      <c r="AN2" s="48" t="s">
         <v>168</v>
       </c>
-      <c r="AJ2" s="48" t="s">
+      <c r="AO2" s="48" t="s">
         <v>53</v>
       </c>
-      <c r="AK2" s="48" t="s">
+      <c r="AP2" s="48" t="s">
         <v>551</v>
       </c>
-      <c r="AL2" s="48" t="s">
+      <c r="AQ2" s="48" t="s">
         <v>552</v>
       </c>
-      <c r="AM2" s="48" t="s">
+      <c r="AR2" s="48" t="s">
         <v>54</v>
       </c>
-      <c r="AN2" s="49" t="s">
-        <v>0</v>
-      </c>
-      <c r="AO2" s="49" t="s">
-        <v>0</v>
-      </c>
-      <c r="AP2" s="49" t="s">
-        <v>0</v>
-      </c>
-      <c r="AQ2" s="49" t="s">
+      <c r="AS2" s="49" t="s">
+        <v>0</v>
+      </c>
+      <c r="AT2" s="49" t="s">
+        <v>0</v>
+      </c>
+      <c r="AU2" s="49" t="s">
+        <v>0</v>
+      </c>
+      <c r="AV2" s="49" t="s">
         <v>53</v>
       </c>
-      <c r="AR2" s="49" t="s">
+      <c r="AW2" s="49" t="s">
         <v>171</v>
       </c>
-      <c r="AS2" s="50" t="s">
+      <c r="AX2" s="50" t="s">
         <v>53</v>
       </c>
-      <c r="AT2" s="50" t="s">
+      <c r="AY2" s="50" t="s">
         <v>484</v>
       </c>
-      <c r="AU2" s="50" t="s">
+      <c r="AZ2" s="50" t="s">
         <v>484</v>
       </c>
-      <c r="AV2" s="50" t="s">
+      <c r="BA2" s="50" t="s">
         <v>484</v>
       </c>
-      <c r="AW2" s="50" t="s">
+      <c r="BB2" s="50" t="s">
         <v>484</v>
       </c>
-      <c r="AX2" s="51" t="s">
+      <c r="BC2" s="51" t="s">
         <v>24</v>
       </c>
-      <c r="AY2" s="51" t="s">
+      <c r="BD2" s="51" t="s">
         <v>24</v>
       </c>
-      <c r="AZ2" s="51" t="s">
+      <c r="BE2" s="51" t="s">
         <v>24</v>
       </c>
-      <c r="BA2" s="51" t="s">
+      <c r="BF2" s="51" t="s">
         <v>24</v>
       </c>
-      <c r="BB2" s="51" t="s">
+      <c r="BG2" s="51" t="s">
         <v>381</v>
       </c>
     </row>
-    <row r="3" spans="1:54" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:59" x14ac:dyDescent="0.15">
       <c r="A3" s="52" t="s">
         <v>58</v>
       </c>
@@ -9222,74 +9607,89 @@
       <c r="AF3" s="55" t="s">
         <v>66</v>
       </c>
-      <c r="AG3" s="55" t="s">
+      <c r="AG3" s="77" t="s">
+        <v>572</v>
+      </c>
+      <c r="AH3" s="77" t="s">
+        <v>573</v>
+      </c>
+      <c r="AI3" s="77" t="s">
+        <v>574</v>
+      </c>
+      <c r="AJ3" s="77" t="s">
+        <v>575</v>
+      </c>
+      <c r="AK3" s="77" t="s">
+        <v>576</v>
+      </c>
+      <c r="AL3" s="55" t="s">
         <v>88</v>
       </c>
-      <c r="AH3" s="55" t="s">
+      <c r="AM3" s="55" t="s">
         <v>32</v>
       </c>
-      <c r="AI3" s="55" t="s">
+      <c r="AN3" s="55" t="s">
         <v>167</v>
       </c>
-      <c r="AJ3" s="55" t="s">
+      <c r="AO3" s="55" t="s">
         <v>392</v>
       </c>
-      <c r="AK3" s="55" t="s">
+      <c r="AP3" s="55" t="s">
         <v>540</v>
       </c>
-      <c r="AL3" s="55" t="s">
+      <c r="AQ3" s="55" t="s">
         <v>541</v>
       </c>
-      <c r="AM3" s="55" t="s">
+      <c r="AR3" s="55" t="s">
         <v>330</v>
       </c>
-      <c r="AN3" s="56" t="s">
+      <c r="AS3" s="56" t="s">
         <v>67</v>
       </c>
-      <c r="AO3" s="56" t="s">
+      <c r="AT3" s="56" t="s">
         <v>68</v>
       </c>
-      <c r="AP3" s="56" t="s">
+      <c r="AU3" s="56" t="s">
         <v>33</v>
       </c>
-      <c r="AQ3" s="56" t="s">
+      <c r="AV3" s="56" t="s">
         <v>7</v>
       </c>
-      <c r="AR3" s="56" t="s">
+      <c r="AW3" s="56" t="s">
         <v>172</v>
       </c>
-      <c r="AS3" s="57" t="s">
+      <c r="AX3" s="57" t="s">
         <v>496</v>
       </c>
-      <c r="AT3" s="57" t="s">
+      <c r="AY3" s="57" t="s">
         <v>488</v>
       </c>
-      <c r="AU3" s="57" t="s">
+      <c r="AZ3" s="57" t="s">
         <v>490</v>
       </c>
-      <c r="AV3" s="57" t="s">
+      <c r="BA3" s="57" t="s">
         <v>485</v>
       </c>
-      <c r="AW3" s="57" t="s">
+      <c r="BB3" s="57" t="s">
         <v>492</v>
       </c>
-      <c r="AX3" s="52" t="s">
+      <c r="BC3" s="52" t="s">
         <v>20</v>
       </c>
-      <c r="AY3" s="52" t="s">
+      <c r="BD3" s="52" t="s">
         <v>21</v>
       </c>
-      <c r="AZ3" s="52" t="s">
+      <c r="BE3" s="52" t="s">
         <v>22</v>
       </c>
-      <c r="BA3" s="52" t="s">
+      <c r="BF3" s="52" t="s">
         <v>23</v>
       </c>
-      <c r="BB3" s="52" t="s">
+      <c r="BG3" s="52" t="s">
         <v>382</v>
       </c>
     </row>
-    <row r="4" spans="1:54" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:59" x14ac:dyDescent="0.15">
       <c r="A4" s="58">
         <v>42110001</v>
       </c>
@@ -9331,18 +9731,18 @@
       <c r="Y4" s="60"/>
       <c r="Z4" s="60"/>
       <c r="AA4" s="60"/>
-      <c r="AX4" s="44">
+      <c r="BC4" s="44">
         <v>-30</v>
       </c>
-      <c r="AZ4" s="44">
+      <c r="BE4" s="44">
         <v>100</v>
       </c>
-      <c r="BA4" s="44">
+      <c r="BF4" s="44">
         <v>100</v>
       </c>
-      <c r="BB4" s="61"/>
-    </row>
-    <row r="5" spans="1:54" x14ac:dyDescent="0.15">
+      <c r="BG4" s="61"/>
+    </row>
+    <row r="5" spans="1:59" x14ac:dyDescent="0.15">
       <c r="A5" s="58">
         <v>42110002</v>
       </c>
@@ -9384,15 +9784,15 @@
       <c r="Y5" s="60"/>
       <c r="Z5" s="60"/>
       <c r="AA5" s="60"/>
-      <c r="AX5" s="44">
+      <c r="BC5" s="44">
         <v>-20</v>
       </c>
-      <c r="AY5" s="44">
+      <c r="BD5" s="44">
         <v>100</v>
       </c>
-      <c r="BB5" s="61"/>
-    </row>
-    <row r="6" spans="1:54" x14ac:dyDescent="0.15">
+      <c r="BG5" s="61"/>
+    </row>
+    <row r="6" spans="1:59" x14ac:dyDescent="0.15">
       <c r="A6" s="58">
         <v>42110003</v>
       </c>
@@ -9434,9 +9834,9 @@
       <c r="Y6" s="60"/>
       <c r="Z6" s="60"/>
       <c r="AA6" s="60"/>
-      <c r="BB6" s="61"/>
-    </row>
-    <row r="7" spans="1:54" x14ac:dyDescent="0.15">
+      <c r="BG6" s="61"/>
+    </row>
+    <row r="7" spans="1:59" x14ac:dyDescent="0.15">
       <c r="A7" s="58">
         <v>42110004</v>
       </c>
@@ -9469,9 +9869,9 @@
       <c r="O7" s="59"/>
       <c r="P7" s="59"/>
       <c r="R7" s="59"/>
-      <c r="BB7" s="61"/>
-    </row>
-    <row r="8" spans="1:54" x14ac:dyDescent="0.15">
+      <c r="BG7" s="61"/>
+    </row>
+    <row r="8" spans="1:59" x14ac:dyDescent="0.15">
       <c r="A8" s="58">
         <v>42110005</v>
       </c>
@@ -9513,9 +9913,9 @@
       <c r="Y8" s="60"/>
       <c r="Z8" s="60"/>
       <c r="AA8" s="60"/>
-      <c r="BB8" s="61"/>
-    </row>
-    <row r="9" spans="1:54" x14ac:dyDescent="0.15">
+      <c r="BG8" s="61"/>
+    </row>
+    <row r="9" spans="1:59" x14ac:dyDescent="0.15">
       <c r="A9" s="58">
         <v>42110101</v>
       </c>
@@ -9559,9 +9959,9 @@
       </c>
       <c r="Z9" s="60"/>
       <c r="AA9" s="60"/>
-      <c r="BB9" s="61"/>
-    </row>
-    <row r="10" spans="1:54" x14ac:dyDescent="0.15">
+      <c r="BG9" s="61"/>
+    </row>
+    <row r="10" spans="1:59" x14ac:dyDescent="0.15">
       <c r="A10" s="58">
         <v>42110102</v>
       </c>
@@ -9605,9 +10005,9 @@
       </c>
       <c r="Z10" s="60"/>
       <c r="AA10" s="60"/>
-      <c r="BB10" s="61"/>
-    </row>
-    <row r="11" spans="1:54" x14ac:dyDescent="0.15">
+      <c r="BG10" s="61"/>
+    </row>
+    <row r="11" spans="1:59" x14ac:dyDescent="0.15">
       <c r="A11" s="58">
         <v>42110103</v>
       </c>
@@ -9651,11 +10051,11 @@
       </c>
       <c r="Z11" s="71"/>
       <c r="AA11" s="71"/>
-      <c r="AK11" s="72"/>
-      <c r="AL11" s="72"/>
-      <c r="BB11" s="73"/>
-    </row>
-    <row r="12" spans="1:54" x14ac:dyDescent="0.15">
+      <c r="AP11" s="72"/>
+      <c r="AQ11" s="72"/>
+      <c r="BG11" s="73"/>
+    </row>
+    <row r="12" spans="1:59" x14ac:dyDescent="0.15">
       <c r="A12" s="44">
         <v>42120001</v>
       </c>
@@ -9697,9 +10097,9 @@
       <c r="Y12" s="60"/>
       <c r="Z12" s="60"/>
       <c r="AA12" s="60"/>
-      <c r="BB12" s="61"/>
-    </row>
-    <row r="13" spans="1:54" x14ac:dyDescent="0.15">
+      <c r="BG12" s="61"/>
+    </row>
+    <row r="13" spans="1:59" x14ac:dyDescent="0.15">
       <c r="A13" s="44">
         <v>42120002</v>
       </c>
@@ -9743,12 +10143,12 @@
       <c r="Y13" s="60"/>
       <c r="Z13" s="60"/>
       <c r="AA13" s="60"/>
-      <c r="AM13" s="44" t="s">
+      <c r="AR13" s="44" t="s">
         <v>331</v>
       </c>
-      <c r="BB13" s="61"/>
-    </row>
-    <row r="14" spans="1:54" x14ac:dyDescent="0.15">
+      <c r="BG13" s="61"/>
+    </row>
+    <row r="14" spans="1:59" x14ac:dyDescent="0.15">
       <c r="A14" s="44">
         <v>42120003</v>
       </c>
@@ -9789,9 +10189,9 @@
       <c r="Y14" s="60"/>
       <c r="Z14" s="60"/>
       <c r="AA14" s="60"/>
-      <c r="BB14" s="61"/>
-    </row>
-    <row r="15" spans="1:54" x14ac:dyDescent="0.15">
+      <c r="BG14" s="61"/>
+    </row>
+    <row r="15" spans="1:59" x14ac:dyDescent="0.15">
       <c r="A15" s="44">
         <v>42120004</v>
       </c>
@@ -9837,12 +10237,12 @@
       <c r="Y15" s="60"/>
       <c r="Z15" s="60"/>
       <c r="AA15" s="60"/>
-      <c r="AM15" s="44" t="s">
+      <c r="AR15" s="44" t="s">
         <v>332</v>
       </c>
-      <c r="BB15" s="61"/>
-    </row>
-    <row r="16" spans="1:54" x14ac:dyDescent="0.15">
+      <c r="BG15" s="61"/>
+    </row>
+    <row r="16" spans="1:59" x14ac:dyDescent="0.15">
       <c r="A16" s="44">
         <v>42120005</v>
       </c>
@@ -9885,9 +10285,9 @@
       </c>
       <c r="Z16" s="60"/>
       <c r="AA16" s="60"/>
-      <c r="BB16" s="61"/>
-    </row>
-    <row r="17" spans="1:54" x14ac:dyDescent="0.15">
+      <c r="BG16" s="61"/>
+    </row>
+    <row r="17" spans="1:59" x14ac:dyDescent="0.15">
       <c r="A17" s="44">
         <v>42120006</v>
       </c>
@@ -9932,9 +10332,9 @@
       <c r="Y17" s="60"/>
       <c r="Z17" s="60"/>
       <c r="AA17" s="60"/>
-      <c r="BB17" s="61"/>
-    </row>
-    <row r="18" spans="1:54" x14ac:dyDescent="0.15">
+      <c r="BG17" s="61"/>
+    </row>
+    <row r="18" spans="1:59" x14ac:dyDescent="0.15">
       <c r="A18" s="44">
         <v>42120007</v>
       </c>
@@ -9976,9 +10376,9 @@
       <c r="Y18" s="60"/>
       <c r="Z18" s="60"/>
       <c r="AA18" s="60"/>
-      <c r="BB18" s="61"/>
-    </row>
-    <row r="19" spans="1:54" x14ac:dyDescent="0.15">
+      <c r="BG18" s="61"/>
+    </row>
+    <row r="19" spans="1:59" x14ac:dyDescent="0.15">
       <c r="A19" s="44">
         <v>42120008</v>
       </c>
@@ -10020,9 +10420,9 @@
       <c r="Y19" s="60"/>
       <c r="Z19" s="60"/>
       <c r="AA19" s="60"/>
-      <c r="BB19" s="61"/>
-    </row>
-    <row r="20" spans="1:54" x14ac:dyDescent="0.15">
+      <c r="BG19" s="61"/>
+    </row>
+    <row r="20" spans="1:59" x14ac:dyDescent="0.15">
       <c r="A20" s="44">
         <v>42120009</v>
       </c>
@@ -10064,9 +10464,9 @@
       <c r="Y20" s="60"/>
       <c r="Z20" s="60"/>
       <c r="AA20" s="60"/>
-      <c r="BB20" s="61"/>
-    </row>
-    <row r="21" spans="1:54" x14ac:dyDescent="0.15">
+      <c r="BG20" s="61"/>
+    </row>
+    <row r="21" spans="1:59" x14ac:dyDescent="0.15">
       <c r="A21" s="44">
         <v>42120010</v>
       </c>
@@ -10108,9 +10508,9 @@
       <c r="Y21" s="60"/>
       <c r="Z21" s="60"/>
       <c r="AA21" s="60"/>
-      <c r="BB21" s="61"/>
-    </row>
-    <row r="22" spans="1:54" x14ac:dyDescent="0.15">
+      <c r="BG21" s="61"/>
+    </row>
+    <row r="22" spans="1:59" x14ac:dyDescent="0.15">
       <c r="A22" s="44">
         <v>42120011</v>
       </c>
@@ -10152,9 +10552,9 @@
       <c r="Y22" s="60"/>
       <c r="Z22" s="60"/>
       <c r="AA22" s="60"/>
-      <c r="BB22" s="61"/>
-    </row>
-    <row r="23" spans="1:54" x14ac:dyDescent="0.15">
+      <c r="BG22" s="61"/>
+    </row>
+    <row r="23" spans="1:59" x14ac:dyDescent="0.15">
       <c r="A23" s="44">
         <v>42120013</v>
       </c>
@@ -10196,9 +10596,9 @@
       <c r="Y23" s="60"/>
       <c r="Z23" s="60"/>
       <c r="AA23" s="60"/>
-      <c r="BB23" s="61"/>
-    </row>
-    <row r="24" spans="1:54" x14ac:dyDescent="0.15">
+      <c r="BG23" s="61"/>
+    </row>
+    <row r="24" spans="1:59" x14ac:dyDescent="0.15">
       <c r="A24" s="44">
         <v>42120014</v>
       </c>
@@ -10240,9 +10640,9 @@
       <c r="Y24" s="60"/>
       <c r="Z24" s="60"/>
       <c r="AA24" s="60"/>
-      <c r="BB24" s="61"/>
-    </row>
-    <row r="25" spans="1:54" x14ac:dyDescent="0.15">
+      <c r="BG24" s="61"/>
+    </row>
+    <row r="25" spans="1:59" x14ac:dyDescent="0.15">
       <c r="A25" s="44">
         <v>42120015</v>
       </c>
@@ -10284,9 +10684,9 @@
       <c r="Y25" s="60"/>
       <c r="Z25" s="60"/>
       <c r="AA25" s="60"/>
-      <c r="BB25" s="61"/>
-    </row>
-    <row r="26" spans="1:54" x14ac:dyDescent="0.15">
+      <c r="BG25" s="61"/>
+    </row>
+    <row r="26" spans="1:59" x14ac:dyDescent="0.15">
       <c r="A26" s="44">
         <v>42120016</v>
       </c>
@@ -10325,9 +10725,9 @@
       <c r="Y26" s="60"/>
       <c r="Z26" s="60"/>
       <c r="AA26" s="60"/>
-      <c r="BB26" s="61"/>
-    </row>
-    <row r="27" spans="1:54" x14ac:dyDescent="0.15">
+      <c r="BG26" s="61"/>
+    </row>
+    <row r="27" spans="1:59" x14ac:dyDescent="0.15">
       <c r="A27" s="44">
         <v>42120017</v>
       </c>
@@ -10374,9 +10774,9 @@
       <c r="AF27" s="44">
         <v>30</v>
       </c>
-      <c r="BB27" s="61"/>
-    </row>
-    <row r="28" spans="1:54" x14ac:dyDescent="0.15">
+      <c r="BG27" s="61"/>
+    </row>
+    <row r="28" spans="1:59" x14ac:dyDescent="0.15">
       <c r="A28" s="44">
         <v>42120018</v>
       </c>
@@ -10423,9 +10823,9 @@
       <c r="AF28" s="44">
         <v>50</v>
       </c>
-      <c r="BB28" s="61"/>
-    </row>
-    <row r="29" spans="1:54" x14ac:dyDescent="0.15">
+      <c r="BG28" s="61"/>
+    </row>
+    <row r="29" spans="1:59" x14ac:dyDescent="0.15">
       <c r="A29" s="44">
         <v>42120019</v>
       </c>
@@ -10471,9 +10871,9 @@
       <c r="Y29" s="63"/>
       <c r="Z29" s="63"/>
       <c r="AA29" s="63"/>
-      <c r="BB29" s="61"/>
-    </row>
-    <row r="30" spans="1:54" x14ac:dyDescent="0.15">
+      <c r="BG29" s="61"/>
+    </row>
+    <row r="30" spans="1:59" x14ac:dyDescent="0.15">
       <c r="A30" s="44">
         <v>42130001</v>
       </c>
@@ -10517,11 +10917,11 @@
       <c r="Y30" s="71"/>
       <c r="Z30" s="71"/>
       <c r="AA30" s="71"/>
-      <c r="AK30" s="72"/>
-      <c r="AL30" s="72"/>
-      <c r="BB30" s="73"/>
-    </row>
-    <row r="31" spans="1:54" x14ac:dyDescent="0.15">
+      <c r="AP30" s="72"/>
+      <c r="AQ30" s="72"/>
+      <c r="BG30" s="73"/>
+    </row>
+    <row r="31" spans="1:59" x14ac:dyDescent="0.15">
       <c r="A31" s="44">
         <v>42130002</v>
       </c>
@@ -10565,9 +10965,9 @@
       <c r="Y31" s="60"/>
       <c r="Z31" s="60"/>
       <c r="AA31" s="60"/>
-      <c r="BB31" s="61"/>
-    </row>
-    <row r="32" spans="1:54" x14ac:dyDescent="0.15">
+      <c r="BG31" s="61"/>
+    </row>
+    <row r="32" spans="1:59" x14ac:dyDescent="0.15">
       <c r="A32" s="44">
         <v>42130003</v>
       </c>
@@ -10613,9 +11013,9 @@
       <c r="Y32" s="60"/>
       <c r="Z32" s="60"/>
       <c r="AA32" s="60"/>
-      <c r="BB32" s="61"/>
-    </row>
-    <row r="33" spans="1:54" x14ac:dyDescent="0.15">
+      <c r="BG32" s="61"/>
+    </row>
+    <row r="33" spans="1:59" x14ac:dyDescent="0.15">
       <c r="A33" s="44">
         <v>42130004</v>
       </c>
@@ -10667,15 +11067,15 @@
       <c r="AF33" s="44">
         <v>300</v>
       </c>
-      <c r="AP33" s="44">
+      <c r="AU33" s="44">
         <v>200</v>
       </c>
-      <c r="AQ33" s="44">
+      <c r="AV33" s="44">
         <v>200</v>
       </c>
-      <c r="BB33" s="61"/>
-    </row>
-    <row r="34" spans="1:54" x14ac:dyDescent="0.15">
+      <c r="BG33" s="61"/>
+    </row>
+    <row r="34" spans="1:59" x14ac:dyDescent="0.15">
       <c r="A34" s="44">
         <v>42130011</v>
       </c>
@@ -10719,9 +11119,9 @@
       <c r="Y34" s="60"/>
       <c r="Z34" s="60"/>
       <c r="AA34" s="60"/>
-      <c r="BB34" s="61"/>
-    </row>
-    <row r="35" spans="1:54" x14ac:dyDescent="0.15">
+      <c r="BG34" s="61"/>
+    </row>
+    <row r="35" spans="1:59" x14ac:dyDescent="0.15">
       <c r="A35" s="44">
         <v>42130021</v>
       </c>
@@ -10765,9 +11165,9 @@
       <c r="Y35" s="60"/>
       <c r="Z35" s="60"/>
       <c r="AA35" s="60"/>
-      <c r="BB35" s="61"/>
-    </row>
-    <row r="36" spans="1:54" x14ac:dyDescent="0.15">
+      <c r="BG35" s="61"/>
+    </row>
+    <row r="36" spans="1:59" x14ac:dyDescent="0.15">
       <c r="A36" s="44">
         <v>42130022</v>
       </c>
@@ -10811,9 +11211,9 @@
       <c r="Y36" s="60"/>
       <c r="Z36" s="60"/>
       <c r="AA36" s="60"/>
-      <c r="BB36" s="61"/>
-    </row>
-    <row r="37" spans="1:54" x14ac:dyDescent="0.15">
+      <c r="BG36" s="61"/>
+    </row>
+    <row r="37" spans="1:59" x14ac:dyDescent="0.15">
       <c r="A37" s="44">
         <v>42130023</v>
       </c>
@@ -10864,15 +11264,15 @@
       <c r="AF37" s="44">
         <v>300</v>
       </c>
-      <c r="AP37" s="44">
+      <c r="AU37" s="44">
         <v>200</v>
       </c>
-      <c r="AQ37" s="44">
+      <c r="AV37" s="44">
         <v>200</v>
       </c>
-      <c r="BB37" s="61"/>
-    </row>
-    <row r="38" spans="1:54" x14ac:dyDescent="0.15">
+      <c r="BG37" s="61"/>
+    </row>
+    <row r="38" spans="1:59" x14ac:dyDescent="0.15">
       <c r="A38" s="44">
         <v>42130031</v>
       </c>
@@ -10910,37 +11310,37 @@
       <c r="U38" s="76">
         <v>18000301</v>
       </c>
-      <c r="BB38" s="61"/>
+      <c r="BG38" s="61"/>
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
-  <conditionalFormatting sqref="J38:Q38 D4:Q10 J11:Q11 R4:BB38 D12:Q29 J30:Q30 D31:Q37">
-    <cfRule type="containsBlanks" dxfId="6" priority="10">
+  <conditionalFormatting sqref="J38:Q38 D4:Q10 J11:Q11 R4:BG38 D12:Q29 J30:Q30 D31:Q37">
+    <cfRule type="containsBlanks" dxfId="10" priority="10">
       <formula>LEN(TRIM(D4))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D38:I38">
-    <cfRule type="containsBlanks" dxfId="5" priority="7">
+    <cfRule type="containsBlanks" dxfId="9" priority="7">
       <formula>LEN(TRIM(D38))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D11:I11">
-    <cfRule type="containsBlanks" dxfId="4" priority="5">
+    <cfRule type="containsBlanks" dxfId="8" priority="5">
       <formula>LEN(TRIM(D11))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D30:E30 I30 G30">
-    <cfRule type="containsBlanks" dxfId="3" priority="4">
+    <cfRule type="containsBlanks" dxfId="7" priority="4">
       <formula>LEN(TRIM(D30))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H30">
-    <cfRule type="containsBlanks" dxfId="2" priority="3">
+    <cfRule type="containsBlanks" dxfId="6" priority="3">
       <formula>LEN(TRIM(H30))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F30">
-    <cfRule type="containsBlanks" dxfId="0" priority="1">
+    <cfRule type="containsBlanks" dxfId="5" priority="1">
       <formula>LEN(TRIM(F30))=0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
finish the trap event
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/SceneQuest.xlsx
+++ b/ConfigData/Xlsx/SceneQuest.xlsx
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1210" uniqueCount="656">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1249" uniqueCount="666">
   <si>
     <t>int</t>
     <phoneticPr fontId="18" type="noConversion"/>
@@ -2570,6 +2570,46 @@
   </si>
   <si>
     <t>agi</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>trapcommon</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>str</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>agi</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>perc</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>intl</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>endu</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>true</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>trapbarrier</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>trapspear</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>trapdrop</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -3757,82 +3797,13 @@
     <cellStyle name="着色 6" xfId="38" builtinId="49" customBuiltin="1"/>
     <cellStyle name="注释" xfId="15" builtinId="10" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="68">
+  <dxfs count="69">
     <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="宋体"/>
-        <family val="2"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="宋体"/>
-        <family val="2"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="宋体"/>
-        <family val="2"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="宋体"/>
-        <family val="2"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <fill>
@@ -3915,6 +3886,18 @@
         <charset val="134"/>
         <scheme val="minor"/>
       </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color theme="4"/>
+        </right>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -3991,18 +3974,6 @@
         <charset val="134"/>
         <scheme val="minor"/>
       </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="thin">
-          <color theme="4"/>
-        </right>
-        <top style="thin">
-          <color theme="4"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
     </dxf>
     <dxf>
       <font>
@@ -4613,6 +4584,82 @@
       </font>
     </dxf>
     <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
     <dxf>
@@ -4694,7 +4741,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="表3" displayName="表3" ref="A3:BN107" totalsRowShown="0" headerRowDxfId="67">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="表3" displayName="表3" ref="A3:BN107" totalsRowShown="0" headerRowDxfId="68">
   <autoFilter ref="A3:BN107" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <sortState ref="A4:BN107">
     <sortCondition ref="A3:A107"/>
@@ -4708,48 +4755,48 @@
     <tableColumn id="24" xr3:uid="{00000000-0010-0000-0000-000018000000}" name="Ename"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Figue"/>
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Script"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="TriggerMulti" dataDxfId="66"/>
-    <tableColumn id="40" xr3:uid="{00000000-0010-0000-0000-000028000000}" name="Catalog" dataDxfId="65"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="TriggerMulti" dataDxfId="67"/>
+    <tableColumn id="40" xr3:uid="{00000000-0010-0000-0000-000028000000}" name="Catalog" dataDxfId="66"/>
     <tableColumn id="29" xr3:uid="{6EBFF016-E9F0-4AC6-926F-95D396DBD009}" name="Catalog2"/>
-    <tableColumn id="35" xr3:uid="{00000000-0010-0000-0000-000023000000}" name="TriggerHourBegin" dataDxfId="64"/>
-    <tableColumn id="34" xr3:uid="{00000000-0010-0000-0000-000022000000}" name="TriggerHourEnd" dataDxfId="63"/>
-    <tableColumn id="36" xr3:uid="{00000000-0010-0000-0000-000024000000}" name="TriggerQuestNotReceive" dataDxfId="62"/>
-    <tableColumn id="37" xr3:uid="{00000000-0010-0000-0000-000025000000}" name="TriggerQuestReceived" dataDxfId="61"/>
-    <tableColumn id="38" xr3:uid="{00000000-0010-0000-0000-000026000000}" name="TriggerQuestFinished" dataDxfId="60"/>
-    <tableColumn id="39" xr3:uid="{00000000-0010-0000-0000-000027000000}" name="TriggerRate" dataDxfId="59"/>
-    <tableColumn id="62" xr3:uid="{151FC2E4-8457-4218-9D14-8ADCD08A1BD0}" name="TriggerOnceInDungeon" dataDxfId="58"/>
+    <tableColumn id="35" xr3:uid="{00000000-0010-0000-0000-000023000000}" name="TriggerHourBegin" dataDxfId="65"/>
+    <tableColumn id="34" xr3:uid="{00000000-0010-0000-0000-000022000000}" name="TriggerHourEnd" dataDxfId="64"/>
+    <tableColumn id="36" xr3:uid="{00000000-0010-0000-0000-000024000000}" name="TriggerQuestNotReceive" dataDxfId="63"/>
+    <tableColumn id="37" xr3:uid="{00000000-0010-0000-0000-000025000000}" name="TriggerQuestReceived" dataDxfId="62"/>
+    <tableColumn id="38" xr3:uid="{00000000-0010-0000-0000-000026000000}" name="TriggerQuestFinished" dataDxfId="61"/>
+    <tableColumn id="39" xr3:uid="{00000000-0010-0000-0000-000027000000}" name="TriggerRate" dataDxfId="60"/>
+    <tableColumn id="62" xr3:uid="{151FC2E4-8457-4218-9D14-8ADCD08A1BD0}" name="TriggerOnceInDungeon" dataDxfId="59"/>
     <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="EnemyName"/>
-    <tableColumn id="51" xr3:uid="{00000000-0010-0000-0000-000033000000}" name="CanBribe" dataDxfId="57"/>
+    <tableColumn id="51" xr3:uid="{00000000-0010-0000-0000-000033000000}" name="CanBribe" dataDxfId="58"/>
     <tableColumn id="32" xr3:uid="{00000000-0010-0000-0000-000020000000}" name="SceneId"/>
-    <tableColumn id="54" xr3:uid="{00000000-0010-0000-0000-000036000000}" name="DungeonId" dataDxfId="56"/>
+    <tableColumn id="54" xr3:uid="{00000000-0010-0000-0000-000036000000}" name="DungeonId" dataDxfId="57"/>
     <tableColumn id="50" xr3:uid="{00000000-0010-0000-0000-000032000000}" name="CheckQuest"/>
     <tableColumn id="27" xr3:uid="{00000000-0010-0000-0000-00001B000000}" name="NextQuest"/>
     <tableColumn id="44" xr3:uid="{00000000-0010-0000-0000-00002C000000}" name="HiddenRoomQuest"/>
     <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="ShopName"/>
     <tableColumn id="41" xr3:uid="{00000000-0010-0000-0000-000029000000}" name="MiniGameId"/>
     <tableColumn id="43" xr3:uid="{00000000-0010-0000-0000-00002B000000}" name="PayKey"/>
-    <tableColumn id="63" xr3:uid="{3265A47D-A027-4E5A-9D90-2C146F029798}" name="TestType1" dataDxfId="16"/>
-    <tableColumn id="64" xr3:uid="{76E4BAA7-7701-49AB-87E9-F08C013C3E37}" name="TestBias1" dataDxfId="15"/>
-    <tableColumn id="65" xr3:uid="{CC1108D3-C833-4D8A-A932-A8B9CEB92600}" name="TestType2" dataDxfId="14"/>
-    <tableColumn id="66" xr3:uid="{06E3173E-47B8-4A21-A1BD-D49F6A0F9F9F}" name="TestBias2" dataDxfId="13"/>
+    <tableColumn id="63" xr3:uid="{3265A47D-A027-4E5A-9D90-2C146F029798}" name="TestType1" dataDxfId="56"/>
+    <tableColumn id="64" xr3:uid="{76E4BAA7-7701-49AB-87E9-F08C013C3E37}" name="TestBias1" dataDxfId="55"/>
+    <tableColumn id="65" xr3:uid="{CC1108D3-C833-4D8A-A932-A8B9CEB92600}" name="TestType2" dataDxfId="54"/>
+    <tableColumn id="66" xr3:uid="{06E3173E-47B8-4A21-A1BD-D49F6A0F9F9F}" name="TestBias2" dataDxfId="53"/>
     <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="RewardGold"/>
     <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="RewardFood"/>
     <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="RewardHealth"/>
     <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="RewardMental"/>
     <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="RewardExp"/>
-    <tableColumn id="56" xr3:uid="{00000000-0010-0000-0000-000038000000}" name="RewardStr" dataDxfId="55"/>
-    <tableColumn id="57" xr3:uid="{00000000-0010-0000-0000-000039000000}" name="RewardAgi" dataDxfId="54"/>
-    <tableColumn id="58" xr3:uid="{00000000-0010-0000-0000-00003A000000}" name="RewardIntl" dataDxfId="53"/>
-    <tableColumn id="59" xr3:uid="{00000000-0010-0000-0000-00003B000000}" name="RewardPerc" dataDxfId="52"/>
-    <tableColumn id="60" xr3:uid="{00000000-0010-0000-0000-00003C000000}" name="RewardEndu" dataDxfId="51"/>
+    <tableColumn id="56" xr3:uid="{00000000-0010-0000-0000-000038000000}" name="RewardStr" dataDxfId="52"/>
+    <tableColumn id="57" xr3:uid="{00000000-0010-0000-0000-000039000000}" name="RewardAgi" dataDxfId="51"/>
+    <tableColumn id="58" xr3:uid="{00000000-0010-0000-0000-00003A000000}" name="RewardIntl" dataDxfId="50"/>
+    <tableColumn id="59" xr3:uid="{00000000-0010-0000-0000-00003B000000}" name="RewardPerc" dataDxfId="49"/>
+    <tableColumn id="60" xr3:uid="{00000000-0010-0000-0000-00003C000000}" name="RewardEndu" dataDxfId="48"/>
     <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="RewardItem"/>
     <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="RewardDrop"/>
-    <tableColumn id="55" xr3:uid="{66604B07-BEB8-4B96-990A-AF48EE1D3850}" name="DungeonItemId" dataDxfId="50"/>
-    <tableColumn id="61" xr3:uid="{6B318330-F7A2-4EDC-8ED9-B4CF6FD1A4A3}" name="DungeonItemCount" dataDxfId="49"/>
+    <tableColumn id="55" xr3:uid="{66604B07-BEB8-4B96-990A-AF48EE1D3850}" name="DungeonItemId" dataDxfId="47"/>
+    <tableColumn id="61" xr3:uid="{6B318330-F7A2-4EDC-8ED9-B4CF6FD1A4A3}" name="DungeonItemCount" dataDxfId="46"/>
     <tableColumn id="30" xr3:uid="{00000000-0010-0000-0000-00001E000000}" name="RewardBlessLevel"/>
     <tableColumn id="42" xr3:uid="{00000000-0010-0000-0000-00002A000000}" name="RewardBlessId"/>
-    <tableColumn id="52" xr3:uid="{00000000-0010-0000-0000-000034000000}" name="RewardResId" dataDxfId="48"/>
-    <tableColumn id="53" xr3:uid="{00000000-0010-0000-0000-000035000000}" name="RewardResAmount" dataDxfId="47"/>
+    <tableColumn id="52" xr3:uid="{00000000-0010-0000-0000-000034000000}" name="RewardResId" dataDxfId="45"/>
+    <tableColumn id="53" xr3:uid="{00000000-0010-0000-0000-000035000000}" name="RewardResAmount" dataDxfId="44"/>
     <tableColumn id="26" xr3:uid="{00000000-0010-0000-0000-00001A000000}" name="UnlockRival"/>
     <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="PunishGold"/>
     <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="PunishFood"/>
@@ -4772,7 +4819,7 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="表3_5" displayName="表3_5" ref="A3:BN39" totalsRowShown="0" headerRowDxfId="46">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="表3_5" displayName="表3_5" ref="A3:BN39" totalsRowShown="0" headerRowDxfId="43">
   <autoFilter ref="A3:BN39" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
   <sortState ref="A4:AR6">
     <sortCondition ref="A3:A6"/>
@@ -4780,54 +4827,54 @@
   <tableColumns count="66">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Id"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Name"/>
-    <tableColumn id="27" xr3:uid="{00000000-0010-0000-0100-00001B000000}" name="Type" dataDxfId="45"/>
+    <tableColumn id="27" xr3:uid="{00000000-0010-0000-0100-00001B000000}" name="Type" dataDxfId="42"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Level"/>
     <tableColumn id="25" xr3:uid="{00000000-0010-0000-0100-000019000000}" name="Danger"/>
     <tableColumn id="24" xr3:uid="{00000000-0010-0000-0100-000018000000}" name="Ename"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Figue"/>
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="Script"/>
     <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="TriggerMulti"/>
-    <tableColumn id="40" xr3:uid="{00000000-0010-0000-0100-000028000000}" name="Catalog" dataDxfId="44"/>
-    <tableColumn id="29" xr3:uid="{7A22C88C-F68C-4686-BCB4-5D43AB534572}" name="Catalog2" dataDxfId="43"/>
-    <tableColumn id="35" xr3:uid="{00000000-0010-0000-0100-000023000000}" name="TriggerHourBegin" dataDxfId="42"/>
-    <tableColumn id="34" xr3:uid="{00000000-0010-0000-0100-000022000000}" name="TriggerHourEnd" dataDxfId="41"/>
-    <tableColumn id="37" xr3:uid="{00000000-0010-0000-0100-000025000000}" name="TriggerQuestNotReceive" dataDxfId="40"/>
-    <tableColumn id="38" xr3:uid="{00000000-0010-0000-0100-000026000000}" name="TriggerQuestReceived" dataDxfId="39"/>
-    <tableColumn id="36" xr3:uid="{00000000-0010-0000-0100-000024000000}" name="TriggerQuestFinished" dataDxfId="38"/>
-    <tableColumn id="39" xr3:uid="{00000000-0010-0000-0100-000027000000}" name="TriggerRate" dataDxfId="37"/>
-    <tableColumn id="62" xr3:uid="{5CFB435A-0FEA-4777-A286-DA4BED0A22C8}" name="TriggerOnceInDungeon" dataDxfId="36"/>
+    <tableColumn id="40" xr3:uid="{00000000-0010-0000-0100-000028000000}" name="Catalog" dataDxfId="41"/>
+    <tableColumn id="29" xr3:uid="{7A22C88C-F68C-4686-BCB4-5D43AB534572}" name="Catalog2" dataDxfId="40"/>
+    <tableColumn id="35" xr3:uid="{00000000-0010-0000-0100-000023000000}" name="TriggerHourBegin" dataDxfId="39"/>
+    <tableColumn id="34" xr3:uid="{00000000-0010-0000-0100-000022000000}" name="TriggerHourEnd" dataDxfId="38"/>
+    <tableColumn id="37" xr3:uid="{00000000-0010-0000-0100-000025000000}" name="TriggerQuestNotReceive" dataDxfId="37"/>
+    <tableColumn id="38" xr3:uid="{00000000-0010-0000-0100-000026000000}" name="TriggerQuestReceived" dataDxfId="36"/>
+    <tableColumn id="36" xr3:uid="{00000000-0010-0000-0100-000024000000}" name="TriggerQuestFinished" dataDxfId="35"/>
+    <tableColumn id="39" xr3:uid="{00000000-0010-0000-0100-000027000000}" name="TriggerRate" dataDxfId="34"/>
+    <tableColumn id="62" xr3:uid="{5CFB435A-0FEA-4777-A286-DA4BED0A22C8}" name="TriggerOnceInDungeon" dataDxfId="33"/>
     <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="EnemyName"/>
-    <tableColumn id="51" xr3:uid="{00000000-0010-0000-0100-000033000000}" name="CanBribe" dataDxfId="35"/>
-    <tableColumn id="32" xr3:uid="{00000000-0010-0000-0100-000020000000}" name="SceneId" dataDxfId="34"/>
-    <tableColumn id="54" xr3:uid="{00000000-0010-0000-0100-000036000000}" name="DungeonId" dataDxfId="33"/>
-    <tableColumn id="50" xr3:uid="{00000000-0010-0000-0100-000032000000}" name="CheckQuest" dataDxfId="32"/>
-    <tableColumn id="28" xr3:uid="{00000000-0010-0000-0100-00001C000000}" name="NextQuest" dataDxfId="31"/>
-    <tableColumn id="44" xr3:uid="{00000000-0010-0000-0100-00002C000000}" name="HiddenRoomQuest" dataDxfId="30"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="ShopName" dataDxfId="29"/>
-    <tableColumn id="41" xr3:uid="{00000000-0010-0000-0100-000029000000}" name="MiniGameId" dataDxfId="28"/>
-    <tableColumn id="43" xr3:uid="{00000000-0010-0000-0100-00002B000000}" name="PayKey" dataDxfId="27"/>
-    <tableColumn id="63" xr3:uid="{A0E937E2-FC67-48CB-819B-04EB181C6AB2}" name="TestType1" dataDxfId="3"/>
-    <tableColumn id="64" xr3:uid="{B1B890BD-85C7-4099-BCA8-5A07C6BEF746}" name="TestBias1" dataDxfId="2"/>
-    <tableColumn id="65" xr3:uid="{1647E8EA-3DDE-49E6-B212-9302181F6C2E}" name="TestType2" dataDxfId="1"/>
-    <tableColumn id="66" xr3:uid="{2598FD95-5FD4-4C25-BB8C-D897F7496DE0}" name="TestBias2" dataDxfId="0"/>
+    <tableColumn id="51" xr3:uid="{00000000-0010-0000-0100-000033000000}" name="CanBribe" dataDxfId="32"/>
+    <tableColumn id="32" xr3:uid="{00000000-0010-0000-0100-000020000000}" name="SceneId" dataDxfId="31"/>
+    <tableColumn id="54" xr3:uid="{00000000-0010-0000-0100-000036000000}" name="DungeonId" dataDxfId="30"/>
+    <tableColumn id="50" xr3:uid="{00000000-0010-0000-0100-000032000000}" name="CheckQuest" dataDxfId="29"/>
+    <tableColumn id="28" xr3:uid="{00000000-0010-0000-0100-00001C000000}" name="NextQuest" dataDxfId="28"/>
+    <tableColumn id="44" xr3:uid="{00000000-0010-0000-0100-00002C000000}" name="HiddenRoomQuest" dataDxfId="27"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="ShopName" dataDxfId="26"/>
+    <tableColumn id="41" xr3:uid="{00000000-0010-0000-0100-000029000000}" name="MiniGameId" dataDxfId="25"/>
+    <tableColumn id="43" xr3:uid="{00000000-0010-0000-0100-00002B000000}" name="PayKey" dataDxfId="24"/>
+    <tableColumn id="63" xr3:uid="{A0E937E2-FC67-48CB-819B-04EB181C6AB2}" name="TestType1" dataDxfId="23"/>
+    <tableColumn id="64" xr3:uid="{B1B890BD-85C7-4099-BCA8-5A07C6BEF746}" name="TestBias1" dataDxfId="22"/>
+    <tableColumn id="65" xr3:uid="{1647E8EA-3DDE-49E6-B212-9302181F6C2E}" name="TestType2" dataDxfId="21"/>
+    <tableColumn id="66" xr3:uid="{2598FD95-5FD4-4C25-BB8C-D897F7496DE0}" name="TestBias2" dataDxfId="20"/>
     <tableColumn id="9" xr3:uid="{00000000-0010-0000-0100-000009000000}" name="RewardGold"/>
     <tableColumn id="10" xr3:uid="{00000000-0010-0000-0100-00000A000000}" name="RewardFood"/>
     <tableColumn id="11" xr3:uid="{00000000-0010-0000-0100-00000B000000}" name="RewardHealth"/>
     <tableColumn id="12" xr3:uid="{00000000-0010-0000-0100-00000C000000}" name="RewardMental"/>
     <tableColumn id="13" xr3:uid="{00000000-0010-0000-0100-00000D000000}" name="RewardExp"/>
-    <tableColumn id="55" xr3:uid="{00000000-0010-0000-0100-000037000000}" name="RewardStr" dataDxfId="26"/>
-    <tableColumn id="56" xr3:uid="{00000000-0010-0000-0100-000038000000}" name="RewardAgi" dataDxfId="25"/>
-    <tableColumn id="57" xr3:uid="{00000000-0010-0000-0100-000039000000}" name="RewardIntl" dataDxfId="24"/>
-    <tableColumn id="58" xr3:uid="{00000000-0010-0000-0100-00003A000000}" name="RewardPerc" dataDxfId="23"/>
-    <tableColumn id="59" xr3:uid="{00000000-0010-0000-0100-00003B000000}" name="RewardEndu" dataDxfId="22"/>
+    <tableColumn id="55" xr3:uid="{00000000-0010-0000-0100-000037000000}" name="RewardStr" dataDxfId="19"/>
+    <tableColumn id="56" xr3:uid="{00000000-0010-0000-0100-000038000000}" name="RewardAgi" dataDxfId="18"/>
+    <tableColumn id="57" xr3:uid="{00000000-0010-0000-0100-000039000000}" name="RewardIntl" dataDxfId="17"/>
+    <tableColumn id="58" xr3:uid="{00000000-0010-0000-0100-00003A000000}" name="RewardPerc" dataDxfId="16"/>
+    <tableColumn id="59" xr3:uid="{00000000-0010-0000-0100-00003B000000}" name="RewardEndu" dataDxfId="15"/>
     <tableColumn id="14" xr3:uid="{00000000-0010-0000-0100-00000E000000}" name="RewardItem"/>
     <tableColumn id="15" xr3:uid="{00000000-0010-0000-0100-00000F000000}" name="RewardDrop"/>
-    <tableColumn id="60" xr3:uid="{8E772862-4F57-4995-B4CB-741582410CBE}" name="DungeonItemId" dataDxfId="21"/>
-    <tableColumn id="61" xr3:uid="{F97F64E4-CEE6-4F78-847D-4CAA7CE8E3EE}" name="DungeonItemCount" dataDxfId="20"/>
+    <tableColumn id="60" xr3:uid="{8E772862-4F57-4995-B4CB-741582410CBE}" name="DungeonItemId" dataDxfId="14"/>
+    <tableColumn id="61" xr3:uid="{F97F64E4-CEE6-4F78-847D-4CAA7CE8E3EE}" name="DungeonItemCount" dataDxfId="13"/>
     <tableColumn id="31" xr3:uid="{00000000-0010-0000-0100-00001F000000}" name="RewardBlessLevel"/>
     <tableColumn id="42" xr3:uid="{00000000-0010-0000-0100-00002A000000}" name="RewardBlessId"/>
-    <tableColumn id="52" xr3:uid="{00000000-0010-0000-0100-000034000000}" name="RewardResId" dataDxfId="19"/>
-    <tableColumn id="53" xr3:uid="{00000000-0010-0000-0100-000035000000}" name="RewardResAmount" dataDxfId="18"/>
+    <tableColumn id="52" xr3:uid="{00000000-0010-0000-0100-000034000000}" name="RewardResId" dataDxfId="12"/>
+    <tableColumn id="53" xr3:uid="{00000000-0010-0000-0100-000035000000}" name="RewardResAmount" dataDxfId="11"/>
     <tableColumn id="26" xr3:uid="{00000000-0010-0000-0100-00001A000000}" name="UnlockRival"/>
     <tableColumn id="16" xr3:uid="{00000000-0010-0000-0100-000010000000}" name="PunishGold"/>
     <tableColumn id="17" xr3:uid="{00000000-0010-0000-0100-000011000000}" name="PunishFood"/>
@@ -4843,7 +4890,7 @@
     <tableColumn id="21" xr3:uid="{00000000-0010-0000-0100-000015000000}" name="TradeFood"/>
     <tableColumn id="22" xr3:uid="{00000000-0010-0000-0100-000016000000}" name="TradeHealth"/>
     <tableColumn id="23" xr3:uid="{00000000-0010-0000-0100-000017000000}" name="TradeMental"/>
-    <tableColumn id="33" xr3:uid="{00000000-0010-0000-0100-000021000000}" name="TradeDropItem" dataDxfId="17"/>
+    <tableColumn id="33" xr3:uid="{00000000-0010-0000-0100-000021000000}" name="TradeDropItem" dataDxfId="10"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5172,9 +5219,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BN107"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A46" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AD69" sqref="AD69"/>
+    <sheetView tabSelected="1" topLeftCell="T1" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A74" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A86" sqref="A86:XFD86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -9491,7 +9538,9 @@
       <c r="G76" s="72" t="s">
         <v>617</v>
       </c>
-      <c r="H76" s="72"/>
+      <c r="H76" s="72" t="s">
+        <v>656</v>
+      </c>
       <c r="I76" s="69"/>
       <c r="J76" s="78" t="s">
         <v>562</v>
@@ -9507,6 +9556,12 @@
       <c r="S76" s="24"/>
       <c r="T76" s="69"/>
       <c r="V76" s="72"/>
+      <c r="AC76" s="72" t="s">
+        <v>657</v>
+      </c>
+      <c r="AD76" s="8">
+        <v>1</v>
+      </c>
       <c r="AL76" s="72"/>
       <c r="AM76" s="72"/>
       <c r="AN76" s="72"/>
@@ -9516,6 +9571,9 @@
       <c r="AT76" s="72"/>
       <c r="AW76" s="72"/>
       <c r="AX76" s="72"/>
+      <c r="BB76" s="8">
+        <v>150</v>
+      </c>
     </row>
     <row r="77" spans="1:61" x14ac:dyDescent="0.15">
       <c r="A77" s="8">
@@ -9539,8 +9597,12 @@
       <c r="G77" s="72" t="s">
         <v>619</v>
       </c>
-      <c r="H77" s="72"/>
-      <c r="I77" s="69"/>
+      <c r="H77" s="72" t="s">
+        <v>663</v>
+      </c>
+      <c r="I77" s="69" t="s">
+        <v>662</v>
+      </c>
       <c r="J77" s="78" t="s">
         <v>562</v>
       </c>
@@ -9564,6 +9626,9 @@
       <c r="AT77" s="72"/>
       <c r="AW77" s="72"/>
       <c r="AX77" s="72"/>
+      <c r="BA77" s="8">
+        <v>50</v>
+      </c>
     </row>
     <row r="78" spans="1:61" x14ac:dyDescent="0.15">
       <c r="A78" s="8">
@@ -9579,15 +9644,17 @@
         <v>0</v>
       </c>
       <c r="E78" s="8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F78" s="72" t="s">
-        <v>621</v>
+        <v>665</v>
       </c>
       <c r="G78" s="72" t="s">
         <v>621</v>
       </c>
-      <c r="H78" s="72"/>
+      <c r="H78" s="72" t="s">
+        <v>656</v>
+      </c>
       <c r="I78" s="69"/>
       <c r="J78" s="78" t="s">
         <v>562</v>
@@ -9603,6 +9670,18 @@
       <c r="S78" s="24"/>
       <c r="T78" s="69"/>
       <c r="V78" s="72"/>
+      <c r="AC78" s="72" t="s">
+        <v>658</v>
+      </c>
+      <c r="AD78" s="8">
+        <v>2</v>
+      </c>
+      <c r="AE78" s="72" t="s">
+        <v>659</v>
+      </c>
+      <c r="AF78" s="8">
+        <v>0</v>
+      </c>
       <c r="AL78" s="72"/>
       <c r="AM78" s="72"/>
       <c r="AN78" s="72"/>
@@ -9612,6 +9691,9 @@
       <c r="AT78" s="72"/>
       <c r="AW78" s="72"/>
       <c r="AX78" s="72"/>
+      <c r="BB78" s="8">
+        <v>150</v>
+      </c>
     </row>
     <row r="79" spans="1:61" x14ac:dyDescent="0.15">
       <c r="A79" s="8">
@@ -9635,7 +9717,9 @@
       <c r="G79" s="72" t="s">
         <v>623</v>
       </c>
-      <c r="H79" s="72"/>
+      <c r="H79" s="72" t="s">
+        <v>656</v>
+      </c>
       <c r="I79" s="69"/>
       <c r="J79" s="78" t="s">
         <v>562</v>
@@ -9651,6 +9735,12 @@
       <c r="S79" s="24"/>
       <c r="T79" s="69"/>
       <c r="V79" s="72"/>
+      <c r="AC79" s="72" t="s">
+        <v>660</v>
+      </c>
+      <c r="AD79" s="8">
+        <v>1</v>
+      </c>
       <c r="AL79" s="72"/>
       <c r="AM79" s="72"/>
       <c r="AN79" s="72"/>
@@ -9660,6 +9750,12 @@
       <c r="AT79" s="72"/>
       <c r="AW79" s="72"/>
       <c r="AX79" s="72"/>
+      <c r="BB79" s="8">
+        <v>50</v>
+      </c>
+      <c r="BC79" s="8">
+        <v>100</v>
+      </c>
     </row>
     <row r="80" spans="1:61" x14ac:dyDescent="0.15">
       <c r="A80" s="8">
@@ -9683,7 +9779,9 @@
       <c r="G80" s="72" t="s">
         <v>625</v>
       </c>
-      <c r="H80" s="72"/>
+      <c r="H80" s="72" t="s">
+        <v>656</v>
+      </c>
       <c r="I80" s="69"/>
       <c r="J80" s="78" t="s">
         <v>562</v>
@@ -9699,6 +9797,12 @@
       <c r="S80" s="24"/>
       <c r="T80" s="69"/>
       <c r="V80" s="72"/>
+      <c r="AC80" s="72" t="s">
+        <v>658</v>
+      </c>
+      <c r="AD80" s="8">
+        <v>1</v>
+      </c>
       <c r="AL80" s="72"/>
       <c r="AM80" s="72"/>
       <c r="AN80" s="72"/>
@@ -9708,6 +9812,9 @@
       <c r="AT80" s="72"/>
       <c r="AW80" s="72"/>
       <c r="AX80" s="72"/>
+      <c r="BB80" s="8">
+        <v>120</v>
+      </c>
     </row>
     <row r="81" spans="1:56" x14ac:dyDescent="0.15">
       <c r="A81" s="8">
@@ -9723,7 +9830,7 @@
         <v>0</v>
       </c>
       <c r="E81" s="8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F81" s="72" t="s">
         <v>627</v>
@@ -9731,8 +9838,12 @@
       <c r="G81" s="72" t="s">
         <v>627</v>
       </c>
-      <c r="H81" s="72"/>
-      <c r="I81" s="69"/>
+      <c r="H81" s="72" t="s">
+        <v>656</v>
+      </c>
+      <c r="I81" s="69" t="s">
+        <v>662</v>
+      </c>
       <c r="J81" s="78" t="s">
         <v>562</v>
       </c>
@@ -9747,6 +9858,18 @@
       <c r="S81" s="24"/>
       <c r="T81" s="69"/>
       <c r="V81" s="72"/>
+      <c r="AC81" s="72" t="s">
+        <v>657</v>
+      </c>
+      <c r="AD81" s="8">
+        <v>2</v>
+      </c>
+      <c r="AE81" s="72" t="s">
+        <v>661</v>
+      </c>
+      <c r="AF81" s="8">
+        <v>0</v>
+      </c>
       <c r="AL81" s="72"/>
       <c r="AM81" s="72"/>
       <c r="AN81" s="72"/>
@@ -9756,6 +9879,9 @@
       <c r="AT81" s="72"/>
       <c r="AW81" s="72"/>
       <c r="AX81" s="72"/>
+      <c r="BB81" s="8">
+        <v>150</v>
+      </c>
     </row>
     <row r="82" spans="1:56" x14ac:dyDescent="0.15">
       <c r="A82" s="8">
@@ -9779,8 +9905,12 @@
       <c r="G82" s="72" t="s">
         <v>629</v>
       </c>
-      <c r="H82" s="72"/>
-      <c r="I82" s="69"/>
+      <c r="H82" s="72" t="s">
+        <v>656</v>
+      </c>
+      <c r="I82" s="69" t="s">
+        <v>662</v>
+      </c>
       <c r="J82" s="78" t="s">
         <v>562</v>
       </c>
@@ -9795,6 +9925,18 @@
       <c r="S82" s="24"/>
       <c r="T82" s="69"/>
       <c r="V82" s="72"/>
+      <c r="AC82" s="72" t="s">
+        <v>658</v>
+      </c>
+      <c r="AD82" s="8">
+        <v>0</v>
+      </c>
+      <c r="AE82" s="72" t="s">
+        <v>660</v>
+      </c>
+      <c r="AF82" s="8">
+        <v>0</v>
+      </c>
       <c r="AL82" s="72"/>
       <c r="AM82" s="72"/>
       <c r="AN82" s="72"/>
@@ -9804,6 +9946,12 @@
       <c r="AT82" s="72"/>
       <c r="AW82" s="72"/>
       <c r="AX82" s="72"/>
+      <c r="BA82" s="8">
+        <v>50</v>
+      </c>
+      <c r="BD82" s="8">
+        <v>1</v>
+      </c>
     </row>
     <row r="83" spans="1:56" x14ac:dyDescent="0.15">
       <c r="A83" s="8">
@@ -9827,7 +9975,9 @@
       <c r="G83" s="72" t="s">
         <v>631</v>
       </c>
-      <c r="H83" s="72"/>
+      <c r="H83" s="72" t="s">
+        <v>656</v>
+      </c>
       <c r="I83" s="69"/>
       <c r="J83" s="78" t="s">
         <v>562</v>
@@ -9843,6 +9993,18 @@
       <c r="S83" s="24"/>
       <c r="T83" s="69"/>
       <c r="V83" s="72"/>
+      <c r="AC83" s="72" t="s">
+        <v>657</v>
+      </c>
+      <c r="AD83" s="8">
+        <v>0</v>
+      </c>
+      <c r="AE83" s="72" t="s">
+        <v>659</v>
+      </c>
+      <c r="AF83" s="8">
+        <v>1</v>
+      </c>
       <c r="AL83" s="72"/>
       <c r="AM83" s="72"/>
       <c r="AN83" s="72"/>
@@ -9852,6 +10014,9 @@
       <c r="AT83" s="72"/>
       <c r="AW83" s="72"/>
       <c r="AX83" s="72"/>
+      <c r="BB83" s="8">
+        <v>100</v>
+      </c>
     </row>
     <row r="84" spans="1:56" x14ac:dyDescent="0.15">
       <c r="A84" s="8">
@@ -9870,13 +10035,17 @@
         <v>1</v>
       </c>
       <c r="F84" s="72" t="s">
-        <v>633</v>
+        <v>664</v>
       </c>
       <c r="G84" s="72" t="s">
         <v>633</v>
       </c>
-      <c r="H84" s="72"/>
-      <c r="I84" s="69"/>
+      <c r="H84" s="72" t="s">
+        <v>656</v>
+      </c>
+      <c r="I84" s="69" t="s">
+        <v>662</v>
+      </c>
       <c r="J84" s="78" t="s">
         <v>562</v>
       </c>
@@ -9891,6 +10060,12 @@
       <c r="S84" s="24"/>
       <c r="T84" s="69"/>
       <c r="V84" s="72"/>
+      <c r="AC84" s="72" t="s">
+        <v>658</v>
+      </c>
+      <c r="AD84" s="8">
+        <v>1</v>
+      </c>
       <c r="AL84" s="72"/>
       <c r="AM84" s="72"/>
       <c r="AN84" s="72"/>
@@ -9900,6 +10075,9 @@
       <c r="AT84" s="72"/>
       <c r="AW84" s="72"/>
       <c r="AX84" s="72"/>
+      <c r="BB84" s="8">
+        <v>100</v>
+      </c>
     </row>
     <row r="85" spans="1:56" x14ac:dyDescent="0.15">
       <c r="A85" s="8">
@@ -9915,7 +10093,7 @@
         <v>0</v>
       </c>
       <c r="E85" s="8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F85" s="72" t="s">
         <v>635</v>
@@ -9923,8 +10101,12 @@
       <c r="G85" s="72" t="s">
         <v>635</v>
       </c>
-      <c r="H85" s="72"/>
-      <c r="I85" s="69"/>
+      <c r="H85" s="72" t="s">
+        <v>619</v>
+      </c>
+      <c r="I85" s="69" t="s">
+        <v>662</v>
+      </c>
       <c r="J85" s="78" t="s">
         <v>562</v>
       </c>
@@ -9939,6 +10121,18 @@
       <c r="S85" s="24"/>
       <c r="T85" s="69"/>
       <c r="V85" s="72"/>
+      <c r="AC85" s="72" t="s">
+        <v>658</v>
+      </c>
+      <c r="AD85" s="8">
+        <v>2</v>
+      </c>
+      <c r="AE85" s="72" t="s">
+        <v>661</v>
+      </c>
+      <c r="AF85" s="8">
+        <v>2</v>
+      </c>
       <c r="AL85" s="72"/>
       <c r="AM85" s="72"/>
       <c r="AN85" s="72"/>
@@ -9948,6 +10142,9 @@
       <c r="AT85" s="72"/>
       <c r="AW85" s="72"/>
       <c r="AX85" s="72"/>
+      <c r="BB85" s="8">
+        <v>150</v>
+      </c>
     </row>
     <row r="86" spans="1:56" x14ac:dyDescent="0.15">
       <c r="A86" s="8">
@@ -9971,7 +10168,9 @@
       <c r="G86" s="72" t="s">
         <v>637</v>
       </c>
-      <c r="H86" s="72"/>
+      <c r="H86" s="72" t="s">
+        <v>637</v>
+      </c>
       <c r="I86" s="69"/>
       <c r="J86" s="78" t="s">
         <v>562</v>
@@ -9987,6 +10186,18 @@
       <c r="S86" s="24"/>
       <c r="T86" s="69"/>
       <c r="V86" s="72"/>
+      <c r="AC86" s="72" t="s">
+        <v>658</v>
+      </c>
+      <c r="AD86" s="8">
+        <v>3</v>
+      </c>
+      <c r="AE86" s="72" t="s">
+        <v>659</v>
+      </c>
+      <c r="AF86" s="8">
+        <v>2</v>
+      </c>
       <c r="AL86" s="72"/>
       <c r="AM86" s="72"/>
       <c r="AN86" s="72"/>
@@ -9996,6 +10207,12 @@
       <c r="AT86" s="72"/>
       <c r="AW86" s="72"/>
       <c r="AX86" s="72"/>
+      <c r="BB86" s="8">
+        <v>30</v>
+      </c>
+      <c r="BC86" s="8">
+        <v>30</v>
+      </c>
     </row>
     <row r="87" spans="1:56" x14ac:dyDescent="0.15">
       <c r="A87" s="8">
@@ -10019,8 +10236,12 @@
       <c r="G87" s="72" t="s">
         <v>639</v>
       </c>
-      <c r="H87" s="72"/>
-      <c r="I87" s="69"/>
+      <c r="H87" s="72" t="s">
+        <v>656</v>
+      </c>
+      <c r="I87" s="69" t="s">
+        <v>662</v>
+      </c>
       <c r="J87" s="78" t="s">
         <v>562</v>
       </c>
@@ -10035,6 +10256,12 @@
       <c r="S87" s="24"/>
       <c r="T87" s="69"/>
       <c r="V87" s="72"/>
+      <c r="AC87" s="72" t="s">
+        <v>659</v>
+      </c>
+      <c r="AD87" s="8">
+        <v>3</v>
+      </c>
       <c r="AL87" s="72"/>
       <c r="AM87" s="72"/>
       <c r="AN87" s="72"/>
@@ -10044,6 +10271,9 @@
       <c r="AT87" s="72"/>
       <c r="AW87" s="72"/>
       <c r="AX87" s="72"/>
+      <c r="BB87" s="8">
+        <v>100</v>
+      </c>
     </row>
     <row r="88" spans="1:56" x14ac:dyDescent="0.15">
       <c r="A88" s="8">
@@ -10059,7 +10289,7 @@
         <v>0</v>
       </c>
       <c r="E88" s="8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F88" s="72" t="s">
         <v>641</v>
@@ -10067,8 +10297,12 @@
       <c r="G88" s="72" t="s">
         <v>641</v>
       </c>
-      <c r="H88" s="72"/>
-      <c r="I88" s="69"/>
+      <c r="H88" s="72" t="s">
+        <v>656</v>
+      </c>
+      <c r="I88" s="69" t="s">
+        <v>662</v>
+      </c>
       <c r="J88" s="78" t="s">
         <v>562</v>
       </c>
@@ -10083,6 +10317,18 @@
       <c r="S88" s="24"/>
       <c r="T88" s="69"/>
       <c r="V88" s="72"/>
+      <c r="AC88" s="72" t="s">
+        <v>657</v>
+      </c>
+      <c r="AD88" s="8">
+        <v>1</v>
+      </c>
+      <c r="AE88" s="72" t="s">
+        <v>655</v>
+      </c>
+      <c r="AF88" s="8">
+        <v>1</v>
+      </c>
       <c r="AL88" s="72"/>
       <c r="AM88" s="72"/>
       <c r="AN88" s="72"/>
@@ -10092,6 +10338,9 @@
       <c r="AT88" s="72"/>
       <c r="AW88" s="72"/>
       <c r="AX88" s="72"/>
+      <c r="BB88" s="8">
+        <v>200</v>
+      </c>
     </row>
     <row r="89" spans="1:56" x14ac:dyDescent="0.15">
       <c r="A89" s="8">
@@ -11067,7 +11316,7 @@
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <conditionalFormatting sqref="B4:BN107">
-    <cfRule type="containsBlanks" dxfId="12" priority="13">
+    <cfRule type="containsBlanks" dxfId="1" priority="13">
       <formula>LEN(TRIM(B4))=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13564,42 +13813,42 @@
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <conditionalFormatting sqref="J39:S39 D4:S10 J11:S11 D12:S29 J30:S30 T4:BN39 D31:S34 D36:S37 J35:S35 D38:Q38 S38">
-    <cfRule type="containsBlanks" dxfId="11" priority="12">
+    <cfRule type="containsBlanks" dxfId="9" priority="12">
       <formula>LEN(TRIM(D4))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D39:I39">
-    <cfRule type="containsBlanks" dxfId="10" priority="9">
+    <cfRule type="containsBlanks" dxfId="8" priority="9">
       <formula>LEN(TRIM(D39))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D11:I11">
-    <cfRule type="containsBlanks" dxfId="9" priority="7">
+    <cfRule type="containsBlanks" dxfId="7" priority="7">
       <formula>LEN(TRIM(D11))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D30:E30 I30 G30">
-    <cfRule type="containsBlanks" dxfId="8" priority="6">
+    <cfRule type="containsBlanks" dxfId="6" priority="6">
       <formula>LEN(TRIM(D30))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H30">
-    <cfRule type="containsBlanks" dxfId="7" priority="5">
+    <cfRule type="containsBlanks" dxfId="5" priority="5">
       <formula>LEN(TRIM(H30))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F30">
-    <cfRule type="containsBlanks" dxfId="6" priority="3">
+    <cfRule type="containsBlanks" dxfId="4" priority="3">
       <formula>LEN(TRIM(F30))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D35:I35">
-    <cfRule type="containsBlanks" dxfId="5" priority="2">
+    <cfRule type="containsBlanks" dxfId="3" priority="2">
       <formula>LEN(TRIM(D35))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R38">
-    <cfRule type="containsBlanks" dxfId="4" priority="1">
+    <cfRule type="containsBlanks" dxfId="2" priority="1">
       <formula>LEN(TRIM(R38))=0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
sort the scenequest data
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/SceneQuest.xlsx
+++ b/ConfigData/Xlsx/SceneQuest.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385"/>
+    <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="4" r:id="rId1"/>
@@ -22,10 +22,108 @@
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
+    <author>Real</author>
     <author>real</author>
   </authors>
   <commentList>
-    <comment ref="E1" authorId="0" shapeId="0">
+    <comment ref="C1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t>Real:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t xml:space="preserve">
+Common = 1,
+MapSetting = 2,
+Rare = 3,
+Series = 4,
+Dungeon = 5</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E1" authorId="1" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t>real:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t xml:space="preserve">
+0-3</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Real</author>
+    <author>real</author>
+  </authors>
+  <commentList>
+    <comment ref="C1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t>Real:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t xml:space="preserve">
+Common = 1,
+MapSetting = 2,
+Rare = 3,
+Series = 4,
+Dungeon = 5</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E1" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -56,7 +154,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1269" uniqueCount="675">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1282" uniqueCount="675">
   <si>
     <t>int</t>
     <phoneticPr fontId="18" type="noConversion"/>
@@ -2898,7 +2996,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="61">
+  <fills count="62">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3246,6 +3344,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="12">
     <border>
@@ -3511,7 +3615,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="97">
+  <cellXfs count="99">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -3800,7 +3904,13 @@
     <xf numFmtId="0" fontId="24" fillId="60" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="23" fillId="61" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="23" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="61" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -5357,9 +5467,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BP108"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A70" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K82" sqref="K82"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -9199,86 +9309,90 @@
       <c r="AZ66" s="72"/>
     </row>
     <row r="67" spans="1:58" x14ac:dyDescent="0.15">
-      <c r="A67" s="8">
-        <v>42010059</v>
-      </c>
-      <c r="B67" s="72" t="s">
-        <v>595</v>
+      <c r="A67" s="97">
+        <v>42020001</v>
+      </c>
+      <c r="B67" s="97" t="s">
+        <v>124</v>
       </c>
       <c r="C67" s="8">
+        <v>3</v>
+      </c>
+      <c r="D67" s="8">
+        <v>0</v>
+      </c>
+      <c r="E67" s="8">
         <v>1</v>
       </c>
-      <c r="D67" s="8">
-        <v>0</v>
-      </c>
-      <c r="F67" s="72" t="s">
-        <v>606</v>
-      </c>
-      <c r="G67" s="72" t="s">
-        <v>598</v>
-      </c>
-      <c r="H67" s="72" t="s">
-        <v>598</v>
-      </c>
-      <c r="I67" s="69"/>
-      <c r="J67" s="31" t="s">
-        <v>251</v>
-      </c>
-      <c r="K67" s="90" t="s">
-        <v>601</v>
-      </c>
+      <c r="F67" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="G67" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="H67" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="I67" s="22"/>
+      <c r="J67" s="30" t="s">
+        <v>248</v>
+      </c>
+      <c r="K67" s="30"/>
       <c r="L67" s="22"/>
       <c r="M67" s="22"/>
       <c r="N67" s="22"/>
       <c r="O67" s="22"/>
       <c r="P67" s="22"/>
       <c r="Q67" s="22"/>
-      <c r="R67" s="69" t="s">
-        <v>605</v>
-      </c>
-      <c r="S67" s="23"/>
-      <c r="T67" s="69"/>
-      <c r="V67" s="72"/>
-      <c r="AN67" s="72">
-        <v>1</v>
-      </c>
-      <c r="AO67" s="72"/>
-      <c r="AP67" s="72"/>
-      <c r="AQ67" s="72"/>
-      <c r="AR67" s="72"/>
-      <c r="AU67" s="89"/>
-      <c r="AV67" s="72"/>
-      <c r="AY67" s="72"/>
-      <c r="AZ67" s="72"/>
+      <c r="R67" s="22"/>
+      <c r="S67" s="23" t="s">
+        <v>337</v>
+      </c>
+      <c r="T67" s="22"/>
+      <c r="AM67" s="8">
+        <v>100</v>
+      </c>
+      <c r="BA67" s="8" t="s">
+        <v>337</v>
+      </c>
+      <c r="BD67" s="8">
+        <v>200</v>
+      </c>
+      <c r="BE67" s="8">
+        <v>200</v>
+      </c>
     </row>
     <row r="68" spans="1:58" x14ac:dyDescent="0.15">
-      <c r="A68" s="8">
-        <v>42010060</v>
-      </c>
-      <c r="B68" s="72" t="s">
-        <v>597</v>
+      <c r="A68" s="97">
+        <v>42020002</v>
+      </c>
+      <c r="B68" s="97" t="s">
+        <v>103</v>
       </c>
       <c r="C68" s="8">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D68" s="8">
         <v>0</v>
       </c>
+      <c r="E68" s="8">
+        <v>2</v>
+      </c>
       <c r="F68" s="72" t="s">
-        <v>607</v>
+        <v>129</v>
       </c>
       <c r="G68" s="72" t="s">
-        <v>599</v>
-      </c>
-      <c r="H68" s="72" t="s">
-        <v>599</v>
-      </c>
-      <c r="I68" s="69"/>
-      <c r="J68" s="31" t="s">
-        <v>251</v>
-      </c>
-      <c r="K68" s="90" t="s">
-        <v>601</v>
+        <v>575</v>
+      </c>
+      <c r="H68" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="I68" s="22"/>
+      <c r="J68" s="29" t="s">
+        <v>250</v>
+      </c>
+      <c r="K68" s="30" t="s">
+        <v>248</v>
       </c>
       <c r="L68" s="22"/>
       <c r="M68" s="22"/>
@@ -9286,158 +9400,157 @@
       <c r="O68" s="22"/>
       <c r="P68" s="22"/>
       <c r="Q68" s="22"/>
-      <c r="R68" s="69" t="s">
-        <v>605</v>
-      </c>
-      <c r="S68" s="24"/>
-      <c r="T68" s="69"/>
-      <c r="V68" s="72"/>
-      <c r="AN68" s="72"/>
-      <c r="AO68" s="72">
-        <v>1</v>
-      </c>
-      <c r="AP68" s="72"/>
-      <c r="AQ68" s="72"/>
-      <c r="AR68" s="72"/>
-      <c r="AU68" s="89"/>
-      <c r="AV68" s="72"/>
-      <c r="AY68" s="72"/>
-      <c r="AZ68" s="72"/>
+      <c r="R68" s="22"/>
+      <c r="S68" s="24" t="s">
+        <v>334</v>
+      </c>
+      <c r="T68" s="22" t="s">
+        <v>508</v>
+      </c>
+      <c r="AI68" s="8">
+        <v>200</v>
+      </c>
+      <c r="AJ68" s="8">
+        <v>50</v>
+      </c>
+      <c r="AT68" s="8" t="s">
+        <v>400</v>
+      </c>
+      <c r="AY68" s="8">
+        <v>5</v>
+      </c>
+      <c r="AZ68" s="8">
+        <v>100</v>
+      </c>
+      <c r="BD68" s="8">
+        <v>150</v>
+      </c>
+      <c r="BE68" s="8">
+        <v>150</v>
+      </c>
     </row>
     <row r="69" spans="1:58" x14ac:dyDescent="0.15">
-      <c r="A69" s="8">
-        <v>42010061</v>
-      </c>
-      <c r="B69" s="72" t="s">
-        <v>596</v>
+      <c r="A69" s="97">
+        <v>42020003</v>
+      </c>
+      <c r="B69" s="97" t="s">
+        <v>131</v>
       </c>
       <c r="C69" s="8">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D69" s="8">
         <v>0</v>
       </c>
+      <c r="E69" s="8">
+        <v>3</v>
+      </c>
       <c r="F69" s="72" t="s">
-        <v>608</v>
-      </c>
-      <c r="G69" s="72" t="s">
-        <v>600</v>
-      </c>
-      <c r="H69" s="72" t="s">
-        <v>600</v>
-      </c>
-      <c r="I69" s="69"/>
-      <c r="J69" s="31" t="s">
-        <v>251</v>
-      </c>
-      <c r="K69" s="90" t="s">
-        <v>601</v>
-      </c>
+        <v>132</v>
+      </c>
+      <c r="G69" s="8" t="s">
+        <v>130</v>
+      </c>
+      <c r="H69" s="8" t="s">
+        <v>130</v>
+      </c>
+      <c r="I69" s="22"/>
+      <c r="J69" s="29" t="s">
+        <v>250</v>
+      </c>
+      <c r="K69" s="29"/>
       <c r="L69" s="22"/>
       <c r="M69" s="22"/>
       <c r="N69" s="22"/>
       <c r="O69" s="22"/>
       <c r="P69" s="22"/>
       <c r="Q69" s="22"/>
-      <c r="R69" s="69" t="s">
-        <v>605</v>
-      </c>
+      <c r="R69" s="22"/>
       <c r="S69" s="24"/>
-      <c r="T69" s="69"/>
-      <c r="V69" s="72"/>
-      <c r="AN69" s="72"/>
-      <c r="AO69" s="72"/>
-      <c r="AP69" s="72">
+      <c r="T69" s="22"/>
+      <c r="BB69" s="8">
+        <v>100</v>
+      </c>
+      <c r="BD69" s="8">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="70" spans="1:58" x14ac:dyDescent="0.15">
+      <c r="A70" s="97">
+        <v>42020004</v>
+      </c>
+      <c r="B70" s="97" t="s">
+        <v>172</v>
+      </c>
+      <c r="C70" s="8">
+        <v>3</v>
+      </c>
+      <c r="D70" s="8">
+        <v>0</v>
+      </c>
+      <c r="E70" s="8">
         <v>1</v>
       </c>
-      <c r="AQ69" s="72"/>
-      <c r="AR69" s="72"/>
-      <c r="AU69" s="89"/>
-      <c r="AV69" s="72"/>
-      <c r="AY69" s="72"/>
-      <c r="AZ69" s="72"/>
-    </row>
-    <row r="70" spans="1:58" x14ac:dyDescent="0.15">
-      <c r="A70" s="8">
-        <v>42010062</v>
-      </c>
-      <c r="B70" s="72" t="s">
-        <v>612</v>
-      </c>
-      <c r="C70" s="8">
-        <v>1</v>
-      </c>
-      <c r="D70" s="8">
-        <v>0</v>
-      </c>
       <c r="F70" s="72" t="s">
-        <v>609</v>
+        <v>578</v>
       </c>
       <c r="G70" s="72" t="s">
-        <v>616</v>
-      </c>
-      <c r="H70" s="72" t="s">
-        <v>611</v>
-      </c>
-      <c r="I70" s="69"/>
-      <c r="J70" s="31" t="s">
-        <v>251</v>
-      </c>
-      <c r="K70" s="90" t="s">
-        <v>601</v>
-      </c>
+        <v>578</v>
+      </c>
+      <c r="H70" s="8" t="s">
+        <v>171</v>
+      </c>
+      <c r="I70" s="22"/>
+      <c r="J70" s="29" t="s">
+        <v>250</v>
+      </c>
+      <c r="K70" s="29"/>
       <c r="L70" s="22"/>
       <c r="M70" s="22"/>
       <c r="N70" s="22"/>
       <c r="O70" s="22"/>
       <c r="P70" s="22"/>
       <c r="Q70" s="22"/>
-      <c r="R70" s="69" t="s">
-        <v>605</v>
-      </c>
-      <c r="S70" s="24"/>
-      <c r="T70" s="69"/>
-      <c r="V70" s="72"/>
-      <c r="AN70" s="72"/>
-      <c r="AO70" s="72"/>
-      <c r="AP70" s="72"/>
-      <c r="AQ70" s="72">
+      <c r="R70" s="22"/>
+      <c r="T70" s="22"/>
+      <c r="AW70" s="8">
         <v>1</v>
       </c>
-      <c r="AR70" s="72"/>
-      <c r="AU70" s="89"/>
-      <c r="AV70" s="72"/>
-      <c r="AY70" s="72"/>
-      <c r="AZ70" s="72"/>
+      <c r="BF70" s="8">
+        <v>1</v>
+      </c>
     </row>
     <row r="71" spans="1:58" x14ac:dyDescent="0.15">
-      <c r="A71" s="8">
-        <v>42010063</v>
-      </c>
-      <c r="B71" s="72" t="s">
-        <v>614</v>
+      <c r="A71" s="97">
+        <v>42020005</v>
+      </c>
+      <c r="B71" s="97" t="s">
+        <v>188</v>
       </c>
       <c r="C71" s="8">
+        <v>3</v>
+      </c>
+      <c r="D71" s="8">
+        <v>0</v>
+      </c>
+      <c r="E71" s="8">
         <v>1</v>
       </c>
-      <c r="D71" s="8">
-        <v>0</v>
-      </c>
-      <c r="F71" s="72" t="s">
-        <v>610</v>
-      </c>
-      <c r="G71" s="72" t="s">
-        <v>615</v>
+      <c r="F71" s="8" t="s">
+        <v>189</v>
+      </c>
+      <c r="G71" s="8" t="s">
+        <v>187</v>
       </c>
       <c r="H71" s="72" t="s">
-        <v>613</v>
-      </c>
-      <c r="I71" s="69"/>
-      <c r="J71" s="31" t="s">
-        <v>251</v>
-      </c>
-      <c r="K71" s="90" t="s">
-        <v>601</v>
+        <v>579</v>
+      </c>
+      <c r="I71" s="22"/>
+      <c r="J71" s="29" t="s">
+        <v>250</v>
+      </c>
+      <c r="K71" s="30" t="s">
+        <v>248</v>
       </c>
       <c r="L71" s="22"/>
       <c r="M71" s="22"/>
@@ -9445,945 +9558,750 @@
       <c r="O71" s="22"/>
       <c r="P71" s="22"/>
       <c r="Q71" s="22"/>
-      <c r="R71" s="69" t="s">
-        <v>605</v>
-      </c>
-      <c r="S71" s="24"/>
-      <c r="T71" s="69"/>
-      <c r="V71" s="72"/>
-      <c r="AN71" s="72"/>
-      <c r="AO71" s="72"/>
-      <c r="AP71" s="72"/>
-      <c r="AQ71" s="72"/>
-      <c r="AR71" s="72">
-        <v>1</v>
-      </c>
-      <c r="AU71" s="89"/>
-      <c r="AV71" s="72"/>
-      <c r="AY71" s="72"/>
-      <c r="AZ71" s="72"/>
+      <c r="R71" s="22"/>
+      <c r="S71" s="24" t="s">
+        <v>335</v>
+      </c>
+      <c r="T71" s="22" t="s">
+        <v>508</v>
+      </c>
+      <c r="AI71" s="8">
+        <v>150</v>
+      </c>
+      <c r="AJ71" s="8">
+        <v>150</v>
+      </c>
+      <c r="AY71" s="8">
+        <v>4</v>
+      </c>
+      <c r="AZ71" s="8">
+        <v>70</v>
+      </c>
+      <c r="BB71" s="8">
+        <v>200</v>
+      </c>
+      <c r="BC71" s="8">
+        <v>200</v>
+      </c>
     </row>
     <row r="72" spans="1:58" x14ac:dyDescent="0.15">
-      <c r="A72" s="8">
-        <v>42010064</v>
-      </c>
-      <c r="B72" s="72" t="s">
-        <v>618</v>
+      <c r="A72" s="97">
+        <v>42020006</v>
+      </c>
+      <c r="B72" s="97" t="s">
+        <v>190</v>
       </c>
       <c r="C72" s="8">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D72" s="8">
         <v>0</v>
       </c>
       <c r="E72" s="8">
-        <v>1</v>
-      </c>
-      <c r="F72" s="72" t="s">
-        <v>617</v>
-      </c>
-      <c r="G72" s="72" t="s">
-        <v>617</v>
+        <v>3</v>
+      </c>
+      <c r="F72" s="8" t="s">
+        <v>191</v>
+      </c>
+      <c r="G72" s="8" t="s">
+        <v>191</v>
       </c>
       <c r="H72" s="72" t="s">
-        <v>656</v>
-      </c>
-      <c r="I72" s="69"/>
-      <c r="J72" s="78" t="s">
-        <v>562</v>
-      </c>
-      <c r="K72" s="90"/>
+        <v>191</v>
+      </c>
+      <c r="I72" s="22"/>
+      <c r="J72" s="30" t="s">
+        <v>248</v>
+      </c>
+      <c r="K72" s="30"/>
       <c r="L72" s="22"/>
       <c r="M72" s="22"/>
       <c r="N72" s="22"/>
       <c r="O72" s="22"/>
       <c r="P72" s="22"/>
       <c r="Q72" s="22"/>
-      <c r="R72" s="69"/>
-      <c r="S72" s="24"/>
-      <c r="T72" s="69"/>
-      <c r="V72" s="72"/>
-      <c r="AE72" s="72" t="s">
-        <v>657</v>
-      </c>
-      <c r="AF72" s="8">
-        <v>1</v>
-      </c>
-      <c r="AN72" s="72"/>
-      <c r="AO72" s="72"/>
-      <c r="AP72" s="72"/>
-      <c r="AQ72" s="72"/>
-      <c r="AR72" s="72"/>
-      <c r="AU72" s="89"/>
-      <c r="AV72" s="72"/>
-      <c r="AY72" s="72"/>
-      <c r="AZ72" s="72"/>
+      <c r="R72" s="22"/>
+      <c r="S72" s="24" t="s">
+        <v>336</v>
+      </c>
+      <c r="T72" s="22" t="s">
+        <v>508</v>
+      </c>
+      <c r="AI72" s="8">
+        <v>300</v>
+      </c>
+      <c r="AM72" s="8">
+        <v>200</v>
+      </c>
       <c r="BD72" s="8">
-        <v>150</v>
+        <v>300</v>
       </c>
     </row>
     <row r="73" spans="1:58" x14ac:dyDescent="0.15">
-      <c r="A73" s="8">
-        <v>42010065</v>
-      </c>
-      <c r="B73" s="72" t="s">
-        <v>620</v>
+      <c r="A73" s="97">
+        <v>42020007</v>
+      </c>
+      <c r="B73" s="97" t="s">
+        <v>241</v>
       </c>
       <c r="C73" s="8">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D73" s="8">
         <v>0</v>
       </c>
-      <c r="E73" s="8">
-        <v>1</v>
-      </c>
-      <c r="F73" s="72" t="s">
-        <v>619</v>
-      </c>
-      <c r="G73" s="72" t="s">
-        <v>619</v>
-      </c>
-      <c r="H73" s="72" t="s">
-        <v>663</v>
-      </c>
-      <c r="I73" s="69" t="s">
-        <v>662</v>
-      </c>
-      <c r="J73" s="78" t="s">
-        <v>562</v>
-      </c>
-      <c r="K73" s="90"/>
+      <c r="F73" s="8" t="s">
+        <v>243</v>
+      </c>
+      <c r="G73" s="8" t="s">
+        <v>242</v>
+      </c>
+      <c r="H73" s="8" t="s">
+        <v>460</v>
+      </c>
+      <c r="I73" s="22"/>
+      <c r="J73" s="34" t="s">
+        <v>249</v>
+      </c>
+      <c r="K73" s="34"/>
       <c r="L73" s="22"/>
       <c r="M73" s="22"/>
       <c r="N73" s="22"/>
       <c r="O73" s="22"/>
       <c r="P73" s="22"/>
       <c r="Q73" s="22"/>
-      <c r="R73" s="69"/>
+      <c r="R73" s="22"/>
       <c r="S73" s="24"/>
-      <c r="T73" s="69"/>
-      <c r="V73" s="72"/>
-      <c r="AN73" s="72"/>
-      <c r="AO73" s="72"/>
-      <c r="AP73" s="72"/>
-      <c r="AQ73" s="72"/>
-      <c r="AR73" s="72"/>
-      <c r="AU73" s="89"/>
-      <c r="AV73" s="72"/>
-      <c r="AY73" s="72"/>
-      <c r="AZ73" s="72"/>
-      <c r="BC73" s="8">
-        <v>50</v>
-      </c>
+      <c r="T73" s="22"/>
     </row>
     <row r="74" spans="1:58" x14ac:dyDescent="0.15">
-      <c r="A74" s="8">
-        <v>42010066</v>
-      </c>
-      <c r="B74" s="72" t="s">
-        <v>622</v>
+      <c r="A74" s="97">
+        <v>42020008</v>
+      </c>
+      <c r="B74" s="97" t="s">
+        <v>254</v>
       </c>
       <c r="C74" s="8">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D74" s="8">
         <v>0</v>
       </c>
-      <c r="E74" s="8">
-        <v>2</v>
-      </c>
-      <c r="F74" s="72" t="s">
-        <v>665</v>
-      </c>
-      <c r="G74" s="72" t="s">
-        <v>621</v>
-      </c>
-      <c r="H74" s="72" t="s">
-        <v>656</v>
-      </c>
-      <c r="I74" s="69"/>
-      <c r="J74" s="78" t="s">
-        <v>562</v>
-      </c>
-      <c r="K74" s="90"/>
+      <c r="F74" s="8" t="s">
+        <v>253</v>
+      </c>
+      <c r="G74" s="8" t="s">
+        <v>253</v>
+      </c>
+      <c r="H74" s="8" t="s">
+        <v>459</v>
+      </c>
+      <c r="I74" s="22"/>
+      <c r="J74" s="34" t="s">
+        <v>249</v>
+      </c>
+      <c r="K74" s="34"/>
       <c r="L74" s="22"/>
       <c r="M74" s="22"/>
       <c r="N74" s="22"/>
       <c r="O74" s="22"/>
       <c r="P74" s="22"/>
       <c r="Q74" s="22"/>
-      <c r="R74" s="69"/>
-      <c r="S74" s="24"/>
-      <c r="T74" s="69"/>
-      <c r="V74" s="72"/>
-      <c r="AE74" s="72" t="s">
-        <v>658</v>
-      </c>
-      <c r="AF74" s="8">
-        <v>2</v>
-      </c>
-      <c r="AG74" s="72" t="s">
-        <v>659</v>
-      </c>
-      <c r="AH74" s="8">
-        <v>0</v>
-      </c>
-      <c r="AN74" s="72"/>
-      <c r="AO74" s="72"/>
-      <c r="AP74" s="72"/>
-      <c r="AQ74" s="72"/>
-      <c r="AR74" s="72"/>
-      <c r="AU74" s="89"/>
-      <c r="AV74" s="72"/>
-      <c r="AY74" s="72"/>
-      <c r="AZ74" s="72"/>
-      <c r="BD74" s="8">
-        <v>150</v>
-      </c>
+      <c r="R74" s="22"/>
+      <c r="T74" s="22"/>
     </row>
     <row r="75" spans="1:58" x14ac:dyDescent="0.15">
-      <c r="A75" s="8">
-        <v>42010067</v>
-      </c>
-      <c r="B75" s="72" t="s">
-        <v>624</v>
+      <c r="A75" s="97">
+        <v>42020009</v>
+      </c>
+      <c r="B75" s="97" t="s">
+        <v>259</v>
       </c>
       <c r="C75" s="8">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D75" s="8">
         <v>0</v>
       </c>
-      <c r="E75" s="8">
-        <v>1</v>
-      </c>
-      <c r="F75" s="72" t="s">
-        <v>623</v>
-      </c>
-      <c r="G75" s="72" t="s">
-        <v>623</v>
-      </c>
-      <c r="H75" s="72" t="s">
-        <v>656</v>
-      </c>
-      <c r="I75" s="69"/>
-      <c r="J75" s="78" t="s">
-        <v>562</v>
-      </c>
-      <c r="K75" s="90"/>
+      <c r="F75" s="8" t="s">
+        <v>258</v>
+      </c>
+      <c r="G75" s="8" t="s">
+        <v>258</v>
+      </c>
+      <c r="H75" s="8" t="s">
+        <v>258</v>
+      </c>
+      <c r="I75" s="22"/>
+      <c r="J75" s="32" t="s">
+        <v>260</v>
+      </c>
+      <c r="K75" s="32"/>
       <c r="L75" s="22"/>
       <c r="M75" s="22"/>
       <c r="N75" s="22"/>
       <c r="O75" s="22"/>
       <c r="P75" s="22"/>
       <c r="Q75" s="22"/>
-      <c r="R75" s="69"/>
+      <c r="R75" s="22"/>
       <c r="S75" s="24"/>
-      <c r="T75" s="69"/>
-      <c r="V75" s="72"/>
-      <c r="AE75" s="72" t="s">
-        <v>660</v>
-      </c>
-      <c r="AF75" s="8">
-        <v>1</v>
-      </c>
-      <c r="AN75" s="72"/>
-      <c r="AO75" s="72"/>
-      <c r="AP75" s="72"/>
-      <c r="AQ75" s="72"/>
-      <c r="AR75" s="72"/>
-      <c r="AU75" s="89"/>
-      <c r="AV75" s="72"/>
-      <c r="AY75" s="72"/>
-      <c r="AZ75" s="72"/>
-      <c r="BD75" s="8">
-        <v>50</v>
-      </c>
-      <c r="BE75" s="8">
+      <c r="T75" s="22"/>
+      <c r="AA75" s="8">
+        <v>17000001</v>
+      </c>
+      <c r="AI75" s="8">
+        <v>200</v>
+      </c>
+      <c r="AJ75" s="8">
+        <v>150</v>
+      </c>
+      <c r="AS75" s="8" t="s">
+        <v>293</v>
+      </c>
+      <c r="AY75" s="8">
+        <v>2</v>
+      </c>
+      <c r="AZ75" s="8">
         <v>100</v>
       </c>
     </row>
     <row r="76" spans="1:58" x14ac:dyDescent="0.15">
-      <c r="A76" s="8">
-        <v>42010068</v>
-      </c>
-      <c r="B76" s="72" t="s">
-        <v>626</v>
+      <c r="A76" s="97">
+        <v>42020010</v>
+      </c>
+      <c r="B76" s="97" t="s">
+        <v>266</v>
       </c>
       <c r="C76" s="8">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D76" s="8">
         <v>0</v>
       </c>
-      <c r="E76" s="8">
-        <v>1</v>
-      </c>
-      <c r="F76" s="72" t="s">
-        <v>625</v>
-      </c>
-      <c r="G76" s="72" t="s">
-        <v>625</v>
-      </c>
-      <c r="H76" s="72" t="s">
-        <v>656</v>
-      </c>
-      <c r="I76" s="69"/>
-      <c r="J76" s="78" t="s">
-        <v>562</v>
-      </c>
-      <c r="K76" s="90"/>
+      <c r="F76" s="8" t="s">
+        <v>267</v>
+      </c>
+      <c r="G76" s="8" t="s">
+        <v>265</v>
+      </c>
+      <c r="H76" s="8" t="s">
+        <v>265</v>
+      </c>
+      <c r="I76" s="22"/>
+      <c r="J76" s="32" t="s">
+        <v>260</v>
+      </c>
+      <c r="K76" s="32"/>
       <c r="L76" s="22"/>
       <c r="M76" s="22"/>
       <c r="N76" s="22"/>
       <c r="O76" s="22"/>
       <c r="P76" s="22"/>
       <c r="Q76" s="22"/>
-      <c r="R76" s="69"/>
+      <c r="R76" s="22"/>
       <c r="S76" s="24"/>
-      <c r="T76" s="69"/>
-      <c r="V76" s="72"/>
-      <c r="AE76" s="72" t="s">
-        <v>658</v>
-      </c>
-      <c r="AF76" s="8">
-        <v>1</v>
-      </c>
-      <c r="AN76" s="72"/>
-      <c r="AO76" s="72"/>
-      <c r="AP76" s="72"/>
-      <c r="AQ76" s="72"/>
-      <c r="AR76" s="72"/>
-      <c r="AU76" s="89"/>
-      <c r="AV76" s="72"/>
-      <c r="AY76" s="72"/>
-      <c r="AZ76" s="72"/>
-      <c r="BD76" s="8">
-        <v>120</v>
+      <c r="T76" s="22"/>
+      <c r="AA76" s="8">
+        <v>17000003</v>
+      </c>
+      <c r="AI76" s="8">
+        <v>250</v>
+      </c>
+      <c r="AY76" s="8">
+        <v>5</v>
+      </c>
+      <c r="AZ76" s="8">
+        <v>100</v>
+      </c>
+      <c r="BE76" s="8">
+        <v>100</v>
       </c>
     </row>
     <row r="77" spans="1:58" x14ac:dyDescent="0.15">
-      <c r="A77" s="8">
-        <v>42010069</v>
-      </c>
-      <c r="B77" s="72" t="s">
-        <v>628</v>
+      <c r="A77" s="97">
+        <v>42020011</v>
+      </c>
+      <c r="B77" s="97" t="s">
+        <v>269</v>
       </c>
       <c r="C77" s="8">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D77" s="8">
         <v>0</v>
       </c>
-      <c r="E77" s="8">
-        <v>2</v>
-      </c>
-      <c r="F77" s="72" t="s">
-        <v>627</v>
-      </c>
-      <c r="G77" s="72" t="s">
-        <v>627</v>
-      </c>
-      <c r="H77" s="72" t="s">
-        <v>656</v>
-      </c>
-      <c r="I77" s="69" t="s">
-        <v>662</v>
-      </c>
-      <c r="J77" s="78" t="s">
-        <v>562</v>
-      </c>
-      <c r="K77" s="90"/>
+      <c r="F77" s="8" t="s">
+        <v>270</v>
+      </c>
+      <c r="G77" s="8" t="s">
+        <v>268</v>
+      </c>
+      <c r="H77" s="8" t="s">
+        <v>268</v>
+      </c>
+      <c r="I77" s="22"/>
+      <c r="J77" s="32" t="s">
+        <v>260</v>
+      </c>
+      <c r="K77" s="32"/>
       <c r="L77" s="22"/>
       <c r="M77" s="22"/>
       <c r="N77" s="22"/>
       <c r="O77" s="22"/>
       <c r="P77" s="22"/>
       <c r="Q77" s="22"/>
-      <c r="R77" s="69"/>
-      <c r="S77" s="24"/>
-      <c r="T77" s="69"/>
-      <c r="V77" s="72"/>
-      <c r="AE77" s="72" t="s">
-        <v>657</v>
-      </c>
-      <c r="AF77" s="8">
-        <v>2</v>
-      </c>
-      <c r="AG77" s="72" t="s">
-        <v>661</v>
-      </c>
-      <c r="AH77" s="8">
-        <v>0</v>
-      </c>
-      <c r="AN77" s="72"/>
-      <c r="AO77" s="72"/>
-      <c r="AP77" s="72"/>
-      <c r="AQ77" s="72"/>
-      <c r="AR77" s="72"/>
-      <c r="AU77" s="89"/>
-      <c r="AV77" s="72"/>
-      <c r="AY77" s="72"/>
-      <c r="AZ77" s="72"/>
-      <c r="BD77" s="8">
-        <v>150</v>
+      <c r="R77" s="22"/>
+      <c r="T77" s="22"/>
+      <c r="AA77" s="8">
+        <v>17000002</v>
+      </c>
+      <c r="AS77" s="8" t="s">
+        <v>294</v>
+      </c>
+      <c r="AW77" s="8">
+        <v>1</v>
       </c>
     </row>
     <row r="78" spans="1:58" x14ac:dyDescent="0.15">
-      <c r="A78" s="8">
-        <v>42010070</v>
-      </c>
-      <c r="B78" s="72" t="s">
-        <v>630</v>
+      <c r="A78" s="97">
+        <v>42020012</v>
+      </c>
+      <c r="B78" s="97" t="s">
+        <v>398</v>
       </c>
       <c r="C78" s="8">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D78" s="8">
         <v>0</v>
       </c>
-      <c r="E78" s="8">
-        <v>1</v>
-      </c>
-      <c r="F78" s="72" t="s">
-        <v>629</v>
-      </c>
-      <c r="G78" s="72" t="s">
-        <v>629</v>
+      <c r="F78" s="8" t="s">
+        <v>412</v>
+      </c>
+      <c r="G78" s="8" t="s">
+        <v>402</v>
       </c>
       <c r="H78" s="72" t="s">
-        <v>656</v>
-      </c>
-      <c r="I78" s="69" t="s">
-        <v>662</v>
-      </c>
-      <c r="J78" s="78" t="s">
-        <v>562</v>
-      </c>
-      <c r="K78" s="90"/>
+        <v>402</v>
+      </c>
+      <c r="I78" s="22"/>
+      <c r="J78" s="35" t="s">
+        <v>396</v>
+      </c>
+      <c r="K78" s="35"/>
       <c r="L78" s="22"/>
       <c r="M78" s="22"/>
       <c r="N78" s="22"/>
       <c r="O78" s="22"/>
       <c r="P78" s="22"/>
       <c r="Q78" s="22"/>
-      <c r="R78" s="69"/>
-      <c r="S78" s="24"/>
-      <c r="T78" s="69"/>
-      <c r="V78" s="72"/>
-      <c r="AE78" s="72" t="s">
-        <v>658</v>
-      </c>
-      <c r="AF78" s="8">
-        <v>0</v>
-      </c>
-      <c r="AG78" s="72" t="s">
-        <v>660</v>
-      </c>
-      <c r="AH78" s="8">
-        <v>0</v>
-      </c>
-      <c r="AN78" s="72"/>
-      <c r="AO78" s="72"/>
-      <c r="AP78" s="72"/>
-      <c r="AQ78" s="72"/>
-      <c r="AR78" s="72"/>
-      <c r="AU78" s="89"/>
-      <c r="AV78" s="72"/>
-      <c r="AY78" s="72"/>
-      <c r="AZ78" s="72"/>
-      <c r="BC78" s="8">
-        <v>50</v>
-      </c>
-      <c r="BF78" s="8">
-        <v>1</v>
+      <c r="R78" s="22"/>
+      <c r="T78" s="22"/>
+      <c r="AB78" s="8" t="s">
+        <v>397</v>
+      </c>
+      <c r="AI78" s="8">
+        <v>150</v>
+      </c>
+      <c r="AT78" s="24" t="s">
+        <v>399</v>
+      </c>
+      <c r="AU78" s="24"/>
+      <c r="AV78" s="24"/>
+      <c r="AY78" s="8">
+        <v>6</v>
+      </c>
+      <c r="AZ78" s="8">
+        <v>100</v>
       </c>
     </row>
     <row r="79" spans="1:58" x14ac:dyDescent="0.15">
-      <c r="A79" s="8">
-        <v>42010071</v>
-      </c>
-      <c r="B79" s="72" t="s">
-        <v>632</v>
+      <c r="A79" s="97">
+        <v>42020013</v>
+      </c>
+      <c r="B79" s="97" t="s">
+        <v>423</v>
       </c>
       <c r="C79" s="8">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D79" s="8">
         <v>0</v>
       </c>
-      <c r="E79" s="8">
-        <v>1</v>
-      </c>
-      <c r="F79" s="72" t="s">
-        <v>631</v>
-      </c>
-      <c r="G79" s="72" t="s">
-        <v>631</v>
-      </c>
-      <c r="H79" s="72" t="s">
-        <v>656</v>
-      </c>
-      <c r="I79" s="69"/>
-      <c r="J79" s="78" t="s">
-        <v>562</v>
-      </c>
-      <c r="K79" s="90"/>
+      <c r="F79" s="8" t="s">
+        <v>438</v>
+      </c>
+      <c r="G79" s="8" t="s">
+        <v>425</v>
+      </c>
+      <c r="H79" s="8" t="s">
+        <v>424</v>
+      </c>
+      <c r="I79" s="22"/>
+      <c r="J79" s="36" t="s">
+        <v>431</v>
+      </c>
+      <c r="K79" s="36"/>
       <c r="L79" s="22"/>
       <c r="M79" s="22"/>
       <c r="N79" s="22"/>
       <c r="O79" s="22"/>
       <c r="P79" s="22"/>
       <c r="Q79" s="22"/>
-      <c r="R79" s="69"/>
-      <c r="S79" s="24"/>
-      <c r="T79" s="69"/>
-      <c r="V79" s="72"/>
-      <c r="AE79" s="72" t="s">
-        <v>657</v>
-      </c>
-      <c r="AF79" s="8">
-        <v>0</v>
-      </c>
-      <c r="AG79" s="72" t="s">
-        <v>659</v>
-      </c>
-      <c r="AH79" s="8">
-        <v>1</v>
-      </c>
-      <c r="AN79" s="72"/>
-      <c r="AO79" s="72"/>
-      <c r="AP79" s="72"/>
-      <c r="AQ79" s="72"/>
-      <c r="AR79" s="72"/>
-      <c r="AU79" s="89"/>
-      <c r="AV79" s="72"/>
-      <c r="AY79" s="72"/>
-      <c r="AZ79" s="72"/>
-      <c r="BD79" s="8">
-        <v>100</v>
-      </c>
+      <c r="R79" s="22"/>
+      <c r="T79" s="22"/>
+      <c r="Y79" s="8" t="s">
+        <v>428</v>
+      </c>
+      <c r="AT79" s="24"/>
+      <c r="AU79" s="24"/>
+      <c r="AV79" s="24"/>
     </row>
     <row r="80" spans="1:58" x14ac:dyDescent="0.15">
-      <c r="A80" s="8">
-        <v>42010072</v>
-      </c>
-      <c r="B80" s="72" t="s">
-        <v>634</v>
+      <c r="A80" s="97">
+        <v>42020014</v>
+      </c>
+      <c r="B80" s="97" t="s">
+        <v>426</v>
       </c>
       <c r="C80" s="8">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D80" s="8">
         <v>0</v>
       </c>
-      <c r="E80" s="8">
-        <v>1</v>
-      </c>
-      <c r="F80" s="72" t="s">
-        <v>664</v>
-      </c>
-      <c r="G80" s="72" t="s">
-        <v>633</v>
-      </c>
-      <c r="H80" s="72" t="s">
-        <v>656</v>
-      </c>
-      <c r="I80" s="69" t="s">
-        <v>662</v>
-      </c>
-      <c r="J80" s="78" t="s">
-        <v>562</v>
-      </c>
-      <c r="K80" s="90"/>
+      <c r="F80" s="8" t="s">
+        <v>427</v>
+      </c>
+      <c r="G80" s="8" t="s">
+        <v>425</v>
+      </c>
+      <c r="H80" s="8" t="s">
+        <v>427</v>
+      </c>
+      <c r="I80" s="22"/>
+      <c r="J80" s="31" t="s">
+        <v>251</v>
+      </c>
+      <c r="K80" s="31"/>
       <c r="L80" s="22"/>
       <c r="M80" s="22"/>
       <c r="N80" s="22"/>
       <c r="O80" s="22"/>
       <c r="P80" s="22"/>
       <c r="Q80" s="22"/>
-      <c r="R80" s="69"/>
-      <c r="S80" s="24"/>
-      <c r="T80" s="69"/>
-      <c r="V80" s="72"/>
-      <c r="AE80" s="72" t="s">
-        <v>658</v>
-      </c>
-      <c r="AF80" s="8">
+      <c r="R80" s="22"/>
+      <c r="T80" s="22"/>
+      <c r="AJ80" s="8">
+        <v>50</v>
+      </c>
+      <c r="AK80" s="8">
+        <v>50</v>
+      </c>
+      <c r="AL80" s="8">
+        <v>50</v>
+      </c>
+      <c r="AM80" s="8">
+        <v>50</v>
+      </c>
+      <c r="AT80" s="24"/>
+      <c r="AU80" s="24"/>
+      <c r="AV80" s="24"/>
+      <c r="AW80" s="8">
         <v>1</v>
       </c>
-      <c r="AN80" s="72"/>
-      <c r="AO80" s="72"/>
-      <c r="AP80" s="72"/>
-      <c r="AQ80" s="72"/>
-      <c r="AR80" s="72"/>
-      <c r="AU80" s="89"/>
-      <c r="AV80" s="72"/>
-      <c r="AY80" s="72"/>
-      <c r="AZ80" s="72"/>
-      <c r="BD80" s="8">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="81" spans="1:58" x14ac:dyDescent="0.15">
-      <c r="A81" s="8">
-        <v>42010073</v>
-      </c>
-      <c r="B81" s="72" t="s">
-        <v>636</v>
+    </row>
+    <row r="81" spans="1:68" x14ac:dyDescent="0.15">
+      <c r="A81" s="97">
+        <v>42020015</v>
+      </c>
+      <c r="B81" s="97" t="s">
+        <v>429</v>
       </c>
       <c r="C81" s="8">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D81" s="8">
         <v>0</v>
       </c>
-      <c r="E81" s="8">
-        <v>2</v>
-      </c>
-      <c r="F81" s="72" t="s">
-        <v>635</v>
-      </c>
-      <c r="G81" s="72" t="s">
-        <v>635</v>
-      </c>
-      <c r="H81" s="72" t="s">
-        <v>619</v>
-      </c>
-      <c r="I81" s="69" t="s">
-        <v>662</v>
-      </c>
-      <c r="J81" s="78" t="s">
-        <v>562</v>
-      </c>
-      <c r="K81" s="90"/>
+      <c r="F81" s="8" t="s">
+        <v>432</v>
+      </c>
+      <c r="G81" s="8" t="s">
+        <v>441</v>
+      </c>
+      <c r="H81" s="8" t="s">
+        <v>432</v>
+      </c>
+      <c r="I81" s="22"/>
+      <c r="J81" s="36" t="s">
+        <v>431</v>
+      </c>
+      <c r="K81" s="36"/>
       <c r="L81" s="22"/>
       <c r="M81" s="22"/>
       <c r="N81" s="22"/>
       <c r="O81" s="22"/>
       <c r="P81" s="22"/>
       <c r="Q81" s="22"/>
-      <c r="R81" s="69"/>
-      <c r="S81" s="24"/>
-      <c r="T81" s="69"/>
-      <c r="V81" s="72"/>
-      <c r="AE81" s="72" t="s">
-        <v>658</v>
-      </c>
-      <c r="AF81" s="8">
-        <v>2</v>
-      </c>
-      <c r="AG81" s="72" t="s">
-        <v>661</v>
-      </c>
-      <c r="AH81" s="8">
-        <v>2</v>
-      </c>
-      <c r="AN81" s="72"/>
-      <c r="AO81" s="72"/>
-      <c r="AP81" s="72"/>
-      <c r="AQ81" s="72"/>
-      <c r="AR81" s="72"/>
-      <c r="AU81" s="89"/>
-      <c r="AV81" s="72"/>
-      <c r="AY81" s="72"/>
-      <c r="AZ81" s="72"/>
-      <c r="BD81" s="8">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="82" spans="1:58" x14ac:dyDescent="0.15">
-      <c r="A82" s="8">
-        <v>42010074</v>
-      </c>
-      <c r="B82" s="72" t="s">
-        <v>638</v>
+      <c r="R81" s="22"/>
+      <c r="T81" s="22"/>
+      <c r="Y81" s="8" t="s">
+        <v>437</v>
+      </c>
+      <c r="AJ81" s="8">
+        <v>50</v>
+      </c>
+      <c r="AK81" s="8">
+        <v>50</v>
+      </c>
+      <c r="AT81" s="24"/>
+      <c r="AU81" s="24"/>
+      <c r="AV81" s="24"/>
+    </row>
+    <row r="82" spans="1:68" x14ac:dyDescent="0.15">
+      <c r="A82" s="97">
+        <v>42020016</v>
+      </c>
+      <c r="B82" s="97" t="s">
+        <v>430</v>
       </c>
       <c r="C82" s="8">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D82" s="8">
         <v>0</v>
       </c>
-      <c r="E82" s="8">
-        <v>1</v>
-      </c>
-      <c r="F82" s="72" t="s">
-        <v>637</v>
-      </c>
-      <c r="G82" s="72" t="s">
-        <v>637</v>
-      </c>
-      <c r="H82" s="72" t="s">
-        <v>637</v>
-      </c>
-      <c r="I82" s="69"/>
-      <c r="J82" s="78" t="s">
-        <v>562</v>
-      </c>
-      <c r="K82" s="28" t="s">
-        <v>247</v>
-      </c>
+      <c r="F82" s="8" t="s">
+        <v>434</v>
+      </c>
+      <c r="G82" s="8" t="s">
+        <v>433</v>
+      </c>
+      <c r="H82" s="8" t="s">
+        <v>434</v>
+      </c>
+      <c r="I82" s="22"/>
+      <c r="J82" s="31" t="s">
+        <v>251</v>
+      </c>
+      <c r="K82" s="31"/>
       <c r="L82" s="22"/>
       <c r="M82" s="22"/>
       <c r="N82" s="22"/>
       <c r="O82" s="22"/>
       <c r="P82" s="22"/>
       <c r="Q82" s="22"/>
-      <c r="R82" s="69"/>
-      <c r="S82" s="24"/>
-      <c r="T82" s="69"/>
-      <c r="V82" s="72"/>
-      <c r="AE82" s="72" t="s">
-        <v>658</v>
-      </c>
-      <c r="AF82" s="8">
+      <c r="R82" s="22"/>
+      <c r="S82" s="8" t="s">
+        <v>439</v>
+      </c>
+      <c r="T82" s="22" t="s">
+        <v>508</v>
+      </c>
+      <c r="AI82" s="8">
+        <v>400</v>
+      </c>
+      <c r="AK82" s="8">
+        <v>150</v>
+      </c>
+      <c r="AL82" s="8">
+        <v>150</v>
+      </c>
+      <c r="AS82" s="8" t="s">
+        <v>440</v>
+      </c>
+      <c r="AT82" s="24"/>
+      <c r="AU82" s="24"/>
+      <c r="AV82" s="24"/>
+      <c r="AY82" s="8">
+        <v>7</v>
+      </c>
+      <c r="AZ82" s="8">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="83" spans="1:68" x14ac:dyDescent="0.15">
+      <c r="A83" s="97">
+        <v>42020017</v>
+      </c>
+      <c r="B83" s="97" t="s">
+        <v>449</v>
+      </c>
+      <c r="C83" s="8">
         <v>3</v>
       </c>
-      <c r="AG82" s="72" t="s">
-        <v>659</v>
-      </c>
-      <c r="AH82" s="8">
-        <v>2</v>
-      </c>
-      <c r="AN82" s="72"/>
-      <c r="AO82" s="72"/>
-      <c r="AP82" s="72"/>
-      <c r="AQ82" s="72"/>
-      <c r="AR82" s="72"/>
-      <c r="AU82" s="89"/>
-      <c r="AV82" s="72"/>
-      <c r="AY82" s="72"/>
-      <c r="AZ82" s="72"/>
-      <c r="BD82" s="8">
-        <v>30</v>
-      </c>
-      <c r="BE82" s="8">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="83" spans="1:58" x14ac:dyDescent="0.15">
-      <c r="A83" s="8">
-        <v>42010075</v>
-      </c>
-      <c r="B83" s="72" t="s">
-        <v>640</v>
-      </c>
-      <c r="C83" s="8">
-        <v>1</v>
-      </c>
       <c r="D83" s="8">
         <v>0</v>
       </c>
-      <c r="E83" s="8">
-        <v>1</v>
-      </c>
-      <c r="F83" s="72" t="s">
-        <v>639</v>
-      </c>
-      <c r="G83" s="72" t="s">
-        <v>639</v>
-      </c>
-      <c r="H83" s="72" t="s">
-        <v>656</v>
-      </c>
-      <c r="I83" s="69" t="s">
-        <v>662</v>
-      </c>
-      <c r="J83" s="78" t="s">
-        <v>562</v>
-      </c>
-      <c r="K83" s="90"/>
+      <c r="F83" s="8" t="s">
+        <v>453</v>
+      </c>
+      <c r="G83" s="8" t="s">
+        <v>448</v>
+      </c>
+      <c r="H83" s="8" t="s">
+        <v>451</v>
+      </c>
+      <c r="I83" s="22"/>
+      <c r="J83" s="31" t="s">
+        <v>251</v>
+      </c>
+      <c r="K83" s="31"/>
       <c r="L83" s="22"/>
       <c r="M83" s="22"/>
       <c r="N83" s="22"/>
       <c r="O83" s="22"/>
       <c r="P83" s="22"/>
       <c r="Q83" s="22"/>
-      <c r="R83" s="69"/>
-      <c r="S83" s="24"/>
-      <c r="T83" s="69"/>
-      <c r="V83" s="72"/>
-      <c r="AE83" s="72" t="s">
-        <v>659</v>
-      </c>
-      <c r="AF83" s="8">
+      <c r="R83" s="22"/>
+      <c r="T83" s="22"/>
+      <c r="AS83" s="8" t="s">
+        <v>452</v>
+      </c>
+      <c r="AT83" s="24"/>
+      <c r="AU83" s="24"/>
+      <c r="AV83" s="24"/>
+    </row>
+    <row r="84" spans="1:68" x14ac:dyDescent="0.15">
+      <c r="A84" s="97">
+        <v>42020018</v>
+      </c>
+      <c r="B84" s="97" t="s">
+        <v>492</v>
+      </c>
+      <c r="C84" s="8">
         <v>3</v>
       </c>
-      <c r="AN83" s="72"/>
-      <c r="AO83" s="72"/>
-      <c r="AP83" s="72"/>
-      <c r="AQ83" s="72"/>
-      <c r="AR83" s="72"/>
-      <c r="AU83" s="89"/>
-      <c r="AV83" s="72"/>
-      <c r="AY83" s="72"/>
-      <c r="AZ83" s="72"/>
-      <c r="BD83" s="8">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="84" spans="1:58" x14ac:dyDescent="0.15">
-      <c r="A84" s="8">
-        <v>42010076</v>
-      </c>
-      <c r="B84" s="72" t="s">
-        <v>642</v>
-      </c>
-      <c r="C84" s="8">
-        <v>1</v>
-      </c>
       <c r="D84" s="8">
         <v>0</v>
       </c>
       <c r="E84" s="8">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F84" s="72" t="s">
-        <v>641</v>
+        <v>491</v>
       </c>
       <c r="G84" s="72" t="s">
-        <v>641</v>
-      </c>
-      <c r="H84" s="72" t="s">
-        <v>656</v>
-      </c>
-      <c r="I84" s="69" t="s">
-        <v>662</v>
-      </c>
-      <c r="J84" s="78" t="s">
-        <v>562</v>
-      </c>
-      <c r="K84" s="90"/>
+        <v>491</v>
+      </c>
+      <c r="H84" s="8" t="s">
+        <v>491</v>
+      </c>
+      <c r="I84" s="22"/>
+      <c r="J84" s="30" t="s">
+        <v>248</v>
+      </c>
+      <c r="K84" s="30"/>
       <c r="L84" s="22"/>
       <c r="M84" s="22"/>
       <c r="N84" s="22"/>
       <c r="O84" s="22"/>
       <c r="P84" s="22"/>
       <c r="Q84" s="22"/>
-      <c r="R84" s="69"/>
-      <c r="S84" s="24"/>
-      <c r="T84" s="69"/>
-      <c r="V84" s="72"/>
-      <c r="AE84" s="72" t="s">
-        <v>657</v>
-      </c>
-      <c r="AF84" s="8">
+      <c r="R84" s="22"/>
+      <c r="S84" s="24" t="s">
+        <v>493</v>
+      </c>
+      <c r="T84" s="22" t="s">
+        <v>508</v>
+      </c>
+      <c r="AI84" s="8">
+        <v>150</v>
+      </c>
+      <c r="AM84" s="8">
+        <v>300</v>
+      </c>
+      <c r="AT84" s="24" t="s">
+        <v>494</v>
+      </c>
+      <c r="AU84" s="24"/>
+      <c r="AV84" s="24"/>
+      <c r="AY84" s="8">
+        <v>7</v>
+      </c>
+      <c r="AZ84" s="8">
+        <v>100</v>
+      </c>
+      <c r="BD84" s="8">
+        <v>100</v>
+      </c>
+      <c r="BE84" s="8">
+        <v>60</v>
+      </c>
+      <c r="BF84" s="8">
         <v>1</v>
       </c>
-      <c r="AG84" s="72" t="s">
-        <v>655</v>
-      </c>
-      <c r="AH84" s="8">
-        <v>1</v>
-      </c>
-      <c r="AN84" s="72"/>
-      <c r="AO84" s="72"/>
-      <c r="AP84" s="72"/>
-      <c r="AQ84" s="72"/>
-      <c r="AR84" s="72"/>
-      <c r="AU84" s="89"/>
-      <c r="AV84" s="72"/>
-      <c r="AY84" s="72"/>
-      <c r="AZ84" s="72"/>
-      <c r="BD84" s="8">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="85" spans="1:58" x14ac:dyDescent="0.15">
-      <c r="A85" s="8">
-        <v>42010077</v>
-      </c>
-      <c r="B85" s="72" t="s">
-        <v>670</v>
+    </row>
+    <row r="85" spans="1:68" x14ac:dyDescent="0.15">
+      <c r="A85" s="97">
+        <v>42020019</v>
+      </c>
+      <c r="B85" s="97" t="s">
+        <v>510</v>
       </c>
       <c r="C85" s="8">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D85" s="8">
         <v>0</v>
       </c>
-      <c r="F85" s="72" t="s">
-        <v>671</v>
-      </c>
-      <c r="G85" s="72" t="s">
-        <v>671</v>
-      </c>
-      <c r="H85" s="72" t="s">
-        <v>671</v>
-      </c>
-      <c r="I85" s="69"/>
-      <c r="J85" s="87" t="s">
-        <v>589</v>
-      </c>
-      <c r="K85" s="31"/>
+      <c r="F85" s="8" t="s">
+        <v>509</v>
+      </c>
+      <c r="G85" s="8" t="s">
+        <v>509</v>
+      </c>
+      <c r="H85" s="8" t="s">
+        <v>509</v>
+      </c>
+      <c r="I85" s="22"/>
+      <c r="J85" s="27" t="s">
+        <v>513</v>
+      </c>
+      <c r="K85" s="27"/>
       <c r="L85" s="22"/>
       <c r="M85" s="22"/>
       <c r="N85" s="22"/>
       <c r="O85" s="22"/>
       <c r="P85" s="22"/>
       <c r="Q85" s="22"/>
-      <c r="R85" s="69"/>
-      <c r="S85" s="24"/>
-      <c r="T85" s="69"/>
-      <c r="V85" s="72"/>
-      <c r="AC85" s="88" t="s">
-        <v>588</v>
-      </c>
-      <c r="AD85" s="8">
-        <v>5</v>
-      </c>
-      <c r="AE85" s="72"/>
-      <c r="AF85" s="72"/>
-      <c r="AG85" s="72"/>
-      <c r="AH85" s="72"/>
-      <c r="AI85" s="8">
-        <v>300</v>
-      </c>
-      <c r="AJ85" s="8">
-        <v>300</v>
-      </c>
-      <c r="AN85" s="72"/>
-      <c r="AO85" s="72"/>
-      <c r="AP85" s="72"/>
-      <c r="AQ85" s="72"/>
-      <c r="AR85" s="72"/>
-      <c r="AU85" s="89"/>
-      <c r="AV85" s="72"/>
-      <c r="AY85" s="72"/>
-      <c r="AZ85" s="72"/>
-    </row>
-    <row r="86" spans="1:58" x14ac:dyDescent="0.15">
-      <c r="A86" s="96">
-        <v>42020001</v>
-      </c>
-      <c r="B86" s="96" t="s">
-        <v>124</v>
+      <c r="R85" s="22"/>
+      <c r="T85" s="22"/>
+      <c r="BL85" s="8">
+        <v>-1</v>
+      </c>
+      <c r="BP85" s="8" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="86" spans="1:68" x14ac:dyDescent="0.15">
+      <c r="A86" s="8">
+        <v>42030001</v>
+      </c>
+      <c r="B86" s="8" t="s">
+        <v>117</v>
       </c>
       <c r="C86" s="8">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D86" s="8">
         <v>0</v>
       </c>
-      <c r="E86" s="8">
-        <v>1</v>
-      </c>
       <c r="F86" s="8" t="s">
-        <v>125</v>
+        <v>312</v>
       </c>
       <c r="G86" s="8" t="s">
-        <v>125</v>
-      </c>
-      <c r="H86" s="8" t="s">
-        <v>125</v>
+        <v>119</v>
+      </c>
+      <c r="H86" s="72" t="s">
+        <v>120</v>
       </c>
       <c r="I86" s="22"/>
-      <c r="J86" s="30" t="s">
-        <v>248</v>
-      </c>
-      <c r="K86" s="30"/>
+      <c r="J86" s="29" t="s">
+        <v>250</v>
+      </c>
+      <c r="K86" s="29"/>
       <c r="L86" s="22"/>
       <c r="M86" s="22"/>
       <c r="N86" s="22"/>
@@ -10391,32 +10309,24 @@
       <c r="P86" s="22"/>
       <c r="Q86" s="22"/>
       <c r="R86" s="22"/>
-      <c r="S86" s="24" t="s">
-        <v>337</v>
-      </c>
+      <c r="S86" s="24"/>
       <c r="T86" s="22"/>
-      <c r="AM86" s="8">
-        <v>100</v>
-      </c>
-      <c r="BA86" s="8" t="s">
-        <v>337</v>
-      </c>
-      <c r="BD86" s="8">
-        <v>200</v>
-      </c>
-      <c r="BE86" s="8">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="87" spans="1:58" x14ac:dyDescent="0.15">
-      <c r="A87" s="96">
-        <v>42020002</v>
-      </c>
-      <c r="B87" s="96" t="s">
-        <v>103</v>
+      <c r="X86" s="8" t="s">
+        <v>348</v>
+      </c>
+      <c r="AJ86" s="8">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="87" spans="1:68" x14ac:dyDescent="0.15">
+      <c r="A87" s="8">
+        <v>42030002</v>
+      </c>
+      <c r="B87" s="8" t="s">
+        <v>118</v>
       </c>
       <c r="C87" s="8">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D87" s="8">
         <v>0</v>
@@ -10424,22 +10334,20 @@
       <c r="E87" s="8">
         <v>2</v>
       </c>
-      <c r="F87" s="72" t="s">
-        <v>129</v>
-      </c>
-      <c r="G87" s="72" t="s">
-        <v>575</v>
+      <c r="F87" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="G87" s="8" t="s">
+        <v>119</v>
       </c>
       <c r="H87" s="8" t="s">
-        <v>102</v>
+        <v>122</v>
       </c>
       <c r="I87" s="22"/>
-      <c r="J87" s="29" t="s">
-        <v>250</v>
-      </c>
-      <c r="K87" s="30" t="s">
+      <c r="J87" s="30" t="s">
         <v>248</v>
       </c>
+      <c r="K87" s="30"/>
       <c r="L87" s="22"/>
       <c r="M87" s="22"/>
       <c r="N87" s="22"/>
@@ -10448,7 +10356,7 @@
       <c r="Q87" s="22"/>
       <c r="R87" s="22"/>
       <c r="S87" s="24" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
       <c r="T87" s="22" t="s">
         <v>508</v>
@@ -10457,9 +10365,12 @@
         <v>200</v>
       </c>
       <c r="AJ87" s="8">
-        <v>50</v>
-      </c>
-      <c r="AT87" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="AM87" s="8">
+        <v>100</v>
+      </c>
+      <c r="AT87" s="24" t="s">
         <v>400</v>
       </c>
       <c r="AY87" s="8">
@@ -10469,21 +10380,18 @@
         <v>100</v>
       </c>
       <c r="BD87" s="8">
-        <v>150</v>
-      </c>
-      <c r="BE87" s="8">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="88" spans="1:58" x14ac:dyDescent="0.15">
-      <c r="A88" s="96">
-        <v>42020003</v>
-      </c>
-      <c r="B88" s="96" t="s">
-        <v>131</v>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="88" spans="1:68" x14ac:dyDescent="0.15">
+      <c r="A88" s="8">
+        <v>42030003</v>
+      </c>
+      <c r="B88" s="8" t="s">
+        <v>463</v>
       </c>
       <c r="C88" s="8">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D88" s="8">
         <v>0</v>
@@ -10491,14 +10399,14 @@
       <c r="E88" s="8">
         <v>3</v>
       </c>
-      <c r="F88" s="72" t="s">
-        <v>132</v>
+      <c r="F88" s="8" t="s">
+        <v>465</v>
       </c>
       <c r="G88" s="8" t="s">
-        <v>130</v>
+        <v>462</v>
       </c>
       <c r="H88" s="8" t="s">
-        <v>130</v>
+        <v>465</v>
       </c>
       <c r="I88" s="22"/>
       <c r="J88" s="29" t="s">
@@ -10512,45 +10420,47 @@
       <c r="P88" s="22"/>
       <c r="Q88" s="22"/>
       <c r="R88" s="22"/>
-      <c r="S88" s="24"/>
       <c r="T88" s="22"/>
-      <c r="BB88" s="8">
-        <v>100</v>
+      <c r="X88" s="8" t="s">
+        <v>467</v>
       </c>
       <c r="BD88" s="8">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="89" spans="1:58" x14ac:dyDescent="0.15">
-      <c r="A89" s="96">
-        <v>42020004</v>
-      </c>
-      <c r="B89" s="96" t="s">
-        <v>172</v>
+        <v>150</v>
+      </c>
+      <c r="BE88" s="8">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="89" spans="1:68" x14ac:dyDescent="0.15">
+      <c r="A89" s="8">
+        <v>42030004</v>
+      </c>
+      <c r="B89" s="8" t="s">
+        <v>464</v>
       </c>
       <c r="C89" s="8">
+        <v>4</v>
+      </c>
+      <c r="D89" s="8">
+        <v>0</v>
+      </c>
+      <c r="E89" s="8">
         <v>3</v>
       </c>
-      <c r="D89" s="8">
-        <v>0</v>
-      </c>
-      <c r="E89" s="8">
-        <v>1</v>
-      </c>
-      <c r="F89" s="72" t="s">
-        <v>578</v>
-      </c>
-      <c r="G89" s="72" t="s">
-        <v>578</v>
+      <c r="F89" s="8" t="s">
+        <v>467</v>
+      </c>
+      <c r="G89" s="8" t="s">
+        <v>462</v>
       </c>
       <c r="H89" s="8" t="s">
-        <v>171</v>
+        <v>466</v>
       </c>
       <c r="I89" s="22"/>
-      <c r="J89" s="29" t="s">
-        <v>250</v>
-      </c>
-      <c r="K89" s="29"/>
+      <c r="J89" s="30" t="s">
+        <v>248</v>
+      </c>
+      <c r="K89" s="30"/>
       <c r="L89" s="22"/>
       <c r="M89" s="22"/>
       <c r="N89" s="22"/>
@@ -10558,45 +10468,62 @@
       <c r="P89" s="22"/>
       <c r="Q89" s="22"/>
       <c r="R89" s="22"/>
-      <c r="T89" s="22"/>
-      <c r="AW89" s="8">
-        <v>1</v>
-      </c>
-      <c r="BF89" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="90" spans="1:58" x14ac:dyDescent="0.15">
+      <c r="S89" s="8" t="s">
+        <v>468</v>
+      </c>
+      <c r="T89" s="22" t="s">
+        <v>508</v>
+      </c>
+      <c r="AI89" s="8">
+        <v>300</v>
+      </c>
+      <c r="AJ89" s="8">
+        <v>200</v>
+      </c>
+      <c r="AM89" s="8">
+        <v>70</v>
+      </c>
+      <c r="AT89" s="8" t="s">
+        <v>401</v>
+      </c>
+      <c r="AY89" s="8">
+        <v>7</v>
+      </c>
+      <c r="AZ89" s="8">
+        <v>150</v>
+      </c>
+      <c r="BD89" s="8">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="90" spans="1:68" x14ac:dyDescent="0.15">
       <c r="A90" s="96">
-        <v>42020005</v>
-      </c>
-      <c r="B90" s="96" t="s">
-        <v>188</v>
+        <v>42040001</v>
+      </c>
+      <c r="B90" s="98" t="s">
+        <v>595</v>
       </c>
       <c r="C90" s="8">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D90" s="8">
         <v>0</v>
       </c>
-      <c r="E90" s="8">
-        <v>1</v>
-      </c>
-      <c r="F90" s="8" t="s">
-        <v>189</v>
-      </c>
-      <c r="G90" s="8" t="s">
-        <v>187</v>
+      <c r="F90" s="72" t="s">
+        <v>606</v>
+      </c>
+      <c r="G90" s="72" t="s">
+        <v>598</v>
       </c>
       <c r="H90" s="72" t="s">
-        <v>579</v>
-      </c>
-      <c r="I90" s="22"/>
-      <c r="J90" s="29" t="s">
-        <v>250</v>
-      </c>
-      <c r="K90" s="30" t="s">
-        <v>248</v>
+        <v>598</v>
+      </c>
+      <c r="I90" s="69"/>
+      <c r="J90" s="31" t="s">
+        <v>251</v>
+      </c>
+      <c r="K90" s="90" t="s">
+        <v>601</v>
       </c>
       <c r="L90" s="22"/>
       <c r="M90" s="22"/>
@@ -10604,947 +10531,1158 @@
       <c r="O90" s="22"/>
       <c r="P90" s="22"/>
       <c r="Q90" s="22"/>
-      <c r="R90" s="22"/>
-      <c r="S90" s="24" t="s">
-        <v>335</v>
-      </c>
-      <c r="T90" s="22" t="s">
-        <v>508</v>
-      </c>
-      <c r="AI90" s="8">
-        <v>150</v>
-      </c>
-      <c r="AJ90" s="8">
-        <v>150</v>
-      </c>
-      <c r="AY90" s="8">
-        <v>4</v>
-      </c>
-      <c r="AZ90" s="8">
-        <v>70</v>
-      </c>
-      <c r="BB90" s="8">
-        <v>200</v>
-      </c>
-      <c r="BC90" s="8">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="91" spans="1:58" x14ac:dyDescent="0.15">
+      <c r="R90" s="69" t="s">
+        <v>605</v>
+      </c>
+      <c r="S90" s="24"/>
+      <c r="T90" s="69"/>
+      <c r="V90" s="72"/>
+      <c r="AN90" s="72">
+        <v>1</v>
+      </c>
+      <c r="AO90" s="72"/>
+      <c r="AP90" s="72"/>
+      <c r="AQ90" s="72"/>
+      <c r="AR90" s="72"/>
+      <c r="AU90" s="89"/>
+      <c r="AV90" s="72"/>
+      <c r="AY90" s="72"/>
+      <c r="AZ90" s="72"/>
+    </row>
+    <row r="91" spans="1:68" x14ac:dyDescent="0.15">
       <c r="A91" s="96">
-        <v>42020006</v>
-      </c>
-      <c r="B91" s="96" t="s">
-        <v>190</v>
+        <v>42040002</v>
+      </c>
+      <c r="B91" s="98" t="s">
+        <v>597</v>
       </c>
       <c r="C91" s="8">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D91" s="8">
         <v>0</v>
       </c>
-      <c r="E91" s="8">
-        <v>3</v>
-      </c>
-      <c r="F91" s="8" t="s">
-        <v>191</v>
-      </c>
-      <c r="G91" s="8" t="s">
-        <v>191</v>
+      <c r="F91" s="72" t="s">
+        <v>607</v>
+      </c>
+      <c r="G91" s="72" t="s">
+        <v>599</v>
       </c>
       <c r="H91" s="72" t="s">
-        <v>191</v>
-      </c>
-      <c r="I91" s="22"/>
-      <c r="J91" s="30" t="s">
-        <v>248</v>
-      </c>
-      <c r="K91" s="30"/>
+        <v>599</v>
+      </c>
+      <c r="I91" s="69"/>
+      <c r="J91" s="31" t="s">
+        <v>251</v>
+      </c>
+      <c r="K91" s="90" t="s">
+        <v>601</v>
+      </c>
       <c r="L91" s="22"/>
       <c r="M91" s="22"/>
       <c r="N91" s="22"/>
       <c r="O91" s="22"/>
       <c r="P91" s="22"/>
       <c r="Q91" s="22"/>
-      <c r="R91" s="22"/>
-      <c r="S91" s="23" t="s">
-        <v>336</v>
-      </c>
-      <c r="T91" s="22" t="s">
-        <v>508</v>
-      </c>
-      <c r="AI91" s="8">
-        <v>300</v>
-      </c>
-      <c r="AM91" s="8">
-        <v>200</v>
-      </c>
-      <c r="BD91" s="8">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="92" spans="1:58" x14ac:dyDescent="0.15">
+      <c r="R91" s="69" t="s">
+        <v>605</v>
+      </c>
+      <c r="S91" s="23"/>
+      <c r="T91" s="69"/>
+      <c r="V91" s="72"/>
+      <c r="AN91" s="72"/>
+      <c r="AO91" s="72">
+        <v>1</v>
+      </c>
+      <c r="AP91" s="72"/>
+      <c r="AQ91" s="72"/>
+      <c r="AR91" s="72"/>
+      <c r="AU91" s="89"/>
+      <c r="AV91" s="72"/>
+      <c r="AY91" s="72"/>
+      <c r="AZ91" s="72"/>
+    </row>
+    <row r="92" spans="1:68" x14ac:dyDescent="0.15">
       <c r="A92" s="96">
-        <v>42020007</v>
-      </c>
-      <c r="B92" s="96" t="s">
-        <v>241</v>
+        <v>42040003</v>
+      </c>
+      <c r="B92" s="98" t="s">
+        <v>596</v>
       </c>
       <c r="C92" s="8">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D92" s="8">
         <v>0</v>
       </c>
-      <c r="F92" s="8" t="s">
-        <v>243</v>
-      </c>
-      <c r="G92" s="8" t="s">
-        <v>242</v>
-      </c>
-      <c r="H92" s="8" t="s">
-        <v>460</v>
-      </c>
-      <c r="I92" s="22"/>
-      <c r="J92" s="34" t="s">
-        <v>249</v>
-      </c>
-      <c r="K92" s="34"/>
+      <c r="F92" s="72" t="s">
+        <v>608</v>
+      </c>
+      <c r="G92" s="72" t="s">
+        <v>600</v>
+      </c>
+      <c r="H92" s="72" t="s">
+        <v>600</v>
+      </c>
+      <c r="I92" s="69"/>
+      <c r="J92" s="31" t="s">
+        <v>251</v>
+      </c>
+      <c r="K92" s="90" t="s">
+        <v>601</v>
+      </c>
       <c r="L92" s="22"/>
       <c r="M92" s="22"/>
       <c r="N92" s="22"/>
       <c r="O92" s="22"/>
       <c r="P92" s="22"/>
       <c r="Q92" s="22"/>
-      <c r="R92" s="22"/>
+      <c r="R92" s="69" t="s">
+        <v>605</v>
+      </c>
       <c r="S92" s="24"/>
-      <c r="T92" s="22"/>
-    </row>
-    <row r="93" spans="1:58" x14ac:dyDescent="0.15">
+      <c r="T92" s="69"/>
+      <c r="V92" s="72"/>
+      <c r="AN92" s="72"/>
+      <c r="AO92" s="72"/>
+      <c r="AP92" s="72">
+        <v>1</v>
+      </c>
+      <c r="AQ92" s="72"/>
+      <c r="AR92" s="72"/>
+      <c r="AU92" s="89"/>
+      <c r="AV92" s="72"/>
+      <c r="AY92" s="72"/>
+      <c r="AZ92" s="72"/>
+    </row>
+    <row r="93" spans="1:68" x14ac:dyDescent="0.15">
       <c r="A93" s="96">
-        <v>42020008</v>
-      </c>
-      <c r="B93" s="96" t="s">
-        <v>254</v>
+        <v>42040004</v>
+      </c>
+      <c r="B93" s="98" t="s">
+        <v>612</v>
       </c>
       <c r="C93" s="8">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D93" s="8">
         <v>0</v>
       </c>
-      <c r="F93" s="8" t="s">
-        <v>253</v>
-      </c>
-      <c r="G93" s="8" t="s">
-        <v>253</v>
-      </c>
-      <c r="H93" s="8" t="s">
-        <v>459</v>
-      </c>
-      <c r="I93" s="22"/>
-      <c r="J93" s="34" t="s">
-        <v>249</v>
-      </c>
-      <c r="K93" s="34"/>
+      <c r="F93" s="72" t="s">
+        <v>609</v>
+      </c>
+      <c r="G93" s="72" t="s">
+        <v>616</v>
+      </c>
+      <c r="H93" s="72" t="s">
+        <v>611</v>
+      </c>
+      <c r="I93" s="69"/>
+      <c r="J93" s="31" t="s">
+        <v>251</v>
+      </c>
+      <c r="K93" s="90" t="s">
+        <v>601</v>
+      </c>
       <c r="L93" s="22"/>
       <c r="M93" s="22"/>
       <c r="N93" s="22"/>
       <c r="O93" s="22"/>
       <c r="P93" s="22"/>
       <c r="Q93" s="22"/>
-      <c r="R93" s="22"/>
-      <c r="T93" s="22"/>
-    </row>
-    <row r="94" spans="1:58" x14ac:dyDescent="0.15">
+      <c r="R93" s="69" t="s">
+        <v>605</v>
+      </c>
+      <c r="S93" s="24"/>
+      <c r="T93" s="69"/>
+      <c r="V93" s="72"/>
+      <c r="AN93" s="72"/>
+      <c r="AO93" s="72"/>
+      <c r="AP93" s="72"/>
+      <c r="AQ93" s="72">
+        <v>1</v>
+      </c>
+      <c r="AR93" s="72"/>
+      <c r="AU93" s="89"/>
+      <c r="AV93" s="72"/>
+      <c r="AY93" s="72"/>
+      <c r="AZ93" s="72"/>
+    </row>
+    <row r="94" spans="1:68" x14ac:dyDescent="0.15">
       <c r="A94" s="96">
-        <v>42020009</v>
-      </c>
-      <c r="B94" s="96" t="s">
-        <v>259</v>
+        <v>42040005</v>
+      </c>
+      <c r="B94" s="98" t="s">
+        <v>614</v>
       </c>
       <c r="C94" s="8">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D94" s="8">
         <v>0</v>
       </c>
-      <c r="F94" s="8" t="s">
-        <v>258</v>
-      </c>
-      <c r="G94" s="8" t="s">
-        <v>258</v>
-      </c>
-      <c r="H94" s="8" t="s">
-        <v>258</v>
-      </c>
-      <c r="I94" s="22"/>
-      <c r="J94" s="32" t="s">
-        <v>260</v>
-      </c>
-      <c r="K94" s="32"/>
+      <c r="F94" s="72" t="s">
+        <v>610</v>
+      </c>
+      <c r="G94" s="72" t="s">
+        <v>615</v>
+      </c>
+      <c r="H94" s="72" t="s">
+        <v>613</v>
+      </c>
+      <c r="I94" s="69"/>
+      <c r="J94" s="31" t="s">
+        <v>251</v>
+      </c>
+      <c r="K94" s="90" t="s">
+        <v>601</v>
+      </c>
       <c r="L94" s="22"/>
       <c r="M94" s="22"/>
       <c r="N94" s="22"/>
       <c r="O94" s="22"/>
       <c r="P94" s="22"/>
       <c r="Q94" s="22"/>
-      <c r="R94" s="22"/>
+      <c r="R94" s="69" t="s">
+        <v>605</v>
+      </c>
       <c r="S94" s="23"/>
-      <c r="T94" s="22"/>
-      <c r="AA94" s="8">
-        <v>17000001</v>
-      </c>
-      <c r="AI94" s="8">
-        <v>200</v>
-      </c>
-      <c r="AJ94" s="8">
-        <v>150</v>
-      </c>
-      <c r="AS94" s="8" t="s">
-        <v>293</v>
-      </c>
-      <c r="AY94" s="8">
-        <v>2</v>
-      </c>
-      <c r="AZ94" s="8">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="95" spans="1:58" x14ac:dyDescent="0.15">
+      <c r="T94" s="69"/>
+      <c r="V94" s="72"/>
+      <c r="AN94" s="72"/>
+      <c r="AO94" s="72"/>
+      <c r="AP94" s="72"/>
+      <c r="AQ94" s="72"/>
+      <c r="AR94" s="72">
+        <v>1</v>
+      </c>
+      <c r="AU94" s="89"/>
+      <c r="AV94" s="72"/>
+      <c r="AY94" s="72"/>
+      <c r="AZ94" s="72"/>
+    </row>
+    <row r="95" spans="1:68" x14ac:dyDescent="0.15">
       <c r="A95" s="96">
-        <v>42020010</v>
-      </c>
-      <c r="B95" s="96" t="s">
-        <v>266</v>
+        <v>42040006</v>
+      </c>
+      <c r="B95" s="98" t="s">
+        <v>618</v>
       </c>
       <c r="C95" s="8">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D95" s="8">
         <v>0</v>
       </c>
-      <c r="F95" s="8" t="s">
-        <v>267</v>
-      </c>
-      <c r="G95" s="8" t="s">
-        <v>265</v>
-      </c>
-      <c r="H95" s="8" t="s">
-        <v>265</v>
-      </c>
-      <c r="I95" s="22"/>
-      <c r="J95" s="32" t="s">
-        <v>260</v>
-      </c>
-      <c r="K95" s="32"/>
+      <c r="E95" s="8">
+        <v>1</v>
+      </c>
+      <c r="F95" s="72" t="s">
+        <v>617</v>
+      </c>
+      <c r="G95" s="72" t="s">
+        <v>617</v>
+      </c>
+      <c r="H95" s="72" t="s">
+        <v>656</v>
+      </c>
+      <c r="I95" s="69"/>
+      <c r="J95" s="78" t="s">
+        <v>562</v>
+      </c>
+      <c r="K95" s="90" t="s">
+        <v>601</v>
+      </c>
       <c r="L95" s="22"/>
       <c r="M95" s="22"/>
       <c r="N95" s="22"/>
       <c r="O95" s="22"/>
       <c r="P95" s="22"/>
       <c r="Q95" s="22"/>
-      <c r="R95" s="22"/>
+      <c r="R95" s="69"/>
       <c r="S95" s="23"/>
-      <c r="T95" s="22"/>
-      <c r="AA95" s="8">
-        <v>17000003</v>
-      </c>
-      <c r="AI95" s="8">
-        <v>250</v>
-      </c>
-      <c r="AY95" s="8">
+      <c r="T95" s="69"/>
+      <c r="V95" s="72"/>
+      <c r="AE95" s="72" t="s">
+        <v>657</v>
+      </c>
+      <c r="AF95" s="8">
+        <v>1</v>
+      </c>
+      <c r="AN95" s="72"/>
+      <c r="AO95" s="72"/>
+      <c r="AP95" s="72"/>
+      <c r="AQ95" s="72"/>
+      <c r="AR95" s="72"/>
+      <c r="AU95" s="89"/>
+      <c r="AV95" s="72"/>
+      <c r="AY95" s="72"/>
+      <c r="AZ95" s="72"/>
+      <c r="BD95" s="8">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="96" spans="1:68" x14ac:dyDescent="0.15">
+      <c r="A96" s="96">
+        <v>42040007</v>
+      </c>
+      <c r="B96" s="98" t="s">
+        <v>620</v>
+      </c>
+      <c r="C96" s="8">
         <v>5</v>
       </c>
-      <c r="AZ95" s="8">
-        <v>100</v>
-      </c>
-      <c r="BE95" s="8">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="96" spans="1:58" x14ac:dyDescent="0.15">
-      <c r="A96" s="96">
-        <v>42020011</v>
-      </c>
-      <c r="B96" s="96" t="s">
-        <v>269</v>
-      </c>
-      <c r="C96" s="8">
-        <v>3</v>
-      </c>
       <c r="D96" s="8">
         <v>0</v>
       </c>
-      <c r="F96" s="8" t="s">
-        <v>270</v>
-      </c>
-      <c r="G96" s="8" t="s">
-        <v>268</v>
-      </c>
-      <c r="H96" s="8" t="s">
-        <v>268</v>
-      </c>
-      <c r="I96" s="22"/>
-      <c r="J96" s="32" t="s">
-        <v>260</v>
-      </c>
-      <c r="K96" s="32"/>
+      <c r="E96" s="8">
+        <v>1</v>
+      </c>
+      <c r="F96" s="72" t="s">
+        <v>619</v>
+      </c>
+      <c r="G96" s="72" t="s">
+        <v>619</v>
+      </c>
+      <c r="H96" s="72" t="s">
+        <v>663</v>
+      </c>
+      <c r="I96" s="69" t="s">
+        <v>662</v>
+      </c>
+      <c r="J96" s="78" t="s">
+        <v>562</v>
+      </c>
+      <c r="K96" s="90" t="s">
+        <v>601</v>
+      </c>
       <c r="L96" s="22"/>
       <c r="M96" s="22"/>
       <c r="N96" s="22"/>
       <c r="O96" s="22"/>
       <c r="P96" s="22"/>
       <c r="Q96" s="22"/>
-      <c r="R96" s="22"/>
-      <c r="T96" s="22"/>
-      <c r="AA96" s="8">
-        <v>17000002</v>
-      </c>
-      <c r="AS96" s="8" t="s">
-        <v>294</v>
-      </c>
-      <c r="AW96" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="97" spans="1:68" x14ac:dyDescent="0.15">
+      <c r="R96" s="69"/>
+      <c r="S96" s="24"/>
+      <c r="T96" s="69"/>
+      <c r="V96" s="72"/>
+      <c r="AN96" s="72"/>
+      <c r="AO96" s="72"/>
+      <c r="AP96" s="72"/>
+      <c r="AQ96" s="72"/>
+      <c r="AR96" s="72"/>
+      <c r="AU96" s="89"/>
+      <c r="AV96" s="72"/>
+      <c r="AY96" s="72"/>
+      <c r="AZ96" s="72"/>
+      <c r="BC96" s="8">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="97" spans="1:58" x14ac:dyDescent="0.15">
       <c r="A97" s="96">
-        <v>42020012</v>
-      </c>
-      <c r="B97" s="96" t="s">
-        <v>398</v>
+        <v>42040008</v>
+      </c>
+      <c r="B97" s="98" t="s">
+        <v>622</v>
       </c>
       <c r="C97" s="8">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D97" s="8">
         <v>0</v>
       </c>
-      <c r="F97" s="8" t="s">
-        <v>412</v>
-      </c>
-      <c r="G97" s="8" t="s">
-        <v>402</v>
+      <c r="E97" s="8">
+        <v>2</v>
+      </c>
+      <c r="F97" s="72" t="s">
+        <v>665</v>
+      </c>
+      <c r="G97" s="72" t="s">
+        <v>621</v>
       </c>
       <c r="H97" s="72" t="s">
-        <v>402</v>
-      </c>
-      <c r="I97" s="22"/>
-      <c r="J97" s="35" t="s">
-        <v>396</v>
-      </c>
-      <c r="K97" s="35"/>
+        <v>656</v>
+      </c>
+      <c r="I97" s="69"/>
+      <c r="J97" s="78" t="s">
+        <v>562</v>
+      </c>
+      <c r="K97" s="90" t="s">
+        <v>601</v>
+      </c>
       <c r="L97" s="22"/>
       <c r="M97" s="22"/>
       <c r="N97" s="22"/>
       <c r="O97" s="22"/>
       <c r="P97" s="22"/>
       <c r="Q97" s="22"/>
-      <c r="R97" s="22"/>
-      <c r="T97" s="22"/>
-      <c r="AB97" s="8" t="s">
-        <v>397</v>
-      </c>
-      <c r="AI97" s="8">
+      <c r="R97" s="69"/>
+      <c r="S97" s="24"/>
+      <c r="T97" s="69"/>
+      <c r="V97" s="72"/>
+      <c r="AE97" s="72" t="s">
+        <v>658</v>
+      </c>
+      <c r="AF97" s="8">
+        <v>2</v>
+      </c>
+      <c r="AG97" s="72" t="s">
+        <v>659</v>
+      </c>
+      <c r="AH97" s="8">
+        <v>0</v>
+      </c>
+      <c r="AN97" s="72"/>
+      <c r="AO97" s="72"/>
+      <c r="AP97" s="72"/>
+      <c r="AQ97" s="72"/>
+      <c r="AR97" s="72"/>
+      <c r="AU97" s="89"/>
+      <c r="AV97" s="72"/>
+      <c r="AY97" s="72"/>
+      <c r="AZ97" s="72"/>
+      <c r="BD97" s="8">
         <v>150</v>
       </c>
-      <c r="AT97" s="24" t="s">
-        <v>399</v>
-      </c>
-      <c r="AU97" s="24"/>
-      <c r="AV97" s="24"/>
-      <c r="AY97" s="8">
-        <v>6</v>
-      </c>
-      <c r="AZ97" s="8">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="98" spans="1:68" x14ac:dyDescent="0.15">
+    </row>
+    <row r="98" spans="1:58" x14ac:dyDescent="0.15">
       <c r="A98" s="96">
-        <v>42020013</v>
-      </c>
-      <c r="B98" s="96" t="s">
-        <v>423</v>
+        <v>42040009</v>
+      </c>
+      <c r="B98" s="98" t="s">
+        <v>624</v>
       </c>
       <c r="C98" s="8">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D98" s="8">
         <v>0</v>
       </c>
-      <c r="F98" s="8" t="s">
-        <v>438</v>
-      </c>
-      <c r="G98" s="8" t="s">
-        <v>425</v>
-      </c>
-      <c r="H98" s="8" t="s">
-        <v>424</v>
-      </c>
-      <c r="I98" s="22"/>
-      <c r="J98" s="36" t="s">
-        <v>431</v>
-      </c>
-      <c r="K98" s="36"/>
+      <c r="E98" s="8">
+        <v>1</v>
+      </c>
+      <c r="F98" s="72" t="s">
+        <v>623</v>
+      </c>
+      <c r="G98" s="72" t="s">
+        <v>623</v>
+      </c>
+      <c r="H98" s="72" t="s">
+        <v>656</v>
+      </c>
+      <c r="I98" s="69"/>
+      <c r="J98" s="78" t="s">
+        <v>562</v>
+      </c>
+      <c r="K98" s="90" t="s">
+        <v>601</v>
+      </c>
       <c r="L98" s="22"/>
       <c r="M98" s="22"/>
       <c r="N98" s="22"/>
       <c r="O98" s="22"/>
       <c r="P98" s="22"/>
       <c r="Q98" s="22"/>
-      <c r="R98" s="22"/>
-      <c r="T98" s="22"/>
-      <c r="Y98" s="8" t="s">
-        <v>428</v>
-      </c>
-      <c r="AT98" s="24"/>
-      <c r="AU98" s="24"/>
-      <c r="AV98" s="24"/>
-    </row>
-    <row r="99" spans="1:68" x14ac:dyDescent="0.15">
+      <c r="R98" s="69"/>
+      <c r="S98" s="24"/>
+      <c r="T98" s="69"/>
+      <c r="V98" s="72"/>
+      <c r="AE98" s="72" t="s">
+        <v>660</v>
+      </c>
+      <c r="AF98" s="8">
+        <v>1</v>
+      </c>
+      <c r="AN98" s="72"/>
+      <c r="AO98" s="72"/>
+      <c r="AP98" s="72"/>
+      <c r="AQ98" s="72"/>
+      <c r="AR98" s="72"/>
+      <c r="AU98" s="89"/>
+      <c r="AV98" s="72"/>
+      <c r="AY98" s="72"/>
+      <c r="AZ98" s="72"/>
+      <c r="BD98" s="8">
+        <v>50</v>
+      </c>
+      <c r="BE98" s="8">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="99" spans="1:58" x14ac:dyDescent="0.15">
       <c r="A99" s="96">
-        <v>42020014</v>
-      </c>
-      <c r="B99" s="96" t="s">
-        <v>426</v>
+        <v>42040010</v>
+      </c>
+      <c r="B99" s="98" t="s">
+        <v>626</v>
       </c>
       <c r="C99" s="8">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D99" s="8">
         <v>0</v>
       </c>
-      <c r="F99" s="8" t="s">
-        <v>427</v>
-      </c>
-      <c r="G99" s="8" t="s">
-        <v>425</v>
-      </c>
-      <c r="H99" s="8" t="s">
-        <v>427</v>
-      </c>
-      <c r="I99" s="22"/>
-      <c r="J99" s="31" t="s">
-        <v>251</v>
-      </c>
-      <c r="K99" s="31"/>
+      <c r="E99" s="8">
+        <v>1</v>
+      </c>
+      <c r="F99" s="72" t="s">
+        <v>625</v>
+      </c>
+      <c r="G99" s="72" t="s">
+        <v>625</v>
+      </c>
+      <c r="H99" s="72" t="s">
+        <v>656</v>
+      </c>
+      <c r="I99" s="69"/>
+      <c r="J99" s="78" t="s">
+        <v>562</v>
+      </c>
+      <c r="K99" s="90" t="s">
+        <v>601</v>
+      </c>
       <c r="L99" s="22"/>
       <c r="M99" s="22"/>
       <c r="N99" s="22"/>
       <c r="O99" s="22"/>
       <c r="P99" s="22"/>
       <c r="Q99" s="22"/>
-      <c r="R99" s="22"/>
-      <c r="T99" s="22"/>
-      <c r="AJ99" s="8">
-        <v>50</v>
-      </c>
-      <c r="AK99" s="8">
-        <v>50</v>
-      </c>
-      <c r="AL99" s="8">
-        <v>50</v>
-      </c>
-      <c r="AM99" s="8">
-        <v>50</v>
-      </c>
-      <c r="AT99" s="24"/>
-      <c r="AU99" s="24"/>
-      <c r="AV99" s="24"/>
-      <c r="AW99" s="8">
+      <c r="R99" s="69"/>
+      <c r="S99" s="24"/>
+      <c r="T99" s="69"/>
+      <c r="V99" s="72"/>
+      <c r="AE99" s="72" t="s">
+        <v>658</v>
+      </c>
+      <c r="AF99" s="8">
         <v>1</v>
       </c>
-    </row>
-    <row r="100" spans="1:68" x14ac:dyDescent="0.15">
+      <c r="AN99" s="72"/>
+      <c r="AO99" s="72"/>
+      <c r="AP99" s="72"/>
+      <c r="AQ99" s="72"/>
+      <c r="AR99" s="72"/>
+      <c r="AU99" s="89"/>
+      <c r="AV99" s="72"/>
+      <c r="AY99" s="72"/>
+      <c r="AZ99" s="72"/>
+      <c r="BD99" s="8">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="100" spans="1:58" x14ac:dyDescent="0.15">
       <c r="A100" s="96">
-        <v>42020015</v>
-      </c>
-      <c r="B100" s="96" t="s">
-        <v>429</v>
+        <v>42040011</v>
+      </c>
+      <c r="B100" s="98" t="s">
+        <v>628</v>
       </c>
       <c r="C100" s="8">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D100" s="8">
         <v>0</v>
       </c>
-      <c r="F100" s="8" t="s">
-        <v>432</v>
-      </c>
-      <c r="G100" s="8" t="s">
-        <v>441</v>
-      </c>
-      <c r="H100" s="8" t="s">
-        <v>432</v>
-      </c>
-      <c r="I100" s="22"/>
-      <c r="J100" s="36" t="s">
-        <v>431</v>
-      </c>
-      <c r="K100" s="36"/>
+      <c r="E100" s="8">
+        <v>2</v>
+      </c>
+      <c r="F100" s="72" t="s">
+        <v>627</v>
+      </c>
+      <c r="G100" s="72" t="s">
+        <v>627</v>
+      </c>
+      <c r="H100" s="72" t="s">
+        <v>656</v>
+      </c>
+      <c r="I100" s="69" t="s">
+        <v>662</v>
+      </c>
+      <c r="J100" s="78" t="s">
+        <v>562</v>
+      </c>
+      <c r="K100" s="90" t="s">
+        <v>601</v>
+      </c>
       <c r="L100" s="22"/>
       <c r="M100" s="22"/>
       <c r="N100" s="22"/>
       <c r="O100" s="22"/>
       <c r="P100" s="22"/>
       <c r="Q100" s="22"/>
-      <c r="R100" s="22"/>
-      <c r="T100" s="22"/>
-      <c r="Y100" s="8" t="s">
-        <v>437</v>
-      </c>
-      <c r="AJ100" s="8">
-        <v>50</v>
-      </c>
-      <c r="AK100" s="8">
-        <v>50</v>
-      </c>
-      <c r="AT100" s="24"/>
-      <c r="AU100" s="24"/>
-      <c r="AV100" s="24"/>
-    </row>
-    <row r="101" spans="1:68" x14ac:dyDescent="0.15">
+      <c r="R100" s="69"/>
+      <c r="S100" s="24"/>
+      <c r="T100" s="69"/>
+      <c r="V100" s="72"/>
+      <c r="AE100" s="72" t="s">
+        <v>657</v>
+      </c>
+      <c r="AF100" s="8">
+        <v>2</v>
+      </c>
+      <c r="AG100" s="72" t="s">
+        <v>661</v>
+      </c>
+      <c r="AH100" s="8">
+        <v>0</v>
+      </c>
+      <c r="AN100" s="72"/>
+      <c r="AO100" s="72"/>
+      <c r="AP100" s="72"/>
+      <c r="AQ100" s="72"/>
+      <c r="AR100" s="72"/>
+      <c r="AU100" s="89"/>
+      <c r="AV100" s="72"/>
+      <c r="AY100" s="72"/>
+      <c r="AZ100" s="72"/>
+      <c r="BD100" s="8">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="101" spans="1:58" x14ac:dyDescent="0.15">
       <c r="A101" s="96">
-        <v>42020016</v>
-      </c>
-      <c r="B101" s="96" t="s">
-        <v>430</v>
+        <v>42040012</v>
+      </c>
+      <c r="B101" s="98" t="s">
+        <v>630</v>
       </c>
       <c r="C101" s="8">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D101" s="8">
         <v>0</v>
       </c>
-      <c r="F101" s="8" t="s">
-        <v>434</v>
-      </c>
-      <c r="G101" s="8" t="s">
-        <v>433</v>
-      </c>
-      <c r="H101" s="8" t="s">
-        <v>434</v>
-      </c>
-      <c r="I101" s="22"/>
-      <c r="J101" s="31" t="s">
-        <v>251</v>
-      </c>
-      <c r="K101" s="31"/>
+      <c r="E101" s="8">
+        <v>1</v>
+      </c>
+      <c r="F101" s="72" t="s">
+        <v>629</v>
+      </c>
+      <c r="G101" s="72" t="s">
+        <v>629</v>
+      </c>
+      <c r="H101" s="72" t="s">
+        <v>656</v>
+      </c>
+      <c r="I101" s="69" t="s">
+        <v>662</v>
+      </c>
+      <c r="J101" s="78" t="s">
+        <v>562</v>
+      </c>
+      <c r="K101" s="90" t="s">
+        <v>601</v>
+      </c>
       <c r="L101" s="22"/>
       <c r="M101" s="22"/>
       <c r="N101" s="22"/>
       <c r="O101" s="22"/>
       <c r="P101" s="22"/>
       <c r="Q101" s="22"/>
-      <c r="R101" s="22"/>
-      <c r="S101" s="8" t="s">
-        <v>439</v>
-      </c>
-      <c r="T101" s="22" t="s">
-        <v>508</v>
-      </c>
-      <c r="AI101" s="8">
-        <v>400</v>
-      </c>
-      <c r="AK101" s="8">
-        <v>150</v>
-      </c>
-      <c r="AL101" s="8">
-        <v>150</v>
-      </c>
-      <c r="AS101" s="8" t="s">
-        <v>440</v>
-      </c>
-      <c r="AT101" s="24"/>
-      <c r="AU101" s="24"/>
-      <c r="AV101" s="24"/>
-      <c r="AY101" s="8">
-        <v>7</v>
-      </c>
-      <c r="AZ101" s="8">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="102" spans="1:68" x14ac:dyDescent="0.15">
+      <c r="R101" s="69"/>
+      <c r="S101" s="24"/>
+      <c r="T101" s="69"/>
+      <c r="V101" s="72"/>
+      <c r="AE101" s="72" t="s">
+        <v>658</v>
+      </c>
+      <c r="AF101" s="8">
+        <v>0</v>
+      </c>
+      <c r="AG101" s="72" t="s">
+        <v>660</v>
+      </c>
+      <c r="AH101" s="8">
+        <v>0</v>
+      </c>
+      <c r="AN101" s="72"/>
+      <c r="AO101" s="72"/>
+      <c r="AP101" s="72"/>
+      <c r="AQ101" s="72"/>
+      <c r="AR101" s="72"/>
+      <c r="AU101" s="89"/>
+      <c r="AV101" s="72"/>
+      <c r="AY101" s="72"/>
+      <c r="AZ101" s="72"/>
+      <c r="BC101" s="8">
+        <v>50</v>
+      </c>
+      <c r="BF101" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="102" spans="1:58" x14ac:dyDescent="0.15">
       <c r="A102" s="96">
-        <v>42020017</v>
-      </c>
-      <c r="B102" s="96" t="s">
-        <v>449</v>
+        <v>42040013</v>
+      </c>
+      <c r="B102" s="98" t="s">
+        <v>632</v>
       </c>
       <c r="C102" s="8">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D102" s="8">
         <v>0</v>
       </c>
-      <c r="F102" s="8" t="s">
-        <v>453</v>
-      </c>
-      <c r="G102" s="8" t="s">
-        <v>448</v>
-      </c>
-      <c r="H102" s="8" t="s">
-        <v>451</v>
-      </c>
-      <c r="I102" s="22"/>
-      <c r="J102" s="31" t="s">
-        <v>251</v>
-      </c>
-      <c r="K102" s="31"/>
+      <c r="E102" s="8">
+        <v>1</v>
+      </c>
+      <c r="F102" s="72" t="s">
+        <v>631</v>
+      </c>
+      <c r="G102" s="72" t="s">
+        <v>631</v>
+      </c>
+      <c r="H102" s="72" t="s">
+        <v>656</v>
+      </c>
+      <c r="I102" s="69"/>
+      <c r="J102" s="78" t="s">
+        <v>562</v>
+      </c>
+      <c r="K102" s="90" t="s">
+        <v>601</v>
+      </c>
       <c r="L102" s="22"/>
       <c r="M102" s="22"/>
       <c r="N102" s="22"/>
       <c r="O102" s="22"/>
       <c r="P102" s="22"/>
       <c r="Q102" s="22"/>
-      <c r="R102" s="22"/>
-      <c r="T102" s="22"/>
-      <c r="AS102" s="8" t="s">
-        <v>452</v>
-      </c>
-      <c r="AT102" s="24"/>
-      <c r="AU102" s="24"/>
-      <c r="AV102" s="24"/>
-    </row>
-    <row r="103" spans="1:68" x14ac:dyDescent="0.15">
+      <c r="R102" s="69"/>
+      <c r="S102" s="24"/>
+      <c r="T102" s="69"/>
+      <c r="V102" s="72"/>
+      <c r="AE102" s="72" t="s">
+        <v>657</v>
+      </c>
+      <c r="AF102" s="8">
+        <v>0</v>
+      </c>
+      <c r="AG102" s="72" t="s">
+        <v>659</v>
+      </c>
+      <c r="AH102" s="8">
+        <v>1</v>
+      </c>
+      <c r="AN102" s="72"/>
+      <c r="AO102" s="72"/>
+      <c r="AP102" s="72"/>
+      <c r="AQ102" s="72"/>
+      <c r="AR102" s="72"/>
+      <c r="AU102" s="89"/>
+      <c r="AV102" s="72"/>
+      <c r="AY102" s="72"/>
+      <c r="AZ102" s="72"/>
+      <c r="BD102" s="8">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="103" spans="1:58" x14ac:dyDescent="0.15">
       <c r="A103" s="96">
-        <v>42020018</v>
-      </c>
-      <c r="B103" s="96" t="s">
-        <v>492</v>
+        <v>42040014</v>
+      </c>
+      <c r="B103" s="98" t="s">
+        <v>634</v>
       </c>
       <c r="C103" s="8">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D103" s="8">
         <v>0</v>
       </c>
       <c r="E103" s="8">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F103" s="72" t="s">
-        <v>491</v>
+        <v>664</v>
       </c>
       <c r="G103" s="72" t="s">
-        <v>491</v>
-      </c>
-      <c r="H103" s="8" t="s">
-        <v>491</v>
-      </c>
-      <c r="I103" s="22"/>
-      <c r="J103" s="30" t="s">
-        <v>248</v>
-      </c>
-      <c r="K103" s="30"/>
+        <v>633</v>
+      </c>
+      <c r="H103" s="72" t="s">
+        <v>656</v>
+      </c>
+      <c r="I103" s="69" t="s">
+        <v>662</v>
+      </c>
+      <c r="J103" s="78" t="s">
+        <v>562</v>
+      </c>
+      <c r="K103" s="90" t="s">
+        <v>601</v>
+      </c>
       <c r="L103" s="22"/>
       <c r="M103" s="22"/>
       <c r="N103" s="22"/>
       <c r="O103" s="22"/>
       <c r="P103" s="22"/>
       <c r="Q103" s="22"/>
-      <c r="R103" s="22"/>
-      <c r="S103" s="24" t="s">
-        <v>493</v>
-      </c>
-      <c r="T103" s="22" t="s">
-        <v>508</v>
-      </c>
-      <c r="AI103" s="8">
-        <v>150</v>
-      </c>
-      <c r="AM103" s="8">
-        <v>300</v>
-      </c>
-      <c r="AT103" s="24" t="s">
-        <v>494</v>
-      </c>
-      <c r="AU103" s="24"/>
-      <c r="AV103" s="24"/>
-      <c r="AY103" s="8">
-        <v>7</v>
-      </c>
-      <c r="AZ103" s="8">
-        <v>100</v>
-      </c>
+      <c r="R103" s="69"/>
+      <c r="S103" s="24"/>
+      <c r="T103" s="69"/>
+      <c r="V103" s="72"/>
+      <c r="AE103" s="72" t="s">
+        <v>658</v>
+      </c>
+      <c r="AF103" s="8">
+        <v>1</v>
+      </c>
+      <c r="AN103" s="72"/>
+      <c r="AO103" s="72"/>
+      <c r="AP103" s="72"/>
+      <c r="AQ103" s="72"/>
+      <c r="AR103" s="72"/>
+      <c r="AU103" s="89"/>
+      <c r="AV103" s="72"/>
+      <c r="AY103" s="72"/>
+      <c r="AZ103" s="72"/>
       <c r="BD103" s="8">
         <v>100</v>
       </c>
-      <c r="BE103" s="8">
-        <v>60</v>
-      </c>
-      <c r="BF103" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="104" spans="1:68" x14ac:dyDescent="0.15">
+    </row>
+    <row r="104" spans="1:58" x14ac:dyDescent="0.15">
       <c r="A104" s="96">
-        <v>42020019</v>
-      </c>
-      <c r="B104" s="96" t="s">
-        <v>510</v>
+        <v>42040015</v>
+      </c>
+      <c r="B104" s="98" t="s">
+        <v>636</v>
       </c>
       <c r="C104" s="8">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D104" s="8">
         <v>0</v>
       </c>
-      <c r="F104" s="8" t="s">
-        <v>509</v>
-      </c>
-      <c r="G104" s="8" t="s">
-        <v>509</v>
-      </c>
-      <c r="H104" s="8" t="s">
-        <v>509</v>
-      </c>
-      <c r="I104" s="22"/>
-      <c r="J104" s="27" t="s">
-        <v>513</v>
-      </c>
-      <c r="K104" s="27"/>
+      <c r="E104" s="8">
+        <v>2</v>
+      </c>
+      <c r="F104" s="72" t="s">
+        <v>635</v>
+      </c>
+      <c r="G104" s="72" t="s">
+        <v>635</v>
+      </c>
+      <c r="H104" s="72" t="s">
+        <v>619</v>
+      </c>
+      <c r="I104" s="69" t="s">
+        <v>662</v>
+      </c>
+      <c r="J104" s="78" t="s">
+        <v>562</v>
+      </c>
+      <c r="K104" s="90" t="s">
+        <v>601</v>
+      </c>
       <c r="L104" s="22"/>
       <c r="M104" s="22"/>
       <c r="N104" s="22"/>
       <c r="O104" s="22"/>
       <c r="P104" s="22"/>
       <c r="Q104" s="22"/>
-      <c r="R104" s="22"/>
-      <c r="T104" s="22"/>
-      <c r="BL104" s="8">
-        <v>-1</v>
-      </c>
-      <c r="BP104" s="8" t="s">
-        <v>511</v>
-      </c>
-    </row>
-    <row r="105" spans="1:68" x14ac:dyDescent="0.15">
-      <c r="A105" s="8">
-        <v>42030001</v>
-      </c>
-      <c r="B105" s="8" t="s">
-        <v>117</v>
+      <c r="R104" s="69"/>
+      <c r="S104" s="24"/>
+      <c r="T104" s="69"/>
+      <c r="V104" s="72"/>
+      <c r="AE104" s="72" t="s">
+        <v>658</v>
+      </c>
+      <c r="AF104" s="8">
+        <v>2</v>
+      </c>
+      <c r="AG104" s="72" t="s">
+        <v>661</v>
+      </c>
+      <c r="AH104" s="8">
+        <v>2</v>
+      </c>
+      <c r="AN104" s="72"/>
+      <c r="AO104" s="72"/>
+      <c r="AP104" s="72"/>
+      <c r="AQ104" s="72"/>
+      <c r="AR104" s="72"/>
+      <c r="AU104" s="89"/>
+      <c r="AV104" s="72"/>
+      <c r="AY104" s="72"/>
+      <c r="AZ104" s="72"/>
+      <c r="BD104" s="8">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="105" spans="1:58" x14ac:dyDescent="0.15">
+      <c r="A105" s="96">
+        <v>42040016</v>
+      </c>
+      <c r="B105" s="98" t="s">
+        <v>638</v>
       </c>
       <c r="C105" s="8">
+        <v>5</v>
+      </c>
+      <c r="D105" s="8">
+        <v>0</v>
+      </c>
+      <c r="E105" s="8">
         <v>1</v>
       </c>
-      <c r="D105" s="8">
-        <v>0</v>
-      </c>
-      <c r="F105" s="8" t="s">
-        <v>312</v>
-      </c>
-      <c r="G105" s="8" t="s">
-        <v>119</v>
+      <c r="F105" s="72" t="s">
+        <v>637</v>
+      </c>
+      <c r="G105" s="72" t="s">
+        <v>637</v>
       </c>
       <c r="H105" s="72" t="s">
-        <v>120</v>
-      </c>
-      <c r="I105" s="22"/>
-      <c r="J105" s="29" t="s">
-        <v>250</v>
-      </c>
-      <c r="K105" s="29"/>
+        <v>637</v>
+      </c>
+      <c r="I105" s="69"/>
+      <c r="J105" s="78" t="s">
+        <v>562</v>
+      </c>
+      <c r="K105" s="28" t="s">
+        <v>247</v>
+      </c>
       <c r="L105" s="22"/>
       <c r="M105" s="22"/>
       <c r="N105" s="22"/>
       <c r="O105" s="22"/>
       <c r="P105" s="22"/>
       <c r="Q105" s="22"/>
-      <c r="R105" s="22"/>
+      <c r="R105" s="69"/>
       <c r="S105" s="24"/>
-      <c r="T105" s="22"/>
-      <c r="X105" s="8" t="s">
-        <v>348</v>
-      </c>
-      <c r="AJ105" s="8">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="106" spans="1:68" x14ac:dyDescent="0.15">
-      <c r="A106" s="8">
-        <v>42030002</v>
-      </c>
-      <c r="B106" s="8" t="s">
-        <v>118</v>
+      <c r="T105" s="69"/>
+      <c r="V105" s="72"/>
+      <c r="AE105" s="72" t="s">
+        <v>658</v>
+      </c>
+      <c r="AF105" s="8">
+        <v>3</v>
+      </c>
+      <c r="AG105" s="72" t="s">
+        <v>659</v>
+      </c>
+      <c r="AH105" s="8">
+        <v>2</v>
+      </c>
+      <c r="AN105" s="72"/>
+      <c r="AO105" s="72"/>
+      <c r="AP105" s="72"/>
+      <c r="AQ105" s="72"/>
+      <c r="AR105" s="72"/>
+      <c r="AT105" s="24"/>
+      <c r="AU105" s="89"/>
+      <c r="AV105" s="72"/>
+      <c r="AY105" s="72"/>
+      <c r="AZ105" s="72"/>
+      <c r="BD105" s="8">
+        <v>30</v>
+      </c>
+      <c r="BE105" s="8">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="106" spans="1:58" x14ac:dyDescent="0.15">
+      <c r="A106" s="96">
+        <v>42040017</v>
+      </c>
+      <c r="B106" s="98" t="s">
+        <v>640</v>
       </c>
       <c r="C106" s="8">
+        <v>5</v>
+      </c>
+      <c r="D106" s="8">
+        <v>0</v>
+      </c>
+      <c r="E106" s="8">
         <v>1</v>
       </c>
-      <c r="D106" s="8">
-        <v>0</v>
-      </c>
-      <c r="E106" s="8">
-        <v>2</v>
-      </c>
-      <c r="F106" s="8" t="s">
-        <v>121</v>
-      </c>
-      <c r="G106" s="8" t="s">
-        <v>119</v>
-      </c>
-      <c r="H106" s="8" t="s">
-        <v>122</v>
-      </c>
-      <c r="I106" s="22"/>
-      <c r="J106" s="30" t="s">
-        <v>248</v>
-      </c>
-      <c r="K106" s="30"/>
+      <c r="F106" s="72" t="s">
+        <v>639</v>
+      </c>
+      <c r="G106" s="72" t="s">
+        <v>639</v>
+      </c>
+      <c r="H106" s="72" t="s">
+        <v>656</v>
+      </c>
+      <c r="I106" s="69" t="s">
+        <v>662</v>
+      </c>
+      <c r="J106" s="78" t="s">
+        <v>562</v>
+      </c>
+      <c r="K106" s="90" t="s">
+        <v>601</v>
+      </c>
       <c r="L106" s="22"/>
       <c r="M106" s="22"/>
       <c r="N106" s="22"/>
       <c r="O106" s="22"/>
       <c r="P106" s="22"/>
       <c r="Q106" s="22"/>
-      <c r="R106" s="22"/>
-      <c r="S106" s="24" t="s">
-        <v>330</v>
-      </c>
-      <c r="T106" s="22" t="s">
-        <v>508</v>
-      </c>
-      <c r="AI106" s="8">
-        <v>200</v>
-      </c>
-      <c r="AJ106" s="8">
-        <v>100</v>
-      </c>
-      <c r="AM106" s="8">
-        <v>100</v>
-      </c>
-      <c r="AT106" s="23" t="s">
-        <v>400</v>
-      </c>
-      <c r="AY106" s="8">
-        <v>5</v>
-      </c>
-      <c r="AZ106" s="8">
-        <v>100</v>
-      </c>
+      <c r="R106" s="69"/>
+      <c r="S106" s="24"/>
+      <c r="T106" s="69"/>
+      <c r="V106" s="72"/>
+      <c r="AE106" s="72" t="s">
+        <v>659</v>
+      </c>
+      <c r="AF106" s="8">
+        <v>3</v>
+      </c>
+      <c r="AN106" s="72"/>
+      <c r="AO106" s="72"/>
+      <c r="AP106" s="72"/>
+      <c r="AQ106" s="72"/>
+      <c r="AR106" s="72"/>
+      <c r="AT106" s="23"/>
+      <c r="AU106" s="89"/>
+      <c r="AV106" s="72"/>
+      <c r="AY106" s="72"/>
+      <c r="AZ106" s="72"/>
       <c r="BD106" s="8">
         <v>100</v>
       </c>
     </row>
-    <row r="107" spans="1:68" x14ac:dyDescent="0.15">
-      <c r="A107" s="8">
-        <v>42030003</v>
-      </c>
-      <c r="B107" s="8" t="s">
-        <v>463</v>
+    <row r="107" spans="1:58" x14ac:dyDescent="0.15">
+      <c r="A107" s="96">
+        <v>42040018</v>
+      </c>
+      <c r="B107" s="98" t="s">
+        <v>642</v>
       </c>
       <c r="C107" s="8">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D107" s="8">
         <v>0</v>
       </c>
       <c r="E107" s="8">
-        <v>3</v>
-      </c>
-      <c r="F107" s="8" t="s">
-        <v>465</v>
-      </c>
-      <c r="G107" s="8" t="s">
-        <v>462</v>
-      </c>
-      <c r="H107" s="8" t="s">
-        <v>465</v>
-      </c>
-      <c r="I107" s="22"/>
-      <c r="J107" s="29" t="s">
-        <v>250</v>
-      </c>
-      <c r="K107" s="29"/>
+        <v>2</v>
+      </c>
+      <c r="F107" s="72" t="s">
+        <v>641</v>
+      </c>
+      <c r="G107" s="72" t="s">
+        <v>641</v>
+      </c>
+      <c r="H107" s="72" t="s">
+        <v>656</v>
+      </c>
+      <c r="I107" s="69" t="s">
+        <v>662</v>
+      </c>
+      <c r="J107" s="78" t="s">
+        <v>562</v>
+      </c>
+      <c r="K107" s="90" t="s">
+        <v>601</v>
+      </c>
       <c r="L107" s="22"/>
       <c r="M107" s="22"/>
       <c r="N107" s="22"/>
       <c r="O107" s="22"/>
       <c r="P107" s="22"/>
       <c r="Q107" s="22"/>
-      <c r="R107" s="22"/>
-      <c r="T107" s="22"/>
-      <c r="X107" s="8" t="s">
-        <v>467</v>
-      </c>
+      <c r="R107" s="69"/>
+      <c r="S107" s="24"/>
+      <c r="T107" s="69"/>
+      <c r="V107" s="72"/>
+      <c r="AE107" s="72" t="s">
+        <v>657</v>
+      </c>
+      <c r="AF107" s="8">
+        <v>1</v>
+      </c>
+      <c r="AG107" s="72" t="s">
+        <v>655</v>
+      </c>
+      <c r="AH107" s="8">
+        <v>1</v>
+      </c>
+      <c r="AN107" s="72"/>
+      <c r="AO107" s="72"/>
+      <c r="AP107" s="72"/>
+      <c r="AQ107" s="72"/>
+      <c r="AR107" s="72"/>
+      <c r="AU107" s="89"/>
+      <c r="AV107" s="72"/>
+      <c r="AY107" s="72"/>
+      <c r="AZ107" s="72"/>
       <c r="BD107" s="8">
-        <v>150</v>
-      </c>
-      <c r="BE107" s="8">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="108" spans="1:68" x14ac:dyDescent="0.15">
-      <c r="A108" s="8">
-        <v>42030004</v>
-      </c>
-      <c r="B108" s="8" t="s">
-        <v>464</v>
+        <v>200</v>
+      </c>
+    </row>
+    <row r="108" spans="1:58" x14ac:dyDescent="0.15">
+      <c r="A108" s="96">
+        <v>42040019</v>
+      </c>
+      <c r="B108" s="98" t="s">
+        <v>670</v>
       </c>
       <c r="C108" s="8">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D108" s="8">
         <v>0</v>
       </c>
-      <c r="E108" s="8">
-        <v>3</v>
-      </c>
-      <c r="F108" s="8" t="s">
-        <v>467</v>
-      </c>
-      <c r="G108" s="8" t="s">
-        <v>462</v>
-      </c>
-      <c r="H108" s="8" t="s">
-        <v>466</v>
-      </c>
-      <c r="I108" s="22"/>
-      <c r="J108" s="30" t="s">
-        <v>248</v>
-      </c>
-      <c r="K108" s="30"/>
+      <c r="F108" s="72" t="s">
+        <v>671</v>
+      </c>
+      <c r="G108" s="72" t="s">
+        <v>671</v>
+      </c>
+      <c r="H108" s="72" t="s">
+        <v>671</v>
+      </c>
+      <c r="I108" s="69"/>
+      <c r="J108" s="87" t="s">
+        <v>589</v>
+      </c>
+      <c r="K108" s="90" t="s">
+        <v>601</v>
+      </c>
       <c r="L108" s="22"/>
       <c r="M108" s="22"/>
       <c r="N108" s="22"/>
       <c r="O108" s="22"/>
       <c r="P108" s="22"/>
       <c r="Q108" s="22"/>
-      <c r="R108" s="22"/>
-      <c r="S108" s="8" t="s">
-        <v>468</v>
-      </c>
-      <c r="T108" s="22" t="s">
-        <v>508</v>
-      </c>
+      <c r="R108" s="69"/>
+      <c r="S108" s="24"/>
+      <c r="T108" s="69"/>
+      <c r="V108" s="72"/>
+      <c r="AC108" s="88" t="s">
+        <v>588</v>
+      </c>
+      <c r="AD108" s="8">
+        <v>5</v>
+      </c>
+      <c r="AE108" s="72"/>
+      <c r="AF108" s="72"/>
+      <c r="AG108" s="72"/>
+      <c r="AH108" s="72"/>
       <c r="AI108" s="8">
         <v>300</v>
       </c>
       <c r="AJ108" s="8">
-        <v>200</v>
-      </c>
-      <c r="AM108" s="8">
-        <v>70</v>
-      </c>
-      <c r="AT108" s="8" t="s">
-        <v>401</v>
-      </c>
-      <c r="AY108" s="8">
-        <v>7</v>
-      </c>
-      <c r="AZ108" s="8">
-        <v>150</v>
-      </c>
-      <c r="BD108" s="8">
-        <v>250</v>
-      </c>
+        <v>300</v>
+      </c>
+      <c r="AN108" s="72"/>
+      <c r="AO108" s="72"/>
+      <c r="AP108" s="72"/>
+      <c r="AQ108" s="72"/>
+      <c r="AR108" s="72"/>
+      <c r="AU108" s="89"/>
+      <c r="AV108" s="72"/>
+      <c r="AY108" s="72"/>
+      <c r="AZ108" s="72"/>
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
-  <conditionalFormatting sqref="B90:BP108 K89:BP89 B4:BP88">
+  <conditionalFormatting sqref="K89:BP89 B4:BP88 B90:BP108">
     <cfRule type="containsBlanks" dxfId="73" priority="15">
       <formula>LEN(TRIM(B4))=0</formula>
     </cfRule>
@@ -11569,12 +11707,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BP39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AC1" sqref="AC1"/>
+      <selection pane="bottomLeft" activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -11608,13 +11746,13 @@
       <c r="B1" s="37" t="s">
         <v>72</v>
       </c>
-      <c r="C1" s="37" t="s">
+      <c r="C1" s="1" t="s">
         <v>126</v>
       </c>
       <c r="D1" s="37" t="s">
         <v>73</v>
       </c>
-      <c r="E1" s="37" t="s">
+      <c r="E1" s="1" t="s">
         <v>114</v>
       </c>
       <c r="F1" s="37" t="s">
@@ -14181,8 +14319,9 @@
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
a nearly finished quest
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/SceneQuest.xlsx
+++ b/ConfigData/Xlsx/SceneQuest.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385" activeTab="1"/>
+    <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="4" r:id="rId1"/>
@@ -154,7 +154,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1283" uniqueCount="671">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1294" uniqueCount="678">
   <si>
     <t>int</t>
     <phoneticPr fontId="18" type="noConversion"/>
@@ -2729,6 +2729,32 @@
   </si>
   <si>
     <t>给于的祝福</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>thief</t>
+  </si>
+  <si>
+    <t>thief</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>thief1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>盗贼I</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>thief2</t>
+  </si>
+  <si>
+    <t>盗贼II</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>thief2</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -3933,6 +3959,83 @@
   </cellStyles>
   <dxfs count="74">
     <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -4496,62 +4599,6 @@
       </fill>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -4910,27 +4957,6 @@
         </patternFill>
       </fill>
     </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -4958,10 +4984,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="表3" displayName="表3" ref="A3:BP108" totalsRowShown="0" headerRowDxfId="70">
-  <autoFilter ref="A3:BP108"/>
-  <sortState ref="A4:BP108">
-    <sortCondition ref="A3:A108"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="表3" displayName="表3" ref="A3:BP110" totalsRowShown="0" headerRowDxfId="73">
+  <autoFilter ref="A3:BP110"/>
+  <sortState ref="A4:BP110">
+    <sortCondition ref="A3:A110"/>
   </sortState>
   <tableColumns count="68">
     <tableColumn id="1" name="Id"/>
@@ -4972,50 +4998,50 @@
     <tableColumn id="24" name="Ename"/>
     <tableColumn id="4" name="Figue"/>
     <tableColumn id="5" name="Script"/>
-    <tableColumn id="6" name="TriggerMulti" dataDxfId="69"/>
-    <tableColumn id="40" name="Catalog" dataDxfId="68"/>
+    <tableColumn id="6" name="TriggerMulti" dataDxfId="72"/>
+    <tableColumn id="40" name="Catalog" dataDxfId="71"/>
     <tableColumn id="29" name="Catalog2"/>
-    <tableColumn id="35" name="TriggerHourBegin" dataDxfId="67"/>
-    <tableColumn id="34" name="TriggerHourEnd" dataDxfId="66"/>
-    <tableColumn id="36" name="TriggerQuestNotReceive" dataDxfId="65"/>
-    <tableColumn id="37" name="TriggerQuestReceived" dataDxfId="64"/>
-    <tableColumn id="38" name="TriggerQuestFinished" dataDxfId="63"/>
-    <tableColumn id="39" name="TriggerRate" dataDxfId="62"/>
-    <tableColumn id="62" name="TriggerOnceInDungeon" dataDxfId="61"/>
+    <tableColumn id="35" name="TriggerHourBegin" dataDxfId="70"/>
+    <tableColumn id="34" name="TriggerHourEnd" dataDxfId="69"/>
+    <tableColumn id="36" name="TriggerQuestNotReceive" dataDxfId="68"/>
+    <tableColumn id="37" name="TriggerQuestReceived" dataDxfId="67"/>
+    <tableColumn id="38" name="TriggerQuestFinished" dataDxfId="66"/>
+    <tableColumn id="39" name="TriggerRate" dataDxfId="65"/>
+    <tableColumn id="62" name="TriggerOnceInDungeon" dataDxfId="64"/>
     <tableColumn id="7" name="EnemyName"/>
-    <tableColumn id="51" name="CanBribe" dataDxfId="60"/>
+    <tableColumn id="51" name="CanBribe" dataDxfId="63"/>
     <tableColumn id="32" name="SceneId"/>
-    <tableColumn id="54" name="DungeonId" dataDxfId="59"/>
+    <tableColumn id="54" name="DungeonId" dataDxfId="62"/>
     <tableColumn id="50" name="CheckQuest"/>
     <tableColumn id="27" name="NextQuest"/>
     <tableColumn id="44" name="HiddenRoomQuest"/>
     <tableColumn id="8" name="ShopName"/>
     <tableColumn id="41" name="MiniGameId"/>
     <tableColumn id="43" name="PayKey"/>
-    <tableColumn id="67" name="NeedDungeonItemId" dataDxfId="58"/>
-    <tableColumn id="68" name="NeedDungeonItemCount" dataDxfId="57"/>
-    <tableColumn id="63" name="TestType1" dataDxfId="56"/>
-    <tableColumn id="64" name="TestBias1" dataDxfId="55"/>
-    <tableColumn id="65" name="TestType2" dataDxfId="54"/>
-    <tableColumn id="66" name="TestBias2" dataDxfId="53"/>
+    <tableColumn id="67" name="NeedDungeonItemId" dataDxfId="61"/>
+    <tableColumn id="68" name="NeedDungeonItemCount" dataDxfId="60"/>
+    <tableColumn id="63" name="TestType1" dataDxfId="59"/>
+    <tableColumn id="64" name="TestBias1" dataDxfId="58"/>
+    <tableColumn id="65" name="TestType2" dataDxfId="57"/>
+    <tableColumn id="66" name="TestBias2" dataDxfId="56"/>
     <tableColumn id="9" name="RewardGold"/>
     <tableColumn id="10" name="RewardFood"/>
     <tableColumn id="11" name="RewardHealth"/>
     <tableColumn id="12" name="RewardMental"/>
     <tableColumn id="13" name="RewardExp"/>
-    <tableColumn id="56" name="RewardStr" dataDxfId="52"/>
-    <tableColumn id="57" name="RewardAgi" dataDxfId="51"/>
-    <tableColumn id="58" name="RewardIntl" dataDxfId="50"/>
-    <tableColumn id="59" name="RewardPerc" dataDxfId="49"/>
-    <tableColumn id="60" name="RewardEndu" dataDxfId="48"/>
+    <tableColumn id="56" name="RewardStr" dataDxfId="55"/>
+    <tableColumn id="57" name="RewardAgi" dataDxfId="54"/>
+    <tableColumn id="58" name="RewardIntl" dataDxfId="53"/>
+    <tableColumn id="59" name="RewardPerc" dataDxfId="52"/>
+    <tableColumn id="60" name="RewardEndu" dataDxfId="51"/>
     <tableColumn id="14" name="RewardItem"/>
     <tableColumn id="15" name="RewardDrop"/>
-    <tableColumn id="55" name="RewardDungeonItemId" dataDxfId="47"/>
-    <tableColumn id="61" name="RewardDungeonItemCount" dataDxfId="46"/>
+    <tableColumn id="55" name="RewardDungeonItemId" dataDxfId="50"/>
+    <tableColumn id="61" name="RewardDungeonItemCount" dataDxfId="49"/>
     <tableColumn id="30" name="RewardBlessLevel"/>
     <tableColumn id="42" name="RewardBlessName"/>
-    <tableColumn id="52" name="RewardResId" dataDxfId="45"/>
-    <tableColumn id="53" name="RewardResAmount" dataDxfId="44"/>
+    <tableColumn id="52" name="RewardResId" dataDxfId="48"/>
+    <tableColumn id="53" name="RewardResAmount" dataDxfId="47"/>
     <tableColumn id="26" name="UnlockRival"/>
     <tableColumn id="16" name="PunishGold"/>
     <tableColumn id="17" name="PunishFood"/>
@@ -5038,7 +5064,7 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="表3_5" displayName="表3_5" ref="A3:BP39" totalsRowShown="0" headerRowDxfId="35">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="表3_5" displayName="表3_5" ref="A3:BP39" totalsRowShown="0" headerRowDxfId="46">
   <autoFilter ref="A3:BP39"/>
   <sortState ref="A4:AT6">
     <sortCondition ref="A3:A6"/>
@@ -5046,56 +5072,56 @@
   <tableColumns count="68">
     <tableColumn id="1" name="Id"/>
     <tableColumn id="2" name="Name"/>
-    <tableColumn id="27" name="Type" dataDxfId="34"/>
+    <tableColumn id="27" name="Type" dataDxfId="45"/>
     <tableColumn id="3" name="Level"/>
     <tableColumn id="25" name="Danger"/>
     <tableColumn id="24" name="Ename"/>
     <tableColumn id="4" name="Figue"/>
     <tableColumn id="5" name="Script"/>
     <tableColumn id="6" name="TriggerMulti"/>
-    <tableColumn id="40" name="Catalog" dataDxfId="33"/>
-    <tableColumn id="29" name="Catalog2" dataDxfId="32"/>
-    <tableColumn id="35" name="TriggerHourBegin" dataDxfId="31"/>
-    <tableColumn id="34" name="TriggerHourEnd" dataDxfId="30"/>
-    <tableColumn id="37" name="TriggerQuestNotReceive" dataDxfId="29"/>
-    <tableColumn id="38" name="TriggerQuestReceived" dataDxfId="28"/>
-    <tableColumn id="36" name="TriggerQuestFinished" dataDxfId="27"/>
-    <tableColumn id="39" name="TriggerRate" dataDxfId="26"/>
-    <tableColumn id="62" name="TriggerOnceInDungeon" dataDxfId="25"/>
+    <tableColumn id="40" name="Catalog" dataDxfId="44"/>
+    <tableColumn id="29" name="Catalog2" dataDxfId="43"/>
+    <tableColumn id="35" name="TriggerHourBegin" dataDxfId="42"/>
+    <tableColumn id="34" name="TriggerHourEnd" dataDxfId="41"/>
+    <tableColumn id="37" name="TriggerQuestNotReceive" dataDxfId="40"/>
+    <tableColumn id="38" name="TriggerQuestReceived" dataDxfId="39"/>
+    <tableColumn id="36" name="TriggerQuestFinished" dataDxfId="38"/>
+    <tableColumn id="39" name="TriggerRate" dataDxfId="37"/>
+    <tableColumn id="62" name="TriggerOnceInDungeon" dataDxfId="36"/>
     <tableColumn id="7" name="EnemyName"/>
-    <tableColumn id="51" name="CanBribe" dataDxfId="24"/>
-    <tableColumn id="32" name="SceneId" dataDxfId="23"/>
-    <tableColumn id="54" name="DungeonId" dataDxfId="22"/>
-    <tableColumn id="50" name="CheckQuest" dataDxfId="21"/>
-    <tableColumn id="28" name="NextQuest" dataDxfId="20"/>
-    <tableColumn id="44" name="HiddenRoomQuest" dataDxfId="19"/>
-    <tableColumn id="8" name="ShopName" dataDxfId="18"/>
-    <tableColumn id="41" name="MiniGameId" dataDxfId="17"/>
-    <tableColumn id="43" name="PayKey" dataDxfId="16"/>
-    <tableColumn id="67" name="NeedDungeonItemId" dataDxfId="15"/>
-    <tableColumn id="68" name="NeedDungeonItemCount" dataDxfId="14"/>
-    <tableColumn id="63" name="TestType1" dataDxfId="13"/>
-    <tableColumn id="64" name="TestBias1" dataDxfId="12"/>
-    <tableColumn id="65" name="TestType2" dataDxfId="11"/>
-    <tableColumn id="66" name="TestBias2" dataDxfId="10"/>
+    <tableColumn id="51" name="CanBribe" dataDxfId="35"/>
+    <tableColumn id="32" name="SceneId" dataDxfId="34"/>
+    <tableColumn id="54" name="DungeonId" dataDxfId="33"/>
+    <tableColumn id="50" name="CheckQuest" dataDxfId="32"/>
+    <tableColumn id="28" name="NextQuest" dataDxfId="31"/>
+    <tableColumn id="44" name="HiddenRoomQuest" dataDxfId="30"/>
+    <tableColumn id="8" name="ShopName" dataDxfId="29"/>
+    <tableColumn id="41" name="MiniGameId" dataDxfId="28"/>
+    <tableColumn id="43" name="PayKey" dataDxfId="27"/>
+    <tableColumn id="67" name="NeedDungeonItemId" dataDxfId="26"/>
+    <tableColumn id="68" name="NeedDungeonItemCount" dataDxfId="25"/>
+    <tableColumn id="63" name="TestType1" dataDxfId="24"/>
+    <tableColumn id="64" name="TestBias1" dataDxfId="23"/>
+    <tableColumn id="65" name="TestType2" dataDxfId="22"/>
+    <tableColumn id="66" name="TestBias2" dataDxfId="21"/>
     <tableColumn id="9" name="RewardGold"/>
     <tableColumn id="10" name="RewardFood"/>
     <tableColumn id="11" name="RewardHealth"/>
     <tableColumn id="12" name="RewardMental"/>
     <tableColumn id="13" name="RewardExp"/>
-    <tableColumn id="55" name="RewardStr" dataDxfId="9"/>
-    <tableColumn id="56" name="RewardAgi" dataDxfId="8"/>
-    <tableColumn id="57" name="RewardIntl" dataDxfId="7"/>
-    <tableColumn id="58" name="RewardPerc" dataDxfId="6"/>
-    <tableColumn id="59" name="RewardEndu" dataDxfId="5"/>
+    <tableColumn id="55" name="RewardStr" dataDxfId="20"/>
+    <tableColumn id="56" name="RewardAgi" dataDxfId="19"/>
+    <tableColumn id="57" name="RewardIntl" dataDxfId="18"/>
+    <tableColumn id="58" name="RewardPerc" dataDxfId="17"/>
+    <tableColumn id="59" name="RewardEndu" dataDxfId="16"/>
     <tableColumn id="14" name="RewardItem"/>
     <tableColumn id="15" name="RewardDrop"/>
-    <tableColumn id="60" name="RewardDungeonItemId" dataDxfId="4"/>
-    <tableColumn id="61" name="RewardDungeonItemCount" dataDxfId="3"/>
+    <tableColumn id="60" name="RewardDungeonItemId" dataDxfId="15"/>
+    <tableColumn id="61" name="RewardDungeonItemCount" dataDxfId="14"/>
     <tableColumn id="31" name="RewardBlessLevel"/>
     <tableColumn id="42" name="RewardBlessName"/>
-    <tableColumn id="52" name="RewardResId" dataDxfId="2"/>
-    <tableColumn id="53" name="RewardResAmount" dataDxfId="1"/>
+    <tableColumn id="52" name="RewardResId" dataDxfId="13"/>
+    <tableColumn id="53" name="RewardResAmount" dataDxfId="12"/>
     <tableColumn id="26" name="UnlockRival"/>
     <tableColumn id="16" name="PunishGold"/>
     <tableColumn id="17" name="PunishFood"/>
@@ -5111,7 +5137,7 @@
     <tableColumn id="21" name="TradeFood"/>
     <tableColumn id="22" name="TradeHealth"/>
     <tableColumn id="23" name="TradeMental"/>
-    <tableColumn id="33" name="TradeDropItem" dataDxfId="0"/>
+    <tableColumn id="33" name="TradeDropItem" dataDxfId="11"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5438,11 +5464,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BP108"/>
+  <dimension ref="A1:BP110"/>
   <sheetViews>
-    <sheetView topLeftCell="AC1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AW1" sqref="AW1:AX3"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A77" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="X91" sqref="X91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -10360,7 +10386,7 @@
       <c r="A88" s="8">
         <v>42030003</v>
       </c>
-      <c r="B88" s="8" t="s">
+      <c r="B88" s="72" t="s">
         <v>459</v>
       </c>
       <c r="C88" s="8">
@@ -10470,117 +10496,128 @@
       </c>
     </row>
     <row r="90" spans="1:68" x14ac:dyDescent="0.15">
-      <c r="A90" s="94">
-        <v>42040001</v>
-      </c>
-      <c r="B90" s="96" t="s">
-        <v>589</v>
+      <c r="A90" s="8">
+        <v>42030005</v>
+      </c>
+      <c r="B90" s="72" t="s">
+        <v>674</v>
       </c>
       <c r="C90" s="8">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D90" s="8">
         <v>0</v>
       </c>
+      <c r="E90" s="8">
+        <v>1</v>
+      </c>
       <c r="F90" s="72" t="s">
-        <v>600</v>
+        <v>673</v>
       </c>
       <c r="G90" s="72" t="s">
-        <v>592</v>
+        <v>672</v>
       </c>
       <c r="H90" s="72" t="s">
-        <v>592</v>
-      </c>
-      <c r="I90" s="69"/>
-      <c r="J90" s="31" t="s">
-        <v>250</v>
-      </c>
-      <c r="K90" s="88" t="s">
-        <v>595</v>
-      </c>
+        <v>673</v>
+      </c>
+      <c r="I90" s="22"/>
+      <c r="J90" s="29" t="s">
+        <v>249</v>
+      </c>
+      <c r="K90" s="30"/>
       <c r="L90" s="22"/>
       <c r="M90" s="22"/>
       <c r="N90" s="22"/>
       <c r="O90" s="22"/>
       <c r="P90" s="22"/>
       <c r="Q90" s="22"/>
-      <c r="R90" s="69" t="s">
-        <v>599</v>
-      </c>
-      <c r="S90" s="24"/>
-      <c r="T90" s="69"/>
+      <c r="R90" s="69"/>
+      <c r="T90" s="22"/>
       <c r="V90" s="72"/>
-      <c r="AN90" s="72">
-        <v>1</v>
-      </c>
+      <c r="X90" s="8" t="s">
+        <v>675</v>
+      </c>
+      <c r="AC90" s="72"/>
+      <c r="AD90" s="72"/>
+      <c r="AE90" s="72"/>
+      <c r="AF90" s="72"/>
+      <c r="AG90" s="72"/>
+      <c r="AH90" s="72"/>
+      <c r="AN90" s="72"/>
       <c r="AO90" s="72"/>
       <c r="AP90" s="72"/>
       <c r="AQ90" s="72"/>
       <c r="AR90" s="72"/>
-      <c r="AU90" s="87"/>
+      <c r="AU90" s="72"/>
       <c r="AV90" s="72"/>
       <c r="AY90" s="72"/>
       <c r="AZ90" s="72"/>
+      <c r="BB90" s="8">
+        <v>200</v>
+      </c>
     </row>
     <row r="91" spans="1:68" x14ac:dyDescent="0.15">
-      <c r="A91" s="94">
-        <v>42040002</v>
-      </c>
-      <c r="B91" s="96" t="s">
-        <v>591</v>
+      <c r="A91" s="8">
+        <v>42030006</v>
+      </c>
+      <c r="B91" s="72" t="s">
+        <v>676</v>
       </c>
       <c r="C91" s="8">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D91" s="8">
         <v>0</v>
       </c>
+      <c r="E91" s="8">
+        <v>2</v>
+      </c>
       <c r="F91" s="72" t="s">
-        <v>601</v>
-      </c>
-      <c r="G91" s="72" t="s">
-        <v>593</v>
+        <v>677</v>
+      </c>
+      <c r="G91" s="8" t="s">
+        <v>671</v>
       </c>
       <c r="H91" s="72" t="s">
-        <v>593</v>
-      </c>
-      <c r="I91" s="69"/>
-      <c r="J91" s="31" t="s">
-        <v>250</v>
-      </c>
-      <c r="K91" s="88" t="s">
-        <v>595</v>
-      </c>
+        <v>675</v>
+      </c>
+      <c r="I91" s="22"/>
+      <c r="J91" s="30"/>
+      <c r="K91" s="30"/>
       <c r="L91" s="22"/>
       <c r="M91" s="22"/>
       <c r="N91" s="22"/>
       <c r="O91" s="22"/>
       <c r="P91" s="22"/>
       <c r="Q91" s="22"/>
-      <c r="R91" s="69" t="s">
-        <v>599</v>
-      </c>
-      <c r="S91" s="23"/>
-      <c r="T91" s="69"/>
+      <c r="R91" s="69"/>
+      <c r="T91" s="22"/>
       <c r="V91" s="72"/>
+      <c r="X91" s="8" t="s">
+        <v>675</v>
+      </c>
+      <c r="AC91" s="72"/>
+      <c r="AD91" s="72"/>
+      <c r="AE91" s="72"/>
+      <c r="AF91" s="72"/>
+      <c r="AG91" s="72"/>
+      <c r="AH91" s="72"/>
       <c r="AN91" s="72"/>
-      <c r="AO91" s="72">
-        <v>1</v>
-      </c>
+      <c r="AO91" s="72"/>
       <c r="AP91" s="72"/>
       <c r="AQ91" s="72"/>
       <c r="AR91" s="72"/>
-      <c r="AU91" s="87"/>
+      <c r="AU91" s="72"/>
       <c r="AV91" s="72"/>
       <c r="AY91" s="72"/>
       <c r="AZ91" s="72"/>
     </row>
     <row r="92" spans="1:68" x14ac:dyDescent="0.15">
       <c r="A92" s="94">
-        <v>42040003</v>
+        <v>42040001</v>
       </c>
       <c r="B92" s="96" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="C92" s="8">
         <v>5</v>
@@ -10589,13 +10626,13 @@
         <v>0</v>
       </c>
       <c r="F92" s="72" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
       <c r="G92" s="72" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="H92" s="72" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="I92" s="69"/>
       <c r="J92" s="31" t="s">
@@ -10616,11 +10653,11 @@
       <c r="S92" s="24"/>
       <c r="T92" s="69"/>
       <c r="V92" s="72"/>
-      <c r="AN92" s="72"/>
+      <c r="AN92" s="72">
+        <v>1</v>
+      </c>
       <c r="AO92" s="72"/>
-      <c r="AP92" s="72">
-        <v>1</v>
-      </c>
+      <c r="AP92" s="72"/>
       <c r="AQ92" s="72"/>
       <c r="AR92" s="72"/>
       <c r="AU92" s="87"/>
@@ -10630,10 +10667,10 @@
     </row>
     <row r="93" spans="1:68" x14ac:dyDescent="0.15">
       <c r="A93" s="94">
-        <v>42040004</v>
+        <v>42040002</v>
       </c>
       <c r="B93" s="96" t="s">
-        <v>606</v>
+        <v>591</v>
       </c>
       <c r="C93" s="8">
         <v>5</v>
@@ -10642,13 +10679,13 @@
         <v>0</v>
       </c>
       <c r="F93" s="72" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="G93" s="72" t="s">
-        <v>610</v>
+        <v>593</v>
       </c>
       <c r="H93" s="72" t="s">
-        <v>605</v>
+        <v>593</v>
       </c>
       <c r="I93" s="69"/>
       <c r="J93" s="31" t="s">
@@ -10666,15 +10703,15 @@
       <c r="R93" s="69" t="s">
         <v>599</v>
       </c>
-      <c r="S93" s="24"/>
+      <c r="S93" s="23"/>
       <c r="T93" s="69"/>
       <c r="V93" s="72"/>
       <c r="AN93" s="72"/>
-      <c r="AO93" s="72"/>
+      <c r="AO93" s="72">
+        <v>1</v>
+      </c>
       <c r="AP93" s="72"/>
-      <c r="AQ93" s="72">
-        <v>1</v>
-      </c>
+      <c r="AQ93" s="72"/>
       <c r="AR93" s="72"/>
       <c r="AU93" s="87"/>
       <c r="AV93" s="72"/>
@@ -10683,10 +10720,10 @@
     </row>
     <row r="94" spans="1:68" x14ac:dyDescent="0.15">
       <c r="A94" s="94">
-        <v>42040005</v>
+        <v>42040003</v>
       </c>
       <c r="B94" s="96" t="s">
-        <v>608</v>
+        <v>590</v>
       </c>
       <c r="C94" s="8">
         <v>5</v>
@@ -10695,13 +10732,13 @@
         <v>0</v>
       </c>
       <c r="F94" s="72" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
       <c r="G94" s="72" t="s">
-        <v>609</v>
+        <v>594</v>
       </c>
       <c r="H94" s="72" t="s">
-        <v>607</v>
+        <v>594</v>
       </c>
       <c r="I94" s="69"/>
       <c r="J94" s="31" t="s">
@@ -10719,16 +10756,16 @@
       <c r="R94" s="69" t="s">
         <v>599</v>
       </c>
-      <c r="S94" s="23"/>
+      <c r="S94" s="24"/>
       <c r="T94" s="69"/>
       <c r="V94" s="72"/>
       <c r="AN94" s="72"/>
       <c r="AO94" s="72"/>
-      <c r="AP94" s="72"/>
+      <c r="AP94" s="72">
+        <v>1</v>
+      </c>
       <c r="AQ94" s="72"/>
-      <c r="AR94" s="72">
-        <v>1</v>
-      </c>
+      <c r="AR94" s="72"/>
       <c r="AU94" s="87"/>
       <c r="AV94" s="72"/>
       <c r="AY94" s="72"/>
@@ -10736,10 +10773,10 @@
     </row>
     <row r="95" spans="1:68" x14ac:dyDescent="0.15">
       <c r="A95" s="94">
-        <v>42040006</v>
+        <v>42040004</v>
       </c>
       <c r="B95" s="96" t="s">
-        <v>612</v>
+        <v>606</v>
       </c>
       <c r="C95" s="8">
         <v>5</v>
@@ -10747,21 +10784,18 @@
       <c r="D95" s="8">
         <v>0</v>
       </c>
-      <c r="E95" s="8">
-        <v>1</v>
-      </c>
       <c r="F95" s="72" t="s">
-        <v>611</v>
+        <v>603</v>
       </c>
       <c r="G95" s="72" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="H95" s="72" t="s">
-        <v>650</v>
+        <v>605</v>
       </c>
       <c r="I95" s="69"/>
-      <c r="J95" s="78" t="s">
-        <v>558</v>
+      <c r="J95" s="31" t="s">
+        <v>250</v>
       </c>
       <c r="K95" s="88" t="s">
         <v>595</v>
@@ -10772,35 +10806,30 @@
       <c r="O95" s="22"/>
       <c r="P95" s="22"/>
       <c r="Q95" s="22"/>
-      <c r="R95" s="69"/>
-      <c r="S95" s="23"/>
+      <c r="R95" s="69" t="s">
+        <v>599</v>
+      </c>
+      <c r="S95" s="24"/>
       <c r="T95" s="69"/>
       <c r="V95" s="72"/>
-      <c r="AE95" s="72" t="s">
-        <v>651</v>
-      </c>
-      <c r="AF95" s="8">
-        <v>1</v>
-      </c>
       <c r="AN95" s="72"/>
       <c r="AO95" s="72"/>
       <c r="AP95" s="72"/>
-      <c r="AQ95" s="72"/>
+      <c r="AQ95" s="72">
+        <v>1</v>
+      </c>
       <c r="AR95" s="72"/>
       <c r="AU95" s="87"/>
       <c r="AV95" s="72"/>
       <c r="AY95" s="72"/>
       <c r="AZ95" s="72"/>
-      <c r="BD95" s="8">
-        <v>150</v>
-      </c>
     </row>
     <row r="96" spans="1:68" x14ac:dyDescent="0.15">
       <c r="A96" s="94">
-        <v>42040007</v>
+        <v>42040005</v>
       </c>
       <c r="B96" s="96" t="s">
-        <v>614</v>
+        <v>608</v>
       </c>
       <c r="C96" s="8">
         <v>5</v>
@@ -10808,23 +10837,18 @@
       <c r="D96" s="8">
         <v>0</v>
       </c>
-      <c r="E96" s="8">
-        <v>1</v>
-      </c>
       <c r="F96" s="72" t="s">
-        <v>613</v>
+        <v>604</v>
       </c>
       <c r="G96" s="72" t="s">
-        <v>613</v>
+        <v>609</v>
       </c>
       <c r="H96" s="72" t="s">
-        <v>657</v>
-      </c>
-      <c r="I96" s="69" t="s">
-        <v>656</v>
-      </c>
-      <c r="J96" s="78" t="s">
-        <v>558</v>
+        <v>607</v>
+      </c>
+      <c r="I96" s="69"/>
+      <c r="J96" s="31" t="s">
+        <v>250</v>
       </c>
       <c r="K96" s="88" t="s">
         <v>595</v>
@@ -10835,29 +10859,30 @@
       <c r="O96" s="22"/>
       <c r="P96" s="22"/>
       <c r="Q96" s="22"/>
-      <c r="R96" s="69"/>
-      <c r="S96" s="24"/>
+      <c r="R96" s="69" t="s">
+        <v>599</v>
+      </c>
+      <c r="S96" s="23"/>
       <c r="T96" s="69"/>
       <c r="V96" s="72"/>
       <c r="AN96" s="72"/>
       <c r="AO96" s="72"/>
       <c r="AP96" s="72"/>
       <c r="AQ96" s="72"/>
-      <c r="AR96" s="72"/>
+      <c r="AR96" s="72">
+        <v>1</v>
+      </c>
       <c r="AU96" s="87"/>
       <c r="AV96" s="72"/>
       <c r="AY96" s="72"/>
       <c r="AZ96" s="72"/>
-      <c r="BC96" s="8">
-        <v>50</v>
-      </c>
     </row>
     <row r="97" spans="1:58" x14ac:dyDescent="0.15">
       <c r="A97" s="94">
-        <v>42040008</v>
+        <v>42040006</v>
       </c>
       <c r="B97" s="96" t="s">
-        <v>616</v>
+        <v>612</v>
       </c>
       <c r="C97" s="8">
         <v>5</v>
@@ -10866,13 +10891,13 @@
         <v>0</v>
       </c>
       <c r="E97" s="8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F97" s="72" t="s">
-        <v>659</v>
+        <v>611</v>
       </c>
       <c r="G97" s="72" t="s">
-        <v>615</v>
+        <v>611</v>
       </c>
       <c r="H97" s="72" t="s">
         <v>650</v>
@@ -10891,20 +10916,14 @@
       <c r="P97" s="22"/>
       <c r="Q97" s="22"/>
       <c r="R97" s="69"/>
-      <c r="S97" s="24"/>
+      <c r="S97" s="23"/>
       <c r="T97" s="69"/>
       <c r="V97" s="72"/>
       <c r="AE97" s="72" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="AF97" s="8">
-        <v>2</v>
-      </c>
-      <c r="AG97" s="72" t="s">
-        <v>653</v>
-      </c>
-      <c r="AH97" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AN97" s="72"/>
       <c r="AO97" s="72"/>
@@ -10921,10 +10940,10 @@
     </row>
     <row r="98" spans="1:58" x14ac:dyDescent="0.15">
       <c r="A98" s="94">
-        <v>42040009</v>
+        <v>42040007</v>
       </c>
       <c r="B98" s="96" t="s">
-        <v>618</v>
+        <v>614</v>
       </c>
       <c r="C98" s="8">
         <v>5</v>
@@ -10936,15 +10955,17 @@
         <v>1</v>
       </c>
       <c r="F98" s="72" t="s">
-        <v>617</v>
+        <v>613</v>
       </c>
       <c r="G98" s="72" t="s">
-        <v>617</v>
+        <v>613</v>
       </c>
       <c r="H98" s="72" t="s">
-        <v>650</v>
-      </c>
-      <c r="I98" s="69"/>
+        <v>657</v>
+      </c>
+      <c r="I98" s="69" t="s">
+        <v>656</v>
+      </c>
       <c r="J98" s="78" t="s">
         <v>558</v>
       </c>
@@ -10961,12 +10982,6 @@
       <c r="S98" s="24"/>
       <c r="T98" s="69"/>
       <c r="V98" s="72"/>
-      <c r="AE98" s="72" t="s">
-        <v>654</v>
-      </c>
-      <c r="AF98" s="8">
-        <v>1</v>
-      </c>
       <c r="AN98" s="72"/>
       <c r="AO98" s="72"/>
       <c r="AP98" s="72"/>
@@ -10976,19 +10991,16 @@
       <c r="AV98" s="72"/>
       <c r="AY98" s="72"/>
       <c r="AZ98" s="72"/>
-      <c r="BD98" s="8">
+      <c r="BC98" s="8">
         <v>50</v>
-      </c>
-      <c r="BE98" s="8">
-        <v>100</v>
       </c>
     </row>
     <row r="99" spans="1:58" x14ac:dyDescent="0.15">
       <c r="A99" s="94">
-        <v>42040010</v>
+        <v>42040008</v>
       </c>
       <c r="B99" s="96" t="s">
-        <v>620</v>
+        <v>616</v>
       </c>
       <c r="C99" s="8">
         <v>5</v>
@@ -10997,13 +11009,13 @@
         <v>0</v>
       </c>
       <c r="E99" s="8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F99" s="72" t="s">
-        <v>619</v>
+        <v>659</v>
       </c>
       <c r="G99" s="72" t="s">
-        <v>619</v>
+        <v>615</v>
       </c>
       <c r="H99" s="72" t="s">
         <v>650</v>
@@ -11029,7 +11041,13 @@
         <v>652</v>
       </c>
       <c r="AF99" s="8">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="AG99" s="72" t="s">
+        <v>653</v>
+      </c>
+      <c r="AH99" s="8">
+        <v>0</v>
       </c>
       <c r="AN99" s="72"/>
       <c r="AO99" s="72"/>
@@ -11041,15 +11059,15 @@
       <c r="AY99" s="72"/>
       <c r="AZ99" s="72"/>
       <c r="BD99" s="8">
-        <v>120</v>
+        <v>150</v>
       </c>
     </row>
     <row r="100" spans="1:58" x14ac:dyDescent="0.15">
       <c r="A100" s="94">
-        <v>42040011</v>
+        <v>42040009</v>
       </c>
       <c r="B100" s="96" t="s">
-        <v>622</v>
+        <v>618</v>
       </c>
       <c r="C100" s="8">
         <v>5</v>
@@ -11058,20 +11076,18 @@
         <v>0</v>
       </c>
       <c r="E100" s="8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F100" s="72" t="s">
-        <v>621</v>
+        <v>617</v>
       </c>
       <c r="G100" s="72" t="s">
-        <v>621</v>
+        <v>617</v>
       </c>
       <c r="H100" s="72" t="s">
         <v>650</v>
       </c>
-      <c r="I100" s="69" t="s">
-        <v>656</v>
-      </c>
+      <c r="I100" s="69"/>
       <c r="J100" s="78" t="s">
         <v>558</v>
       </c>
@@ -11089,16 +11105,10 @@
       <c r="T100" s="69"/>
       <c r="V100" s="72"/>
       <c r="AE100" s="72" t="s">
-        <v>651</v>
+        <v>654</v>
       </c>
       <c r="AF100" s="8">
-        <v>2</v>
-      </c>
-      <c r="AG100" s="72" t="s">
-        <v>655</v>
-      </c>
-      <c r="AH100" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AN100" s="72"/>
       <c r="AO100" s="72"/>
@@ -11110,15 +11120,18 @@
       <c r="AY100" s="72"/>
       <c r="AZ100" s="72"/>
       <c r="BD100" s="8">
-        <v>150</v>
+        <v>50</v>
+      </c>
+      <c r="BE100" s="8">
+        <v>100</v>
       </c>
     </row>
     <row r="101" spans="1:58" x14ac:dyDescent="0.15">
       <c r="A101" s="94">
-        <v>42040012</v>
+        <v>42040010</v>
       </c>
       <c r="B101" s="96" t="s">
-        <v>624</v>
+        <v>620</v>
       </c>
       <c r="C101" s="8">
         <v>5</v>
@@ -11130,17 +11143,15 @@
         <v>1</v>
       </c>
       <c r="F101" s="72" t="s">
-        <v>623</v>
+        <v>619</v>
       </c>
       <c r="G101" s="72" t="s">
-        <v>623</v>
+        <v>619</v>
       </c>
       <c r="H101" s="72" t="s">
         <v>650</v>
       </c>
-      <c r="I101" s="69" t="s">
-        <v>656</v>
-      </c>
+      <c r="I101" s="69"/>
       <c r="J101" s="78" t="s">
         <v>558</v>
       </c>
@@ -11161,13 +11172,7 @@
         <v>652</v>
       </c>
       <c r="AF101" s="8">
-        <v>0</v>
-      </c>
-      <c r="AG101" s="72" t="s">
-        <v>654</v>
-      </c>
-      <c r="AH101" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AN101" s="72"/>
       <c r="AO101" s="72"/>
@@ -11178,19 +11183,16 @@
       <c r="AV101" s="72"/>
       <c r="AY101" s="72"/>
       <c r="AZ101" s="72"/>
-      <c r="BC101" s="8">
-        <v>50</v>
-      </c>
-      <c r="BF101" s="8">
-        <v>1</v>
+      <c r="BD101" s="8">
+        <v>120</v>
       </c>
     </row>
     <row r="102" spans="1:58" x14ac:dyDescent="0.15">
       <c r="A102" s="94">
-        <v>42040013</v>
+        <v>42040011</v>
       </c>
       <c r="B102" s="96" t="s">
-        <v>626</v>
+        <v>622</v>
       </c>
       <c r="C102" s="8">
         <v>5</v>
@@ -11199,18 +11201,20 @@
         <v>0</v>
       </c>
       <c r="E102" s="8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F102" s="72" t="s">
-        <v>625</v>
+        <v>621</v>
       </c>
       <c r="G102" s="72" t="s">
-        <v>625</v>
+        <v>621</v>
       </c>
       <c r="H102" s="72" t="s">
         <v>650</v>
       </c>
-      <c r="I102" s="69"/>
+      <c r="I102" s="69" t="s">
+        <v>656</v>
+      </c>
       <c r="J102" s="78" t="s">
         <v>558</v>
       </c>
@@ -11231,13 +11235,13 @@
         <v>651</v>
       </c>
       <c r="AF102" s="8">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AG102" s="72" t="s">
-        <v>653</v>
+        <v>655</v>
       </c>
       <c r="AH102" s="8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AN102" s="72"/>
       <c r="AO102" s="72"/>
@@ -11249,15 +11253,15 @@
       <c r="AY102" s="72"/>
       <c r="AZ102" s="72"/>
       <c r="BD102" s="8">
-        <v>100</v>
+        <v>150</v>
       </c>
     </row>
     <row r="103" spans="1:58" x14ac:dyDescent="0.15">
       <c r="A103" s="94">
-        <v>42040014</v>
+        <v>42040012</v>
       </c>
       <c r="B103" s="96" t="s">
-        <v>628</v>
+        <v>624</v>
       </c>
       <c r="C103" s="8">
         <v>5</v>
@@ -11269,10 +11273,10 @@
         <v>1</v>
       </c>
       <c r="F103" s="72" t="s">
-        <v>658</v>
+        <v>623</v>
       </c>
       <c r="G103" s="72" t="s">
-        <v>627</v>
+        <v>623</v>
       </c>
       <c r="H103" s="72" t="s">
         <v>650</v>
@@ -11300,7 +11304,13 @@
         <v>652</v>
       </c>
       <c r="AF103" s="8">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="AG103" s="72" t="s">
+        <v>654</v>
+      </c>
+      <c r="AH103" s="8">
+        <v>0</v>
       </c>
       <c r="AN103" s="72"/>
       <c r="AO103" s="72"/>
@@ -11311,16 +11321,19 @@
       <c r="AV103" s="72"/>
       <c r="AY103" s="72"/>
       <c r="AZ103" s="72"/>
-      <c r="BD103" s="8">
-        <v>100</v>
+      <c r="BC103" s="8">
+        <v>50</v>
+      </c>
+      <c r="BF103" s="8">
+        <v>1</v>
       </c>
     </row>
     <row r="104" spans="1:58" x14ac:dyDescent="0.15">
       <c r="A104" s="94">
-        <v>42040015</v>
+        <v>42040013</v>
       </c>
       <c r="B104" s="96" t="s">
-        <v>630</v>
+        <v>626</v>
       </c>
       <c r="C104" s="8">
         <v>5</v>
@@ -11329,20 +11342,18 @@
         <v>0</v>
       </c>
       <c r="E104" s="8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F104" s="72" t="s">
-        <v>629</v>
+        <v>625</v>
       </c>
       <c r="G104" s="72" t="s">
-        <v>629</v>
+        <v>625</v>
       </c>
       <c r="H104" s="72" t="s">
-        <v>613</v>
-      </c>
-      <c r="I104" s="69" t="s">
-        <v>656</v>
-      </c>
+        <v>650</v>
+      </c>
+      <c r="I104" s="69"/>
       <c r="J104" s="78" t="s">
         <v>558</v>
       </c>
@@ -11360,16 +11371,16 @@
       <c r="T104" s="69"/>
       <c r="V104" s="72"/>
       <c r="AE104" s="72" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="AF104" s="8">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AG104" s="72" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
       <c r="AH104" s="8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AN104" s="72"/>
       <c r="AO104" s="72"/>
@@ -11381,15 +11392,15 @@
       <c r="AY104" s="72"/>
       <c r="AZ104" s="72"/>
       <c r="BD104" s="8">
-        <v>150</v>
+        <v>100</v>
       </c>
     </row>
     <row r="105" spans="1:58" x14ac:dyDescent="0.15">
       <c r="A105" s="94">
-        <v>42040016</v>
+        <v>42040014</v>
       </c>
       <c r="B105" s="96" t="s">
-        <v>632</v>
+        <v>628</v>
       </c>
       <c r="C105" s="8">
         <v>5</v>
@@ -11401,20 +11412,22 @@
         <v>1</v>
       </c>
       <c r="F105" s="72" t="s">
-        <v>631</v>
+        <v>658</v>
       </c>
       <c r="G105" s="72" t="s">
-        <v>631</v>
+        <v>627</v>
       </c>
       <c r="H105" s="72" t="s">
-        <v>631</v>
-      </c>
-      <c r="I105" s="69"/>
+        <v>650</v>
+      </c>
+      <c r="I105" s="69" t="s">
+        <v>656</v>
+      </c>
       <c r="J105" s="78" t="s">
         <v>558</v>
       </c>
-      <c r="K105" s="28" t="s">
-        <v>246</v>
+      <c r="K105" s="88" t="s">
+        <v>595</v>
       </c>
       <c r="L105" s="22"/>
       <c r="M105" s="22"/>
@@ -11430,37 +11443,27 @@
         <v>652</v>
       </c>
       <c r="AF105" s="8">
-        <v>3</v>
-      </c>
-      <c r="AG105" s="72" t="s">
-        <v>653</v>
-      </c>
-      <c r="AH105" s="8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AN105" s="72"/>
       <c r="AO105" s="72"/>
       <c r="AP105" s="72"/>
       <c r="AQ105" s="72"/>
       <c r="AR105" s="72"/>
-      <c r="AT105" s="24"/>
       <c r="AU105" s="87"/>
       <c r="AV105" s="72"/>
       <c r="AY105" s="72"/>
       <c r="AZ105" s="72"/>
       <c r="BD105" s="8">
-        <v>30</v>
-      </c>
-      <c r="BE105" s="8">
-        <v>30</v>
+        <v>100</v>
       </c>
     </row>
     <row r="106" spans="1:58" x14ac:dyDescent="0.15">
       <c r="A106" s="94">
-        <v>42040017</v>
+        <v>42040015</v>
       </c>
       <c r="B106" s="96" t="s">
-        <v>634</v>
+        <v>630</v>
       </c>
       <c r="C106" s="8">
         <v>5</v>
@@ -11469,16 +11472,16 @@
         <v>0</v>
       </c>
       <c r="E106" s="8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F106" s="72" t="s">
-        <v>633</v>
+        <v>629</v>
       </c>
       <c r="G106" s="72" t="s">
-        <v>633</v>
+        <v>629</v>
       </c>
       <c r="H106" s="72" t="s">
-        <v>650</v>
+        <v>613</v>
       </c>
       <c r="I106" s="69" t="s">
         <v>656</v>
@@ -11500,31 +11503,36 @@
       <c r="T106" s="69"/>
       <c r="V106" s="72"/>
       <c r="AE106" s="72" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="AF106" s="8">
-        <v>3</v>
+        <v>2</v>
+      </c>
+      <c r="AG106" s="72" t="s">
+        <v>655</v>
+      </c>
+      <c r="AH106" s="8">
+        <v>2</v>
       </c>
       <c r="AN106" s="72"/>
       <c r="AO106" s="72"/>
       <c r="AP106" s="72"/>
       <c r="AQ106" s="72"/>
       <c r="AR106" s="72"/>
-      <c r="AT106" s="23"/>
       <c r="AU106" s="87"/>
       <c r="AV106" s="72"/>
       <c r="AY106" s="72"/>
       <c r="AZ106" s="72"/>
       <c r="BD106" s="8">
-        <v>100</v>
+        <v>150</v>
       </c>
     </row>
     <row r="107" spans="1:58" x14ac:dyDescent="0.15">
       <c r="A107" s="94">
-        <v>42040018</v>
+        <v>42040016</v>
       </c>
       <c r="B107" s="96" t="s">
-        <v>636</v>
+        <v>632</v>
       </c>
       <c r="C107" s="8">
         <v>5</v>
@@ -11533,25 +11541,23 @@
         <v>0</v>
       </c>
       <c r="E107" s="8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F107" s="72" t="s">
-        <v>635</v>
+        <v>631</v>
       </c>
       <c r="G107" s="72" t="s">
-        <v>635</v>
+        <v>631</v>
       </c>
       <c r="H107" s="72" t="s">
-        <v>650</v>
-      </c>
-      <c r="I107" s="69" t="s">
-        <v>656</v>
-      </c>
+        <v>631</v>
+      </c>
+      <c r="I107" s="69"/>
       <c r="J107" s="78" t="s">
         <v>558</v>
       </c>
-      <c r="K107" s="88" t="s">
-        <v>595</v>
+      <c r="K107" s="28" t="s">
+        <v>246</v>
       </c>
       <c r="L107" s="22"/>
       <c r="M107" s="22"/>
@@ -11564,36 +11570,40 @@
       <c r="T107" s="69"/>
       <c r="V107" s="72"/>
       <c r="AE107" s="72" t="s">
-        <v>651</v>
+        <v>652</v>
       </c>
       <c r="AF107" s="8">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="AG107" s="72" t="s">
-        <v>649</v>
+        <v>653</v>
       </c>
       <c r="AH107" s="8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AN107" s="72"/>
       <c r="AO107" s="72"/>
       <c r="AP107" s="72"/>
       <c r="AQ107" s="72"/>
       <c r="AR107" s="72"/>
+      <c r="AT107" s="24"/>
       <c r="AU107" s="87"/>
       <c r="AV107" s="72"/>
       <c r="AY107" s="72"/>
       <c r="AZ107" s="72"/>
       <c r="BD107" s="8">
-        <v>200</v>
+        <v>30</v>
+      </c>
+      <c r="BE107" s="8">
+        <v>30</v>
       </c>
     </row>
     <row r="108" spans="1:58" x14ac:dyDescent="0.15">
       <c r="A108" s="94">
-        <v>42040019</v>
+        <v>42040017</v>
       </c>
       <c r="B108" s="96" t="s">
-        <v>664</v>
+        <v>634</v>
       </c>
       <c r="C108" s="8">
         <v>5</v>
@@ -11601,18 +11611,23 @@
       <c r="D108" s="8">
         <v>0</v>
       </c>
+      <c r="E108" s="8">
+        <v>1</v>
+      </c>
       <c r="F108" s="72" t="s">
-        <v>665</v>
+        <v>633</v>
       </c>
       <c r="G108" s="72" t="s">
-        <v>665</v>
+        <v>633</v>
       </c>
       <c r="H108" s="72" t="s">
-        <v>665</v>
-      </c>
-      <c r="I108" s="69"/>
-      <c r="J108" s="85" t="s">
-        <v>583</v>
+        <v>650</v>
+      </c>
+      <c r="I108" s="69" t="s">
+        <v>656</v>
+      </c>
+      <c r="J108" s="78" t="s">
+        <v>558</v>
       </c>
       <c r="K108" s="88" t="s">
         <v>595</v>
@@ -11627,46 +11642,174 @@
       <c r="S108" s="24"/>
       <c r="T108" s="69"/>
       <c r="V108" s="72"/>
-      <c r="AC108" s="86" t="s">
-        <v>582</v>
-      </c>
-      <c r="AD108" s="8">
-        <v>5</v>
-      </c>
-      <c r="AE108" s="72"/>
-      <c r="AF108" s="72"/>
-      <c r="AG108" s="72"/>
-      <c r="AH108" s="72"/>
-      <c r="AI108" s="8">
-        <v>300</v>
-      </c>
-      <c r="AJ108" s="8">
-        <v>300</v>
+      <c r="AE108" s="72" t="s">
+        <v>653</v>
+      </c>
+      <c r="AF108" s="8">
+        <v>3</v>
       </c>
       <c r="AN108" s="72"/>
       <c r="AO108" s="72"/>
       <c r="AP108" s="72"/>
       <c r="AQ108" s="72"/>
       <c r="AR108" s="72"/>
+      <c r="AT108" s="23"/>
       <c r="AU108" s="87"/>
       <c r="AV108" s="72"/>
       <c r="AY108" s="72"/>
       <c r="AZ108" s="72"/>
+      <c r="BD108" s="8">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="109" spans="1:58" x14ac:dyDescent="0.15">
+      <c r="A109" s="94">
+        <v>42040018</v>
+      </c>
+      <c r="B109" s="96" t="s">
+        <v>636</v>
+      </c>
+      <c r="C109" s="8">
+        <v>5</v>
+      </c>
+      <c r="D109" s="8">
+        <v>0</v>
+      </c>
+      <c r="E109" s="8">
+        <v>2</v>
+      </c>
+      <c r="F109" s="72" t="s">
+        <v>635</v>
+      </c>
+      <c r="G109" s="72" t="s">
+        <v>635</v>
+      </c>
+      <c r="H109" s="72" t="s">
+        <v>650</v>
+      </c>
+      <c r="I109" s="69" t="s">
+        <v>656</v>
+      </c>
+      <c r="J109" s="78" t="s">
+        <v>558</v>
+      </c>
+      <c r="K109" s="88" t="s">
+        <v>595</v>
+      </c>
+      <c r="L109" s="22"/>
+      <c r="M109" s="22"/>
+      <c r="N109" s="22"/>
+      <c r="O109" s="22"/>
+      <c r="P109" s="22"/>
+      <c r="Q109" s="22"/>
+      <c r="R109" s="69"/>
+      <c r="S109" s="24"/>
+      <c r="T109" s="69"/>
+      <c r="V109" s="72"/>
+      <c r="AE109" s="72" t="s">
+        <v>651</v>
+      </c>
+      <c r="AF109" s="8">
+        <v>1</v>
+      </c>
+      <c r="AG109" s="72" t="s">
+        <v>649</v>
+      </c>
+      <c r="AH109" s="8">
+        <v>1</v>
+      </c>
+      <c r="AN109" s="72"/>
+      <c r="AO109" s="72"/>
+      <c r="AP109" s="72"/>
+      <c r="AQ109" s="72"/>
+      <c r="AR109" s="72"/>
+      <c r="AU109" s="87"/>
+      <c r="AV109" s="72"/>
+      <c r="AY109" s="72"/>
+      <c r="AZ109" s="72"/>
+      <c r="BD109" s="8">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="110" spans="1:58" x14ac:dyDescent="0.15">
+      <c r="A110" s="94">
+        <v>42040019</v>
+      </c>
+      <c r="B110" s="96" t="s">
+        <v>664</v>
+      </c>
+      <c r="C110" s="8">
+        <v>5</v>
+      </c>
+      <c r="D110" s="8">
+        <v>0</v>
+      </c>
+      <c r="F110" s="72" t="s">
+        <v>665</v>
+      </c>
+      <c r="G110" s="72" t="s">
+        <v>665</v>
+      </c>
+      <c r="H110" s="72" t="s">
+        <v>665</v>
+      </c>
+      <c r="I110" s="69"/>
+      <c r="J110" s="85" t="s">
+        <v>583</v>
+      </c>
+      <c r="K110" s="88" t="s">
+        <v>595</v>
+      </c>
+      <c r="L110" s="22"/>
+      <c r="M110" s="22"/>
+      <c r="N110" s="22"/>
+      <c r="O110" s="22"/>
+      <c r="P110" s="22"/>
+      <c r="Q110" s="22"/>
+      <c r="R110" s="69"/>
+      <c r="S110" s="24"/>
+      <c r="T110" s="69"/>
+      <c r="V110" s="72"/>
+      <c r="AC110" s="86" t="s">
+        <v>582</v>
+      </c>
+      <c r="AD110" s="8">
+        <v>5</v>
+      </c>
+      <c r="AE110" s="72"/>
+      <c r="AF110" s="72"/>
+      <c r="AG110" s="72"/>
+      <c r="AH110" s="72"/>
+      <c r="AI110" s="8">
+        <v>300</v>
+      </c>
+      <c r="AJ110" s="8">
+        <v>300</v>
+      </c>
+      <c r="AN110" s="72"/>
+      <c r="AO110" s="72"/>
+      <c r="AP110" s="72"/>
+      <c r="AQ110" s="72"/>
+      <c r="AR110" s="72"/>
+      <c r="AU110" s="87"/>
+      <c r="AV110" s="72"/>
+      <c r="AY110" s="72"/>
+      <c r="AZ110" s="72"/>
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
-  <conditionalFormatting sqref="K89:BP89 B4:BP88 B90:BP108">
-    <cfRule type="containsBlanks" dxfId="73" priority="15">
+  <conditionalFormatting sqref="K89:BP89 B4:BP88 B90:BP110">
+    <cfRule type="containsBlanks" dxfId="10" priority="15">
       <formula>LEN(TRIM(B4))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B89:I89">
-    <cfRule type="containsBlanks" dxfId="72" priority="2">
+    <cfRule type="containsBlanks" dxfId="9" priority="2">
       <formula>LEN(TRIM(B89))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J89">
-    <cfRule type="containsBlanks" dxfId="71" priority="1">
+    <cfRule type="containsBlanks" dxfId="8" priority="1">
       <formula>LEN(TRIM(J89))=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11683,8 +11826,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BP39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AD1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="AW1" sqref="AW1:AX3"/>
     </sheetView>
   </sheetViews>
@@ -14251,42 +14394,42 @@
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <conditionalFormatting sqref="J39:S39 D4:S10 J11:S11 D12:S29 J30:S30 T4:BP39 D31:S34 D36:S37 J35:S35 D38:Q38 S38">
-    <cfRule type="containsBlanks" dxfId="43" priority="12">
+    <cfRule type="containsBlanks" dxfId="7" priority="12">
       <formula>LEN(TRIM(D4))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D39:I39">
-    <cfRule type="containsBlanks" dxfId="42" priority="9">
+    <cfRule type="containsBlanks" dxfId="6" priority="9">
       <formula>LEN(TRIM(D39))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D11:I11">
-    <cfRule type="containsBlanks" dxfId="41" priority="7">
+    <cfRule type="containsBlanks" dxfId="5" priority="7">
       <formula>LEN(TRIM(D11))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D30:E30 I30 G30">
-    <cfRule type="containsBlanks" dxfId="40" priority="6">
+    <cfRule type="containsBlanks" dxfId="4" priority="6">
       <formula>LEN(TRIM(D30))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H30">
-    <cfRule type="containsBlanks" dxfId="39" priority="5">
+    <cfRule type="containsBlanks" dxfId="3" priority="5">
       <formula>LEN(TRIM(H30))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F30">
-    <cfRule type="containsBlanks" dxfId="38" priority="3">
+    <cfRule type="containsBlanks" dxfId="2" priority="3">
       <formula>LEN(TRIM(F30))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D35:I35">
-    <cfRule type="containsBlanks" dxfId="37" priority="2">
+    <cfRule type="containsBlanks" dxfId="1" priority="2">
       <formula>LEN(TRIM(D35))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R38">
-    <cfRule type="containsBlanks" dxfId="36" priority="1">
+    <cfRule type="containsBlanks" dxfId="0" priority="1">
       <formula>LEN(TRIM(R38))=0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
add basically select card form
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/SceneQuest.xlsx
+++ b/ConfigData/Xlsx/SceneQuest.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18625"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Code\TOMClassicGit\ConfigData\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TOMClassic\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -154,7 +154,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1341" uniqueCount="693">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1344" uniqueCount="696">
   <si>
     <t>int</t>
     <phoneticPr fontId="18" type="noConversion"/>
@@ -2811,6 +2811,18 @@
   </si>
   <si>
     <t>临时卡关键词3</t>
+  </si>
+  <si>
+    <t>attr.2</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>attr.3</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>attr.4</t>
+    <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -4010,77 +4022,7 @@
     <cellStyle name="着色 6" xfId="38" builtinId="49" customBuiltin="1"/>
     <cellStyle name="注释" xfId="15" builtinId="10" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="89">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="73">
     <dxf>
       <font>
         <b val="0"/>
@@ -4166,119 +4108,6 @@
         </top>
         <bottom/>
       </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="宋体"/>
-        <family val="2"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="宋体"/>
-        <family val="2"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="宋体"/>
-        <family val="2"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <font>
@@ -4833,6 +4662,70 @@
       </fill>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -5211,75 +5104,16 @@
         </patternFill>
       </fill>
     </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
     <mruColors>
       <color rgb="FFADADDD"/>
       <color rgb="FFD9A7A7"/>
@@ -5304,7 +5138,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="表3" displayName="表3" ref="A3:BT111" totalsRowShown="0" headerRowDxfId="88">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="表3" displayName="表3" ref="A3:BT111" totalsRowShown="0" headerRowDxfId="71">
   <autoFilter ref="A3:BT111"/>
   <sortState ref="A4:BQ111">
     <sortCondition ref="A3:A111"/>
@@ -5318,51 +5152,51 @@
     <tableColumn id="24" name="Ename"/>
     <tableColumn id="4" name="Figue"/>
     <tableColumn id="5" name="Script"/>
-    <tableColumn id="6" name="TriggerMulti" dataDxfId="87"/>
-    <tableColumn id="69" name="Tag" dataDxfId="86"/>
-    <tableColumn id="40" name="Catalog" dataDxfId="85"/>
+    <tableColumn id="6" name="TriggerMulti" dataDxfId="70"/>
+    <tableColumn id="69" name="Tag" dataDxfId="69"/>
+    <tableColumn id="40" name="Catalog" dataDxfId="68"/>
     <tableColumn id="29" name="Catalog2"/>
-    <tableColumn id="35" name="TriggerHourBegin" dataDxfId="84"/>
-    <tableColumn id="34" name="TriggerHourEnd" dataDxfId="83"/>
-    <tableColumn id="36" name="TriggerQuestNotReceive" dataDxfId="82"/>
-    <tableColumn id="37" name="TriggerQuestReceived" dataDxfId="81"/>
-    <tableColumn id="38" name="TriggerQuestFinished" dataDxfId="80"/>
-    <tableColumn id="39" name="TriggerRate" dataDxfId="79"/>
-    <tableColumn id="62" name="TriggerOnceInDungeon" dataDxfId="78"/>
+    <tableColumn id="35" name="TriggerHourBegin" dataDxfId="67"/>
+    <tableColumn id="34" name="TriggerHourEnd" dataDxfId="66"/>
+    <tableColumn id="36" name="TriggerQuestNotReceive" dataDxfId="65"/>
+    <tableColumn id="37" name="TriggerQuestReceived" dataDxfId="64"/>
+    <tableColumn id="38" name="TriggerQuestFinished" dataDxfId="63"/>
+    <tableColumn id="39" name="TriggerRate" dataDxfId="62"/>
+    <tableColumn id="62" name="TriggerOnceInDungeon" dataDxfId="61"/>
     <tableColumn id="7" name="EnemyName"/>
-    <tableColumn id="51" name="CanBribe" dataDxfId="77"/>
+    <tableColumn id="51" name="CanBribe" dataDxfId="60"/>
     <tableColumn id="32" name="SceneId"/>
-    <tableColumn id="54" name="DungeonId" dataDxfId="76"/>
+    <tableColumn id="54" name="DungeonId" dataDxfId="59"/>
     <tableColumn id="50" name="CheckQuest"/>
     <tableColumn id="27" name="NextQuest"/>
     <tableColumn id="44" name="HiddenRoomQuest"/>
     <tableColumn id="8" name="ShopName"/>
     <tableColumn id="41" name="MiniGameId"/>
     <tableColumn id="43" name="PayKey"/>
-    <tableColumn id="67" name="NeedDungeonItemId" dataDxfId="75"/>
-    <tableColumn id="68" name="NeedDungeonItemCount" dataDxfId="74"/>
-    <tableColumn id="63" name="TestType1" dataDxfId="73"/>
-    <tableColumn id="64" name="TestBias1" dataDxfId="72"/>
-    <tableColumn id="65" name="TestType2" dataDxfId="71"/>
-    <tableColumn id="66" name="TestBias2" dataDxfId="70"/>
+    <tableColumn id="67" name="NeedDungeonItemId" dataDxfId="58"/>
+    <tableColumn id="68" name="NeedDungeonItemCount" dataDxfId="57"/>
+    <tableColumn id="63" name="TestType1" dataDxfId="56"/>
+    <tableColumn id="64" name="TestBias1" dataDxfId="55"/>
+    <tableColumn id="65" name="TestType2" dataDxfId="54"/>
+    <tableColumn id="66" name="TestBias2" dataDxfId="53"/>
     <tableColumn id="9" name="RewardGold"/>
     <tableColumn id="10" name="RewardFood"/>
     <tableColumn id="11" name="RewardHealth"/>
     <tableColumn id="12" name="RewardMental"/>
     <tableColumn id="13" name="RewardExp"/>
-    <tableColumn id="56" name="RewardStr" dataDxfId="69"/>
-    <tableColumn id="57" name="RewardAgi" dataDxfId="68"/>
-    <tableColumn id="58" name="RewardIntl" dataDxfId="67"/>
-    <tableColumn id="59" name="RewardPerc" dataDxfId="66"/>
-    <tableColumn id="60" name="RewardEndu" dataDxfId="65"/>
+    <tableColumn id="56" name="RewardStr" dataDxfId="52"/>
+    <tableColumn id="57" name="RewardAgi" dataDxfId="51"/>
+    <tableColumn id="58" name="RewardIntl" dataDxfId="50"/>
+    <tableColumn id="59" name="RewardPerc" dataDxfId="49"/>
+    <tableColumn id="60" name="RewardEndu" dataDxfId="48"/>
     <tableColumn id="14" name="RewardItem"/>
     <tableColumn id="15" name="RewardDrop"/>
-    <tableColumn id="55" name="RewardDungeonItemId" dataDxfId="64"/>
-    <tableColumn id="61" name="RewardDungeonItemCount" dataDxfId="63"/>
+    <tableColumn id="55" name="RewardDungeonItemId" dataDxfId="47"/>
+    <tableColumn id="61" name="RewardDungeonItemCount" dataDxfId="46"/>
     <tableColumn id="30" name="RewardBlessLevel"/>
     <tableColumn id="42" name="RewardBlessName"/>
-    <tableColumn id="52" name="RewardResId" dataDxfId="62"/>
-    <tableColumn id="53" name="RewardResAmount" dataDxfId="61"/>
+    <tableColumn id="52" name="RewardResId" dataDxfId="45"/>
+    <tableColumn id="53" name="RewardResAmount" dataDxfId="44"/>
     <tableColumn id="26" name="UnlockRival"/>
     <tableColumn id="16" name="PunishGold"/>
     <tableColumn id="17" name="PunishFood"/>
@@ -5379,16 +5213,16 @@
     <tableColumn id="22" name="TradeHealth"/>
     <tableColumn id="23" name="TradeMental"/>
     <tableColumn id="33" name="TradeDropItem"/>
-    <tableColumn id="70" name="DeckCardAttr1" dataDxfId="16"/>
-    <tableColumn id="71" name="DeckCardAttr2" dataDxfId="15"/>
-    <tableColumn id="72" name="DeckCardAttr3" dataDxfId="14"/>
+    <tableColumn id="70" name="DeckCardAttr1" dataDxfId="43"/>
+    <tableColumn id="71" name="DeckCardAttr2" dataDxfId="42"/>
+    <tableColumn id="72" name="DeckCardAttr3" dataDxfId="41"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="表3_5" displayName="表3_5" ref="A3:BT39" totalsRowShown="0" headerRowDxfId="60">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="表3_5" displayName="表3_5" ref="A3:BT39" totalsRowShown="0" headerRowDxfId="39">
   <autoFilter ref="A3:BT39"/>
   <sortState ref="A4:AU6">
     <sortCondition ref="A3:A6"/>
@@ -5396,57 +5230,57 @@
   <tableColumns count="72">
     <tableColumn id="1" name="Id"/>
     <tableColumn id="2" name="Name"/>
-    <tableColumn id="27" name="Type" dataDxfId="59"/>
+    <tableColumn id="27" name="Type" dataDxfId="38"/>
     <tableColumn id="3" name="Level"/>
     <tableColumn id="25" name="Danger"/>
     <tableColumn id="24" name="Ename"/>
     <tableColumn id="4" name="Figue"/>
     <tableColumn id="5" name="Script"/>
     <tableColumn id="6" name="TriggerMulti"/>
-    <tableColumn id="69" name="Tag" dataDxfId="58"/>
-    <tableColumn id="40" name="Catalog" dataDxfId="57"/>
-    <tableColumn id="29" name="Catalog2" dataDxfId="56"/>
-    <tableColumn id="35" name="TriggerHourBegin" dataDxfId="55"/>
-    <tableColumn id="34" name="TriggerHourEnd" dataDxfId="54"/>
-    <tableColumn id="37" name="TriggerQuestNotReceive" dataDxfId="53"/>
-    <tableColumn id="38" name="TriggerQuestReceived" dataDxfId="52"/>
-    <tableColumn id="36" name="TriggerQuestFinished" dataDxfId="51"/>
-    <tableColumn id="39" name="TriggerRate" dataDxfId="50"/>
-    <tableColumn id="62" name="TriggerOnceInDungeon" dataDxfId="49"/>
+    <tableColumn id="69" name="Tag" dataDxfId="37"/>
+    <tableColumn id="40" name="Catalog" dataDxfId="36"/>
+    <tableColumn id="29" name="Catalog2" dataDxfId="35"/>
+    <tableColumn id="35" name="TriggerHourBegin" dataDxfId="34"/>
+    <tableColumn id="34" name="TriggerHourEnd" dataDxfId="33"/>
+    <tableColumn id="37" name="TriggerQuestNotReceive" dataDxfId="32"/>
+    <tableColumn id="38" name="TriggerQuestReceived" dataDxfId="31"/>
+    <tableColumn id="36" name="TriggerQuestFinished" dataDxfId="30"/>
+    <tableColumn id="39" name="TriggerRate" dataDxfId="29"/>
+    <tableColumn id="62" name="TriggerOnceInDungeon" dataDxfId="28"/>
     <tableColumn id="7" name="EnemyName"/>
-    <tableColumn id="51" name="CanBribe" dataDxfId="48"/>
-    <tableColumn id="32" name="SceneId" dataDxfId="47"/>
-    <tableColumn id="54" name="DungeonId" dataDxfId="46"/>
-    <tableColumn id="50" name="CheckQuest" dataDxfId="45"/>
-    <tableColumn id="28" name="NextQuest" dataDxfId="44"/>
-    <tableColumn id="44" name="HiddenRoomQuest" dataDxfId="43"/>
-    <tableColumn id="8" name="ShopName" dataDxfId="42"/>
-    <tableColumn id="41" name="MiniGameId" dataDxfId="41"/>
-    <tableColumn id="43" name="PayKey" dataDxfId="40"/>
-    <tableColumn id="67" name="NeedDungeonItemId" dataDxfId="39"/>
-    <tableColumn id="68" name="NeedDungeonItemCount" dataDxfId="38"/>
-    <tableColumn id="63" name="TestType1" dataDxfId="37"/>
-    <tableColumn id="64" name="TestBias1" dataDxfId="36"/>
-    <tableColumn id="65" name="TestType2" dataDxfId="35"/>
-    <tableColumn id="66" name="TestBias2" dataDxfId="34"/>
+    <tableColumn id="51" name="CanBribe" dataDxfId="27"/>
+    <tableColumn id="32" name="SceneId" dataDxfId="26"/>
+    <tableColumn id="54" name="DungeonId" dataDxfId="25"/>
+    <tableColumn id="50" name="CheckQuest" dataDxfId="24"/>
+    <tableColumn id="28" name="NextQuest" dataDxfId="23"/>
+    <tableColumn id="44" name="HiddenRoomQuest" dataDxfId="22"/>
+    <tableColumn id="8" name="ShopName" dataDxfId="21"/>
+    <tableColumn id="41" name="MiniGameId" dataDxfId="20"/>
+    <tableColumn id="43" name="PayKey" dataDxfId="19"/>
+    <tableColumn id="67" name="NeedDungeonItemId" dataDxfId="18"/>
+    <tableColumn id="68" name="NeedDungeonItemCount" dataDxfId="17"/>
+    <tableColumn id="63" name="TestType1" dataDxfId="16"/>
+    <tableColumn id="64" name="TestBias1" dataDxfId="15"/>
+    <tableColumn id="65" name="TestType2" dataDxfId="14"/>
+    <tableColumn id="66" name="TestBias2" dataDxfId="13"/>
     <tableColumn id="9" name="RewardGold"/>
     <tableColumn id="10" name="RewardFood"/>
     <tableColumn id="11" name="RewardHealth"/>
     <tableColumn id="12" name="RewardMental"/>
     <tableColumn id="13" name="RewardExp"/>
-    <tableColumn id="55" name="RewardStr" dataDxfId="33"/>
-    <tableColumn id="56" name="RewardAgi" dataDxfId="32"/>
-    <tableColumn id="57" name="RewardIntl" dataDxfId="31"/>
-    <tableColumn id="58" name="RewardPerc" dataDxfId="30"/>
-    <tableColumn id="59" name="RewardEndu" dataDxfId="29"/>
+    <tableColumn id="55" name="RewardStr" dataDxfId="12"/>
+    <tableColumn id="56" name="RewardAgi" dataDxfId="11"/>
+    <tableColumn id="57" name="RewardIntl" dataDxfId="10"/>
+    <tableColumn id="58" name="RewardPerc" dataDxfId="9"/>
+    <tableColumn id="59" name="RewardEndu" dataDxfId="8"/>
     <tableColumn id="14" name="RewardItem"/>
     <tableColumn id="15" name="RewardDrop"/>
-    <tableColumn id="60" name="RewardDungeonItemId" dataDxfId="28"/>
-    <tableColumn id="61" name="RewardDungeonItemCount" dataDxfId="27"/>
+    <tableColumn id="60" name="RewardDungeonItemId" dataDxfId="7"/>
+    <tableColumn id="61" name="RewardDungeonItemCount" dataDxfId="6"/>
     <tableColumn id="31" name="RewardBlessLevel"/>
     <tableColumn id="42" name="RewardBlessName"/>
-    <tableColumn id="52" name="RewardResId" dataDxfId="26"/>
-    <tableColumn id="53" name="RewardResAmount" dataDxfId="25"/>
+    <tableColumn id="52" name="RewardResId" dataDxfId="5"/>
+    <tableColumn id="53" name="RewardResAmount" dataDxfId="4"/>
     <tableColumn id="26" name="UnlockRival"/>
     <tableColumn id="16" name="PunishGold"/>
     <tableColumn id="17" name="PunishFood"/>
@@ -5462,10 +5296,10 @@
     <tableColumn id="21" name="TradeFood"/>
     <tableColumn id="22" name="TradeHealth"/>
     <tableColumn id="23" name="TradeMental"/>
-    <tableColumn id="33" name="TradeDropItem" dataDxfId="13"/>
-    <tableColumn id="70" name="DeckCardAttr1" dataDxfId="12"/>
-    <tableColumn id="71" name="DeckCardAttr2" dataDxfId="11"/>
-    <tableColumn id="72" name="DeckCardAttr3" dataDxfId="10"/>
+    <tableColumn id="33" name="TradeDropItem" dataDxfId="3"/>
+    <tableColumn id="70" name="DeckCardAttr1" dataDxfId="2"/>
+    <tableColumn id="71" name="DeckCardAttr2" dataDxfId="1"/>
+    <tableColumn id="72" name="DeckCardAttr3" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5479,7 +5313,7 @@
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="C7EDCC"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -5794,9 +5628,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BT111"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A79" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M93" sqref="M93"/>
+    <sheetView tabSelected="1" topLeftCell="AM1" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="BT4" sqref="BT4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -6606,6 +6440,15 @@
       <c r="BL4" s="8">
         <v>35</v>
       </c>
+      <c r="BR4" s="70" t="s">
+        <v>693</v>
+      </c>
+      <c r="BS4" s="70" t="s">
+        <v>694</v>
+      </c>
+      <c r="BT4" s="70" t="s">
+        <v>695</v>
+      </c>
     </row>
     <row r="5" spans="1:72" x14ac:dyDescent="0.15">
       <c r="A5" s="25">
@@ -12390,7 +12233,7 @@
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <conditionalFormatting sqref="E4:BT111">
-    <cfRule type="containsBlanks" dxfId="5" priority="17">
+    <cfRule type="containsBlanks" dxfId="72" priority="17">
       <formula>LEN(TRIM(E4))=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -15012,7 +14855,7 @@
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <conditionalFormatting sqref="E4:BT39">
-    <cfRule type="containsBlanks" dxfId="7" priority="13">
+    <cfRule type="containsBlanks" dxfId="40" priority="13">
       <formula>LEN(TRIM(E4))=0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
fnish the drop by attr
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/SceneQuest.xlsx
+++ b/ConfigData/Xlsx/SceneQuest.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="4" r:id="rId1"/>
@@ -154,7 +154,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1366" uniqueCount="708">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1362" uniqueCount="706">
   <si>
     <t>int</t>
     <phoneticPr fontId="18" type="noConversion"/>
@@ -2856,19 +2856,11 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>是否是采集</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>bool</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>RewardCollect</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>true</t>
+    <t>采集组id</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>RewardCollectType</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -4055,7 +4047,7 @@
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -4104,58 +4096,6 @@
     <cellStyle name="注释" xfId="15" builtinId="10" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="75">
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="宋体"/>
-        <family val="2"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="宋体"/>
-        <family val="2"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -4241,6 +4181,25 @@
         </top>
         <bottom/>
       </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </font>
     </dxf>
     <dxf>
       <font>
@@ -4795,6 +4754,32 @@
       </fill>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -5230,6 +5215,13 @@
         </patternFill>
       </fill>
     </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -5257,7 +5249,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="表3" displayName="表3" ref="A3:BU113" totalsRowShown="0" headerRowDxfId="74">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="表3" displayName="表3" ref="A3:BU113" totalsRowShown="0" headerRowDxfId="73">
   <autoFilter ref="A3:BU113" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <sortState ref="A4:BR112">
     <sortCondition ref="A3:A112"/>
@@ -5271,52 +5263,52 @@
     <tableColumn id="24" xr3:uid="{00000000-0010-0000-0000-000018000000}" name="Ename"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Figue"/>
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Script"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="TriggerMulti" dataDxfId="73"/>
-    <tableColumn id="69" xr3:uid="{00000000-0010-0000-0000-000045000000}" name="Tag" dataDxfId="72"/>
-    <tableColumn id="40" xr3:uid="{00000000-0010-0000-0000-000028000000}" name="Catalog" dataDxfId="71"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="TriggerMulti" dataDxfId="72"/>
+    <tableColumn id="69" xr3:uid="{00000000-0010-0000-0000-000045000000}" name="Tag" dataDxfId="71"/>
+    <tableColumn id="40" xr3:uid="{00000000-0010-0000-0000-000028000000}" name="Catalog" dataDxfId="70"/>
     <tableColumn id="29" xr3:uid="{00000000-0010-0000-0000-00001D000000}" name="Catalog2"/>
-    <tableColumn id="35" xr3:uid="{00000000-0010-0000-0000-000023000000}" name="TriggerHourBegin" dataDxfId="70"/>
-    <tableColumn id="34" xr3:uid="{00000000-0010-0000-0000-000022000000}" name="TriggerHourEnd" dataDxfId="69"/>
-    <tableColumn id="36" xr3:uid="{00000000-0010-0000-0000-000024000000}" name="TriggerQuestNotReceive" dataDxfId="68"/>
-    <tableColumn id="37" xr3:uid="{00000000-0010-0000-0000-000025000000}" name="TriggerQuestReceived" dataDxfId="67"/>
-    <tableColumn id="38" xr3:uid="{00000000-0010-0000-0000-000026000000}" name="TriggerQuestFinished" dataDxfId="66"/>
-    <tableColumn id="39" xr3:uid="{00000000-0010-0000-0000-000027000000}" name="TriggerRate" dataDxfId="65"/>
-    <tableColumn id="62" xr3:uid="{00000000-0010-0000-0000-00003E000000}" name="TriggerOnceInDungeon" dataDxfId="64"/>
+    <tableColumn id="35" xr3:uid="{00000000-0010-0000-0000-000023000000}" name="TriggerHourBegin" dataDxfId="69"/>
+    <tableColumn id="34" xr3:uid="{00000000-0010-0000-0000-000022000000}" name="TriggerHourEnd" dataDxfId="68"/>
+    <tableColumn id="36" xr3:uid="{00000000-0010-0000-0000-000024000000}" name="TriggerQuestNotReceive" dataDxfId="67"/>
+    <tableColumn id="37" xr3:uid="{00000000-0010-0000-0000-000025000000}" name="TriggerQuestReceived" dataDxfId="66"/>
+    <tableColumn id="38" xr3:uid="{00000000-0010-0000-0000-000026000000}" name="TriggerQuestFinished" dataDxfId="65"/>
+    <tableColumn id="39" xr3:uid="{00000000-0010-0000-0000-000027000000}" name="TriggerRate" dataDxfId="64"/>
+    <tableColumn id="62" xr3:uid="{00000000-0010-0000-0000-00003E000000}" name="TriggerOnceInDungeon" dataDxfId="63"/>
     <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="EnemyName"/>
-    <tableColumn id="51" xr3:uid="{00000000-0010-0000-0000-000033000000}" name="CanBribe" dataDxfId="63"/>
+    <tableColumn id="51" xr3:uid="{00000000-0010-0000-0000-000033000000}" name="CanBribe" dataDxfId="62"/>
     <tableColumn id="32" xr3:uid="{00000000-0010-0000-0000-000020000000}" name="SceneId"/>
-    <tableColumn id="54" xr3:uid="{00000000-0010-0000-0000-000036000000}" name="DungeonId" dataDxfId="62"/>
+    <tableColumn id="54" xr3:uid="{00000000-0010-0000-0000-000036000000}" name="DungeonId" dataDxfId="61"/>
     <tableColumn id="50" xr3:uid="{00000000-0010-0000-0000-000032000000}" name="CheckQuest"/>
     <tableColumn id="27" xr3:uid="{00000000-0010-0000-0000-00001B000000}" name="NextQuest"/>
     <tableColumn id="44" xr3:uid="{00000000-0010-0000-0000-00002C000000}" name="HiddenRoomQuest"/>
     <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="ShopName"/>
     <tableColumn id="41" xr3:uid="{00000000-0010-0000-0000-000029000000}" name="MiniGameId"/>
     <tableColumn id="43" xr3:uid="{00000000-0010-0000-0000-00002B000000}" name="PayKey"/>
-    <tableColumn id="67" xr3:uid="{00000000-0010-0000-0000-000043000000}" name="NeedDungeonItemId" dataDxfId="61"/>
-    <tableColumn id="68" xr3:uid="{00000000-0010-0000-0000-000044000000}" name="NeedDungeonItemCount" dataDxfId="60"/>
-    <tableColumn id="63" xr3:uid="{00000000-0010-0000-0000-00003F000000}" name="TestType1" dataDxfId="59"/>
-    <tableColumn id="64" xr3:uid="{00000000-0010-0000-0000-000040000000}" name="TestBias1" dataDxfId="58"/>
-    <tableColumn id="65" xr3:uid="{00000000-0010-0000-0000-000041000000}" name="TestType2" dataDxfId="57"/>
-    <tableColumn id="66" xr3:uid="{00000000-0010-0000-0000-000042000000}" name="TestBias2" dataDxfId="56"/>
+    <tableColumn id="67" xr3:uid="{00000000-0010-0000-0000-000043000000}" name="NeedDungeonItemId" dataDxfId="60"/>
+    <tableColumn id="68" xr3:uid="{00000000-0010-0000-0000-000044000000}" name="NeedDungeonItemCount" dataDxfId="59"/>
+    <tableColumn id="63" xr3:uid="{00000000-0010-0000-0000-00003F000000}" name="TestType1" dataDxfId="58"/>
+    <tableColumn id="64" xr3:uid="{00000000-0010-0000-0000-000040000000}" name="TestBias1" dataDxfId="57"/>
+    <tableColumn id="65" xr3:uid="{00000000-0010-0000-0000-000041000000}" name="TestType2" dataDxfId="56"/>
+    <tableColumn id="66" xr3:uid="{00000000-0010-0000-0000-000042000000}" name="TestBias2" dataDxfId="55"/>
     <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="RewardGold"/>
     <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="RewardFood"/>
     <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="RewardHealth"/>
     <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="RewardMental"/>
     <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="RewardExp"/>
-    <tableColumn id="56" xr3:uid="{00000000-0010-0000-0000-000038000000}" name="RewardStr" dataDxfId="55"/>
-    <tableColumn id="57" xr3:uid="{00000000-0010-0000-0000-000039000000}" name="RewardAgi" dataDxfId="54"/>
-    <tableColumn id="58" xr3:uid="{00000000-0010-0000-0000-00003A000000}" name="RewardIntl" dataDxfId="53"/>
-    <tableColumn id="59" xr3:uid="{00000000-0010-0000-0000-00003B000000}" name="RewardPerc" dataDxfId="52"/>
-    <tableColumn id="60" xr3:uid="{00000000-0010-0000-0000-00003C000000}" name="RewardEndu" dataDxfId="51"/>
+    <tableColumn id="56" xr3:uid="{00000000-0010-0000-0000-000038000000}" name="RewardStr" dataDxfId="54"/>
+    <tableColumn id="57" xr3:uid="{00000000-0010-0000-0000-000039000000}" name="RewardAgi" dataDxfId="53"/>
+    <tableColumn id="58" xr3:uid="{00000000-0010-0000-0000-00003A000000}" name="RewardIntl" dataDxfId="52"/>
+    <tableColumn id="59" xr3:uid="{00000000-0010-0000-0000-00003B000000}" name="RewardPerc" dataDxfId="51"/>
+    <tableColumn id="60" xr3:uid="{00000000-0010-0000-0000-00003C000000}" name="RewardEndu" dataDxfId="50"/>
     <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="RewardItem"/>
     <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="RewardDrop"/>
-    <tableColumn id="73" xr3:uid="{157DA62A-68A2-4B19-BA98-29123331AFFC}" name="RewardCollect" dataDxfId="3"/>
-    <tableColumn id="55" xr3:uid="{00000000-0010-0000-0000-000037000000}" name="RewardDungeonItemId" dataDxfId="50"/>
-    <tableColumn id="61" xr3:uid="{00000000-0010-0000-0000-00003D000000}" name="RewardDungeonItemCount" dataDxfId="49"/>
+    <tableColumn id="73" xr3:uid="{157DA62A-68A2-4B19-BA98-29123331AFFC}" name="RewardCollectType" dataDxfId="49"/>
+    <tableColumn id="55" xr3:uid="{00000000-0010-0000-0000-000037000000}" name="RewardDungeonItemId" dataDxfId="48"/>
+    <tableColumn id="61" xr3:uid="{00000000-0010-0000-0000-00003D000000}" name="RewardDungeonItemCount" dataDxfId="47"/>
     <tableColumn id="30" xr3:uid="{00000000-0010-0000-0000-00001E000000}" name="RewardBlessLevel"/>
     <tableColumn id="42" xr3:uid="{00000000-0010-0000-0000-00002A000000}" name="RewardBlessName"/>
-    <tableColumn id="52" xr3:uid="{00000000-0010-0000-0000-000034000000}" name="RewardResId" dataDxfId="48"/>
-    <tableColumn id="53" xr3:uid="{00000000-0010-0000-0000-000035000000}" name="RewardResAmount" dataDxfId="47"/>
+    <tableColumn id="52" xr3:uid="{00000000-0010-0000-0000-000034000000}" name="RewardResId" dataDxfId="46"/>
+    <tableColumn id="53" xr3:uid="{00000000-0010-0000-0000-000035000000}" name="RewardResAmount" dataDxfId="45"/>
     <tableColumn id="26" xr3:uid="{00000000-0010-0000-0000-00001A000000}" name="UnlockRival"/>
     <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="PunishGold"/>
     <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="PunishFood"/>
@@ -5333,16 +5325,16 @@
     <tableColumn id="22" xr3:uid="{00000000-0010-0000-0000-000016000000}" name="TradeHealth"/>
     <tableColumn id="23" xr3:uid="{00000000-0010-0000-0000-000017000000}" name="TradeMental"/>
     <tableColumn id="33" xr3:uid="{00000000-0010-0000-0000-000021000000}" name="TradeDropItem"/>
-    <tableColumn id="70" xr3:uid="{00000000-0010-0000-0000-000046000000}" name="DeckCardAttr1" dataDxfId="46"/>
-    <tableColumn id="71" xr3:uid="{00000000-0010-0000-0000-000047000000}" name="DeckCardAttr2" dataDxfId="45"/>
-    <tableColumn id="72" xr3:uid="{00000000-0010-0000-0000-000048000000}" name="DeckCardAttr3" dataDxfId="44"/>
+    <tableColumn id="70" xr3:uid="{00000000-0010-0000-0000-000046000000}" name="DeckCardAttr1" dataDxfId="44"/>
+    <tableColumn id="71" xr3:uid="{00000000-0010-0000-0000-000047000000}" name="DeckCardAttr2" dataDxfId="43"/>
+    <tableColumn id="72" xr3:uid="{00000000-0010-0000-0000-000048000000}" name="DeckCardAttr3" dataDxfId="42"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="表3_5" displayName="表3_5" ref="A3:BU39" totalsRowShown="0" headerRowDxfId="43">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="表3_5" displayName="表3_5" ref="A3:BU39" totalsRowShown="0" headerRowDxfId="40">
   <autoFilter ref="A3:BU39" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
   <sortState ref="A4:AU6">
     <sortCondition ref="A3:A6"/>
@@ -5350,58 +5342,58 @@
   <tableColumns count="73">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Id"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Name"/>
-    <tableColumn id="27" xr3:uid="{00000000-0010-0000-0100-00001B000000}" name="Type" dataDxfId="42"/>
+    <tableColumn id="27" xr3:uid="{00000000-0010-0000-0100-00001B000000}" name="Type" dataDxfId="39"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Level"/>
     <tableColumn id="25" xr3:uid="{00000000-0010-0000-0100-000019000000}" name="Danger"/>
     <tableColumn id="24" xr3:uid="{00000000-0010-0000-0100-000018000000}" name="Ename"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Figue"/>
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="Script"/>
     <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="TriggerMulti"/>
-    <tableColumn id="69" xr3:uid="{00000000-0010-0000-0100-000045000000}" name="Tag" dataDxfId="41"/>
-    <tableColumn id="40" xr3:uid="{00000000-0010-0000-0100-000028000000}" name="Catalog" dataDxfId="40"/>
-    <tableColumn id="29" xr3:uid="{00000000-0010-0000-0100-00001D000000}" name="Catalog2" dataDxfId="39"/>
-    <tableColumn id="35" xr3:uid="{00000000-0010-0000-0100-000023000000}" name="TriggerHourBegin" dataDxfId="38"/>
-    <tableColumn id="34" xr3:uid="{00000000-0010-0000-0100-000022000000}" name="TriggerHourEnd" dataDxfId="37"/>
-    <tableColumn id="37" xr3:uid="{00000000-0010-0000-0100-000025000000}" name="TriggerQuestNotReceive" dataDxfId="36"/>
-    <tableColumn id="38" xr3:uid="{00000000-0010-0000-0100-000026000000}" name="TriggerQuestReceived" dataDxfId="35"/>
-    <tableColumn id="36" xr3:uid="{00000000-0010-0000-0100-000024000000}" name="TriggerQuestFinished" dataDxfId="34"/>
-    <tableColumn id="39" xr3:uid="{00000000-0010-0000-0100-000027000000}" name="TriggerRate" dataDxfId="33"/>
-    <tableColumn id="62" xr3:uid="{00000000-0010-0000-0100-00003E000000}" name="TriggerOnceInDungeon" dataDxfId="32"/>
+    <tableColumn id="69" xr3:uid="{00000000-0010-0000-0100-000045000000}" name="Tag" dataDxfId="38"/>
+    <tableColumn id="40" xr3:uid="{00000000-0010-0000-0100-000028000000}" name="Catalog" dataDxfId="37"/>
+    <tableColumn id="29" xr3:uid="{00000000-0010-0000-0100-00001D000000}" name="Catalog2" dataDxfId="36"/>
+    <tableColumn id="35" xr3:uid="{00000000-0010-0000-0100-000023000000}" name="TriggerHourBegin" dataDxfId="35"/>
+    <tableColumn id="34" xr3:uid="{00000000-0010-0000-0100-000022000000}" name="TriggerHourEnd" dataDxfId="34"/>
+    <tableColumn id="37" xr3:uid="{00000000-0010-0000-0100-000025000000}" name="TriggerQuestNotReceive" dataDxfId="33"/>
+    <tableColumn id="38" xr3:uid="{00000000-0010-0000-0100-000026000000}" name="TriggerQuestReceived" dataDxfId="32"/>
+    <tableColumn id="36" xr3:uid="{00000000-0010-0000-0100-000024000000}" name="TriggerQuestFinished" dataDxfId="31"/>
+    <tableColumn id="39" xr3:uid="{00000000-0010-0000-0100-000027000000}" name="TriggerRate" dataDxfId="30"/>
+    <tableColumn id="62" xr3:uid="{00000000-0010-0000-0100-00003E000000}" name="TriggerOnceInDungeon" dataDxfId="29"/>
     <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="EnemyName"/>
-    <tableColumn id="51" xr3:uid="{00000000-0010-0000-0100-000033000000}" name="CanBribe" dataDxfId="31"/>
-    <tableColumn id="32" xr3:uid="{00000000-0010-0000-0100-000020000000}" name="SceneId" dataDxfId="30"/>
-    <tableColumn id="54" xr3:uid="{00000000-0010-0000-0100-000036000000}" name="DungeonId" dataDxfId="29"/>
-    <tableColumn id="50" xr3:uid="{00000000-0010-0000-0100-000032000000}" name="CheckQuest" dataDxfId="28"/>
-    <tableColumn id="28" xr3:uid="{00000000-0010-0000-0100-00001C000000}" name="NextQuest" dataDxfId="27"/>
-    <tableColumn id="44" xr3:uid="{00000000-0010-0000-0100-00002C000000}" name="HiddenRoomQuest" dataDxfId="26"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="ShopName" dataDxfId="25"/>
-    <tableColumn id="41" xr3:uid="{00000000-0010-0000-0100-000029000000}" name="MiniGameId" dataDxfId="24"/>
-    <tableColumn id="43" xr3:uid="{00000000-0010-0000-0100-00002B000000}" name="PayKey" dataDxfId="23"/>
-    <tableColumn id="67" xr3:uid="{00000000-0010-0000-0100-000043000000}" name="NeedDungeonItemId" dataDxfId="22"/>
-    <tableColumn id="68" xr3:uid="{00000000-0010-0000-0100-000044000000}" name="NeedDungeonItemCount" dataDxfId="21"/>
-    <tableColumn id="63" xr3:uid="{00000000-0010-0000-0100-00003F000000}" name="TestType1" dataDxfId="20"/>
-    <tableColumn id="64" xr3:uid="{00000000-0010-0000-0100-000040000000}" name="TestBias1" dataDxfId="19"/>
-    <tableColumn id="65" xr3:uid="{00000000-0010-0000-0100-000041000000}" name="TestType2" dataDxfId="18"/>
-    <tableColumn id="66" xr3:uid="{00000000-0010-0000-0100-000042000000}" name="TestBias2" dataDxfId="17"/>
+    <tableColumn id="51" xr3:uid="{00000000-0010-0000-0100-000033000000}" name="CanBribe" dataDxfId="28"/>
+    <tableColumn id="32" xr3:uid="{00000000-0010-0000-0100-000020000000}" name="SceneId" dataDxfId="27"/>
+    <tableColumn id="54" xr3:uid="{00000000-0010-0000-0100-000036000000}" name="DungeonId" dataDxfId="26"/>
+    <tableColumn id="50" xr3:uid="{00000000-0010-0000-0100-000032000000}" name="CheckQuest" dataDxfId="25"/>
+    <tableColumn id="28" xr3:uid="{00000000-0010-0000-0100-00001C000000}" name="NextQuest" dataDxfId="24"/>
+    <tableColumn id="44" xr3:uid="{00000000-0010-0000-0100-00002C000000}" name="HiddenRoomQuest" dataDxfId="23"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="ShopName" dataDxfId="22"/>
+    <tableColumn id="41" xr3:uid="{00000000-0010-0000-0100-000029000000}" name="MiniGameId" dataDxfId="21"/>
+    <tableColumn id="43" xr3:uid="{00000000-0010-0000-0100-00002B000000}" name="PayKey" dataDxfId="20"/>
+    <tableColumn id="67" xr3:uid="{00000000-0010-0000-0100-000043000000}" name="NeedDungeonItemId" dataDxfId="19"/>
+    <tableColumn id="68" xr3:uid="{00000000-0010-0000-0100-000044000000}" name="NeedDungeonItemCount" dataDxfId="18"/>
+    <tableColumn id="63" xr3:uid="{00000000-0010-0000-0100-00003F000000}" name="TestType1" dataDxfId="17"/>
+    <tableColumn id="64" xr3:uid="{00000000-0010-0000-0100-000040000000}" name="TestBias1" dataDxfId="16"/>
+    <tableColumn id="65" xr3:uid="{00000000-0010-0000-0100-000041000000}" name="TestType2" dataDxfId="15"/>
+    <tableColumn id="66" xr3:uid="{00000000-0010-0000-0100-000042000000}" name="TestBias2" dataDxfId="14"/>
     <tableColumn id="9" xr3:uid="{00000000-0010-0000-0100-000009000000}" name="RewardGold"/>
     <tableColumn id="10" xr3:uid="{00000000-0010-0000-0100-00000A000000}" name="RewardFood"/>
     <tableColumn id="11" xr3:uid="{00000000-0010-0000-0100-00000B000000}" name="RewardHealth"/>
     <tableColumn id="12" xr3:uid="{00000000-0010-0000-0100-00000C000000}" name="RewardMental"/>
     <tableColumn id="13" xr3:uid="{00000000-0010-0000-0100-00000D000000}" name="RewardExp"/>
-    <tableColumn id="55" xr3:uid="{00000000-0010-0000-0100-000037000000}" name="RewardStr" dataDxfId="16"/>
-    <tableColumn id="56" xr3:uid="{00000000-0010-0000-0100-000038000000}" name="RewardAgi" dataDxfId="15"/>
-    <tableColumn id="57" xr3:uid="{00000000-0010-0000-0100-000039000000}" name="RewardIntl" dataDxfId="14"/>
-    <tableColumn id="58" xr3:uid="{00000000-0010-0000-0100-00003A000000}" name="RewardPerc" dataDxfId="13"/>
-    <tableColumn id="59" xr3:uid="{00000000-0010-0000-0100-00003B000000}" name="RewardEndu" dataDxfId="12"/>
+    <tableColumn id="55" xr3:uid="{00000000-0010-0000-0100-000037000000}" name="RewardStr" dataDxfId="13"/>
+    <tableColumn id="56" xr3:uid="{00000000-0010-0000-0100-000038000000}" name="RewardAgi" dataDxfId="12"/>
+    <tableColumn id="57" xr3:uid="{00000000-0010-0000-0100-000039000000}" name="RewardIntl" dataDxfId="11"/>
+    <tableColumn id="58" xr3:uid="{00000000-0010-0000-0100-00003A000000}" name="RewardPerc" dataDxfId="10"/>
+    <tableColumn id="59" xr3:uid="{00000000-0010-0000-0100-00003B000000}" name="RewardEndu" dataDxfId="9"/>
     <tableColumn id="14" xr3:uid="{00000000-0010-0000-0100-00000E000000}" name="RewardItem"/>
     <tableColumn id="15" xr3:uid="{00000000-0010-0000-0100-00000F000000}" name="RewardDrop"/>
-    <tableColumn id="73" xr3:uid="{B572E65F-D291-4CBE-9F49-DA1CA2F632F1}" name="RewardCollect" dataDxfId="0"/>
-    <tableColumn id="60" xr3:uid="{00000000-0010-0000-0100-00003C000000}" name="RewardDungeonItemId" dataDxfId="11"/>
-    <tableColumn id="61" xr3:uid="{00000000-0010-0000-0100-00003D000000}" name="RewardDungeonItemCount" dataDxfId="10"/>
+    <tableColumn id="73" xr3:uid="{B572E65F-D291-4CBE-9F49-DA1CA2F632F1}" name="RewardCollectType" dataDxfId="8"/>
+    <tableColumn id="60" xr3:uid="{00000000-0010-0000-0100-00003C000000}" name="RewardDungeonItemId" dataDxfId="7"/>
+    <tableColumn id="61" xr3:uid="{00000000-0010-0000-0100-00003D000000}" name="RewardDungeonItemCount" dataDxfId="6"/>
     <tableColumn id="31" xr3:uid="{00000000-0010-0000-0100-00001F000000}" name="RewardBlessLevel"/>
     <tableColumn id="42" xr3:uid="{00000000-0010-0000-0100-00002A000000}" name="RewardBlessName"/>
-    <tableColumn id="52" xr3:uid="{00000000-0010-0000-0100-000034000000}" name="RewardResId" dataDxfId="9"/>
-    <tableColumn id="53" xr3:uid="{00000000-0010-0000-0100-000035000000}" name="RewardResAmount" dataDxfId="8"/>
+    <tableColumn id="52" xr3:uid="{00000000-0010-0000-0100-000034000000}" name="RewardResId" dataDxfId="5"/>
+    <tableColumn id="53" xr3:uid="{00000000-0010-0000-0100-000035000000}" name="RewardResAmount" dataDxfId="4"/>
     <tableColumn id="26" xr3:uid="{00000000-0010-0000-0100-00001A000000}" name="UnlockRival"/>
     <tableColumn id="16" xr3:uid="{00000000-0010-0000-0100-000010000000}" name="PunishGold"/>
     <tableColumn id="17" xr3:uid="{00000000-0010-0000-0100-000011000000}" name="PunishFood"/>
@@ -5417,10 +5409,10 @@
     <tableColumn id="21" xr3:uid="{00000000-0010-0000-0100-000015000000}" name="TradeFood"/>
     <tableColumn id="22" xr3:uid="{00000000-0010-0000-0100-000016000000}" name="TradeHealth"/>
     <tableColumn id="23" xr3:uid="{00000000-0010-0000-0100-000017000000}" name="TradeMental"/>
-    <tableColumn id="33" xr3:uid="{00000000-0010-0000-0100-000021000000}" name="TradeDropItem" dataDxfId="7"/>
-    <tableColumn id="70" xr3:uid="{00000000-0010-0000-0100-000046000000}" name="DeckCardAttr1" dataDxfId="6"/>
-    <tableColumn id="71" xr3:uid="{00000000-0010-0000-0100-000047000000}" name="DeckCardAttr2" dataDxfId="5"/>
-    <tableColumn id="72" xr3:uid="{00000000-0010-0000-0100-000048000000}" name="DeckCardAttr3" dataDxfId="4"/>
+    <tableColumn id="33" xr3:uid="{00000000-0010-0000-0100-000021000000}" name="TradeDropItem" dataDxfId="3"/>
+    <tableColumn id="70" xr3:uid="{00000000-0010-0000-0100-000046000000}" name="DeckCardAttr1" dataDxfId="2"/>
+    <tableColumn id="71" xr3:uid="{00000000-0010-0000-0100-000047000000}" name="DeckCardAttr2" dataDxfId="1"/>
+    <tableColumn id="72" xr3:uid="{00000000-0010-0000-0100-000048000000}" name="DeckCardAttr3" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5749,9 +5741,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BU113"/>
   <sheetViews>
-    <sheetView topLeftCell="Q1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AV1" sqref="AV1:AV3"/>
+      <selection pane="bottomLeft" activeCell="AV17" sqref="AV17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -6147,7 +6139,7 @@
         <v>56</v>
       </c>
       <c r="AV2" s="89" t="s">
-        <v>705</v>
+        <v>0</v>
       </c>
       <c r="AW2" s="89" t="s">
         <v>572</v>
@@ -6368,7 +6360,7 @@
         <v>659</v>
       </c>
       <c r="AV3" s="80" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="AW3" s="80" t="s">
         <v>660</v>
@@ -7050,8 +7042,8 @@
         <v>100</v>
       </c>
       <c r="AU16" s="24"/>
-      <c r="AV16" s="102" t="s">
-        <v>707</v>
+      <c r="AV16" s="102">
+        <v>2</v>
       </c>
       <c r="AW16" s="24"/>
       <c r="AX16" s="24"/>
@@ -7093,8 +7085,8 @@
       <c r="S17" s="22"/>
       <c r="T17" s="23"/>
       <c r="U17" s="22"/>
-      <c r="AV17" s="102" t="s">
-        <v>707</v>
+      <c r="AV17" s="102">
+        <v>3</v>
       </c>
     </row>
     <row r="18" spans="1:73" x14ac:dyDescent="0.15">
@@ -7133,8 +7125,8 @@
       <c r="R18" s="22"/>
       <c r="S18" s="22"/>
       <c r="U18" s="22"/>
-      <c r="AV18" s="102" t="s">
-        <v>707</v>
+      <c r="AV18" s="102">
+        <v>4</v>
       </c>
       <c r="BF18" s="8">
         <v>50</v>
@@ -7181,8 +7173,8 @@
         <v>150</v>
       </c>
       <c r="AU19" s="23"/>
-      <c r="AV19" s="102" t="s">
-        <v>707</v>
+      <c r="AV19" s="102">
+        <v>5</v>
       </c>
     </row>
     <row r="20" spans="1:73" x14ac:dyDescent="0.15">
@@ -12503,7 +12495,7 @@
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <conditionalFormatting sqref="E4:BU113">
-    <cfRule type="containsBlanks" dxfId="2" priority="17">
+    <cfRule type="containsBlanks" dxfId="74" priority="17">
       <formula>LEN(TRIM(E4))=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -12520,9 +12512,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:BU39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="X1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AV1" sqref="AV1:AV3"/>
+    <sheetView topLeftCell="X1" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AV3" sqref="AV1:AV3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -12914,7 +12906,7 @@
         <v>53</v>
       </c>
       <c r="AV2" s="89" t="s">
-        <v>705</v>
+        <v>0</v>
       </c>
       <c r="AW2" s="89" t="s">
         <v>53</v>
@@ -13135,7 +13127,7 @@
         <v>659</v>
       </c>
       <c r="AV3" s="80" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="AW3" s="80" t="s">
         <v>660</v>
@@ -15142,7 +15134,7 @@
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <conditionalFormatting sqref="E4:BU39">
-    <cfRule type="containsBlanks" dxfId="1" priority="13">
+    <cfRule type="containsBlanks" dxfId="41" priority="13">
       <formula>LEN(TRIM(E4))=0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
fix a dungeon swap bug, and set scenequest repeat time in dungeon
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/SceneQuest.xlsx
+++ b/ConfigData/Xlsx/SceneQuest.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\code\TOMClassicGit\ConfigData\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TOMClassic\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385" activeTab="1"/>
+    <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="4" r:id="rId1"/>
@@ -154,7 +154,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1397" uniqueCount="724">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1386" uniqueCount="721">
   <si>
     <t>int</t>
     <phoneticPr fontId="18" type="noConversion"/>
@@ -2404,15 +2404,211 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>副本中出现一次</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>bool</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>TriggerOnceInDungeon</t>
+    <t>booststr</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>boostagi</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>boostintl</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>boostperc</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>boostendu</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>gemwall</t>
+  </si>
+  <si>
+    <t>水晶墙</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>horsing</t>
+  </si>
+  <si>
+    <t>骑术</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>horsing</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>gemwall</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>trapball</t>
+  </si>
+  <si>
+    <t>铁球陷阱</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>trapbarrier</t>
+  </si>
+  <si>
+    <t>障碍陷阱</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>trapdrop</t>
+  </si>
+  <si>
+    <t>落石陷阱</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>trapelect</t>
+  </si>
+  <si>
+    <t>电击陷阱</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>trapfireball</t>
+  </si>
+  <si>
+    <t>火球陷阱</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>traphotstone</t>
+  </si>
+  <si>
+    <t>熔岩陷阱</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>trappoison</t>
+  </si>
+  <si>
+    <t>沥青陷阱</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>trapslow</t>
+  </si>
+  <si>
+    <t>蛛丝陷阱</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>trapspear</t>
+  </si>
+  <si>
+    <t>地刺陷阱</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>trapspearwall</t>
+  </si>
+  <si>
+    <t>刺墙陷阱</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>trapspring</t>
+  </si>
+  <si>
+    <t>弹簧陷阱</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>trapsteam</t>
+  </si>
+  <si>
+    <t>蒸汽陷阱</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>trapweapon</t>
+  </si>
+  <si>
+    <t>斧刃陷阱</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>主鉴定</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>string</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>TestType1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>主鉴定修正</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>int</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>TestBias1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>副鉴定</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>TestType2</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>TestBias2</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>副鉴定修正</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>intl</t>
+  </si>
+  <si>
+    <t>intl</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>agi</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>trapcommon</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>str</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>agi</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>perc</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>intl</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>endu</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
@@ -2420,520 +2616,312 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>booststr</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>boostagi</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>boostintl</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>boostperc</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>boostendu</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>gemwall</t>
-  </si>
-  <si>
-    <t>水晶墙</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>horsing</t>
-  </si>
-  <si>
-    <t>骑术</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>horsing</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>gemwall</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>trapball</t>
-  </si>
-  <si>
-    <t>铁球陷阱</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>trapbarrier</t>
-  </si>
-  <si>
-    <t>障碍陷阱</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>trapspear</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
     <t>trapdrop</t>
-  </si>
-  <si>
-    <t>落石陷阱</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>trapelect</t>
-  </si>
-  <si>
-    <t>电击陷阱</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>trapfireball</t>
-  </si>
-  <si>
-    <t>火球陷阱</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>traphotstone</t>
-  </si>
-  <si>
-    <t>熔岩陷阱</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>trappoison</t>
-  </si>
-  <si>
-    <t>沥青陷阱</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>trapslow</t>
-  </si>
-  <si>
-    <t>蛛丝陷阱</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>trapspear</t>
-  </si>
-  <si>
-    <t>地刺陷阱</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>NeedDungeonItemId</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>NeedDungeonItemCount</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>需求副本道具</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>需求副本道具数量</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>古玩收集者</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>potteryman</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>RewardDrop</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>RewardDungeonItemId</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>RewardDungeonItemCount</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>RewardBlessName</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>给于的祝福</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>thief</t>
+  </si>
+  <si>
+    <t>thief</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>thief1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>盗贼I</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>thief2</t>
+  </si>
+  <si>
+    <t>盗贼II</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>thief2</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>dlthief</t>
+  </si>
+  <si>
+    <t>thief</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>厚重石门</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>stonedoor2</t>
+  </si>
+  <si>
+    <t>str</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>stonedoor2</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>wildking</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>标签</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>string</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Tag</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>trap</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>DeckCardAttr1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>DeckCardAttr2</t>
+  </si>
+  <si>
+    <t>DeckCardAttr3</t>
+  </si>
+  <si>
+    <t>临时卡关键词1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>临时卡关键词2</t>
+  </si>
+  <si>
+    <t>临时卡关键词3</t>
+  </si>
+  <si>
+    <t>attr.2</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>attr.3</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>attr.4</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>卡牌</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>zookeeper</t>
+  </si>
+  <si>
+    <t>race.11.2</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>race.11.1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>type.1.1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>驯兽师</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>agi</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>迷迭香田</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>rosemaryfield</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>poppyfield</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>森林出口</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>forestexit</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>采集组id</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>RewardCollectType</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>水池</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>矿洞</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>蘑菇</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>枯木</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>草药</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>brushwood</t>
+  </si>
+  <si>
+    <t>brushwood</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>mushroom</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>boss</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>塔力克</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>马道克</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>科力克</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>bosstalic</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>ancienttower</t>
+  </si>
+  <si>
+    <t>ancienttower</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>bossmadawc</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>bosskorlic</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>talic</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>madawc</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>korlic</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>dihunshi</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
     <t>trapspearwall</t>
-  </si>
-  <si>
-    <t>刺墙陷阱</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>trapspring</t>
-  </si>
-  <si>
-    <t>弹簧陷阱</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>trapsteam</t>
-  </si>
-  <si>
-    <t>蒸汽陷阱</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>trapweapon</t>
-  </si>
-  <si>
-    <t>斧刃陷阱</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>主鉴定</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>string</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>TestType1</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>主鉴定修正</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>int</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>TestBias1</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>副鉴定</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>TestType2</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>TestBias2</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>副鉴定修正</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>intl</t>
-  </si>
-  <si>
-    <t>intl</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>agi</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>trapcommon</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>str</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>agi</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>perc</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>intl</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>endu</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>true</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>trapbarrier</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>trapspear</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>trapdrop</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>NeedDungeonItemId</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>NeedDungeonItemCount</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>需求副本道具</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>需求副本道具数量</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>古玩收集者</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>potteryman</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>RewardDrop</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>RewardDungeonItemId</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>RewardDungeonItemCount</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>RewardBlessName</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>给于的祝福</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>thief</t>
-  </si>
-  <si>
-    <t>thief</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>thief1</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>盗贼I</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>thief2</t>
-  </si>
-  <si>
-    <t>盗贼II</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>thief2</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>dlthief</t>
-  </si>
-  <si>
-    <t>thief</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>厚重石门</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>stonedoor2</t>
-  </si>
-  <si>
-    <t>str</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>stonedoor2</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>wildking</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>标签</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>string</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>Tag</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>trap</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>DeckCardAttr1</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>DeckCardAttr2</t>
-  </si>
-  <si>
-    <t>DeckCardAttr3</t>
-  </si>
-  <si>
-    <t>临时卡关键词1</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>临时卡关键词2</t>
-  </si>
-  <si>
-    <t>临时卡关键词3</t>
-  </si>
-  <si>
-    <t>attr.2</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>attr.3</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>attr.4</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>卡牌</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>true</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
     <t>zookeeper</t>
-  </si>
-  <si>
-    <t>race.11.2</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>race.11.1</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>type.1.1</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>驯兽师</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>agi</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>迷迭香田</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>rosemaryfield</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>poppyfield</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>森林出口</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>forestexit</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>采集组id</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>RewardCollectType</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>水池</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>矿洞</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>蘑菇</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>枯木</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>草药</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>brushwood</t>
-  </si>
-  <si>
-    <t>brushwood</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>mushroom</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>boss</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>塔力克</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>马道克</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>科力克</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>bosstalic</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>ancienttower</t>
-  </si>
-  <si>
-    <t>ancienttower</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>bossmadawc</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>bosskorlic</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>talic</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>madawc</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>korlic</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>dihunshi</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>trapspearwall</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>false</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>副本中最大出现次数</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>TriggerLimitInDungeon</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -4173,27 +4161,6 @@
   </cellStyles>
   <dxfs count="79">
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -4865,6 +4832,27 @@
       </fill>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -5377,7 +5365,7 @@
     <tableColumn id="37" name="TriggerQuestReceived" dataDxfId="70"/>
     <tableColumn id="38" name="TriggerQuestFinished" dataDxfId="69"/>
     <tableColumn id="39" name="TriggerRate" dataDxfId="68"/>
-    <tableColumn id="62" name="TriggerOnceInDungeon" dataDxfId="67"/>
+    <tableColumn id="62" name="TriggerLimitInDungeon" dataDxfId="67"/>
     <tableColumn id="7" name="EnemyName"/>
     <tableColumn id="51" name="CanBribe" dataDxfId="66"/>
     <tableColumn id="32" name="SceneId"/>
@@ -5438,7 +5426,7 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="表3_5" displayName="表3_5" ref="A3:BU42" totalsRowShown="0" headerRowDxfId="43">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="表3_5" displayName="表3_5" ref="A3:BU42" totalsRowShown="0" headerRowDxfId="40">
   <autoFilter ref="A3:BU42"/>
   <sortState ref="A4:AU6">
     <sortCondition ref="A3:A6"/>
@@ -5446,58 +5434,58 @@
   <tableColumns count="73">
     <tableColumn id="1" name="Id"/>
     <tableColumn id="2" name="Name"/>
-    <tableColumn id="27" name="Type" dataDxfId="42"/>
+    <tableColumn id="27" name="Type" dataDxfId="39"/>
     <tableColumn id="3" name="Level"/>
     <tableColumn id="25" name="Danger"/>
     <tableColumn id="24" name="Ename"/>
     <tableColumn id="4" name="Figue"/>
     <tableColumn id="5" name="Script"/>
     <tableColumn id="6" name="TriggerMulti"/>
-    <tableColumn id="69" name="Tag" dataDxfId="41"/>
-    <tableColumn id="40" name="Catalog" dataDxfId="40"/>
-    <tableColumn id="29" name="Catalog2" dataDxfId="39"/>
-    <tableColumn id="35" name="TriggerHourBegin" dataDxfId="38"/>
-    <tableColumn id="34" name="TriggerHourEnd" dataDxfId="37"/>
-    <tableColumn id="37" name="TriggerQuestNotReceive" dataDxfId="36"/>
-    <tableColumn id="38" name="TriggerQuestReceived" dataDxfId="35"/>
-    <tableColumn id="36" name="TriggerQuestFinished" dataDxfId="34"/>
-    <tableColumn id="39" name="TriggerRate" dataDxfId="33"/>
-    <tableColumn id="62" name="TriggerOnceInDungeon" dataDxfId="32"/>
+    <tableColumn id="69" name="Tag" dataDxfId="38"/>
+    <tableColumn id="40" name="Catalog" dataDxfId="37"/>
+    <tableColumn id="29" name="Catalog2" dataDxfId="36"/>
+    <tableColumn id="35" name="TriggerHourBegin" dataDxfId="35"/>
+    <tableColumn id="34" name="TriggerHourEnd" dataDxfId="34"/>
+    <tableColumn id="37" name="TriggerQuestNotReceive" dataDxfId="33"/>
+    <tableColumn id="38" name="TriggerQuestReceived" dataDxfId="32"/>
+    <tableColumn id="36" name="TriggerQuestFinished" dataDxfId="31"/>
+    <tableColumn id="39" name="TriggerRate" dataDxfId="30"/>
+    <tableColumn id="62" name="TriggerLimitInDungeon" dataDxfId="29"/>
     <tableColumn id="7" name="EnemyName"/>
-    <tableColumn id="51" name="CanBribe" dataDxfId="31"/>
-    <tableColumn id="32" name="SceneId" dataDxfId="30"/>
-    <tableColumn id="54" name="DungeonId" dataDxfId="29"/>
-    <tableColumn id="50" name="CheckQuest" dataDxfId="28"/>
-    <tableColumn id="28" name="NextQuest" dataDxfId="27"/>
-    <tableColumn id="44" name="HiddenRoomQuest" dataDxfId="26"/>
-    <tableColumn id="8" name="ShopName" dataDxfId="25"/>
-    <tableColumn id="41" name="MiniGameId" dataDxfId="24"/>
-    <tableColumn id="43" name="PayKey" dataDxfId="23"/>
-    <tableColumn id="67" name="NeedDungeonItemId" dataDxfId="22"/>
-    <tableColumn id="68" name="NeedDungeonItemCount" dataDxfId="21"/>
-    <tableColumn id="63" name="TestType1" dataDxfId="20"/>
-    <tableColumn id="64" name="TestBias1" dataDxfId="19"/>
-    <tableColumn id="65" name="TestType2" dataDxfId="18"/>
-    <tableColumn id="66" name="TestBias2" dataDxfId="17"/>
+    <tableColumn id="51" name="CanBribe" dataDxfId="28"/>
+    <tableColumn id="32" name="SceneId" dataDxfId="27"/>
+    <tableColumn id="54" name="DungeonId" dataDxfId="26"/>
+    <tableColumn id="50" name="CheckQuest" dataDxfId="25"/>
+    <tableColumn id="28" name="NextQuest" dataDxfId="24"/>
+    <tableColumn id="44" name="HiddenRoomQuest" dataDxfId="23"/>
+    <tableColumn id="8" name="ShopName" dataDxfId="22"/>
+    <tableColumn id="41" name="MiniGameId" dataDxfId="21"/>
+    <tableColumn id="43" name="PayKey" dataDxfId="20"/>
+    <tableColumn id="67" name="NeedDungeonItemId" dataDxfId="19"/>
+    <tableColumn id="68" name="NeedDungeonItemCount" dataDxfId="18"/>
+    <tableColumn id="63" name="TestType1" dataDxfId="17"/>
+    <tableColumn id="64" name="TestBias1" dataDxfId="16"/>
+    <tableColumn id="65" name="TestType2" dataDxfId="15"/>
+    <tableColumn id="66" name="TestBias2" dataDxfId="14"/>
     <tableColumn id="9" name="RewardGold"/>
     <tableColumn id="10" name="RewardFood"/>
     <tableColumn id="11" name="RewardHealth"/>
     <tableColumn id="12" name="RewardMental"/>
     <tableColumn id="13" name="RewardExp"/>
-    <tableColumn id="55" name="RewardStr" dataDxfId="16"/>
-    <tableColumn id="56" name="RewardAgi" dataDxfId="15"/>
-    <tableColumn id="57" name="RewardIntl" dataDxfId="14"/>
-    <tableColumn id="58" name="RewardPerc" dataDxfId="13"/>
-    <tableColumn id="59" name="RewardEndu" dataDxfId="12"/>
+    <tableColumn id="55" name="RewardStr" dataDxfId="13"/>
+    <tableColumn id="56" name="RewardAgi" dataDxfId="12"/>
+    <tableColumn id="57" name="RewardIntl" dataDxfId="11"/>
+    <tableColumn id="58" name="RewardPerc" dataDxfId="10"/>
+    <tableColumn id="59" name="RewardEndu" dataDxfId="9"/>
     <tableColumn id="14" name="RewardItem"/>
     <tableColumn id="15" name="RewardDrop"/>
-    <tableColumn id="73" name="RewardCollectType" dataDxfId="11"/>
-    <tableColumn id="60" name="RewardDungeonItemId" dataDxfId="10"/>
-    <tableColumn id="61" name="RewardDungeonItemCount" dataDxfId="9"/>
+    <tableColumn id="73" name="RewardCollectType" dataDxfId="8"/>
+    <tableColumn id="60" name="RewardDungeonItemId" dataDxfId="7"/>
+    <tableColumn id="61" name="RewardDungeonItemCount" dataDxfId="6"/>
     <tableColumn id="31" name="RewardBlessLevel"/>
     <tableColumn id="42" name="RewardBlessName"/>
-    <tableColumn id="52" name="RewardResId" dataDxfId="8"/>
-    <tableColumn id="53" name="RewardResAmount" dataDxfId="7"/>
+    <tableColumn id="52" name="RewardResId" dataDxfId="5"/>
+    <tableColumn id="53" name="RewardResAmount" dataDxfId="4"/>
     <tableColumn id="26" name="UnlockRival"/>
     <tableColumn id="16" name="PunishGold"/>
     <tableColumn id="17" name="PunishFood"/>
@@ -5513,10 +5501,10 @@
     <tableColumn id="21" name="TradeFood"/>
     <tableColumn id="22" name="TradeHealth"/>
     <tableColumn id="23" name="TradeMental"/>
-    <tableColumn id="33" name="TradeDropItem" dataDxfId="6"/>
-    <tableColumn id="70" name="DeckCardAttr1" dataDxfId="5"/>
-    <tableColumn id="71" name="DeckCardAttr2" dataDxfId="4"/>
-    <tableColumn id="72" name="DeckCardAttr3" dataDxfId="3"/>
+    <tableColumn id="33" name="TradeDropItem" dataDxfId="3"/>
+    <tableColumn id="70" name="DeckCardAttr1" dataDxfId="2"/>
+    <tableColumn id="71" name="DeckCardAttr2" dataDxfId="1"/>
+    <tableColumn id="72" name="DeckCardAttr3" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5845,9 +5833,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BU114"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A76" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F47" sqref="F47"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A103" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="S114" sqref="S114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -5908,7 +5896,7 @@
         <v>71</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>673</v>
+        <v>669</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>241</v>
@@ -5935,7 +5923,7 @@
         <v>215</v>
       </c>
       <c r="S1" s="2" t="s">
-        <v>584</v>
+        <v>719</v>
       </c>
       <c r="T1" s="3" t="s">
         <v>316</v>
@@ -5968,22 +5956,22 @@
         <v>378</v>
       </c>
       <c r="AD1" s="3" t="s">
-        <v>650</v>
+        <v>646</v>
       </c>
       <c r="AE1" s="3" t="s">
-        <v>651</v>
+        <v>647</v>
       </c>
       <c r="AF1" s="85" t="s">
-        <v>625</v>
+        <v>621</v>
       </c>
       <c r="AG1" s="85" t="s">
-        <v>628</v>
+        <v>624</v>
       </c>
       <c r="AH1" s="85" t="s">
-        <v>631</v>
+        <v>627</v>
       </c>
       <c r="AI1" s="85" t="s">
-        <v>634</v>
+        <v>630</v>
       </c>
       <c r="AJ1" s="4" t="s">
         <v>2</v>
@@ -6022,7 +6010,7 @@
         <v>65</v>
       </c>
       <c r="AV1" s="88" t="s">
-        <v>699</v>
+        <v>694</v>
       </c>
       <c r="AW1" s="88" t="s">
         <v>566</v>
@@ -6034,7 +6022,7 @@
         <v>162</v>
       </c>
       <c r="AZ1" s="4" t="s">
-        <v>658</v>
+        <v>654</v>
       </c>
       <c r="BA1" s="4" t="s">
         <v>514</v>
@@ -6091,13 +6079,13 @@
         <v>357</v>
       </c>
       <c r="BS1" s="96" t="s">
-        <v>680</v>
+        <v>676</v>
       </c>
       <c r="BT1" s="96" t="s">
-        <v>681</v>
+        <v>677</v>
       </c>
       <c r="BU1" s="96" t="s">
-        <v>682</v>
+        <v>678</v>
       </c>
     </row>
     <row r="2" spans="1:73" x14ac:dyDescent="0.15">
@@ -6129,7 +6117,7 @@
         <v>52</v>
       </c>
       <c r="J2" s="9" t="s">
-        <v>674</v>
+        <v>670</v>
       </c>
       <c r="K2" s="9" t="s">
         <v>239</v>
@@ -6156,7 +6144,7 @@
         <v>216</v>
       </c>
       <c r="S2" s="10" t="s">
-        <v>585</v>
+        <v>0</v>
       </c>
       <c r="T2" s="11" t="s">
         <v>50</v>
@@ -6195,16 +6183,16 @@
         <v>0</v>
       </c>
       <c r="AF2" s="86" t="s">
-        <v>626</v>
+        <v>622</v>
       </c>
       <c r="AG2" s="86" t="s">
-        <v>629</v>
+        <v>625</v>
       </c>
       <c r="AH2" s="86" t="s">
-        <v>626</v>
+        <v>622</v>
       </c>
       <c r="AI2" s="86" t="s">
-        <v>629</v>
+        <v>625</v>
       </c>
       <c r="AJ2" s="12" t="s">
         <v>49</v>
@@ -6350,7 +6338,7 @@
         <v>12</v>
       </c>
       <c r="J3" s="80" t="s">
-        <v>675</v>
+        <v>671</v>
       </c>
       <c r="K3" s="16" t="s">
         <v>240</v>
@@ -6377,7 +6365,7 @@
         <v>217</v>
       </c>
       <c r="S3" s="78" t="s">
-        <v>586</v>
+        <v>720</v>
       </c>
       <c r="T3" s="18" t="s">
         <v>315</v>
@@ -6410,22 +6398,22 @@
         <v>380</v>
       </c>
       <c r="AD3" s="18" t="s">
-        <v>648</v>
+        <v>644</v>
       </c>
       <c r="AE3" s="18" t="s">
-        <v>649</v>
+        <v>645</v>
       </c>
       <c r="AF3" s="87" t="s">
-        <v>627</v>
+        <v>623</v>
       </c>
       <c r="AG3" s="87" t="s">
-        <v>630</v>
+        <v>626</v>
       </c>
       <c r="AH3" s="87" t="s">
-        <v>632</v>
+        <v>628</v>
       </c>
       <c r="AI3" s="87" t="s">
-        <v>633</v>
+        <v>629</v>
       </c>
       <c r="AJ3" s="19" t="s">
         <v>59</v>
@@ -6461,22 +6449,22 @@
         <v>9</v>
       </c>
       <c r="AU3" s="80" t="s">
-        <v>654</v>
+        <v>650</v>
       </c>
       <c r="AV3" s="80" t="s">
-        <v>700</v>
+        <v>695</v>
       </c>
       <c r="AW3" s="80" t="s">
-        <v>655</v>
+        <v>651</v>
       </c>
       <c r="AX3" s="80" t="s">
-        <v>656</v>
+        <v>652</v>
       </c>
       <c r="AY3" s="19" t="s">
         <v>160</v>
       </c>
       <c r="AZ3" s="74" t="s">
-        <v>657</v>
+        <v>653</v>
       </c>
       <c r="BA3" s="19" t="s">
         <v>510</v>
@@ -6533,13 +6521,13 @@
         <v>359</v>
       </c>
       <c r="BS3" s="95" t="s">
-        <v>677</v>
+        <v>673</v>
       </c>
       <c r="BT3" s="95" t="s">
-        <v>678</v>
+        <v>674</v>
       </c>
       <c r="BU3" s="95" t="s">
-        <v>679</v>
+        <v>675</v>
       </c>
     </row>
     <row r="4" spans="1:73" x14ac:dyDescent="0.15">
@@ -6602,13 +6590,13 @@
         <v>1</v>
       </c>
       <c r="AF4" s="69" t="s">
-        <v>636</v>
+        <v>632</v>
       </c>
       <c r="AG4" s="24">
         <v>0</v>
       </c>
       <c r="AH4" s="69" t="s">
-        <v>637</v>
+        <v>633</v>
       </c>
       <c r="AI4" s="24">
         <v>-1</v>
@@ -6668,13 +6656,13 @@
         <v>35</v>
       </c>
       <c r="BS4" s="70" t="s">
-        <v>683</v>
+        <v>679</v>
       </c>
       <c r="BT4" s="70" t="s">
-        <v>684</v>
+        <v>680</v>
       </c>
       <c r="BU4" s="70" t="s">
-        <v>685</v>
+        <v>681</v>
       </c>
     </row>
     <row r="5" spans="1:73" x14ac:dyDescent="0.15">
@@ -6994,7 +6982,7 @@
         <v>42000010</v>
       </c>
       <c r="B13" s="71" t="s">
-        <v>705</v>
+        <v>700</v>
       </c>
       <c r="C13" s="8">
         <v>1</v>
@@ -7003,13 +6991,13 @@
         <v>0</v>
       </c>
       <c r="F13" s="70" t="s">
-        <v>707</v>
+        <v>702</v>
       </c>
       <c r="G13" s="70" t="s">
-        <v>706</v>
+        <v>701</v>
       </c>
       <c r="H13" s="70" t="s">
-        <v>707</v>
+        <v>702</v>
       </c>
       <c r="I13" s="22"/>
       <c r="J13" s="67"/>
@@ -7055,7 +7043,7 @@
         <v>42000011</v>
       </c>
       <c r="B14" s="25" t="s">
-        <v>701</v>
+        <v>696</v>
       </c>
       <c r="C14" s="8">
         <v>1</v>
@@ -7102,7 +7090,7 @@
         <v>42000012</v>
       </c>
       <c r="B15" s="25" t="s">
-        <v>702</v>
+        <v>697</v>
       </c>
       <c r="C15" s="8">
         <v>1</v>
@@ -7143,7 +7131,7 @@
         <v>42000013</v>
       </c>
       <c r="B16" s="25" t="s">
-        <v>703</v>
+        <v>698</v>
       </c>
       <c r="C16" s="8">
         <v>1</v>
@@ -7152,7 +7140,7 @@
         <v>0</v>
       </c>
       <c r="F16" s="70" t="s">
-        <v>708</v>
+        <v>703</v>
       </c>
       <c r="G16" s="8" t="s">
         <v>227</v>
@@ -7186,7 +7174,7 @@
         <v>42000014</v>
       </c>
       <c r="B17" s="25" t="s">
-        <v>704</v>
+        <v>699</v>
       </c>
       <c r="C17" s="8">
         <v>1</v>
@@ -7947,7 +7935,7 @@
         <v>42010021</v>
       </c>
       <c r="B33" s="70" t="s">
-        <v>694</v>
+        <v>689</v>
       </c>
       <c r="C33" s="8">
         <v>1</v>
@@ -7956,13 +7944,13 @@
         <v>0</v>
       </c>
       <c r="F33" s="70" t="s">
-        <v>695</v>
+        <v>690</v>
       </c>
       <c r="G33" s="70" t="s">
-        <v>695</v>
+        <v>690</v>
       </c>
       <c r="H33" s="70" t="s">
-        <v>695</v>
+        <v>690</v>
       </c>
       <c r="I33" s="22"/>
       <c r="J33" s="67"/>
@@ -8018,7 +8006,7 @@
         <v>5</v>
       </c>
       <c r="H34" s="70" t="s">
-        <v>696</v>
+        <v>691</v>
       </c>
       <c r="I34" s="22"/>
       <c r="J34" s="22"/>
@@ -9768,7 +9756,7 @@
       <c r="U66" s="22"/>
       <c r="W66" s="70"/>
       <c r="AF66" s="8" t="s">
-        <v>635</v>
+        <v>631</v>
       </c>
       <c r="AG66" s="8">
         <v>0</v>
@@ -9822,7 +9810,7 @@
       <c r="U67" s="22"/>
       <c r="W67" s="70"/>
       <c r="AF67" s="8" t="s">
-        <v>635</v>
+        <v>631</v>
       </c>
       <c r="AG67" s="8">
         <v>1</v>
@@ -9919,7 +9907,7 @@
         <v>42010059</v>
       </c>
       <c r="B69" s="70" t="s">
-        <v>668</v>
+        <v>664</v>
       </c>
       <c r="C69" s="8">
         <v>1</v>
@@ -9928,13 +9916,13 @@
         <v>0</v>
       </c>
       <c r="F69" s="70" t="s">
-        <v>671</v>
+        <v>667</v>
       </c>
       <c r="G69" s="70" t="s">
-        <v>669</v>
+        <v>665</v>
       </c>
       <c r="H69" s="70" t="s">
-        <v>669</v>
+        <v>665</v>
       </c>
       <c r="I69" s="67"/>
       <c r="J69" s="67"/>
@@ -9955,7 +9943,7 @@
       <c r="AD69" s="70"/>
       <c r="AE69" s="70"/>
       <c r="AF69" s="70" t="s">
-        <v>670</v>
+        <v>666</v>
       </c>
       <c r="AG69" s="70">
         <v>2</v>
@@ -11230,7 +11218,7 @@
         <v>42030005</v>
       </c>
       <c r="B93" s="70" t="s">
-        <v>662</v>
+        <v>658</v>
       </c>
       <c r="C93" s="8">
         <v>4</v>
@@ -11242,13 +11230,13 @@
         <v>1</v>
       </c>
       <c r="F93" s="70" t="s">
-        <v>661</v>
+        <v>657</v>
       </c>
       <c r="G93" s="70" t="s">
-        <v>660</v>
+        <v>656</v>
       </c>
       <c r="H93" s="70" t="s">
-        <v>661</v>
+        <v>657</v>
       </c>
       <c r="I93" s="22"/>
       <c r="J93" s="22"/>
@@ -11262,13 +11250,13 @@
       <c r="P93" s="22"/>
       <c r="Q93" s="22"/>
       <c r="R93" s="22"/>
-      <c r="S93" s="67" t="s">
-        <v>13</v>
+      <c r="S93" s="103">
+        <v>1</v>
       </c>
       <c r="U93" s="22"/>
       <c r="W93" s="70"/>
       <c r="Y93" s="8" t="s">
-        <v>663</v>
+        <v>659</v>
       </c>
       <c r="AD93" s="70"/>
       <c r="AE93" s="70"/>
@@ -11294,7 +11282,7 @@
         <v>42030006</v>
       </c>
       <c r="B94" s="70" t="s">
-        <v>664</v>
+        <v>660</v>
       </c>
       <c r="C94" s="8">
         <v>4</v>
@@ -11306,13 +11294,13 @@
         <v>2</v>
       </c>
       <c r="F94" s="70" t="s">
-        <v>665</v>
+        <v>661</v>
       </c>
       <c r="G94" s="8" t="s">
+        <v>655</v>
+      </c>
+      <c r="H94" s="70" t="s">
         <v>659</v>
-      </c>
-      <c r="H94" s="70" t="s">
-        <v>663</v>
       </c>
       <c r="I94" s="22"/>
       <c r="J94" s="22"/>
@@ -11328,12 +11316,12 @@
       <c r="R94" s="22"/>
       <c r="S94" s="67"/>
       <c r="T94" s="70" t="s">
-        <v>667</v>
+        <v>663</v>
       </c>
       <c r="U94" s="22"/>
       <c r="W94" s="70"/>
       <c r="Y94" s="8" t="s">
-        <v>663</v>
+        <v>659</v>
       </c>
       <c r="AD94" s="70"/>
       <c r="AE94" s="70"/>
@@ -11350,7 +11338,7 @@
       <c r="AR94" s="70"/>
       <c r="AS94" s="70"/>
       <c r="AU94" s="8" t="s">
-        <v>666</v>
+        <v>662</v>
       </c>
       <c r="AW94" s="70"/>
       <c r="AX94" s="70"/>
@@ -11380,7 +11368,7 @@
         <v>0</v>
       </c>
       <c r="F95" s="70" t="s">
-        <v>588</v>
+        <v>584</v>
       </c>
       <c r="G95" s="70" t="s">
         <v>580</v>
@@ -11402,8 +11390,8 @@
       <c r="P95" s="22"/>
       <c r="Q95" s="22"/>
       <c r="R95" s="22"/>
-      <c r="S95" s="67" t="s">
-        <v>587</v>
+      <c r="S95" s="103">
+        <v>1</v>
       </c>
       <c r="T95" s="24"/>
       <c r="U95" s="67"/>
@@ -11434,7 +11422,7 @@
         <v>0</v>
       </c>
       <c r="F96" s="70" t="s">
-        <v>589</v>
+        <v>585</v>
       </c>
       <c r="G96" s="70" t="s">
         <v>581</v>
@@ -11456,8 +11444,8 @@
       <c r="P96" s="22"/>
       <c r="Q96" s="22"/>
       <c r="R96" s="22"/>
-      <c r="S96" s="67" t="s">
-        <v>587</v>
+      <c r="S96" s="103">
+        <v>1</v>
       </c>
       <c r="T96" s="23"/>
       <c r="U96" s="67"/>
@@ -11488,7 +11476,7 @@
         <v>0</v>
       </c>
       <c r="F97" s="70" t="s">
-        <v>590</v>
+        <v>586</v>
       </c>
       <c r="G97" s="70" t="s">
         <v>582</v>
@@ -11510,8 +11498,8 @@
       <c r="P97" s="22"/>
       <c r="Q97" s="22"/>
       <c r="R97" s="22"/>
-      <c r="S97" s="67" t="s">
-        <v>587</v>
+      <c r="S97" s="103">
+        <v>1</v>
       </c>
       <c r="T97" s="24"/>
       <c r="U97" s="67"/>
@@ -11533,7 +11521,7 @@
         <v>42040004</v>
       </c>
       <c r="B98" s="92" t="s">
-        <v>594</v>
+        <v>590</v>
       </c>
       <c r="C98" s="8">
         <v>5</v>
@@ -11542,13 +11530,13 @@
         <v>0</v>
       </c>
       <c r="F98" s="70" t="s">
-        <v>591</v>
+        <v>587</v>
       </c>
       <c r="G98" s="70" t="s">
-        <v>598</v>
+        <v>594</v>
       </c>
       <c r="H98" s="70" t="s">
-        <v>593</v>
+        <v>589</v>
       </c>
       <c r="I98" s="67"/>
       <c r="J98" s="67"/>
@@ -11564,8 +11552,8 @@
       <c r="P98" s="22"/>
       <c r="Q98" s="22"/>
       <c r="R98" s="22"/>
-      <c r="S98" s="67" t="s">
-        <v>587</v>
+      <c r="S98" s="103">
+        <v>1</v>
       </c>
       <c r="T98" s="24"/>
       <c r="U98" s="67"/>
@@ -11587,7 +11575,7 @@
         <v>42040005</v>
       </c>
       <c r="B99" s="92" t="s">
-        <v>596</v>
+        <v>592</v>
       </c>
       <c r="C99" s="8">
         <v>5</v>
@@ -11596,13 +11584,13 @@
         <v>0</v>
       </c>
       <c r="F99" s="70" t="s">
-        <v>592</v>
+        <v>588</v>
       </c>
       <c r="G99" s="70" t="s">
-        <v>597</v>
+        <v>593</v>
       </c>
       <c r="H99" s="70" t="s">
-        <v>595</v>
+        <v>591</v>
       </c>
       <c r="I99" s="67"/>
       <c r="J99" s="67"/>
@@ -11618,8 +11606,8 @@
       <c r="P99" s="22"/>
       <c r="Q99" s="22"/>
       <c r="R99" s="22"/>
-      <c r="S99" s="67" t="s">
-        <v>587</v>
+      <c r="S99" s="103">
+        <v>1</v>
       </c>
       <c r="T99" s="23"/>
       <c r="U99" s="67"/>
@@ -11641,7 +11629,7 @@
         <v>42040006</v>
       </c>
       <c r="B100" s="92" t="s">
-        <v>600</v>
+        <v>596</v>
       </c>
       <c r="C100" s="8">
         <v>5</v>
@@ -11653,17 +11641,17 @@
         <v>1</v>
       </c>
       <c r="F100" s="70" t="s">
-        <v>599</v>
+        <v>595</v>
       </c>
       <c r="G100" s="70" t="s">
-        <v>599</v>
+        <v>595</v>
       </c>
       <c r="H100" s="70" t="s">
-        <v>638</v>
+        <v>634</v>
       </c>
       <c r="I100" s="67"/>
       <c r="J100" s="67" t="s">
-        <v>676</v>
+        <v>672</v>
       </c>
       <c r="K100" s="75" t="s">
         <v>547</v>
@@ -11682,7 +11670,7 @@
       <c r="U100" s="67"/>
       <c r="W100" s="70"/>
       <c r="AF100" s="70" t="s">
-        <v>639</v>
+        <v>635</v>
       </c>
       <c r="AG100" s="8">
         <v>1</v>
@@ -11705,7 +11693,7 @@
         <v>42040007</v>
       </c>
       <c r="B101" s="92" t="s">
-        <v>602</v>
+        <v>598</v>
       </c>
       <c r="C101" s="8">
         <v>5</v>
@@ -11717,19 +11705,19 @@
         <v>1</v>
       </c>
       <c r="F101" s="70" t="s">
-        <v>601</v>
+        <v>597</v>
       </c>
       <c r="G101" s="70" t="s">
-        <v>601</v>
+        <v>597</v>
       </c>
       <c r="H101" s="70" t="s">
-        <v>645</v>
+        <v>641</v>
       </c>
       <c r="I101" s="67" t="s">
-        <v>644</v>
+        <v>640</v>
       </c>
       <c r="J101" s="67" t="s">
-        <v>676</v>
+        <v>672</v>
       </c>
       <c r="K101" s="75" t="s">
         <v>547</v>
@@ -11765,7 +11753,7 @@
         <v>42040008</v>
       </c>
       <c r="B102" s="92" t="s">
-        <v>604</v>
+        <v>600</v>
       </c>
       <c r="C102" s="8">
         <v>5</v>
@@ -11777,17 +11765,17 @@
         <v>2</v>
       </c>
       <c r="F102" s="70" t="s">
-        <v>647</v>
+        <v>643</v>
       </c>
       <c r="G102" s="70" t="s">
-        <v>603</v>
+        <v>599</v>
       </c>
       <c r="H102" s="70" t="s">
-        <v>638</v>
+        <v>634</v>
       </c>
       <c r="I102" s="67"/>
       <c r="J102" s="67" t="s">
-        <v>676</v>
+        <v>672</v>
       </c>
       <c r="K102" s="75" t="s">
         <v>547</v>
@@ -11806,13 +11794,13 @@
       <c r="U102" s="67"/>
       <c r="W102" s="70"/>
       <c r="AF102" s="70" t="s">
-        <v>640</v>
+        <v>636</v>
       </c>
       <c r="AG102" s="8">
         <v>2</v>
       </c>
       <c r="AH102" s="70" t="s">
-        <v>641</v>
+        <v>637</v>
       </c>
       <c r="AI102" s="8">
         <v>0</v>
@@ -11835,7 +11823,7 @@
         <v>42040009</v>
       </c>
       <c r="B103" s="92" t="s">
-        <v>606</v>
+        <v>602</v>
       </c>
       <c r="C103" s="8">
         <v>5</v>
@@ -11847,17 +11835,17 @@
         <v>1</v>
       </c>
       <c r="F103" s="70" t="s">
-        <v>605</v>
+        <v>601</v>
       </c>
       <c r="G103" s="70" t="s">
-        <v>605</v>
+        <v>601</v>
       </c>
       <c r="H103" s="70" t="s">
-        <v>638</v>
+        <v>634</v>
       </c>
       <c r="I103" s="67"/>
       <c r="J103" s="67" t="s">
-        <v>676</v>
+        <v>672</v>
       </c>
       <c r="K103" s="75" t="s">
         <v>547</v>
@@ -11876,7 +11864,7 @@
       <c r="U103" s="67"/>
       <c r="W103" s="70"/>
       <c r="AF103" s="70" t="s">
-        <v>642</v>
+        <v>638</v>
       </c>
       <c r="AG103" s="8">
         <v>1</v>
@@ -11902,7 +11890,7 @@
         <v>42040010</v>
       </c>
       <c r="B104" s="92" t="s">
-        <v>608</v>
+        <v>604</v>
       </c>
       <c r="C104" s="8">
         <v>5</v>
@@ -11914,17 +11902,17 @@
         <v>1</v>
       </c>
       <c r="F104" s="70" t="s">
-        <v>607</v>
+        <v>603</v>
       </c>
       <c r="G104" s="70" t="s">
-        <v>607</v>
+        <v>603</v>
       </c>
       <c r="H104" s="70" t="s">
-        <v>638</v>
+        <v>634</v>
       </c>
       <c r="I104" s="67"/>
       <c r="J104" s="67" t="s">
-        <v>676</v>
+        <v>672</v>
       </c>
       <c r="K104" s="75" t="s">
         <v>547</v>
@@ -11943,7 +11931,7 @@
       <c r="U104" s="67"/>
       <c r="W104" s="70"/>
       <c r="AF104" s="70" t="s">
-        <v>640</v>
+        <v>636</v>
       </c>
       <c r="AG104" s="8">
         <v>1</v>
@@ -11966,7 +11954,7 @@
         <v>42040011</v>
       </c>
       <c r="B105" s="92" t="s">
-        <v>610</v>
+        <v>606</v>
       </c>
       <c r="C105" s="8">
         <v>5</v>
@@ -11978,19 +11966,19 @@
         <v>2</v>
       </c>
       <c r="F105" s="70" t="s">
-        <v>609</v>
+        <v>605</v>
       </c>
       <c r="G105" s="70" t="s">
-        <v>609</v>
+        <v>605</v>
       </c>
       <c r="H105" s="70" t="s">
-        <v>638</v>
+        <v>634</v>
       </c>
       <c r="I105" s="67" t="s">
-        <v>644</v>
+        <v>640</v>
       </c>
       <c r="J105" s="67" t="s">
-        <v>676</v>
+        <v>672</v>
       </c>
       <c r="K105" s="75" t="s">
         <v>547</v>
@@ -12009,13 +11997,13 @@
       <c r="U105" s="67"/>
       <c r="W105" s="70"/>
       <c r="AF105" s="70" t="s">
-        <v>639</v>
+        <v>635</v>
       </c>
       <c r="AG105" s="8">
         <v>2</v>
       </c>
       <c r="AH105" s="70" t="s">
-        <v>643</v>
+        <v>639</v>
       </c>
       <c r="AI105" s="8">
         <v>0</v>
@@ -12038,7 +12026,7 @@
         <v>42040012</v>
       </c>
       <c r="B106" s="92" t="s">
-        <v>612</v>
+        <v>608</v>
       </c>
       <c r="C106" s="8">
         <v>5</v>
@@ -12050,19 +12038,19 @@
         <v>1</v>
       </c>
       <c r="F106" s="70" t="s">
-        <v>611</v>
+        <v>607</v>
       </c>
       <c r="G106" s="70" t="s">
-        <v>611</v>
+        <v>607</v>
       </c>
       <c r="H106" s="70" t="s">
-        <v>638</v>
+        <v>634</v>
       </c>
       <c r="I106" s="67" t="s">
-        <v>644</v>
+        <v>640</v>
       </c>
       <c r="J106" s="67" t="s">
-        <v>676</v>
+        <v>672</v>
       </c>
       <c r="K106" s="75" t="s">
         <v>547</v>
@@ -12081,13 +12069,13 @@
       <c r="U106" s="67"/>
       <c r="W106" s="70"/>
       <c r="AF106" s="70" t="s">
-        <v>640</v>
+        <v>636</v>
       </c>
       <c r="AG106" s="8">
         <v>0</v>
       </c>
       <c r="AH106" s="70" t="s">
-        <v>642</v>
+        <v>638</v>
       </c>
       <c r="AI106" s="8">
         <v>0</v>
@@ -12113,7 +12101,7 @@
         <v>42040013</v>
       </c>
       <c r="B107" s="92" t="s">
-        <v>614</v>
+        <v>610</v>
       </c>
       <c r="C107" s="8">
         <v>5</v>
@@ -12125,17 +12113,17 @@
         <v>1</v>
       </c>
       <c r="F107" s="70" t="s">
-        <v>613</v>
+        <v>609</v>
       </c>
       <c r="G107" s="70" t="s">
-        <v>613</v>
+        <v>609</v>
       </c>
       <c r="H107" s="70" t="s">
-        <v>638</v>
+        <v>634</v>
       </c>
       <c r="I107" s="67"/>
       <c r="J107" s="67" t="s">
-        <v>676</v>
+        <v>672</v>
       </c>
       <c r="K107" s="75" t="s">
         <v>547</v>
@@ -12154,13 +12142,13 @@
       <c r="U107" s="67"/>
       <c r="W107" s="70"/>
       <c r="AF107" s="70" t="s">
-        <v>639</v>
+        <v>635</v>
       </c>
       <c r="AG107" s="8">
         <v>0</v>
       </c>
       <c r="AH107" s="70" t="s">
-        <v>641</v>
+        <v>637</v>
       </c>
       <c r="AI107" s="8">
         <v>1</v>
@@ -12183,7 +12171,7 @@
         <v>42040014</v>
       </c>
       <c r="B108" s="92" t="s">
-        <v>616</v>
+        <v>612</v>
       </c>
       <c r="C108" s="8">
         <v>5</v>
@@ -12195,19 +12183,19 @@
         <v>1</v>
       </c>
       <c r="F108" s="70" t="s">
-        <v>646</v>
+        <v>642</v>
       </c>
       <c r="G108" s="70" t="s">
-        <v>615</v>
+        <v>611</v>
       </c>
       <c r="H108" s="70" t="s">
-        <v>638</v>
+        <v>634</v>
       </c>
       <c r="I108" s="67" t="s">
-        <v>644</v>
+        <v>640</v>
       </c>
       <c r="J108" s="67" t="s">
-        <v>676</v>
+        <v>672</v>
       </c>
       <c r="K108" s="75" t="s">
         <v>547</v>
@@ -12226,7 +12214,7 @@
       <c r="U108" s="67"/>
       <c r="W108" s="70"/>
       <c r="AF108" s="70" t="s">
-        <v>640</v>
+        <v>636</v>
       </c>
       <c r="AG108" s="8">
         <v>1</v>
@@ -12249,7 +12237,7 @@
         <v>42040015</v>
       </c>
       <c r="B109" s="92" t="s">
-        <v>618</v>
+        <v>614</v>
       </c>
       <c r="C109" s="8">
         <v>5</v>
@@ -12261,19 +12249,19 @@
         <v>2</v>
       </c>
       <c r="F109" s="70" t="s">
-        <v>722</v>
+        <v>717</v>
       </c>
       <c r="G109" s="70" t="s">
-        <v>617</v>
+        <v>613</v>
       </c>
       <c r="H109" s="70" t="s">
-        <v>601</v>
+        <v>597</v>
       </c>
       <c r="I109" s="67" t="s">
-        <v>644</v>
+        <v>640</v>
       </c>
       <c r="J109" s="67" t="s">
-        <v>676</v>
+        <v>672</v>
       </c>
       <c r="K109" s="75" t="s">
         <v>547</v>
@@ -12292,13 +12280,13 @@
       <c r="U109" s="67"/>
       <c r="W109" s="70"/>
       <c r="AF109" s="70" t="s">
-        <v>640</v>
+        <v>636</v>
       </c>
       <c r="AG109" s="8">
         <v>2</v>
       </c>
       <c r="AH109" s="70" t="s">
-        <v>643</v>
+        <v>639</v>
       </c>
       <c r="AI109" s="8">
         <v>2</v>
@@ -12321,7 +12309,7 @@
         <v>42040016</v>
       </c>
       <c r="B110" s="92" t="s">
-        <v>620</v>
+        <v>616</v>
       </c>
       <c r="C110" s="8">
         <v>5</v>
@@ -12333,17 +12321,17 @@
         <v>1</v>
       </c>
       <c r="F110" s="70" t="s">
-        <v>619</v>
+        <v>615</v>
       </c>
       <c r="G110" s="70" t="s">
-        <v>619</v>
+        <v>615</v>
       </c>
       <c r="H110" s="70" t="s">
-        <v>619</v>
+        <v>615</v>
       </c>
       <c r="I110" s="67"/>
       <c r="J110" s="67" t="s">
-        <v>676</v>
+        <v>672</v>
       </c>
       <c r="K110" s="75" t="s">
         <v>547</v>
@@ -12362,13 +12350,13 @@
       <c r="U110" s="67"/>
       <c r="W110" s="70"/>
       <c r="AF110" s="70" t="s">
-        <v>640</v>
+        <v>636</v>
       </c>
       <c r="AG110" s="8">
         <v>3</v>
       </c>
       <c r="AH110" s="70" t="s">
-        <v>641</v>
+        <v>637</v>
       </c>
       <c r="AI110" s="8">
         <v>2</v>
@@ -12396,7 +12384,7 @@
         <v>42040017</v>
       </c>
       <c r="B111" s="92" t="s">
-        <v>622</v>
+        <v>618</v>
       </c>
       <c r="C111" s="8">
         <v>5</v>
@@ -12408,19 +12396,19 @@
         <v>1</v>
       </c>
       <c r="F111" s="70" t="s">
-        <v>621</v>
+        <v>617</v>
       </c>
       <c r="G111" s="70" t="s">
-        <v>621</v>
+        <v>617</v>
       </c>
       <c r="H111" s="70" t="s">
-        <v>638</v>
+        <v>634</v>
       </c>
       <c r="I111" s="67" t="s">
-        <v>644</v>
+        <v>640</v>
       </c>
       <c r="J111" s="67" t="s">
-        <v>676</v>
+        <v>672</v>
       </c>
       <c r="K111" s="75" t="s">
         <v>547</v>
@@ -12439,7 +12427,7 @@
       <c r="U111" s="67"/>
       <c r="W111" s="70"/>
       <c r="AF111" s="70" t="s">
-        <v>641</v>
+        <v>637</v>
       </c>
       <c r="AG111" s="8">
         <v>3</v>
@@ -12464,7 +12452,7 @@
         <v>42040018</v>
       </c>
       <c r="B112" s="92" t="s">
-        <v>624</v>
+        <v>620</v>
       </c>
       <c r="C112" s="8">
         <v>5</v>
@@ -12476,19 +12464,19 @@
         <v>2</v>
       </c>
       <c r="F112" s="70" t="s">
-        <v>623</v>
+        <v>619</v>
       </c>
       <c r="G112" s="70" t="s">
-        <v>623</v>
+        <v>619</v>
       </c>
       <c r="H112" s="70" t="s">
-        <v>638</v>
+        <v>634</v>
       </c>
       <c r="I112" s="67" t="s">
-        <v>644</v>
+        <v>640</v>
       </c>
       <c r="J112" s="67" t="s">
-        <v>676</v>
+        <v>672</v>
       </c>
       <c r="K112" s="75" t="s">
         <v>547</v>
@@ -12507,13 +12495,13 @@
       <c r="U112" s="67"/>
       <c r="W112" s="70"/>
       <c r="AF112" s="70" t="s">
-        <v>639</v>
+        <v>635</v>
       </c>
       <c r="AG112" s="8">
         <v>1</v>
       </c>
       <c r="AH112" s="70" t="s">
-        <v>637</v>
+        <v>633</v>
       </c>
       <c r="AI112" s="8">
         <v>1</v>
@@ -12536,7 +12524,7 @@
         <v>42040019</v>
       </c>
       <c r="B113" s="92" t="s">
-        <v>652</v>
+        <v>648</v>
       </c>
       <c r="C113" s="8">
         <v>5</v>
@@ -12545,13 +12533,13 @@
         <v>0</v>
       </c>
       <c r="F113" s="70" t="s">
-        <v>653</v>
+        <v>649</v>
       </c>
       <c r="G113" s="70" t="s">
-        <v>653</v>
+        <v>649</v>
       </c>
       <c r="H113" s="70" t="s">
-        <v>653</v>
+        <v>649</v>
       </c>
       <c r="I113" s="67"/>
       <c r="J113" s="67"/>
@@ -12602,7 +12590,7 @@
         <v>42040020</v>
       </c>
       <c r="B114" s="92" t="s">
-        <v>692</v>
+        <v>687</v>
       </c>
       <c r="C114" s="8">
         <v>5</v>
@@ -12611,18 +12599,18 @@
         <v>0</v>
       </c>
       <c r="F114" s="8" t="s">
-        <v>688</v>
+        <v>683</v>
       </c>
       <c r="G114" s="8" t="s">
-        <v>688</v>
-      </c>
-      <c r="H114" s="8" t="s">
-        <v>688</v>
+        <v>683</v>
+      </c>
+      <c r="H114" s="70" t="s">
+        <v>718</v>
       </c>
       <c r="I114" s="22"/>
       <c r="J114" s="67"/>
       <c r="K114" s="99" t="s">
-        <v>686</v>
+        <v>682</v>
       </c>
       <c r="L114" s="84" t="s">
         <v>583</v>
@@ -12633,8 +12621,8 @@
       <c r="P114" s="22"/>
       <c r="Q114" s="22"/>
       <c r="R114" s="22"/>
-      <c r="S114" s="67" t="s">
-        <v>687</v>
+      <c r="S114" s="103">
+        <v>1</v>
       </c>
       <c r="U114" s="22"/>
       <c r="W114" s="70"/>
@@ -12654,13 +12642,13 @@
       <c r="BA114" s="70"/>
       <c r="BB114" s="70"/>
       <c r="BS114" s="70" t="s">
-        <v>690</v>
+        <v>685</v>
       </c>
       <c r="BT114" s="70" t="s">
-        <v>689</v>
+        <v>684</v>
       </c>
       <c r="BU114" s="70" t="s">
-        <v>691</v>
+        <v>686</v>
       </c>
     </row>
   </sheetData>
@@ -12683,9 +12671,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BU42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="S39" sqref="S39:S41"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A34" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="S37" sqref="S37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -12742,7 +12730,7 @@
         <v>71</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>673</v>
+        <v>669</v>
       </c>
       <c r="K1" s="37" t="s">
         <v>241</v>
@@ -12769,7 +12757,7 @@
         <v>215</v>
       </c>
       <c r="S1" s="2" t="s">
-        <v>584</v>
+        <v>719</v>
       </c>
       <c r="T1" s="39" t="s">
         <v>316</v>
@@ -12802,22 +12790,22 @@
         <v>378</v>
       </c>
       <c r="AD1" s="3" t="s">
-        <v>650</v>
+        <v>646</v>
       </c>
       <c r="AE1" s="3" t="s">
-        <v>651</v>
+        <v>647</v>
       </c>
       <c r="AF1" s="85" t="s">
-        <v>625</v>
+        <v>621</v>
       </c>
       <c r="AG1" s="85" t="s">
-        <v>628</v>
+        <v>624</v>
       </c>
       <c r="AH1" s="85" t="s">
-        <v>631</v>
+        <v>627</v>
       </c>
       <c r="AI1" s="85" t="s">
-        <v>634</v>
+        <v>630</v>
       </c>
       <c r="AJ1" s="40" t="s">
         <v>2</v>
@@ -12856,7 +12844,7 @@
         <v>65</v>
       </c>
       <c r="AV1" s="88" t="s">
-        <v>699</v>
+        <v>694</v>
       </c>
       <c r="AW1" s="88" t="s">
         <v>566</v>
@@ -12868,7 +12856,7 @@
         <v>162</v>
       </c>
       <c r="AZ1" s="4" t="s">
-        <v>658</v>
+        <v>654</v>
       </c>
       <c r="BA1" s="40" t="s">
         <v>519</v>
@@ -12925,13 +12913,13 @@
         <v>357</v>
       </c>
       <c r="BS1" s="96" t="s">
-        <v>680</v>
+        <v>676</v>
       </c>
       <c r="BT1" s="96" t="s">
-        <v>681</v>
+        <v>677</v>
       </c>
       <c r="BU1" s="96" t="s">
-        <v>682</v>
+        <v>678</v>
       </c>
     </row>
     <row r="2" spans="1:73" x14ac:dyDescent="0.15">
@@ -12963,7 +12951,7 @@
         <v>52</v>
       </c>
       <c r="J2" s="9" t="s">
-        <v>674</v>
+        <v>670</v>
       </c>
       <c r="K2" s="45" t="s">
         <v>239</v>
@@ -12990,7 +12978,7 @@
         <v>216</v>
       </c>
       <c r="S2" s="10" t="s">
-        <v>585</v>
+        <v>0</v>
       </c>
       <c r="T2" s="47" t="s">
         <v>50</v>
@@ -13029,16 +13017,16 @@
         <v>0</v>
       </c>
       <c r="AF2" s="86" t="s">
-        <v>626</v>
+        <v>622</v>
       </c>
       <c r="AG2" s="86" t="s">
-        <v>629</v>
+        <v>625</v>
       </c>
       <c r="AH2" s="86" t="s">
-        <v>626</v>
+        <v>622</v>
       </c>
       <c r="AI2" s="86" t="s">
-        <v>629</v>
+        <v>625</v>
       </c>
       <c r="AJ2" s="48" t="s">
         <v>49</v>
@@ -13184,7 +13172,7 @@
         <v>12</v>
       </c>
       <c r="J3" s="80" t="s">
-        <v>675</v>
+        <v>671</v>
       </c>
       <c r="K3" s="52" t="s">
         <v>240</v>
@@ -13211,7 +13199,7 @@
         <v>217</v>
       </c>
       <c r="S3" s="78" t="s">
-        <v>586</v>
+        <v>720</v>
       </c>
       <c r="T3" s="54" t="s">
         <v>315</v>
@@ -13244,22 +13232,22 @@
         <v>380</v>
       </c>
       <c r="AD3" s="18" t="s">
-        <v>648</v>
+        <v>644</v>
       </c>
       <c r="AE3" s="18" t="s">
-        <v>649</v>
+        <v>645</v>
       </c>
       <c r="AF3" s="87" t="s">
-        <v>627</v>
+        <v>623</v>
       </c>
       <c r="AG3" s="87" t="s">
-        <v>630</v>
+        <v>626</v>
       </c>
       <c r="AH3" s="87" t="s">
-        <v>632</v>
+        <v>628</v>
       </c>
       <c r="AI3" s="87" t="s">
-        <v>633</v>
+        <v>629</v>
       </c>
       <c r="AJ3" s="55" t="s">
         <v>59</v>
@@ -13295,22 +13283,22 @@
         <v>9</v>
       </c>
       <c r="AU3" s="80" t="s">
-        <v>654</v>
+        <v>650</v>
       </c>
       <c r="AV3" s="80" t="s">
-        <v>700</v>
+        <v>695</v>
       </c>
       <c r="AW3" s="80" t="s">
-        <v>655</v>
+        <v>651</v>
       </c>
       <c r="AX3" s="80" t="s">
-        <v>656</v>
+        <v>652</v>
       </c>
       <c r="AY3" s="19" t="s">
         <v>160</v>
       </c>
       <c r="AZ3" s="74" t="s">
-        <v>657</v>
+        <v>653</v>
       </c>
       <c r="BA3" s="55" t="s">
         <v>510</v>
@@ -13367,13 +13355,13 @@
         <v>359</v>
       </c>
       <c r="BS3" s="95" t="s">
-        <v>677</v>
+        <v>673</v>
       </c>
       <c r="BT3" s="95" t="s">
-        <v>678</v>
+        <v>674</v>
       </c>
       <c r="BU3" s="95" t="s">
-        <v>679</v>
+        <v>675</v>
       </c>
     </row>
     <row r="4" spans="1:73" x14ac:dyDescent="0.15">
@@ -14915,7 +14903,7 @@
       </c>
       <c r="I33" s="59"/>
       <c r="J33" s="67" t="s">
-        <v>709</v>
+        <v>704</v>
       </c>
       <c r="K33" s="59"/>
       <c r="L33" s="59"/>
@@ -14980,7 +14968,7 @@
       </c>
       <c r="I34" s="59"/>
       <c r="J34" s="67" t="s">
-        <v>709</v>
+        <v>704</v>
       </c>
       <c r="K34" s="59"/>
       <c r="L34" s="59"/>
@@ -15006,7 +14994,7 @@
       <c r="AD34" s="69"/>
       <c r="AE34" s="69"/>
       <c r="AF34" s="69" t="s">
-        <v>693</v>
+        <v>688</v>
       </c>
       <c r="AG34" s="69">
         <v>2</v>
@@ -15035,7 +15023,7 @@
         <v>42130006</v>
       </c>
       <c r="B35" s="98" t="s">
-        <v>697</v>
+        <v>692</v>
       </c>
       <c r="C35" s="58">
         <v>2</v>
@@ -15044,13 +15032,13 @@
         <v>0</v>
       </c>
       <c r="F35" s="70" t="s">
-        <v>698</v>
+        <v>693</v>
       </c>
       <c r="G35" s="70" t="s">
-        <v>698</v>
+        <v>693</v>
       </c>
       <c r="H35" s="70" t="s">
-        <v>698</v>
+        <v>693</v>
       </c>
       <c r="I35" s="59"/>
       <c r="J35" s="67"/>
@@ -15226,7 +15214,7 @@
       </c>
       <c r="I38" s="59"/>
       <c r="J38" s="67" t="s">
-        <v>709</v>
+        <v>704</v>
       </c>
       <c r="K38" s="59"/>
       <c r="L38" s="59"/>
@@ -15236,11 +15224,11 @@
       <c r="P38" s="59"/>
       <c r="Q38" s="59"/>
       <c r="R38" s="59"/>
-      <c r="S38" s="67" t="s">
-        <v>13</v>
+      <c r="S38" s="103">
+        <v>1</v>
       </c>
       <c r="T38" s="93" t="s">
-        <v>672</v>
+        <v>668</v>
       </c>
       <c r="U38" s="59"/>
       <c r="V38" s="62"/>
@@ -15272,7 +15260,7 @@
         <v>42130023</v>
       </c>
       <c r="B39" s="98" t="s">
-        <v>710</v>
+        <v>705</v>
       </c>
       <c r="C39" s="58">
         <v>2</v>
@@ -15281,19 +15269,19 @@
         <v>0</v>
       </c>
       <c r="F39" s="70" t="s">
-        <v>713</v>
+        <v>708</v>
       </c>
       <c r="G39" s="70" t="s">
-        <v>715</v>
+        <v>710</v>
       </c>
       <c r="H39" s="70" t="s">
-        <v>715</v>
+        <v>710</v>
       </c>
       <c r="I39" s="59" t="s">
         <v>13</v>
       </c>
       <c r="J39" s="67" t="s">
-        <v>709</v>
+        <v>704</v>
       </c>
       <c r="K39" s="59"/>
       <c r="L39" s="67"/>
@@ -15303,11 +15291,9 @@
       <c r="P39" s="59"/>
       <c r="Q39" s="59"/>
       <c r="R39" s="59"/>
-      <c r="S39" s="67" t="s">
-        <v>723</v>
-      </c>
+      <c r="S39" s="67"/>
       <c r="T39" s="70" t="s">
-        <v>718</v>
+        <v>713</v>
       </c>
       <c r="U39" s="67"/>
       <c r="V39" s="68"/>
@@ -15337,7 +15323,7 @@
       <c r="AS39" s="70"/>
       <c r="AV39" s="70"/>
       <c r="AW39" s="78" t="s">
-        <v>721</v>
+        <v>716</v>
       </c>
       <c r="AX39" s="8">
         <v>1</v>
@@ -15354,7 +15340,7 @@
         <v>42130024</v>
       </c>
       <c r="B40" s="98" t="s">
-        <v>711</v>
+        <v>706</v>
       </c>
       <c r="C40" s="58">
         <v>2</v>
@@ -15363,19 +15349,19 @@
         <v>0</v>
       </c>
       <c r="F40" s="70" t="s">
-        <v>716</v>
+        <v>711</v>
       </c>
       <c r="G40" s="70" t="s">
-        <v>714</v>
+        <v>709</v>
       </c>
       <c r="H40" s="70" t="s">
-        <v>715</v>
+        <v>710</v>
       </c>
       <c r="I40" s="59" t="s">
         <v>13</v>
       </c>
       <c r="J40" s="67" t="s">
-        <v>709</v>
+        <v>704</v>
       </c>
       <c r="K40" s="59"/>
       <c r="L40" s="67"/>
@@ -15385,11 +15371,9 @@
       <c r="P40" s="59"/>
       <c r="Q40" s="59"/>
       <c r="R40" s="59"/>
-      <c r="S40" s="67" t="s">
-        <v>723</v>
-      </c>
+      <c r="S40" s="67"/>
       <c r="T40" s="70" t="s">
-        <v>719</v>
+        <v>714</v>
       </c>
       <c r="U40" s="67"/>
       <c r="V40" s="68"/>
@@ -15419,7 +15403,7 @@
       <c r="AS40" s="70"/>
       <c r="AV40" s="70"/>
       <c r="AW40" s="78" t="s">
-        <v>721</v>
+        <v>716</v>
       </c>
       <c r="AX40" s="8">
         <v>1</v>
@@ -15436,7 +15420,7 @@
         <v>42130025</v>
       </c>
       <c r="B41" s="98" t="s">
-        <v>712</v>
+        <v>707</v>
       </c>
       <c r="C41" s="58">
         <v>2</v>
@@ -15445,19 +15429,19 @@
         <v>0</v>
       </c>
       <c r="F41" s="70" t="s">
-        <v>717</v>
+        <v>712</v>
       </c>
       <c r="G41" s="70" t="s">
-        <v>714</v>
+        <v>709</v>
       </c>
       <c r="H41" s="70" t="s">
-        <v>715</v>
+        <v>710</v>
       </c>
       <c r="I41" s="59" t="s">
         <v>13</v>
       </c>
       <c r="J41" s="67" t="s">
-        <v>709</v>
+        <v>704</v>
       </c>
       <c r="K41" s="59"/>
       <c r="L41" s="67"/>
@@ -15467,11 +15451,9 @@
       <c r="P41" s="59"/>
       <c r="Q41" s="59"/>
       <c r="R41" s="59"/>
-      <c r="S41" s="67" t="s">
-        <v>723</v>
-      </c>
+      <c r="S41" s="67"/>
       <c r="T41" s="70" t="s">
-        <v>720</v>
+        <v>715</v>
       </c>
       <c r="U41" s="67"/>
       <c r="V41" s="68"/>
@@ -15501,7 +15483,7 @@
       <c r="AS41" s="70"/>
       <c r="AV41" s="70"/>
       <c r="AW41" s="78" t="s">
-        <v>721</v>
+        <v>716</v>
       </c>
       <c r="AX41" s="8">
         <v>1</v>
@@ -15567,17 +15549,17 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AW41:AX41">
-    <cfRule type="containsBlanks" dxfId="2" priority="3">
+    <cfRule type="containsBlanks" dxfId="43" priority="3">
       <formula>LEN(TRIM(AW41))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AW40:AX40">
-    <cfRule type="containsBlanks" dxfId="1" priority="2">
+    <cfRule type="containsBlanks" dxfId="42" priority="2">
       <formula>LEN(TRIM(AW40))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AW39:AX39">
-    <cfRule type="containsBlanks" dxfId="0" priority="1">
+    <cfRule type="containsBlanks" dxfId="41" priority="1">
       <formula>LEN(TRIM(AW39))=0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
finish the dna showing effect
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/SceneQuest.xlsx
+++ b/ConfigData/Xlsx/SceneQuest.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19029"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Code\TOMClassicGit\ConfigData\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TOMClassic\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -154,7 +154,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1458" uniqueCount="749">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1460" uniqueCount="751">
   <si>
     <t>int</t>
     <phoneticPr fontId="18" type="noConversion"/>
@@ -3035,6 +3035,14 @@
   </si>
   <si>
     <t>TriggerDNAHard</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>kil;3</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>kil;1;kin;1;wat;1</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -5578,72 +5586,6 @@
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
     <mruColors>
       <color rgb="FFADADDD"/>
       <color rgb="FFD9A7A7"/>
@@ -5853,7 +5795,7 @@
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="C7EDCC"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -6170,7 +6112,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="U1" sqref="U1:V3"/>
+      <selection pane="bottomLeft" activeCell="V4" sqref="V4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -6935,8 +6877,12 @@
       <c r="R4" s="22"/>
       <c r="S4" s="103"/>
       <c r="T4" s="22"/>
-      <c r="U4" s="22"/>
-      <c r="V4" s="22"/>
+      <c r="U4" s="67" t="s">
+        <v>749</v>
+      </c>
+      <c r="V4" s="67" t="s">
+        <v>750</v>
+      </c>
       <c r="W4" s="23" t="s">
         <v>315</v>
       </c>

</xml_diff>

<commit_message>
new data format for dna effect
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/SceneQuest.xlsx
+++ b/ConfigData/Xlsx/SceneQuest.xlsx
@@ -154,7 +154,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1460" uniqueCount="752">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1492" uniqueCount="777">
   <si>
     <t>int</t>
     <phoneticPr fontId="18" type="noConversion"/>
@@ -3047,6 +3047,97 @@
   </si>
   <si>
     <t>hiddeway</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>boss</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>cod-;wat+</t>
+  </si>
+  <si>
+    <t>hot+;ord-</t>
+  </si>
+  <si>
+    <t>cod-</t>
+  </si>
+  <si>
+    <t>lef+</t>
+  </si>
+  <si>
+    <t>die-;anl+</t>
+  </si>
+  <si>
+    <t>die-</t>
+  </si>
+  <si>
+    <t>wat+++</t>
+  </si>
+  <si>
+    <t>kin++</t>
+  </si>
+  <si>
+    <t>cao+</t>
+  </si>
+  <si>
+    <t>hot+;ang+;ret-</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>kin++;kil-;frt+</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>cil+</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>pos+</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>ang+;ord-</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>cod-</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>thk-</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>kin+;ord-;ged+</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>die+;lef+</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>cao+</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>thk-;sky+</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>spd-;lef+</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>src-</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>ret+;src-</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>src-;anl+</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -6115,8 +6206,8 @@
   <dimension ref="A1:BY117"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A91" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P27" sqref="P27"/>
+      <pane ySplit="3" topLeftCell="A73" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="T16" sqref="T16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -6126,7 +6217,9 @@
     <col min="3" max="5" width="2.75" style="8" customWidth="1"/>
     <col min="6" max="6" width="8.75" style="8" customWidth="1"/>
     <col min="7" max="8" width="9" style="8"/>
-    <col min="9" max="22" width="4.875" style="8" customWidth="1"/>
+    <col min="9" max="20" width="4.875" style="8" customWidth="1"/>
+    <col min="21" max="21" width="11.875" style="8" customWidth="1"/>
+    <col min="22" max="22" width="10.625" style="8" customWidth="1"/>
     <col min="23" max="24" width="7" style="8" customWidth="1"/>
     <col min="25" max="25" width="9.375" style="8" customWidth="1"/>
     <col min="26" max="30" width="6.5" style="8" customWidth="1"/>
@@ -10687,8 +10780,12 @@
         <v>30</v>
       </c>
       <c r="T71" s="22"/>
-      <c r="U71" s="22"/>
-      <c r="V71" s="22"/>
+      <c r="U71" s="67" t="s">
+        <v>753</v>
+      </c>
+      <c r="V71" s="67" t="s">
+        <v>770</v>
+      </c>
       <c r="W71" s="24" t="s">
         <v>326</v>
       </c>
@@ -10750,8 +10847,12 @@
         <v>25</v>
       </c>
       <c r="T72" s="22"/>
-      <c r="U72" s="22"/>
-      <c r="V72" s="22"/>
+      <c r="U72" s="67" t="s">
+        <v>754</v>
+      </c>
+      <c r="V72" s="67" t="s">
+        <v>755</v>
+      </c>
       <c r="W72" s="24" t="s">
         <v>323</v>
       </c>
@@ -10822,8 +10923,12 @@
         <v>35</v>
       </c>
       <c r="T73" s="22"/>
-      <c r="U73" s="22"/>
-      <c r="V73" s="22"/>
+      <c r="U73" s="67" t="s">
+        <v>772</v>
+      </c>
+      <c r="V73" s="67" t="s">
+        <v>775</v>
+      </c>
       <c r="W73" s="24"/>
       <c r="X73" s="22"/>
       <c r="BG73" s="8">
@@ -10875,8 +10980,12 @@
         <v>30</v>
       </c>
       <c r="T74" s="22"/>
-      <c r="U74" s="22"/>
-      <c r="V74" s="22"/>
+      <c r="U74" s="67" t="s">
+        <v>772</v>
+      </c>
+      <c r="V74" s="67" t="s">
+        <v>774</v>
+      </c>
       <c r="X74" s="22"/>
       <c r="BB74" s="8">
         <v>1</v>
@@ -10929,8 +11038,12 @@
         <v>35</v>
       </c>
       <c r="T75" s="22"/>
-      <c r="U75" s="22"/>
-      <c r="V75" s="22"/>
+      <c r="U75" s="67" t="s">
+        <v>766</v>
+      </c>
+      <c r="V75" s="67" t="s">
+        <v>767</v>
+      </c>
       <c r="W75" s="24" t="s">
         <v>324</v>
       </c>
@@ -10998,8 +11111,12 @@
         <v>25</v>
       </c>
       <c r="T76" s="22"/>
-      <c r="U76" s="22"/>
-      <c r="V76" s="22"/>
+      <c r="U76" s="67" t="s">
+        <v>762</v>
+      </c>
+      <c r="V76" s="67" t="s">
+        <v>763</v>
+      </c>
       <c r="W76" s="24" t="s">
         <v>325</v>
       </c>
@@ -11098,8 +11215,12 @@
         <v>20</v>
       </c>
       <c r="T78" s="22"/>
-      <c r="U78" s="22"/>
-      <c r="V78" s="22"/>
+      <c r="U78" s="67" t="s">
+        <v>756</v>
+      </c>
+      <c r="V78" s="67" t="s">
+        <v>757</v>
+      </c>
       <c r="W78" s="24"/>
       <c r="X78" s="22"/>
       <c r="AE78" s="8">
@@ -11160,8 +11281,12 @@
         <v>20</v>
       </c>
       <c r="T79" s="22"/>
-      <c r="U79" s="22"/>
-      <c r="V79" s="22"/>
+      <c r="U79" s="67" t="s">
+        <v>764</v>
+      </c>
+      <c r="V79" s="67" t="s">
+        <v>757</v>
+      </c>
       <c r="W79" s="24"/>
       <c r="X79" s="22"/>
       <c r="AE79" s="8">
@@ -11219,8 +11344,12 @@
         <v>15</v>
       </c>
       <c r="T80" s="22"/>
-      <c r="U80" s="22"/>
-      <c r="V80" s="22"/>
+      <c r="U80" s="67" t="s">
+        <v>756</v>
+      </c>
+      <c r="V80" s="67" t="s">
+        <v>758</v>
+      </c>
       <c r="X80" s="22"/>
       <c r="AE80" s="8">
         <v>17000002</v>
@@ -11271,7 +11400,9 @@
         <v>20</v>
       </c>
       <c r="T81" s="22"/>
-      <c r="U81" s="22"/>
+      <c r="U81" s="67" t="s">
+        <v>773</v>
+      </c>
       <c r="V81" s="22"/>
       <c r="X81" s="22"/>
       <c r="AF81" s="8" t="s">
@@ -11332,7 +11463,7 @@
         <v>30</v>
       </c>
       <c r="T82" s="22"/>
-      <c r="U82" s="22"/>
+      <c r="U82" s="67"/>
       <c r="V82" s="22"/>
       <c r="X82" s="22"/>
       <c r="AC82" s="8" t="s">
@@ -11442,7 +11573,9 @@
         <v>50</v>
       </c>
       <c r="T84" s="22"/>
-      <c r="U84" s="22"/>
+      <c r="U84" s="67" t="s">
+        <v>765</v>
+      </c>
       <c r="V84" s="22"/>
       <c r="X84" s="22"/>
       <c r="AC84" s="8" t="s">
@@ -11496,8 +11629,12 @@
       <c r="R85" s="22"/>
       <c r="S85" s="102"/>
       <c r="T85" s="22"/>
-      <c r="U85" s="22"/>
-      <c r="V85" s="22"/>
+      <c r="U85" s="22" t="s">
+        <v>759</v>
+      </c>
+      <c r="V85" s="22" t="s">
+        <v>760</v>
+      </c>
       <c r="W85" s="8" t="s">
         <v>423</v>
       </c>
@@ -11566,8 +11703,12 @@
         <v>50</v>
       </c>
       <c r="T86" s="22"/>
-      <c r="U86" s="22"/>
-      <c r="V86" s="22"/>
+      <c r="U86" s="67" t="s">
+        <v>776</v>
+      </c>
+      <c r="V86" s="67" t="s">
+        <v>771</v>
+      </c>
       <c r="X86" s="22"/>
       <c r="AW86" s="8" t="s">
         <v>435</v>
@@ -11605,7 +11746,9 @@
       </c>
       <c r="I87" s="22"/>
       <c r="J87" s="22"/>
-      <c r="K87" s="22"/>
+      <c r="K87" s="67" t="s">
+        <v>752</v>
+      </c>
       <c r="L87" s="30" t="s">
         <v>243</v>
       </c>
@@ -11619,8 +11762,12 @@
         <v>20</v>
       </c>
       <c r="T87" s="22"/>
-      <c r="U87" s="22"/>
-      <c r="V87" s="22"/>
+      <c r="U87" s="67" t="s">
+        <v>759</v>
+      </c>
+      <c r="V87" s="67" t="s">
+        <v>760</v>
+      </c>
       <c r="W87" s="24" t="s">
         <v>474</v>
       </c>
@@ -13445,7 +13592,9 @@
       <c r="T114" s="102">
         <v>1</v>
       </c>
-      <c r="U114" s="102"/>
+      <c r="U114" s="102" t="s">
+        <v>761</v>
+      </c>
       <c r="V114" s="102"/>
       <c r="X114" s="22"/>
       <c r="Z114" s="70"/>
@@ -13517,7 +13666,9 @@
       <c r="T115" s="102">
         <v>1</v>
       </c>
-      <c r="U115" s="102"/>
+      <c r="U115" s="102" t="s">
+        <v>761</v>
+      </c>
       <c r="V115" s="102"/>
       <c r="X115" s="22"/>
       <c r="Z115" s="70"/>
@@ -13589,7 +13740,9 @@
       <c r="T116" s="102">
         <v>1</v>
       </c>
-      <c r="U116" s="102"/>
+      <c r="U116" s="102" t="s">
+        <v>761</v>
+      </c>
       <c r="V116" s="102"/>
       <c r="X116" s="22"/>
       <c r="Z116" s="70"/>
@@ -13665,8 +13818,12 @@
       <c r="T117" s="102">
         <v>1</v>
       </c>
-      <c r="U117" s="102"/>
-      <c r="V117" s="102"/>
+      <c r="U117" s="102" t="s">
+        <v>769</v>
+      </c>
+      <c r="V117" s="102" t="s">
+        <v>768</v>
+      </c>
       <c r="X117" s="22"/>
       <c r="Z117" s="70"/>
       <c r="AG117" s="70"/>
@@ -13720,8 +13877,8 @@
   <dimension ref="A1:BY42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="U1" sqref="U1:V3"/>
+      <pane ySplit="3" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="T33" sqref="T33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>

</xml_diff>

<commit_message>
add the card upgrade effect
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/SceneQuest.xlsx
+++ b/ConfigData/Xlsx/SceneQuest.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView minimized="1" xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385"/>
+    <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="4" r:id="rId1"/>
@@ -154,7 +154,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1493" uniqueCount="754">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1496" uniqueCount="754">
   <si>
     <t>int</t>
     <phoneticPr fontId="18" type="noConversion"/>
@@ -6167,8 +6167,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BV113"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A80" workbookViewId="0">
-      <selection activeCell="G95" sqref="G95"/>
+    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="J94" sqref="J94:J96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -12361,7 +12361,9 @@
         <v>564</v>
       </c>
       <c r="I94" s="67"/>
-      <c r="J94" s="67"/>
+      <c r="J94" s="67" t="s">
+        <v>747</v>
+      </c>
       <c r="K94" s="67"/>
       <c r="L94" s="31" t="s">
         <v>240</v>
@@ -12423,7 +12425,9 @@
         <v>565</v>
       </c>
       <c r="I95" s="67"/>
-      <c r="J95" s="67"/>
+      <c r="J95" s="67" t="s">
+        <v>747</v>
+      </c>
       <c r="K95" s="67"/>
       <c r="L95" s="31" t="s">
         <v>240</v>
@@ -12483,7 +12487,9 @@
         <v>752</v>
       </c>
       <c r="I96" s="67"/>
-      <c r="J96" s="67"/>
+      <c r="J96" s="67" t="s">
+        <v>747</v>
+      </c>
       <c r="K96" s="67"/>
       <c r="L96" s="31" t="s">
         <v>240</v>
@@ -13775,7 +13781,7 @@
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
-  <conditionalFormatting sqref="E17:BV25 E28:BV28 E26:I27 K26:AZ27 E32:BV37 E29:I31 K29:AZ31 E39:BV44 E38:I38 K38:AZ38 E48:BV48 E45:I47 K45:AZ47 E53:BV59 E52:I52 K52:AZ52 E50:BV51 E49:I49 K49:AZ49 E61:BV61 E60:I60 K60:AZ60 E62:I63 K62:AZ63 BC26:BV27 BC29:BV31 BC38:BV38 BC45:BV47 BC49:BV49 BC52:BV52 BC60:BV60 BC62:BV63 E113:AZ113 BC113:BV113 E4:BV15 E64:BV95 E97:BV112">
+  <conditionalFormatting sqref="E17:BV25 E28:BV28 E26:I27 K26:AZ27 E32:BV37 E29:I31 K29:AZ31 E39:BV44 E38:I38 K38:AZ38 E48:BV48 E45:I47 K45:AZ47 E53:BV59 E52:I52 K52:AZ52 E50:BV51 E49:I49 K49:AZ49 E61:BV61 E60:I60 K60:AZ60 E62:I63 K62:AZ63 BC26:BV27 BC29:BV31 BC38:BV38 BC45:BV47 BC49:BV49 BC52:BV52 BC60:BV60 BC62:BV63 E113:AZ113 BC113:BV113 E4:BV15 E97:BV112 E64:BV95 J94:J96">
     <cfRule type="containsBlanks" dxfId="16" priority="33">
       <formula>LEN(TRIM(E4))=0</formula>
     </cfRule>

</xml_diff>

<commit_message>
support eventcount for chess
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/SceneQuest.xlsx
+++ b/ConfigData/Xlsx/SceneQuest.xlsx
@@ -154,7 +154,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1674" uniqueCount="773">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1682" uniqueCount="780">
   <si>
     <t>int</t>
     <phoneticPr fontId="18" type="noConversion"/>
@@ -3131,6 +3131,32 @@
   </si>
   <si>
     <t>npcgailu</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>aolai</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>weia</t>
+  </si>
+  <si>
+    <t>milanda</t>
+  </si>
+  <si>
+    <t>gailu</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>beilukai</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>leiluo</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>baludi</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -4383,167 +4409,6 @@
   </cellStyles>
   <dxfs count="102">
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -5262,6 +5127,20 @@
       </fill>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -5777,6 +5656,153 @@
         </patternFill>
       </fill>
     </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -5871,7 +5897,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="表3" displayName="表3" ref="A3:BW115" totalsRowShown="0" headerRowDxfId="101">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="表3" displayName="表3" ref="A3:BW115" totalsRowShown="0" headerRowDxfId="80">
   <autoFilter ref="A3:BW115"/>
   <sortState ref="A4:BU115">
     <sortCondition ref="A3:A115"/>
@@ -5884,56 +5910,56 @@
     <tableColumn id="25" name="Danger"/>
     <tableColumn id="24" name="Ename"/>
     <tableColumn id="5" name="Script"/>
-    <tableColumn id="6" name="TriggerMulti" dataDxfId="100"/>
-    <tableColumn id="74" name="MapIcon" dataDxfId="99"/>
-    <tableColumn id="69" name="Tag" dataDxfId="98"/>
-    <tableColumn id="40" name="Catalog" dataDxfId="97"/>
+    <tableColumn id="6" name="TriggerMulti" dataDxfId="79"/>
+    <tableColumn id="74" name="MapIcon" dataDxfId="78"/>
+    <tableColumn id="69" name="Tag" dataDxfId="77"/>
+    <tableColumn id="40" name="Catalog" dataDxfId="76"/>
     <tableColumn id="29" name="Catalog2"/>
-    <tableColumn id="35" name="TriggerHourBegin" dataDxfId="96"/>
-    <tableColumn id="34" name="TriggerHourEnd" dataDxfId="95"/>
-    <tableColumn id="36" name="TriggerQuestNotReceive" dataDxfId="94"/>
-    <tableColumn id="37" name="TriggerQuestReceived" dataDxfId="93"/>
-    <tableColumn id="38" name="TriggerQuestFinished" dataDxfId="92"/>
-    <tableColumn id="39" name="TriggerRate" dataDxfId="91"/>
-    <tableColumn id="62" name="TriggerLimitInDungeon" dataDxfId="90"/>
-    <tableColumn id="77" name="TriggerDNARate" dataDxfId="89"/>
-    <tableColumn id="76" name="TriggerDNAHard" dataDxfId="88"/>
-    <tableColumn id="78" name="DnaInfo" dataDxfId="87"/>
+    <tableColumn id="35" name="TriggerHourBegin" dataDxfId="75"/>
+    <tableColumn id="34" name="TriggerHourEnd" dataDxfId="74"/>
+    <tableColumn id="36" name="TriggerQuestNotReceive" dataDxfId="73"/>
+    <tableColumn id="37" name="TriggerQuestReceived" dataDxfId="72"/>
+    <tableColumn id="38" name="TriggerQuestFinished" dataDxfId="71"/>
+    <tableColumn id="39" name="TriggerRate" dataDxfId="70"/>
+    <tableColumn id="62" name="TriggerLimitInDungeon" dataDxfId="69"/>
+    <tableColumn id="77" name="TriggerDNARate" dataDxfId="68"/>
+    <tableColumn id="76" name="TriggerDNAHard" dataDxfId="67"/>
+    <tableColumn id="78" name="DnaInfo" dataDxfId="66"/>
     <tableColumn id="7" name="EnemyName"/>
-    <tableColumn id="51" name="CanBribe" dataDxfId="86"/>
+    <tableColumn id="51" name="CanBribe" dataDxfId="65"/>
     <tableColumn id="32" name="SceneId"/>
-    <tableColumn id="54" name="DungeonId" dataDxfId="85"/>
+    <tableColumn id="54" name="DungeonId" dataDxfId="64"/>
     <tableColumn id="50" name="CheckQuest"/>
     <tableColumn id="27" name="NextQuest"/>
     <tableColumn id="44" name="HiddenRoomQuest"/>
     <tableColumn id="8" name="ShopName"/>
     <tableColumn id="41" name="MiniGameId"/>
     <tableColumn id="43" name="PayKey"/>
-    <tableColumn id="67" name="NeedDungeonItemId" dataDxfId="84"/>
-    <tableColumn id="68" name="NeedDungeonItemCount" dataDxfId="83"/>
-    <tableColumn id="63" name="TestType1" dataDxfId="82"/>
-    <tableColumn id="64" name="TestBias1" dataDxfId="81"/>
-    <tableColumn id="65" name="TestType2" dataDxfId="80"/>
-    <tableColumn id="66" name="TestBias2" dataDxfId="79"/>
+    <tableColumn id="67" name="NeedDungeonItemId" dataDxfId="63"/>
+    <tableColumn id="68" name="NeedDungeonItemCount" dataDxfId="62"/>
+    <tableColumn id="63" name="TestType1" dataDxfId="61"/>
+    <tableColumn id="64" name="TestBias1" dataDxfId="60"/>
+    <tableColumn id="65" name="TestType2" dataDxfId="59"/>
+    <tableColumn id="66" name="TestBias2" dataDxfId="58"/>
     <tableColumn id="9" name="RewardGold"/>
     <tableColumn id="10" name="RewardFood"/>
     <tableColumn id="11" name="RewardHealth"/>
     <tableColumn id="12" name="RewardMental"/>
     <tableColumn id="13" name="RewardExp"/>
-    <tableColumn id="56" name="RewardStr" dataDxfId="78"/>
-    <tableColumn id="57" name="RewardAgi" dataDxfId="77"/>
-    <tableColumn id="58" name="RewardIntl" dataDxfId="76"/>
-    <tableColumn id="59" name="RewardPerc" dataDxfId="75"/>
-    <tableColumn id="60" name="RewardEndu" dataDxfId="74"/>
+    <tableColumn id="56" name="RewardStr" dataDxfId="57"/>
+    <tableColumn id="57" name="RewardAgi" dataDxfId="56"/>
+    <tableColumn id="58" name="RewardIntl" dataDxfId="55"/>
+    <tableColumn id="59" name="RewardPerc" dataDxfId="54"/>
+    <tableColumn id="60" name="RewardEndu" dataDxfId="53"/>
     <tableColumn id="14" name="RewardItem"/>
     <tableColumn id="15" name="RewardDrop"/>
-    <tableColumn id="73" name="RewardCollectType" dataDxfId="73"/>
-    <tableColumn id="55" name="RewardDungeonItemId" dataDxfId="72"/>
-    <tableColumn id="61" name="RewardDungeonItemCount" dataDxfId="71"/>
+    <tableColumn id="73" name="RewardCollectType" dataDxfId="52"/>
+    <tableColumn id="55" name="RewardDungeonItemId" dataDxfId="51"/>
+    <tableColumn id="61" name="RewardDungeonItemCount" dataDxfId="50"/>
     <tableColumn id="30" name="RewardBlessLevel"/>
     <tableColumn id="42" name="RewardBlessName"/>
-    <tableColumn id="52" name="RewardResId" dataDxfId="70"/>
-    <tableColumn id="53" name="RewardResAmount" dataDxfId="69"/>
+    <tableColumn id="52" name="RewardResId" dataDxfId="49"/>
+    <tableColumn id="53" name="RewardResAmount" dataDxfId="48"/>
     <tableColumn id="26" name="UnlockRival"/>
     <tableColumn id="16" name="PunishGold"/>
     <tableColumn id="17" name="PunishFood"/>
@@ -5950,15 +5976,15 @@
     <tableColumn id="22" name="TradeHealth"/>
     <tableColumn id="23" name="TradeMental"/>
     <tableColumn id="33" name="TradeDropItem"/>
-    <tableColumn id="4" name="FigueScene" dataDxfId="68"/>
-    <tableColumn id="70" name="FigueBig" dataDxfId="67"/>
+    <tableColumn id="4" name="FigueScene" dataDxfId="47"/>
+    <tableColumn id="70" name="FigueBig" dataDxfId="46"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="表3_5" displayName="表3_5" ref="A3:BW42" totalsRowShown="0" headerRowDxfId="66">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="表3_5" displayName="表3_5" ref="A3:BW42" totalsRowShown="0" headerRowDxfId="43">
   <autoFilter ref="A3:BW42"/>
   <sortState ref="A4:BU42">
     <sortCondition ref="A3:A6"/>
@@ -5966,61 +5992,61 @@
   <tableColumns count="75">
     <tableColumn id="1" name="Id"/>
     <tableColumn id="2" name="Name"/>
-    <tableColumn id="27" name="Type" dataDxfId="65"/>
+    <tableColumn id="27" name="Type" dataDxfId="42"/>
     <tableColumn id="3" name="Level"/>
     <tableColumn id="25" name="Danger"/>
     <tableColumn id="24" name="Ename"/>
     <tableColumn id="5" name="Script"/>
     <tableColumn id="6" name="TriggerMulti"/>
-    <tableColumn id="74" name="MapIcon" dataDxfId="64"/>
-    <tableColumn id="69" name="Tag" dataDxfId="63"/>
-    <tableColumn id="40" name="Catalog" dataDxfId="62"/>
-    <tableColumn id="29" name="Catalog2" dataDxfId="61"/>
-    <tableColumn id="35" name="TriggerHourBegin" dataDxfId="60"/>
-    <tableColumn id="34" name="TriggerHourEnd" dataDxfId="59"/>
-    <tableColumn id="37" name="TriggerQuestNotReceive" dataDxfId="58"/>
-    <tableColumn id="38" name="TriggerQuestReceived" dataDxfId="57"/>
-    <tableColumn id="36" name="TriggerQuestFinished" dataDxfId="56"/>
-    <tableColumn id="39" name="TriggerRate" dataDxfId="55"/>
-    <tableColumn id="62" name="TriggerLimitInDungeon" dataDxfId="54"/>
-    <tableColumn id="76" name="TriggerDNARate" dataDxfId="53"/>
-    <tableColumn id="77" name="TriggerDNAHard" dataDxfId="52"/>
-    <tableColumn id="78" name="DnaInfo" dataDxfId="51"/>
+    <tableColumn id="74" name="MapIcon" dataDxfId="41"/>
+    <tableColumn id="69" name="Tag" dataDxfId="40"/>
+    <tableColumn id="40" name="Catalog" dataDxfId="39"/>
+    <tableColumn id="29" name="Catalog2" dataDxfId="38"/>
+    <tableColumn id="35" name="TriggerHourBegin" dataDxfId="37"/>
+    <tableColumn id="34" name="TriggerHourEnd" dataDxfId="36"/>
+    <tableColumn id="37" name="TriggerQuestNotReceive" dataDxfId="35"/>
+    <tableColumn id="38" name="TriggerQuestReceived" dataDxfId="34"/>
+    <tableColumn id="36" name="TriggerQuestFinished" dataDxfId="33"/>
+    <tableColumn id="39" name="TriggerRate" dataDxfId="32"/>
+    <tableColumn id="62" name="TriggerLimitInDungeon" dataDxfId="31"/>
+    <tableColumn id="76" name="TriggerDNARate" dataDxfId="30"/>
+    <tableColumn id="77" name="TriggerDNAHard" dataDxfId="29"/>
+    <tableColumn id="78" name="DnaInfo" dataDxfId="28"/>
     <tableColumn id="7" name="EnemyName"/>
-    <tableColumn id="51" name="CanBribe" dataDxfId="50"/>
-    <tableColumn id="32" name="SceneId" dataDxfId="49"/>
-    <tableColumn id="54" name="DungeonId" dataDxfId="48"/>
-    <tableColumn id="50" name="CheckQuest" dataDxfId="47"/>
-    <tableColumn id="28" name="NextQuest" dataDxfId="46"/>
-    <tableColumn id="44" name="HiddenRoomQuest" dataDxfId="45"/>
-    <tableColumn id="8" name="ShopName" dataDxfId="44"/>
-    <tableColumn id="41" name="MiniGameId" dataDxfId="43"/>
-    <tableColumn id="43" name="PayKey" dataDxfId="42"/>
-    <tableColumn id="67" name="NeedDungeonItemId" dataDxfId="41"/>
-    <tableColumn id="68" name="NeedDungeonItemCount" dataDxfId="40"/>
-    <tableColumn id="63" name="TestType1" dataDxfId="39"/>
-    <tableColumn id="64" name="TestBias1" dataDxfId="38"/>
-    <tableColumn id="65" name="TestType2" dataDxfId="37"/>
-    <tableColumn id="66" name="TestBias2" dataDxfId="36"/>
+    <tableColumn id="51" name="CanBribe" dataDxfId="27"/>
+    <tableColumn id="32" name="SceneId" dataDxfId="26"/>
+    <tableColumn id="54" name="DungeonId" dataDxfId="25"/>
+    <tableColumn id="50" name="CheckQuest" dataDxfId="24"/>
+    <tableColumn id="28" name="NextQuest" dataDxfId="23"/>
+    <tableColumn id="44" name="HiddenRoomQuest" dataDxfId="22"/>
+    <tableColumn id="8" name="ShopName" dataDxfId="21"/>
+    <tableColumn id="41" name="MiniGameId" dataDxfId="20"/>
+    <tableColumn id="43" name="PayKey" dataDxfId="19"/>
+    <tableColumn id="67" name="NeedDungeonItemId" dataDxfId="18"/>
+    <tableColumn id="68" name="NeedDungeonItemCount" dataDxfId="17"/>
+    <tableColumn id="63" name="TestType1" dataDxfId="16"/>
+    <tableColumn id="64" name="TestBias1" dataDxfId="15"/>
+    <tableColumn id="65" name="TestType2" dataDxfId="14"/>
+    <tableColumn id="66" name="TestBias2" dataDxfId="13"/>
     <tableColumn id="9" name="RewardGold"/>
     <tableColumn id="10" name="RewardFood"/>
     <tableColumn id="11" name="RewardHealth"/>
     <tableColumn id="12" name="RewardMental"/>
     <tableColumn id="13" name="RewardExp"/>
-    <tableColumn id="55" name="RewardStr" dataDxfId="35"/>
-    <tableColumn id="56" name="RewardAgi" dataDxfId="34"/>
-    <tableColumn id="57" name="RewardIntl" dataDxfId="33"/>
-    <tableColumn id="58" name="RewardPerc" dataDxfId="32"/>
-    <tableColumn id="59" name="RewardEndu" dataDxfId="31"/>
+    <tableColumn id="55" name="RewardStr" dataDxfId="12"/>
+    <tableColumn id="56" name="RewardAgi" dataDxfId="11"/>
+    <tableColumn id="57" name="RewardIntl" dataDxfId="10"/>
+    <tableColumn id="58" name="RewardPerc" dataDxfId="9"/>
+    <tableColumn id="59" name="RewardEndu" dataDxfId="8"/>
     <tableColumn id="14" name="RewardItem"/>
     <tableColumn id="15" name="RewardDrop"/>
-    <tableColumn id="73" name="RewardCollectType" dataDxfId="30"/>
-    <tableColumn id="60" name="RewardDungeonItemId" dataDxfId="29"/>
-    <tableColumn id="61" name="RewardDungeonItemCount" dataDxfId="28"/>
+    <tableColumn id="73" name="RewardCollectType" dataDxfId="7"/>
+    <tableColumn id="60" name="RewardDungeonItemId" dataDxfId="6"/>
+    <tableColumn id="61" name="RewardDungeonItemCount" dataDxfId="5"/>
     <tableColumn id="31" name="RewardBlessLevel"/>
     <tableColumn id="42" name="RewardBlessName"/>
-    <tableColumn id="52" name="RewardResId" dataDxfId="27"/>
-    <tableColumn id="53" name="RewardResAmount" dataDxfId="26"/>
+    <tableColumn id="52" name="RewardResId" dataDxfId="4"/>
+    <tableColumn id="53" name="RewardResAmount" dataDxfId="3"/>
     <tableColumn id="26" name="UnlockRival"/>
     <tableColumn id="16" name="PunishGold"/>
     <tableColumn id="17" name="PunishFood"/>
@@ -6036,9 +6062,9 @@
     <tableColumn id="21" name="TradeFood"/>
     <tableColumn id="22" name="TradeHealth"/>
     <tableColumn id="23" name="TradeMental"/>
-    <tableColumn id="33" name="TradeDropItem" dataDxfId="25"/>
-    <tableColumn id="70" name="FigueScene" dataDxfId="24"/>
-    <tableColumn id="71" name="FigueBig" dataDxfId="23"/>
+    <tableColumn id="33" name="TradeDropItem" dataDxfId="2"/>
+    <tableColumn id="70" name="FigueScene" dataDxfId="1"/>
+    <tableColumn id="71" name="FigueBig" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -14451,107 +14477,107 @@
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <conditionalFormatting sqref="J27:AY28 J30:AY32 J39:AY39 J46:AY48 J53:AY53 J50:AY50 J61:AY61 J63:AY64 BB27:BU28 BB30:BU32 BB39:BU39 BB46:BU48 BB50:BU50 BB53:BU53 BB61:BU61 BB63:BU64 I95:I97 G18:BU26 G29:BU29 G27:H28 G33:BU38 G30:H32 G40:BU45 G39:H39 G49:BU49 G46:H48 G54:BU60 G53:H53 G51:BU52 G50:H50 G62:BU62 G61:H61 G63:H64 G115:AY115 BB115:BV115 G65:BU66 G97:BV114 G16:AY16 BV18:BV96 E18:F115 BW18:BW115 G68:BU96 G67:H67 J67:BU67 G4:BU15 E4:F16 BV4:BW16">
-    <cfRule type="containsBlanks" dxfId="22" priority="46">
+    <cfRule type="containsBlanks" dxfId="101" priority="46">
       <formula>LEN(TRIM(E4))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BA16:BU16">
-    <cfRule type="containsBlanks" dxfId="21" priority="28">
+    <cfRule type="containsBlanks" dxfId="100" priority="28">
       <formula>LEN(TRIM(BA16))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I27:I28">
-    <cfRule type="containsBlanks" dxfId="20" priority="27">
+    <cfRule type="containsBlanks" dxfId="99" priority="27">
       <formula>LEN(TRIM(I27))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I30:I31">
-    <cfRule type="containsBlanks" dxfId="19" priority="26">
+    <cfRule type="containsBlanks" dxfId="98" priority="26">
       <formula>LEN(TRIM(I30))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I50">
-    <cfRule type="containsBlanks" dxfId="18" priority="22">
+    <cfRule type="containsBlanks" dxfId="97" priority="22">
       <formula>LEN(TRIM(I50))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AZ16">
-    <cfRule type="containsBlanks" dxfId="17" priority="19">
+    <cfRule type="containsBlanks" dxfId="96" priority="19">
       <formula>LEN(TRIM(AZ16))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BA63:BA64 BA61 BA53 BA50 BA46:BA48 BA39 BA30:BA32 BA27:BA28">
-    <cfRule type="containsBlanks" dxfId="16" priority="18">
+    <cfRule type="containsBlanks" dxfId="95" priority="18">
       <formula>LEN(TRIM(BA27))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AZ63:AZ64 AZ61 AZ53 AZ50 AZ46:AZ48 AZ39 AZ30:AZ32 AZ27:AZ28">
-    <cfRule type="containsBlanks" dxfId="15" priority="17">
+    <cfRule type="containsBlanks" dxfId="94" priority="17">
       <formula>LEN(TRIM(AZ27))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BA115">
-    <cfRule type="containsBlanks" dxfId="14" priority="16">
+    <cfRule type="containsBlanks" dxfId="93" priority="16">
       <formula>LEN(TRIM(BA115))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AZ115">
-    <cfRule type="containsBlanks" dxfId="13" priority="15">
+    <cfRule type="containsBlanks" dxfId="92" priority="15">
       <formula>LEN(TRIM(AZ115))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I98">
-    <cfRule type="containsBlanks" dxfId="12" priority="13">
+    <cfRule type="containsBlanks" dxfId="91" priority="13">
       <formula>LEN(TRIM(I98))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E17:AY17 BV17:BW17">
-    <cfRule type="containsBlanks" dxfId="11" priority="10">
+    <cfRule type="containsBlanks" dxfId="90" priority="10">
       <formula>LEN(TRIM(E17))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BA17:BU17">
-    <cfRule type="containsBlanks" dxfId="10" priority="9">
+    <cfRule type="containsBlanks" dxfId="89" priority="9">
       <formula>LEN(TRIM(BA17))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AZ17">
-    <cfRule type="containsBlanks" dxfId="9" priority="8">
+    <cfRule type="containsBlanks" dxfId="88" priority="8">
       <formula>LEN(TRIM(AZ17))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I32">
-    <cfRule type="containsBlanks" dxfId="8" priority="7">
+    <cfRule type="containsBlanks" dxfId="87" priority="7">
       <formula>LEN(TRIM(I32))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I39">
-    <cfRule type="containsBlanks" dxfId="7" priority="6">
+    <cfRule type="containsBlanks" dxfId="86" priority="6">
       <formula>LEN(TRIM(I39))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I46:I48">
-    <cfRule type="containsBlanks" dxfId="6" priority="5">
+    <cfRule type="containsBlanks" dxfId="85" priority="5">
       <formula>LEN(TRIM(I46))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I53">
-    <cfRule type="containsBlanks" dxfId="5" priority="4">
+    <cfRule type="containsBlanks" dxfId="84" priority="4">
       <formula>LEN(TRIM(I53))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I61">
-    <cfRule type="containsBlanks" dxfId="4" priority="3">
+    <cfRule type="containsBlanks" dxfId="83" priority="3">
       <formula>LEN(TRIM(I61))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I63:I64">
-    <cfRule type="containsBlanks" dxfId="3" priority="2">
+    <cfRule type="containsBlanks" dxfId="82" priority="2">
       <formula>LEN(TRIM(I63))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I67">
-    <cfRule type="containsBlanks" dxfId="2" priority="1">
+    <cfRule type="containsBlanks" dxfId="81" priority="1">
       <formula>LEN(TRIM(I67))=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -14570,7 +14596,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G22" sqref="G22"/>
+      <selection pane="bottomLeft" activeCell="W22" sqref="W22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -15859,7 +15885,9 @@
       <c r="T13" s="59"/>
       <c r="U13" s="59"/>
       <c r="V13" s="59"/>
-      <c r="W13" s="60"/>
+      <c r="W13" s="60" t="s">
+        <v>295</v>
+      </c>
       <c r="X13" s="59"/>
       <c r="Y13" s="60"/>
       <c r="Z13" s="60"/>
@@ -15980,6 +16008,9 @@
       <c r="T15" s="59"/>
       <c r="U15" s="59"/>
       <c r="V15" s="59"/>
+      <c r="W15" s="70" t="s">
+        <v>773</v>
+      </c>
       <c r="X15" s="59"/>
       <c r="Y15" s="60"/>
       <c r="Z15" s="60"/>
@@ -16101,6 +16132,9 @@
       <c r="T17" s="59"/>
       <c r="U17" s="59"/>
       <c r="V17" s="59"/>
+      <c r="W17" s="44" t="s">
+        <v>774</v>
+      </c>
       <c r="X17" s="59"/>
       <c r="Y17" s="60"/>
       <c r="Z17" s="60"/>
@@ -16159,6 +16193,9 @@
       <c r="T18" s="59"/>
       <c r="U18" s="59"/>
       <c r="V18" s="59"/>
+      <c r="W18" s="44" t="s">
+        <v>775</v>
+      </c>
       <c r="X18" s="59"/>
       <c r="Y18" s="60"/>
       <c r="Z18" s="60"/>
@@ -16217,6 +16254,9 @@
       <c r="T19" s="59"/>
       <c r="U19" s="59"/>
       <c r="V19" s="59"/>
+      <c r="W19" s="70" t="s">
+        <v>777</v>
+      </c>
       <c r="X19" s="59"/>
       <c r="Y19" s="60"/>
       <c r="Z19" s="60"/>
@@ -16275,6 +16315,9 @@
       <c r="T20" s="59"/>
       <c r="U20" s="59"/>
       <c r="V20" s="59"/>
+      <c r="W20" s="70" t="s">
+        <v>778</v>
+      </c>
       <c r="X20" s="59"/>
       <c r="Y20" s="60"/>
       <c r="Z20" s="60"/>
@@ -16333,6 +16376,9 @@
       <c r="T21" s="59"/>
       <c r="U21" s="59"/>
       <c r="V21" s="59"/>
+      <c r="W21" s="70" t="s">
+        <v>779</v>
+      </c>
       <c r="X21" s="59"/>
       <c r="Y21" s="60"/>
       <c r="Z21" s="60"/>
@@ -16391,6 +16437,9 @@
       <c r="T22" s="59"/>
       <c r="U22" s="59"/>
       <c r="V22" s="59"/>
+      <c r="W22" s="70" t="s">
+        <v>776</v>
+      </c>
       <c r="X22" s="59"/>
       <c r="Y22" s="60"/>
       <c r="Z22" s="60"/>
@@ -17739,12 +17788,12 @@
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <conditionalFormatting sqref="E4:BW21 E23:BW42">
-    <cfRule type="containsBlanks" dxfId="1" priority="19">
+    <cfRule type="containsBlanks" dxfId="45" priority="19">
       <formula>LEN(TRIM(E4))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E22:BW22">
-    <cfRule type="containsBlanks" dxfId="0" priority="1">
+    <cfRule type="containsBlanks" dxfId="44" priority="1">
       <formula>LEN(TRIM(E22))=0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
optimise some answer tips
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/SceneQuest.xlsx
+++ b/ConfigData/Xlsx/SceneQuest.xlsx
@@ -154,7 +154,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1673" uniqueCount="776">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1674" uniqueCount="776">
   <si>
     <t>int</t>
     <phoneticPr fontId="18" type="noConversion"/>
@@ -4394,146 +4394,6 @@
   </cellStyles>
   <dxfs count="99">
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -5252,6 +5112,13 @@
       </fill>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -5767,6 +5634,139 @@
         </patternFill>
       </fill>
     </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -5861,7 +5861,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="表3" displayName="表3" ref="A3:BV115" totalsRowShown="0" headerRowDxfId="98">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="表3" displayName="表3" ref="A3:BV115" totalsRowShown="0" headerRowDxfId="79">
   <autoFilter ref="A3:BV115"/>
   <sortState ref="A4:BT115">
     <sortCondition ref="A3:A115"/>
@@ -5874,56 +5874,56 @@
     <tableColumn id="25" name="Danger"/>
     <tableColumn id="24" name="Ename"/>
     <tableColumn id="5" name="Script"/>
-    <tableColumn id="6" name="TriggerMulti" dataDxfId="97"/>
-    <tableColumn id="74" name="MapIcon" dataDxfId="96"/>
-    <tableColumn id="69" name="Tag" dataDxfId="95"/>
-    <tableColumn id="40" name="Catalog" dataDxfId="94"/>
+    <tableColumn id="6" name="TriggerMulti" dataDxfId="78"/>
+    <tableColumn id="74" name="MapIcon" dataDxfId="77"/>
+    <tableColumn id="69" name="Tag" dataDxfId="76"/>
+    <tableColumn id="40" name="Catalog" dataDxfId="75"/>
     <tableColumn id="29" name="Catalog2"/>
-    <tableColumn id="35" name="TriggerHourBegin" dataDxfId="93"/>
-    <tableColumn id="34" name="TriggerHourEnd" dataDxfId="92"/>
-    <tableColumn id="36" name="TriggerQuestNotReceive" dataDxfId="91"/>
-    <tableColumn id="37" name="TriggerQuestReceived" dataDxfId="90"/>
-    <tableColumn id="38" name="TriggerQuestFinished" dataDxfId="89"/>
-    <tableColumn id="39" name="TriggerRate" dataDxfId="88"/>
-    <tableColumn id="62" name="TriggerLimitInDungeon" dataDxfId="87"/>
-    <tableColumn id="77" name="TriggerDNARate" dataDxfId="86"/>
-    <tableColumn id="76" name="TriggerDNAHard" dataDxfId="85"/>
-    <tableColumn id="78" name="DnaInfo" dataDxfId="84"/>
+    <tableColumn id="35" name="TriggerHourBegin" dataDxfId="74"/>
+    <tableColumn id="34" name="TriggerHourEnd" dataDxfId="73"/>
+    <tableColumn id="36" name="TriggerQuestNotReceive" dataDxfId="72"/>
+    <tableColumn id="37" name="TriggerQuestReceived" dataDxfId="71"/>
+    <tableColumn id="38" name="TriggerQuestFinished" dataDxfId="70"/>
+    <tableColumn id="39" name="TriggerRate" dataDxfId="69"/>
+    <tableColumn id="62" name="TriggerLimitInDungeon" dataDxfId="68"/>
+    <tableColumn id="77" name="TriggerDNARate" dataDxfId="67"/>
+    <tableColumn id="76" name="TriggerDNAHard" dataDxfId="66"/>
+    <tableColumn id="78" name="DnaInfo" dataDxfId="65"/>
     <tableColumn id="7" name="EnemyName"/>
-    <tableColumn id="51" name="CanBribe" dataDxfId="83"/>
+    <tableColumn id="51" name="CanBribe" dataDxfId="64"/>
     <tableColumn id="32" name="SceneId"/>
-    <tableColumn id="54" name="DungeonId" dataDxfId="82"/>
+    <tableColumn id="54" name="DungeonId" dataDxfId="63"/>
     <tableColumn id="50" name="CheckQuest"/>
     <tableColumn id="27" name="NextQuest"/>
     <tableColumn id="44" name="HiddenRoomQuest"/>
     <tableColumn id="8" name="ShopName"/>
     <tableColumn id="41" name="MiniGameId"/>
     <tableColumn id="43" name="PayKey"/>
-    <tableColumn id="67" name="NeedDungeonItemId" dataDxfId="81"/>
-    <tableColumn id="68" name="NeedDungeonItemCount" dataDxfId="80"/>
-    <tableColumn id="63" name="TestType1" dataDxfId="79"/>
-    <tableColumn id="64" name="TestBias1" dataDxfId="78"/>
-    <tableColumn id="65" name="TestType2" dataDxfId="77"/>
-    <tableColumn id="66" name="TestBias2" dataDxfId="76"/>
+    <tableColumn id="67" name="NeedDungeonItemId" dataDxfId="62"/>
+    <tableColumn id="68" name="NeedDungeonItemCount" dataDxfId="61"/>
+    <tableColumn id="63" name="TestType1" dataDxfId="60"/>
+    <tableColumn id="64" name="TestBias1" dataDxfId="59"/>
+    <tableColumn id="65" name="TestType2" dataDxfId="58"/>
+    <tableColumn id="66" name="TestBias2" dataDxfId="57"/>
     <tableColumn id="9" name="RewardGold"/>
     <tableColumn id="10" name="RewardFood"/>
     <tableColumn id="11" name="RewardHealth"/>
     <tableColumn id="12" name="RewardMental"/>
     <tableColumn id="13" name="RewardExp"/>
-    <tableColumn id="56" name="RewardStr" dataDxfId="75"/>
-    <tableColumn id="57" name="RewardAgi" dataDxfId="74"/>
-    <tableColumn id="58" name="RewardIntl" dataDxfId="73"/>
-    <tableColumn id="59" name="RewardPerc" dataDxfId="72"/>
-    <tableColumn id="60" name="RewardEndu" dataDxfId="71"/>
+    <tableColumn id="56" name="RewardStr" dataDxfId="56"/>
+    <tableColumn id="57" name="RewardAgi" dataDxfId="55"/>
+    <tableColumn id="58" name="RewardIntl" dataDxfId="54"/>
+    <tableColumn id="59" name="RewardPerc" dataDxfId="53"/>
+    <tableColumn id="60" name="RewardEndu" dataDxfId="52"/>
     <tableColumn id="14" name="RewardItem"/>
     <tableColumn id="15" name="RewardDrop"/>
-    <tableColumn id="73" name="RewardCollectType" dataDxfId="70"/>
-    <tableColumn id="55" name="RewardDungeonItemId" dataDxfId="69"/>
-    <tableColumn id="61" name="RewardDungeonItemCount" dataDxfId="68"/>
+    <tableColumn id="73" name="RewardCollectType" dataDxfId="51"/>
+    <tableColumn id="55" name="RewardDungeonItemId" dataDxfId="50"/>
+    <tableColumn id="61" name="RewardDungeonItemCount" dataDxfId="49"/>
     <tableColumn id="30" name="RewardBlessLevel"/>
     <tableColumn id="42" name="RewardBlessName"/>
-    <tableColumn id="52" name="RewardResId" dataDxfId="67"/>
-    <tableColumn id="53" name="RewardResAmount" dataDxfId="66"/>
+    <tableColumn id="52" name="RewardResId" dataDxfId="48"/>
+    <tableColumn id="53" name="RewardResAmount" dataDxfId="47"/>
     <tableColumn id="16" name="PunishGold"/>
     <tableColumn id="17" name="PunishFood"/>
     <tableColumn id="18" name="PunishHealth"/>
@@ -5939,15 +5939,15 @@
     <tableColumn id="22" name="TradeHealth"/>
     <tableColumn id="23" name="TradeMental"/>
     <tableColumn id="33" name="TradeDropItem"/>
-    <tableColumn id="4" name="FigueScene" dataDxfId="65"/>
-    <tableColumn id="70" name="FigueBig" dataDxfId="64"/>
+    <tableColumn id="4" name="FigueScene" dataDxfId="46"/>
+    <tableColumn id="70" name="FigueBig" dataDxfId="45"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="表3_5" displayName="表3_5" ref="A3:BV42" totalsRowShown="0" headerRowDxfId="63">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="表3_5" displayName="表3_5" ref="A3:BV42" totalsRowShown="0" headerRowDxfId="43">
   <autoFilter ref="A3:BV42"/>
   <sortState ref="A4:BT42">
     <sortCondition ref="A3:A6"/>
@@ -5955,61 +5955,61 @@
   <tableColumns count="74">
     <tableColumn id="1" name="Id"/>
     <tableColumn id="2" name="Name"/>
-    <tableColumn id="27" name="Type" dataDxfId="62"/>
+    <tableColumn id="27" name="Type" dataDxfId="42"/>
     <tableColumn id="3" name="Level"/>
     <tableColumn id="25" name="Danger"/>
     <tableColumn id="24" name="Ename"/>
     <tableColumn id="5" name="Script"/>
     <tableColumn id="6" name="TriggerMulti"/>
-    <tableColumn id="74" name="MapIcon" dataDxfId="61"/>
-    <tableColumn id="69" name="Tag" dataDxfId="60"/>
-    <tableColumn id="40" name="Catalog" dataDxfId="59"/>
-    <tableColumn id="29" name="Catalog2" dataDxfId="58"/>
-    <tableColumn id="35" name="TriggerHourBegin" dataDxfId="57"/>
-    <tableColumn id="34" name="TriggerHourEnd" dataDxfId="56"/>
-    <tableColumn id="37" name="TriggerQuestNotReceive" dataDxfId="55"/>
-    <tableColumn id="38" name="TriggerQuestReceived" dataDxfId="54"/>
-    <tableColumn id="36" name="TriggerQuestFinished" dataDxfId="53"/>
-    <tableColumn id="39" name="TriggerRate" dataDxfId="52"/>
-    <tableColumn id="62" name="TriggerLimitInDungeon" dataDxfId="51"/>
-    <tableColumn id="76" name="TriggerDNARate" dataDxfId="50"/>
-    <tableColumn id="77" name="TriggerDNAHard" dataDxfId="49"/>
-    <tableColumn id="78" name="DnaInfo" dataDxfId="48"/>
+    <tableColumn id="74" name="MapIcon" dataDxfId="41"/>
+    <tableColumn id="69" name="Tag" dataDxfId="40"/>
+    <tableColumn id="40" name="Catalog" dataDxfId="39"/>
+    <tableColumn id="29" name="Catalog2" dataDxfId="38"/>
+    <tableColumn id="35" name="TriggerHourBegin" dataDxfId="37"/>
+    <tableColumn id="34" name="TriggerHourEnd" dataDxfId="36"/>
+    <tableColumn id="37" name="TriggerQuestNotReceive" dataDxfId="35"/>
+    <tableColumn id="38" name="TriggerQuestReceived" dataDxfId="34"/>
+    <tableColumn id="36" name="TriggerQuestFinished" dataDxfId="33"/>
+    <tableColumn id="39" name="TriggerRate" dataDxfId="32"/>
+    <tableColumn id="62" name="TriggerLimitInDungeon" dataDxfId="31"/>
+    <tableColumn id="76" name="TriggerDNARate" dataDxfId="30"/>
+    <tableColumn id="77" name="TriggerDNAHard" dataDxfId="29"/>
+    <tableColumn id="78" name="DnaInfo" dataDxfId="28"/>
     <tableColumn id="7" name="EnemyName"/>
-    <tableColumn id="51" name="CanBribe" dataDxfId="47"/>
-    <tableColumn id="32" name="SceneId" dataDxfId="46"/>
-    <tableColumn id="54" name="DungeonId" dataDxfId="45"/>
-    <tableColumn id="50" name="CheckQuest" dataDxfId="44"/>
-    <tableColumn id="28" name="NextQuest" dataDxfId="43"/>
-    <tableColumn id="44" name="HiddenRoomQuest" dataDxfId="42"/>
-    <tableColumn id="8" name="ShopName" dataDxfId="41"/>
-    <tableColumn id="41" name="MiniGameId" dataDxfId="40"/>
-    <tableColumn id="43" name="PayKey" dataDxfId="39"/>
-    <tableColumn id="67" name="NeedDungeonItemId" dataDxfId="38"/>
-    <tableColumn id="68" name="NeedDungeonItemCount" dataDxfId="37"/>
-    <tableColumn id="63" name="TestType1" dataDxfId="36"/>
-    <tableColumn id="64" name="TestBias1" dataDxfId="35"/>
-    <tableColumn id="65" name="TestType2" dataDxfId="34"/>
-    <tableColumn id="66" name="TestBias2" dataDxfId="33"/>
+    <tableColumn id="51" name="CanBribe" dataDxfId="27"/>
+    <tableColumn id="32" name="SceneId" dataDxfId="26"/>
+    <tableColumn id="54" name="DungeonId" dataDxfId="25"/>
+    <tableColumn id="50" name="CheckQuest" dataDxfId="24"/>
+    <tableColumn id="28" name="NextQuest" dataDxfId="23"/>
+    <tableColumn id="44" name="HiddenRoomQuest" dataDxfId="22"/>
+    <tableColumn id="8" name="ShopName" dataDxfId="21"/>
+    <tableColumn id="41" name="MiniGameId" dataDxfId="20"/>
+    <tableColumn id="43" name="PayKey" dataDxfId="19"/>
+    <tableColumn id="67" name="NeedDungeonItemId" dataDxfId="18"/>
+    <tableColumn id="68" name="NeedDungeonItemCount" dataDxfId="17"/>
+    <tableColumn id="63" name="TestType1" dataDxfId="16"/>
+    <tableColumn id="64" name="TestBias1" dataDxfId="15"/>
+    <tableColumn id="65" name="TestType2" dataDxfId="14"/>
+    <tableColumn id="66" name="TestBias2" dataDxfId="13"/>
     <tableColumn id="9" name="RewardGold"/>
     <tableColumn id="10" name="RewardFood"/>
     <tableColumn id="11" name="RewardHealth"/>
     <tableColumn id="12" name="RewardMental"/>
     <tableColumn id="13" name="RewardExp"/>
-    <tableColumn id="55" name="RewardStr" dataDxfId="32"/>
-    <tableColumn id="56" name="RewardAgi" dataDxfId="31"/>
-    <tableColumn id="57" name="RewardIntl" dataDxfId="30"/>
-    <tableColumn id="58" name="RewardPerc" dataDxfId="29"/>
-    <tableColumn id="59" name="RewardEndu" dataDxfId="28"/>
+    <tableColumn id="55" name="RewardStr" dataDxfId="12"/>
+    <tableColumn id="56" name="RewardAgi" dataDxfId="11"/>
+    <tableColumn id="57" name="RewardIntl" dataDxfId="10"/>
+    <tableColumn id="58" name="RewardPerc" dataDxfId="9"/>
+    <tableColumn id="59" name="RewardEndu" dataDxfId="8"/>
     <tableColumn id="14" name="RewardItem"/>
     <tableColumn id="15" name="RewardDrop"/>
-    <tableColumn id="73" name="RewardCollectType" dataDxfId="27"/>
-    <tableColumn id="60" name="RewardDungeonItemId" dataDxfId="26"/>
-    <tableColumn id="61" name="RewardDungeonItemCount" dataDxfId="25"/>
+    <tableColumn id="73" name="RewardCollectType" dataDxfId="7"/>
+    <tableColumn id="60" name="RewardDungeonItemId" dataDxfId="6"/>
+    <tableColumn id="61" name="RewardDungeonItemCount" dataDxfId="5"/>
     <tableColumn id="31" name="RewardBlessLevel"/>
     <tableColumn id="42" name="RewardBlessName"/>
-    <tableColumn id="52" name="RewardResId" dataDxfId="24"/>
-    <tableColumn id="53" name="RewardResAmount" dataDxfId="23"/>
+    <tableColumn id="52" name="RewardResId" dataDxfId="4"/>
+    <tableColumn id="53" name="RewardResAmount" dataDxfId="3"/>
     <tableColumn id="16" name="PunishGold"/>
     <tableColumn id="17" name="PunishFood"/>
     <tableColumn id="18" name="PunishHealth"/>
@@ -6024,9 +6024,9 @@
     <tableColumn id="21" name="TradeFood"/>
     <tableColumn id="22" name="TradeHealth"/>
     <tableColumn id="23" name="TradeMental"/>
-    <tableColumn id="33" name="TradeDropItem" dataDxfId="22"/>
-    <tableColumn id="70" name="FigueScene" dataDxfId="21"/>
-    <tableColumn id="71" name="FigueBig" dataDxfId="20"/>
+    <tableColumn id="33" name="TradeDropItem" dataDxfId="2"/>
+    <tableColumn id="70" name="FigueScene" dataDxfId="1"/>
+    <tableColumn id="71" name="FigueBig" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -6355,8 +6355,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BV115"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AD1" workbookViewId="0">
-      <selection activeCell="AZ12" sqref="AZ12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="X16" sqref="X16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -7805,7 +7805,9 @@
       <c r="W16" s="66" t="s">
         <v>719</v>
       </c>
-      <c r="X16" s="22"/>
+      <c r="X16" s="22" t="s">
+        <v>11</v>
+      </c>
       <c r="AQ16" s="8">
         <v>100</v>
       </c>
@@ -14424,98 +14426,98 @@
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
-  <conditionalFormatting sqref="J27:AY28 J30:AY32 J39:AY39 J46:AY48 J53:AY53 J50:AY50 J61:AY61 J63:AY64 I95:I97 G27:H28 G30:H32 G39:H39 G46:H48 G53:H53 G50:H50 G61:H61 G63:H64 G115:AY115 G16:AY16 BU18:BU96 E18:F115 BV18:BV115 G67:H67 E4:F16 BU4:BV16 BB27:BT28 BB30:BT32 BB39:BT39 BB46:BT48 BB50:BT50 BB53:BT53 BB61:BT61 BB63:BT64 G18:BT26 G29:BT29 G33:BT38 G40:BT45 G49:BT49 G54:BT60 G51:BT52 G62:BT62 BB115:BU115 G65:BT66 G97:BU114 G68:BT96 J67:BT67 G4:BT15 BA16:BT17">
-    <cfRule type="containsBlanks" dxfId="19" priority="46">
+  <conditionalFormatting sqref="J27:AY28 J30:AY32 J39:AY39 J46:AY48 J53:AY53 J50:AY50 J61:AY61 J63:AY64 I95:I97 G27:H28 G30:H32 G39:H39 G46:H48 G53:H53 G50:H50 G61:H61 G63:H64 G115:AY115 BU18:BU96 E18:F115 BV18:BV115 G67:H67 E4:F16 BU4:BV16 BB27:BT28 BB30:BT32 BB39:BT39 BB46:BT48 BB50:BT50 BB53:BT53 BB61:BT61 BB63:BT64 G18:BT26 G29:BT29 G33:BT38 G40:BT45 G49:BT49 G54:BT60 G51:BT52 G62:BT62 BB115:BU115 G65:BT66 G97:BU114 G68:BT96 J67:BT67 G4:BT15 BA16:BT17 G16:AY16">
+    <cfRule type="containsBlanks" dxfId="98" priority="46">
       <formula>LEN(TRIM(E4))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I27:I28">
-    <cfRule type="containsBlanks" dxfId="18" priority="27">
+    <cfRule type="containsBlanks" dxfId="97" priority="27">
       <formula>LEN(TRIM(I27))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I30:I31">
-    <cfRule type="containsBlanks" dxfId="17" priority="26">
+    <cfRule type="containsBlanks" dxfId="96" priority="26">
       <formula>LEN(TRIM(I30))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I50">
-    <cfRule type="containsBlanks" dxfId="16" priority="22">
+    <cfRule type="containsBlanks" dxfId="95" priority="22">
       <formula>LEN(TRIM(I50))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AZ16">
-    <cfRule type="containsBlanks" dxfId="15" priority="19">
+    <cfRule type="containsBlanks" dxfId="94" priority="19">
       <formula>LEN(TRIM(AZ16))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BA63:BA64 BA61 BA53 BA50 BA46:BA48 BA39 BA30:BA32 BA27:BA28">
-    <cfRule type="containsBlanks" dxfId="14" priority="18">
+    <cfRule type="containsBlanks" dxfId="93" priority="18">
       <formula>LEN(TRIM(BA27))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AZ63:AZ64 AZ61 AZ53 AZ50 AZ46:AZ48 AZ39 AZ30:AZ32 AZ27:AZ28">
-    <cfRule type="containsBlanks" dxfId="13" priority="17">
+    <cfRule type="containsBlanks" dxfId="92" priority="17">
       <formula>LEN(TRIM(AZ27))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BA115">
-    <cfRule type="containsBlanks" dxfId="12" priority="16">
+    <cfRule type="containsBlanks" dxfId="91" priority="16">
       <formula>LEN(TRIM(BA115))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AZ115">
-    <cfRule type="containsBlanks" dxfId="11" priority="15">
+    <cfRule type="containsBlanks" dxfId="90" priority="15">
       <formula>LEN(TRIM(AZ115))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I98">
-    <cfRule type="containsBlanks" dxfId="10" priority="13">
+    <cfRule type="containsBlanks" dxfId="89" priority="13">
       <formula>LEN(TRIM(I98))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E17:AY17 BU17:BV17">
-    <cfRule type="containsBlanks" dxfId="9" priority="10">
+    <cfRule type="containsBlanks" dxfId="88" priority="10">
       <formula>LEN(TRIM(E17))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AZ17">
-    <cfRule type="containsBlanks" dxfId="8" priority="8">
+    <cfRule type="containsBlanks" dxfId="87" priority="8">
       <formula>LEN(TRIM(AZ17))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I32">
-    <cfRule type="containsBlanks" dxfId="7" priority="7">
+    <cfRule type="containsBlanks" dxfId="86" priority="7">
       <formula>LEN(TRIM(I32))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I39">
-    <cfRule type="containsBlanks" dxfId="6" priority="6">
+    <cfRule type="containsBlanks" dxfId="85" priority="6">
       <formula>LEN(TRIM(I39))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I46:I48">
-    <cfRule type="containsBlanks" dxfId="5" priority="5">
+    <cfRule type="containsBlanks" dxfId="84" priority="5">
       <formula>LEN(TRIM(I46))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I53">
-    <cfRule type="containsBlanks" dxfId="4" priority="4">
+    <cfRule type="containsBlanks" dxfId="83" priority="4">
       <formula>LEN(TRIM(I53))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I61">
-    <cfRule type="containsBlanks" dxfId="3" priority="3">
+    <cfRule type="containsBlanks" dxfId="82" priority="3">
       <formula>LEN(TRIM(I61))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I63:I64">
-    <cfRule type="containsBlanks" dxfId="2" priority="2">
+    <cfRule type="containsBlanks" dxfId="81" priority="2">
       <formula>LEN(TRIM(I63))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I67">
-    <cfRule type="containsBlanks" dxfId="1" priority="1">
+    <cfRule type="containsBlanks" dxfId="80" priority="1">
       <formula>LEN(TRIM(I67))=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -17710,7 +17712,7 @@
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <conditionalFormatting sqref="E4:BV42">
-    <cfRule type="containsBlanks" dxfId="0" priority="19">
+    <cfRule type="containsBlanks" dxfId="44" priority="19">
       <formula>LEN(TRIM(E4))=0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>